<commit_message>
feat: Added GPU processing for faster inference
</commit_message>
<xml_diff>
--- a/src/clustered_articles_with_themes.xlsx
+++ b/src/clustered_articles_with_themes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,170 +453,1700 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Time to wrap up… The energy regulator for Britain, Ofgem, has said it will increase the cap on energy bills from October by 2%, the equivalent of a £35 rise in annual bills for the average home, despite a 2% fall in the wholesale price in the energy markets over the last three months. Prices for households will go up just as the colder weather sets in because money is needed to cover the rising cost of the government’s energy policies. About £15 of the £35 increase will fund an expansion of the warm home discount scheme to provide an extra 2.7 million households with a £150 reduction in their bills. Thames Water has agreed a payment plan for £123m sewage and dividend fines, as it races to secure funding to avoid temporary government nationalisation. Earlier this month the government approved the appointment of insolvency advisers to consult on plans for Thames Water to be placed into a special administration regime (SAR). The debt-laden utility firm was hit with a record £104m fine by Ofwat in May over environmental breaches involving sewage spills, after failing to operate and manage its treatment works and wastewater networks effectively. At the same time, a further £18.2m fine was levied on Thames for breaking dividend rules, the first penalty of its kind in the water industry. The penalties were originally due to be paid by 20 August but the regulator gave the company some breathing space to pay the fines. Ofwat has now approved Thames’s request for a payment plan, which will result in it paying £24.5m, or 20% of the penalties, by the end of September, with the rest to be paid later. Lego builds record sales of £4bn as parents steer children away from smartphones. The Danish toy company said sales increased by 12% to a record 34.6bn Danish kroner (£4bn) in the first half of the year, rising well ahead of the recovering global toy market in which sales rose 7%. Niels B. Christiansen, chief executive, said Lego could be profiting from parents’ desire to keep children away from phones because of the effect of social media on mental health. Over in the US, the highlight of the day will be when the chip designer Nvidia reports its quarterly earnings after the market close, or around 9pm BST. Wall Street has opened flat today, with the S&amp;amp;P 500 share index down by 0.06% at the open. The Nasdaq index is also down slightly by 0.08%. All eyes will be on chip designer Nvidia today when it reports after the US market closes. Victoria Scholar, of the investment broker Interactive Investor, says: Nvidia gets set to release its second quarter results after the bell as the final US tech giant to report this season. There’s a lot of focus on this earnings report given that it comes off the back of a shaky period for tech stocks. The AI darlings like Nvidia, Palantir and Meta have suffered some selling pressure as investors start to question whether the winning streak is running out of steam. Sam Altman, CEO of OpenAI suggested a bubble could be forming in AI stocks and a report from MIT said 95% of organisations are getting zero return on generative AI investments. However this comes after a strong bull run off the April lows for Nvidia which rebounded to become the first public company to achieve a market cap of $4 trillion in July. …According to Refinitiv, Nvidia is expected to report Q2 earnings per share of $1 on revenues of $46 billion, up from 96 cents and $44.06 billion respectively in the previous quarter. There will be a lot riding on guidance for the rest of the year with investors looking for reassurances that Nvidia can continue to deliver growth. China will be another focal point following the resumption of its AI chip sales there after Nvidia agreed to pay the US government 15% of Chinese revenues. Last quarter, Nvidia said it lost out on $2.5 billion because of China export restrictions. Investors will also be paying close attention to its Blackwell business which made up 70% of Nvidia’s data centre sales last quarter. Elsewhere this afternoon, the London-listed warehouse owner Warehouse Reit confirmed that it has ended takeover talks with its rival Tritax Big Box Reit, clearing the way for a takeover by the commercial property investor Blackstone. Blackstone’s latest offer for the company amounts to 115p cash per share, valuing the business at about £489m. Here’s what markets are doing as we go into lunchtime… The FTSE 100 is flat as a pancake today – NatWest is the worst performer, with its shares down 2.4%. The best performer so far is JD Sports, though its shares are only up 1.7%. That is despite the fact that it reported a fall in sales in its second quarter, though investors appear to have taken confidence in the fact that performance in its North American market has improved slightly. The fashion retailer also announced another £100m share buyback. The mid-cap FTSE 250 index is down by 0.3%. The miner Hochschild is the worst performer, with its shares tumbling by roughly 14% today after it cut its production forecasts for the year. The stock market is pretty muted across Europe today, with the Stoxx 600 up slightly by 0.15%. Meanwhile the US dollar index, which tracks the greenback against a basket of other major currencies, is up 0.45%. The pound is now down 0.42% against the dollar to $1.34. The big market news is not landing until later this evening: Nvidia will report its quarterly earnings after the US markets close, after 9pm BST. The chip designer crossed the $4 trillion market capitalisation mark in July, becoming the biggest company in the world. Nvidia shares are up by 0.6% in pre-market trading. For now, futures for both the S&amp;amp;P 500 index and the Nasdaq are up just 0.03%. More bad news from the retail sector this morning: sales volumes fell in August, marking 11 consecutive months of decline, according to a survey by the Confederation of British Industry (CBI). The CBI’s monthly gauge of how retail sales compared with a year earlier stood at -32 this month, a slight improvement of -34 in July. Martin Sartorius, principal economist at the CBI, said: Retailers endured another tough month in August, with annual sales volumes falling for the eleventh consecutive month. Weak demand and higher labour costs continue to put pressure on margins, dampening sentiment across the retail and wider distribution sector. This downbeat outlook is reflected in firms’ plans to scale back investment and hiring. The government’s fiscal decisions are continuing to bite, and retailers’ struggles send a clear signal: business cannot be asked to balance the books again at the Autumn Budget. Building business confidence through delivery must be the priority — starting with a rethink of the Employment Rights Bill, which risks piling on unnecessary costs and holding back jobs and investment.” Fears that UK consumers will rein in spending sent jitters across the retail sector yesterday, wiping hundreds of millions of pounds off the value of some of the biggest retailers in the country, including the owners of Primark and B&amp;amp;Q, and the home improvement chain Wickes. The UK government has just sold £5bn worth in three-year bonds in a scheduled action. Demand was good, with the auction covered 3.16 times. The bonds were sold with a yield of 4.375%, due in 2028. The gilt market has been rocky lately, with yield on the 30-year bond trading close to its highest level since 1998 yesterday, at 5.62%. Yields rise when prices fall. The yield on the 30-year rose to as high as 5.627% in early trading this morning, but it has since recovered, with the yield now at 5.583%. Mohit Kumar, an analyst at the investment broker Jefferies, paints a gloomy picture of the UK’s economic outlook: We have held a negative view on the UK fiscal picture and maintain the view. We see UK growth disappointing relative to official forecasts which would leave the Chancellor with a bigger budget hole than current official forecast suggests. Tax rises look inevitable in the Autumn statement. However, we are approaching levels where further tax rises start becoming counterproductive. Producer output price inflation rose to 1.9% in the year to June, up from a revised rise of 0.7% in the year to April 2025, according to the Office for National Statistics. The ONS suspended the publication of its producer price indices in March, after it found calculation errors dating back to 2020. The figures published today represent interim data before it resumes regular publication in October. The statistics agency said in July that producer price inflation in previous years had been higher than originally calculated. It comes as pressure grows on the ONS over the reliability of its data. Staff at the Treasury and its independent spending watchdog have said they are struggling to get a clear picture of the economy because of problems at the ONS with producing reliable numbers. Shares in utility stocks are rising this morning after the energy regulator Ofgem announced that it will increase its price cap on bills by 2% from October. National Grid, SSE and Severn Trent are all up roughly 1% this morning, among the best performers in the UK’s blue chip FTSE 100 index. But overall the FTSE is not moving much, up very slightly by 0.03%. Over in Europe, the Stoxx 600 index is up 0.4%. The French Cac 40 share index recovered 0.4%, after a fall earlier in the week over concerns around the potential collapse of Prime Minister François Bayrou’s government. Turning back to energy bills, several UK charities are warning that the 2% rise in the energy price cap (which covers England, Wales and Scotland) will hurt vulnerable people. Official figures showed in May that energy bill defaults hit a record high, with 2.7% of direct debits for gas and electricity failing due to lack of funds. Disability equality charity Scope has said millions of disabled people are being pushed into deeper fuel poverty as prices continue to rise. Abdi Mohamed, head of policy at the charity, said: Life costs more if you are disabled – on average an extra £1,095 a month. We hear from disabled people every day who tell us they are unable to power vital medical and mobility equipment, facing increasing pain and losing their independence. The current support available for disabled people barely scratches the surface. And many no longer get the warm home discount at all, despite enormous energy costs. The government must act with urgency to close the devastating gap in support and tackle this crisis. Joanna Elson, chief executive of the charity Independent Age, argued political intervention is urgently needed, and that the warm homes discount should be extended to at least 2027. She said: Far too often older people in financial hardship are bed bound by the cold, turning in early for the night dressed in hats and scarves in a desperate bid to keep warm through the winter months. …The situation is dire, in the UK over one million older households are living in fuel poverty. The people in later life we speak to are making drastic and dangerous cutbacks because they cannot afford their energy bills. They are routinely switching off heating systems for weeks on end, visiting public places to stay warm and cutting down on food so they can pay their energy bills. This is unacceptable. Jon Sparkes, chief executive of the learning disability charity Mencap, said: People with a learning disability simply must be protected from ever increasing energy costs, or they face being pushed into fuel poverty, unable to stay safe, warm and healthy. The 1.5 million people in the UK with a learning disability are more likely to have unavoidably high energy costs because they may need to charge specialist or medical equipment or heat their homes for longer. …With bill prices set to increase even further this autumn, people with a learning disability and their families will continue to face these dangerous choices which leave them feeling anxious and afraid. Lego has built a bigger share of the toy market as sales rose 12% in the first six months of the year after its Botanicals and Grand Prix-themed sets helped it attract adults as well as children. As sales increased to 34.6bn Danish Kroner (£4bn), the company, which is known for its colourful building bricks, said it would open a new $1.5bn US factory and distribution centre in 2027, its seventh factory worldwide. The company previously said it was not bringing forward the development of the factory despite new import tariffs introduced by the Trump administration this year. The group opened a new site in Vietnam earlier this year and expanded factories in Mexico and Hungary to meet demand. Lego’s net profit increased 10% to 6.5bn Danish Kroner as the company said it had signed deals to produce toys linked to the Bluey and Pokémon cartoon series and launched the She Built That campaign to encourage girls to use Lego creatively. Niels B Christiansen, the chief executive, said: We are very pleased to have maintained our strong performance in the first half of 2025, winning share in the global toy market. This growth is driven by our large and innovative range of products that continues to be relevant across ages and interests. Shares in Rio Tinto have ticked up 1% this morning after the miner’s new boss, Simon Trott, announced he will combine some of its biggest businesses in an effort to simplify the group, just two days after taking leadership of the company. Rio will reorganise into three divisions: iron ore, aluminium and lithium, and copper, the company said on Wednesday. Trott, who took over from Jakob Stausholm on 25 August, previously led Rio’s iron ore operations in northwest Australia, which make up more than half its earnings. The Anglo-Australian miner has recently been trying to diversify its business, acquiring the US lithium producer Arcadium Lithium in a $6.7 billion deal earlier this year. It has made Rio one of the biggest producers of the battery-making metal in the world, alongside Albemarle and SQM. Thames Water has agreed a payment plan with the water regulator for fines it owes worth £123m, as it races to secure funding to avoid temporary government nationalisation. The water company, which serves 16 million customers across London and the south-east, is currently racing to pull together a deal to avoid collapse. Earlier this month the government approved the appointment of insolvency advisers FTI Consulting to consult on plans for Thames Water to be placed into a special administration regime (SAR). The debt-laden utility firm was hit with a record £104m fine by Ofwat in May over environmental breaches involving sewage spills, after failing to operate and manage its treatment works and wastewater networks effectively. At the same time, a further £18.2m fine was levied on Thames for breaking dividend rules, the first penalty of its kind in the water industry. Ofwat said the company had paid out cash to investors despite having fallen short in its services to customers and its environmental record. The penalties were originally due to be paid by 20 August but the regulator has given the company some breathing space to pay the fines. Ofwat had previously told Thames the penalties had to be “paid by the company and its investors, and not by customers”. The regulator has approved Thames’ request for a payment plan, which will see it pay £24.5m, or 20% of the penalties, by the end of September, with the rest to be paid later. Lidl has invested £435m in warehouses in Leeds and London, developments it says will create more than 500 new jobs. The supermarket has completed its extension of its Belvedere warehouse site in London, which now has 800,000 sq ft, a 167% increase compared with when it opened in 2003. Last month Lidl also started construction at a 38-acre site in Gildersome, Leeds, with a new warehouse there expected to create 400 new jobs. The expansion at the site in London will create 120 new jobs, Lidl said. It comes after the Resolution Foundation, a think tank, predicted the unemployment rate could hit 5% in the three months ended in August, the highest level since the start of 2021. The official unemployment rate was 4.7% in the last quarter. Chancellor Rachel Reeves praised Lidl’s investment as “a strong vote of confidence in the UK economy”, though economists have warned that Britain faces serious challenges due to its weak underlying growth and a drop in the number of workers since the pandemic. Reeves said: Lidl’s commitment to new warehouse facilities in London and Leeds will unlock hundreds of new jobs, strengthen supply chains, and ensure families can access affordable, quality food. Through our Plan for Change we’re backing business and working in partnership to deliver growth and opportunity in communities across the country. Over on the corporate front in the UK, fashion retailer JD Sports has reported a 3% drop in like-for-like sales in the 13 weeks ended on 2 August. Chief executive Régis Schultz said the company was going up against tough comparators in Europe and the UK from the Euros football tournament last year, but “across our regions and fascias, in general we see a resilient consumer, albeit very selective on their purchases.” The retailer also said that it would launch another £100m share buyback. Elsewhere, miner Rio Tinto’s new chief executive Simon Trott has announced that he will combine some of its biggest businesses in an effort to simplify the group. Rio will reorganise into three divisions: iron ore, aluminium and lithium, and copper, the company said on Wednesday. Trott said: A simplified business structure, grounded in our fundamental commitment to safety and with sharper focus on the most compelling opportunities we have, will enable us to deliver new standards of operational excellence and value creation. While another rise in energy bills will be unwelcome news for many, analysts at the consultancy Cornwall Insight have said that prices could fall under the next cap, which would start in January 2026. Dr Craig Lowrey, of Cornwall Insight, said: There is better news on the horizon with bills currently expected to ease in January, driven by a forecast fall in wholesale prices. Normally, that drop would have meant even lower bills, however, rising policy costs, such as funding for new nuclear projects are keeping bills a little higher. These policy-driven costs are part of a broader shift in how we fund the energy transition. Nuclear will be one of the cornerstones of a more secure and sustainable energy system, yet some of the funding will ultimately need to come from billpayers. This is a difficult trade off - after all, everyone wants to see bills come down. However, the challenge we face is clear: if we want to build a resilient, low-carbon energy future, we must be prepared to invest in it today.” The energy regulator for Britain, Ofgem, has said it will increase the cap on energy bills from October by 2%, the equivalent of a £35 rise in annual bills for the average home. Here’s more details of the energy price cap just announced, from Ofgem. Electricity rates If you are on a standard variable tariff (default tariff) and pay for your electricity by Direct Debit, you will pay on average 26.35p pence per kilowatt hour (kWh). The daily standing charge is 53.68 pence per day. This is based on the average across England, Scotland and Wales and includes VAT. Gas rates If you are on a standard variable tariff (default tariff) and pay for your gas by Direct Debit, you will pay on average 6.29 pence per kilowatt hour (kWh). The daily standing charge is 34.03 pence per day. This is based on the average across England, Scotland and Wales and includes VAT. Why energy prices have gone up Volatile global wholesale prices for energy are partly behind the increase, as well as the cost of the government’s expansion of its warm home discount policy. Tim Jarvis, director general for Markets at Ofgem, says: While there is still more to do, we are seeing signs of a healthier market. There are more people on fixed tariffs saving themselves money, switching is rising as options for consumers increase, and we’ve seen increases in customer satisfaction, alongside a reduction in complaints. While today’s change is below inflation, we know customers might not be feeling it in their pockets. There are things you can do though – consider a fixed tariff as this could save more than £200 against the new cap. Paying by direct debit or smart pay as you go could also save you money. In the longer term, we will continue to see fluctuations in our energy prices until we are insulated from volatile international gas markets. That’s why we continue to work with government and the sector to diversify our energy mix to reduce the reliance on markets we do not control. Jarvis, speaking to Radio 4’s Today programme, also noted that the cost of running the network and the expansion of the government’s warm home discount scheme had also driven the rise in the cap. The rise in energy costs will hit people already struggling to pay their household bills, warns National Energy Action, the fuel poverty charity. Michael Penhaligon, of the NEA, says: Every day my colleagues and I speak to people in desperate circumstances. They can’t afford the very basics of heat and power. They are rationing their energy usage and they’re cutting back on food and other essentials. The individuals I speak to are left to rely on foodbanks, fuel vouchers and other charitable grants to help restore them to a basic standard of living. This shouldn’t be happening in the UK in 2025. Some may say that the cap rising around £35 won’t have an impact but the people I speak to already can’t afford their bills and many of them are deep in debt. This can have a huge impact on their mental and physical wellbeing. A rise in bills just as temperatures start to drop will put even more pressure on households. My colleagues and I achieve amazing outcomes for households to help them afford their energy; we get debt written off, we get them access to benefits they are entitled to, and we liaise with their suppliers on their behalf. But the scale and depth of fuel poverty is far beyond the remit of any charity. Newsflash: The energy price cap on bills across Great Britain will rise by 2% in October, regulator Ofgem has announced. This will lift the average annual cost of electricity and gas for a typical household to £1,755 per year. This is the fourth consecutive hike in the cap on gas and electricity charges, and is slightly higher than analysts had just expected. The cap limits the amount which a supplier can charge for a unit of electricity or gas. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. The cost of living could be about to get even tighter, as households find out whether their energy bills will rise again this autumn. Ofgem, the energy regulator, is due to announce the latest price cap on the cost of a unit of energy at 7am. Analysts expect the cap to rise due to recent increases in wholesale gas and electricity prices. Consultancy Cornwall Insight have predicted Ofgem will increase the cap by about 1% to £1,737 a year for a dual-fuel household, from the current level of £1,720. A rise in energy prices would act as yet another driver for high inflation. Official figures showed last week that UK inflation rose in July to a higher-than-expected 3.8% amid higher food prices and travel costs. It marked the 10th consecutive month that inflation has sat above the Bank of England’s 2% target. The new cap will come into effect in October and remain in place until the end of the year. The energy price cap sets the maximum that a supplier can charge for a unit of energy (there’s no cap on how high a bill can go). Elsewhere, overnight Donald Trump has imposed 50% tariffs on most US imports from India, following through on his threat to punish one of the world’s largest economies over its purchases of discounted Russian oil. The tariffs, which came into effect just after midnight on Wednesday in Washington, risk inflicting significant damage on the Indian economy and further disrupting global supply chains. US tariffs of 25% on Indian goods went into force earlier this month, but Trump announced plans to double the rate, citing India’s purchases of Russian oil, which the White House has argued is indirectly funding Russia’s war against Ukraine. The agenda 7:00AM BST: Energy regulator Ofgem announces UK energy price cap for October-December 10:00AM BST: UK 2028 gilt auction After 9:00PM BST: Nvidia quarterly earnings report</t>
+          <t>It’s back to school this week for MPs and government ministers – and few can be facing a more challenging new term than Rachel Reeves. After being moved to tears in the unforgiving glare of the cameras before the summer break, the chancellor’s allies say she is returning to the frontline with a renewed sense of purpose. She is ready, as the kids would say, to “lock in”. But team Reeves is also well aware of the scale of the economic and political obstacles ahead. Most pressing, yet out of the chancellor’s hands, is the Office for Budget Responsibility’s (OBR) summer “supply stocktake” of its economic model. As we reported in June, it looks likely that the OBR will move its key productivity forecast closer to the less-positive consensus. Given the crucial importance of productivity in determining economic growth, this shift could create a £20bn headache for the Treasury. The downgrade – not anything Labour has actually done – is likely to be the biggest factor pushing Reeves off track from her fiscal rules. That creates a formidable challenge in explaining what has gone awry – and why she needs to come back with more tax increases, after last year’s historic £40bn budget package. Expect to hear much more of the kind of language Reeves used in her recent Guardian article, in which she argued that “if renewal is our mission and productivity is our challenge, then investment and reform are our tools”. She does have a story to tell here: changing the fiscal rules to prioritise investment has allowed the Treasury to give the green light to scores of pro-productivity infrastructure projects (with the next expected to be Northern Powerhouse Rail). In the same vein, expect tax rises to be badged as efficiency enhancing, as well as revenue raising. Officials do not yet know the scale of the fiscal gap they will need to fill, though they expect it to be large. Reeves’s decision to involve Torsten Bell, formally the pensions minister, in budget preparations points to a willingness to think more radically. Bell has argued in the past for changes to the taxation of unearned income, property wealth – which we know the Treasury is looking at closely – and pensions. Reeves made moves in this direction last autumn, with changes to inheritance and capital gains taxes, but this budget must be the moment to “go big”, as Bell’s former boss Ed Miliband would put it. (Arguably, the moment was, in fact, last July, but here we are.) Yet as she draws up her plans, Reeves must have her eye on at least three different audiences, each in their way as tough as the meanest girls in the dining hall. The first, and most important, is the public, to whom the chancellor may be best known as the author of last year’s botched removal of the winter fuel allowance. While she is claiming to have been “fixing the foundations” in her first year in the job, it may not feel like it for families facing resurgent inflation, which hits low earners hardest. And unfortunately, “Labour crashed the economy”, while unfair, is a much cleaner explanation for fresh tax rises than “the OBR has systemically overestimated productivity, which hasn’t recovered since the financial crisis”. Reeves will need to convince cash-strapped voters she understands their struggles and has a plan to help. Also watching Reeves closely will be those behind her, in her own party. Once seen as a potential future leader, she is blamed by some Labour MPs for a series of dire missteps, including on winter fuel and the botched spring statement welfare cuts. Keir Starmer’s decision to bring in the former Bank of England deputy governor Minouche Shafik as his economic adviser, and the senior Treasury civil servant Dan York-Smith as principal private secretary, appears to indicate a new determination in No 10 to shape the government’s economic project instead of subcontracting it wholesale to Reeves. Given the prime minister’s temperamental caution, these hires seem unlikely to presage any dramatic change of course. But they do raise the prospect of cracks emerging between No 10 and No 11, which rarely ends well. Reeves’s third audience is among what her battle-scarred Labour predecessor Denis Healey called “the faceless men” (and, these days, women) managing the “atomic cloud of footloose funds” in financial markets. Talk of an IMF bailout is well wide of the mark but with debt interest expected to cost the taxpayer more than £100bn this year, even modest moves in government bond markets can be extremely costly. Judging by the bond sell-off in July when Reeves’s tears were read as a sign that she was on the way out, investors are minded to trust her – or at least, more than any potential alternative. But to keep the support of this tough crowd, tax rises will have to be straightforward (and big) enough to close any fiscal gap convincingly, yet calibrated not to put the kibosh on growth or jack up inflation. Given the 10 weeks’ formal notice the Treasury gives the OBR of the budget date, it cannot now happen until November. Reeves will want to set some parameters in public long before that, to contain what has already become frenzied speculation, but she would be wise not to waste what may be Labour’s best crack at reforming our out-of-kilter tax system.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ofgem has said it will increase the cap on energy bills from October by 2%. This is the equivalent of a £35 rise in annual bills for the average home. Prices will go up just as the colder weather sets in because money is needed to cover the rising cost of the government's energy policies.</t>
+          <t>Chancellor's allies say she is returning to the frontline with a renewed sense of purpose. But team Reeves is also well aware of the scale of the economic and political obstacles ahead. Office for Budget Responsibility’s (OBR) summer “supply stocktake’ of its economic model.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Economic and Market Volatility</t>
+          <t>UK Economic Challenges Overview</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Time to wrap up… UK retailer stocks sold off today after a downbeat note from analysts at Deutsche Bank. Associated British Foods, which owns Primark as well as a range of other food and drink brands such as Twinings, fell by as much as 5% today, after analysts at the bank downgraded their view on the stock from a neutral “hold” to “sell”. Deutsche also downgraded its view on home improvement retailer Wickes to a “sell”, and B&amp;amp;Q owner Kingfisher was moved down from a “buy” to a “hold”. Meanwhile, the US stock market has had a rather subdued open, with the S&amp;amp;P 500 rising slightly by 0.5% in early trading as the stock market seems to shake off worries about Trump’s latest attack on the Fed. Trump has moved to oust Lisa Cook, a governor at the Federal Reserve, in his latest attack on the American central bank. It is an unprecedented intervention by a US president, which threatens to undermine the independence of the central bank of the biggest economy in the world. Meanwhile, Trump has also threatened to impose tariffs and export restrictions on countries whose taxes, legislation and regulations target US big tech companies such as Google, Meta, Amazon and Apple. In a post on his social media platform, Truth Social, the US president said: “Digital taxes, legislation, rules or regulations are all designed to harm, or discriminate against, American technology.” He said such measures – which include the UK’s digital services tax, which raises about £800m annually from global tech companies through a 2% levy on revenues – also “outrageously give a complete pass to China’s largest tech companies”. Trump said: “As the president of the United States, I will stand up to countries that attack our incredible American tech companies. Unless these discriminatory actions are removed, I, as president of the United States, will impose substantial additional tariffs on that country’s exports to the USA, and institute export restrictions on our highly protected technology and chips.” UK tech firm Filtronic has announced its biggest ever contract worth £47.3m with Elon Musk’s SpaceX. Shares in the County Durham-based defence and telecoms equipment maker rose nearly 5% on Tuesday after the announcement. The contract covers supply of a type of radio frequency tech designed for high-performance wireless communication, using next-generation gallium nitride (GaN) E-band technology. Nat Edington, Filtronic CEO, said: We are extremely proud to announce this landmark contract, which not only sets a new commercial record for Filtronic, but also reflect the success of our partnership with world-leading satellite company SpaceX, supporting the Starlink constellation. It comes after Filtronic announced a £16.8 million contract in February with the US aerospace firm. The Bank of England policymaker Catherine Mann has said that while she thinks it is appropriate to hold interest rates at their current level, she stands ready to cut forcefully if there are serious risks to economic growth. Mann, who will appear at the Future of Central Banking conference at the Banco de México today, will say in a speech: A more persistent hold on Bank Rate is appropriate right now, to maintain the tight (but not tighter) monetary policy stance needed to lean against inflation persistence persisting. However, I stand ready for a forceful policy action, in the form of larger, more rapid Bank Rate cuts, should the downside risks to domestic demand start materializing. The Bank of England’s monetary policy committee cut interest rates to 4% earlier this month, in line with projections of falling inflation over the next two years. However, several of its members, including Mann, voted to hold interest rates until the trend became clearer. She will say in her speech today: In my assessment, the scenario outlining upside risks to inflation through inflation persistence (which included additional second round effects in domestic price and wage-setting, amplified by weak potential productivity growth) is playing out, whereas the ‘downside risk to demand’ scenario remains a risk and is not my central case. Full year results for Debenhams have just landed: revenue fell 1% in the year ended in 28 February to £790.3m, while its continuing loss before tax widened from £164.4m in its last financial year to a loss of £263.9m. However, shares in the retailer, which also owns brands boohoo and Karen Millen, are up by 2.2%. Investors are taking confidence in the fact that the company says all of its brands are now trading profitably in terms of adjusted Ebitda, and that it expects this measure of profit to be higher in its next half compared with the year prior. The company also said it is exploring a potential sale of PrettyLittleThing, the fast fashion brand aimed at young women, as part of its business review. Dan Finley, who has been chief executive of the group since November, said: The business has been through a very challenging period which is reflected in these results. I want to assure shareholders that the business is taking the necessary actions, quickly and decisively, to address the challenges that we face. No stone will be left unturned. …We are focused on delivering on the huge opportunity ahead for the Debenhams brand. Work is progressing to reposition and right size the Youth Brands, with a laser focus on profitability and cash generation under new management. This will be a multi-year turnaround as was the case with the Debenhams brand. As part of our ongoing business review, we are exploring a potential sale of PLT. We are also assessing long-term options for our US and Burnley distribution sites to enhance efficiency and ensure alignment with our stock-lite strategy. A strikes by hold baggage screeners at Gatwick airport scheduled for the end of this month has been called off, after workers voted to accept an improved pay deal. The workers, employed by ICTS, will receive a 7% pay rise back paid to April 2025, the Unite union said. The deal means that strikes scheduled from 29 August to 2 September will now not take place. The yield on the 30-year US Treasury has risen by 0.022 percentage points to 4.909%, as investors worry that Donald Trump’s latest attempt to intervene with the Federal Reserve could undermine the independence of the American central bank. Meanwhile, the yield on the two-year Treasury has dropped by 0.028 percentage points to 3.694%, as investors expect that pressure from the US president could lead to faster rate cuts. The market is pricing in an 82% chance of a cut in mid-September, when the rate-setting Federal Open Market Committee is next scheduled to meet. The US stock market looks like it will fall slightly at the open, with futures for the blue chip S&amp;amp;P 500 index down by 0.06%, and futures for the Nasdaq down 0.03%. The blue-chip FTSE 100 index is trading down 0.5% so far today. B&amp;amp;Q owner Kingfisher is the worst performer in the group, with its shares down 4.1%. Primark owner Associated British Foods is a close second, down 3.8%, after a downbeat note from analysts at Deutsche Bank about the outlook for British retail. The mid-cap FTSE 250 index is also down by 0.9%, led by an 8% drop at home improvement retailer Wickes. Distributor Bunzl is the best performer in the FTSE 100, with its shares up 5% after it told investors that it would restart its share buyback programme. British American Tobacco is among the worst performers, down 2.5%, after it told investors this morning that its chief financial officer, Soraya Benchikh, will step down from her role effective today. Vacancies for entry-level jobs have hit their lowest level in five years, according to the job search site Adzuna. The proportion of new entry-level jobs has dropped to just over a fifth of the overall market, it found, its lowest share since 2020. The number of overall vacancies dropped 1.2% in July to 864,705, Adzuna found. Graduate jobs nudged up 2.5% against June, but are still down 28% compared with the same time last year. Salaries for listed jobs also fell by 0.3%, as competition for work has heated up: there are now roughly 2 jobseekers per vacancy, Adzuna said. Andrew Hunter, co-founder of Adzuna, said: After a hopeful uptick in June, July saw the pendulum swing back with vacancies falling again. While salary growth remains one of the few consistent positives – continuing to outpace inflation – hiring appetite is clearly uneven. The ongoing strength in sectors like construction is in stark contrast to another consecutive monthly drop in healthcare roles – traditionally one of the most stable sectors. This speaks to a market still finding its footing. Until we see greater stability across the board, it’s likely this stop-start pattern will continue. Vacancies in healthcare have dropped 25.4% since April, when the government changed the rules for employer national insurance contributions and the minimum wage. The decline in entry-level jobs come as official figures show the number of young people not in education, employment or training (Neet) has leapt by more than a quarter in the past five years to reach almost 1 million. Liz Kendall, the work and pensions secretary, told my colleague Richard Partington that Labour has a “mountain to climb” to bring down the numbers: The cost of insuring French government debt against default has risen today, but remains extremely low. Data from S&amp;amp;P Global show that the cost of a five-year French credit default swap has risen to 37 basis points, the highest since May, Reuters reports. That level indicates there’s very little chance of France defaulting. For comparison, during the eurozone debt crisis of 2015, Greece’s 5-year credit default swaps rose over 1,900bps, amid heightened fears that Athens could default on its debts. There’s also gloom in the UK hospitality sector, where late-night venues have been closing at an alarming rate. More than one in four late-night venues have shut their doors since 2020, according to new data from the Night Time Industries Association (NTIA), who are calling on the government to cut VAT, reverse the increase in employers’ national insurance contributions, and maintain business rates relief for the sector. More here: Wood Group has come a step closer to becoming the latest company to leave the London Stock Exchange, after the board of the British oil services company said it was minded to accept a reduced takeover offer from a Dubai-based suitor. Sidara, the Middle Eastern engineering company, initially proposed a 35p-a-share offer in April. However, on Tuesday the company said that having completed due diligence Sidara would make a lower offer of 30p a share, once remaining preconditions had been met. The FTSE 250-listed company said it had evaluated the new offer with its financial advisers and concluded that it was “at a value the board would be minded to recommend to shareholders”. As a result the deadline for Sidara to announce a firm intention or withdraw its offer has been extended, again, to 5pm on 28 August. UK retail stocks are selling off this morning after a downbeat note from analysts at Deutsche Bank. Associated British Foods, which owns Primark as well as a range of other food and drink brands such as Twinings, has fallen by 5% this morning, after analysts at the bank downgraded their view on the stock from a neutral “hold” to “sell”. Deutsche also downgraded its view on home improvement retailer Wickes to a “sell”, with its shares falling by as much as 9% this morning, making it the worst laggard in the mid-cap FTSE 250 index today. B&amp;amp;Q owner Kingfisher was moved down from a “buy” to a “hold” rating, sending its shares down by as much as 4% this morning. Adam Cochrane and Benjamin Yokyong-Zoega, of the bank, said: We are taking a more cautious view on the UK consumer. The end of 2024 and early 2025 are likely to have been the sweet spot with real wage growth set to slow and fear of unemployment set to build from here. Our Household Cash Flow model shows discretionary spending lagging spending power and, unless consumers reduce savings, there will be a 4ppt slowdown in discretionary spend to +3% in 2H from +7% in 1H. Retail sales have been resilient into Q2 helped by warm weather although there is some variance by category. Consumer confidence metrics remain subdued and our new DB “Fear Index” suggests things may be getting worse. The bank also lowered its target prices for Dunelm and Marks &amp;amp; Spencer, although still retained their “buy” ratings on the stocks. The shares are down 0.6% and 0.5% respectively this morning. The wobble in the UK bond market also follows a high reading for food inflation from the British Retail Consortium. It found that shop prices had risen at their fastest pace for 18 months, with food inflation hitting 4.2% in August. That was driven by a jump in the cost of grocery staples such as eggs and butter, the industry body said. Helen Dickinson, chief executive of the BRC, said the rapid rise added to the pressure on people already struggling with the cost of living. Staples such as butter and eggs saw significant increases due to high demand, tightening supply, and increased labour costs. Chocolate also got more expensive as global prices of cocoa remain high owing to poor harvests. UK bonds are falling this morning: the yield on the two-year gilt rose by as much as 6 basis points to 4.008%, while the yield on the 30-year gilt also rose by 5.634%, its highest point since April. Bond yields rise when prices fall. It follows a rise in US Treasury yields after Donald Trump ordered the removal of Lisa Cook from the board of governors on the Federal Reserve, the US central bank. The sell-off in the bond market also follows reports over the weekend that the UK is facing an “IMF bailout”. Jagjit Chadha, a professor of economics at the University of Cambridge and former head of the National Institute for Economic and Social Research, claimed the economy was at risk of “collapse”. He said the financial situation was “as perilous the period leading up to the IMF loan of 1976”, when Britain had to be bailed out by the global banking body. He told the When the Facts Change Substack, written by Liam Halligan: I’m in a world in which I could imagine it [an IMF bailout] happening, and we’ll be bereft in that case. We will not be able to roll over debt, we will not be able to meet pensions payments, benefits will be hard to pay out.” The pound is also a bit weaker this morning, down by 0.01% against the US dollar to $1.3456. European shares are broadly down this morning, with the European Stoxx 600 index down by 0.7%. That was led by France’s Cac 40 index, which has dropped by 1.4%, mirroring a fall in its bond market. The UK’s blue chip FTSE 100 index is down by 0.6% this morning, with Associated British Foods, the owner of Primark, the biggest faller, down 3.9%. Meanwhile, the German Dax index has dropped 0.9%, while the Italian FTSE MIB has fallen by 1.2%. Political uncertainty in France is shaking its bond market, with its 10-year bond yield rising by as much as 2 basis points this morning to trade around 3.51%, its highest level since March. Bond yields rise when prices fall. It comes after Prime minister François Bayrou called a confidence vote that could topple the French government next month, as he tries to find support for plans to shore up the government’s ailing public finances. Bayrou has said France is going through a “decisive moment”. If the government secures a majority in the confidence vote, it would be confirmed, he said, but “if it does not have a majority, the government will fall”. Charlotte de Montpellier, senior economist at the broker ING, says the “obstacle is almost impossible to overcome”. Bayrou’s centrist coalition holds just 210 of 577 seats in the Assembly. The far-right RN, far-left LFI, Greens, and Communists—together 264 MPs—have already declared they will vote against him. Only the Socialist Party could tip the balance, but early signals suggest they are unwilling to support the government without major revisions to the budget, which seems unlikely. …If Bayrou loses the vote, President Macron will face a difficult choice: appoint a new prime minister capable of forming a government in a fragmented Assembly, or dissolve Parliament and call new elections—something he has previously ruled out. Either path would inject fresh uncertainty into an already fragile political landscape. The likely fall of the government will weigh heavily on the French economy. With only 0.8% GDP growth expected this year, the economy was already weak, and the political crisis adds a new layer of uncertainty. Drafting and passing a 2026 budget will become even harder, delaying fiscal consolidation and potentially worsening France’s debt trajectory. The longer reforms are postponed, the greater the eventual adjustment will need to be. In short, France’s political instability is becoming an economic liability. Investors and institutions will be watching closely—not just for what happens on 8 September, but for what comes next. Closer to home, there are a few corporate updates after the bank holiday. Soraya Benchikh, chief financial officer at British American Tobacco, is stepping down today, the company said in a statement. Javed Iqbal will act as the interim CFO until the company appoints a permanent successor. Meanwhile the FTSE 100 distribution group Bunzl has reported that its first-half sales rose by 0.8% to £5.76bn, in line with expectations. Pre-tax profit fell by 10.5% to £250.2m in the six months ended in June. However, the company said it would resume the remaining £86m of its previously announced £200m share buyback, after pausing it in April. Trump’s attempt to intervene at the Federal Reserve has spooked investors, with gold, which is viewed as a safe haven asset, rising this morning. Economists at Deutsche Bank write: Gold spiked by +1% and is holding on to most of this overnight gain, while futures on the S&amp;amp;P 500 (-0.14%) and the Nasdaq (-0.18%) are modestly lower. Meanwhile, the Treasury curve has seen a sizeable steepening, with the 2yr yield trading -0.7bps lower but the 10yr up +2.9bps and the 30yr +4.5bps to 4.93%. This has brought the 2s30s slope to 122bps, its steepest since January 2022 when the Fed had not yet started its post-Covid hiking cycle. Cook’s removal could push the Fed to a more dovish stance, say economists at Deutsche Bank. They write: Were Cook’s dismissal to hold, it would open up another seat for Trump to fill on the seven-person Federal Reserve Board. With Stephen Miran nominated for the seat recently vacated by Governor Kugler and with Governors Waller and Bowman dissenting in favour of a rate cut at the July meeting, this would increase the prospects of a dovish majority on the Board. Cook, who was appointed by President Joe Biden in 2022, was working a term that was not due to expire until 2038. If she were to be removed, it would give Trump the change to secure a four-person majority on the Fed’s board of governors. Market bets suggest there is an 82% chance that the Fed will vote to cut its key interest rate at its next meeting in mid-September. However, economic data coming out this week on inflation and the labour market could still sway the decision. Here is Justin Wolfers, an economics professor at the University of Michigan, drawing a parallel with Turkey’s president Recep Tayyip Erdoğan. Donald Trump has moved to oust Lisa Cook, a governor at the Federal Reserve, in his latest attack on the American central bank. It is an unprecedented intervention by a US president, which threatens to undermine the independence of the central bank of the biggest economy in the world. Trump posted a letter on his social media platform Truth Social on Monday, claiming he had “sufficient cause” to fire Cook, based on allegations she made false statements on one or more mortgage loans. Cook, who is the first black woman to serve on the Fed Board in Washington, has sad that Trump has no authority to fire her and that she will not quit. She said: I do intend to take any questions about my financial history seriously as a member of the Federal Reserve and so I am gathering the accurate information to answer any legitimate questions and provide the facts. The news has spooked markets, with the US dollar and long-dated Treasuries both falling on Tuesday. The US dollar index, which tracks the greenback against a basket of other major currencies, fell by 0.1%. Trump’s latest attack on the Fed follows “relentless pressure” on Fed Chair Jerome Powell, notes Tony Sycamore, of the broker IG. He says: In the short term, the removal of Cook who has tended to vote with the FOMC majority, increases the likelihood of a Fed rate cut at the September FOMC meeting. A prospect expected to weigh on the US dollar and lend support to equities and other risk assets, including Bitcoin. However, beyond the “sugar hit” of a rate cut in September, recent developments around key Fed personal, heighten concerns over rising political interference, raising the risk that traders view the Fed as politically compromised. This could trigger a rerun of the “Sell US assets” theme seen earlier this year. In such a scenario, both the US dollar and US equities could experience sharp declines. The agenda 1:30pm BST: US durable goods orders 2:00pm BST: Case-Shiller US house prices 3:00pm BST: US CB consumer confidence report</t>
+          <t>Time to wrap up… Former UK prime minister Liz Truss has claimed that “a reckoning” is coming for central banks in the UK,, US and the eurozone. Truss also backed Donald Trump’s attempts to exert greater control over the US Federal Reserve, telling Bloomberg’s Odd Lots podcast it was wrong that unelected central bankers could thwart elected politicians. Trump’s bid to shake up the Fed faces a legal battle, though – Federal Reserve governor Lisa Cook has filed a lawsuit claiming the US president has no authority to fire her. But there was good news for the Trump White House today – US economic growth was faster than expected in April-June. The economy grew at an annual rate of 3.3% in April-June, lifted by investment in computer hardware for AI systems. Tesla is still paying the price for Elon Musk’s brush with politics. Its sales across Europe tumbled by 40% in July, at a time when Chinese rival BYD is growing its market share. The power generator Drax has revealed it is under investigation by the City watchdog over “historical statements” made about the sourcing of wood pellets for its biomass power station,, knocking its shares down almost 7%. Stocks have opened calmly on Wall Street, despite some disappointment with Nvidia after its financial results last night. The S&amp;amp;P 500 share index has dipped by just one points, or 0.026%, in early trading while the tech-focused Nasdaq index is 0.2% higher. Nvidia’s shares have dropped by around 2% in early trading, after it missed forecasts for data center revenue but also beat expectations for adjusted earnings per share. Overall, revenues were up 56% compared with a year ago, which might calm concerns that the AI boom was fading. Kathleen Brooks, research director at XTB, reports that there is disappointment that Nvidia didn’t report any sales of its H20 chip to China last quarter, even though China export restrictions were eased. Brooks adds: Ultimately, the market does not know how big the China market is for Nvidia, or the impact of the Chinese government encouraging a move away from Nvidia’s chips, especially for government systems. Thus, this earnings report does not give us too much information on future sales growth to China, and it also fails to deliver what analysts want to know: the potential sales growth for Nvidia’s chip that has been designed specifically for the Chinese market. The upward revision to US growth in April-June was partly due to the hi-tech investment boom as companies race to build artificial intelligence data systems. Capital Economics explain: That revision was partly a consumption story – with consumer spending now estimated to have rebounded to 1.6% in the second quarter from 0.5% in the first. Even more encouraging, however, is the increasingly concrete signs of an AI-related boom in tech investment. Investment in computer hardware increased by 61.2% annualised, slightly more than in the initial estimate. But the big revision came in software investment, which is now estimated to have expanded at a 26.4% annualised pace – the biggest quarterly gain since at least 2007. Just in: Federal Reserve Governor Lisa Cook filed a lawsuit challenging President Donald Trump’s attempt to fire her over claims she lied on mortgage applications, Bloomberg reports. The move, which was expected, kicks off a historic fight over independence of the US central bank. Cook filed the suit Thursday in federal court in Washington, according to court records. Donald Trump announced he was firing Cook on Monday night, over unconfirmed allegations of mortgage fraud. Over in the US, economic growth last spring was stronger than first estimated. The latest assessment of US GDP, just released, shows the economy expanded at an annualised rate of 3.3% in April-June, up from the initial estimate of 3% growth. That confirms that the world’s largest economy returned to growth after shrinking by 0.5%/year in January-March, when a surge of imports dragged down GDP. The US Bureau of Economic Analysis reports that the upturn in real GDP in the second quarter primarily reflected a downturn in imports and an acceleration in consumer spending that were partly offset by a downturn in investment. Today’s revision is due to the BEA lifting its estimate for investment and consumer spending in the last quarter, though this was partly offset by a downward revision to government spending and an upward revision to imports. Back in the UK car industry, Lotus has said it plans to cut 550 jobs in Britain. The job cuts will affect almost half the 1,300 staff at the company’s UK headquarters in Hethel, Norfolk. Lotus put some of the blame on Donald Trump’s trade war, saying: “We believe this is necessary in order to secure a sustainable future for the company in today’s rapidly evolving automotive environment, which is seeing uncertainty with rapid changes in global policies including tariffs. “The brand remains fully committed to the UK, and Norfolk will remain the home of the Lotus’ sports car, motorsports and engineering consulting operations. “It is actively exploring future growth opportunities to diversify Lotus Cars’ business model, including through third-party manufacturing.” Back in June, there were reports that Lotus was planning to end production of its sportscars in the UK. But after holding meetings with the government, Chinese owner Geely insisted it had no intention of shutting its Norfolk factory Eleven people, including former directors of Entain, the gambling company that owns Ladbrokes and Coral, have been charged with offences including bribery, fraud, cheating the public revenue, tax evasion and perverting the course of justice. The Crown Prosecution Service said this morning that it had authorised the prosecution of 11 individuals for seven offences, in relation to the provision of gambling services in Turkey between 2011 and 2018. Those charged include Kenny Alexander, the former chief executive of Entain, its former chairman, Lee Feldman, former legal director Robert Hoskin, and James Humberstone, who held several roles with the company. Ten of the individuals were charged with offences allegedly committed between 2011 and 2018, while one person was charged for an offence relating to the investigation by HMRC. Richard Las, director of HMRC’s Fraud Investigation Service, said: “This has been a complex and international investigation. These are serious charges that relate to conspiracy to defraud, bribery, cheating the public revenue, evasion of income tax and perverting the course of justice among others. “We remind everyone that proceedings are now active and we won’t be adding anything further.” These are difficult times at the Treasury, as speculation swirls that the UK could be in a race with France to agree an IMF bailout. But there is something for Number 11 to celebrate, though. Neil Amin-Smith, special advisor to chancellor Rachel Reeves, has topped a list of the 100 sexiest Londoners. Before becoming a top SPAD, Amin-Smith (Westminster School, Cambridge) was known for his role in music group Clean Bandit. This isn’t really our area, so we’ll defer to the Evening Standard, which reports: Spotted tie-less by the Chancellor’s side, he turns Treasury heads like hungry owls. With broad shoulders, tousled chocolate hair, statement earrings, and a smile that could melt decades of geopolitical tension, it’s no wonder Reeves keeps Amin-Smith close (how she manages to cry at work with him on her team is unbeknownst to us). The full list is here. It’s light on other names from the the world of business and finance, apart from banker Frederick Windsor and Phillips principal auctioneer Henry Highley. The financial markets aren’t convinced that the Bank of England will be able to cut interest rate again this year. After five quarter-point cuts since last summer, the Bank may struggle to agree a sixth until 2026. Shane O’Neill, head of interest rates at Validus Risk Management, explains: Knife-edge cut to 4.0% [earlier this month]: The MPC trimmed Bank Rate from 4.25% by a razor-thin 5–4 vote after an initial 4–4–1 split and re-vote. Markets price roughly 50/50 odds of another cut this year and ~1.5 cuts by mid-2026. • Growth flattered by the state: GDP rose 1.2% y/y vs 1.1% expected, but gains were driven by government spending; private consumption was flat and investment slipped after Q1 front-loading. • Cracks in jobs: Since the last Budget, the economy has shed 165k jobs; unemployment is 4.7%—the highest since 2016 outside Covid. The latest print showed a smaller-than-feared 8k decline vs 20k expected. As this clip shows, Liz Truss fears the UK is further down the “negative spiral” created by slow growth and the shortfall between tax revenues and spending: Liz Truss also told Bloomberg that she is even more convinced that the UK is at risk of a 1970s-style economic crisis than a year ago, when she warned of the risk of a bailout. Today, though, the bond market is calm. UK government borrowing costs are unchanged today, with the yield (or interest rate) on 30-year British debt pretty-much flat at 5.594%. Earlier this week it hit 5.63%, close to the 27-year high (5.663%) reached in April. Professor Costas Milas, of the Management School at the University of Liverpool, is very troubled by Liz truss’s comments about central banks and the conduct of monetary policy. Prof Milas tells us: Clearly, Trump wants to take full control of US monetary policy and is not shy of saying so. Is it the case of Liz Truss advocating a similar scenario for the UK? More worryingly, Liz Truss needs to explain how to go about that. In the US, Trump is forcing Fed Governor Lisa Cook out of the Fed with a series of unproved (so far) accusations, at the same time while giving a “signal” that he will follow similar tactics with the remaining Fed Governors. Is former PM Liz Truss advocating a similar strategy to be pursued by Sir Keir Starmer, or something else in order to bring monetary policy back in the hands of the UK government? Keir Starmer enjoyed a boost from the rural community during the 2024 general election after he and environment secretary Steve Reed went on tour of the farming conferences and other countryside events to assure those in attendance that they understood their struggles. But now, that support has evaporated, according to farmers polled by the Country Land and Business Association (CLA). This is due to fury over the inheritance tax on agricultural assets brought in at last year’s budget, which is projected to put some farms out of business when they are passed on. A survey of 490 farmers and landowners by the rural business group puts Reform UK (36%) just behind the Conservatives (38%) in farmer support, with Labour attracting 0%. “The Treasury says these reforms will barely touch rural Britain,” CLA president Victoria Vyvyan said, adding: “Our polling shows they will force hard choices on farms that have sustained communities for generations – selling land, laying off workers, shelving future plans. “Rural Labour MPs can see what’s coming. They know it will drain the life from the countryside and strip away the trust of the people who sent them to Westminster. “If they support it, their voters won’t forget.” Supporters of central bank independence argue that it has played an important role in recent decades in subduing inflation, and persuading investors that governments wouldn’t inflate their debts away. Finland’s central bank chief Olli Rehn (who we heard from earlier) has made this point this morning. Rehn told a panel discussion on democracy held in Turku, Finland: “If the central bank’s independence were truly to crumble, and the U.S. Federal Reserve began making decisions on grounds other than sound monetary policy principles — for example, because the president demands lower interest rates — the inevitable consequence would be inflation picking up.” Liz Truss’s comments show how Trump’s efforts to roll back the decades-old consensus on the value of independent monetary policy has “an eager audience in some of the world’s largest economies”, point out Bloomberg. They add: In the UK, officials for the populist Reform UK, which has led public opinion polls for months, have suggested they might be willing to rein in some of the BOE’s powers. And Reform’s leader, Nigel Farage — a long-time Trump supporter — has privately discussed the possibility of taking back independence from the central bank, Bloomberg reported in June, citing people familiar with the discussions. With UK food inflation now hitting 4.2%, we would like to hear from people on how they feel about food inflation and if it’s affected their shopping habits…. Former UK prime minister Liz Truss is backing Donald Trump in his fight with the Federal Reserve. Truss has told Bloomberg’s Odd Lots podcast that it is wrong that unelected central bankers can undermine (as she sees it) elected politicians. Truss, who was briefly prime minister in September and October 2022, said: “I think the Bank of England needs to be accountable to politicians. I think the current system doesn’t work. This is why I’m very sympathetic to what Donald Trump is saying about the Fed.” In the interview, Truss explains that people who owned assets and capital had done very well from the easy money created by the Bank of England (BoE) since the financial crisis, while that loose policy also made it hard for young people to buy homes. Given the importance of monetary policy of setting the allocation of assets within society, she argues that it’s wrong that people who make those decisions aren’t accountable to the electorate. She says: “It’s also very difficult, as I found as prime minister, to combine fiscal and monetary policy if you don’t hold one of the levers. So, I think it’s got to change. I think there is a reckoning coming for the central banks, not just in Britain but also in the United States, also the ECB. The current system does not work. Truss, who lost power after her mini-budget spooked the financial markets, crashing the pound and driving up borrowing costs, also claimed the BoE had “sabotaged” what she tried to do because she had been a critic of central banks, and wanted the Treasury to have a larger role setting the Bank’s mandate. “They didn’t like their power being challenged.” Truss has previously blamed the Bank of England for failing to anticipate the market consequences of her budget. Governor Andrew Bailey has rejected that criticism, pointing out that the Bank used its intervention tools to stabilise the bond market and protect pension funds. In her Bloomberg interview, Truss argues that democratically elected leaders shouldn’t “cowtow”, criticises the “failing economic orthodoxy” and warns that Britain is heading for a “very, very serious crisis.” Truss, who lost her parliamentary seat in last year’s general election, says the UK now faces an “economic doom loop of higher taxes, lower growth, higher debt, and it’s very difficult now to see the political way out of that.” Finland’s central bank chief has warned that President Donald Trump’s attacks on the US. Federal Reserve have a significant impact on the financial markets and the world economy. Olli Rehn warned in a speech this morning that the Fed’s independence has remained an inviolable principle since the 1980s, but was now under attack, Reuters reports. Rehn explained: “Now, however, this principle is wobbling badly. This could have substantial, global knock-on effects on both the financial markets and the real economy.” Rehn’s comments follow Donald Trump’s attempt to fire Federal Reserve governor Lisa Cook over unconfirmed allegations of mortgage fraud; Cook is refusing to step down, and pledging to sue the Trump administration. Trump has also repeatedly criticised the Fed, and its chair Jerome Powell, for not cutting US interest rates. The FCA’s investigation into Drax comes five months after the company’s former top lobbyist accused it of “misleading the public, government and its regulator” over its sourcing of wood for biomass pellets. In a claim for unfair dismissal, Rowaa Ahmar, Drax’s former head of public affairs, said evidence suggested Drax was “unable to prove that it only sourced sustainable wood for its biomass, and that it was in fact using unsustainable wood”. More here. An accounting probe at WH Smith has delayed its former finance chief from joining high street baker Greggs. Greggs has told the City that Robert Moorhead has asked to defer his appointment until Deloitte has conducted its review into a profit overstatement which rocked WH Smith’s share price last week. WH Smith startled investors on 21 August by slashing its full-year profit forecasts and reveaing it had discovered an overstatement in profits at its US arm. The problem is due to the “accelerated recognition of supplier income” in the US – the practice where retailers receive money from their suppliers for, for example, promoting certain products or hitting certain sales targets. Under accounting rules, such income can only be recorded in the financial year it is received. Economic growth in Switzerland has slowed, as the country braces for a bruising hit from Donald Trump’s trade wars. Switzerland’s GDP adjusted for sporting events increased by just 0.1% in the second quarter of this year, down on the 0.7% gorwth recorded in January-March. Switzerland’s State Secretariat for Economic Affairs (SECO) warned that new tariffs on sales to the US will hurt growth, saying: After the above-average growth seen in the previous quarter, the anticipated correction has now occurred. Industrial value added and exports declined sharply, whereas the services sector delivered broadbased growth. An updated economic scenario from SECO shows that, as a result of higher US import tariffs, the Swiss economy is likely to grow more slowly than previously expected, particularly in 2026. Trump has set a 39% tariff on Swiss exports to the US, leaving the country scrambling to agree a better trade deal. Shares in power generator Drax have tumbled by 10% after it revealed this morning it is being investigated by the City watchdog. Traders drove Drax’s share price down to 630p in early London trading, down from 703.5p last night, following the news that the FCA is probing whether its recent annual reports comply with UK Listing Rules. As covered earlier (see 7.18am post for more details), the investigation appears to centre on Drax’s statements regarding the sourcing of the biomass it uses in its wood-burning power station. Over in Manila, the Philippines central bank has cut interest rates despite trade war concerns. The Bangko Sentral ng Pilipinas lowered its overnight target reverse repurchase rate by 25 basis points (a quarter of one percentage point) to 5% today, in line with expectations. It cut borrowing costs after concluding that inflation expectations remain well-anchored, with inflation forecast to average 1.7% this year. But, it added: Meanwhile, possible electricity rate adjustments and higher rice tariffs could raise inflationary pressures over the policy horizon. The Monetary Board observed that domestic demand has held firm. However, the impact of US policies on global trade and investment continue to weigh on global economic activity. This could temper the outlook for the Philippine economy. Back in the car sector, Ford has today become the first manufacturer to be awarded the UK’s full electric car grant of £3,750, cutting the cost paid by consumers. Two Ford models, the Puma Gen-E and e-Tourneo Courier, now qualify for the grant, the Department for Transport has announced. They are the first to benefit from the full £3,750 subsidy. Another 26 models now get the smaller grant, which knocks £1,500 off their price. The scheme is meant to make it cheaper and easier to own an electric car. Transport Secretary Heidi Alexander said: We’re putting money back in people’s pockets and making it easier and cheaper for families to make the switch to electric, by delivering discounts of up to £3,750 on EVs. Our measures are driving competition in the UK EV market, boosting economic growth and supporting jobs and skills as part of our Plan for Change. Newsflash: UK energy producer Drax is being investigated by the Financial Conduct Authority (FCA). Drax has told the City that it learned on Tuesday that the City watchdog had begun an investigation into “historical statements regarding Drax’s biomass sourcing and the compliance of Drax’s 2021, 2022 and 2023 Annual Reports with the Listing Rules and Disclosure Guidance and Transparency Rules.” Drax, which operates a wood-burning power station in North Yorkshire, added that it will cooperate with the FCA’s investigation. The FCA has confirmed that it has opened an investigation, without giving more information. The company has faced pressure to disclose full details of its tree consumption; last year it agreed to pay £25m for submitting inaccurate data on the sourcing of wood pellets. Elsewhere in the auto industry this morning, new data shows that Britain’s car production grew for the second month in a row in July. Car production rose 5.6% in July from last year to 69,127 units, the Society of Motor Manufacturers and Traders (SMMT) reported. However, total vehicle production dropped by 10.8% at 72,006 units, due to a fall in commercial vehicle manufacturing. The European Automobile Manufacturers’ Association are also concerned that European take-up of electric cars is not rising faster. Sigrid de Vries, director general of ACEA, says: “Battery-electric vehicles still account for just 15.6% of the EU car market. Not only is this well below the level where it needs to be at this point in the transition the share in unevenly distributed across member states. To accelerate uptake, Europe must continue to expand public recharging infrastructure, secure lower recharging prices, and ensure well-coordinated purchase incentives schemes. The market data demonstrates why a technology-neutral approach must drive this transition. EVs will lead the charge, but there must also be space for (plug-in) hybrids, range extenders, highly efficient internal combustion-engine (ICE) vehicles, hydrogen and decarbonised fuels.” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Tesla’s European sales slump has continued, as it faces rising competition in the battery-powered electric car market. New sales figures released by the European Automobile Manufacturers Association (ACEA) this morning show that Tesla shipments tumbled 40% last month. The company sold 8,837 vehicles across the European Union, the EFTA trade block and the UK in July, down from 14,769 in July 2024. The sales slump, which began at the start of this year, continued despite the recent revamp of Tesla’s signature Model Y, indicating that the backlash against CEO Elon Musk’s political views could still be hurting the company. Musk’s recent break-up with Donald Trump hasn’t, yet, revived the company’s fortunes. July’s 40% sales fall was worse than the total for 2025 to date, which are down 33% for the January-July period. Tesla also faces rising competition, particularly from Chinese manufacturers. BYD, the Shenzhen-headquartered carmaker, more than tripled its sales year-on-year in July, up from 4,151 a year earlier to 13,503 last month, a rise of 225%. This gave BYD a 1.2% market share, higher than Tesla’s 0.8%. BYD, which overtook Tesla for European sales back in April, recently launched its Dolphin Surf EV car, which is priced from £18,650 in the UK. ACEA also reports that in the first seven months of 2025, 1,011,903 new battery-electric cars were registered, accounting for 15.6% of the EU market share. Hybrid-electric car registrations proved more popular, though, with 2,255,080 units sold across the EU so far this year. This was driven by growth in the four biggest markets: France (+30.5%), Spain (+30.2%), Germany (+10.7%), and Italy (+9.4%). Hybrid-electric models now account for almost 35% of the total EU market. Overall, new car sales in Europe rose 5.9% in July, to 1.085 million. The agenda 10am BST: Eurozone confidence data 1.30pm BST: US Q2 GDP (second estimate) 1.30pm BST: US weekly jobless claims</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>UK retailer stocks sold off today after a downbeat note from analysts at Deutsche Bank. Associated British Foods, which owns Primark, fell by as much as 5% today. Deutsche also downgraded its view on home improvement retailer Wickes to a ‘sell’</t>
+          <t>US economic growth was faster than expected in April-June. The economy grew at an annual rate of 3.3% in the second quarter. Tesla is still paying the price for Elon Musk’s brush with politics.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Economic and Market Volatility</t>
+          <t>Trade War Impacts Markets</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Time to wrap up… Donald Trump will announce tariffs on imports of semiconductors and steel in the coming weeks, he told reporters aboard Air Force One while travelling to Alaska for his meeting with Vladimir Putin. The US president said: I’ll be setting tariffs next week and the week after on steel and on, I would say, chips…I’m going to have a rate that is going to be lower at the beginning - that gives them a chance to come in and build - and very high after a certain period of time. Shares in Intel jumped by as much as 8.9% in early trading on Friday, also boosted by a report that the Trump administration is considering taking a stake in the chipmaker. Meanwhile in the UK, the FTSE 100 briefly surpassed its intraday high this morning, although it is now trading down 0.3% at 9,150.90 points. The owner of Kingsmill also agreed to buy its rival bakery business Hovis today, in a deal that could make the biggest bread brand in the country if it gets the green light from regulators. Elsewhere Shein, the online fast-fashion retailer founded in China, increased sales in the UK by about a third to more than £2bn last year, overtaking the British rival Boohoo and closing in on Asos. It is a slow open for Wall Street, with the blue chip S&amp;amp;P 500 index slipping by 0.1% in early trading. It hit an all-time high earlier this week. The Dow Jones Industrial Average, another key US stock index, also hit an all-time intraday high, briefly surpassing its previous peak of 45,073.63 points. It was helped by a big jump in UnitedHealth Group shares, which are up by more than 9%, after it emerged that Warren Buffett’s Berkshire Hathaway has invested in the insurer. The Dow is now at 45,076.20 points. Donald Trump will announce tariffs on imports of semiconductors and steel in the coming weeks, he told reporters aboard Air Force One while travelling to Alaska for his meeting with Vladimir Putin. The US president said: I’ll be setting tariffs next week and the week after on steel and on, I would say, chips…I’m going to have a rate that is going to be lower at the beginning - that gives them a chance to come in and build - and very high after a certain period of time. Last week the president threatened a 100% tariff on imported semiconductors and chips, which could favour US-based companies such as Intel. Shares in Intel jumped by as much as 8.9% in early trading on Friday, also boosted by a report that the Trump administration is considering taking a stake in the chipmaker. US retail sales rose in July, up 0.5%, slowing from a 0.9% gain in June, official data shows. Retail spending was helped by strong demand for cars, as well as promotional campaigns from Walmart and Amazon’s extended Prime Day. Excluding cars, sales in the period were up by just 0.3%, according to the US Commerce Department’s Census Bureau. Traders are starting to trim back their bets that the US central bank, the Federal Reserve, will cut interest rates next month. The probability of a quarter-point reduction has fallen from 94% to about 89%, per Reuters. It is the biggest reunion in British music in decades, with fans expected to splash out more than £1bn on the Oasis comeback. But for economists it presents a difficult question: how do you factor the Gallagher brothers into the UK’s inflation figures? The Office for National Statistics will not be including Oasis ticket prices in their basket of goods for inflation, according to Morgan Stanley, as it “excludes big-name bands with highly distinctive and unique abilities to charge diverse prices.” But fans flocking to hotels and driving up prices could have a big impact on the inflation reading for July, analysts believe. Analysts at Deutsche Bank expect the headline consumer price index rate rate for July will be 3.8% year on year, while Morgan Stanley has forecast a rate of 3.7%. It is not the first time that superstar tours have moved the dial on crucial economic data. In June 2023, economists blamed Beyoncé’s concert in Stockholm for unexpectedly high Swedish inflation. The ONS is scheduled to report the inflation figure for July on Wednesday 20 August. The FTSE 100 has pulled back from its intraday high, and is up now by just 0.1% to 9,186.59. The FTSE 250 mid-cap index is performing better, up 0.4%. Its best performer is Bytes Technology Group, which announced a £25m share buyback programme this morning. Shares in the IT reseller are up 7%. Shein, the online fast-fashion retailer founded in China, increased sales in the UK by almost a third to more than £2bn last year, overtaking the British rival Boohoo and closing in on Asos. The company, which had been considering a £50bn float on the London Stock Exchange but is now expected to list in Hong Kong, said profits rose 56% to £38.2m last year on which it paid £9.6m corporation tax, according to accounts filed at Companies House this week. Shein, which mainly sells fashion but has also moved into other products including toys and beauty, said it had benefited from the opening of two new offices in King’s Cross and Manchester, the launch of a pop-up shop in Liverpool and a Christmas bus tour across 12 cities in the UK. Oil prices are edging lower this morning ahead of a meeting between US President Donald Trump and Russian leader Vladimir Putin later today in Alaska. Brent crude futures fell by as much as 0.8% to $66.34 a barrel this morning, while US West Texas Intermediate crude futures fell by as much as 0.9% to $63.39. Giovanni Staunovo, commodity analyst at UBS, told Reuters: The market is watching out for whether there is a ceasefire or not. An expectation of a ceasefire translates into more Russian production…The question is will there be escalation or de-escalation?” A potential deal could significantly lower geopolitical risk in the oil market. Analysts at the investment bank Citigroup said this month that a deal to end the war in Ukraine could push Brent crude to the low $60s range by the end of the year. Recent weak economic data from China has also hurt the outlook for fuel demand. Shares in Intel have jumped 7.4% after it was reported that the Trump administration is considering taking a stake in the struggling US chipmaker. The potential investment, which would be paid for by the US government, would be used to develop Intel’s factory hub in Ohio, according to Bloomberg. It would also help shore up the chipmaker’s finances at a time when Intel has been slashing jobs as part of a wider cost-cutting drive. Talks over the potential investment stem from a meeting that took place between Donald Trump, and the Intel chief executive, Lip-Bu Tan, this week, days after Trump called for Tan to resign, accusing him of having ties to the Chinese Communist party. Bloomberg suggested Tan was likely to stay in charge of the chipmaker. Elsewhere in Europe, estimates suggest that economic growth in Switzerland slowed sharply in the second quarter. Switzerland has estimated that its economy grew by just 0.1% quarter-on-quarter in the three months ended in June, down from 0.8% in the prior period. It comes as Trump hits Switzerland with one of the highest tariff rates in the world, at 39%. Melanie Debono, a senior economist at Pantheon Macroeconomics, said “luck is running out for the Swiss economy”. We think the Swiss economy will enter a short, shallow recession in H2 as the rise in US trade tariffs (to a whopping 39% for most goods) hits exports, while trade uncertainty more widely hurts investment. We currently expect GDP to fall by 0.3% quarter-to-quarter in both Q3 and Q4. Barring any revisions, this would mean that GDP in Switzerland will have risen by 1.3% this year, a touch more than the 1.0% recorded in 2024. Swiss companies, whose exports to the US account for about one-sixth of their total foreign sales, face one of the steepest US tariffs in the world – only Laos, Myanmar and Syria had higher figures, at 40-41%. The blue chip FTSE 100 index has hit another record this morning, rising by as much as 0.4% to 9,222.07, its highest point since the end of July. It has pared back some of these gains, now up by around 0.1% 9,188.67, although it is still trading ahead of the high it set at the close yesterday of 9,177.24. Axel Rudolph, senior technical analyst at the broker IG, says: The FTSE 100 has joined the global push to fresh record highs, buoyed by improved risk appetite, supportive global trends and strong corporate earnings. With investors drawing confidence from a friendlier interest rate outlook and resilient corporate earnings, the UK benchmark has finally broken through its previous ceiling. With a stellar over 11% rise since the start of the year, it is outperforming peers such as the S&amp;amp;P 500 and Nikkei 225. The move underlines how global market momentum can lift all boats, even in the face of lingering domestic economic concerns.” London’s listed miners are leading the charge this morning, with Antofagasta, Glencore and Anglo American the top three risers across the index, up by 3.4%, 2.7% and 2.7% respectively. Meanwhile the Stoxx Europe 600 index rose by 0.3%, led by the Danish cable group NKT, whose shares are up by around 8% this morning. The Danish jewellery business Pandora is the worst performer, with its shares slumping 13% after it missed earning expectations for its second quarter. The owner of Kingsmill has agreed to buy its rival bakery business Hovis, in a deal that could make the biggest bread brand in the country if it gets the green light from regulators. Associated British Foods, a FTSE 100 company which also owns the retailer Primark, has agreed to buy Hovis from the private equity firm Endless. The deal between the second and third biggest bread brands in the country is expected to draw attention from the Competition and Markets Authority. Both companies have struggled recently against Warburtons, the biggest brand in the sector. Revenue at Hovis dropped almost 9% to £447m in the year to 28 September 2024, with pre-tax losses widening to £4.7m, compared with a loss of £3.6m the year prior. That included £530,000 in one-off costs, largely related to restructuring. ABF’s bakery division, Allied Bakeries (which includes Kingsmill, Allinson’s and Sunblest) made an annual loss about £30m despite sales of about £400m last year, according to analysts at the broker Panmure Liberum. ABF said the deal will combine the production and distribution activities of Allied Bakeries and Hovis, which would create cost savings and efficiencies, so it would turn into a “profitable UK bread business that is sustainable over the long term”. George Weston, ABF’s chief executive, said: This transaction will create a UK bakeries business that is both profitable and sustainable over the long term. Supporting the Hovis and Kingsmill brands with well-invested and efficient operations will also enable innovation and growth. This solution will create value for shareholders, provide greater choice for consumers and increase efficiencies for customers. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. New data suggest the Chinese economy slowed in July, as Donald Trump’s trade war began to bite at the second biggest economy in the world. Figures coming out of Beijing last night showed that Chinese industrial production rose at the slowest rate since November and expanded by 5.7% compared with the same point last year, worse than an expected 6%. Meanwhile Chinese retail sales grew by 3.7% year-on-year in July, its slowest pace so far this year and down from 4.8% the previous month. Yuhan Zhang, principal economist at The Conference Board’s China Center, said: Firms may be running on existing capacity rather than building new plants…The July industrial value-add breakdown tells a more nuanced story than the weak fixed asset investment headline. He pointed to China’s automobile manufacturing, railway, shipbuilding, aerospace and other transport equipment industries as “outliers (that) indicate policy-driven, high-tech and strategic sectors are still attracting substantial capital.” The Chinese CSI 300 stock index rose 0.8% after the release of the economic data, as it fed speculation that Beijing could introduce fresh stimulus in the market. Meanwhile in the UK, the FTSE 100 blue chip share index is set to end the week at a new record high. It is poised to rise by 0.5% when the market opens at 8:00AM, led by gains in the finance and defence sectors. The defence sector has been one of the best performers in London’s stock market, thanks to a wave of rearmament across much of Europe in the wake of the war in Ukraine. All eyes will be on Alaska later today, when Vladimir Putin is set to meet Donald Trump. The US president has said he believes the Russian leader is ready to make a deal on the Ukraine war. The agenda 8.00pm BST: Donald Trump and Vladimir Putin meet in Alaska</t>
+          <t>Time to wrap up… The energy regulator for Britain, Ofgem, has said it will increase the cap on energy bills from October by 2%, the equivalent of a £35 rise in annual bills for the average home, despite a 2% fall in the wholesale price in the energy markets over the last three months. Prices for households will go up just as the colder weather sets in because money is needed to cover the rising cost of the government’s energy policies. About £15 of the £35 increase will fund an expansion of the warm home discount scheme to provide an extra 2.7 million households with a £150 reduction in their bills. Thames Water has agreed a payment plan for £123m sewage and dividend fines, as it races to secure funding to avoid temporary government nationalisation. Earlier this month the government approved the appointment of insolvency advisers to consult on plans for Thames Water to be placed into a special administration regime (SAR). The debt-laden utility firm was hit with a record £104m fine by Ofwat in May over environmental breaches involving sewage spills, after failing to operate and manage its treatment works and wastewater networks effectively. At the same time, a further £18.2m fine was levied on Thames for breaking dividend rules, the first penalty of its kind in the water industry. The penalties were originally due to be paid by 20 August but the regulator gave the company some breathing space to pay the fines. Ofwat has now approved Thames’s request for a payment plan, which will result in it paying £24.5m, or 20% of the penalties, by the end of September, with the rest to be paid later. Lego builds record sales of £4bn as parents steer children away from smartphones. The Danish toy company said sales increased by 12% to a record 34.6bn Danish kroner (£4bn) in the first half of the year, rising well ahead of the recovering global toy market in which sales rose 7%. Niels B. Christiansen, chief executive, said Lego could be profiting from parents’ desire to keep children away from phones because of the effect of social media on mental health. Over in the US, the highlight of the day will be when the chip designer Nvidia reports its quarterly earnings after the market close, or around 9pm BST. Wall Street has opened flat today, with the S&amp;amp;P 500 share index down by 0.06% at the open. The Nasdaq index is also down slightly by 0.08%. All eyes will be on chip designer Nvidia today when it reports after the US market closes. Victoria Scholar, of the investment broker Interactive Investor, says: Nvidia gets set to release its second quarter results after the bell as the final US tech giant to report this season. There’s a lot of focus on this earnings report given that it comes off the back of a shaky period for tech stocks. The AI darlings like Nvidia, Palantir and Meta have suffered some selling pressure as investors start to question whether the winning streak is running out of steam. Sam Altman, CEO of OpenAI suggested a bubble could be forming in AI stocks and a report from MIT said 95% of organisations are getting zero return on generative AI investments. However this comes after a strong bull run off the April lows for Nvidia which rebounded to become the first public company to achieve a market cap of $4 trillion in July. …According to Refinitiv, Nvidia is expected to report Q2 earnings per share of $1 on revenues of $46 billion, up from 96 cents and $44.06 billion respectively in the previous quarter. There will be a lot riding on guidance for the rest of the year with investors looking for reassurances that Nvidia can continue to deliver growth. China will be another focal point following the resumption of its AI chip sales there after Nvidia agreed to pay the US government 15% of Chinese revenues. Last quarter, Nvidia said it lost out on $2.5 billion because of China export restrictions. Investors will also be paying close attention to its Blackwell business which made up 70% of Nvidia’s data centre sales last quarter. Elsewhere this afternoon, the London-listed warehouse owner Warehouse Reit confirmed that it has ended takeover talks with its rival Tritax Big Box Reit, clearing the way for a takeover by the commercial property investor Blackstone. Blackstone’s latest offer for the company amounts to 115p cash per share, valuing the business at about £489m. Here’s what markets are doing as we go into lunchtime… The FTSE 100 is flat as a pancake today – NatWest is the worst performer, with its shares down 2.4%. The best performer so far is JD Sports, though its shares are only up 1.7%. That is despite the fact that it reported a fall in sales in its second quarter, though investors appear to have taken confidence in the fact that performance in its North American market has improved slightly. The fashion retailer also announced another £100m share buyback. The mid-cap FTSE 250 index is down by 0.3%. The miner Hochschild is the worst performer, with its shares tumbling by roughly 14% today after it cut its production forecasts for the year. The stock market is pretty muted across Europe today, with the Stoxx 600 up slightly by 0.15%. Meanwhile the US dollar index, which tracks the greenback against a basket of other major currencies, is up 0.45%. The pound is now down 0.42% against the dollar to $1.34. The big market news is not landing until later this evening: Nvidia will report its quarterly earnings after the US markets close, after 9pm BST. The chip designer crossed the $4 trillion market capitalisation mark in July, becoming the biggest company in the world. Nvidia shares are up by 0.6% in pre-market trading. For now, futures for both the S&amp;amp;P 500 index and the Nasdaq are up just 0.03%. More bad news from the retail sector this morning: sales volumes fell in August, marking 11 consecutive months of decline, according to a survey by the Confederation of British Industry (CBI). The CBI’s monthly gauge of how retail sales compared with a year earlier stood at -32 this month, a slight improvement of -34 in July. Martin Sartorius, principal economist at the CBI, said: Retailers endured another tough month in August, with annual sales volumes falling for the eleventh consecutive month. Weak demand and higher labour costs continue to put pressure on margins, dampening sentiment across the retail and wider distribution sector. This downbeat outlook is reflected in firms’ plans to scale back investment and hiring. The government’s fiscal decisions are continuing to bite, and retailers’ struggles send a clear signal: business cannot be asked to balance the books again at the Autumn Budget. Building business confidence through delivery must be the priority — starting with a rethink of the Employment Rights Bill, which risks piling on unnecessary costs and holding back jobs and investment.” Fears that UK consumers will rein in spending sent jitters across the retail sector yesterday, wiping hundreds of millions of pounds off the value of some of the biggest retailers in the country, including the owners of Primark and B&amp;amp;Q, and the home improvement chain Wickes. The UK government has just sold £5bn worth in three-year bonds in a scheduled action. Demand was good, with the auction covered 3.16 times. The bonds were sold with a yield of 4.375%, due in 2028. The gilt market has been rocky lately, with yield on the 30-year bond trading close to its highest level since 1998 yesterday, at 5.62%. Yields rise when prices fall. The yield on the 30-year rose to as high as 5.627% in early trading this morning, but it has since recovered, with the yield now at 5.583%. Mohit Kumar, an analyst at the investment broker Jefferies, paints a gloomy picture of the UK’s economic outlook: We have held a negative view on the UK fiscal picture and maintain the view. We see UK growth disappointing relative to official forecasts which would leave the Chancellor with a bigger budget hole than current official forecast suggests. Tax rises look inevitable in the Autumn statement. However, we are approaching levels where further tax rises start becoming counterproductive. Producer output price inflation rose to 1.9% in the year to June, up from a revised rise of 0.7% in the year to April 2025, according to the Office for National Statistics. The ONS suspended the publication of its producer price indices in March, after it found calculation errors dating back to 2020. The figures published today represent interim data before it resumes regular publication in October. The statistics agency said in July that producer price inflation in previous years had been higher than originally calculated. It comes as pressure grows on the ONS over the reliability of its data. Staff at the Treasury and its independent spending watchdog have said they are struggling to get a clear picture of the economy because of problems at the ONS with producing reliable numbers. Shares in utility stocks are rising this morning after the energy regulator Ofgem announced that it will increase its price cap on bills by 2% from October. National Grid, SSE and Severn Trent are all up roughly 1% this morning, among the best performers in the UK’s blue chip FTSE 100 index. But overall the FTSE is not moving much, up very slightly by 0.03%. Over in Europe, the Stoxx 600 index is up 0.4%. The French Cac 40 share index recovered 0.4%, after a fall earlier in the week over concerns around the potential collapse of Prime Minister François Bayrou’s government. Turning back to energy bills, several UK charities are warning that the 2% rise in the energy price cap (which covers England, Wales and Scotland) will hurt vulnerable people. Official figures showed in May that energy bill defaults hit a record high, with 2.7% of direct debits for gas and electricity failing due to lack of funds. Disability equality charity Scope has said millions of disabled people are being pushed into deeper fuel poverty as prices continue to rise. Abdi Mohamed, head of policy at the charity, said: Life costs more if you are disabled – on average an extra £1,095 a month. We hear from disabled people every day who tell us they are unable to power vital medical and mobility equipment, facing increasing pain and losing their independence. The current support available for disabled people barely scratches the surface. And many no longer get the warm home discount at all, despite enormous energy costs. The government must act with urgency to close the devastating gap in support and tackle this crisis. Joanna Elson, chief executive of the charity Independent Age, argued political intervention is urgently needed, and that the warm homes discount should be extended to at least 2027. She said: Far too often older people in financial hardship are bed bound by the cold, turning in early for the night dressed in hats and scarves in a desperate bid to keep warm through the winter months. …The situation is dire, in the UK over one million older households are living in fuel poverty. The people in later life we speak to are making drastic and dangerous cutbacks because they cannot afford their energy bills. They are routinely switching off heating systems for weeks on end, visiting public places to stay warm and cutting down on food so they can pay their energy bills. This is unacceptable. Jon Sparkes, chief executive of the learning disability charity Mencap, said: People with a learning disability simply must be protected from ever increasing energy costs, or they face being pushed into fuel poverty, unable to stay safe, warm and healthy. The 1.5 million people in the UK with a learning disability are more likely to have unavoidably high energy costs because they may need to charge specialist or medical equipment or heat their homes for longer. …With bill prices set to increase even further this autumn, people with a learning disability and their families will continue to face these dangerous choices which leave them feeling anxious and afraid. Lego has built a bigger share of the toy market as sales rose 12% in the first six months of the year after its Botanicals and Grand Prix-themed sets helped it attract adults as well as children. As sales increased to 34.6bn Danish Kroner (£4bn), the company, which is known for its colourful building bricks, said it would open a new $1.5bn US factory and distribution centre in 2027, its seventh factory worldwide. The company previously said it was not bringing forward the development of the factory despite new import tariffs introduced by the Trump administration this year. The group opened a new site in Vietnam earlier this year and expanded factories in Mexico and Hungary to meet demand. Lego’s net profit increased 10% to 6.5bn Danish Kroner as the company said it had signed deals to produce toys linked to the Bluey and Pokémon cartoon series and launched the She Built That campaign to encourage girls to use Lego creatively. Niels B Christiansen, the chief executive, said: We are very pleased to have maintained our strong performance in the first half of 2025, winning share in the global toy market. This growth is driven by our large and innovative range of products that continues to be relevant across ages and interests. Shares in Rio Tinto have ticked up 1% this morning after the miner’s new boss, Simon Trott, announced he will combine some of its biggest businesses in an effort to simplify the group, just two days after taking leadership of the company. Rio will reorganise into three divisions: iron ore, aluminium and lithium, and copper, the company said on Wednesday. Trott, who took over from Jakob Stausholm on 25 August, previously led Rio’s iron ore operations in northwest Australia, which make up more than half its earnings. The Anglo-Australian miner has recently been trying to diversify its business, acquiring the US lithium producer Arcadium Lithium in a $6.7 billion deal earlier this year. It has made Rio one of the biggest producers of the battery-making metal in the world, alongside Albemarle and SQM. Thames Water has agreed a payment plan with the water regulator for fines it owes worth £123m, as it races to secure funding to avoid temporary government nationalisation. The water company, which serves 16 million customers across London and the south-east, is currently racing to pull together a deal to avoid collapse. Earlier this month the government approved the appointment of insolvency advisers FTI Consulting to consult on plans for Thames Water to be placed into a special administration regime (SAR). The debt-laden utility firm was hit with a record £104m fine by Ofwat in May over environmental breaches involving sewage spills, after failing to operate and manage its treatment works and wastewater networks effectively. At the same time, a further £18.2m fine was levied on Thames for breaking dividend rules, the first penalty of its kind in the water industry. Ofwat said the company had paid out cash to investors despite having fallen short in its services to customers and its environmental record. The penalties were originally due to be paid by 20 August but the regulator has given the company some breathing space to pay the fines. Ofwat had previously told Thames the penalties had to be “paid by the company and its investors, and not by customers”. The regulator has approved Thames’ request for a payment plan, which will see it pay £24.5m, or 20% of the penalties, by the end of September, with the rest to be paid later. Lidl has invested £435m in warehouses in Leeds and London, developments it says will create more than 500 new jobs. The supermarket has completed its extension of its Belvedere warehouse site in London, which now has 800,000 sq ft, a 167% increase compared with when it opened in 2003. Last month Lidl also started construction at a 38-acre site in Gildersome, Leeds, with a new warehouse there expected to create 400 new jobs. The expansion at the site in London will create 120 new jobs, Lidl said. It comes after the Resolution Foundation, a think tank, predicted the unemployment rate could hit 5% in the three months ended in August, the highest level since the start of 2021. The official unemployment rate was 4.7% in the last quarter. Chancellor Rachel Reeves praised Lidl’s investment as “a strong vote of confidence in the UK economy”, though economists have warned that Britain faces serious challenges due to its weak underlying growth and a drop in the number of workers since the pandemic. Reeves said: Lidl’s commitment to new warehouse facilities in London and Leeds will unlock hundreds of new jobs, strengthen supply chains, and ensure families can access affordable, quality food. Through our Plan for Change we’re backing business and working in partnership to deliver growth and opportunity in communities across the country. Over on the corporate front in the UK, fashion retailer JD Sports has reported a 3% drop in like-for-like sales in the 13 weeks ended on 2 August. Chief executive Régis Schultz said the company was going up against tough comparators in Europe and the UK from the Euros football tournament last year, but “across our regions and fascias, in general we see a resilient consumer, albeit very selective on their purchases.” The retailer also said that it would launch another £100m share buyback. Elsewhere, miner Rio Tinto’s new chief executive Simon Trott has announced that he will combine some of its biggest businesses in an effort to simplify the group. Rio will reorganise into three divisions: iron ore, aluminium and lithium, and copper, the company said on Wednesday. Trott said: A simplified business structure, grounded in our fundamental commitment to safety and with sharper focus on the most compelling opportunities we have, will enable us to deliver new standards of operational excellence and value creation. While another rise in energy bills will be unwelcome news for many, analysts at the consultancy Cornwall Insight have said that prices could fall under the next cap, which would start in January 2026. Dr Craig Lowrey, of Cornwall Insight, said: There is better news on the horizon with bills currently expected to ease in January, driven by a forecast fall in wholesale prices. Normally, that drop would have meant even lower bills, however, rising policy costs, such as funding for new nuclear projects are keeping bills a little higher. These policy-driven costs are part of a broader shift in how we fund the energy transition. Nuclear will be one of the cornerstones of a more secure and sustainable energy system, yet some of the funding will ultimately need to come from billpayers. This is a difficult trade off - after all, everyone wants to see bills come down. However, the challenge we face is clear: if we want to build a resilient, low-carbon energy future, we must be prepared to invest in it today.” The energy regulator for Britain, Ofgem, has said it will increase the cap on energy bills from October by 2%, the equivalent of a £35 rise in annual bills for the average home. Here’s more details of the energy price cap just announced, from Ofgem. Electricity rates If you are on a standard variable tariff (default tariff) and pay for your electricity by Direct Debit, you will pay on average 26.35p pence per kilowatt hour (kWh). The daily standing charge is 53.68 pence per day. This is based on the average across England, Scotland and Wales and includes VAT. Gas rates If you are on a standard variable tariff (default tariff) and pay for your gas by Direct Debit, you will pay on average 6.29 pence per kilowatt hour (kWh). The daily standing charge is 34.03 pence per day. This is based on the average across England, Scotland and Wales and includes VAT. Why energy prices have gone up Volatile global wholesale prices for energy are partly behind the increase, as well as the cost of the government’s expansion of its warm home discount policy. Tim Jarvis, director general for Markets at Ofgem, says: While there is still more to do, we are seeing signs of a healthier market. There are more people on fixed tariffs saving themselves money, switching is rising as options for consumers increase, and we’ve seen increases in customer satisfaction, alongside a reduction in complaints. While today’s change is below inflation, we know customers might not be feeling it in their pockets. There are things you can do though – consider a fixed tariff as this could save more than £200 against the new cap. Paying by direct debit or smart pay as you go could also save you money. In the longer term, we will continue to see fluctuations in our energy prices until we are insulated from volatile international gas markets. That’s why we continue to work with government and the sector to diversify our energy mix to reduce the reliance on markets we do not control. Jarvis, speaking to Radio 4’s Today programme, also noted that the cost of running the network and the expansion of the government’s warm home discount scheme had also driven the rise in the cap. The rise in energy costs will hit people already struggling to pay their household bills, warns National Energy Action, the fuel poverty charity. Michael Penhaligon, of the NEA, says: Every day my colleagues and I speak to people in desperate circumstances. They can’t afford the very basics of heat and power. They are rationing their energy usage and they’re cutting back on food and other essentials. The individuals I speak to are left to rely on foodbanks, fuel vouchers and other charitable grants to help restore them to a basic standard of living. This shouldn’t be happening in the UK in 2025. Some may say that the cap rising around £35 won’t have an impact but the people I speak to already can’t afford their bills and many of them are deep in debt. This can have a huge impact on their mental and physical wellbeing. A rise in bills just as temperatures start to drop will put even more pressure on households. My colleagues and I achieve amazing outcomes for households to help them afford their energy; we get debt written off, we get them access to benefits they are entitled to, and we liaise with their suppliers on their behalf. But the scale and depth of fuel poverty is far beyond the remit of any charity. Newsflash: The energy price cap on bills across Great Britain will rise by 2% in October, regulator Ofgem has announced. This will lift the average annual cost of electricity and gas for a typical household to £1,755 per year. This is the fourth consecutive hike in the cap on gas and electricity charges, and is slightly higher than analysts had just expected. The cap limits the amount which a supplier can charge for a unit of electricity or gas. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. The cost of living could be about to get even tighter, as households find out whether their energy bills will rise again this autumn. Ofgem, the energy regulator, is due to announce the latest price cap on the cost of a unit of energy at 7am. Analysts expect the cap to rise due to recent increases in wholesale gas and electricity prices. Consultancy Cornwall Insight have predicted Ofgem will increase the cap by about 1% to £1,737 a year for a dual-fuel household, from the current level of £1,720. A rise in energy prices would act as yet another driver for high inflation. Official figures showed last week that UK inflation rose in July to a higher-than-expected 3.8% amid higher food prices and travel costs. It marked the 10th consecutive month that inflation has sat above the Bank of England’s 2% target. The new cap will come into effect in October and remain in place until the end of the year. The energy price cap sets the maximum that a supplier can charge for a unit of energy (there’s no cap on how high a bill can go). Elsewhere, overnight Donald Trump has imposed 50% tariffs on most US imports from India, following through on his threat to punish one of the world’s largest economies over its purchases of discounted Russian oil. The tariffs, which came into effect just after midnight on Wednesday in Washington, risk inflicting significant damage on the Indian economy and further disrupting global supply chains. US tariffs of 25% on Indian goods went into force earlier this month, but Trump announced plans to double the rate, citing India’s purchases of Russian oil, which the White House has argued is indirectly funding Russia’s war against Ukraine. The agenda 7:00AM BST: Energy regulator Ofgem announces UK energy price cap for October-December 10:00AM BST: UK 2028 gilt auction After 9:00PM BST: Nvidia quarterly earnings report</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Shares in Intel jumped by as much as 8.9% in early trading on Friday. FTSE 100 briefly surpassed its intraday high this morning, although it is now trading down 0.3% at 9,150.90 points. It is a slow open for Wall Street, with the blue chip S&amp;amp;P 500 index slipping by 0.1%.</t>
+          <t>Ofgem has said it will increase the cap on energy bills from October by 2%. This is the equivalent of a £35 rise in annual bills for the average home. Prices will go up just as the colder weather sets in because money is needed to cover the rising cost of the government's energy policies.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Economic and Market Volatility</t>
+          <t>UK Economic Challenges Overview</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Time to wrap up… River Island’s rescue restructure has received approval from a high court judge, a move which will help stop the fashion retailer from falling into administration. The plan received approval from a high court judge on Friday after the majority of creditors gave their backing to the plan earlier this week. The bidding battle for NHS landlord Assura also intensified today. Its US suitor KKR lobbied the board to accept its offer, while the competition watchdog stepped up its investigation of Assura’s £1.7bn takeover by a rival UK healthcare investor. Assura is still recommending that its shareholders accept the PHP offer. Meanwhile, the chief economist at the Bank of England has warned that “persistent inflation” could slow the pace of future interest rate cuts. Huw Pill is one of four members of the monetary policy committee who voted against the rate cut to 4% this week. Profits at Jaguar Land Rover slumped in its quarter ended in June, as the British luxury carmaker has grappled with US trade tariffs and a slowdown in sales. Underlying pre-tax profit dropped by 49% to £351m in the quarter, with revenue falling by 9% to £6.6bn, thanks partly to a temporary pause in exports to the US and the planned wind down of older Jaguar models before the launch of new electric models next year. JLR said US tariffs had a “direct and material impact on profitability and cash flow in the period”, but that the “US-UK trade deal will significantly reduce the financial impact of US tariffs going forward”. The car maker, which is owned by the Indian group Tata Motors, said last month that it would axe up to 500 management jobs in the UK, impacting 1.5% of its UK workforce. Chief executive Adrian Mardell said the results came amid “challenging global economic conditions”. We are grateful to the UK and US governments for delivering at speed the new UK-US trade deal, which will lessen the significant US tariff impact in subsequent quarters, as will, in due course, the EU-US trade deal announced on July 27.” River Island has secured approval for a restructure plan designed to stop the fashion retailer from falling into administration. The plan received approval from a high court judge on Friday after the majority of creditors gave their backing to the plan earlier this week. Ben Lewis, the retailer’s chief executive, said approval of the plan would enable the company to “align our store estate to our customers’ needs. We are pleased that River Island’s restructuring plan has been approved by the High Court. We have a clear transformation strategy to ensure the long-term viability of the business, and this decision gives us a strong platform to deliver this. Recent improvements in our fashion offer and shopping experience are starting to show results, and the restructuring plan will enable us to align our store estate to our customers’ needs.” You can read the full story by my colleague Sarah Butler here: Huw Pill, chief economist at the Bank of England and one of four members of the monetary policy committee who voted against the interest rate cut this week, has warned “persistent inflation” could slow the pace of future rate cuts. Pill said in an online presentation to businesses: There’s still a little bit further downward to go with Bank Rate. I think the pace at which those downward moves perhaps go forward is a little bit less clear than the pace that we’ve seen over the last year. On Thursday, the Bank of England’s monetary policy committee (MPC) voted to cut the base rate by a quarter point to 4%, its lowest level for more than two years. It was one of the closest decisions since its independence more than 25 years ago, with the vote split 5-4. Pill was one of the MPC members who voted to keep rates unchanged. The latest official figures show that inflation rose to 3.6% in June, ahead of the Bank’s 2% target. Pill said: There is some shift in the balance of risks on inflation. There is a risk of spillover into more persistent inflation. When inflation is high due to external forces, we need to be aware of the risk they might affect domestic price-setting. …Our mandate is that we will get inflation to 2%, that’s the target, on a sustainable rate. We will do whatever we need with the Bank rate to do that. They may be a bit lower than where we are but nothing is set. On Thursday, the Bank warned that rising food prices could dirve to inflation to 4% in September. The Competition and Markets Authority (CMA) has cleared Boeing’s $4.7bn (£3.5bn) deal to buy Spirit AeroSystems, the parts supplier it spun out nearly 20 years ago. The US plane manufacturer agreed to buy Spirit last year in an all-stock deal which valued it at $4.7bn. The total transaction value, including Spirit’s net debt, was $8.3bn. The CMA started to investigate the deal in June to determine whether it would affect competition in the UK. It has not yet released the full details behind its decision but it has said it has cleared the acquisition. The deal to bring Spirit back in-house marks a move away from Boeing outsourcing key components for its planes. Spirit was spun off from the business in 2005, but last year it still accounted for about 70% of all of its orders. Around 25% came from Boeing’s rival, Airbus. Turning to the world of healthcare, shares in the US pharmaceutical company Eli Lilly slumped by 14% last night, after disappointing results from its obesity pill. Eli Lilly said on Thursday that patients taking its pill orforglipron lost an average of 12.4% of their body weight, at the lower end of expectations. People taking a placebo lost 0.9%. Shares in rival Novo Nordisk, the Danish drugmaker behind the Ozempic and Wegovy weight-loss drugs, are up 4% this morning. Elsewhere in the sector, FTSE 100 pharmaceutical company GSK said this morning that it will receive $370m as part of a US patent settlement between CureVac and BioNTech related to its Covid-19 jab. It will also receive a 1% royalty on future US sales of influenza, Covid-19 and related combination mRNA vaccine products by BioNTech and Pfizer. Shares in GSK are up about 1% this morning There has been another twist in the attempted takeover of the NHS landlord Assura: this morning the competition watchdog blocked the full integration of Primary Health Properties (PHP) with Assura, as it investigates the £1.79 bllion deal. A bidding war for the company between PHP and the private equity firm KKR had been going on since February – but in June Assura’s board recommended a cash offer from PHP which valued it at £1.79bn. But the Competition and Markets Authority (CMA) launched the first stage of its investigation into the deal last month, and has now served an initial enforcement order on the firms. KKR still argues that its bid for Assura is superior to the offer from Primary Health. The firm said it had met with Assura in recent days to lobby for its own cash takeover of the company. Assura owns a property portfolio worth about £3.1bn, including a number of NHS buildings such as doctors’ surgeries. Oil prices are headed for their worst week since June, as investors prepare for the possibility of talks between Donald Trump and Vladimir Putin, and as the latest round of US tariffs weigh on the global economic outlook. Brent crude futures are on track to fall by around 4% this week, currently trading at $66.36. West Texas Intermediate crude futures are on track to fall by about 6% compared with last week. Analysts think this is largely because of the impact that Trump’s latest tariffs will have on the global economy. This week, more than 60 countries were hit by sweeping “reciprocal” rates, which range from 10% to 39%, 40% and 41% for Switzerland, Brazil and Syria. A widely expected meeting between the US president and the Russian leader is also affecting the market, with investors anticipating that eased sanctions on Russia could increase the oil supply. This week Trump increased tariffs on India, in a move he described as punishment for continuing to buy Russian oil. The UK’s blue chip FTSE 100 stock index has opened slightly higher this morning, up 0.26%. JD Sports is the strongest riser in the index, with its shares up 2.2%. It is followed by Glencore, with its shares up 1.9% after news this week that the miner decided to keep its primary listing in London, ditching a possible plan to move to New York. The mid-cap FTSE 250 index is not performing as well, down by about 0.1%. TBC Bank is the worst performer, with its shares falling by as much as 12% in early trading, though the Georgian bank reported a 5% rise in its profits for the second quarter, as well as a new buyback. Meanwhile, the pound is slipping against the US dollar this morning, even after the Bank of England’s monetary policy committee (MPC) voted to cut its key base rate by a quarter-point to 4% yesterday. The pound is down 0.13% against the dollar, although it is still above $1.34. While the Bank has cut rates, it was one of the closest decisions since its independence more than 25 years ago with a 5-4 vote split. The market has lowered its expectations of another quarter cut point this year, in contrast to growing expectations that the Federal Reserve will cut interest rates in the US next month. On Thursday, Donald Trump said he will nominate Stephen Miran to the Fed’s board of governors for four months, and reports suggest that current governor Christopher Waller is the favourite candidate to serve as the next Fed chair. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, says both men are viewed as dovish, which should align with Trump’s ambition for lower rates. However, the US 2-year yield has barely reacted—reminding us (again) that rate cuts don’t always lower borrowing costs if they aren’t seen as credible or justified. Remember last September, when the Fed unexpectedly slashed rates by 50bps? The 2-year yield jumped nearly 30bps over the following two months. For now, markets still expect the next cut to come in September, keeping the S&amp;amp;P 500 near record highs despite trade uncertainty and policy inconsistency. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Gold futures hit a record high on Friday after a Financial Times report that the United States has imposed tariffs on imports of one-kilo gold bars, a move that is expected to ramp up pressure on Switzerland, the biggest precious metal hubs in the world. The FT has seen a letter from the Customs Border Protection agency which said one-kilo and 100 ounce gold bars should be classified under a customs code subject to higher tariffs. One-kilo bars are the most popular form of the metal traded on Comex, the biggest gold futures market, and make up most of Switzerland’s bullion exports to the US. US gold futures rose by. 1.3% at $3,499.30, after hitting an all-time high of $3,534.10. Meanwhile, the price spread between New York futures and spot prices widened by about $100. It marks another blow for Switzerland, which Donald Trump has hit with a shock 39% export tariff. Swiss companies, whose exports to the US account for about one-sixth of their total foreign sales, face one of the steepest tariff rates in Trump’s trade war regime. Only Laos, Myanmar and Syria had higher figures, at 40-41%. The EU and the UK have negotiated 15% and 10% respectively. Switzerland exported $61.5bn of gold to the US in the 12 months ending in June, the FT said. This would be subject to a further $24bn in levies under Switzerland’s 39% tariff rate, which came into effect on Thursday, according to the report. The agenda 9am BST: UN Food and Agricultural Organization Price Index</t>
+          <t>Time to wrap up… UK retailer stocks sold off today after a downbeat note from analysts at Deutsche Bank. Associated British Foods, which owns Primark as well as a range of other food and drink brands such as Twinings, fell by as much as 5% today, after analysts at the bank downgraded their view on the stock from a neutral “hold” to “sell”. Deutsche also downgraded its view on home improvement retailer Wickes to a “sell”, and B&amp;amp;Q owner Kingfisher was moved down from a “buy” to a “hold”. Meanwhile, the US stock market has had a rather subdued open, with the S&amp;amp;P 500 rising slightly by 0.5% in early trading as the stock market seems to shake off worries about Trump’s latest attack on the Fed. Trump has moved to oust Lisa Cook, a governor at the Federal Reserve, in his latest attack on the American central bank. It is an unprecedented intervention by a US president, which threatens to undermine the independence of the central bank of the biggest economy in the world. Meanwhile, Trump has also threatened to impose tariffs and export restrictions on countries whose taxes, legislation and regulations target US big tech companies such as Google, Meta, Amazon and Apple. In a post on his social media platform, Truth Social, the US president said: “Digital taxes, legislation, rules or regulations are all designed to harm, or discriminate against, American technology.” He said such measures – which include the UK’s digital services tax, which raises about £800m annually from global tech companies through a 2% levy on revenues – also “outrageously give a complete pass to China’s largest tech companies”. Trump said: “As the president of the United States, I will stand up to countries that attack our incredible American tech companies. Unless these discriminatory actions are removed, I, as president of the United States, will impose substantial additional tariffs on that country’s exports to the USA, and institute export restrictions on our highly protected technology and chips.” UK tech firm Filtronic has announced its biggest ever contract worth £47.3m with Elon Musk’s SpaceX. Shares in the County Durham-based defence and telecoms equipment maker rose nearly 5% on Tuesday after the announcement. The contract covers supply of a type of radio frequency tech designed for high-performance wireless communication, using next-generation gallium nitride (GaN) E-band technology. Nat Edington, Filtronic CEO, said: We are extremely proud to announce this landmark contract, which not only sets a new commercial record for Filtronic, but also reflect the success of our partnership with world-leading satellite company SpaceX, supporting the Starlink constellation. It comes after Filtronic announced a £16.8 million contract in February with the US aerospace firm. The Bank of England policymaker Catherine Mann has said that while she thinks it is appropriate to hold interest rates at their current level, she stands ready to cut forcefully if there are serious risks to economic growth. Mann, who will appear at the Future of Central Banking conference at the Banco de México today, will say in a speech: A more persistent hold on Bank Rate is appropriate right now, to maintain the tight (but not tighter) monetary policy stance needed to lean against inflation persistence persisting. However, I stand ready for a forceful policy action, in the form of larger, more rapid Bank Rate cuts, should the downside risks to domestic demand start materializing. The Bank of England’s monetary policy committee cut interest rates to 4% earlier this month, in line with projections of falling inflation over the next two years. However, several of its members, including Mann, voted to hold interest rates until the trend became clearer. She will say in her speech today: In my assessment, the scenario outlining upside risks to inflation through inflation persistence (which included additional second round effects in domestic price and wage-setting, amplified by weak potential productivity growth) is playing out, whereas the ‘downside risk to demand’ scenario remains a risk and is not my central case. Full year results for Debenhams have just landed: revenue fell 1% in the year ended in 28 February to £790.3m, while its continuing loss before tax widened from £164.4m in its last financial year to a loss of £263.9m. However, shares in the retailer, which also owns brands boohoo and Karen Millen, are up by 2.2%. Investors are taking confidence in the fact that the company says all of its brands are now trading profitably in terms of adjusted Ebitda, and that it expects this measure of profit to be higher in its next half compared with the year prior. The company also said it is exploring a potential sale of PrettyLittleThing, the fast fashion brand aimed at young women, as part of its business review. Dan Finley, who has been chief executive of the group since November, said: The business has been through a very challenging period which is reflected in these results. I want to assure shareholders that the business is taking the necessary actions, quickly and decisively, to address the challenges that we face. No stone will be left unturned. …We are focused on delivering on the huge opportunity ahead for the Debenhams brand. Work is progressing to reposition and right size the Youth Brands, with a laser focus on profitability and cash generation under new management. This will be a multi-year turnaround as was the case with the Debenhams brand. As part of our ongoing business review, we are exploring a potential sale of PLT. We are also assessing long-term options for our US and Burnley distribution sites to enhance efficiency and ensure alignment with our stock-lite strategy. A strikes by hold baggage screeners at Gatwick airport scheduled for the end of this month has been called off, after workers voted to accept an improved pay deal. The workers, employed by ICTS, will receive a 7% pay rise back paid to April 2025, the Unite union said. The deal means that strikes scheduled from 29 August to 2 September will now not take place. The yield on the 30-year US Treasury has risen by 0.022 percentage points to 4.909%, as investors worry that Donald Trump’s latest attempt to intervene with the Federal Reserve could undermine the independence of the American central bank. Meanwhile, the yield on the two-year Treasury has dropped by 0.028 percentage points to 3.694%, as investors expect that pressure from the US president could lead to faster rate cuts. The market is pricing in an 82% chance of a cut in mid-September, when the rate-setting Federal Open Market Committee is next scheduled to meet. The US stock market looks like it will fall slightly at the open, with futures for the blue chip S&amp;amp;P 500 index down by 0.06%, and futures for the Nasdaq down 0.03%. The blue-chip FTSE 100 index is trading down 0.5% so far today. B&amp;amp;Q owner Kingfisher is the worst performer in the group, with its shares down 4.1%. Primark owner Associated British Foods is a close second, down 3.8%, after a downbeat note from analysts at Deutsche Bank about the outlook for British retail. The mid-cap FTSE 250 index is also down by 0.9%, led by an 8% drop at home improvement retailer Wickes. Distributor Bunzl is the best performer in the FTSE 100, with its shares up 5% after it told investors that it would restart its share buyback programme. British American Tobacco is among the worst performers, down 2.5%, after it told investors this morning that its chief financial officer, Soraya Benchikh, will step down from her role effective today. Vacancies for entry-level jobs have hit their lowest level in five years, according to the job search site Adzuna. The proportion of new entry-level jobs has dropped to just over a fifth of the overall market, it found, its lowest share since 2020. The number of overall vacancies dropped 1.2% in July to 864,705, Adzuna found. Graduate jobs nudged up 2.5% against June, but are still down 28% compared with the same time last year. Salaries for listed jobs also fell by 0.3%, as competition for work has heated up: there are now roughly 2 jobseekers per vacancy, Adzuna said. Andrew Hunter, co-founder of Adzuna, said: After a hopeful uptick in June, July saw the pendulum swing back with vacancies falling again. While salary growth remains one of the few consistent positives – continuing to outpace inflation – hiring appetite is clearly uneven. The ongoing strength in sectors like construction is in stark contrast to another consecutive monthly drop in healthcare roles – traditionally one of the most stable sectors. This speaks to a market still finding its footing. Until we see greater stability across the board, it’s likely this stop-start pattern will continue. Vacancies in healthcare have dropped 25.4% since April, when the government changed the rules for employer national insurance contributions and the minimum wage. The decline in entry-level jobs come as official figures show the number of young people not in education, employment or training (Neet) has leapt by more than a quarter in the past five years to reach almost 1 million. Liz Kendall, the work and pensions secretary, told my colleague Richard Partington that Labour has a “mountain to climb” to bring down the numbers: The cost of insuring French government debt against default has risen today, but remains extremely low. Data from S&amp;amp;P Global show that the cost of a five-year French credit default swap has risen to 37 basis points, the highest since May, Reuters reports. That level indicates there’s very little chance of France defaulting. For comparison, during the eurozone debt crisis of 2015, Greece’s 5-year credit default swaps rose over 1,900bps, amid heightened fears that Athens could default on its debts. There’s also gloom in the UK hospitality sector, where late-night venues have been closing at an alarming rate. More than one in four late-night venues have shut their doors since 2020, according to new data from the Night Time Industries Association (NTIA), who are calling on the government to cut VAT, reverse the increase in employers’ national insurance contributions, and maintain business rates relief for the sector. More here: Wood Group has come a step closer to becoming the latest company to leave the London Stock Exchange, after the board of the British oil services company said it was minded to accept a reduced takeover offer from a Dubai-based suitor. Sidara, the Middle Eastern engineering company, initially proposed a 35p-a-share offer in April. However, on Tuesday the company said that having completed due diligence Sidara would make a lower offer of 30p a share, once remaining preconditions had been met. The FTSE 250-listed company said it had evaluated the new offer with its financial advisers and concluded that it was “at a value the board would be minded to recommend to shareholders”. As a result the deadline for Sidara to announce a firm intention or withdraw its offer has been extended, again, to 5pm on 28 August. UK retail stocks are selling off this morning after a downbeat note from analysts at Deutsche Bank. Associated British Foods, which owns Primark as well as a range of other food and drink brands such as Twinings, has fallen by 5% this morning, after analysts at the bank downgraded their view on the stock from a neutral “hold” to “sell”. Deutsche also downgraded its view on home improvement retailer Wickes to a “sell”, with its shares falling by as much as 9% this morning, making it the worst laggard in the mid-cap FTSE 250 index today. B&amp;amp;Q owner Kingfisher was moved down from a “buy” to a “hold” rating, sending its shares down by as much as 4% this morning. Adam Cochrane and Benjamin Yokyong-Zoega, of the bank, said: We are taking a more cautious view on the UK consumer. The end of 2024 and early 2025 are likely to have been the sweet spot with real wage growth set to slow and fear of unemployment set to build from here. Our Household Cash Flow model shows discretionary spending lagging spending power and, unless consumers reduce savings, there will be a 4ppt slowdown in discretionary spend to +3% in 2H from +7% in 1H. Retail sales have been resilient into Q2 helped by warm weather although there is some variance by category. Consumer confidence metrics remain subdued and our new DB “Fear Index” suggests things may be getting worse. The bank also lowered its target prices for Dunelm and Marks &amp;amp; Spencer, although still retained their “buy” ratings on the stocks. The shares are down 0.6% and 0.5% respectively this morning. The wobble in the UK bond market also follows a high reading for food inflation from the British Retail Consortium. It found that shop prices had risen at their fastest pace for 18 months, with food inflation hitting 4.2% in August. That was driven by a jump in the cost of grocery staples such as eggs and butter, the industry body said. Helen Dickinson, chief executive of the BRC, said the rapid rise added to the pressure on people already struggling with the cost of living. Staples such as butter and eggs saw significant increases due to high demand, tightening supply, and increased labour costs. Chocolate also got more expensive as global prices of cocoa remain high owing to poor harvests. UK bonds are falling this morning: the yield on the two-year gilt rose by as much as 6 basis points to 4.008%, while the yield on the 30-year gilt also rose by 5.634%, its highest point since April. Bond yields rise when prices fall. It follows a rise in US Treasury yields after Donald Trump ordered the removal of Lisa Cook from the board of governors on the Federal Reserve, the US central bank. The sell-off in the bond market also follows reports over the weekend that the UK is facing an “IMF bailout”. Jagjit Chadha, a professor of economics at the University of Cambridge and former head of the National Institute for Economic and Social Research, claimed the economy was at risk of “collapse”. He said the financial situation was “as perilous the period leading up to the IMF loan of 1976”, when Britain had to be bailed out by the global banking body. He told the When the Facts Change Substack, written by Liam Halligan: I’m in a world in which I could imagine it [an IMF bailout] happening, and we’ll be bereft in that case. We will not be able to roll over debt, we will not be able to meet pensions payments, benefits will be hard to pay out.” The pound is also a bit weaker this morning, down by 0.01% against the US dollar to $1.3456. European shares are broadly down this morning, with the European Stoxx 600 index down by 0.7%. That was led by France’s Cac 40 index, which has dropped by 1.4%, mirroring a fall in its bond market. The UK’s blue chip FTSE 100 index is down by 0.6% this morning, with Associated British Foods, the owner of Primark, the biggest faller, down 3.9%. Meanwhile, the German Dax index has dropped 0.9%, while the Italian FTSE MIB has fallen by 1.2%. Political uncertainty in France is shaking its bond market, with its 10-year bond yield rising by as much as 2 basis points this morning to trade around 3.51%, its highest level since March. Bond yields rise when prices fall. It comes after Prime minister François Bayrou called a confidence vote that could topple the French government next month, as he tries to find support for plans to shore up the government’s ailing public finances. Bayrou has said France is going through a “decisive moment”. If the government secures a majority in the confidence vote, it would be confirmed, he said, but “if it does not have a majority, the government will fall”. Charlotte de Montpellier, senior economist at the broker ING, says the “obstacle is almost impossible to overcome”. Bayrou’s centrist coalition holds just 210 of 577 seats in the Assembly. The far-right RN, far-left LFI, Greens, and Communists—together 264 MPs—have already declared they will vote against him. Only the Socialist Party could tip the balance, but early signals suggest they are unwilling to support the government without major revisions to the budget, which seems unlikely. …If Bayrou loses the vote, President Macron will face a difficult choice: appoint a new prime minister capable of forming a government in a fragmented Assembly, or dissolve Parliament and call new elections—something he has previously ruled out. Either path would inject fresh uncertainty into an already fragile political landscape. The likely fall of the government will weigh heavily on the French economy. With only 0.8% GDP growth expected this year, the economy was already weak, and the political crisis adds a new layer of uncertainty. Drafting and passing a 2026 budget will become even harder, delaying fiscal consolidation and potentially worsening France’s debt trajectory. The longer reforms are postponed, the greater the eventual adjustment will need to be. In short, France’s political instability is becoming an economic liability. Investors and institutions will be watching closely—not just for what happens on 8 September, but for what comes next. Closer to home, there are a few corporate updates after the bank holiday. Soraya Benchikh, chief financial officer at British American Tobacco, is stepping down today, the company said in a statement. Javed Iqbal will act as the interim CFO until the company appoints a permanent successor. Meanwhile the FTSE 100 distribution group Bunzl has reported that its first-half sales rose by 0.8% to £5.76bn, in line with expectations. Pre-tax profit fell by 10.5% to £250.2m in the six months ended in June. However, the company said it would resume the remaining £86m of its previously announced £200m share buyback, after pausing it in April. Trump’s attempt to intervene at the Federal Reserve has spooked investors, with gold, which is viewed as a safe haven asset, rising this morning. Economists at Deutsche Bank write: Gold spiked by +1% and is holding on to most of this overnight gain, while futures on the S&amp;amp;P 500 (-0.14%) and the Nasdaq (-0.18%) are modestly lower. Meanwhile, the Treasury curve has seen a sizeable steepening, with the 2yr yield trading -0.7bps lower but the 10yr up +2.9bps and the 30yr +4.5bps to 4.93%. This has brought the 2s30s slope to 122bps, its steepest since January 2022 when the Fed had not yet started its post-Covid hiking cycle. Cook’s removal could push the Fed to a more dovish stance, say economists at Deutsche Bank. They write: Were Cook’s dismissal to hold, it would open up another seat for Trump to fill on the seven-person Federal Reserve Board. With Stephen Miran nominated for the seat recently vacated by Governor Kugler and with Governors Waller and Bowman dissenting in favour of a rate cut at the July meeting, this would increase the prospects of a dovish majority on the Board. Cook, who was appointed by President Joe Biden in 2022, was working a term that was not due to expire until 2038. If she were to be removed, it would give Trump the change to secure a four-person majority on the Fed’s board of governors. Market bets suggest there is an 82% chance that the Fed will vote to cut its key interest rate at its next meeting in mid-September. However, economic data coming out this week on inflation and the labour market could still sway the decision. Here is Justin Wolfers, an economics professor at the University of Michigan, drawing a parallel with Turkey’s president Recep Tayyip Erdoğan. Donald Trump has moved to oust Lisa Cook, a governor at the Federal Reserve, in his latest attack on the American central bank. It is an unprecedented intervention by a US president, which threatens to undermine the independence of the central bank of the biggest economy in the world. Trump posted a letter on his social media platform Truth Social on Monday, claiming he had “sufficient cause” to fire Cook, based on allegations she made false statements on one or more mortgage loans. Cook, who is the first black woman to serve on the Fed Board in Washington, has sad that Trump has no authority to fire her and that she will not quit. She said: I do intend to take any questions about my financial history seriously as a member of the Federal Reserve and so I am gathering the accurate information to answer any legitimate questions and provide the facts. The news has spooked markets, with the US dollar and long-dated Treasuries both falling on Tuesday. The US dollar index, which tracks the greenback against a basket of other major currencies, fell by 0.1%. Trump’s latest attack on the Fed follows “relentless pressure” on Fed Chair Jerome Powell, notes Tony Sycamore, of the broker IG. He says: In the short term, the removal of Cook who has tended to vote with the FOMC majority, increases the likelihood of a Fed rate cut at the September FOMC meeting. A prospect expected to weigh on the US dollar and lend support to equities and other risk assets, including Bitcoin. However, beyond the “sugar hit” of a rate cut in September, recent developments around key Fed personal, heighten concerns over rising political interference, raising the risk that traders view the Fed as politically compromised. This could trigger a rerun of the “Sell US assets” theme seen earlier this year. In such a scenario, both the US dollar and US equities could experience sharp declines. The agenda 1:30pm BST: US durable goods orders 2:00pm BST: Case-Shiller US house prices 3:00pm BST: US CB consumer confidence report</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>River Island has secured approval for a restructure plan designed to stop the fashion retailer from falling into administration. The plan received approval from a high court judge on Friday after the majority of creditors gave their backing to the plan earlier this week.</t>
+          <t>UK retailer stocks sold off today after a downbeat note from analysts at Deutsche Bank. Associated British Foods, which owns Primark, fell by as much as 5% today. Deutsche also downgraded its view on home improvement retailer Wickes to a ‘sell’</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Financial Regulation Expansion</t>
+          <t>UK Economic Challenges Overview</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Time to wrap up…. Sales of new Tesla cars slumped by 59% year-on-year in the UK last month, but Chinese carmakers led by BYD reported big jumps in UK sales. BYD sales quadrupled year on year to reach 3,200 in July, even as overall sales of all types of car declined by 5% to 140,000, according to data published on Tuesday by the Society of Motor Manufacturers and Traders (SMMT), a lobby group. Former star stock picker Neil Woodford and his investment management company have been fined almost £46m by the UK’s financial regulator over the collapse of his popular equity fund. The Financial Conduct Authority (FCA) has given Woodford a penalty of £5.89m and banned him from holding senior manager roles and managing funds for retail investors and fined Woodford Investment Management (WIM) £40m. Donald Trump has attacked Jaguar Land Rover’s divisive rebranding strategy, hours after Britain’s largest carmaker announced its new boss. Trump posted on his Truth Social platform that the auto company, owned by India’s Tata Motors, was “in absolute turmoil” and claimed that the “CEO resigned in disgrace”. The UK’s dominant service sector has reported its biggest drop in new orders in almost three years in July, adding to pressure on the Bank of England to cut interest rates on Thursday. The oil and gas group BP is launching a fresh cost-cutting scheme, despite reporting better-than-expected profits, as it tries to do more for its shareholders to fend off pressure from activist investors. The fossil fuel company said it would begin a fresh review of its business when its new chair, Albert Manifold, joins the board in September. Awkwardly, a rival survey of America’s services sector paints a darker picture. According to the Institute of Supply Management, US service sector firms barely grew in July as Donald Trump’s trade wars pushed up costs, and led to job losses. The ISM’s service sector PMI has dropped to 50.1% last month from 50.8% in June, a level that shows growth almost petered out. One company, in the Agriculture, Forestry, Fishing &amp;amp; Hunting sector, told ISM: “Higher tariffs are increasing the cost of imported feed ingredients and trace minerals for livestock and poultry feeds. Business and customer concerns over additional cost risk due to additional tariffs.” Encouraging economic news from the US: America’s service sector grew at a faster rate last month. The latest poll of purchasing managers from S&amp;amp;P Global has found that business activity in the services sector increased at the sharpest pace in the year-to-date amid a solid and accelerated expansion in new business. S&amp;amp;P Global adds: Companies responded to higher workloads by hiring additional staff, albeit only modestly. Meanwhile, tariffs continued to add to inflationary pressures, resulting in faster increases in both input costs and output prices. Its services PMI Business Activity Index rose to a seven-month high of 55.7 in July, up from 52.9 in June, showing faster growth. Google has outlined its latest step towards artificial general intelligence (AGI) with a new model that allows AI systems to interact with a convincing simulation of the real world. The Genie 3 “world model” could be used to train robots and autonomous vehicles as they engage with realistic recreations of environments such as warehouses, according to Google. The US technology and search company’s AI division, Google DeepMind, argues that world models are a key step to achieving AGI, a hypothetical level of AI where a system can carry out most tasks on a par with humans – not just individual tasks such as playing chess or translating languages – and potentially do someone’s job. DeepMind said such models would play an important role in the development of AI agents, or systems that carry out tasks autonomously. “We expect this technology to play a critical role as we push toward AGI, and agents play a greater role in the world,” DeepMind said. There’s been disruption at London’s Heathrow Airport today, after a key road tunnel was closed. Passengers hoping to get away on their summer break faced delays after the Central Terminal Area tunnel to Terminals 2 and 3 is was closed. Heathrow blamed a technical issue, and urged passengers to use public transport to Terminal 5, where train services were available to all other terminals. The closure lead to heavy queues on the roads leading to Heathrow….. …and chaotic scenes inside the airport. Heathrow says that the road tunnel to Terminals 2 and 3 has now reopened, but warned that there is still congestion at the airport, and so they recommend allowing extra time for your journey. The US trade deficit with the rest of the world has narrowed, as the rush to import goods into America ahead of Donald Trump’s tariffs ended. The US’s goods and services deficit dipped to $60.2bn in June, down $11.5bn from $71.7bn in May. This decline was due to a narrowing in the US goods deficit, while its services surplus grew a little. Imports into the US fell by $12.8bn to $337.5bn in June, while exports dipped by $1.3bn to $277.3bn. Harry Chambers, assistant economist at Capital Economics, explains: The narrowing of the trade deficit was mainly due to a normalisation in pharmaceutical imports and while exports appeared weak, this was primarily due to a fall in gold exports. The big picture is that, despite June’s fall, imports aren’t collapsing and are roughly in line with their levels last year. That said, with export orders weak, it seems likely that exports will struggle over the coming months. Showing his inate ability to commit news, Donald Trump revealed during today’s CNBC interview that he will unveil new tariffs on semiconductors and chips as soon as next week. He told the “Squawk Box” show that an announcement will come “within the next week or so,” saying: “We’re going to be announcing on semiconductors and chips, which is a separate category, because we want them made in the United States.” U.S. President Donald Trump has also said recent falls in energy prices could pressure Russian President Vladimir Putin to halt the war in Ukraine. In his inerview with CNBC, Trump said: “If energy goes down enough, Putin is going to stop killing people. If you get energy down, another $10 a barrel, he’s going to have no choice because his economy stinks.” Brent crude is curently trading at $67.82 per barrel, down 1.35% today, down from over $76 per barrel a year ago. Donald Trump has revealed he is considering four candidates — including former Federal Reserve Governor Kevin Warsh and National Economic Council Director Kevin Hassett — to become the next head of America’s central bank. In an interview with CNBC, Trump said: “I think I say Kevin and Kevin, both Kevins are very good, and there are other people that are very good too.” Current Federal Reserve chair Jerome Powell’s term expires next May. Trump also revealed that Treasury Secretary Scott Bessent told him he did not want to be nominated to replace Powell at the Fed, as he wants to stay in his current role. Neil Woodford is also facing calls for his CBE to be revoked. The Woodford Campaign Group and Transparency Task Force have repeated their request for Mr Woodford’s CBE to be forfeited now that the Financial Conduct Authority’s investigation has been completed. More than 500 people have so far signed a petition drawn up by the Woodford Campaign Group calling for the forfeiture. In an open letter to Sir Chris Wormald, chairman of the Honours Forfeiture Committee at the Cabinet Office, Andy Agathangelou, who founded both campaign groups, said: “This scandal is obviously a matter of great public interest – hundreds of thousands of people have been directly impacted by it, many having lost life-changing amounts of money. Trade war news: Swiss president Karin Keller-Sutter and business minister Guy Parmelin will fly to Washington on Tuesday, the government said, to try to avoid the 39% tariffs announced by President Donald Trump on exports to the United States. The pair will “facilitate meetings with the US authorities at short notice and hold talks with a view to improving the tariff situation for Switzerland,” the government said. The trip comes after Keller-Sutter was accused of mishandling a vital phone call with the White House, leading Trump to hit Switzerland with a shock 39% export tariff. Over on Wall Street, construction and mining equipment company Caterpillar has missed second-quarter profit expectations. Caterpillar’s adjusted profit per share in the second quarter of 2025 fell to $4.72, down from $5.99 in Q2 2024. The drop in earnings was due to a fall in profit margins. Sales and revenues for the second quarter of 2025 dipped by 1% to $16.6bn, Britain’s main minimum wage rate will probably need to rise by around 4.1% next year to £12.71 an hour to keep up with the government’s goal for it to match two thirds of median earnings, according to the body which sets the rate. The Low Pay Commission said today the final figure for the National Living Wage could range between £12.55 and £12.86 an hour. The commission is due to provide a firm recommendation to the government by the end of October. The national living wage is currently set at £12.21 for those aged 21 and over. Britain’s service sector companies were hit by a drop in orders last month, as demand at home and abroad remained sluggish. Service sector growth slowed last month amid a decline in new work, according to the latest survey of purchasing managers from data firm S&amp;amp;P Global. It’s UK Services PMI Business Activity Index has dropped to 51.8, from 52.8 in June, showing a slowdown in growth. The survey found that total new work decreased in July, at the fastest rate since November 2022. Export sales also fell in July, blamed on fragile global economic conditions and elevated geopolitical tensions. Worryingly, services firms cut staff again. Tim Moore, economics director at S&amp;amp;P Global Market Intelligence, says: “UK service providers recorded a third consecutive monthly rise in business activity, but they were unable to maintain the growth rate achieved in June. Moreover, new business intakes swung back into contraction during July, with the downturn in order books the fastest for just over two-and-a-half years. Risk aversion and low confidence among clients were the main reasons provided for sluggish sales pipelines, alongside an unfavourable global economic backdrop. Hiring trends were especially subdued, with total workforce numbers decreasing to the greatest extent since February. Worries about rising payroll costs were cited as the main factor holding back recruitment. Newsflash: The UK’s financial regulator has decided to fine former star fund manager Neil Woodford and his investment management company nearly £46m, over the collapse of his popular equity fund. The Financial Conduct Authority says it has decided to fine Woodford £5,888,800 and ban him from holding senior manager roles and managing funds for retail investors. The FCA has also decided to fine Woodford Investment Management (WIM) £40,000,000. The penalties result from failures in their management of the Woodford Equity Income Fund (WEIF), the FCA says, which collapsed in October 2019 after investors rushed to withdraw money in response to a raft of poorly performing company investments, including some hard-to-sell, illiquid assets. The fund was frozen and later closed and wound up. About 300,000 people had invested in the fund, including 130,000 through Hargreaves Lansdown, which is being sued by thousands of investors. In today’s ruling, the FCA explains that between July 2018 and June 2019 WIM and Woodford made “unreasonable and inappropriate investment decisions”, including selling sold more liquid investments (where it’s easier to find a buyer) and buying less liquid ones (which are harder to shift quickly at a good price). They also failed to react appropriately as the fund’s value declined, its liquidity worsened and more investors withdrew their money, the regulator says. However, these findings are only “provisional”, as Neil Woodford and Woodford Investment Management have referred the Decision Notices to the UK’s Upper Tribunal. The FCA is also critical of Woodford – a former star investment manager – today, saying he held “a defective and unreasonably narrow understanding of his responsibilities.” Steve Smart, joint executive director of enforcement and market oversight at the FCA, said: ‘Being a leader in financial services comes with responsibilities as well as profile. Mr Woodford simply doesn’t accept he had any role in managing the liquidity of the fund. The very minimum investors should expect is those managing their money make sensible decisions and take their senior role seriously. Neither Neil Woodford nor Woodford Investment Management did so, putting at risk the money people had entrusted them with.’ It appears that the UK government’s offer to subsidise new electric car purchases may have actually dampened the car market last month. The grants, which offer up to 10% off the price of many electric cars costing less than £37,000, were announced in mid-July. But the government only revealed the first eligible cars today – four Citroën models. The discount scheme won’t apply to Teslas (as they’re too expensive), or models from China as they don’t pass the government’s rules on environmentally sustainable manufacturing practices. The SMMT explain: The newly announced Electric Car Grant (ECG) provides a welcome and much-needed fiscal incentive for BEV uptake, but full model eligibility has yet to be confirmed, causing some buyers to hold off pending confirmation of which vehicles will qualify for a discount of up to £3,750. Its sales figures show that registrations of plug-in hybrid electric vehicles (PHEVs) rose 33.0% in July while battery electric vehicles (BEVs) rose 9.1%, but there was a 10% drop in hybrids (HEVs). Petrol sales fell 14.7% and diesel were down 7.9%. BYD wasn’t the only Chinese EV maker growing its UK market share last month. Jaecoo, a brand from Chinese vehicle manufacturer Chery, sold 1,915 cars in the UK in July – a year ago, it didn’t sell any, as it only launched in the UK early in 2025. Omoda, another Chery brand, also made its debut this year – with 1,874 of its cars registered in the UK in July. Just in: Sales of Teslas in the UK more than halved, year-on-year, in the UK last month as the electric carmaker’s struggles continue. Industry body data just released shows that just 987 new Teslas were registered in the UK in July, almost 60% less than the 2,462 registered in July 2024. This means Tesla’s UK market share shrank to 0.7% in July, from 1.67% a year ago. For 2025 to date, Tesla sales in the UK are 7% lower, during a year in which CEO Elon Musk has faced heavy criticism for his – now-soured – relationship with Donald Trump. The wider UK electric car sector grew in July, though. Sales of battery-powered vehicles (BEVs) rose by 9.1% to 29,825, giving BEVs a 21.3% share of the market. China’s BYD more than quadrupled its sales last month, to 3,184 in July from 768 a year ago. The company recently launched a relatively cheap electric car, the Dolphin Surf, in the UK. BYD’s sales are up 514% during 2025 to 22,574, up from 3,672 in January-July 2024. That’s only slightly fewer than Tesla which has shifted 23,708 cars so far this year. Last month Tesla reported a large drop in quarterly deliveries, as demand faltered due to the backlash over CEO Elon Musk’s political stance. Tesla’s sales have also been hurt by its aging model line-up – the company has been rolling out an updated Model Y this year, dubbed the “Juniper” refresh. Yesterday, Tesla announced it was handing Musk stock options worth almost $30bn, in an attempt to keep him committed to the company for the next few years. Overall, the UK’s new car market shrank by 5% in July with 140,154 units registered, which is the weakest July since 2022. Mike Hawes, SMMT chief executive, says: July’s dip shows yet again the new car market’s sensitivity to external factors, and the pressing need for consumer certainty. Confirming which models qualify for the new EV grant, alongside compelling manufacturer discounts on a huge choice of exciting new vehicles, should send a strong signal to buyers that now is the time to switch. That would mean increased demand for the rest of this year and into next, which is good news for the industry, car buyers and our environmental ambitions. The UK’s Domino’s Pizza Group has cut its profit forecast this morning, warning that costs are climbing as sales fall. The group, which has the exclusive rights to the Domino’s brand in the UK and Ireland, reported that total orders were flat in the first half of this year, and that like-for-like sales fell 0.7% in April-June. Pre-tax profits have fallen by almost a third, on a statutory basis, from £59.4m to £40.5m. Domino’s now expect underlying profits to come in between £130m to £140m, down from a previous forecast of £140.8m-£149.7m. Several factors were blamed, including weak consumer confidence and rising employment costs. CEO Andrew Rennie blamed higher employment costs – following last year’s budget – and uncertainty over what chancellor Rachel Reeves might announce this autumn, saying: “There’s no getting away from the fact that the market has become tougher both for us and our franchisees, and that’s meant that the positive performance across the first four months didn’t continue into May and June. Given weaker consumer confidence, increased employment costs and uncertainty ahead of the Autumn Statement, franchisees are taking a more cautious approach to store openings for the time being. Shares in Domino’s Pizza Group have fallen by 19% in early trading. Overnight, UK luxury-car maker Jaguar Land Rover has named a new CEO – winning a blast from Donald Trump. JLR named P B Balaji, the finance boss of parent company Tata Motors, as its new chief executive, increasing the Indian owner’s influence over the company. Balaji will replace Adrian Mardell, who had run JLR for the last few years. Mardell’s tenure will be remembered for last year’s rebranding, and the launch of a new concept electric car which looked nothing like a traditional Jag, which captured attention and wound-up the rightwing commentariat. Anti-woke cheerleader Donald Trump was quick to give Mardell a hoofing on his way out the door. Posting on his Truth Social site, Trump declared that Jaguar’s “stupid, and seriously WOKE advertisement” had been “A TOTAL DISASTER!”, adding: The CEO just resigned in disgrace, and the company is in absolute turmoil. Who wants to buy a Jaguar after looking at that disgraceful ad. Shouldn’t they have learned a lesson from Bud Lite, which went Woke and essentially destroyed, in a short campaign, the Company. Trump also hailed actor Sydney Sweeney’s new advert for American Eagle as a triumph, saying the “HOTTEST” ad meant jeans were now “flying off the shelves.” Sweeney is probably in Trump’s good books after it emerged she was a registered Republican voter in Florida. BP is also planning to pump more cash to its shareholders. The company is raising its quarterly dividend by 4 per cent to 8.32 cents a share, subject to board approval. It has also announced a new $750m share buyback programme. Oil giant BP is launching a new cost-cutting scheme, despite reporting better than expected profits, as its incoming chairman gets to grips with the company in the face of pressure from activist investors. BP has beaten City expectations this morning by reporting a smaller drop in underlying profits than expected in the last quarter. On an underlying replacement cost basis, profits rose to $2.35bn in April-June. That’s 15% lower than the same quarter a year ago when the company benefitted from higher oil and gas prices, but also a jump on the $1.38bn profits posted in January-March. Analysts had forecast a smaller rise in underlying profits, to $1.8bn. But despite this beat, CEO Murray Auchincloss says “there’s much more to do”. Auchincloss tells shareholders this morning: In advance of chair elect, Albert Manifold joining the board on 1 September, he and I have been in discussions and have agreed that we will conduct a thorough review of our portfolio of businesses to ensure we are maximizing shareholder value moving forward - allocating capital effectively. We are also initiating a further cost review and, whilst we will not compromise on safety, we are doing this with a view to being best in class in our industry. Earlier this year, BP announced plans to cut more than $5bn from its previous green investment plan. But activist investor Elliott Management has been pushing BP to cut its operating expenses more aggressively and demanding more cost reductions. Manifold is due to become chairman on 1 October, a month after joining the board as a non-executive director. Good morning, and welcome to our rolling coverage of business, the financial markets, and the world economy. UK car sales dipped last month, after a bumper June. British new car registrations fell about 5% year-on-year in July, according to preliminary data released this morning by the Society of Motor Manufacturers and Traders (SMMT). Battery electric vehicles are now projected to account for 23.8% of new registrations in 2025, slightly up from SMMT’s previous forecast of 23.5%. The SMMT should release its final figures for July at 9am. The data comes as the UK government announces that France’s Citroën will be the first company to benefit from its new discount scheme, which cuts the cost of a new EV for consumers. Transport Secretary Heidi Alexander has confirmed buyers will get discounts of £1,500 off 4 Citroën models – the Citroën ë-C3, ë–C4, ë-C5 and the ë-Berlingo - from today. The scheme aims to bring down the price of electric cars to more closely match their petrol and diesel counterparts. The agenda 9am BST: UK new car sales for July 9am BST: eurozone service sector PMI for July 9.30am BST: UK service sector PMI for July 1.30pm BST: US trade data for June 2.45pm BST: US service sector PMI for July</t>
+          <t>David Cameron’s “bonfire of the quangos” decision to abolish England’s council spending watchdog has left a broken system that is costing taxpayers more money than it was promised to save. In a highly critical report, academics at the University of Sheffield said the coalition government of the Conservatives and Liberal Democrats had promised savings of £100m a year by abolishing the Audit Commission. However, replacing the public body with a private-sector model had resulted in “chaos” and soaring costs to audit councils amid the financial crisis hitting England’s town halls. Several councils have declared effective bankruptcy linked to years of austerity, soaring costs amid pressure on services, as well as local missteps. They include Birmingham, Nottingham and Woking. The Audit Reform Lab at Sheffield said the average cost of external auditors checking a local authority’s finances was now at least £50,000 higher in cash terms than when the Audit Commission was disbanded in 2015. Private-sector accountancy firms took over the job of auditing local government accounts in England after the agency was abolished, in an austerity-driven push by Tory and Lib Dem ministers to find savings and efficiencies. “Ten years on, however, it now seems clear that these reform ambitions have failed,” the authors of the report wrote. “Only 1% of audits were delivered on time in 2022-23, with many audits delayed by several years. Audit costs have risen dramatically in response. An unwieldy, but ultimately operational centralised bureaucracy was replaced by market chaos. The £100m per annum savings heralded by the UK government in 2014 are now a distant memory.” The report found that average audit costs in England had more than tripled – an average increase of 238% – in the year to 2023-24. It blamed most of this increase on private-sector auditors hiking their rates. It compared the large rise in audit costs in England to much smaller increases in Scotland and Wales, where it said there was a much stronger level of central oversight of private-sector auditing. Some of the biggest increases were at financially stricken councils, including a 620% rise in audit fees at Woking, as well as leaps of 470% at Runnymede and 450% at Spelthorne. In total 13 councils had fee scale increases of 300% or more in 2022-23. Birmingham city council paid an audit fee above the £1m mark, representing a 314% increase. The councils were approached for comment. Three auditors dominate the local audit market: EY, Grant Thornton and Forvis Mazars. Others including Deloitte and BDO have exited because profit margins are considered too low, while complexity and risks have risen. EY and Grant Thornton declined to comment. A spokesperson for Forvis Mazars said: “We are working closely with all stakeholders including MHCLG [Ministry of Housing, Communities and Local Government] and remain committed to supporting the return to the delivery of good quality audits for local authorities.” While audit costs have risen sharply, so has the complexity of checking council finances at a time when growing numbers of local authorities are running into severe financial difficulties. Experts have also long warned local audit fees have been too low to attract accountancy firms to do the job, compared with the money available in private-sector auditing. In 2020, an independent review by Sir Tony Redmond found fees were “at least 25% lower than required to fulfil current local audit requirements effectively”. The breakdown in local audit reached crisis point two years ago when only 1% of English councils had their 2022-23 accounts signed off in time. Ministers then allowed accounts to be completed with qualifications – whereby an auditor signs off but expresses reservations – to clear the backlog. A new Local Audit Office is also being established to centralise previously fragmented oversight of the process. An MHCLG spokesperson said: “We have taken decisive action to restore the broken audit system, providing £49m to help councils clear backlogs – but we know there is more to do. This is why we will set up a new Local Audit Office to simplify the system and increase capacity by establishing public sector audit provision. “This will ensure the local audit system provides accountability, transparency, and value for money for taxpayers.” Runnymede council said it was on a sound financial footing and did not recognise the fees quoted in the Audit Reform Lab report.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sales of new Tesla cars slumped by 59% year-on-year in the UK last month. Chinese carmakers led by BYD reported big jumps in UK sales. US service sector barely grew in July as Donald Trump’s trade wars pushed up costs, and led to job losses.</t>
+          <t>Academics at the University of Sheffield said the coalition government had promised savings of £100m a year by abolishing the Audit Commission. But replacing the public body with a private-sector model had resulted in ‘chaos’ and soaring costs to audit councils. Several councils have declared effective bankruptcy linked to years of austerity, soaring costs amid pressure on services.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Economic and Market Volatility</t>
+          <t>UK Economic Challenges Overview</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Time to wrap up… Analysts have welcomed a small fall in company insolvencies across England and Wales. The Insolvency Service has reported that there were 2,043 registered company insolvencies in England and Wales in June, 8% lower than in May 2025 (2,230) and 16% lower than in June 2024, when 2,430 companies failed. Donald Trump has claimed that Federal Reserve chair Jerome Powell was “truly one of my worst appointments,” and also criticised the Fed Board for not forcing rate cuts. Federal Reserve governor Christopher Waller has said he would accept the job as Fed chair if asked by President Donald Trump. G20 finance leaders have agreed a final communique on Friday that stressed the importance of central bank independence, saying: “Central banks are strongly committed to ensuring price stability, consistent with their respective mandates, and will continue to adjust their policies in a data-dependent manner. Central bank independence is crucial to achieving this goal.” Elsewhere… China has welcomed the US’s decision to allow Nvidia to ship its H20 AI chips England and Wales’ embattled water regulator Ofwat will be abolished under recommendations from a government-commissioned review due on Monday, the Guardian understands. US consumer sentiment has risen to a five-month high. Goodnight, and have a lovely weekend. GW Britain’s stock market has ended the week close to its record high. The FTSE 100 index has finished today’s session at 8992.12 points, up 19.5 points or 0.22%. That’s only a handful of points shy of Monday’s record closing high of 8998 points. Rentokil (+3%) and Antofagasta (+2.6%) led the risers. Mexico’s president Claudia Sheinbaum may not have got the memo about central bank independence….. The US dollar is closing out the week weaker as the fallout from the latest threat from President Trump to fire Fed Chair Powell lingers. The dollar index is down 0.45% today, while the pound is up 0.2% at $1.3443. Derek Halpenny and Lee Hardman of MUFG explain: We see this as more than just about whether Trump fires Powell. The comments from Fed Governor Waller indicate potential political influence with his comments much more explicit in calling for a July rate cut than in the past (see here). Governor Bowman is also open to cutting in July. Is Trump’s influence already playing a role? That’s key given Trump likely has two more picks for Governors next year (to replace Kugler and Powell – we assume he will leave although technically he doesn’t have to). Consumer confidence across the US has inched up this month, according to the latest data. The University of Michigan consumer sentiment index has risen to 61.8 points in July, up from 60.7 in june, lifted by an improvement in people’s economic conditions and consumer expectations. That’s its highest reading in five months, since the early days of Donald Trump’s trade war. Surveys of Consumers director Joanne Hsu points out, though, that sentiment remains a substantial 16% below December 2024 and is well below its historical average. Hsu adds: Consumers are unlikely to regain their confidence in the economy unless they feel assured that inflation is unlikely to worsen, for example if trade policy stabilizes for the foreseeable future. At this time, the interviews reveal little evidence that other policy developments, including the recent passage of the tax and spending bill, moved the needle much on consumer sentiment. Thomas Ryan, North America economist at Capital Economics, says: The small rise in the University of Michigan consumer sentiment index in July and further drop-back in inflation expectations shows that, while overall confidence remains weak, households are less worried than they were about how Trump’s policies might hit the economy, their finances, and purchasing power. British travellers to the EU will likely have to pay a €20 visa-waiver charge to enter the European Union from 2026, in a near-tripling of the original fee, my colleague Jennifer Rankin in Brussels reports. The €20 fee represents a nearly three-fold increase on the original €7 fee. It is expected to raise €2bn in revenues, although part of this sum will pay for operating costs. The European commission published plans for a €2 trillion budget for 2028-34 earlier this week, with proposed taxes on big companies, e-waste and tobacco. Buried in the small print, the commission also suggests “additional other revenue” could be generated by adjusting fees for the European Travel Information and Authorisation scheme, the EU equivalent to the US Esta. The ETIAS €7 fee was agreed in 2018, but the commission said that inflation and additional operational costs meant “the fee will be adjusted to €20 per application”. The higher fee becomes law, unless EU member states and the European parliament raise objections in the next two months. The €20 fee will apply to nationals from dozens of countries, including Ukraine, Canada, the United States, Brazil and Japan. The visa-waiver status will last for three years, or the expiry of a passport. Travellers will have to pay the fee from the final quarter of 2026 when Etias comes into force. British citizens who live in the EU with status guaranteed under the Brexit withdrawal agreement will be exempt, as will children and people aged over 70 when they made the application. A top official at the International Monetary Fund has warned that “high levels of policy uncertainty” remained a key theme at the meeting of G20 finance ministers in Durban this week. Gita Gopinath, the IMF’s First Deputy Managing Director, says economic indicators have reflected a complex backdrop shaped by trade tensions since April (when the Fund released its latest forecasts, and Donald Trump announced his ‘Liberation Day’ tariffs). Gopinath says: We have seen strong evidence of front-loading ahead of tariff increases and some trade diversion. We have also seen an improvement in global financial conditions as select trade deals lowered average tariffs. On inflation, cooling demand and falling energy prices point to a continued decline, albeit with variation across countries. And on Financial Sector issues, Gopinath warned of risks and urged close monitoring of non-bank financial institutions (NBFIs) (such as investment funds, insurance companies, pension funds and other financial intermediaries). Even though financial conditions have eased since April, with trade and geopolitical uncertainty still elevated, financial stability risks remain in focus. Asset valuations are once again stretched, the use of leverage remains high in parts of the financial system, and periodic pressure observed on government bond yields and market functioning carries the risk of broad repercussions, particularly against a backdrop of large fiscal deficits and increased illiquidity. Vigilant surveillance and robust supervision remain paramount and recent progress in financial sector oversight must continue, particularly for NBFIs which now account for more than 50 percent of the financial sector Shares in Netflix have dropped in early trading, after its results last night. Netflix raised its full-year revenue outlook yesterday, and reported $11bn revenue for the quarter to the end of June, a 16% year-on-year increase. But traders may have hoped for more – Netflix’s shares are down 4.7% in early trading. The company also revealed overnight that it had used artificial intelligence in one of its TV shows for the first time, by including generative AI footage in its Argentinian science fiction series El Eternauta (The Eternaut). Wall Street has opened higher, as investors weigh up the chances of early cuts to US interest rates. The Dow Jones Industrial Average rose 54.46 points, or 0.13%, at the start of trading to 44,542.97. The broader S&amp;amp;P 500 index gained 0.23% while the Nasdaq Composite is up 0.34%. News is emerging from Durban that G20 finance leaders have agreed a final communique on Friday that stressed the importance of central bank independence. That’s a timely reminder to Donald Trump of the dangers of undermining the Federal Reserve, as he continues to throw insults their way. The communique says: “Central banks are strongly committed to ensuring price stability, consistent with their respective mandates, and will continue to adjust their policies in a data-dependent manner. Central bank independence is crucial to achieving this goal.” The G20 also “recognise the importance of the world trade organisation to advance trade issues”, and say they are “committed to international policy cooperation to further promote global prosperity”. But they also warn that the global economy is facing “heightened uncertainty and complex challenges”. Hello hello….Federal Reserve governor Christopher Waller has said he would accept the job as Fed chair if asked by President Donald Trump. Waller made the comments today, just hours after throwing his weight behind calls for a rate cut this month (see earlier post). According to Reuters, Waller said: “In 2019 the president contacted me and said, ‘Would you serve?’ And I said yes. “If the president contacted me and said, ‘I want you to serve,’ I would do it. But he has not contacted me.” Big news in the water industry: England and Wales’ embattled water regulator will be abolished under recommendations from a government-commissioned review due on Monday, the Guardian understands. Ministers will next week announce a consultation into creating a new regulator, to coincide with the results of a review into the water industry directed by former Bank of England deputy governor Sir Jon Cunliffe. This consultation is likely to conclude in the abolishment of Ofwat, the embattled watchdog that polices how much water companies can charge for their services in England and Wales, sources said. Ofwat has faced intense criticism over its failure to prevent sewage spills, hefty payment of dividends and ballooning debts across England and Wales’s water companies. The review will recommend the creation of new regulatory system. More here. Back in the City, fashion group Burberry is one of the best performers on the London stock market today, after slowing its decline in sales. Surprisingly, demand for Burberry wellies, scarves and light jackets to wear at music festivals have helped the fashion brand to its best sales performance in 18 months, my colleague Sarah Butler reports. Sales of the luxury British brand fell by 2% to £433m in the three months to the end of June, with a 1% decline at established stores, an improvement from the 6% fall in the previous quarter and the best performance since Christmas 2023. Shares in Burberry are up almost 5%, making it one of the top risers on the FTSE 250 share index. One member of the Federal Reserve board, Christopher Waller, should be in president Trump’s good books, though. Last night, Waller argued that the Fed should cut rates by the end of this month, and cited growing risks to the economy and (he argued) limited inflationary risks from trade tariffs. Waller told a gathering of Money Marketeers of New York University: I believe it makes sense to cut the FOMC’s policy rate by 25 basis points two weeks from now. And looking to later this year, if, as I expect, underlying inflation remains in check—with headline inflation data reporting modest, temporary increases from tariffs that are not unanchoring inflation expectations—and the economy continues to grow slowly, I would support further 25 basis point cuts to move monetary policy toward neutral. The Fed’s next two-day meeting starts on 29 July, with a decision scheduled for the 30th. Brad Bechtel of investment bank Jefferies says Waller’s speech is getting some attention, explaining: Waller not typically a politically motivated character on the Fed, so his strong view on this matter is important in that context. His main arguments are that 1) tariffs are a one-off price increase and not a consistent impact to inflation, 2) GDP is below trend and a little too soft, arguing for rates closer to neutral, 3) employment looks fine on the surface, but downside risks have increased and private sector payroll growth is near ‘stall speed’. He therefore thinks we should cut rates by a quarter this month. Pretty strong view from Waller as the Fed gets close to entering their blackout period before the next meeting. Donald Trump has just declared that choosing Jerome Powell in 2017 to run the US Federal Reserve was one of his “worst” decisions, calling America’s top central banker a “numbskull” for not lowering borrowing costs. Trump blames president Biden, who he dubs “Sleepy Joe”, for renominating Powell in 2021, and also blasts the Fed’s board for not lowering rates. Posting on his Truth Social site, Trump again refers to Powell as “Too Late”, and again claims that US interest rates (currently a 4.25%-4.5% range) should be considerable lower, at just 1% (!). Trump writes: “Too Late,” and the Fed, are choking out the housing market with their high rate, making it difficult for people, especially the young, to buy a house. He is truly one of my worst appointments. Sleepy Joe saw how bad he was and reappointed him anyway - And the Fed Board has done nothing to stop this “numbskull” from hurting so many people. In many ways the Board is equally to blame! The USA is Rockin’, there is VERY LOW INFLATION, and we deserve to be at 1%, saving One Trillion Dollars a year on Interest Costs. I can’t tell you how dumb Too Late is - So bad for our Country! Stock markets wobbled earlier this week following reports that Trump was preparing to fire Powell, but recovered when the president denied it. The Fed’s board makes up a majority on the FOMC committee which vote to set US interest rates. The FOMC have voted to leave interest rates on hold so far this year, partly due to concerns that Trump’s trade war will be inflationary. The Insolvency Service has also reported that 10,279 individuals entered insolvency in England and Wales last month. This was similar to the numbers in both May 2025 and June 2024. They explain: The individual insolvencies consisted of 596 bankruptcies, 4,135 debt relief orders (DROs) and 5,548 individual voluntary arrangements (IVAs). The number of DROs in June 2025 was close to the record monthly high seen in June 2024. IVA numbers in the first six months of 2025 were similar to the monthly average in 2024. Bankruptcy numbers remained at about half of pre-2020 levels and were also 10% lower than in June 2024. Shares in Sweden’s fighter jet maker Saab have jumped 12% this morning, after the company announced strong sales growth amid the rush to spend more on defence. Saab reported organic sales growth of 32% in the last quarter, driven by strong growth in small and medium-sized orders. Micael Johansson, president and CEO of Saab, says: “We are strengthening our market position and see a continued large interest in our products and solutions. Saab’s sales growth is high and we continue to invest to build capacity and meet long-term strong demand from the defence sector. At the same time, we continue to deliver strong profitability.” Risk advisory firm Kroll point out that 2025 has been challenging for many businesses, including in leisure and retail. Benjamin Wiles, head of UK restructuring at Kroll: “There’s no doubt that 2025 has been a tough year for businesses so far, particularly those in the retail and leisure industry. Yet, the overall decline in company administrations compared to this period last year shows a level of resilience that shouldn’t be overlooked. We saw a lot of restructuring activity at the end of last year with many companies looking to get ahead of cost pressures and there is still a lot of capital available to borrow. “The question we are asking is whether businesses are fundamentally stronger or are they simply treading water. The second half of the year will be critical in determining whether this resilience can be sustained or if further pressures will tip more companies into distress.” Kroll also produced this table, based on their internal data, which tracks administrations throughout the year. Yesterday’s UK unemployment data showed that more than half the fall in payroll numbers over the last year was due to job losses in accommodation and food services. The recent hot weather may have helped some hospitality firms and retailers avoid collapse, suggests Jennifer Lockhart, partner and insolvency specialist at purpose-led independent law firm Brabners. Lockhart says: A fall in insolvencies is welcome and reflects the positive impact that the warmer summer months can have on business performance – especially in the retail, construction and hospitality sectors that have borne the brunt of failures to date. However, amid these soaring temperatures it’s important to recognise that this likely represents a period of reprieve for businesses, rather than a turning point. “Consumer confidence remains fragile, and the one-two punch of contracting GDP in May and growing inflation in June will do little to assuage concerns over what the next six months will hold for struggling businesses. Indeed, with many industries dialing back hiring plans – in part due to the influence of employment taxes and the impact of AI – the much-needed uptick in consumer demand is unlikely to materialize, putting more firms at risk.” Businesses are still in “tough” times, despite the drop in insolvencies in June, cautions David Hudson, restructuring advisory partner at FRP. Hudson says: “The slight fall in insolvencies this month offers a glimmer of relief – especially for hospitality and retail businesses, which are now reaping the benefits of record hot weather. However, we’re still in tough territory. Consumer confidence remains stubbornly low, growth is stuttering – with GDP dipping again in May. June’s unexpected jump in inflation will only serve to continue eroding profit margins and consumer demand. “This environment is forcing businesses to fight on multiple fronts. Many will likely only be experiencing breathing space after dramatically paring back costs. Until demand shows a more sustained recovery and input costs ease further, there’s a risk that this reprieve is just a pause rather than a turning point.” Just in: the number of companies in England and Wales falling into insolvency dropped last month. The Insolvency Service has reported that there were 2,043 registered company insolvencies in England and Wales in June, 8% lower than in May 2025 (2,230) and 16% lower than in June 2024, when 2,430 companies failed. That could ease some concerns over the health of the UK economy, as companies tackle rising inflation and higher taxes. Despite the drop, monthly company insolvency numbers in the first six months of 2025 were slightly higher than the second half of 2024, but remain lower than the 30-year annual high seen in 2023. The Insolvency Service says: Company insolvencies in June 2025 consisted of 332 compulsory liquidations, 1,585 creditors’ voluntary liquidations (CVLs), 111 administrations and 15 company voluntary arrangements (CVAs). There were no receivership appointments. Goldman Sachs has predicted the Bank of England will take a slightly slower approach to cutting interest rates, following this week’s data. Goldman still expect a rate cut in August (from 4.25% to 4%), even though inflation rose in June and private sector pay growth in March-May was higher than expected. But they have now dropped their forecast for a September cut. Sven Jari Stehn, Goldman’s chief European economist, told clients: While the hurdle for speeding up cuts in September looks higher after this week’s data, we now expect sequential cuts from November until reaching a 3% terminal rate in March 2026 (versus February before). That is, we now expect a total of five cuts this year (previously six) and two next year (previously one). That would mean rate cuts in August, November and December this year, and February and March 2026. The Bank has already cut rates twice this year, at its meetings in February and May. Shares in pharmaceuticals firm GSK have dropped over 6% in early trading, after its blood cancer drug Blenrep hit a regulatory hurdle in the US. Yesterday, the US FDA’s panel of independent advisers recommended against Blenrep, citing earlier concerns over eye-related side effects. GSK told the City that it remains confident in the benefit/risk profile of Blenrep and said it will continue to work closely with the FDA as they complete their review of the drug. The final decision on whether to approve a drug rests with the FDA, which will consider the view of its Oncologic Drugs Advisory Committee (ODAC), which voted 5-3 against Blenrep. The company added that Blenrep combinations are approved for refractory multiple myeloma (cancer that does not respond to treatment) in several markets including the UK and Japan, and that applications in other markets including the EU and China are being reviewed. The European Union has announced the approval of a fresh sanctions package on Russia over its war against Ukraine, which includes a revised oil price cap and new banking restrictions. EU member states gave the package the green light this morning after Slovakia lifted its veto. Kaja Kallas, the EU’s High Representative for Foreign Affairs and Security Policy, says the sanctions package – the EU’s 18th – is one of the strongest put together against Russia so far. It includes a ban on more Russian banks accessing the SWIFT international payments system, sanctions on the Nord Stream gas pipelines, and a lower cap on Russian oil sales. Diplomat have told Reuters that the package will lower the G7’s price cap for crude oil to $47.6 per barrel. Bloomberg reports that the new price cap, which is currently set at $60 per barrel, will now be set “dynamically” at $15 below market rates. This follows criticism that Europe has been spending tens of billion on Russian energy since the Ukraine war began, exceeding the cost of it support for Kviv. Energy news: BP has continued its push to pivot back to oil and gas, by agreeing a deal to sell its US onshore wind business to LS Power. The wind business operates nine onshore wind energy assets across seven US states, and are grid-connected and are providing power to customers. William Lin, bp’s executive vice president for gas &amp;amp; low carbon energy, says: “We have been clear that while low carbon energy has a role to play in a simpler, more focused bp, we will continue to rationalize and optimize our portfolio to generate value. The onshore US wind business has great assets and fantastic people, but we have concluded we are no longer the best owners to take it forward. The price of the deal hasn’t been revealed; BP says it is part of its $20bn divestment program to simplify and focus its business. In the City of London, consumer goods maker Reckitt Benckiser has agreed to sell a majority stake in its Cillit Bang and Calgon arm to private equity firm Advent International. The deal is worth up to £3.6bn, and will see Reckitt retain a 30% stake in the essential home business - also including brands such as Air Wick, Woolite, Resolve, Sole and Easy-Off Kris Licht, Reckitt’s chief executive, says: “We are executing our strategic plan at pace. The divestment of Essential Home represents a significant step forward in unlocking the substantial value in our business. This moves Reckitt towards becoming a simpler, more effective world-class consumer health and hygiene company and it will enable us to focus on a core portfolio of high-growth, high-margin powerbrands.” Shares in Reckitt have risen 1.5% at the start of trading, putting it among the FTSE 100 top risers. Katsunobu Kato’s criticism of US tariffs come after Japan’s exports to the United States fell for the third straight month. Data released on Thursday showed that the value of shipments fell 11.4 percent in yen terms in June, compared with the same month last year. The car sector was hit hard, with exports were down 26.7%. The number of vehicles was up, but their average price was down nearly 30%. That could be a sign that automakers are cutting prices or shipping cheaper models to offset the tariffs. Donald Trump’s trade war has loomed over the meeting of G20 finance ministers in South Africa this week. Japan told the gathering of advanced economies in Durban that tariffs aren’t the right way to fix trade imbalances. Finance minister Katsunobu Kato told reporters at the G20: “Japan said that tariffs aren’t really the right tool to fix excessive current accounts imbalances.” Kato argued that countries facing such situations need to address them through domestic efforts, rather than slapping new levies on imports. The US’s trade balance (rarely the healthiest) has actually worsened this year, as American companies raced to import goods before tariffs were imposed. However, US Treasury secretary Scott Bessent won’t have heard Kato’s message as he’s not attending the G20. A finance ministry official accompanying Kato explained that many G20 members argued that market stresses appear to have eased somewhat, Bloomberg reports, as the world economy hasn’t suffered as much as expected from the trade war [although, of course, some of Trump’s new tariffs now don’t start until 1 August]. Good morning and welcome to our rolling coverage of business, the financial markets and the world economy. Relations between the US and China appear to have warmed, slightly, after chipmaker Nvidia was given a green light by Washington to resume sales of its H20 AI chip to Chinese companies. Nvidia’s CEO, Jensen Huang, revealed earlier this week that the US government has assured his company that licences for H20 chip sales to China would be granted, and that deliveries could start soon. That reverses a restriction announced in April, when the White House announced tighter controls on exports of computer chips used for artificial intelligence. And today, Beijing has welcomed this change of heart, confirming that the US has ‘taken initiatives” to approve H20 sales to China again. China’s Commerce Ministry said in a statement that “win-win cooperation” was the right path to go down, and that it hopes the two countries can “meet each other half way” and work together. The ministry also urged the US to abandon its “zero-sum mentality” and cancel ‘unreasonable’ trade restrictions on China, warning that “suppression” will not lead to solutions. The H20 graphics processing unit, or GPU, is an advanced chip for use in AI systems. But it’s less powerful than Nvidia’s top semiconductors today, as it was designed to comply with US restrictions for exports of AI chips to China. Earlier this week, commerce secretary Howard Lutnick revealed that the renewed sale of H20 chips to China was linked to a rare earths magnet deal. He also claimed Nvidia would only be selling China its “fourth best” chip. Even so, the prospect of more sales to China pushed Nvidia’s shares to record highs this week. Orders from Chinese companies for H20 chips need to be sent by Nvidia to the U.S. government for approval. The agenda 9.30am BST: UK insolvency data 10am BST: Eurozone construction output data for May 1.30pm BST: US housing starts data for June 3pm BST: University of Michigan consumer confidence report</t>
+          <t>The bosses of Britain’s largest listed companies took home record high pay packets for the third successive year, according to a report. Analysis found that the record set in the last financial year means the average FTSE 100 chief executive is now paid 122 times the salary of the average full-time UK worker. Executive pay has been on the rise for the past four years, partly as a consequence of pay cuts taken during the pandemic, at a time when many households are still struggling with a cost of living crisis. The median pay of a FTSE chief executive climbed to £4.58m in the last financial year, up from £4.29m a year earlier, an increase of nearly 7%, according to analysis by the High Pay Centre. The thinktank report also shows FTSE 100 companies spent more than £1bn on pay during the last financial year, handed out to just 217 executives, representing an almost quarter of a billion pound increase from the same period a year earlier, when executive pay totalled £757m. Luke Hildyard, the director of the High Pay Centre, said: “These figures will feed a growing sense that low and middle earners don’t get a fair share of the wealth that their work helps to create, while those at the top take much more than they merit or need.” Much of the rise reflects pay awards at the UK engineering firm Melrose Industries, which was accused of “robber baron capitalism” after it bought the aerospace and automotive group GKN for £8bn in a hostile takeover in 2018. Its executives were paid a total of £212m, according to the analysis. The High Pay Centre, which campaigns for fairer pay, found that the highest paid chief executives were the current and former boss of Melrose, Peter Dilnot and Simon Peckham respectively, who between them took home nearly £59m for the last financial year, mostly thanks to long-term incentive payments. Melrose sparked outrage last June by handing out a reward pot worth more than £175m to 21 current and former executives in shares under a bonus scheme set up in 2020. The lion’s share was received by Peckham, one of the business’s co-founders, along with the company’s former chair Christopher Miller and the former finance director Geoffrey Martin. The use of long-term incentive payments (LTIPs) by large listed companies rose in the last financial year, with 84 out of 100 chief executives paid an LTIP in the last financial year, compared with 81% a year earlier. Pascal Soriot, the chief executive of pharmaceutical company AstraZeneca, who spent the last two years as the FTSE 100’s highest paid boss, was pushed into third place in the last financial year after earning £14.7m. Soriot is now ranked behind the Melrose executives as well as the current and former bosses of the education publisher Pearson on the High Pay Centre’s league table. Andy Bird and his successor as Pearson’s chief executive, Omar Abbosh, together earned almost £19m in the last financial year. The number of FTSE 100 companies paying their leaders £10m or more increased in the past year, rising from 10 to 13, at a time when Britain’s cash-strapped households continue to feel the squeeze of the cost of living crisis, and the Bank of England has warned that rising food prices could fuel further inflation. The figures also revealed a gender pay gap at the top of corporate Britain, as female leaders of the largest listed companies still tend to earn less than their male counterparts. For the nine companies that had a female leader for the entire financial year, median chief executive pay was £3.27m, compared with £4.64m for companies run for the entire year by a man. The High Pay Centre believes that what it calls “excessive spending” on top earnings by large listed companies often comes at the expense of pay increases for the rest of the workforce. The High Pay Centre is calling for reforms to regulations governing the pay-setting process followed by corporates, including the full implementation of Labour’s employment rights bill, which includes measures that workers are informed by their employers of their trade union rights. In addition, the group is calling for more workers to have the power to elect directors to company boards, as well as the reform of corporate reporting on pay, through clearer information being set out in businesses’ annual reports. “The government now needs to make sure these measures are implemented in full, and supplemented by a real voice for elected worker directors in company boardrooms,” Hildyard said.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>There were 2,043 registered company insolvencies in England and Wales in June. That is 8% lower than in May 2025 (2,230) and 16% less than in June 2024. Consumer confidence across the US has inched up this month, according to the latest data.</t>
+          <t>The average FTSE 100 chief executive is now paid 122 times the salary of the average full-time UK worker. Executive pay has been on the rise for the past four years, partly as a consequence of pay cuts taken during the pandemic. Much of the rise reflects pay awards at the UK engineering firm Melrose Industries.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Economic and Market Volatility</t>
+          <t>UK Economic Challenges Overview</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Barclays has been fined £42m over “poor handling” of financial crime risks linked to two clients, including a gold bullion business run by James Stunt, the former son-in-law of Formula One tycoon Bernie Ecclestone. The Financial Conduct Authority (FCA) said the bulk of the penalties, about £39.3m, related to Barclays’ failure to properly screen Stunt’s business – Stunt &amp;amp; Co – and its relationship with Fowler Oldfield, a Bradford jeweller now infamously linked to a large money-laundering operation. The failures spanned 2015 to 2021, and Stunt &amp;amp; Co ultimately received £46.8m from Fowler Oldfield. Barclays was made aware of the fact that Fowler Oldfield was the subject of a criminal investigation involving potential money laundering in August 2016. But the bank only started to review its exposure to the company five years later, when a court fined NatWest more than £264m over its relationship with the purported jeweller, in a case brought by the FCA. The case gained widespread press attention, given the extraordinary details, including that staff had been depositing “big black bin liners” full of cash at a NatWest branch that overwhelmed its floor-to-ceiling safes. The FCA said on Wednesday that Barclays “did not gather enough information at the start of the relationship or carry out proper ongoing monitoring”. In March, two directors for Fowler Oldfield were convicted of money laundering and sentenced to more than a decade in prison each. Stunt was cleared at Leeds crown court of any money-laundering charges in relations to funds received from the purported jeweller. Barclays was also fined £3.1m on Wednesday for failing to check it had enough information to understand the money-laundering risk before opening a client money account for the now-collapsed wealth management firm WealthTek. The FCA in December charged WealthTek’s former head partner John Dance with fraud and laundering more than £64m from the firm’s client accounts. Dance is due to face a criminal trial at Southwark crown court in September 2027. Commenting on the fines, the FCA’s joint executive director of enforcement and market oversight, Therese Chambers, said: “The consequences of poor financial crime controls are very real – they allow criminals to launder the proceeds of their crimes, and they allow fraudsters to defraud consumers. “Banks need to take responsibility and act promptly, particularly when obvious risks are brought to their attention. In the first of these cases, Barclays secured a significant reduction in its fine through its extensive cooperation with our investigation and through making a voluntary payment to affected consumers at our request.” Barclays said the bank remained “deeply committed to the fight against financial crime and fraud”. It added: “The FCA’s investigation relating to Stunt &amp;amp; Co was centred around historical money-laundering activity and made no findings that the bank had breached money-laundering regulations. “As acknowledged by the FCA, Barclays undertook an extensive review and self-reported its findings to the FCA. Barclays fully cooperated with both investigations and has further strengthened its financial crime and other control capabilities.” • This article was amended on 17 July 2025. It was a court that fined NatWest more than £264m, not the FCA; however, the case was prosecuted by the FCA.</t>
+          <t>Time to wrap up… Donald Trump will announce tariffs on imports of semiconductors and steel in the coming weeks, he told reporters aboard Air Force One while travelling to Alaska for his meeting with Vladimir Putin. The US president said: I’ll be setting tariffs next week and the week after on steel and on, I would say, chips…I’m going to have a rate that is going to be lower at the beginning - that gives them a chance to come in and build - and very high after a certain period of time. Shares in Intel jumped by as much as 8.9% in early trading on Friday, also boosted by a report that the Trump administration is considering taking a stake in the chipmaker. Meanwhile in the UK, the FTSE 100 briefly surpassed its intraday high this morning, although it is now trading down 0.3% at 9,150.90 points. The owner of Kingsmill also agreed to buy its rival bakery business Hovis today, in a deal that could make the biggest bread brand in the country if it gets the green light from regulators. Elsewhere Shein, the online fast-fashion retailer founded in China, increased sales in the UK by about a third to more than £2bn last year, overtaking the British rival Boohoo and closing in on Asos. It is a slow open for Wall Street, with the blue chip S&amp;amp;P 500 index slipping by 0.1% in early trading. It hit an all-time high earlier this week. The Dow Jones Industrial Average, another key US stock index, also hit an all-time intraday high, briefly surpassing its previous peak of 45,073.63 points. It was helped by a big jump in UnitedHealth Group shares, which are up by more than 9%, after it emerged that Warren Buffett’s Berkshire Hathaway has invested in the insurer. The Dow is now at 45,076.20 points. Donald Trump will announce tariffs on imports of semiconductors and steel in the coming weeks, he told reporters aboard Air Force One while travelling to Alaska for his meeting with Vladimir Putin. The US president said: I’ll be setting tariffs next week and the week after on steel and on, I would say, chips…I’m going to have a rate that is going to be lower at the beginning - that gives them a chance to come in and build - and very high after a certain period of time. Last week the president threatened a 100% tariff on imported semiconductors and chips, which could favour US-based companies such as Intel. Shares in Intel jumped by as much as 8.9% in early trading on Friday, also boosted by a report that the Trump administration is considering taking a stake in the chipmaker. US retail sales rose in July, up 0.5%, slowing from a 0.9% gain in June, official data shows. Retail spending was helped by strong demand for cars, as well as promotional campaigns from Walmart and Amazon’s extended Prime Day. Excluding cars, sales in the period were up by just 0.3%, according to the US Commerce Department’s Census Bureau. Traders are starting to trim back their bets that the US central bank, the Federal Reserve, will cut interest rates next month. The probability of a quarter-point reduction has fallen from 94% to about 89%, per Reuters. It is the biggest reunion in British music in decades, with fans expected to splash out more than £1bn on the Oasis comeback. But for economists it presents a difficult question: how do you factor the Gallagher brothers into the UK’s inflation figures? The Office for National Statistics will not be including Oasis ticket prices in their basket of goods for inflation, according to Morgan Stanley, as it “excludes big-name bands with highly distinctive and unique abilities to charge diverse prices.” But fans flocking to hotels and driving up prices could have a big impact on the inflation reading for July, analysts believe. Analysts at Deutsche Bank expect the headline consumer price index rate rate for July will be 3.8% year on year, while Morgan Stanley has forecast a rate of 3.7%. It is not the first time that superstar tours have moved the dial on crucial economic data. In June 2023, economists blamed Beyoncé’s concert in Stockholm for unexpectedly high Swedish inflation. The ONS is scheduled to report the inflation figure for July on Wednesday 20 August. The FTSE 100 has pulled back from its intraday high, and is up now by just 0.1% to 9,186.59. The FTSE 250 mid-cap index is performing better, up 0.4%. Its best performer is Bytes Technology Group, which announced a £25m share buyback programme this morning. Shares in the IT reseller are up 7%. Shein, the online fast-fashion retailer founded in China, increased sales in the UK by almost a third to more than £2bn last year, overtaking the British rival Boohoo and closing in on Asos. The company, which had been considering a £50bn float on the London Stock Exchange but is now expected to list in Hong Kong, said profits rose 56% to £38.2m last year on which it paid £9.6m corporation tax, according to accounts filed at Companies House this week. Shein, which mainly sells fashion but has also moved into other products including toys and beauty, said it had benefited from the opening of two new offices in King’s Cross and Manchester, the launch of a pop-up shop in Liverpool and a Christmas bus tour across 12 cities in the UK. Oil prices are edging lower this morning ahead of a meeting between US President Donald Trump and Russian leader Vladimir Putin later today in Alaska. Brent crude futures fell by as much as 0.8% to $66.34 a barrel this morning, while US West Texas Intermediate crude futures fell by as much as 0.9% to $63.39. Giovanni Staunovo, commodity analyst at UBS, told Reuters: The market is watching out for whether there is a ceasefire or not. An expectation of a ceasefire translates into more Russian production…The question is will there be escalation or de-escalation?” A potential deal could significantly lower geopolitical risk in the oil market. Analysts at the investment bank Citigroup said this month that a deal to end the war in Ukraine could push Brent crude to the low $60s range by the end of the year. Recent weak economic data from China has also hurt the outlook for fuel demand. Shares in Intel have jumped 7.4% after it was reported that the Trump administration is considering taking a stake in the struggling US chipmaker. The potential investment, which would be paid for by the US government, would be used to develop Intel’s factory hub in Ohio, according to Bloomberg. It would also help shore up the chipmaker’s finances at a time when Intel has been slashing jobs as part of a wider cost-cutting drive. Talks over the potential investment stem from a meeting that took place between Donald Trump, and the Intel chief executive, Lip-Bu Tan, this week, days after Trump called for Tan to resign, accusing him of having ties to the Chinese Communist party. Bloomberg suggested Tan was likely to stay in charge of the chipmaker. Elsewhere in Europe, estimates suggest that economic growth in Switzerland slowed sharply in the second quarter. Switzerland has estimated that its economy grew by just 0.1% quarter-on-quarter in the three months ended in June, down from 0.8% in the prior period. It comes as Trump hits Switzerland with one of the highest tariff rates in the world, at 39%. Melanie Debono, a senior economist at Pantheon Macroeconomics, said “luck is running out for the Swiss economy”. We think the Swiss economy will enter a short, shallow recession in H2 as the rise in US trade tariffs (to a whopping 39% for most goods) hits exports, while trade uncertainty more widely hurts investment. We currently expect GDP to fall by 0.3% quarter-to-quarter in both Q3 and Q4. Barring any revisions, this would mean that GDP in Switzerland will have risen by 1.3% this year, a touch more than the 1.0% recorded in 2024. Swiss companies, whose exports to the US account for about one-sixth of their total foreign sales, face one of the steepest US tariffs in the world – only Laos, Myanmar and Syria had higher figures, at 40-41%. The blue chip FTSE 100 index has hit another record this morning, rising by as much as 0.4% to 9,222.07, its highest point since the end of July. It has pared back some of these gains, now up by around 0.1% 9,188.67, although it is still trading ahead of the high it set at the close yesterday of 9,177.24. Axel Rudolph, senior technical analyst at the broker IG, says: The FTSE 100 has joined the global push to fresh record highs, buoyed by improved risk appetite, supportive global trends and strong corporate earnings. With investors drawing confidence from a friendlier interest rate outlook and resilient corporate earnings, the UK benchmark has finally broken through its previous ceiling. With a stellar over 11% rise since the start of the year, it is outperforming peers such as the S&amp;amp;P 500 and Nikkei 225. The move underlines how global market momentum can lift all boats, even in the face of lingering domestic economic concerns.” London’s listed miners are leading the charge this morning, with Antofagasta, Glencore and Anglo American the top three risers across the index, up by 3.4%, 2.7% and 2.7% respectively. Meanwhile the Stoxx Europe 600 index rose by 0.3%, led by the Danish cable group NKT, whose shares are up by around 8% this morning. The Danish jewellery business Pandora is the worst performer, with its shares slumping 13% after it missed earning expectations for its second quarter. The owner of Kingsmill has agreed to buy its rival bakery business Hovis, in a deal that could make the biggest bread brand in the country if it gets the green light from regulators. Associated British Foods, a FTSE 100 company which also owns the retailer Primark, has agreed to buy Hovis from the private equity firm Endless. The deal between the second and third biggest bread brands in the country is expected to draw attention from the Competition and Markets Authority. Both companies have struggled recently against Warburtons, the biggest brand in the sector. Revenue at Hovis dropped almost 9% to £447m in the year to 28 September 2024, with pre-tax losses widening to £4.7m, compared with a loss of £3.6m the year prior. That included £530,000 in one-off costs, largely related to restructuring. ABF’s bakery division, Allied Bakeries (which includes Kingsmill, Allinson’s and Sunblest) made an annual loss about £30m despite sales of about £400m last year, according to analysts at the broker Panmure Liberum. ABF said the deal will combine the production and distribution activities of Allied Bakeries and Hovis, which would create cost savings and efficiencies, so it would turn into a “profitable UK bread business that is sustainable over the long term”. George Weston, ABF’s chief executive, said: This transaction will create a UK bakeries business that is both profitable and sustainable over the long term. Supporting the Hovis and Kingsmill brands with well-invested and efficient operations will also enable innovation and growth. This solution will create value for shareholders, provide greater choice for consumers and increase efficiencies for customers. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. New data suggest the Chinese economy slowed in July, as Donald Trump’s trade war began to bite at the second biggest economy in the world. Figures coming out of Beijing last night showed that Chinese industrial production rose at the slowest rate since November and expanded by 5.7% compared with the same point last year, worse than an expected 6%. Meanwhile Chinese retail sales grew by 3.7% year-on-year in July, its slowest pace so far this year and down from 4.8% the previous month. Yuhan Zhang, principal economist at The Conference Board’s China Center, said: Firms may be running on existing capacity rather than building new plants…The July industrial value-add breakdown tells a more nuanced story than the weak fixed asset investment headline. He pointed to China’s automobile manufacturing, railway, shipbuilding, aerospace and other transport equipment industries as “outliers (that) indicate policy-driven, high-tech and strategic sectors are still attracting substantial capital.” The Chinese CSI 300 stock index rose 0.8% after the release of the economic data, as it fed speculation that Beijing could introduce fresh stimulus in the market. Meanwhile in the UK, the FTSE 100 blue chip share index is set to end the week at a new record high. It is poised to rise by 0.5% when the market opens at 8:00AM, led by gains in the finance and defence sectors. The defence sector has been one of the best performers in London’s stock market, thanks to a wave of rearmament across much of Europe in the wake of the war in Ukraine. All eyes will be on Alaska later today, when Vladimir Putin is set to meet Donald Trump. The US president has said he believes the Russian leader is ready to make a deal on the Ukraine war. The agenda 8.00pm BST: Donald Trump and Vladimir Putin meet in Alaska</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Barclays has been fined £42m over 'poor handling' of financial crime risks. Bank failed to properly screen James Stunt's business and relationship with Fowler Oldfield, a Bradford jeweller now linked to a large money-laundering operation. Barclays was also fined £3.1m for failing to check it had enough information to understand the money- laundering risk.</t>
+          <t>Shares in Intel jumped by as much as 8.9% in early trading on Friday. FTSE 100 briefly surpassed its intraday high this morning, although it is now trading down 0.3% at 9,150.90 points. It is a slow open for Wall Street, with the blue chip S&amp;amp;P 500 index slipping by 0.1%.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Economic and Market Volatility</t>
+          <t>Trade War Impacts Markets</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>The UK’s financial watchdog is expanding bullying and harassment rules to more than 37,000 City firms, in an effort to crack down on “rolling bad apples” who avoid consequences by hopping from firm to firm. It means that “serious, substantiated cases of poor personal behaviour” by senior managers at a range of firms including hedge funds, insurers and pension firms will have to be reported to the Financial Conduct Authority (FCA), as well as future employers who are assessing whether new hires are fit and proper for the job. Previously, only banks were required to report bad behaviour to the watchdog. The rules will now apply to tens of thousands of other firms across the City that are bound by the so-called senior managers and certification regime (SM&amp;amp;CR) that is meant to hold senior bosses accountable for wrongdoing at their firms. The regulator said the expanded rules would help “prevent ‘rolling bad apples’ – people moving from firm to firm without appropriate action being taken or without past serious non-financial misconduct being disclosed”. Sarah Pritchard, the FCA’s deputy chief executive, said: “Too often when we see problems in the market, there are cultural failings in firms. Behaviour like bullying or harassment going unchallenged is one of the reddest flags – a culture where this occurs can raise questions about a firm’s decision-making and risk management. “Our new rules will help drive consistency across industry and support the vast majority of firms that want to do the right thing to deepen trust in financial services.” The expanded rules on non-financial misconduct, which also cover racism, sexual harassment and violence and intimidation, will come into force on 1 September 2026. However, they will not apply to payments and e-money firms, regulated investment exchanges or credit ratings agencies, none of which are subject to SM&amp;amp;CR rules. The FCA recently won a tribunal challenge brought by the former Barclays boss Jes Staley, with judges upholding a lifetime ban against the former chief executive for misleading the regulator over the nature of his relationship with the convicted child sexual abuse offender Jeffrey Epstein and their last point of contact. The new rules come despite the FCA and fellow regulators facing mounting pressure from the government to slash red tape for businesses.</t>
+          <t>Time to wrap up… River Island’s rescue restructure has received approval from a high court judge, a move which will help stop the fashion retailer from falling into administration. The plan received approval from a high court judge on Friday after the majority of creditors gave their backing to the plan earlier this week. The bidding battle for NHS landlord Assura also intensified today. Its US suitor KKR lobbied the board to accept its offer, while the competition watchdog stepped up its investigation of Assura’s £1.7bn takeover by a rival UK healthcare investor. Assura is still recommending that its shareholders accept the PHP offer. Meanwhile, the chief economist at the Bank of England has warned that “persistent inflation” could slow the pace of future interest rate cuts. Huw Pill is one of four members of the monetary policy committee who voted against the rate cut to 4% this week. Profits at Jaguar Land Rover slumped in its quarter ended in June, as the British luxury carmaker has grappled with US trade tariffs and a slowdown in sales. Underlying pre-tax profit dropped by 49% to £351m in the quarter, with revenue falling by 9% to £6.6bn, thanks partly to a temporary pause in exports to the US and the planned wind down of older Jaguar models before the launch of new electric models next year. JLR said US tariffs had a “direct and material impact on profitability and cash flow in the period”, but that the “US-UK trade deal will significantly reduce the financial impact of US tariffs going forward”. The car maker, which is owned by the Indian group Tata Motors, said last month that it would axe up to 500 management jobs in the UK, impacting 1.5% of its UK workforce. Chief executive Adrian Mardell said the results came amid “challenging global economic conditions”. We are grateful to the UK and US governments for delivering at speed the new UK-US trade deal, which will lessen the significant US tariff impact in subsequent quarters, as will, in due course, the EU-US trade deal announced on July 27.” River Island has secured approval for a restructure plan designed to stop the fashion retailer from falling into administration. The plan received approval from a high court judge on Friday after the majority of creditors gave their backing to the plan earlier this week. Ben Lewis, the retailer’s chief executive, said approval of the plan would enable the company to “align our store estate to our customers’ needs. We are pleased that River Island’s restructuring plan has been approved by the High Court. We have a clear transformation strategy to ensure the long-term viability of the business, and this decision gives us a strong platform to deliver this. Recent improvements in our fashion offer and shopping experience are starting to show results, and the restructuring plan will enable us to align our store estate to our customers’ needs.” You can read the full story by my colleague Sarah Butler here: Huw Pill, chief economist at the Bank of England and one of four members of the monetary policy committee who voted against the interest rate cut this week, has warned “persistent inflation” could slow the pace of future rate cuts. Pill said in an online presentation to businesses: There’s still a little bit further downward to go with Bank Rate. I think the pace at which those downward moves perhaps go forward is a little bit less clear than the pace that we’ve seen over the last year. On Thursday, the Bank of England’s monetary policy committee (MPC) voted to cut the base rate by a quarter point to 4%, its lowest level for more than two years. It was one of the closest decisions since its independence more than 25 years ago, with the vote split 5-4. Pill was one of the MPC members who voted to keep rates unchanged. The latest official figures show that inflation rose to 3.6% in June, ahead of the Bank’s 2% target. Pill said: There is some shift in the balance of risks on inflation. There is a risk of spillover into more persistent inflation. When inflation is high due to external forces, we need to be aware of the risk they might affect domestic price-setting. …Our mandate is that we will get inflation to 2%, that’s the target, on a sustainable rate. We will do whatever we need with the Bank rate to do that. They may be a bit lower than where we are but nothing is set. On Thursday, the Bank warned that rising food prices could dirve to inflation to 4% in September. The Competition and Markets Authority (CMA) has cleared Boeing’s $4.7bn (£3.5bn) deal to buy Spirit AeroSystems, the parts supplier it spun out nearly 20 years ago. The US plane manufacturer agreed to buy Spirit last year in an all-stock deal which valued it at $4.7bn. The total transaction value, including Spirit’s net debt, was $8.3bn. The CMA started to investigate the deal in June to determine whether it would affect competition in the UK. It has not yet released the full details behind its decision but it has said it has cleared the acquisition. The deal to bring Spirit back in-house marks a move away from Boeing outsourcing key components for its planes. Spirit was spun off from the business in 2005, but last year it still accounted for about 70% of all of its orders. Around 25% came from Boeing’s rival, Airbus. Turning to the world of healthcare, shares in the US pharmaceutical company Eli Lilly slumped by 14% last night, after disappointing results from its obesity pill. Eli Lilly said on Thursday that patients taking its pill orforglipron lost an average of 12.4% of their body weight, at the lower end of expectations. People taking a placebo lost 0.9%. Shares in rival Novo Nordisk, the Danish drugmaker behind the Ozempic and Wegovy weight-loss drugs, are up 4% this morning. Elsewhere in the sector, FTSE 100 pharmaceutical company GSK said this morning that it will receive $370m as part of a US patent settlement between CureVac and BioNTech related to its Covid-19 jab. It will also receive a 1% royalty on future US sales of influenza, Covid-19 and related combination mRNA vaccine products by BioNTech and Pfizer. Shares in GSK are up about 1% this morning There has been another twist in the attempted takeover of the NHS landlord Assura: this morning the competition watchdog blocked the full integration of Primary Health Properties (PHP) with Assura, as it investigates the £1.79 bllion deal. A bidding war for the company between PHP and the private equity firm KKR had been going on since February – but in June Assura’s board recommended a cash offer from PHP which valued it at £1.79bn. But the Competition and Markets Authority (CMA) launched the first stage of its investigation into the deal last month, and has now served an initial enforcement order on the firms. KKR still argues that its bid for Assura is superior to the offer from Primary Health. The firm said it had met with Assura in recent days to lobby for its own cash takeover of the company. Assura owns a property portfolio worth about £3.1bn, including a number of NHS buildings such as doctors’ surgeries. Oil prices are headed for their worst week since June, as investors prepare for the possibility of talks between Donald Trump and Vladimir Putin, and as the latest round of US tariffs weigh on the global economic outlook. Brent crude futures are on track to fall by around 4% this week, currently trading at $66.36. West Texas Intermediate crude futures are on track to fall by about 6% compared with last week. Analysts think this is largely because of the impact that Trump’s latest tariffs will have on the global economy. This week, more than 60 countries were hit by sweeping “reciprocal” rates, which range from 10% to 39%, 40% and 41% for Switzerland, Brazil and Syria. A widely expected meeting between the US president and the Russian leader is also affecting the market, with investors anticipating that eased sanctions on Russia could increase the oil supply. This week Trump increased tariffs on India, in a move he described as punishment for continuing to buy Russian oil. The UK’s blue chip FTSE 100 stock index has opened slightly higher this morning, up 0.26%. JD Sports is the strongest riser in the index, with its shares up 2.2%. It is followed by Glencore, with its shares up 1.9% after news this week that the miner decided to keep its primary listing in London, ditching a possible plan to move to New York. The mid-cap FTSE 250 index is not performing as well, down by about 0.1%. TBC Bank is the worst performer, with its shares falling by as much as 12% in early trading, though the Georgian bank reported a 5% rise in its profits for the second quarter, as well as a new buyback. Meanwhile, the pound is slipping against the US dollar this morning, even after the Bank of England’s monetary policy committee (MPC) voted to cut its key base rate by a quarter-point to 4% yesterday. The pound is down 0.13% against the dollar, although it is still above $1.34. While the Bank has cut rates, it was one of the closest decisions since its independence more than 25 years ago with a 5-4 vote split. The market has lowered its expectations of another quarter cut point this year, in contrast to growing expectations that the Federal Reserve will cut interest rates in the US next month. On Thursday, Donald Trump said he will nominate Stephen Miran to the Fed’s board of governors for four months, and reports suggest that current governor Christopher Waller is the favourite candidate to serve as the next Fed chair. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, says both men are viewed as dovish, which should align with Trump’s ambition for lower rates. However, the US 2-year yield has barely reacted—reminding us (again) that rate cuts don’t always lower borrowing costs if they aren’t seen as credible or justified. Remember last September, when the Fed unexpectedly slashed rates by 50bps? The 2-year yield jumped nearly 30bps over the following two months. For now, markets still expect the next cut to come in September, keeping the S&amp;amp;P 500 near record highs despite trade uncertainty and policy inconsistency. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Gold futures hit a record high on Friday after a Financial Times report that the United States has imposed tariffs on imports of one-kilo gold bars, a move that is expected to ramp up pressure on Switzerland, the biggest precious metal hubs in the world. The FT has seen a letter from the Customs Border Protection agency which said one-kilo and 100 ounce gold bars should be classified under a customs code subject to higher tariffs. One-kilo bars are the most popular form of the metal traded on Comex, the biggest gold futures market, and make up most of Switzerland’s bullion exports to the US. US gold futures rose by. 1.3% at $3,499.30, after hitting an all-time high of $3,534.10. Meanwhile, the price spread between New York futures and spot prices widened by about $100. It marks another blow for Switzerland, which Donald Trump has hit with a shock 39% export tariff. Swiss companies, whose exports to the US account for about one-sixth of their total foreign sales, face one of the steepest tariff rates in Trump’s trade war regime. Only Laos, Myanmar and Syria had higher figures, at 40-41%. The EU and the UK have negotiated 15% and 10% respectively. Switzerland exported $61.5bn of gold to the US in the 12 months ending in June, the FT said. This would be subject to a further $24bn in levies under Switzerland’s 39% tariff rate, which came into effect on Thursday, according to the report. The agenda 9am BST: UN Food and Agricultural Organization Price Index</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The Financial Conduct Authority is expanding bullying and harassment rules. Previously, only banks were required to report bad behaviour to the watchdog. The rules will now apply to tens of thousands of other firms across the City.</t>
+          <t>River Island has secured approval for a restructure plan designed to stop the fashion retailer from falling into administration. The plan received approval from a high court judge on Friday after the majority of creditors gave their backing to the plan earlier this week.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Financial Regulation Expansion</t>
+          <t>UK Economic Challenges Overview</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Time to wrap up…. The chair of the Federal Reserve, Jerome Powell, has blamed Donald Trump’s tariffs for preventing the immediate interest rate cuts the president has demanded. Trump has repeatedly urged Powell to reduce borrowing costs in the US economy, and on Monday posted a hand-scrawled note on his Truth Social platform saying: “You have cost the USA a fortune – and continue to do so – you should lower the rate by a lot!” But Powell told an event hosted by the European Central Bank (ECB) in Portugal on Tuesday that the Fed was waiting to assess the inflationary impact of the president’s trade policies. Speaking on a panel of central bankers in Sintra, he said: “In effect we went on hold when we saw the size of the tariffs. “Essentially all inflation forecasts for the United States went up materially as a consequence of the tariffs. We didn’t overreact, in fact we didn’t react at all. We’re simply taking some time.” Shortly after Powell’s comments in Sintra, Trump claimed that “anyone” could do a better job as Fed chair. In other news… UK house prices fell in June, as the rise in stamp duty tax deterred buyers The governor of the Bank of England has warned that the UK economy, and the jobs market, are softening – which may clear the way for further cuts to UK interest rates The downturn in UK manufacturing eased last month, but the sector is still shrinking Eurozone inflation has risen to 2% EU trade commissioner Maroš Šefčovič is preparing for crunch talks over tariffs with US trade representative Jamieson Greer Marks &amp;amp; Spencer’s online business should be running “fully” within the next four weeks, its boss has said, as the retailer recovers from a damaging cyber-attack. Over at ‘Alligator Alcatraz’, a detention facility in Florida, Donald Trump has taken another bite at Jerome Powell. Our US Politics Live blog reports that Trump was asked if he intends to announce his pick for the next Fed chair’. In response, the US president gestured to Florida governor Ron DeSantis and US Secretary of Homeland Security Kristi Noem to imply they would both be good candidates, before adding: Anybody would be better than J Powell. He’s costing us a fortune because he keeps the rate way up. There’s an amusing moment at the ECB’s central bank forum, where Christine Lagarde declines to offer any advice to her eventual successor. Lagarde resists, telling the event in Sintra that she remembers being told by her predecessor that “it would be a walk in the park”. Lagarde became ECB president in November 2019, shortly before the Covid-19 pandemic struck the world economy, posing unprecedented challenges for central bankers. Top central bankers in Sintra are also asked what keeps them awake at night. European Central Bank president Christine Lagards says she is worried about “the truth”. Lagarde reveals she is “more and more concerned about the role that artificial intelligence is going to play”, about how things can be distorted, and how public opinion can be manipulated. That extends to fears that the data which the ECB relies on could be changed, she adds, saying: I do have this fear that things can be distorted, and we can fall prey to that. That is of great concern to me. Jerome Powell says that he is kept awake by the challenge of handing on a strong US economy to his successor. Powell explains that he has around 10 months of his term as chair left. All I want, and all anyone at the Fed wants, is to deliver an economy that has price stability, maximum employment, financial stability. What keeps me awake at night is how we get that done, and are we on a path to do that. I want to hand over to my successor an economy in good shape. Korea’s Rhee says he is worried about the perception gap between how fast the economy can grow, and how fast people think it should grow. Andrew Bailey explains that he want to deliver UK inflation sustainably at target. He became chair of the Financial Stability Board (an important watchdog) today, so that creates more vulnerabilities to keep him awake. Federal Reserve chair Jerome Powell also reassured the ECB’s conference today that the Fed isn’t planning to change how it offers dollar liquidity to other centra banks. Powell explained that the Fed’s dollar swap lines are “a big contribution” to global financial stability, and doesn’t plan to change that, saying: “We still have the same authorities, and we’re still prepared to use them in situations where it’s within our legal authorities and where we think it makes sense.” Powell was responding to Bank of Korea Governor Governor Rhee Chang-yong. who noted that countries such as South Korea need to build up dollar reserves in case they are needed. Fed dollar swap lines offer loans to eligible central banks to ensure dollar liquidity is not an issue for the global financial system and have been heavily used in times of crisis. The Financial Times reported last week that central banks are concerned the US could turn off this flow of dollars. Andrew Bailey then calls for policymakers to look at the causes of the problems of the world economy that have led to trade wars and threaten to lead to fragmentation. Christine Lagarde then offers Jerome Powell her support, insisting that all the panel would have acted exactly the same as the Fed chair this year. “Right?” she directs the Bank of Korea’s Rhee Chang Yong, firmly. “Yes,” replies Rhee, who worked under Lagarde at the IMF. Jerome Powell also refuses to respond to the outpouring of criticism from the White House. Bloomberg’s Francine Lacqua, who is moderating today’s session: Q: You get attacked by the president a lot on a personal basis. Does it make your job harder?” Powell insists that he is “very focused on just doing my job”. Sticking to the Fed’s mandate, Powell says: The things that matter are using our tools to achieve the goals that Congress have given us – maximum employment, price stability, financial stability. That’s what we focus on, 100%. At this point, Powell wins a supportive round of applause from the audience in Sintra, and from his fellow panelists – BoE governor Andrew Bailey, ECB president Christine Lagarde, Bank of Japan governor Kazuo Ueda, and Bank of Korea governor Rhee Chang Yong. Asked later if he would remain at the Fed after his term as Chair expires next May, Powell said: “I have nothing for you on that today.” Jerome Powell has also warned that America’s fiscal path is not “sustainable”, even though the current level of debt is sustainable. Andrew Bailey then fends off a cheeky question about how low the Bank of England could cut rates: Q: Will interest rates be closer to 3% or 4% at the end of the easing cycle? BoE governor Bailey says there is huge uncertainty about what the neutral rate of interest (r*) is. The more important thing to realise, Bailey argues, is that UK monetary policy is currently restrictive, and will continue to remain restrictive, but that level of restrictive-ness will come down. Fed chair Jerome Powell weighs in too, saying he thinks US interest rates are “modestly restrictive” at their current levels'; it doesn’t feel that the US economy is suffering from very tight policy. South Korea’s central bank chief fears that an escalation of the Trump trade wars would have a serious impact on its economy. Speaking on the ECB’s panel, alongside Jerome Powell, Rhee Chang-yong explains that global fragmentation has a serious impact on Korea’s economy as it is export-driven. That includes the direct impact of US tariffs, but also indirect impacts through the China, Mexico and Canada. Rhee explains that the Bank of Korea is watching for what happens when Trump’s 90-day tariff pause expires: It really depends what happens on July 9th… We don’t know what’s going to happen. He explains that if Trump reimposes the 26% retaliatory tariff announced on 2 April, added to sectoral tariffs on aluminium, steel, and cars, the impact could easily be more than 1% of Korea’s GDP. Jerome Powell says he can’t say whether the Fed could cut interest rates as soon as this month. It all depends on the data, he insists, adding that the Fed is going ‘meeting by meeting’. Christine Lagarde declines to comment on the strength of the euro, beyond suggesting that it is a reflection on the state of the eurozone economy. She suggests that there are two factors – the depreciation of the US dollar (which had its worst first half to a year since 1973), and an appreciation of the euro. Looking ahead, Jerome Powell says economic data will determine whether US interest rates are cut this year (as Trump has been loudly demanding). Powell explains that “a solid majority” of members of the rate-setting FOMC committee think it will be appropriate to reduce rates later this year (there are still four FOMC meetings scheduled]. But, Powell adds, this will depend on the incoming data, so the Fed will be monitoring the inflation data slowly, as well as the labour market. Kazuo Ueda, governor of the Bank of Japan, resists commenting directly on Donald Trump’s threat to impose more tariffs on Japanese imports. Ueda says the issus is being negotiated by the relevant minister, so he is “yrying to avoid making any specific comments on this.” Trump claimed it was unfair that Japan doesn’t buy US rice (it does, though, as CNN shows here) despite having a massive rice shortage, and hinted the White House will simply sent Toyko a letter laying out the tariffs it will face. Andrew Bailey, governor of the Bank of England, tells the ECB’s forum in Sintra that he is seeing some “softening” in the UK economy and “softening in the labour market”. That means Bailey believes “the direction of UK interest rates continues to be downwards.” Bailey agrees it’s too early to see the price effects from recent action on tariffs; endorsing Jerome Powell’s explanation for not having cut US interest rates this year. The top US central banker has indicated that Donald Trump’s trade war has prevented the cuts to interest rates which the president has been demanding. Jerome Powell, who has been repeatedly criticised by Trump for the Federal Reserve’s failure to cut interest rates this year, has told an audience in Portugal that uncertainty over the impact of Trump’s tariffs prevented the Fed from cutting rates. Powell explains that the US economy is “healthy” and in a good position, with inflation down to 2.3%, core inflation is at 2.7%, and an unemployment rate is 4.2%. Powell explains that “if you ignore tariffs”, inflation is behaving as the Fed expected and hoped. He says: We haven’t seen effects much from tariffs, and we didn’t expect to by now. We’ve always said the timing, amount and persistence of the inflation would be highly uncertain and it’s certainly proved that. We’re watching. We expect to see over the summer some higher readings, but we’re prepared to learn that it can be higher, or lower, or later or sooner than we’d expected. Q: Would the Fed have cut more by now if it wasn’t for the tariffs? Powell replies that “I think that’s right”, before explaining that the Fed is waiting until it knows the impact of the Trump trade war. He explains: In effect we went on hold when we saw the size of the tariffs. Essentially all inflation forecasts for the United States went up materially as a consequence of the tariffs. We didn’t overreact, in fact we didn’t react at all, We’re simply taking some time. Powell concludes by explaining that “the prudent thing to do” is to wait and see the impact of imposing tariffs on US imports, given the US economy is “in solid shape”. Trump has repeatedly accused Powell of being ‘too late’ to cutting rates, pointing out that other major central banks have lowered rates more quickly. The Fed hasn’t cut rates since last December. On Monday, Trump produced a hand-written note showing how US interest rates are much higher than many other countries. Trump wrote that the Fed “should be ashamed of themselves for allowing this to happen to the United States”, and claimed they had “cost the USA a fortune” by not lowering borrowing costs. The session in Sintra begins with Christine Lagarde welcoming this morning’s news that eurozone inflation rose to 2% in June, from 1.9% in May. Lagarde reminds her audience that 2% inflation, in the medium term, is the European Central Bank’s target. I am not saying ‘mission accomplished’, but I say ‘target reached’, OK. The ECB president then warns that “we are facing a lot of uncertainty”, including the risks of fragmentation, and worrying geopolitical developments that are causing a ‘two-sided risk to inflation’. We have to continue to be extremely vigilant, and remain committed to delivering on the inflation target, Lagarde says, insisting: We are well-equipped to navigate the tormented waters that we should anticipate. EU member states have been advised there could be four options emanating from this week crunch talks between trade commissioner Maroš Šefčovič and US trade representative Jamieson Greer over tariffs. One option is no deal but another more likely scenario of the three remaining is a deal in which both signs are aligned “in broad brush strokes” but centre, like the UK’s deal, on a limited number of sectors such as cars and steel. This would leave the threat of future tariffs on other sectors open, risking new crises emerging without warning during the remainder of the Trump term. A third option is a delay, extending talks beyond 9 July. This carries the risk of Donald Trump’s threatened 50% unilateral tariffs being imposed on all imports from the EU from 10 July. And a fourth option is an “imbalanced deal”, the type that would favour the US, something Emmanuel Macron last week said he would not accept. Details of the negotiations were not shared in the 45 minute briefing given by Ursula von der Leyen’s head of cabinet Bjoern Siebart and Sabine Weyand, director general of the trade commission, best known in the UK as Michel Barnier’s right hand woman during Brexit negotiations. EU ambassadors gave also been warned that the 10% blanket tariff may remain but that if they cannot secure a reduction then they will try and extract duty free exemptions in some sectors. A delegation headed by trade adviser Thomas Baert flew to Washington on Monday for technical talks with Šefčovič joining them tomorrow for talks with trade representative Jamieson Greer. He is likely to return to brief member states on Thursday with a possible further of ambassadors meeting on Friday ahead of next week’s deadline. The UK government has just published the timetable for the implementation of its big workers’ rights package, which UK employers will have to get their heads around in the coming months. Some business groups had been lobbying for a longer implementation period, but Labour is keen to press ahead. A new Fair Work Agency, to enforce the rules, will be up and running next year, ministers said. Some changes - such as the repeal of the Tories’ strike-busting minimum service levels legislation, will come into force as soon as the Employment Rights bill gets Royal Assent, expected to be later in the summer. Next April (2026) will mark the end of the two-day wait for statutory sick pay, and stronger protection for whistleblowers; new regulations to set up a fair pay agreement for the social care sector will follow next October. Another slew of changes are expected to come into force in 2027, including new rights to bereavement leave, and day one rights to unfair dismissal. Deputy prime minister Angela Rayner said: “these landmark reforms will kick in within months, demonstrating our commitment to making work pay for millions of workers across the country and delivering real change.” Over in Sintra, Portugal, some of the world’s top central bankers are about to discuss monetary policy and the state of the global economy. The central bank chiefs of the UK, the eurozone, the US, Japan and Korea are all appearing on a panel organised by the European Central Bank, at its Forum on Central Banking 2025. The session is titled: Adapting to change, macroeconomic shifts and policy responses. On the panel, we have: Andrew Bailey, Governor, Bank of England Christine Lagarde, President, European Central Bank Jerome Powell, Chair, Board of Governors of the Federal Reserve System Chang Yong Rhee, Governor, Bank of Korea Kazuo Ueda, Governor, Bank of Japan Elon Musk and Donald Trump are continuing to trade barbs. Trump has told reporters at the White House that he would look into deporting Musk, when asked about the billionaire’s vocal criticism of Trump’s tax and spending legislation. Trump then repeated his threat to unleash the Department of Government Efficency on Musk’s empire, saying: “We might have to put DOGE on Elon. DOGE is the monster that might have to go back and eat Elon. Wouldn’t that be terrible?” In response, Musk has posted enigmatically… So tempting to escalate this. So, so tempting. But I will refrain for now. The row is continuing to hurt Tesla’s shares, they’re now down over 6% in pre-market trading. Speaking of trade deals… US Treasury Secretary Scott Bessent has said America is hopeful China will do more to ease the export of rare earth magnets after last month’s deal between the two countries. Bessent told Fox News that flows had still not returned to levels seen in early April, despite the agreement which the two sides hammered out in London last month. Bessent said: “We are hoping that they will flow at a faster rate. “Rare earth magnets are flowing. They are not flowing as they did before April 4, but we are confident that the Chinese will live up to their side of the deal.” Here’s Susannah Streeter, head of money and markets at Hargreaves Lansdown, on M&amp;amp;S’s recovery from its cyber-attack: “Marks and Spencer is halfway there, but there’s still a lot to get back online before the company can put the cyber attack behind it. 50% of online operations are back up and running, but its popular click and collect services remain suspended. At the company’s AGM, CEO Stuart Machin put the latest timeline on a recovery at four weeks. This should mean the retailer will hit August firing on all cylinders once again. Management have previously estimated that it could cost as much as £300 million in lost sales and operational disruption, although it’s likely that this will be mitigated by insurance claims and cost efficiencies made elsewhere. While services have been suspended the company is believed to have used the opportunity to speed up part of its digital transformation plan, as well as ensuring that its IT systems are robust enough to withstand a future attack. “There will be high hopes that M&amp;amp;S can put this unfortunate chapter behind it, and the early signs are that there is pent up demand, particularly for its summer styles, with many of the popular products sold out online. Its strong set of annual results showed the retailer was in a resilient position before the cyber attackers infiltrated systems. Sales growth in the fashion and home &amp;amp; beauty division reflected improved customer perceptions of value, quality, and style. Demand for M&amp;amp;S food remains robust, with increased volumes driving growth. So, with the underlying performance remaining solid, it bodes well for M&amp;amp;S ahead, but until everything’s back up and running, it’s likely to weigh on investor sentiment. Although shares have been in positive territory today, they remain around 13% lower than the level in mid-April, before the cyber attack took hold.’’ European trade commissioner Maroš Šefčovič will travel to Washington tomorrow hoping to strike a tariff agreement in principle with Donald Trump’s team, my colleague Lisa O’Carroll reports from Brussels. He will meet trade representative Jamieson Greer with hopes rising they will have enough in the coming days to agree the basics ahead of 4 July Independence Day negotiations. At the same time they recognise the volatility on the US side and are working to avert any further threats of tariffs that Trump may like to announce to extract more concessions from the EU. He recently warned tariffs on pharma were coming “very soon”. If an agreement in principle is struck, talks would then continue, possibly beyond 9 July to work out the detail. This would follow the pattern in the UK which took more than a month to get to a final text. Yesterday Šefčovič revealed it was a good time get down to “drafting” an agreement and “drafts of proposals for the eventual agreement in principle”, a significant change of language which suggests they close to settling differences on major issues. EU sources confirm the European Commission is now putting all its efforts into a “quick deal” rather than hold out for a deep and wide one covering up to 1,000 product lines. This follows criticism by German chancellor Friedrich Merz last week that the EU was too complicated. Germany’s priority is get the 27.5% tariffs reduced or eliminated on car exports and the same for steel exports which are facing 25% tariffs. The Baltic states, in particular, area also keen to build on the humouring of Donald Trump at last week’s NATO summit and want to ensure everything is done to keep him on board with weapons supply in Ukraine. Sources say the EU is more or less resigned to a 10% blanket tariff on exports to the US remaining and may offer more imports on semi-conductors to sweeten the deal. However there remain worries that Trump could yet announce tariff on pharma exports as part of his negotiation tactics to extract more from the EU. An EU technical delegation flew to Washington on Monday, ahead of Šefčovič ’s visit with expected meetings with commerce secretary Howard Lutnick, who looks after sectoral deals, and with Greer. With the clock ticking down towards Trump’s self-imposed deadline for a deal of 9 July, there is still plenty of room for a change of mood in the Oval Office. Overnight Trump expressed frustration over Japan trade negotiations on Monday with treasury secretary Scott Bessent warning that countries could be notified of sharply higher tariffs as a July 9 deadline approaches despite good-faith negotiations. Speaking on Monday in Brussels, Šefčovič said “The 9th of July is around the corner. So for me, it’s always a good sign when we kind of move from, I would say, exchange of views, into the drafting process.” “As you know, we received first drafts of proposals for the for the eventual agreement in principle we are working on that,” he told reporters in Brussels. He added the EU was pushing for a deal that “was fair for both sides”. UK retailer Marks &amp;amp; Spencer is optimistic that the worst of its recent cyber attack will be behind it by August. M&amp;amp;S’s chief executive Stuart Machin told shareholders at the retailer’s annual general meeting today that the company Machin explained that the half of M&amp;amp;S’s online store which is not yet open – including its click and collect service – will be fully restored within the next four weeks, and other systems which are currently being rebuilt will be operating by August. He told shareholders: “I have previously highlighted that it would take all of June and all of July, maybe into August but definitely by July. “During the incident we chose to shut things down because we didn’t want the risk of things going wrong. “Currently, half of online is open but not areas like click and collect. Within the next four weeks we are hoping for the whole of online to be fully on. “Then our focus will be getting the Donington site back and running. We’re hoping that by August we will have the vast majority of this behind us and people can see the true M&amp;amp;S.” Last month Marks &amp;amp; Spencer reopened its website to shoppers, six weeks after it was forced to halt online orders after the cyber-attack. Shares in Tesla are set to fall when Wall Street opens, after relation between CEO Elon Musk and US president Donald Trump deteriorated. Tesla’s shares are down 4.5% in pre-market trading. Over the weekend, Musk claimed that Trump’s tax and spending bill was “utterly insane and destructive,” claiming the latest draft of the bill would destroy millions of jobs in America and cause immense strategic harm. Musk also claimed: “It gives handouts to industries of the past while severely damaging industries of the future.” Musk later vowed to unseat lawmakers who support the budget bill: Trump has now hit back, threatening to clamp down on the government subsidies received by Musk’s businesses using The Department of Government Efficiency department which the billionaire used to helm. Trump posted on his Truth Social site: Elon Musk knew, long before he so strongly Endorsed me for President, that I was strongly against the EV Mandate. It is ridiculous, and was always a major part of my campaign. Electric cars are fine, but not everyone should be forced to own one. Elon may get more subsidy than any human being in history, by far, and without subsidies, Elon would probably have to close up shop and head back home to South Africa. No more Rocket launches, Satellites, or Electric Car Production, and our Country would save a FORTUNE. Perhaps we should have DOGE take a good, hard, look at this? BIG MONEY TO BE SAVED!!! The London has moved gingerly into the second half of the year. The FTSE 100 index of blue-chip shares has dropped by 17 points, or 0.2%, to 8743 points. Mining stocks are leading the risers, reflecting optimism that the US may agree more trade deals soon. But housing stocks, and banks, are among the fallers following this morning’s news that UK house prices fell by 0.8% in June. The small pick-up in eurozone inflation last month makes it likely the ECB will leave interest rates on hold at its meeting later this month. Richard Flax, chief investment officer at Moneyfarm, says policymakers will be worried that energy prices could pick up again. Eurozone inflation rose slightly from 1.9% in May to 2.0% YoY in June, aligning with the ECB’s target. The increase was driven by higher energy costs and persistent service sector inflation, which continues to be the main source of upward pressure. Core inflation is expected to remain unchanged, suggesting that underlying price dynamics are stable for now. Energy markets remain a key risk. Prices surged in June due to geopolitical tensions, though a recent ceasefire in the Middle East has helped ease some of the pressure. Still, the potential for renewed volatility could complicate the inflation outlook in the months ahead. With inflation near target and no major surprises in core data, the ECB is expected to hold rates steady at its July meeting. Markets are looking to September for the next potential move, depending on how inflation evolves. Diego Iscaro, head of European economics at S&amp;amp;P Global Market Intelligence, also sees a September cut as more likely: “Inflation edged upwards in June, just as markets expected. The modest increase in inflation is not particularly worrying, given it was mainly driven by a lower fall in energy prices, but the somewhat stronger rise in service price inflation will not be welcome news. “We do not think June’s inflation print will give ammunition to either doves or hawks on the ECB’s governing council. With trade policy-related uncertainty still clouding the picture, there is a risk that the economic outlook may look quite different when the ECB meets later this month. We still expect interest rates to remain unchanged this month, but we see the door opening for a last 25bp cut in September as subdued activity and a stronger euro push underlying inflationary pressures down.” Newsflash: Inflation across the eurozone has risen back to target. Consumer price across the euro area rose by 2.0% in the year to June, statistics body Eurostat reports, up from 1.9% in May. That means inflation is back to the European Central Bank’s 2% target. The increase was partly due to changes in energy prices. Energy inflation rose to -2.7% in June, up from -3.6% in May, following the increase in oil prices last month driven by the crisis in the Middle East. Service sector inflation rose to 3.3%, up from 3.2%, while food, alcohol &amp;amp; tobacco inflatoin dipped to 3.1%, fromh 3.2% in May. Goods inflation slowed to 0.5%, from 0.6% in May. During his interview with CNBC, Andrew Bailey also warned that UK companies are delaying investments due to economic uncertainty. He says: “That increase in uncertainty and predictability is definitely coming through in terms of activity and growth. “When I go around the country talking to businesses, which I do a lot, what they tell me is that they are putting off investment decisions.” The downturn in UK manufacturing has eased last month, new data shows, as output, new orders and employment fell at slower rates than in May. The latest survey of purchasing managers at British factories has also found that business optimism improved to a four-month high in June. This lifted the UK manufacturing PMI to 47.7 in June, its highest reading in five months, but still below the 50-point level separating expansion from contraction. The report found that manufacturers cut output due to weak market conditions, lower demand from clients, trade war uncertainty and geopolitical tensions. Tariffs continued to hit demand, and client confidence, with new export business falling for the forty-first month in a row amid reports of reduced demand from the US, Europe and China, S&amp;amp;P Global says. Manufacturers also cut jobs, for the eighth month running, with the steepest reductions at large-scale producers, despite the UK securing its trade deal with the US last month. Rob Dobson, director at S&amp;amp;P Global Market Intelligence, says: “Although the downturn in UK manufacturing continued in June, the latest PMI survey provides signs of conditions stabilising. Production, new orders and employment all fell at slower rates, while business optimism picked up to a four-month high. The orders-to-inventory ratio, a reliable bellwether of future production trends, also climbed sharply to its highest since August 2024. Inflation of both input costs and selling prices meanwhile nudged lower to hint at a softening inflation trend. “That said, any hoped for stabilisation remains fragile and subject to potential headwinds that could severely impact demand, supply chain reliability and future growth prospects, as manufacturers continue to caution their optimism with concerns about heightened geopolitical tensions, weak global markets, tariff uncertainties and fears over the direction of future government policy.” Sainsbury’s has recorded its strongest growth since last summer after its Argos chain recorded a big step up in sales as shoppers sought out paddling pools and fans during recent hot weather. The retail group said Argos, its catalogue shop, was able to achieve growth of 4.4% in the three months to 21 June, up from 1.9% in the previous quarter. Comparable group sales, excluding fuel, rose 4.7% on a year earlier. The group’s total sales rose 4.9%, helped by the strong trading at Argos and a rise in clothing sales as shoppers snapped up shorts and swimsuits, as well as healthy demand for its premium food ranges. That excludes fuel, where sales fell partly because of price decreases. The retailer said it had achieved the strong sales despite a “subdued, highly competitive and deflationary general merchandise market” as it booked rapid growth in online sales and via its app. Sales in stores declined, partly because of further closures as many Argos sites move from high streets into Sainsbury’s supermarkets. Over in the eurozone, the manufacturing sector has shrunk again but at a slower rate. Data provider S&amp;amp;P Global has reported that its eurozone manufacturing PMI has risen to 49.5, up from 49.4 in May. That’s a 34-month high, but still below the 50-point mark that shows stagnation. Dr. Cyrus de la Rubia, chief economist at Hamburg Commercial Bank, reports that there are signs of stabilization in Europe’s manufacturing sector. Companies have now expanded production slightly for the fourth month in a row, order intake has ceased to fall, and slightly longer delivery times also indicate that demand is picking up a bit. Against the backdrop of numerous uncertainties - US tariffs, the crisis in the Middle East, and Russia’s ongoing war against Ukraine - this can certainly be seen as a sign of resilience. However, it also has to do with the fact that, after years of recession, the economic cycle usually turns at some point because old machines need to be replaced, cars can no longer be repaired, and the necessary modernization of factory buildings can’t be postponed any further. Bank of Engla</t>
+          <t>Time to wrap up…. Sales of new Tesla cars slumped by 59% year-on-year in the UK last month, but Chinese carmakers led by BYD reported big jumps in UK sales. BYD sales quadrupled year on year to reach 3,200 in July, even as overall sales of all types of car declined by 5% to 140,000, according to data published on Tuesday by the Society of Motor Manufacturers and Traders (SMMT), a lobby group. Former star stock picker Neil Woodford and his investment management company have been fined almost £46m by the UK’s financial regulator over the collapse of his popular equity fund. The Financial Conduct Authority (FCA) has given Woodford a penalty of £5.89m and banned him from holding senior manager roles and managing funds for retail investors and fined Woodford Investment Management (WIM) £40m. Donald Trump has attacked Jaguar Land Rover’s divisive rebranding strategy, hours after Britain’s largest carmaker announced its new boss. Trump posted on his Truth Social platform that the auto company, owned by India’s Tata Motors, was “in absolute turmoil” and claimed that the “CEO resigned in disgrace”. The UK’s dominant service sector has reported its biggest drop in new orders in almost three years in July, adding to pressure on the Bank of England to cut interest rates on Thursday. The oil and gas group BP is launching a fresh cost-cutting scheme, despite reporting better-than-expected profits, as it tries to do more for its shareholders to fend off pressure from activist investors. The fossil fuel company said it would begin a fresh review of its business when its new chair, Albert Manifold, joins the board in September. Awkwardly, a rival survey of America’s services sector paints a darker picture. According to the Institute of Supply Management, US service sector firms barely grew in July as Donald Trump’s trade wars pushed up costs, and led to job losses. The ISM’s service sector PMI has dropped to 50.1% last month from 50.8% in June, a level that shows growth almost petered out. One company, in the Agriculture, Forestry, Fishing &amp;amp; Hunting sector, told ISM: “Higher tariffs are increasing the cost of imported feed ingredients and trace minerals for livestock and poultry feeds. Business and customer concerns over additional cost risk due to additional tariffs.” Encouraging economic news from the US: America’s service sector grew at a faster rate last month. The latest poll of purchasing managers from S&amp;amp;P Global has found that business activity in the services sector increased at the sharpest pace in the year-to-date amid a solid and accelerated expansion in new business. S&amp;amp;P Global adds: Companies responded to higher workloads by hiring additional staff, albeit only modestly. Meanwhile, tariffs continued to add to inflationary pressures, resulting in faster increases in both input costs and output prices. Its services PMI Business Activity Index rose to a seven-month high of 55.7 in July, up from 52.9 in June, showing faster growth. Google has outlined its latest step towards artificial general intelligence (AGI) with a new model that allows AI systems to interact with a convincing simulation of the real world. The Genie 3 “world model” could be used to train robots and autonomous vehicles as they engage with realistic recreations of environments such as warehouses, according to Google. The US technology and search company’s AI division, Google DeepMind, argues that world models are a key step to achieving AGI, a hypothetical level of AI where a system can carry out most tasks on a par with humans – not just individual tasks such as playing chess or translating languages – and potentially do someone’s job. DeepMind said such models would play an important role in the development of AI agents, or systems that carry out tasks autonomously. “We expect this technology to play a critical role as we push toward AGI, and agents play a greater role in the world,” DeepMind said. There’s been disruption at London’s Heathrow Airport today, after a key road tunnel was closed. Passengers hoping to get away on their summer break faced delays after the Central Terminal Area tunnel to Terminals 2 and 3 is was closed. Heathrow blamed a technical issue, and urged passengers to use public transport to Terminal 5, where train services were available to all other terminals. The closure lead to heavy queues on the roads leading to Heathrow….. …and chaotic scenes inside the airport. Heathrow says that the road tunnel to Terminals 2 and 3 has now reopened, but warned that there is still congestion at the airport, and so they recommend allowing extra time for your journey. The US trade deficit with the rest of the world has narrowed, as the rush to import goods into America ahead of Donald Trump’s tariffs ended. The US’s goods and services deficit dipped to $60.2bn in June, down $11.5bn from $71.7bn in May. This decline was due to a narrowing in the US goods deficit, while its services surplus grew a little. Imports into the US fell by $12.8bn to $337.5bn in June, while exports dipped by $1.3bn to $277.3bn. Harry Chambers, assistant economist at Capital Economics, explains: The narrowing of the trade deficit was mainly due to a normalisation in pharmaceutical imports and while exports appeared weak, this was primarily due to a fall in gold exports. The big picture is that, despite June’s fall, imports aren’t collapsing and are roughly in line with their levels last year. That said, with export orders weak, it seems likely that exports will struggle over the coming months. Showing his inate ability to commit news, Donald Trump revealed during today’s CNBC interview that he will unveil new tariffs on semiconductors and chips as soon as next week. He told the “Squawk Box” show that an announcement will come “within the next week or so,” saying: “We’re going to be announcing on semiconductors and chips, which is a separate category, because we want them made in the United States.” U.S. President Donald Trump has also said recent falls in energy prices could pressure Russian President Vladimir Putin to halt the war in Ukraine. In his inerview with CNBC, Trump said: “If energy goes down enough, Putin is going to stop killing people. If you get energy down, another $10 a barrel, he’s going to have no choice because his economy stinks.” Brent crude is curently trading at $67.82 per barrel, down 1.35% today, down from over $76 per barrel a year ago. Donald Trump has revealed he is considering four candidates — including former Federal Reserve Governor Kevin Warsh and National Economic Council Director Kevin Hassett — to become the next head of America’s central bank. In an interview with CNBC, Trump said: “I think I say Kevin and Kevin, both Kevins are very good, and there are other people that are very good too.” Current Federal Reserve chair Jerome Powell’s term expires next May. Trump also revealed that Treasury Secretary Scott Bessent told him he did not want to be nominated to replace Powell at the Fed, as he wants to stay in his current role. Neil Woodford is also facing calls for his CBE to be revoked. The Woodford Campaign Group and Transparency Task Force have repeated their request for Mr Woodford’s CBE to be forfeited now that the Financial Conduct Authority’s investigation has been completed. More than 500 people have so far signed a petition drawn up by the Woodford Campaign Group calling for the forfeiture. In an open letter to Sir Chris Wormald, chairman of the Honours Forfeiture Committee at the Cabinet Office, Andy Agathangelou, who founded both campaign groups, said: “This scandal is obviously a matter of great public interest – hundreds of thousands of people have been directly impacted by it, many having lost life-changing amounts of money. Trade war news: Swiss president Karin Keller-Sutter and business minister Guy Parmelin will fly to Washington on Tuesday, the government said, to try to avoid the 39% tariffs announced by President Donald Trump on exports to the United States. The pair will “facilitate meetings with the US authorities at short notice and hold talks with a view to improving the tariff situation for Switzerland,” the government said. The trip comes after Keller-Sutter was accused of mishandling a vital phone call with the White House, leading Trump to hit Switzerland with a shock 39% export tariff. Over on Wall Street, construction and mining equipment company Caterpillar has missed second-quarter profit expectations. Caterpillar’s adjusted profit per share in the second quarter of 2025 fell to $4.72, down from $5.99 in Q2 2024. The drop in earnings was due to a fall in profit margins. Sales and revenues for the second quarter of 2025 dipped by 1% to $16.6bn, Britain’s main minimum wage rate will probably need to rise by around 4.1% next year to £12.71 an hour to keep up with the government’s goal for it to match two thirds of median earnings, according to the body which sets the rate. The Low Pay Commission said today the final figure for the National Living Wage could range between £12.55 and £12.86 an hour. The commission is due to provide a firm recommendation to the government by the end of October. The national living wage is currently set at £12.21 for those aged 21 and over. Britain’s service sector companies were hit by a drop in orders last month, as demand at home and abroad remained sluggish. Service sector growth slowed last month amid a decline in new work, according to the latest survey of purchasing managers from data firm S&amp;amp;P Global. It’s UK Services PMI Business Activity Index has dropped to 51.8, from 52.8 in June, showing a slowdown in growth. The survey found that total new work decreased in July, at the fastest rate since November 2022. Export sales also fell in July, blamed on fragile global economic conditions and elevated geopolitical tensions. Worryingly, services firms cut staff again. Tim Moore, economics director at S&amp;amp;P Global Market Intelligence, says: “UK service providers recorded a third consecutive monthly rise in business activity, but they were unable to maintain the growth rate achieved in June. Moreover, new business intakes swung back into contraction during July, with the downturn in order books the fastest for just over two-and-a-half years. Risk aversion and low confidence among clients were the main reasons provided for sluggish sales pipelines, alongside an unfavourable global economic backdrop. Hiring trends were especially subdued, with total workforce numbers decreasing to the greatest extent since February. Worries about rising payroll costs were cited as the main factor holding back recruitment. Newsflash: The UK’s financial regulator has decided to fine former star fund manager Neil Woodford and his investment management company nearly £46m, over the collapse of his popular equity fund. The Financial Conduct Authority says it has decided to fine Woodford £5,888,800 and ban him from holding senior manager roles and managing funds for retail investors. The FCA has also decided to fine Woodford Investment Management (WIM) £40,000,000. The penalties result from failures in their management of the Woodford Equity Income Fund (WEIF), the FCA says, which collapsed in October 2019 after investors rushed to withdraw money in response to a raft of poorly performing company investments, including some hard-to-sell, illiquid assets. The fund was frozen and later closed and wound up. About 300,000 people had invested in the fund, including 130,000 through Hargreaves Lansdown, which is being sued by thousands of investors. In today’s ruling, the FCA explains that between July 2018 and June 2019 WIM and Woodford made “unreasonable and inappropriate investment decisions”, including selling sold more liquid investments (where it’s easier to find a buyer) and buying less liquid ones (which are harder to shift quickly at a good price). They also failed to react appropriately as the fund’s value declined, its liquidity worsened and more investors withdrew their money, the regulator says. However, these findings are only “provisional”, as Neil Woodford and Woodford Investment Management have referred the Decision Notices to the UK’s Upper Tribunal. The FCA is also critical of Woodford – a former star investment manager – today, saying he held “a defective and unreasonably narrow understanding of his responsibilities.” Steve Smart, joint executive director of enforcement and market oversight at the FCA, said: ‘Being a leader in financial services comes with responsibilities as well as profile. Mr Woodford simply doesn’t accept he had any role in managing the liquidity of the fund. The very minimum investors should expect is those managing their money make sensible decisions and take their senior role seriously. Neither Neil Woodford nor Woodford Investment Management did so, putting at risk the money people had entrusted them with.’ It appears that the UK government’s offer to subsidise new electric car purchases may have actually dampened the car market last month. The grants, which offer up to 10% off the price of many electric cars costing less than £37,000, were announced in mid-July. But the government only revealed the first eligible cars today – four Citroën models. The discount scheme won’t apply to Teslas (as they’re too expensive), or models from China as they don’t pass the government’s rules on environmentally sustainable manufacturing practices. The SMMT explain: The newly announced Electric Car Grant (ECG) provides a welcome and much-needed fiscal incentive for BEV uptake, but full model eligibility has yet to be confirmed, causing some buyers to hold off pending confirmation of which vehicles will qualify for a discount of up to £3,750. Its sales figures show that registrations of plug-in hybrid electric vehicles (PHEVs) rose 33.0% in July while battery electric vehicles (BEVs) rose 9.1%, but there was a 10% drop in hybrids (HEVs). Petrol sales fell 14.7% and diesel were down 7.9%. BYD wasn’t the only Chinese EV maker growing its UK market share last month. Jaecoo, a brand from Chinese vehicle manufacturer Chery, sold 1,915 cars in the UK in July – a year ago, it didn’t sell any, as it only launched in the UK early in 2025. Omoda, another Chery brand, also made its debut this year – with 1,874 of its cars registered in the UK in July. Just in: Sales of Teslas in the UK more than halved, year-on-year, in the UK last month as the electric carmaker’s struggles continue. Industry body data just released shows that just 987 new Teslas were registered in the UK in July, almost 60% less than the 2,462 registered in July 2024. This means Tesla’s UK market share shrank to 0.7% in July, from 1.67% a year ago. For 2025 to date, Tesla sales in the UK are 7% lower, during a year in which CEO Elon Musk has faced heavy criticism for his – now-soured – relationship with Donald Trump. The wider UK electric car sector grew in July, though. Sales of battery-powered vehicles (BEVs) rose by 9.1% to 29,825, giving BEVs a 21.3% share of the market. China’s BYD more than quadrupled its sales last month, to 3,184 in July from 768 a year ago. The company recently launched a relatively cheap electric car, the Dolphin Surf, in the UK. BYD’s sales are up 514% during 2025 to 22,574, up from 3,672 in January-July 2024. That’s only slightly fewer than Tesla which has shifted 23,708 cars so far this year. Last month Tesla reported a large drop in quarterly deliveries, as demand faltered due to the backlash over CEO Elon Musk’s political stance. Tesla’s sales have also been hurt by its aging model line-up – the company has been rolling out an updated Model Y this year, dubbed the “Juniper” refresh. Yesterday, Tesla announced it was handing Musk stock options worth almost $30bn, in an attempt to keep him committed to the company for the next few years. Overall, the UK’s new car market shrank by 5% in July with 140,154 units registered, which is the weakest July since 2022. Mike Hawes, SMMT chief executive, says: July’s dip shows yet again the new car market’s sensitivity to external factors, and the pressing need for consumer certainty. Confirming which models qualify for the new EV grant, alongside compelling manufacturer discounts on a huge choice of exciting new vehicles, should send a strong signal to buyers that now is the time to switch. That would mean increased demand for the rest of this year and into next, which is good news for the industry, car buyers and our environmental ambitions. The UK’s Domino’s Pizza Group has cut its profit forecast this morning, warning that costs are climbing as sales fall. The group, which has the exclusive rights to the Domino’s brand in the UK and Ireland, reported that total orders were flat in the first half of this year, and that like-for-like sales fell 0.7% in April-June. Pre-tax profits have fallen by almost a third, on a statutory basis, from £59.4m to £40.5m. Domino’s now expect underlying profits to come in between £130m to £140m, down from a previous forecast of £140.8m-£149.7m. Several factors were blamed, including weak consumer confidence and rising employment costs. CEO Andrew Rennie blamed higher employment costs – following last year’s budget – and uncertainty over what chancellor Rachel Reeves might announce this autumn, saying: “There’s no getting away from the fact that the market has become tougher both for us and our franchisees, and that’s meant that the positive performance across the first four months didn’t continue into May and June. Given weaker consumer confidence, increased employment costs and uncertainty ahead of the Autumn Statement, franchisees are taking a more cautious approach to store openings for the time being. Shares in Domino’s Pizza Group have fallen by 19% in early trading. Overnight, UK luxury-car maker Jaguar Land Rover has named a new CEO – winning a blast from Donald Trump. JLR named P B Balaji, the finance boss of parent company Tata Motors, as its new chief executive, increasing the Indian owner’s influence over the company. Balaji will replace Adrian Mardell, who had run JLR for the last few years. Mardell’s tenure will be remembered for last year’s rebranding, and the launch of a new concept electric car which looked nothing like a traditional Jag, which captured attention and wound-up the rightwing commentariat. Anti-woke cheerleader Donald Trump was quick to give Mardell a hoofing on his way out the door. Posting on his Truth Social site, Trump declared that Jaguar’s “stupid, and seriously WOKE advertisement” had been “A TOTAL DISASTER!”, adding: The CEO just resigned in disgrace, and the company is in absolute turmoil. Who wants to buy a Jaguar after looking at that disgraceful ad. Shouldn’t they have learned a lesson from Bud Lite, which went Woke and essentially destroyed, in a short campaign, the Company. Trump also hailed actor Sydney Sweeney’s new advert for American Eagle as a triumph, saying the “HOTTEST” ad meant jeans were now “flying off the shelves.” Sweeney is probably in Trump’s good books after it emerged she was a registered Republican voter in Florida. BP is also planning to pump more cash to its shareholders. The company is raising its quarterly dividend by 4 per cent to 8.32 cents a share, subject to board approval. It has also announced a new $750m share buyback programme. Oil giant BP is launching a new cost-cutting scheme, despite reporting better than expected profits, as its incoming chairman gets to grips with the company in the face of pressure from activist investors. BP has beaten City expectations this morning by reporting a smaller drop in underlying profits than expected in the last quarter. On an underlying replacement cost basis, profits rose to $2.35bn in April-June. That’s 15% lower than the same quarter a year ago when the company benefitted from higher oil and gas prices, but also a jump on the $1.38bn profits posted in January-March. Analysts had forecast a smaller rise in underlying profits, to $1.8bn. But despite this beat, CEO Murray Auchincloss says “there’s much more to do”. Auchincloss tells shareholders this morning: In advance of chair elect, Albert Manifold joining the board on 1 September, he and I have been in discussions and have agreed that we will conduct a thorough review of our portfolio of businesses to ensure we are maximizing shareholder value moving forward - allocating capital effectively. We are also initiating a further cost review and, whilst we will not compromise on safety, we are doing this with a view to being best in class in our industry. Earlier this year, BP announced plans to cut more than $5bn from its previous green investment plan. But activist investor Elliott Management has been pushing BP to cut its operating expenses more aggressively and demanding more cost reductions. Manifold is due to become chairman on 1 October, a month after joining the board as a non-executive director. Good morning, and welcome to our rolling coverage of business, the financial markets, and the world economy. UK car sales dipped last month, after a bumper June. British new car registrations fell about 5% year-on-year in July, according to preliminary data released this morning by the Society of Motor Manufacturers and Traders (SMMT). Battery electric vehicles are now projected to account for 23.8% of new registrations in 2025, slightly up from SMMT’s previous forecast of 23.5%. The SMMT should release its final figures for July at 9am. The data comes as the UK government announces that France’s Citroën will be the first company to benefit from its new discount scheme, which cuts the cost of a new EV for consumers. Transport Secretary Heidi Alexander has confirmed buyers will get discounts of £1,500 off 4 Citroën models – the Citroën ë-C3, ë–C4, ë-C5 and the ë-Berlingo - from today. The scheme aims to bring down the price of electric cars to more closely match their petrol and diesel counterparts. The agenda 9am BST: UK new car sales for July 9am BST: eurozone service sector PMI for July 9.30am BST: UK service sector PMI for July 1.30pm BST: US trade data for June 2.45pm BST: US service sector PMI for July</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jerome Powell says the Fed is waiting to assess the inflationary impact of the president’s trade policies. Trump claims that “anyone” could do a better job as Fed chair. Christine Lagarde declines to offer any advice to her eventual successor.</t>
+          <t>Sales of new Tesla cars slumped by 59% year-on-year in the UK last month. Chinese carmakers led by BYD reported big jumps in UK sales. US service sector barely grew in July as Donald Trump’s trade wars pushed up costs, and led to job losses.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Economic and Market Volatility</t>
+          <t>Trade War Impacts Markets</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Time to wrap up…. Investor confidence in the EU has fallen sharply after Donald Trump’s trade agreement with Brussels, amid mounting concern about the economic hit from the US president’s tariff war. The latest snapshot from the Sentix index showed that investor sentiment fell significantly at the start of the month after the deal last week between Trump and the European Commission president, Ursula von der Leyen. The data provider said its weekly survey of thousands of investors in more than 20 countries showed that the pact was a “deal that dampens the mood”, with Trump and the US viewed as “winners” at the expense of the eurozone. “The result is devastating for the eurozone,” said Manfred Hübner, the managing director of the Sentix economic index. “The current situation and expectations are both declining. The wrinkles of concern in the economy are deepening again.” Switzerland, which was hit with a 39% tariff by Trump, is now indicating it might make the US a better offer. Shares on the Swiss stock market dropped this morning, as traders reacted to the prospect of high levies at the US border. Tesla’s board has approved the award of $30bn (£23bn) worth of shares to its chief executive, Elon Musk, after a US court ruled against a previous pay deal for the world’s richest person. Musk will pay $2bn to buy 96m shares in the electric carmaker at the same price as the 10-year pay package agreed in 2018, which is stuck in legal limbo awaiting a court date for an appeal. The award was based on a recommendation from a “special committee” of the board. The announcement in a financial filing was accompanied by a shareholder letter from two members of the committee, Tesla’s chair, Robyn Denholm, and Kathleen Wilson-Thompson. It described the award as a “good faith” payment to Musk after the previous pay deal, worth $56bn, was rescinded in 2024 by a judge in Delaware, where the company was incorporated until June that year. Shares in UK lenders surged on Monday after a favourable supreme court ruling significantly slashed the anticipated bill for companies engulfed in the car finance scandal. The specialist lender Close Brothers, which is the most exposed to the scandal, jumped as much as 27% at the start of trading, and are still up 22%. The UK’s biggest motor loan provider, Lloyds Banking Group, are now up 8%. Shares in Barclays, which no longer provides car finance but is dealing with the fallout for the remaining loans on its books, rose by 1.1%. Shares in FirstRand, one of the lenders involved in the supreme court case, jumped by 4.8%. More tariff news: the European Union will suspend its two packages of countermeasures to U.S. tariffs for six months following the deal agreed with U.S. President Donald Trump. A comission spokesperson explains: “The EU continues to work with the U.S. to finalise a Joint Statement, as agreed on 27 July. “With these objectives in mind, the Commission will take the necessary steps to suspend by 6 months the EU’s countermeasures against the US, which were due to enter into force on 7 August.” The EU had threatened to impose nearly €100bn (£87bn) worth of tariffs on US imports ranging from bourbon to Boeing aircraft in one fell swoop if a trade deal wasn’t reached…. Just in: US factory orders dropped sharply in June, after a busy May. The US Census Bureau has reported that new orders for manufactured goods fell by 4.8% in June, to $611.7bn. That follows an 8,3% jump in orders in May. The drop in June was driven by weaker demand for durable goods – items designed to last several years. Wall Street has opened higher, recovering from Friday’s losses. The Dow Jones industrial average has risen by 317 points, or 0.75%, in early trading to 43,906 points. The broader S&amp;amp;P 500 share index is 1% higher. Shares fell last Friday after a surprisingly weak US jobs report, which prompted Donald Trump to fire the federal government official in charge of labor statistics a few hours later. Shares in Tesla have, as expected, jumped at the start of trading. They’re up 2.5%, to just over $310 each. Over in Zurich, Switzerland’s government says it is ready to make a “more attractive” trade offer to Donald Trump, in the hope of avoiding a 39% tariff on its exports to the US. Following a crisis meeting this morning, the Swiss cabinet says: “Switzerland enters this new phase ready to present a more attractive offer, taking U.S. concerns into account and seeking to ease the current tariff situation.” Switzerland was shocked that Trump announced a 39% tariff on its wares, which prompted the drop on the Swiss stock marked this morning. Wedbush analyst Dan Ives has welcomed Tesla’s decision to hand Elon Musk almost $30bn in share options that will vest in two year’s time. Ives says it“removes an overhang on the stock” adding: “Musk remains Tesla’s big asset and this comp [compensation] issue has been a constant concern of shareholders.” Today’s $30bn share award won’t be the end of the discussions about Elon Musk’s pay. In their letter to shareholders, Robyn Denholm and Kathleen Wilson-Thompson explain that the Tesla board’s special committee will continue its work on “a longer-term CEO compensation strategy”. They intent to put this plan to a shareholder vote at Tesla’s annual meeting on 6 November. Shares in Tesla have risen by over 2% in pre-market trading – a sign that Wall Street approves of Musk’s new share package. They’ve risen by 2.3% to $309 per share, up from $302 on Friday night, which will lift the value of Musk’s 96m share package closer to $30bn. Investors may well be reassured that today’s share package will keep Musk at Tesla, as the shares will vest in two year’s time. Customer loyalty towards Tesla across America has plunged since CEO Elon Musk endorsed President Donald Trump last summer, according to data from research firm S&amp;amp;P Global Mobility. The data shows Tesla’s customer loyalty peaked in June 2024, when 73% of Tesla-owning US households in the market for a new car bought another Tesla, Reuters reports Brand loyalty rate started to nosedive in July, the month when Musk endorsed Trump. The rate bottomed out at 49.9% last March, after Musk launched the Department of Government Efficiency in January and started firing thousands of government workers. S&amp;amp;P analyst Tom Libby called it “unprecedented” to see the runaway leader in customer loyalty fall so quickly to industry-average levels, adding: “I’ve never seen this rapid of a decline in such a short period of time.” Tesla’s US loyalty rate has since ticked back up to 57.4% in May. But even so, this does raise the question about whether Musk really deserves $30bn of shares…. Eurostar passengers travelling and from Paris face long delays and cancellations after a power failure on the high-speed rail line north of the French capital. The cross-Channel train operator warned that trains between London and Paris and Brussels and Paris would be disrupted throughout Monday. It said trains were still running but had been rerouted via slower rail lines, adding up to two hours to departures on Monday morning. A number of afternoon services have been cancelled. The latest disruption comes during peak holiday season, on the main rail route from Britain to the continent. Eurostar said it advised passengers to postpone their journey if possible, and exchange their ticket free of charge or request a full refund. It said extra staff had been deployed in the stations to assist passengers. Just in: Tesla has awarded Elon Musk stock options worth almost $30bn, in its latest attempt to pump up the billionaire’s pay packet, and keep him at the company. Tesla had announced that is has approved an award of 96 million shares of restricted stock to CEO Musk, under its 2019 Equity Incentive Plan. At Tesla’s latest share price, $302, the shares would be worth $29bn. Musk would have to pay just $23.34 per share to get them, which would cost him around $2bn, when they vest in two year’s time. This follows the blocking off Musk’s massive, $56bn, pay packet by a Delaware judge. If the Delaware pay deal is reinstated (there’s an appeal to Delaware’s Supreme Court), these new share options will by immediately forfeited, Tesla add (a sign that it is an attempt to get Musk at least part of that offer). Robyn Denholm and Kathleen Wilson-Thompson, members of the special committee of the Tesla’s board of directors, told shareholders that it was “imperative to retain and motivate our extraordinary talent, beginning with Elon”. In a letter to shareholders, they added: We would also like to stress that prior to recommending this award, we reviewed your letters, read your X posts, and considered the direct feedback we have received from many of you in order to align our recommendation with your expressed views. From those communications, we know that one of your top concerns is keeping Elon’s energies focused on Tesla. This award is a critical first step toward achieving that goal, although it is limited by the capacity of our current equity incentive plan. As such, we are also working on next steps to address that issue. Still, while our work remains ongoing, we feel it is important to communicate directly and transparently with you all, our shareholders and Tesla’s owners. The Swiss franc has weakened again this morning, adding to Friday’s losses, as traders anticipate steep tariffs on Switzerland’s goods at the US border. The euro has climbed by almost 0.5% against the swiss franc, to 0.9355CHF. Raffi Boyadjian, lead market analyst at Trading Point, says: Many investors remain hopeful that some of the steep tariffs announced last week will be renegotiated and reduced. For example, reports suggest that Canadian Prime Minister Mark Carney will meet with Trump later this week to potentially reach a deal that would bring down the 35% levy on Canadian imports into the US. The Canadian dollar is unchanged versus the greenback today, but the Swiss franc is tumbling following the White House’s decision to slap 39% tariffs on Switzerland – something not expected by the Swiss government. The yen, meanwhile, enjoyed a revival in its safe-haven status during Friday’s risk-off trading, although it is paring those gains today, with the dollar rebounding to just below 148 yen. Jean-Philippe Bertschy, an analyst at Vontobel, has warned that 39% tariffs on Swiss exports to the US would be “devastating for numerous brands in Switzerland.” Investor sentiment in the euro zone has taken a tumble, as the EU-US trade deal annnounced a week ago dampened confidence. Data provider Sentix’s latest confidence gauge found that investors are not impressed by the EU’s latest tariff deal with the US. The survey of 1,050 investors, conducted from July 31 to August 2, found a decline in the current economic situation, and also in future expectations. It also found a slump in confidence about the Swiss economy, after Donald Trump announced Switzerland will face a 39% tariff – much higher than the EU’s 15%. Sentix reports: The latest data from the “first mover” provides investors’ initial assessment of the EU-US tariff deal. And the result is devastating for the eurozone. The sentix economic index has fallen significantly to -3.7 points. The current situation and expectations are both declining. The wrinkles of concern in the economy are deepening again. Even German Chancellor Friedrich Merz, who recently raved about a turnaround in the economy, has been proven wrong: the Germany index has collapsed by more than 12 points to -12.8 points. Donald Trump and the US are the winners in the current figures. Advance effects are the main factor pumping up the situation figures. However, expectations are also falling in the US to -7.8 points. Investors are particularly harsh on the Swiss economy. The sentix economic index has slumped by a full 21.2 points here. Sentix managing director Manfred Huebner says: “The tariff agreement is proving to be a real mood killer.” Swatch group chief executive Nick Hayek has called on Swiss President Karin Keller-Sutter to meet US President Donald Trump in Washington to negotiate a better deal than the 39% tariffs announced on Swiss imports into the United States. Hayek told Reuters on Monday he was confident an agreement could still be reached before the tariffs, which were announced on Friday, went into effect on August 7. Hayek said: “Karin Keller-Sutter is the boss of the Swiss government, she is the president. She should take the plane and go to Washington. That would increase the chances of a deal enormously. “It’s not doomsday. Of course a settlement can be reached. Why would Donald Trump say tariffs are coming on August 1 and not implement them until the 7th? The door is always open.” The Swiss stock market has tumbled into the red after Donald Trump shocked Switzerland by announcing a 39% tariff on its imports to the US. The Swiss Main Index (SMI) is down over 1%, after losing almost 2% at the start of trading. The market had been closed on Friday for a public holiday, so this is Zürich traders’ first opportunity to react. Most stocks are in the red, including pharmaceuticals firm Roche (-1%), luxury goods maker Richemont (-0.8%), and bank UBS (-1.8%). Economists have warned that the tariffs would have a serious impact on the export-oriented Swiss economy, increasing the risk of recession. South Africa’s FirstRand has said it may need to update its accounting provisions after Friday’s supreme court ruling on motor finance claims, potentially pushing the lender’s annual earnings growth towards the lower end of its forecast. It told shareholders: On 11 December 2024, FirstRand Bank London Branch obtained permission from the Supreme Court to appeal the UK Court of Appeal’s judgment against it in respect of the Wrench and Johnson motor finance commissions cases. The appeal was heard by the Supreme Court between 1 April 2025 and 3 April 2025. FirstRand welcomes the clarity provided by the judgment. FirstRand Bank London Branch’s main ground of appeal (that car dealers do not owe their customers a fiduciary duty) was upheld, and it is important to note that the successful ground was the most important and substantive issue that required the Supreme Court’s consideration following last year’s UK Court of Appeal ruling. The company had earlier expected to deliver full-year earnings growth in the low double-digit to mid-teens range, Reuters reports. Shares in FirstRand are up 4.7% this morning, on the Johannesburg stock exchange. The trade body for the motor finance sector has criticised the Financial Conduct Authority for proposing to backdate its compensation scheme to 2007. Stephen Haddrill, director general of the Finance &amp;amp; Leasing Association, told Radio 4’s Today programme that while it “makes sense” to have a compensation schem, there rae “major concerns” about the time limit. Haddrill argued: I just think it’s completely impractical. It’s not simply firms that don’t have the details about contracts back then, customers don’t either. The head of the UK’s financial watchdog is urging consumers seeking redress in the car finance scandal not to use claims management companies or law firms to handle their case. Nikhil Rathi, the chief executive of the Financial Conduct Authority, has told Radio 4’s Today Programme that the FCA’s proposed compensation scheme will be free to use. Rathi says: “We have taken action against 225 adverts because there have been exaggerated claims out there. If you sign up to these companies you may lose up to 30% of any money you are owed. He also explains that the FCA will now have to decide which car finance commissions should be classed as ‘unfair’ – based on the guidance from the supreme court. Rathi explains: They [the court] have said that different characteristics determine what is unfair. It could be the level of the commission, how it was disclosed, the characteristics of a consumer…. Rathi also explains that the FCA could start its compensation scheme by October, and hopes that compensation can start to be paid out next year. The regulator is looking to the industry to cooperate over this, he adds. Shares in Barclays are up over 1.8% in early trading. It had previously set aside £90m to cover potential motor finance compensation payouts. Boom! Shares in lenders exposed to the UK car finance scandal have surged at the start of trading in London, as investors react to Friday night’s supreme court ruling. Shares in Close Brothers jumped 27% after the stock market opened, after the court ruled in its favour in a case over car finance. Close Bros are leading the FTSE 250 index of medium-sized companies. Lloyds Banking Group is leading the larger FTSE 100 share index – its shares have jumped by almost 6% in early trading. As flagged earlier, Lloyds had previously set aside £1.2bn to cover compensation claims over car finance commissions paid to car dealers. These share price moves are a clear sign that the Supreme court ruling is a win for the lenders, even though the FCA is now consulting on a compensation scheme for motorists. That’s because the FCA estimates the cost of its scheme will be between £9bn and £18bn. Before the supreme court overturned two of the three rulings against the industry, lenders were facing an estimated bill of £44bn. The announcement of BP’s major oil discovery comes a day after energy producers agreed to boost output again. The Opec+ group agreed on Sunday to raise oil production by 547,000 barrels per day for September, the latest in a series of accelerated hikes designed to regain market share. The move means Opec+ has now fully reversed its largest tranche of output cuts, made as oil demand slumped after the Covid-19 pandemic. The oil price is little changed this morning, though, with Brent crude up 0.25% at $69.83 per barrel. Away from the car finance scandal, BP has made its biggest largest oil discovery in 25 years, off the coast of Brazil. BP has told the City that it has made a significant oil and gas discovery at the Bumerangue prospect in the deepwater offshore Brazil. BP says it made the discovery after drilling an exploration well in the Santos Basin, 404 kilometres from Rio de Janeiro. The site has a water depth of 2,372 metres, and the well was drilled to a total depth of 5,855 metres. It discovered a hydrocarbon column with an estimated depth of 500 metres, in a “pre-salt carbonate reservoir” with an area more than 300 square kilometres. Gordon Birrell, BP’s executive vice president for Production &amp;amp; Operations says: “We are excited to announce this significant discovery at Bumerangue, bp’s largest in 25 years. This is another success in what has been an exceptional year so far for our exploration team, underscoring our commitment to growing our upstream. Brazil is an important country for bp, and our ambition is to explore the potential of establishing a material and advantaged production hub in the country.” The FCA’s decision to consult on an industry-wide compensation scheme for car finance customers could have “significant ramifications” for the UK motor finance industry, says Hyder Jumabhoy, partner at international law firm White &amp;amp; Case. Jumabhoy explains: “While it is too early to predict the full impact with certainty until the FCA’s consultation process is complete, we expect this move to accelerate M&amp;amp;A activity due to some lenders having decreased risk appetite but also because of unused provision amounts becoming available for acquisitions. It could also prompt some car manufacturers to enter the UK motor finance market to steady the supply of finance to buyers of new vehicles. “The next six weeks in the run-up to the launch of the FCA’s consultation will be crucial, as the industry assess the implications of the Supreme Court’s ruling and the emerging shape of the scheme in 2026.” Specialist financier S &amp;amp; U PLC has welcomed last week’s Supreme Court decisions on motor finance commissions as a “victory for common sense”. Anthony Coombs, Chairman of S&amp;amp;U, argues the ruling will significantly boost confidence throughout the motor finance industry and benefit lenders and consumers alike in attracting investment and increasing competition. In a statement to the City this morning, Coombs added: As such, it is entirely consistent with the Treasury’s recent emphasis on regulation which encourages growth and which will, in the words of the Financial Conduct Authority, “ensure the integrity of the motor finance market, so that it works well for future consumers.” S &amp;amp; U are the parent company of Advantage Finance, which they say has never used the discretionary commission arrangements which are at the heart of the car finance scandal. Close Brothers, who have been one of the UK’s biggest providers of car loans, has issued a short statement to the City this morning. The firm says: Further to the group’s announcement issued on 2 August, we note the announcement of the Financial Conduct Authority on 3 August of its intention to consult on an industry wide redress scheme in respect of motor finance commissions. We look forward to engaging with the FCA in respect of the consultation. On 2 August, Close Brothers said it “welcomes the outcome” of the supreme court ruling, adding that it “provides clarity on important legal and commercial principles.” Back in March, the company posted a £103m loss for the first half of its financial year, and estimated that the motor finance commission scandal would cost it a total of £200m this year. Lenders exposed to the car finance scandal are issuing statements this morning, ahead of the opening of the London stock exchange at 8am. Lloyds Banking Group says it has undertaken an initial assessment of the impact of Friday’s supreme court judgment. Lloyds, which had previously set aside £1.2bn to cover compensation payments, has told the City that “whilst the judgment announced on 1 August provides additional clarity, there remain a number of uncertainties that the Group continues to consider in its approach to provisioning.” The bank says: After initial assessment of the Supreme Court judgment, and pending resolution of the outstanding uncertainties, in particular the FCA redress scheme, the Group currently believes that if there is any change to the provision it is unlikely to be material in the context of the Group. The provision will continue to be reviewed for any further information that becomes available, with an update provided as and when necessary. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. The latest twists in the UK car finance scandal could grip the City today, as investors try to estimate where the financial impact will land, and how heavy it will be. Yesterday afternoon, Britain’s financial regulator said it would open a redress scheme for consumers who were treated unfairly when they bought a vehicle using car finance, and “secret” commission payment were made to car dealers. The Financial Conduct Authority (FCA) will consult on the redress scheme, which could cost banks between £9bn and £18bn. Motorists who were mis-sold car finance were warned that they are likely to get less than £950 a claim. Nikhil Rathi, chief executive of the FCA, said last night: “It is clear that some firms have broken the law and our rules. It’s fair for their customers to be compensated. We also want to ensure that the market, relied on by millions each year, can continue to work well and consumers can get a fair deal.” “Our aim is a compensation scheme that’s fair and easy to participate in, so there’s no need to use a claims management company or law firm. If you do, it will cost you a significant chunk of any money you get.” “It will take time to establish a scheme but we hope to start getting people any money they are owed next year.” The FCA is acting after the UK supreme court partly overturned a landmark Court of Appeal case on hidden car finance commission claims on Friday, a move that looks like a partial win for lenders. The court rejected two claims which alleged that commissions paid to car dealers were bribes, and that dealers owed a duty of loyalty to the customer. As my colleague Kalyeena Makortoff explains here, the court appears to have closed the door to compensation except in more serious cases, although they did uphold a third case of a customer, Marcus Johnson, concluding that he had been treated unfairly. Martin Lewis, founder of MoneySavingExpert.com, has told Sky News the consultation is “likely to mean 40% of people who got a car finance deal between 2007 and 2021 will be due some form of redress, likely to be hundreds not thousands of pounds”. The Supreme Court ruling came just after the London stock market close on Friday night. The market reopens at 8am, so we’ll see how the City reacts to the verdict, and the FCA’s compensation scheme, shortly… The agenda 3pm BST: US factory orders report for June</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Investor confidence in the EU has fallen sharply after Donald Trump’s trade agreement with Brussels. Survey of thousands of investors in more than 20 countries showed that the pact was a “deal that dampens the mood” Switzerland, which was hit with a 39% tariff by Trump, is now indicating it might make the US a better offer.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>France’s prime minister, François Bayrou, said the EU had capitulated to Donald Trump, and the euro fell against the US dollar. But there has also been some relief that the US-EU trade deal may at least end the “will they, won’t they” speculation that has dominated the spring and summer. The dollar’s strength may be short-lived, according to Javier Corominas, director of global macro strategy at Oxford Economics, a consultancy. He said: FX markets have punished the greenback this year on two negative US-specific developments: heightened policy uncertainty and the negative real income shock for US consumers following the tariff announcements. On a relative basis, the latter is expected to be worse for US growth than the global demand shock experienced by exporters to the US, where some diversification to other markets might take place, much like the strategy China effectively pursued during the US President Trump’s first term. The uneven terms of the deal suggest that the EU has prioritised its short-term economic health over the longer-term arm wrestle with the US. Jan-Paul van de Kerke, a senior economist at Dutch investment bank ABN Amro, said: The unequal trade deal seems to be largely caused by Europe’s bad hand. Subpar economic performance and the recent bout of inflation meant national governments, especially in Berlin and France were unwilling to suffer economic pain to risk a better outcome. Furthermore, navigating member states’ deviating interests may have proved hard for negotiators. Finally, the EU remains dependent on the US for its security, both in terms of military support as for military imports and remains a net importer of energy. The EU commitment to $750bn of energy imports from the US over the next three years is “unfeasible”, as it would imply a doubling of European gas imports, he added. In other business and economics news today: The Russian airline Aeroflot was forced to cancel dozens of flights on Monday after a shadowy pro-Ukraine hacking group claimed responsibility for what it said was a crippling cyber-attack. Samsung has agreed a $16.5bn (£12.3bn) deal to manufacture artificial intelligence chips for Tesla, in a move hailed by Elon Musk. One of the world’s most prominent hedge fund investors, Ray Dalio, has warned that the UK is stuck in a “doom loop” as it faces a worrying mix of higher taxes, rising debts and slower growth. Britain is at risk of a worsening “climateflation” crisis amid the fallout from increasingly extreme weather that could drive up food prices by more than a third by 2050. Gambling lobbyists are staging a summer charm offensive designed to stop ministers from raising taxes on the sector, the Guardian has learned, including meeting with Treasury insiders and hosting a darts evening with Labour special advisers and MPs’ staff. You can continue to follow our live coverage from around the world: Thank you for reading today, and please do join me bright and early tomorrow for more of the same. JJ Donald Trump is answering questions from British media in Scotland. Amid comments on Gaza and immigration, Trump also suggested that US tariffs on pharmaceuticals are imminent. He said the US will be announcing pharma tariffs in the very near future, according to Reuters. It came after some confusion over whether pharmaceuticals will be included in the US-EU trade deal. Trump has claimed that medicines were not included, but European Commission president Ursula von der Leyen has said that the 15% baseline tariff agreed with Trump will apply. A senior US official later also said that they were in fact covered by the 15% tariff. Yet the confusion highlights the difficulty that many companies still face in working out what will happen if they export to the world’s largest market, despite a “deal” being agreed. (See also: UK steel imports are meant to attract zero US tariffs, but there has been no sign of that deal being honoured.) US stock market indices have risen on Monday at the opening bell on Wall Street – but it is not quite the jump that we saw at the open in Europe. Here are the opening snaps from Reuters: S&amp;amp;P 500 UP 8.37 POINTS, OR 0.13%, AT 6,397.01 NASDAQ UP 62.17 POINTS, OR 0.30%, AT 21,170.49 DOW JONES UP 38.02 POINTS, OR 0.08%, AT 44,939.94 The US dollar has strengthened against the euro in the wake of the trans-Atlantic trade deal, as investors appeared to welcome an easing in Donald Trump’s trade war. The euro dropped by 0.7% on Monday, with one euro buying $1.1648. That was a much bigger decline than other currencies relative to the dollar. The pound was down by less than 0.1%, with a pound buying £1.34. The euro’s decline came after an initial jump (just before halfway along in the below chart) as trading restarted after the weekend break, when Trump and European Commission president Ursula von der Leyen agreed the framework deal. However, investor sentiment quickly shifted to a stronger dollar. The question for investors will be whether that dollar strength will continue: many economists have said that tariffs – essentially taxes on US companies and consumers – will slow economic growth in the world’s largest economy. That would weaken demand for the greenback. The dollar has weakened notably over the course of 2025, with a euro buying 13 cents more than it did on 1 January. Dean Turner, chief eurozone and UK economist at UBS Global Wealth Management, said: From an investment perspective, news of the trade agreement is likely to initially play out in foreign exchange markets. This could provide some support to the US dollar in the short term as trade uncertainty fades. However, we would view any near-term rallies in the USD as opportunities to fade any strength, preferring to continue reducing or hedging USD exposures. Given the broader backdrop of easing trade tensions, our expectation remains that the dollar will gradually weaken into year-end. At lunchtime across Western Europe, stock markets appear to have settled down after the initial excitement of the reaction to the US-EU trade deal. The Stoxx 600, tracking the biggest European companies, is up 0.5%. Germany’s Dax index is flat, while France’s Cac 40 is up 0.3%. Interestingly, the Italian FTSE MIB in Milan is performing more strongly. The lead riser is STMicroelectronics, up 3% amid a broad move up by computer chip companies. Otherwise, Italian banks appear to be performing well, wikth Banco BPM, BPER Banca, Unicredit and Intesa Sanpaolo all up between 1% and 3%. The FTSE 100 is the worst performer of the big European stock markets (perhaps because it is not directly impacted by the trade deal – and has performed relatively well in recent weeks): it is down 0.2%. US futures also suggest that Wall Street indices will rise at the open in about 90 minutes. S&amp;amp;P 500 futures suggest a 0.2% increase, while the tech-focused Nasdaq is set to rise 0.4%. Heineken has said it could brew more beer in the US in order to try to avoid 15% tariffs on EU exports. The world’s second largest beer brewer, behind only AB Inbev, said that it the end of uncertainty around the tariff rate – with a threat of levies of up to 30% – was welcome. However, chief executive Dolf van den Brink said the Dutch company would look at the possibility of shifting some production. Reuters reports that he told journalists on Monday: We look at all options from... continuing with our current setup, a more hybrid version, or otherwise. If and when we deem them financially to be more attractive in the mid- to long-term, we would for sure explore them. Investing in breweries in the US would be costly, and would lock the company into producing with higher American labour costs. However, it could be attractive if if believes that the 15% tariffs will be in place for the long term. The FTSE 100 hit a new record in the opening trades this morning at 9,169.01 points – continuing the recovery from Donald Trump’s trade turmoil in April. London’s blue-chip companies have recovered and then some from the pummeling they and businesses around the world received from the trade war uncertainty. However, the index has lost its momentum in the late morning, and is now marginally down for the day. BT Group is the biggest faller, down 3.6%. UK retail sales slumped for the 10th consecutive month in July, according to a survey of the biggest shops that underlined the weakness of Britain’s consumer spending. A third of retailers said that sales declined in July, according to a survey weighted by the size of the business, according to the Confederation of British Industry, a lobby group – although that was an improvement from the 46% balance who said sales had declined in June. The retailers also reported worse expectations for next month. The last time retailers in the survey reported sales growth was September. Since then the UK economy has struggled, with the economy not helped by the huge uncertainty caused by US tariffs. Data from the Office for National Statistics, this month showed that Britain’s official unemployment rate rose to 4.7% in the three months to May, up 0.1% from April to reach the highest level since June 2021. Martin Sartorius, principal economist at the CBI, said: Retail annual sales volumes continued to fall in July, although the pace of decline moderated from June’s sharp drop. Firms reported that elevated price pressures – driven by rising labour costs – and economic uncertainty continue to weigh on household demand, which has contributed to sales volumes falling since October 2024. These trends of weak demand and uncertainty were mirrored across the wider distribution sector, with wholesale and motor trades also seeing declining sales. The UK economy will grow faster than previously thought after a stronger-than-expected start to the year, according to forecasters at EY – although some of the faster growth might have come from companies bracing for Donald Trump’s tariffs. The EY Item Club, which tries to mimic government modelling, has upgraded its forecast for UK GDP growth in 2025 from 0.8% to 1%. It said that came from a “significant increase in business investment, which rose by 3.9% in Q1”. However, this is thought to partly reflect the acceleration of business investment and purchase decisions by some companies in March, ahead of the implementation of US tariffs in April. That increase in business investment may not be sustainable in the second half of 2025, the forecasters said – and they do not expect any growth in business investment during 2026. Anna Anthony, a regional managing partner at EY,said: After a strong start to the year, uncertainty in the global economy and international trade policy has continued to slow momentum. While the agreement struck with the US offers welcome relief to certain sectors and boosts the trading outlook, the UK’s access to a key export market is still reduced from where it was at the start of 2025, which is likely to weigh on growth. Business investment is expected to remain modest until 2027 and while interest rate cuts should reduce debt service costs and make financing cheaper, this will take time to materialise. Until then, businesses face a period of international uncertainty, alongside elevated labour and energy costs. France’s prime minister, François Bayrou, has described the EU’s trade deal with the US as a “submission”. Writing on the X social network, Bayrou, who leads France’s government and is second only to President Emmanuel Macron, said: It is a dark day when an alliance of free peoples, united to affirm their values and defend their interests, resolves to submission. It is not, then, a rousing reception for the trade deal from EU leaders. However, the leaders are unlikely to try to derail the deal; indeed, complaining about EU policies while quietly accepting them is a well trodden path for leaders of individual countries. Russian airline Aeroflot has said it cancelled more than 40 flights on Monday “due to a failure in our information systems”, with an unverified online statement claiming it was the result of a hack. The state-owned airline announced the cancellations on the Telegram social network. It did not give a reason for the failures. However, an online statement purporting to be from a hacking group called Silent Crow claimed responsibility on Monday for an attack, Reuters reported. Aeroflot told passengers of cancelled flights at Moscow’s Sheremetyevo Airport to collect their previously checked baggage, and to leave the airport. Reuters again: News outlet Baza reported scenes of chaos at the airport, with logjams forming as passengers queued just to get out. Aeroflot has been limited mainly to internal flights since Russia’s full-scale invasion of Ukraine in 2022, as well as cities in allied countries like Minsk in Belarus. Yet it remains a crucial part of transport infrastructure across the world’s biggest country by geographical area. Also on the automotive chip front, the share price of South Korea’s Samsung Electronics jumped 6.8% on Monday after it agreed a semiconductor supply deal with Elon Musk’s Tesla. Musk said the companies signed a $16.5bn supply deal. Samsung agreed to allow Tesla and Musk access to the fab to “maximise manufacturing efficiency” for its newest chip, labelled A16. The deal will be seen as a major fillip for Samsung, which has struggled to keep up particularly with Taiwan’s TSMC when it comes to manufacturing the most advanced chips. It has also been a positive start for European semiconductor companies. A 15% tariff is bad news, but it is not a disaster for the sector – which is crucial to US ambitions to be the world leader in artificial intelligence. No European company is more crucial than ASML, the maker of the advanced lithography machines that use extreme ultraviolet light to etch transistors at the nanometre scale. Its machines are the only ones capable of making the world’s most advanced chips. Its share price gained 4% on Monday. STMicroelectronics, which supplies Apple and Tesla, rises 3.1% in Milan, Germany’s Infineon, which mainly serves the global automotive market, gained 2.2%. Germany’s car industry lobby group has expressed relief that the EU and US could reach a deal – but they are hardly overjoyed. Hildegard Müller, president of the German Association of the Automotive Industry (VDA), said it was “fundamentally positive” that the two sides had prevented further escalation of the dispute started by Donald Trump. However, she added: It is also clear that the US tariff of 15% on automotive products will cost German automotive companies billions annually and place a burden on them in the midst of their transformation. The hit to Germany’s carmakers is expected to come through lost sales if they pass the tariffs on to American buyers, or through a hit to their margins if they absorb the cost themselves. Either way though, the tariffs will function effectively as a tax on US consumers, who must either pay a higher price, or else see protected US manufacturers able to raise prices themselves. The relief for European carmakers is clear. The 15% deal averted a 30% tariff on 1 August. Mercedes-Benz’s share price rose 1.8% to its highest since late March, and Porsche gained 1.7%. Volkswagen gained 0.8%, although its gained were limited by a cut in guidance from its premium brand, Audi, which cut its sales forecasts by a further €2.5bn because of the tariffs. Reuters reported: Audi now expects revenue between €65bn and €70bn, down from a previous range of €67.5bn to €72.5bn, and an operating margin between 5 and 7%, down from a previous range of 7 to 9%. Stellantis, a group forged from a mixture of brands spanning from Detroit, to Italy and France, gained 1.2%. Investors might be cheered, but the reaction this morning from European leaders to the EU’s trade deal with the US is decidedly mixed. Hungary’s prime minister, Viktor Orbán, has long been one of the most divisive voices within the EU, and he wasted no time in criticising European Commission President Ursula von der Leyen for what he described as a worse deal than the UK managed to secure. According to Reuters, Orbán told a podcast: This is not an agreement ... Donald Trump ate Von der Leyen for breakfast, this is what happened and we suspected this would happen as the US President is a heavyweight when it comes to negotiations while Madame President is featherweight. Belgium’s prime minister, Bart de Wever, struck a different tone – firmly placing the blame for tariffs on Donald Trump. He posted on the social network X: This is a moment of relief but not of celebration. I sincerely hope the United States will, in due course, turn away again from the delusion of protectionism and once again embrace the value of free trade – a cornerstone of shared prosperity. In the meantime, Europe must continue to deepen its internal market, cut unnecessary regulation, and forge new partnerships to diversify our global trade network. May Europe become the beacon of open, fair, and reliable trade the world so urgently needs. Good morning, and welcome to our live coverage of business, economics and financial markets. Global stock markets have rallied after the US and EU agreed a trade deal, removing a major source of uncertainty for companies around the world even as it promised a permanent cost to trans-Atlantic goods trade. European stock markets surged on the opening bell on Monday, a day after US President Donald Trump and European Commission President Ursula von der Leyen, shook hands on a deal in Turnberry, Scotland, on Sunday. Germany’s Dax rose 0.8% in early trading, France’s Cac 40 gained 1%, while Spain’s Ibex gained 0.8%. The FTSE 100 in London gained 0.5%. Asian stock markets also mostly rallied. Australia’s ASX200 rose by 0.4%, Hong Kong’s Hang Seng rose 0.4%, Korea’s Kospi index gained 0.6%, while Shanghai’s CSI300 gained 0.1%. However, Japan’s Nikkei 225 fell by 1% amid doubts over the details of its own trade deal with the US. The US-EU deal will put a 15% US tariff on most imports from the EU, including cars and computer chips. Steel and aluminium still face 50% tariffs – but only above certain quotas. There are zero tariffs on aerospace parts, some chemicals and raw materials. The EU will also agree to buy $750bn in US energy, and more military equipment – both of which fit with moves since Russia’s invasion of Ukraine in 2022. There is good news and bad news in the deal, said Holger Schmieding, chief economist at Berenberg, an investment bank: The crippling uncertainty seems to be largely over. The trade deal which the US and the EU struck in Scotland on Sunday with a 15% tariff on most US goods imports from the EU is bearable for the EU, much more so than the 30% tariff would have been which US president Donald Trump had threatened before. However, the outcome remains much worse than the situation before Trump started his new round of trade wars early this year. The extra US tariffs will hurt both the US and the EU. […] The trade tensions with the US will subtract a cumulative 0.3 percentage points from European and 0.5 percentage points from German growth in 2025 and 2026 taken together. The deal is asymmetric. The US gets away with a substantial increase in its tariffs on imports from the EU and has secured further EU concessions to boot. The agenda 11am BST: UK Confederation of British Industry distributive trades (retail) survey (July; previous: -46%; consensus: -26%) 12:30pm BST: Donald Trump press conference in Scotland</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Dollar’s strength may be short-lived, according to Javier Corominas. uneven terms of the deal suggest that the EU has prioritised its short-term economic health over the longer-term arm wrestle with the US. The EU commitment to $750bn of energy imports from the US over the next three years is ‘unfeasible’</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Americans are getting married, having kids, buying a home, and retiring years later than what once was the norm. Many don’t ever reach these milestones. While there is a complex web of factors that go into decisions like having kids or buying a house, a person’s financial situation often plays an major role. In a May Harris/Guardian poll, six out of 10 Americans said that the economy had affected at least one of their major life goals, because of either a lack of affordability or anxiety about where the economy is heading. The Guardian heard from hundreds of readers who shared their stories about how the current economic and political climate has put some of their biggest life decisions on hold. For Martha Knight, the idea of having kids has been a complicated one. In terms of finances, home ownership seems far out of reach. Home prices in Louisville, Kentucky, have soared over the years. While prices are cheaper outside the city in more rural areas of the state, a move would affect their jobs in education and healthcare. And both Knight and her husband have student loan debt. Instability around forgiveness programs have made them question how long it will take them to pay off their debt. “We made peace with the fact that we will probably rent our whole lives, and we’re OK with that,” Knight, 34, said. “That’s where we are.” Besides owning a home to raise a family, there are also deeper questions: What would it be like to raise a child in the world we live in now? It’s a hard question for Knight, who is from eastern Kentucky along the Appalachian mountains. Kentucky is her home state, it’s where she and her husband grew up. But she doesn’t see it as a place where she can raise a family. In 2023, the US fertility rate dropped to its lowest point in almost a century. “We are one of the highest states for child hunger, for the foster care system, things like that,” Knight said. “If we ever have a child, if we are fortunate enough for that to happen, we are really hoping to give them a better future. We want them to grow up with the idea of possibility. As the state is currently, Kentucky doesn’t offer that.” Anxiety about the future didn’t start under Trump’s second administration. The pandemic threw the economy into a tailspin. While the stock market soared, inflation hit a generational high in 2022, and Americans are still feeling the pain of higher bills. And even though mortgage rates have climbed with higher interest rates, housing prices still remain at record highs. In other words, it’s been hard to catch a break. Although Trump promised to provide economic relief, the administration has caused widespread uncertainty for some respondents with his erratic tariff policies and attacks on minority groups and reproductive rights. Danielle, 35, who requested to be identified by her first name only, said that she’s held off on buying a home and having kids given the instability. “I love the community I built here, but as a queer person, I’ve been hesitant to buy a home and even have kids due to rigid abortion bans and economic instability,” said Danielle, who currently lives in Austin, Texas. “This is no longer the country I knew nor grew up in. The American Dream is a farce.” While student loan debt has been a huge barrier to home ownership for many millennials, the Save plan, the Biden administration’s hallmark loan forgiveness program, allowed Stephen Buechel-Rieger, 32, of Cincinnati, Ohio and his partner to purchase their first home. Their goal was to eventually purchase a larger home to accommodate a growing family, but “we have been delaying moving from our first home to our forever home,” Buechel-Rieger said. “Now because of the increase in student loan payments, uncertainty of the future of the Public Service Loan Forgiveness program, stubborn interest rates and uncertainty in the medical field, we cannot take the financial risk,” Buechel-Rieger said. High home prices don’t just affect millennial buyers. William Pollard Jr, 71, said he and his wife have been wanting to move out of Florida to live closer to family, but prices have been too high to buy a new home. “With the stock and bond markets bouncing everywhere, we cannot put together an account to buy a house elsewhere. The markets need to be stable, so we can build more wealth,” Pollard said. “I am very frustrated at having to put a major goal on hold for who knows how long … I am getting no younger. We want to live the rest of our years near family and friends.” Many Americans also said that they were holding off on big purchases, which may not appear to hold the weight of major life decisions, but also play a huge role in people’s lives. Hunter Gale, 39, of Kansas City, Missouri, said his wife is expecting in September, and the family is hoping to purchase a car that will be safer for their new baby. Uncertainty around tariffs, along with the higher cost of baby products, have made it harder to get a better car. “While we are fortunate to have stable jobs and a home that can fit our expanding family, it is stressful knowing costs for essentials for our baby will be higher,” Gale said. When people buy homes and have kids later in life, that often pushes up the retirement age. It’s no surprise, then, that the average age of retirement was 62 in 2024 – five years older than what it was three decades ago. And many Americans continue to hold it off because of economic anxiety. Swantje Agápe, 57, of San Jose, California, said that she and her husband were looking to retire in the next year, but “politically and economically things are too unstable”. “We are no longer confident that three retirement funds and plans we have will be sufficient,” Agápe said. “We are both feeling quite sad and frustrated. After working hard all our lives, we were both really looking forward to an early-ish retirement.” Diane Alaine Bates, 65, of Kenmore, Washington, said that she similarly had been delaying retirement for months because of the instability. “I’ve been scared since the election that tariffs will cause a recession,” Bates said. “I need to know if my 401(k) is going to be stable enough to retire.” People delaying these major life decisions don’t just affect individual lives. On a societal level, the impacts are huge. When people retire later, that leaves less room for younger workers to move up in the workforce. When birth rates drop, it can lead to an ageing population that puts a strain on the healthcare system. And philosophically, it seems to raise questions about agency and freedom. What happens when people feel like larger political and economic forces are controlling their lives? For some, the solution is to leave. Many told the Guardian that they were making plans to leave the country, but for those who don’t have foreign passports, crossing state lines appears to be the next best option. Knight said that she and her husband plan to leave Kentucky for Washington state, which they hope will be a better environment for their family. “We have specifically chosen a blue state that offers some social safety nets. In Washington, they have state paid parental leave, you know, things that will help us hopefully find our feet,” Knight said. “It’s the choice of: do we stay? Do we stay with our community? Do we stay with our families? Or, for our future, do we move and give ourselves a better chance?”</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Six out of 10 Americans said that the economy had affected at least one of their major life goals. The Guardian heard from hundreds of readers who shared their stories about how the current economic and political climate has put some of their biggest life decisions on hold.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Time to wrap up… Rachel Reeves could “easily” breach fiscal rules if growth disappoints or rate shocks materialise, the IMF has warned. While the new Labour government has embarked on a “bold agenda”, the IMF said, delivering it will require overcoming “significant challenges” amid shockwaves from the trade war and the confines of tight fiscal headroom. The British government could reduce pressure for “overly-frequent changes to fiscal policy” by introducing more headroom, the IMF said in the final version of an annual report on Britain’s economy. British retail sales rise in June, official figures show There is some positive news for the retail sector this morning, with official figures showing that monthly sales rose in June by 0.9%. It follows a fall of 2.8% in May. That was helped by warm weather, with supermarkets reporting better trading and an increase in drink purchases, the Office for National Statistics has said. NatWest investors given £1.5bn weeks after full privatisation NatWest will give a further £1.5bn to shareholders only weeks after the UK government sold the final part of its stake in the once bailed-out bank. The high street lender on Friday announced plans to distribute an interim dividend of 9.5p a share, worth a collective £768m, on top of a fresh £750m share buy-back in the second half of the year. It came as the bank beat market forecasts with a 4.4% rise in second-quarter profits to just under £1.8bn, thanks in part to higher income linked to its takeover of Sainsbury’s banking business, which it snapped up last year. US stocks have opened slightly higher, with the blue chip S&amp;amp;P 500 index up 0.14%. The tech heavy Nasdaq index is up by 0.1%. Intel is one of the worst performers, with its shares down by as much as 9.7% after the chipmaker told investors yesterday that it forecasts steeper losses in the third quarter than Wall Street had expected. Pressure is building on Rachel Reeves to find new ways to strengthen public finances, but calls for a wealth tax in some parts of the Labour party are “daft”, the business secretary Jonathan Reynolds has said. Speaking to GB News, Reynolds said: This Labour Government has increased taxes on wealth as opposed to income – the taxes on private jets, private schools, changes through inheritance tax, capital gains tax. But the idea there’s a magic wealth tax, some sort of levy ... that doesn’t exist anywhere in the world. Switzerland has a levy, but they don’t have capital gains or inheritance tax. There’s no kind of magic ... We’re not going to do anything daft like that. And I say to people: ‘Be serious about this.’ The idea you can just levy everyone ... What if your wealth was not in your bank account, what if it was in fine wine or art? How would we tax that? This is why this doesn’t exist. There’s a lot of populism out about this, and I’m frustrated. I see colleagues sometimes say this in Parliament and I say: ‘Come on, get serious’. Earlier this month former Labour leader Neil Kinnock said the government should be bolder and consider a tax on wealth. However, critics argue that such a levy would be difficult for the tax authority to implement in practice. The Nationwide board has come under fire at their AGM, with members calling the building society’s plans to hike CEO Debbie Crosbie’s max pay package by 43% to £7m an “obscenity”. One member, Mr Fisher, asked: Does the CEO see both the irony and the hypocrisy of the size of her bonus: an amount in one year that most people would struggle to spend in a lifetime? While another, Ms Andrews said: “no one needs to earn more than £1m in salary, and certainly not £7m.” Another, Dr Standon, said Nationwide already had the option of paying Crosbie up to £4m, and that pushing that figure to £7m was “an obscenity”. “One would expect Nationwide to set an example to others,” he said. Standon added that while Nationwide expressed principles of mutuality - prioritising people over money and profits - there seemed to be a mismatch in the way it justified the hike, saying it was essential to attract and recruit talented executives. It suggests that unfortunately, your executive team are primarily motivated by money.” She said if executives jumped ship as a result “that would be such a disappointment. But if they do leave purely because of the money, then, is it not the case that they were not in line with Nationwide principles in the first place?” Nationwide’s chairman Kevin Parry said: I don’t think that money is the primary motivation….I’m very confident in saying this is not about personal greed. This is about equity with people that do similar jobs elsewhere. Meanwhile, Tracey Graham, the chair of Nationwide’s remuneration committee said: Our job is to ensure that we have the very best leaders here at Nationwide, and we do operate in a competitive marketplace, and that is what we need to pay them. For us to believe that we are paying them equally or fairly - not as much as the banks, certainly - but we believe that they are performing and paid appropriately. We’d be delighted if the very stretching performance targets that we have set over this period of time are met.” The UK could easily breach its fiscal rules if economic growth disappoints or rate shocks materialise, the International Monetary Fund has warned. While the new Labour government has embarked on a “bold agenda”, the IMF said, delivering it will require overcoming “significant challenges” amid shockwaves from the trade war and operating within the confines of tight fiscal headroom. The British government could reduce pressure for “overly-frequent changes to fiscal policy” by introducing more headroom, the IMF said in the final version of an annual report on Britain’s economy. In an uncertain global environment and with limited fiscal headroom, fiscal rules could easily be breached if growth disappoints or interest rate shocks materialize. …The first best [option] would be to maintain more headroom under the rules, so that small changes in the outlook do not compromise assessments of rule compliance. Chancellor Rachel Reeves said in a statement that her plans would “tackle the deep-rooted economic challenges that we inherited in the face of global headwinds.” Our fiscal rules allow us to confront those challenges by investing in Britain’s renewal. We’re committing billions of pounds into improving transport connections, providing record funding for affordable homes, as well as backing major projects like Sizewell C to drive economic growth. There’s more to do, and that’s why we’re slashing unnecessary red tape and unblocking investment to let British businesses thrive and put more money in working people’s pockets.” The IMF warning comes as Reeves faces intense pressure to respond to a worsening economic outlook with a new round of tax rises in her autumn budget. Official figures showed this week that the UK government borrowed more than expected in June, with net borrowing rising to £20.7bn, up by £6.6bn compared with the same point a year ago. It was the second highest June borrowing figure since monthly records began in 1993. The Fund forecast that the UK economy would grow by 1.2% in 2025, followed by 1.4% in 2026, although it noted that “risks to growth are tilted to the downside”. It warned: Tighter-than-anticipated financial conditions, combined with households maintaining high savings rates for precautionary reasons, may hinder the rebound in private consumption and slow the recovery. In an environment of weak growth, persistent inflationary pressures may create “stagflation” risks, complicating the monetary policy stance and putting pressure on public finances. A significant rise in commodity prices due to international conflicts could further aggravate the situation. It is bad news for British holidaymakers as the pound dropped to as low as 1.1458 against the euro this morning, its weakest since April. The fall comes after a hawkish message from the European Central bank yesterday, with traders paring back bets that it could deliver another interest rate cut this year, and expectations growing that the EU is about to secure a trade deal with the US. Meanwhile market watchers broadly expect at least one more interest rate cut from the Bank of England this year. Weaker retail sales in June have also not helped the pound, as well as data yesterday that showed British businesses are cutting jobs at the fastest pace since February, partly in response to higher taxes. The pound also fall against the US dollar on Friday, down by 0.4% to $1.346. Former Barclays chief executive Jes Staley is not appealing last month’s Upper Tribunal ruling, leaving him banned from the City for life for misleading the watchdog over his relationship with the sex offender Jeffrey Epstein. Staley will now have to pay the Financial Conduct Authority a £1.1m fine by 6 August. The FCA noted on its website on Friday morning that the “expiry” date for Staley to seek permission to appeal the decision had passed. Staley would have had to submit a challenge by 10 July but failed to do so. That paved the way for the FCA to issue a final notice over the ban and its £1.1m fine over the matter. The case centred on a letter that Barclays sent to the FCA in 2019 that stated Staley “did not have a close relationship” with Epstein and his last contact with the financier was “well before” he joined Barclays four years earlier in 2015. However, a subsequent investigation by the FCA – triggered by a cache of 1,200 emails from Staley’s former employer JP Morgan – concluded that the pair were “indeed close” and had a relationship that “went beyond one that was professional in nature”. Staley resigned from Barclays in 2021 over preliminary findings from the FCA’s investigation. He eventually appealed their decision to ban him from the City, leading to a two-week hearing in London in March. The Upper Tribunal ruled against Staley in June, saying: “We agree with the [Financial Conduct] Authority (FCA) that Mr Staley’s breaches of the authority’s rules represented a serious failure of judgment by Mr Staley.” Staley’s lawyer has been contacted for comment. Retail sales were positive in June, but British shoppers are still in a cautious mood ahead of possible tax rises later this year, according to the latest consumer confidence index from market research firm GfK. The index dipped to -19 in July from a six-month high of -18 in June. Economists polled by Reuters had mostly expected a reading of -20. Neil Bellamy, consumer insights director at GfK, said people “may be sensing stormy conditions ahead”. With speculation growing over possible tax rises in the Autumn budget, and price pressure contributing not just to higher inflation already but also to the likelihood of worse inflation to come, the news is worrying. Finance minister Rachel Reeves is expected to raise taxes for a second year in a row in her next annual budget plan after Prime Minister Keir Starmer was forced into u-turns on plans to save billions of pounds on welfare spending. GfK’s savings index … jumped seven points to +34, its highest level since November 2007, shortly before the global financial crisis deepened. European stocks are down by 0.6% this morning, led by the German sportswear brand Puma. Shares in the company dropped by as much as 18.7% after it said it expects US trade tariffs to cost it €80m in gross profit this year, and that it now expects to make a loss in adjusted earnings before interest and taxes. Much of the sportswear industry faces higher costs due to US trade tariffs, as they rely on manufacturing in China, Vietnam, Cambodia, and Bangladesh. Puma’s chief executive Arthur Hoeld, who started in the role this month and was formerly sales chief at Adidas, said the company needed to “course-correct”. This year, 2025, will be a reset for Puma and 2026 will be a transition year for us … We as a company need to take a hard look at ourselves. Chief financial officer Markus Neubrand said Puma would increase prices in the US in its fourth quarter, partly to mitigate the tariff impact, but declined to say how much prices would rise. All eyes will be on the European Union next week as it tries to secure a trade deal with the US ahead of Trump’s 1 August deadline. Negotiators are nearing a deal that would place 15% tariffs on most imports from the bloc, which would mirror a deal struck this week between the US and Japan. Kathleen Brooks, of the broker XTB, has noted however that more hawkish noise from the European Central Bank may also be weighing on appetite for European stocks. A more hawkish than expected ECB has soured the mood for European equities, after Christine Lagarde quashed hopes that the ECB will cut rates again in September. The interest rate futures market is pricing in a 15% chance of a rate cut in September, down from a 42% chance before Thursday’s ECB meeting. There was also some earnings disappointment, with LVMH reporting weaker sales, as consumers continued to shun LVMH’s luxury pricy brands, however, its share price is rising on Friday, as hopes rise for a turnaround in the future. This is why European yields are rising again on Friday and yields in France and Germany are higher by 14 and 15bps this week, suggesting that the market is sensitive to the potential floor in European rates at 2%. Bitcoin fell alongside other high-risk assets on Friday, as hopes for a rate cut from the Fed next week begin to fade. The cryptocurrency dropped to a low of $115,122, its lowest level since 11 July. It comes after Bitcoin hit an all-time high of $123,205 last week, driven by optimism around a more welcoming regulatory environment in the US, which has helped boost demand for crypto products. Bitcoin has rallied by 24% against the US dollar in the year to date. In case you missed it overnight, Donald Trump and Jerome Powell, the Federal Reserve chair, clashed last night during a state visit to inspect the renovation of the central bank’s historic headquarters in Washington. The president claimed the total cost of the renovations was $3.1bn, higher than previously reported. As Trump made this claim, Powell shook his head and said: “I’m not aware of that. I haven’t heard that from anybody at the Fed.” Having branded Powell a “numbskull” for the Fed’s recent decisions not to cut rates, Trump has pressured Powell with criticism of the $2.5bn bill for renovating the Fed’s historical buildings. However, Trump backed away from earlier suggestions that he would fire the Federal Reserve chair: To do that is a big move, and I just don’t think it’s necessary, and I believe he’s going to do the right thing. The president’s visit to the Fed comes less than a week before the central bank’s 19 policymakers gather for a rate-setting meeting. They are widely expected to leave the benchmark interest rate in the 4.25% to 4.5% range. Markets have opened weaker in Europe this morning. Britain’s blue chip FTSE 100 index has slipped 0.2%, while Germany’s Dax has slipped 0.8%. The French CAC 40 index has dropped 0.5%, and the pan-continental Euro Stoxx 600 has slipped 0.4%. In the UK, NatWest is leading the FTSE 100, with its shares trading up 1.2%. The property search platform Rightmove is at the bottom of the pack, with its shares down 2.9% after it warned of slower growth in the second half of the year. Over in the FTSE 250 index, shares in Mitchells &amp;amp; Butlers have risen by more than 4% at the open, after the pub chain reported that recent sunny weather has helped it grow its sales by 4.5% in the 42 weeks ended on 19 July. Phil Urban, chief executive of the company, said this morning that its strong performance meant that it could meet “cost challenges facing the sector”. Meanwhile, shares in Marshalls have dropped by 24.4% after the building materials company issued an unscheduled trading update this morning. It cut its full-year expectations due to macroeconomic uncertainty and said it expects no improvement for the rest of the year. Strong figures from NatWest this morning as it reports its first quarter as a fully privatised bank. The lender has announced a £750m share buyback and raised its guidance for the year. Pre-tax profits of £1.8bn in its second quarter beat expectations, and the bank has told investors that it now expects income for the year to land above £16bn, compared with previous guidance of between £15.2bn and £15.bn. NatWest announced its return to full private ownership at the end of May, ending more than a decade as the government sold the last of its shares in the bank after its bailout in 2008. Shares in NatWest have risen by roughly a quarter in the year to date, as banks have also broadly benefited from interest rates falling at a slower rate than expected. Zoe Gillespie, of the wealth manager RBC Brewin Dolphin, has said the strong figures suggest NatWest’s big turnaround project has taken hold. Its strategy of simplification, cost reduction, and technology integration – combined with sensible bolt-on acquisitions – is driving income growth and greater profitability. The addition of Sainsbury’s Bank, in particular, provides a real platform for further growth in UK retail banking. Now fully in private ownership, NatWest has a freer hand to make its next big strategic move and, in the interim, shareholders are being well rewarded for their patience with a sizeable dividend increase and share buyback programme. There is however a rather gloomy note in NatWest’s results, tucked under the bank’s notes on potential economic scenarios. Since 31 December 2024, the near-term economic growth outlook has weakened. This was mainly due to the weaker economic performance in the second half of 2024 and the drag from international trade policy related uncertainty. Inflation has risen, with underlying price pressure remaining firm, particularly on services inflation. As a result, inflation is assumed to remain a little higher than 3% through most of 2025, taking longer to fall back to the target level of 2%. The labour market has continued to cool. The unemployment rate peak is now assumed to be modestly higher than at 31 December 2024, but it is still expected to remain low. The Bank of England is expected to continue cutting interest rates in a ‘gradual and careful’ manner with an assumed terminal rate in the base case of 3.5%. The housing market continues to show signs of resilience, with prices still expected to grow modestly. There is some positive news for the retail sector this morning, with official figures showing that monthly sales rose in June by 0.9%. It follows a fall of 2.8% in May. That was helped by warm weather, with supermarkets reporting better trading and an increase in drink purchases, the Office for National Statistics has said. While growth is encouraging, the numbers are weaker than expected. A poll by Reuters showed that economists had been expecting a monthly rise of 1.2%. Jacqui Baker, head of retail at RSM UK and chair of ICAEW’s Retail Group, warns that the sunny mood music may not last long. While the June figures are welcome news and consumer confidence ticked up last month, nervousness among consumers persists, and the unexpected rise in inflation won’t have helped. The higher price of essentials such as food and fuel will only add to the reluctance among consumers to spend as their discretionary income shrinks. Concerns remain in the sector, as retailers increasingly run out of headroom to mitigate rising costs. Many will be hoping the government steps in to provide meaningful reductions in business rates, as well as raising the threshold at which employers’ National Insurance becomes payable. It’s also hoped that the reintroduction of tax-free shopping is brought back on the table, so the sector doesn’t miss out further on valuable retail spend.” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Donald Trump, who is due to arrive in Scotland on Friday for a five-day golf trip, is expected to meet with Keir Starmer early next week as the prime minister pushes to finalise their deal on steel trade tariffs. In May, the US agreed to lift tariffs on steel imports from the UK, which currently stand at 25%. However, there are concerns that the steel must be melted and poured in the UK, which could exclude Tata Steel UK as it closed its last blast furnace last year. It has been importing steel from its sister plants in India and the Netherlands, which it then processes in the UK. Starmer is expected to argue for building closer trade ties with the US, including cutting tariffs on Scotch whisky, according to a report by the Financial Times. White House press secretary Karoline Leavitt told reporters this week: “On Friday morning, President Trump will travel to Scotland for a working visit that will include a bilateral meeting with Prime Minister Starmer to refine the historic US-UK trade deal.” The talks will come after Stamer sealed a tradel deal with India on Thursday. The agreement, which is the biggest struck by Britain since Brexit, will cut back the cost of India’s tariffs for the UK and improve exports of products such as Scotch whisky and cars. Starmer told Bloomberg that his government had “re-established the place and position of the UK on the world stage.” “We’re seen as a country which other countries want to be working with and delivering with.” The agenda 7.00am BST: ONS retail sales data 7.00am BST: NatWest Q2 results 11.00am BST: Nationwide AGM</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Official figures show that monthly sales rose in June by 0.9%. It follows a fall of 2.8% in May, helped by warm weather. NatWest will give a further £1.5bn to shareholders weeks after full privatisation.</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Christine Lagarde appeared to be in relatively relaxed mood this afternoon as she took questions from the press pack in Frankfurt: she said the European Central Bank is in a “good place” – or as good as it can be with the threat of Donald Trump’s tariffs. The ECB will be “data-dependent” on whether the next move in interest rates is up or down, she said repeatedly. She said that the prospect of a 15% tariffs between the EU and US remained “conjecture”, but suggested the ECB would not exclude any actions depending on what happens with the trade war. David Rea, chief economist for Europe at JLL, a property company, said: The ECB’s decision to hold rates indicates it is keeping its powder dry as the economic situation continues to evolve. The bank is already significantly ahead of most central banks in terms of rates cut, and so the continuation of the neutral policy now means the ECB is in a good position to move rates in whichever direction necessary in future without the need for large swings. Charlie Cornes, senior economist at the Centre for Economics and Business Research, said: While inflationary pressures have eased considerably and the growth outlook for the Eurozone still relatively subdued, there is impetus for the ECB to move further with its loosening cycle. That said, uncertainty amidst ongoing trade negotiations with the US are holding the ECB back. Maintaining its commitment to price stability, the ECB is likely to proceed cautiously. As such, we expect that the ECB will conduct only one further rate cut before the end of 2025. In other business news: President Donald Trump said on Thursday he would not destroy Elon Musk’s companies by taking away federal subsidies and that he wants the billionaire tech-entrepreneur’s businesses to thrive. “Everyone is stating that I will destroy Elon’s companies by taking away some, if not all, of the large scale subsidies he receives from the U.S. Government. This is not so!,” Trump said in a post on Truth Social. “I want Elon, and all businesses within our Country, to THRIVE.” Tesla sales in Europe have collapsed by one-third this year, data shows, after Elon Musk warned the electric carmaker faced “a few rough quarters” ahead. Donald Trump will heap further pressure on the chief of the Federal Reserve, Jerome Powell, on Thursday when the US president makes a visit to the central bank’s Washington offices. UK businesses are cutting jobs at the fastest pace since February in response to higher taxes and global uncertainty caused by Donald Trump’s tariff threats. Britain may have lower gas stockpiles going into the winter after the owner of British Gas indicated it plans to sell its stored gas to help reduce losses at a North Sea gas storage facility. The boss Lloyds Banking Group has warned Rachel Reeves that increasing taxes on banks in her autumn budget would damage Labour’s plan for the City of London to power an economic recovery. You can continue to follow our live blogs from around the world: Or else why not follow the test match in our sports coverage. Thanks for following today. JJ US markets have followed the lead of European indices, rising at the opening bell on Wall Street. Here are the opening snaps, via Reuters: S&amp;amp;P 500 UP 11.91 POINTS, OR 0.19 %, AT 6,370.82 DOW JONES DOWN 314.67 POINTS, OR 0.70%, AT 44,695.62 NASDAQ UP 80.58 POINTS, OR 0.38%, AT 21,100.59 It is not possible to have more anticipation of the future rate path at this point because of the uncertainty around the trade war, says Christine Lagarde. We will just have to wait and see, Lagarde says – before wishing everyone a rest as Europe heads on its holidays. A German ECB member argued last week that there was a “high bar” for future interest rate cuts. Christine Lagarde says that while some members of the ECB’s governing council have different preferences, there was a “unanimous decision to keep interest rates unchanged. Could rates even go up? If trade tensions are resolved in short order it will clear some of the uncertainty that we have weighing on decisions, she says: Could it lead to different movements? Future will tell. Our work will tell. I will not exclude anything. The jury is out as to how quickly the uncertainty will be cleared, says Christine Lagarde, referring to the trade war launched by Donald Trump. On the ECB’s position, she says: You could argue that we are on hold. We are in this wait and watch situation. Asked about the US’s push to dominate the market for stablecoins, Lagarde says the eurozone is pushing to create its own digital euro, but: Cash will always be there, and banks will still be there intermediating the process. Asked if there is a risk of undershooting on the inflation target, Christine Lagarde points out that the ECB is forecasting an undershoot. However, the central bank will not deviate from its plans on the basis of minor movements in inflation figures, she says – they will focus on 2% over the medium term, rather than worrying about dipping below 2% temporarily. Asked about retaliatory tariffs, Lagarde says the ECB is looking at different rates of retaliatory tariffs in various scenarios – but it is too complicated to work out what will happen yet. For the moment the ECB assumes the trade war will be inflationary, but there could also be bottlenecks and supply chain changes which will all come together to impact prices, she says: There is a lot of uncertainty out there… At this point in time the conclusion is not definite as to which of those forces will prevail. We are in a good place because inflation is at 2%, says Christine Lagarde. Wages are heading in the right direction and are showing a downward trend as expected, she says. We have seen growth developing in a relatively favourable way, she adds. She repeats caveats about the relative strength of first-quarter growth, noting again the “front-loading” of companies to get ahead of US tariffs. Nevertheless, she says there was also some consumption supporting growth. And she appears comfortable with lower rates: The inflationary shock of the past few years is behind us. Our job is now to look at what’s coming. Asked about exchange rates, Christine Lagarde says the ECB does not target a particular exchange rate. On the US’s trade talks with the EU, Lagarde says reports the two sides are reaching a deal are still “conjecture”. However, “We are attentive to where the negotiations are heading”, she says. We take news one day at a time and at the moment we are relying on our baseline models from June, Lagarde says. The sooner this trade uncertainty is resolved… the less uncertainty we will have to deal with. That would be welcome by any economic actors, including ourselves. The ECB will follow a “data-dependent and meeting-by-meeting approach”, Christine Lagarde repeats. The ECB’s governing council is determined to keep inflation at its 2% target, she adds. And with that she will take questions. Risks to economic growth remain tilted to the downside, Christine Lagarde says – hardly a surprise when Donald Trump is looking at the US’s relationship with the EU. Russia’s invasion of Ukraine and the “tragic” conflict in the Middle East also add to uncertainty, she says. The path of inflation is more uncertain than normal because of the trade tensions, she says. Inflation could be higher if trade disruption disrupts supply chains, she adds, as happened during the coronavirus pandemic. Higher investment in defence and infrastructure should support growth, Christine Lagarde says. She repeats the endless call of ECB officials to strengthen integration of the eurozone and its banking system. And then she goes into the easing inflationary pressures. Forward-looking indicators point to a further decline in wage growth, and consumer inflation expectations declined recently, she says. Christine Lagarde takes to the podium in Frankfurt after leaving interest rates unchanged. She starts by reading out the decision. The economy grew more strongly than expected as companies “front-loaded” exports to avoid tariff hikes, but growth was also bostered by consumption, she says. Higher expected tariffs, a stronger euro and persistent uncertainty are making firms unwilling to invest, she says. Could 2% be the end of the road for the latest rate cutting cycle? Mark Wall, chief European economist at Deutsche Bank, said: As effectively telegraphed by Lagarde, the ECB paused the easing cycle in July. The question is, will this be a short pause or a long pause? And could this be a pause that sees 2% policy rates eventually become the terminal rate in this easing cycle? Uncertainty remains high and the ECB rightly wants to keep its options open. But if trade uncertainty fades, the combination of a resilient economy and significant fiscal easing will eventually translate into upside risks to inflation. Markets are not far away from switching focus from the last cut to the first hike. We will hear what Christine Lagarde has to say very shortly. There is very little reason for the ECB to leave its “good place” of standing on the sidelines waiting for more trade developments, said Carsten Brzeski, global head of macro at ING, an investment bank. In a note to clients, he said: After seven consecutive 25 basis point [0.25 percentage point] rate cuts and a total of 200 basis point rate cuts since September 2023, the European Central Bank kept its policy interest rates on hold at today’s meeting. A stronger euro had argued for further cuts, Brzeski said, but that pressure diminished as the euro eased. Not only did the euro’s appreciation come to an end, but the repeatedly postponed showdown in the US-EU trade negotiations also offered another reason to stay put today and keep the powder dry. Still, with two more weaker inflation prints and hard macro data weaker than soft data over the summer, we can still see one final rate cut at the September meeting. The ECB said in its monetary policy decision that the European economy has “proven resilient”, but flagged “exceptionally uncertain” conditions caused by Donald Trump’s trade wars. The central bank said it would take a “meeting-by-meeting approach” on deciding the path of interest rates – and it would not commit to a rate path now. It said: Domestic price pressures have continued to ease, with wages growing more slowly. Partly reflecting the governing council’s past interest rate cuts, the economy has so far proven resilient overall in a challenging global environment. At the same time, the environment remains exceptionally uncertain, especially because of trade disputes. The European Central Bank has left its monetary policy unchanged, after a run of eight quarter-percentage-point cuts in the space of the last year. The ECB’s main policy rate will remain at 2%, while its deposit rate will stay at 2.15%, the Frankfurt-based central bank announced on Thursday. The policy rate has halved from 4% to 2% in an effort to spur the European economy, after inflationary pressures fell back. There are a few minutes left before the European Central Bank announces its latest interest rate decision. All bets are on a hold at 2% for the main interest rate and 2.15% for the deposit rate. Market movements imply a 94% probability of policy staying unchanged (so expect fireworks if anything is different). Matthew Ryan, head of market strategy at financial services firm Ebury, said that Christine Lagarde will try not to rock the boat today. He said: Given this unusually elevated uncertainty, President Lagarde, who has a penchant for providing very little in the way of forward guidance, has even less incentive to hint at the path ahead for rates. She is instead likely to largely repeat her message from June, when she said that policy was “in a good place”, and that the ECB was nearing the end of its cutting campaign. At the same time, she is unlikely to close the doors to further rate adjustments, particularly as tariff escalation could have disinflationary implications for the Eurozone. In the ECB’s “severe” scenario, which assumes higher tariffs and increased trade uncertainty, the bank expects weaker price pressures, particularly in the longer term. The mood at the Society of Motor Manufacturers and Traders (SMMT) today, following their gloomy news that the UK’s car industry output has dropped in the first half of 2025 to levels not seen since 1953 (aside from the coronavirus pandemic lockdown period), is probably quite different from 72 years ago. This upbeat piece by the Manchester Guardian’s motoring correspondent in October 1953 told readers that figures from the SMMT were so positive that the UK car industry had ‘become the mainstay of the national economy’. The income from UK vehicle exports was highlighted in the article, noting that after the war, car manufacturers had got into their stride, with the value of car exports rising from £68 million to £200 million per year during the 1950s. Whereas the uncertainty around the export of UK cars to the US, caused by the Trump administration’s tariffs, has reportedly had a negative impact on current output, back in 1953 the outlook for UK car makers hoping to break into the traditionally tough US market couldn’t have been rosier. One car, the eye-catching UK-made Jaguar XK 120 convertible, had won many admirers in the US, filling the order books of British exporters. Readers here were told that ‘Americans who could afford more than one car demanded that their family vehicle should be American, but their sports car should be characteristically British.’ The number of shoplifting offences in England and Wales rose to a new record high in the year to March, continuing the marked increase in the crime since the coronavirus pandemic. There was a 20% increase in shoplifting offences to 530,643 in the year to March, according to the Office for National Statistics (ONS). “Theft from the person” – which includes pickpocketing and snatching items such as phones – also increased by 15% to 151,220. The ONS said: There have been sharp rises in these offences since the pandemic. Both shoplifting and theft from the person offences are at their highest level since current police recording practices began in YE March 2003. The rise in shoplifting has been partly seen as the result of squeezed household finances amid high inflation in recent years, but the British Retail Consortium (BRC), an industry body, has previously blamed it on organised gangs stealing to order. Tom Ironside, director of business and regulation at the BRC, said: The ONS figures prove what retailers have long been telling us – that retail theft is spiralling out of control. Sadly, such theft is not a victimless crime; it pushes up the cost for honest shoppers and damages the customer experience for everyone. Retail theft costs retailers, and their customers, over £2.2bn a year and are a major trigger for violence and abuse against staff. While the causes are manifold, the rise in organised crime is a significant concern, with gangs hitting store after store, even within a single day. The UK and India have signed a long-awaited trade deal. Keir Starmer said the UK-India agreement was “the biggest and most economically significant” trade deal Britain has made since Brexit. The prime minister said: Look, we both know this is the biggest and most economically significant trade deal that the UK has made since leaving the EU. And I think I can say that it’s one of the most comprehensive deals that India has ever done. So thank you, prime minister, for your leadership and for your pragmatism. The deal will open up trade between the UK and India for cars, whisky, clothing and food products, writes political correspondent Eleni Courea. For the UK, the agreement promises a much-needed economic boost and serves as proof that the country can be nimble on the international stage after Brexit. For India, it acts a signal to governments and international investors that its £3tn economy is opening up after decades of protectionism. India’s average tariff rate is 13%, compared with the UK’s 1.5%. You can read the full analysis here: A passenger plane has crashed in Russia’s far east after disappearing from radar, with 49 people on board feared dead, local officials have said. The flight, operated by Siberia-based Angara Airlines, vanished from radar on Thursday and lost contact with air traffic controllers while approaching its destination of Tynda, a remote town in the Amur region bordering China. An aerial inspection of the Soviet-era An-24 plane crash site found no survivors, the local emergency services told the state news agency, Tass. “According to preliminary information, all onboard were killed. So far, the rescue helicopter has been unable to land at the crash site,” an unnamed emergency official said. The An-24 is a twin turboprop regional aircraft designed by the Soviet Union’s Antonov Design Bureau in the late 1950s. You can read the full report here: The boss of Britain’s largest mortgage lender has warned Rachel Reeves that increasing taxes on banks in her autumn budget would damage Labour’s plan for the City of London to power an economic recovery. Charlie Nunn, the chief executive of Lloyds Banking Group, said a rise in bank taxation “wouldn’t be consistent” with the chancellor’s overtures as the government pushes to reboot growth. Against a backdrop of mounting speculation that Reeves could use her autumn budget to announce a fresh round of tax rises, his comments came as the high street bank reported a 17% jump in second-quarter profits. Nunn told journalists on Thursday the bank had not had any discussions with the government about a potential tax rise, and acknowledged that it was ultimately a “political decision”. However, he said that targeting the financial services sector with higher taxes would mark a stark reversal by the chancellor, who last week announced a raft of changes to cut regulation and boost growth across the sector. You can read the full story here: European Central Bank president Christine Lagarde will be in front of the world’s media this afternoon when she announces the latest interest rate decision, but it might be the Federal Reserve’s Jerome Powell who is having the more nervous wake-up today. That is because the Fed is going to host President Donald Trump for a visit. It is not a social call. Trump has repeatedly expressed his outrage with Powell after the central banker refused to cut interest rates. In response, Trump has zeroed in on a potential weakness for Powell: the over-budget renovation of the Federal Reserve building. The White House claims that the Fed mismanaged funds for renovations, which were approved in 2017 and were estimated to cost $1.9bn in 2019. The costs are now estimated to be closer to $2.5bn. The Associated Press reported: When asked last week if the costly rebuilding could be grounds to fire Powell, Trump said, “I think it is.” “When you spend $2.5bn on, really, a renovation, I think it’s really disgraceful,” Trump said. The Fed has felt forced to respond to the accusations, but it is unclear whether Trump will actually follow through on his threat to fire Powell. Given how central banker independence has become prized by global markets – freeing interest rates from nakedly political influence – firing Powell would almost certainly set off market ructions as investors adjusted to the expectation of higher interest rates. The gain this morning on London’s FTSE 100 has pushed it to the latest record high. The peak this morning was 9,158.21 points. Let’s see if it will go higher today. The FTSE 100 has gained 1% midway through the morning session, helped by bumper results from kitchen supplier Howden Joinery and Dettol-to-Durex manufacturer Reckitt Benckiser. They are up 10% and 9.3% respectively. Airtel Africa’s share price is now up 7.5%, while BT has gained 6.7%. Here’s Reuters on the Howden results: Kitchen and interior fittings supplier Howden Joinery reported a rise in first-half profit on Thursday, helped by price hikes and market share gains in a challenging environment. The company’s pre-tax profit rose 4.4% to £117m for the six months through June 2025. And the Wall Street Journal on Reckitt Benckiser: Consumer-goods company Reckitt Benckiser reported market-beating adjusted profit as cost savings paid off and raised its full-year outlook. The UK company on Thursday said first-half adjusted operating profit, which strips out exceptional and other one-off items, rose 1.8% on year to £1.71bn. Reckitt said the rise reflects efficiency improvements and early delivery of costs savings. British businesses have said they have cut jobs in response to higher taxes and “subdued” demand, according to a closely followed survey. The UK economy slowed in July as manufacturing output shrank and services sector growth slowed, according to early readings from the purchasing managers’ index (PMI) reported by S&amp;amp;P Global. The flash UK PMI composite index fell to 51 points in July, down from 52 in June and the 51.8 expected by economists. The services PMI dropped to 51.2, well below the 52.8 in June, while manufacturing output shrank. Yet it was signs of job cuts that may worry the UK government, with staffing numbers declining at the fastest pace since February. S&amp;amp;P Global said: “Survey respondents widely commented on the need to reduce headcounts in response to higher payroll costs and subdued customer demand.” Payroll costs have risen after the Labour government raised employers’ national insurance contributions. Chris Williamson, chief business economist at S&amp;amp;P Global Market Intelligence, said: Particularly worrying is the sustained impact of the budget measures on employment. Higher staffing costs have exacerbated firms’ existing concerns over payroll numbers in the current environment of weak demand, resulting in another month of sharply reduced headcounts in July. The weak growth trajectory and sustained culling of jobs will add to pressure on the Bank of England to cut rates again at its next policy meeting in August. It seems likely that the disappointing growth and labour market trends will increasingly dominate the inflation forecasting narrative, encouraging policymakers to ‘look through’ the recent rise in price pressures and instead focus on helping to revive growth. In the barrage of PMI economic data this morning, it looks like the European economy is doing marginally better than economists had expected. The European manufacturing purchasing managers’ index (PMI) rose to 49.8 in July, according to a flash reading by S&amp;amp;P Global – just shy of the 50 mark that denotes expansion and the 49.7 expected by economists. If it could edge above 50 it would be the first time in more than three years. On the services front, the Eurozone PMI reached 51, up from 50.6 the month before. Jack Allen-Reynolds, deputy chief eurozone economist at Capital Economics, a consultancy, said that the data were “consistent with the economy doing little more than stagnate” – but signs of easing inflationary pressures will be welcomed by the European Central Bank, ahead of its press conference this afternoon. Policymakers at the ECB will be encouraged by the evidence that services price pressures are continuing to ease. For the ECB, both the input and output price indices for the services sector declined. Both are very close to their levels in 2019, when underlying price pressures were very weak. So this will strengthen policymakers’ conviction that services inflation – which is still above 3% – will continue on its downward trend. It is not just British carmakers who are struggling: Tesla’s European sales are down a third this year, as total new car sales across the EU fell by 7% in June. Tesla’s European sales have slumped 33% during the year so far to 110,000 compared with 165,000 in the first half of 2024, according to new data from the European Automobile Manufacturers Association (ACEA), a lobby group. The figures suggest that Tesla is still struggling to emerge from a sales rut in Europe, even after releasing its refreshed Model Y. Elon Musk, whose shares in Tesla have made him the world’s richest man, has also contributed to the decline in sales by backing Europe’s far-right political parties, and briefly allying himself with Donald Trump, who is deeply unpopular across Europe. The US carmaker’s sales across Europe – including the EU, UK, Norway and Switzerland – were down by more than a fifth year-on-year in June, to 35,000. Tesla shares were down 4% in pre-market trading on Thursday, after Musk last night said that the electric car pioneer “probably could have a few rough quarters” because of falling earnings as Trump clamps down on the hugely profitable sale of emissions credits to other carmakers. The UK has been a rare bright spot for Tesla in Europe, with sales only down by 1.3% year-on-year in the first half of the 2025, according to the Society of Motor Manufacturers and Traders, the British industry’s lobby group. Yet the picture in the EU has been bleak: ACEA’s data show Tesla sales down 40% in June in the EU, and 44% over the course of 2025. Across all of the European markets, Tesla’s share of sales has dropped from 2.4% in 2024 to 1.6% in 2025 – although it may regain some ground as sales of the refreshed Model Y pick up across the continent. Yet rather than physical products bought by consumers, Musk is pinning much of his hopes on future earnings from driverless taxis run by AI. The company has launched a pilot programme in Austin, Texas. Matt Britzman, an equity analyst at Hargreaves Lansdown, an investment platform, said: Elon and the Tesla team failed to ignite a fire on last night’s earnings call. The numbers were objectively poor, but that was already expected, and shares were broadly flat on the initial release. The typical playbook for the past few quarters has been declining fundamentals but enough AI hype to keep investors sleeping at night. Tesla is in a very small cohort of companies with enough growth potential that investors are, for now at least, willing to look past weakening core financials. Output from Germany’s manufacturing industry is likely to shrink in July, according to an early reading of the purchasing managers’ index (PMI). The “flash” reading came in at 49.2 points, below the 50 points that indicates an expansion, but slightly above economists’ expectations of 49, according to data company S&amp;amp;P Global. Cyrus de la Rubia, chief economist at Hamburg Commercial Bank, which sponsors the survey, said: The economic situation in the manufacturing sector remains fragile, as underscored by the headline PMI remaining below the 50 mark. However, the fact that production in this sector has now expanded for five months in a row is encouraging. Given the sustained rise in export orders over the past four months, it is reasonable to anticipate a continued expansion in output. Against this backdrop, manufacturing companies have also slowed the pace of job cuts. Overall, we see increasing signs of a recovery in the manufacturing sector. Business secretary Jonathan Reynolds has said he is “very concerned” about the UK’s car industry, after figures showing that output slumped to its lowest level since 1953 in the first half of 2025, aside from the coronavirus pandemic lockdown period. UK vehicle manufacturing declined by 12% to 417,200 units in the first six months of the year, figures from the Society of Motor Manufacturers and Traders (SMMT), a lobby group, show. Reynolds told BBC Breakfast he was worried about the industry, which he described as the “jewel in the crown” of British manufacturing. He said, according to the PA news agency: I’m very concerned about automotive, the pressures on the system which come from the US trade agenda, but also an incredible increase in capacity from China. It’s why as a government we’ve adopted so many measures specifically around the automotive sector. So that’s everything from the industrial strategy, which reduces the energy costs for British automotive factories making vehicles – cars, vans and buses. It’s also why we changed the regulation that we inherited from the previous government on the transition to electric vehicles, why we negotiated the automotive quota with the US – a key market for us in that regard – and also why we’ve just announced an incentive program for... electric vehicles made in the UK, which will bring the cost down for British consumers. Mike Hawes, the SMMT’s chief executive, said that it was “one of the toughest periods for UK automotive”. The FTSE 100 has gained a bit more momentum, up 0.6%. Elsewhere on European markets, France’s Cac 40 is up 0.4%, but Germany’s Dax index has jumped by 1.1% and Spain’s top stocks on the Ibex are up 1.3%. Shares in Germany’s Deutsche Bank rose by 6% on Thursday morning, driving that Dax rise. Reuters reported that the lender “returned to a better-than-expected profit in the second quarter from a year ago despite mixed results at its global investment banking division and a hit from the jump in the euro’s value.” In Switzerland, Nestlé said it would do a strategic review of its vitamins business that could lead to the divestment of some brands, despite reporting “better-than-expected first-half organic sales growth on Thursday, Reuters reported. ITV has announced another £35m in cost cuts after profits plummeted more than 40% in the first half, as the broadcaster struggled to match the advertising boom delivered by last year’s men’s European football championships. The broadcaster said that pre-tax profits were down 44% year-on-year to £99m in the first six months, as total advertising revenues fell 7% to £824m. ITV said that it struggled to match the “very strong” advertising period last year driven by the men’s Euros, which caused a 17% surge in ad revenue in the second quarter last year as England reached the tournament finals. The broadcaster announced a further £15m in cost savings, taking the total for this year to £45m, which it said will come from a combination of new initiatives and annualised benefits from cuts made last year. Separately, ITV also said that it was trimming programming budget by £20m, from £1.25bn to £1.23bn, “as we further optimise content spend to best reflect viewer dynamics”. Looking ahead, ITV said that it expects total advertising revenue to be “marginally down” in the third quarter, again due to last year’s Euros. However, the decline has been ameliorated by England’s nerve-racking and exhilarating run to make the finals of the women’s Euro 2025 tournament. ITV’s gamble by choosing to have the first pick of the semi-finals in pre-tournament negotiations with the BBC, which in return got live coverage of three of the four quarter finals, has paid off. England’s European Championship semi-final win over Italy on Tuesday night delivered ITV’s highest viewing figures of the year. A peak audience of 10.2m watched as England defeated Italy in the final minutes of extra time to set up a final against Spain, which beat Germany on Wednesday night. The dramatic final – which ran for an advertising haul-friendly 120 minutes – was ITV’s highest average audience of the year among adults and 16 to 34 year olds. It also broke streaming records with ITVX recording its biggest day of the year with 17.2m stream views. Carolyn McCall, chief executive of ITV, said: ITV is now a leaner, more digital business in a strong position to compete and succeed in a changing market. We have the agility and capability to make the most of new revenue opportunities while driving profitable growth, strong cash generation and attractive returns to shareholders. And we’re off on Europe’s stock markets. The FTSE 100 has gained 0.4% in the opening trades. Lloyds Banking Group is up 0.9%, while HSBC has also gained 1%. The biggest riser in the early moves is Airtel Africa, up 4.5% after the telecoms company reported growth in customer numbers, and a 30% increase in quarterly earnings before interest, taxes, depreciation and amortisation. Britain’s largest high street bank, Lloyds Banking Group, has reported a 5% rise in profits even as it said that higher unemployment loomed over the UK economic outlook. The lender said that statutory profit before tax was £3.5bn for the first half of 2025, 5% more than the same period last year. Revenues rose 6% year-on-year to £9.4bn. Lloyds said its money set aside in case of economic turbulence “reflects a modest deterioration to the economic outlook in the second quarter, including a higher unemployment rate peak largely offset by further improvements to house price expectations.” The bank said there had been n</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Christine Lagarde says the ECB will be ‘data-dependent’ on interest rates. She said the prospect of a 15% tariffs between the EU and US remained ‘conjecture’ US markets have followed the lead of European indices, rising at the opening bell on Wall Street.</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Time to wrap up: Chancellor Rachel Reeves has pledged to stick to her fiscal rules, despite UK borrowing rising faster than expected last month. Reeves told the House of Lords economics affairs committee that the government showed the “political courage and strength” to stick to those fiscal rules, adding: “We will continue to do so.” Reeves also resisted an invitation to rule out a wealth tax in the autumn budget, and warned that the UK was still reliant on “the goodwill of strangers” willing to buy its debt, saying: “We are still very reliant on the goodwill of strangers in buying our government bonds. “I’m a Labour politician. I don’t think there’s anything progressive about spending 100 billion pounds a year, often to U.S. hedge funds, when I would rather spend that money on the health service or on defence or on better schools.” Reeves was speaking just hours after the latest UK public finances data showed a jump in borrowing last month. Public sector net borrowing rose to £20.7bn, up by £6.6bn from the same month a year earlier to reach the second-highest June borrowing figure since monthly records began in 1993. The UK’s fiscal watchdog, the Office for Budget Responsibility, pointed out that borrowing so far this financial year was in line with its forecasts. But, several economists still predicted that Reeves would raise taxes in the autumn, given the opposition from Labour MPs to spending cuts. Reeves also urged businesses to hire unemployed and economically inactive members of the UK labour market, rather than relying on migration. Bank of England governor Andrew Bailey warned the chancellor against watering down City banking rules, warning it risks repeating the mistakes that led to the 2008 financial crisis. Members of the Bank’s FPC told MPs that financial stability was crucial to achieving growth. Bailey also hinted that he might not support the introduction of a digital pound, if the Bank’s efforts to embed digital payments technologies into commercial bank payment systems succeeded. And in other news: It’s also been another historic day in the London stock market, where the FTSE 100 share index has hit a new intraday high of 9035 points. Lord Razzell probes chancellor Reeves over her controversial increase in employers’ national insurance contributions. Q: If you had the time to go into your local pub, they’d complain to you about the impact. Did the Treasury model the impact of the NICs changes? Rachel Reeves says the Labour government discovered a number of unfunded spending commitments when it entered office, so she decided to increase taxes on businesses and the wealthiest by £40bn in the budget. She says the government took steps to protect smaller firms from the NICS increase, such as increasing the Employment Allowance, which cut the cost of employing people on the minimum wage. She concede that the NICS increase has been painful for businesses. But the counterfactual, she insists, would either have been higher taxes on working people, cuts to public services, or higher borrowing. Former chancellor Lord Lamont then asks the present chancellor if she will rule out a wealth tax, something which some Labour MPs are demanding. Q: Doesn’t the whiff of a wealth tax undermine confidence? Wouldn’t it be better to just rule it out? Rachel Reeves says the government made commitments before the last election about various taxes related to working people, such as income tax, national insurance and VAT. But she declines to speculate about tax changes, reminding Lamont that he took a similar view about future fiscal policy in his time at Number 11. She says: If you start saying no to other taxes, then as soon as you don’t say no people will assume that’s the one you’re going to increase. It is right, and with respect this is what you did in my position, you rightly said that taxes are a matter for a budget, and we’ll set out our policy there. Yesterday, The Times reported that Reeves was expected to reject pressure from left-wing Labour MPs to implement a wealth tax, due to fears it would not raise any money because wealthy people would simply leave the UK. Reeves then tells their Lordships that she wants to retilt the system so more young people can get an apprenticeship, or go to an FE college. The chancellor points out that those who don’t go to university are missing out, saying: At my school, where I went - quite a lot of years ago now - I was in the very small minority who went to university. The government carried on investing in my education for years, very expensively. In contrast, many of the girls at Reeves’s school left at 16, or 18, despite being bright “because they didn’t have those aspirations” and didn’t get the same opportunities. Q: How can we get the “British dream” going, to lift productivity? Rachel Reeves cites her reforms to savings, to encourage people to put their spare cash into investments, and to provide “long-term, patient capital” for the nation’s entrepreneurs. The chancellor also suggests part of the British dream is to own your own home – that’s why the government is aiming to raise housebuilding levels. Q: What are the fiscal consequences of the government’s u-turn on the welfare bill? Chancellor Rachel Reeves says the changes to the welfare bill will have a cost – probably around £5bn, but the Office for Budget Responsibility will do the calculations. She reiterates her commitment to the fiscal rules, explaining: We are still very relient on the goodwill of strangers in buying our government bonds. One in every ten pounds of government spending is spent servicing government debt. Reeves says there’s nothing “progressive” about spending £100bn per year on debt servicing, which she says often goes to US hedge funds, rather than on health, defence, or schools. Rachel Reeves then criticises the previous government of committing to delivering “lots of lots” of projects, without working out how to pay for them. She tells the House of Lords economic affairs committee: That is how you end up in politics with the levels of distrust of politicians and the democratic system. I do think it is unforgiveable to make a load of commitments without having a single clue about where the money was going to come from. I’m not going to do that. Reeves adds that immigration will continue to play an important part in creating the UK’s "skills mix”, before repeating that “we can’t just turn to the immigration lever”. Chancellor Rachel Reeves is now urging businesses to hire workers from the ranks of the unemployed and economically inactive, rather than relying on migration. She is asked about demographics, with Lord Turnbull citing the “severe worsening” of the dependency ratio. This ratio compares the number of people in a population who are typically not in the workforce (ie, are dependent) with the number of people who are typically in the workforce. Turnbull points the finger of blame at the young, saying it can take people until their mid-20s to get into work today, rather than finding a job at 16. The birth rate is very low, creating a shortage of workers, leading to “very high levels” of net migration, he says. Q: How do you balance protecting the public finances and addressing the needs of the labour market against the social pressures this migration is causing? The chancellor tells the House of Lords economics committe that countries around the world face demographic challenges – the UK’s situation is not the worst by a long way, she says. She says the major independent commission on the pensions system launched yesterday will help address this. Reeves then urges businesses not to turn to migration to fill vacancies. She says there are “a lot of people here in Britain who are not working”, citing that 20% of people of working age are classed as economically inactive, and an unemployment rate of over 4%. I do not think that businesses should always resort to the immigration lever to fill vacancies. We need to do a lot more to train up people who are already in this country. ONS data last week showed there were 736,000 vacancies in March to May. Reeves says: There are plenty of people of working age in this economy, with the right support they should be able to work. The Lords turn to tax. Q: Since the war, no government until now managed to bring in more than 35% of GDP in taxation. It’s now around 37.5% – what level do you think is sustainable? Reeves says the Office for Budget Responsibility (the fiscal watchdog) forecasts tax will hit 38% of GDP at the end of the parliament – that’s not a target though! Increasing GDP is the best way to reduce that ratio without cutting investment in public services, she says. Rachel Reeves is then asked why the UK economy is suffering from slugging growth, rising unemployment, stubborn inflation. Q: What’s your diagnosis of the ills of the UK economy? The key problem is productivity, and investment is the answer, the chancellor replies. Reeves adds that trade policy is another important area of reform. She cites the UK becoming the first country to reach a trade deal with the US, plus the “reset” with the European Union and a trade deal with India. Rachel Reeves then cites the government’s changes to the planning system, which are currently being considered by the House of Lords. She urges the Lords to pass the planning and infrastructure bill quickly, so that the UK can get on with “getting things done”, such as transport and energy infrastructure, or new data centres. The chancellor also points to her pensions review, and yesterday’s review of the water sector, as areas where the government are pushing reforms through. The House of Lords economic affairs committee begins with Lord Wood asking chancellor Rachel Reeves about her growth plans: Q: What is your strategy to achieve growth, without borrowing more than your fiscal rules allow or by boosting current spending more than your tax commitments allow? Reeves says we are living in an “age of insecurity”, and economic policy has to respond to that. She also points to her “challenging economic inheritance”, with high levels of tax as a share of GDP, historic high levels of government debt, and “very poor” economic growth over the last 15 years due to weak productivity growth. So the growth strategy has to address this. Reeves says the government’s growth strategy is about building “resilience and stability”. Stability means fiscal rules which the government sticks to – the pledge to fund day-to-day spending through tax receipts, and to have debt falling as a share of GDP while still delivering investment. Reeves says this stability has allowed the Bank of England to cut interest rates four times in the last year. We have faced challenges this first year. The international geopolitical backdrop is probably not one that any government would want, but that’s what we have. Despite that, Reeves insists that the government showed the “political courage and strength” to stick to those fiscal rules in the budget, in the spring statement and in the spending review. “We will continue to do so,” she pledges. [Reminder: economists believe Reeves may need to raise taxes in the autumn budget, after borrowing surged over City forecasts in June]. Back in parliament, the House of Lords Economic Affairs Committee are holding a session with chancellor Rachel Reeves. You can watch it here: The IMF are also warning that tariffs are not the answer to widening current account balances. In their latest External Sector Report, just released, the Fund says: A further escalation of trade tensions, including with tariffs, would have significant negative macroeconomic effects, with limited efficacy in correcting global imbalances. The IMF also note that higher tariffs would reduce global demand in the short term and add to inflationary pressures through rising import prices. It would be better, they suggest, for countries to address their own domestic imbalances. The International Monetary Fund is concerned that global current account balances are widening, potentially putting strain on the international monetary system (IMS). In a new report, just released, the IMF show that global current account balances widened by “a sizable 0.6 percentage points of world GDP in 2024”. That is a notable reversal of the narrowing since the global financial crisis and may signal a significant structural shift, they warn, with some countries running up larger deficits and others piling up larger surpluses. In a blog post, IMF chief economist Pierre-Olivier Gourinchas says that around two-thirds of the widening in global current account balances in 2024 was “excessive”, writing: The increase in excess balances is the largest in a decade, driven primarily by China (+0.24 percent of global GDP), the US (-0.20 percent) and more modestly by the euro area (+0.07 percent). Gourinchas adds that “a growing asymmetry in global trade and financial networks” is taking hold, and identifies three factors to watch: First, while global imbalances are resurfacing, geopolitical considerations are increasingly shape bilateral trade, direct investment and portfolio flows, reducing direct interactions between more geopolitically distant jurisdictions. Ultimately, this could open the way for a fragmented multipolar IMS. While it is debatable whether an integrated unipolar or integrated multipolar system would be more beneficial to the global economy—history provides little guidance and theory is ambiguous—a fragmented multipolar IMS would almost surely be less desirable than an integrated one, with a potential for increased global financial volatility and greater misallocation of resources. Second, the recent escalation of trade tensions coupled with the threat of possible financial tensions, rising US debt levels and a softening of the US exorbitant privilege may have caused some global investors to reassess the extent of their dollar exposure. So far, markets developments have been orderly, with an increase in demand for dollar hedging and an 8 percent depreciation of the US dollar since January, the largest halfyear decline since 1973, albeit after the multi-decade high of 2024. Third, digital innovation for cross border transactions, such as the rise of US dollar stablecoins, could reinforce dollar dominance but could also create financial stability risks. Another US stalwart, Coca-Cola, has reported sales growth in the last quarter. Coca-Cola has reported that its second-quarter organic revenues grew 5% in April-June, due to a 6% rise in prices while global unit case volume declined 1%. James Quincey, chairman and CEO of The Coca-Cola Company, says: “Amid a shifting external landscape in the second quarter, the ability of our system to stay both focused and flexible enabled us to stay on course in the first half of the year.” The company has also announced it will launch a Coca-Cola offering “made with US cane sugar”, as part of its “ongoing innovation agenda”. Last week, president Trump pre-empted this announcement, posting on Truth Social: I have been speaking to Coca-Cola about using REAL Cane Sugar in Coke in the United States, and they have agreed to do so. I’d like to thank all of those in authority at Coca-Cola. This will be a very good move by them — You’ll see. It’s just better! Over in the US, carmaker General Motors has reported that its profits fell by a third in the last quarter, after Donald Trump’s trade war cost it more than a billion dollars. GM made a profit of $3bn in the second quarter of this year, on an EBIT-adjusted basis, down from $4.4bn in April-June 2024. GM told shareholders that tariffs had a net impact of $1.1bn on its earnings in Q2, “reflecting minimal mitigation offsets” It also warned that it expects the net impact of tariffs to be higher in the third quarter of 2025, due to the “timing of indirect tariff costs”. A 25% import tax on engines, transmissions and other key car parts is now in force in the US, while manufactures also face new tariffs on steel and aluminium imports. GM is sticking with its estimate that the gross impact of tariffs will be between $4bn and $5bn this year, adding that it is making “solid progress to mitigate at least 30% of this impact through manufacturing adjustments, targeted cost initiatives, and consistent pricing”. CEO Mary Barra reminded investors that it is investing more in its US manufacturing, telling them: For example, in June we announced $4 billion of new investment in our U.S. assembly plants to add 300,000 units of capacity for high margin light-duty pickups, full-size SUVs and crossovers. This will help us satisfy unmet customer demand, greatly reduce our tariff exposure, and capture upside opportunities as we launch new models. The capacity begins coming online in just 18 months, after which we project building more than 2 million vehicles in the U.S. each year as we scale. [Reminder, yesterday fellow carmarker Stellantis cut its 2024 profit forecast and warned it will burn through more cash than expected, after being hit by tariffs]. The Bank of England governor has cast doubt on whether the UK’s central bank will introduce a digital currency, having worked on the project for several years. Andrew Bailey told the Treasury committee that he would need “a lot of convincing” to push through the plan, if existing work to push digital technology into the commercial bank payment systems is a success. He tells MPs that the BoE will work with banks and the market to develop digital technology in the commercial bank payments systems, particularly the faster ones, which are the main payment systems of the country. Bailey explains: That’s a sensible place to do it because that’s where most of our money is. My view is, if that’s a success I quesion why we need to introduce a new form of money. Bailey says improving commercial banks’ digital payments systems could lead to “huge benefits”, such as smart contracts, reducing fraud, reducing costs, and improving late payments to small firms. This could be the best way to get digital technology into the payments system, he suggests, compared to the alternative of a retail central bank digital currency (CBDC, or digital pound) or the growth of stablecoins (eg non-bank money). Bailey insists he is “not saying no” to a CBDC, but adds: If the work with the commercial banks is successful, I would need a lot of convincing that the use case was made. Bloomberg reported this morning that Bank of England officials are mulling whether to set aside plans to create a digital pound for households amid growing skepticism about the project’s benefits. Bailey also reminded MPs that China has launched a CBDC, while the European Central Bank is pressing ahead with its plans for a digital euro. Q: Do you have red lines about the deregulation of UK financial rules, governor? Andrew Bailey says he has two very strong red lines. 1) he repeats that there isn’t a trade-off between financial stability and growth 2) he shows exasperation about people who say the financial crisis is deep in the past, and solved, so we can move on. Summing up the challenge of protecting the UK financial system, Bailey says: Success in financial stability is when nothing happens. The fact we’ve had market volatility this year and we haven’t had a financial stability problem, we’re not worrying about banks failing or worrying about the markets, is of course a success. Bailey then declines to back Rachel Reeves’s comment that regulation is acting as a “boot on the neck” of financial firms, saying: “I don’t use those terms, let me say that... It is not a term I use.” Q: But is there a problem with overregulation of financial services firms? Bailey repeats that the Bank is open to looking at the rules, but insists: We can’t compromise on basic financial stability. That would be my overall message. Bank of England governor Andrew Bailey has warned MPs that watering down post-2008 financial crisis bank ringfencing rules would be bad for British households, and would not help banks either. Testifying to the Treasury Committee this morning (highlights start here), Bailey insists that there isn’t a trade-off between financial stability and growth in the economy. He reminds MPs that Parliament created a great deal of detail when they legislated the ringfence rules after the financial crisis. Perhaps some of that detail could be improved, but he insists the ringfence mustn’t be torn up. Ringfencing protects UK retail banking from shocks originating elsewhere in the group and in global financial markets. Last week, chancellor Rachel Reeves promised “meaningful” reforms to the UK’s ring-fencing rules, prompting warnings from some of the architects of the UK’s post-2008 reforms. Today, Bailey says the ringfence rules are an important part of the structure of the financial system. Crucially, he explains, they make it easier to resolve a failing bank. He tells MPs: “It has benefits, particularly, in terms of UK customers and UK consumers; businesses and households. I think that is a helpful feature of it. I don’t think it hinders banks fundamentally in terms of their business models. “Again, at the margins, I am sure there are things that can be improved and we will work constructively to go through that process. “It has established itself as part of the system and to me it would not be sensible to take it away at this point.” Bank of England governor Andrew Bailey then reminds MPs about the surge in certain tech stocks this year, to explain the rebound in markets since their April wobble. He tells the Treasury committee: Here’s a striking fact. The market cap of Nvidia is now larger than the UK’s GDP. Nvidia’s shares are up 27% so far this year, giving it a market capitalisation of $4.18tn (or £3.1tn), thanks to strong demand for its high-powered chips to power artificial intelligence systems. Q: Why have US and global equities bounced back from the initial shock of Donald Trump’s tariffs? FPC committee member Professor Randall Kroszner replies that it is always “very difficult” to assess market movements (indeed!). One factor is that the markets weren’t expecting the level and the breadth of the tariff proposals which Trump announced on 2 April, even though the president had talked about them before. It was then “very helpful for the market” that the president pushed back the date when tariffs will come in, and offered more flexibility for negotiations, Kroszner adds. [that’s a polite way of pointing to the TACO trade] Kroszner also points to the passing of the president’s budget bill, which extends previous tax cuts to investment. That has supported investment in the US. Q: are there any elements in the Leeds reforms that make you nervous, in terms of financial stability? FPC member Randall Kroszner says the committee will weighs up the costs and benefits of the measures, to assess the impact. He doesn’t see “a necessary clash” between the reforms and financial stability, but it will depend on the detail of what is changed. Kroszner also points to risks from the non-bank financial sector. Two Bank of England policymakers have warned the government against undermining the financial system through its deregulation push. Professor Randall Kroszner, external member of the Bank’s Financial Policy Committee, told the Treasury Committee that it is important to maintain resilience in the financial system. Asked about the “Leeds reforms” announced by Rachel Reeves last week, Kroszner says that snything that challenged that stability would be a red line, (but he doesn’t have any concrete examples of concerns). Kroszner explains that undermining financial stability would hurt the government’s growth agenda, saying: “If you don’t have financial stability it is going to be a major challenge to have economic growth”. Reeves’s package of measures, unveiled in Yorkshire, include cutting out “unnecessary” red tape and encourage more financial risk-taking by companies and consumers. Fellow FPC member Carolyn Wilkins points out to MPs that “a lot of the reforms” made since the great financial crisis of 2008 have worked out well, as illustrated by the stresses which the banking sector has experienced since without collapsing. Wilkins adds: “There are ways we can look at those regulations and maybe simplify them, maybe alter them in some way, and still achieve a very good financial stability outcome, with more efficiency”. Part of the FPC’s work is looking at specifically how that can happen to help the growth agenda, Wilkins explains. Over in parliament, the Treasury Committee are starting to question members of the Bank of England’s Financial Policy Committee (FPC) on financial stability. As well as governor Andrew Bailey, two external members of the FPC, Randy Kroszner and Carolyn Wilkins, will also give evidence to the Committee. The committee asks Bailey about the rising cost of government borrowing…. Bailey replies that the cost of long-term borrowing has risen, globally. It’s not unique to the UK, and there have been steeper rises elsewhere. These moves are being driven by increased uncertainty, particularly around trade policy, Bailey explains, and also by global uncertainty around fiscal policy. He says: “It is greater uncertainty, clearly. On two fronts: one is uncertainty around what is going on in trade policy at the moment. The second thing is uncertainty globally around fiscal policy. That’s again a global phenomenon.” If you look over the last decade, Bailey adds, there has been a shift towards greater government borrowing but a smaller increase in business and personal borrowing. Q: Are you unconcerned? Bailey says the moves reflect conditions, both in geopolitics and on pressure on fiscal policies. Britain’s manufacturing sector contracted last year, new sales figures show. The total value of UK manufacturers’ product sales fell byy 3.1% in 2024, to £452.2bn, the Office for National Statistics reported. That included a 2.4% drop in motor vehicle sales. The ONS reports that the manufacturing of fresh or chilled cuts of beef and veal showed the largest value increase, up by £964million or 18.6% to £6.2 billion. Other products showing noticeable increases were beer made from malt, which increased by £793m (17.1%) in 2024 to £5.4bn, and ‘aeroplanes, helicopters or unmanned aircraft’, which rose by £527m (7.8%) to £7.3bn. Britain’s fiscal watchdog isn’t panicking about the jump in government borrowing in June. The Office for Budget Responsibility points out that borrowing in the first three months of this financial year (April to June) is “exactly in line” with its forecast in March, at £57.8bn. Central government receipts and spending are both broadly in line with the forecast profile, the OBR point out, adding: In the monthly profile consistent with the forecast in the March Economic and fiscal outlook we expect lower borrowing in the second half of 2025-26 relative to 2024-25. This is based on a sharp expected rise in capital gains tax around the end-January due date, lower debt interest payments in the second half of the year, and lower central government net social benefits which were unusually backloaded last year. Neil Wilson, UK investor strategist at Saxo, fears UK government bonds could come under attack this summer, saying: The British government’s borrowing rose more than expected in June – second-highest since records began in 1993 for the month...tax hikes are coming. Gilt yields rose with the 30-year jumping after sliding on Monday – we’re not yet back to yesterday’s highs so nothing to get jumpy about. But I do worry that we could see bond vigilantes hit gilts this autumn. Despite the gloomy UK borrowing data, the London stock market has hit a new record peak this morning. The blue-chip FTSE 100 index jumped to 9025 points in early trading, a day after closing above the 9,000 point mark for the first time. The rally was led by food services group Compass, which raised its profit forecast for this year and announced the acquisition of European premium food services business Vermaat Groep. Compass’s shares are up 4.2%. They’re followed by Centrica (+4%), following this morning’s confirmation that it is taking a 15% stake in the Sizewell C nuclear power station. Mining stocks are rallying too, lifted by higher commodity prices. Insurers need to improve the way they handle home and travel claims, the financial regulator said this morning. The Financial Conduct Authority has uncovered “concerning evidence” of poor practice among some home and travel insurers, which has led to delays in settling claims and high numbers of complaints. There has been a “lack of oversight of outsourced services” in some cases, the regulator said, as well as “insufficient management information”. The FCA also found high rejection rates for storm damage claims, with only 32% of claims in its sample receiving a payment in 2024. The regulator also found cases of cash settlements being used “without sufficient consideration of whether they are most suitable”. The watchdog is also reviewing high premiums in the car insurance industry, although it found the rise in costs has been driven by factors largely outside insurers’ control, such as higher prices for cars, parts, labour and energy. The cost of hire vehicles, as well as the number and cost of theft claims and uninsured drivers, have also risen significantly, it said. However, it found evidence in the car insurance market that referral fees from credit hire firms and claims management companies were “associated” with slower claims processing and higher costs. Sarah Pritchard, deputy chief executive of the FCA, said: “External cost pressures are primarily to blame for recent motor premium increases, not increased firm profits, but there is some more work to do on claims handling, particularly in home and travel. That’s why we’re stepping up - making sure claims are handled promptly and fairly and pushing for a coordinated effort to tackle the root causes of rising motor premiums. A well-functioning insurance market helps consumers navigate their financial lives and supports growth by building people’s resilience to financial and personal shocks.” UK bond prices are weakening, which pushes up the cost of borrowing, as traders digest this morning’s public finances report. The yield, or interest rate, on 10-year UK bonds has risen by two basis points (0.02 percentage points) to 4.634%. Longer-dated, 30-year, bond yields have risen by almost three basis points to 5.463%, towards the 27-year highs above 5.5% reached in April. Yields rise when bond prices fall. Although these are small moves, they add to the pressures on the UK public finances, as higher borrowing costs eat into Rachel Reeves’s limited headroom against her fiscal targets. More bad news: UK grocery inflation has jumped to its highest level since January 2024, as the cost of living squeeze intensifies. Data provider Worldpanel by Numerator, has reported that grocery inflation accelerated in the last four weeks, to 5.2% year-on-year. That’s up from 4.7% in the previous month. Fraser McKevitt, head of retail and consumer insight at Worldpanel, says the annual cost of household shopping is rising sharply: With the average household spending £5,283 each year at the grocers, this latest rise could add £275 to bills if people’s shopping habits stay the same. Just under two thirds of households say they are very concerned about the cost of their grocery shopping, and people are adapting their habits to avoid the full impact of price rises. Own label products, which are often cheaper, continue to be some of the big winners and, in fact, sales of these ranges are again outpacing brands, growing by 5.6% versus 4.9%. Despite public borrowing overshooting official forecasts by £3.6bn in June, to over £20bn, borrowing is still in line with the OBR’s forecasts after the first three months of the fiscal year, points out Alex Kerr, UK economist at Capital Economics. But… Kerr fears things will probably get worse for the Chancellor, forcing her to raise between £15-25bn at the Budget later this year, probably mostly through higher taxes. Kerr told clients: Admittedly, the better-than-expected start to the fiscal year means that borrowing is still on track to meet the OBR’s existing forecasts after the first three months of the 2025/26 fiscal year. But the government’s u-turns on spending cuts and potential upward revisions to the OBR’s borrowing forecasts means the Chancellor will probably need to raise £15-25bn at the Autumn Budget to maintain the £9.9bn of headroom against her fiscal mandate. And given that she is struggling to stick to existing spen</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Reeves told the House of Lords economics affairs committee that the government showed the ‘political courage and strength’ to stick to fiscal rules. She also resisted an invitation to rule out a wealth tax in the autumn budget. Reeves was speaking just hours after the latest UK public finances data showed a jump in borrowing last month.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Time to wrap up… Analysts have welcomed a small fall in company insolvencies across England and Wales. The Insolvency Service has reported that there were 2,043 registered company insolvencies in England and Wales in June, 8% lower than in May 2025 (2,230) and 16% lower than in June 2024, when 2,430 companies failed. Donald Trump has claimed that Federal Reserve chair Jerome Powell was “truly one of my worst appointments,” and also criticised the Fed Board for not forcing rate cuts. Federal Reserve governor Christopher Waller has said he would accept the job as Fed chair if asked by President Donald Trump. G20 finance leaders have agreed a final communique on Friday that stressed the importance of central bank independence, saying: “Central banks are strongly committed to ensuring price stability, consistent with their respective mandates, and will continue to adjust their policies in a data-dependent manner. Central bank independence is crucial to achieving this goal.” Elsewhere… China has welcomed the US’s decision to allow Nvidia to ship its H20 AI chips England and Wales’ embattled water regulator Ofwat will be abolished under recommendations from a government-commissioned review due on Monday, the Guardian understands. US consumer sentiment has risen to a five-month high. Goodnight, and have a lovely weekend. GW Britain’s stock market has ended the week close to its record high. The FTSE 100 index has finished today’s session at 8992.12 points, up 19.5 points or 0.22%. That’s only a handful of points shy of Monday’s record closing high of 8998 points. Rentokil (+3%) and Antofagasta (+2.6%) led the risers. Mexico’s president Claudia Sheinbaum may not have got the memo about central bank independence….. The US dollar is closing out the week weaker as the fallout from the latest threat from President Trump to fire Fed Chair Powell lingers. The dollar index is down 0.45% today, while the pound is up 0.2% at $1.3443. Derek Halpenny and Lee Hardman of MUFG explain: We see this as more than just about whether Trump fires Powell. The comments from Fed Governor Waller indicate potential political influence with his comments much more explicit in calling for a July rate cut than in the past (see here). Governor Bowman is also open to cutting in July. Is Trump’s influence already playing a role? That’s key given Trump likely has two more picks for Governors next year (to replace Kugler and Powell – we assume he will leave although technically he doesn’t have to). Consumer confidence across the US has inched up this month, according to the latest data. The University of Michigan consumer sentiment index has risen to 61.8 points in July, up from 60.7 in june, lifted by an improvement in people’s economic conditions and consumer expectations. That’s its highest reading in five months, since the early days of Donald Trump’s trade war. Surveys of Consumers director Joanne Hsu points out, though, that sentiment remains a substantial 16% below December 2024 and is well below its historical average. Hsu adds: Consumers are unlikely to regain their confidence in the economy unless they feel assured that inflation is unlikely to worsen, for example if trade policy stabilizes for the foreseeable future. At this time, the interviews reveal little evidence that other policy developments, including the recent passage of the tax and spending bill, moved the needle much on consumer sentiment. Thomas Ryan, North America economist at Capital Economics, says: The small rise in the University of Michigan consumer sentiment index in July and further drop-back in inflation expectations shows that, while overall confidence remains weak, households are less worried than they were about how Trump’s policies might hit the economy, their finances, and purchasing power. British travellers to the EU will likely have to pay a €20 visa-waiver charge to enter the European Union from 2026, in a near-tripling of the original fee, my colleague Jennifer Rankin in Brussels reports. The €20 fee represents a nearly three-fold increase on the original €7 fee. It is expected to raise €2bn in revenues, although part of this sum will pay for operating costs. The European commission published plans for a €2 trillion budget for 2028-34 earlier this week, with proposed taxes on big companies, e-waste and tobacco. Buried in the small print, the commission also suggests “additional other revenue” could be generated by adjusting fees for the European Travel Information and Authorisation scheme, the EU equivalent to the US Esta. The ETIAS €7 fee was agreed in 2018, but the commission said that inflation and additional operational costs meant “the fee will be adjusted to €20 per application”. The higher fee becomes law, unless EU member states and the European parliament raise objections in the next two months. The €20 fee will apply to nationals from dozens of countries, including Ukraine, Canada, the United States, Brazil and Japan. The visa-waiver status will last for three years, or the expiry of a passport. Travellers will have to pay the fee from the final quarter of 2026 when Etias comes into force. British citizens who live in the EU with status guaranteed under the Brexit withdrawal agreement will be exempt, as will children and people aged over 70 when they made the application. A top official at the International Monetary Fund has warned that “high levels of policy uncertainty” remained a key theme at the meeting of G20 finance ministers in Durban this week. Gita Gopinath, the IMF’s First Deputy Managing Director, says economic indicators have reflected a complex backdrop shaped by trade tensions since April (when the Fund released its latest forecasts, and Donald Trump announced his ‘Liberation Day’ tariffs). Gopinath says: We have seen strong evidence of front-loading ahead of tariff increases and some trade diversion. We have also seen an improvement in global financial conditions as select trade deals lowered average tariffs. On inflation, cooling demand and falling energy prices point to a continued decline, albeit with variation across countries. And on Financial Sector issues, Gopinath warned of risks and urged close monitoring of non-bank financial institutions (NBFIs) (such as investment funds, insurance companies, pension funds and other financial intermediaries). Even though financial conditions have eased since April, with trade and geopolitical uncertainty still elevated, financial stability risks remain in focus. Asset valuations are once again stretched, the use of leverage remains high in parts of the financial system, and periodic pressure observed on government bond yields and market functioning carries the risk of broad repercussions, particularly against a backdrop of large fiscal deficits and increased illiquidity. Vigilant surveillance and robust supervision remain paramount and recent progress in financial sector oversight must continue, particularly for NBFIs which now account for more than 50 percent of the financial sector Shares in Netflix have dropped in early trading, after its results last night. Netflix raised its full-year revenue outlook yesterday, and reported $11bn revenue for the quarter to the end of June, a 16% year-on-year increase. But traders may have hoped for more – Netflix’s shares are down 4.7% in early trading. The company also revealed overnight that it had used artificial intelligence in one of its TV shows for the first time, by including generative AI footage in its Argentinian science fiction series El Eternauta (The Eternaut). Wall Street has opened higher, as investors weigh up the chances of early cuts to US interest rates. The Dow Jones Industrial Average rose 54.46 points, or 0.13%, at the start of trading to 44,542.97. The broader S&amp;amp;P 500 index gained 0.23% while the Nasdaq Composite is up 0.34%. News is emerging from Durban that G20 finance leaders have agreed a final communique on Friday that stressed the importance of central bank independence. That’s a timely reminder to Donald Trump of the dangers of undermining the Federal Reserve, as he continues to throw insults their way. The communique says: “Central banks are strongly committed to ensuring price stability, consistent with their respective mandates, and will continue to adjust their policies in a data-dependent manner. Central bank independence is crucial to achieving this goal.” The G20 also “recognise the importance of the world trade organisation to advance trade issues”, and say they are “committed to international policy cooperation to further promote global prosperity”. But they also warn that the global economy is facing “heightened uncertainty and complex challenges”. Hello hello….Federal Reserve governor Christopher Waller has said he would accept the job as Fed chair if asked by President Donald Trump. Waller made the comments today, just hours after throwing his weight behind calls for a rate cut this month (see earlier post). According to Reuters, Waller said: “In 2019 the president contacted me and said, ‘Would you serve?’ And I said yes. “If the president contacted me and said, ‘I want you to serve,’ I would do it. But he has not contacted me.” Big news in the water industry: England and Wales’ embattled water regulator will be abolished under recommendations from a government-commissioned review due on Monday, the Guardian understands. Ministers will next week announce a consultation into creating a new regulator, to coincide with the results of a review into the water industry directed by former Bank of England deputy governor Sir Jon Cunliffe. This consultation is likely to conclude in the abolishment of Ofwat, the embattled watchdog that polices how much water companies can charge for their services in England and Wales, sources said. Ofwat has faced intense criticism over its failure to prevent sewage spills, hefty payment of dividends and ballooning debts across England and Wales’s water companies. The review will recommend the creation of new regulatory system. More here. Back in the City, fashion group Burberry is one of the best performers on the London stock market today, after slowing its decline in sales. Surprisingly, demand for Burberry wellies, scarves and light jackets to wear at music festivals have helped the fashion brand to its best sales performance in 18 months, my colleague Sarah Butler reports. Sales of the luxury British brand fell by 2% to £433m in the three months to the end of June, with a 1% decline at established stores, an improvement from the 6% fall in the previous quarter and the best performance since Christmas 2023. Shares in Burberry are up almost 5%, making it one of the top risers on the FTSE 250 share index. One member of the Federal Reserve board, Christopher Waller, should be in president Trump’s good books, though. Last night, Waller argued that the Fed should cut rates by the end of this month, and cited growing risks to the economy and (he argued) limited inflationary risks from trade tariffs. Waller told a gathering of Money Marketeers of New York University: I believe it makes sense to cut the FOMC’s policy rate by 25 basis points two weeks from now. And looking to later this year, if, as I expect, underlying inflation remains in check—with headline inflation data reporting modest, temporary increases from tariffs that are not unanchoring inflation expectations—and the economy continues to grow slowly, I would support further 25 basis point cuts to move monetary policy toward neutral. The Fed’s next two-day meeting starts on 29 July, with a decision scheduled for the 30th. Brad Bechtel of investment bank Jefferies says Waller’s speech is getting some attention, explaining: Waller not typically a politically motivated character on the Fed, so his strong view on this matter is important in that context. His main arguments are that 1) tariffs are a one-off price increase and not a consistent impact to inflation, 2) GDP is below trend and a little too soft, arguing for rates closer to neutral, 3) employment looks fine on the surface, but downside risks have increased and private sector payroll growth is near ‘stall speed’. He therefore thinks we should cut rates by a quarter this month. Pretty strong view from Waller as the Fed gets close to entering their blackout period before the next meeting. Donald Trump has just declared that choosing Jerome Powell in 2017 to run the US Federal Reserve was one of his “worst” decisions, calling America’s top central banker a “numbskull” for not lowering borrowing costs. Trump blames president Biden, who he dubs “Sleepy Joe”, for renominating Powell in 2021, and also blasts the Fed’s board for not lowering rates. Posting on his Truth Social site, Trump again refers to Powell as “Too Late”, and again claims that US interest rates (currently a 4.25%-4.5% range) should be considerable lower, at just 1% (!). Trump writes: “Too Late,” and the Fed, are choking out the housing market with their high rate, making it difficult for people, especially the young, to buy a house. He is truly one of my worst appointments. Sleepy Joe saw how bad he was and reappointed him anyway - And the Fed Board has done nothing to stop this “numbskull” from hurting so many people. In many ways the Board is equally to blame! The USA is Rockin’, there is VERY LOW INFLATION, and we deserve to be at 1%, saving One Trillion Dollars a year on Interest Costs. I can’t tell you how dumb Too Late is - So bad for our Country! Stock markets wobbled earlier this week following reports that Trump was preparing to fire Powell, but recovered when the president denied it. The Fed’s board makes up a majority on the FOMC committee which vote to set US interest rates. The FOMC have voted to leave interest rates on hold so far this year, partly due to concerns that Trump’s trade war will be inflationary. The Insolvency Service has also reported that 10,279 individuals entered insolvency in England and Wales last month. This was similar to the numbers in both May 2025 and June 2024. They explain: The individual insolvencies consisted of 596 bankruptcies, 4,135 debt relief orders (DROs) and 5,548 individual voluntary arrangements (IVAs). The number of DROs in June 2025 was close to the record monthly high seen in June 2024. IVA numbers in the first six months of 2025 were similar to the monthly average in 2024. Bankruptcy numbers remained at about half of pre-2020 levels and were also 10% lower than in June 2024. Shares in Sweden’s fighter jet maker Saab have jumped 12% this morning, after the company announced strong sales growth amid the rush to spend more on defence. Saab reported organic sales growth of 32% in the last quarter, driven by strong growth in small and medium-sized orders. Micael Johansson, president and CEO of Saab, says: “We are strengthening our market position and see a continued large interest in our products and solutions. Saab’s sales growth is high and we continue to invest to build capacity and meet long-term strong demand from the defence sector. At the same time, we continue to deliver strong profitability.” Risk advisory firm Kroll point out that 2025 has been challenging for many businesses, including in leisure and retail. Benjamin Wiles, head of UK restructuring at Kroll: “There’s no doubt that 2025 has been a tough year for businesses so far, particularly those in the retail and leisure industry. Yet, the overall decline in company administrations compared to this period last year shows a level of resilience that shouldn’t be overlooked. We saw a lot of restructuring activity at the end of last year with many companies looking to get ahead of cost pressures and there is still a lot of capital available to borrow. “The question we are asking is whether businesses are fundamentally stronger or are they simply treading water. The second half of the year will be critical in determining whether this resilience can be sustained or if further pressures will tip more companies into distress.” Kroll also produced this table, based on their internal data, which tracks administrations throughout the year. Yesterday’s UK unemployment data showed that more than half the fall in payroll numbers over the last year was due to job losses in accommodation and food services. The recent hot weather may have helped some hospitality firms and retailers avoid collapse, suggests Jennifer Lockhart, partner and insolvency specialist at purpose-led independent law firm Brabners. Lockhart says: A fall in insolvencies is welcome and reflects the positive impact that the warmer summer months can have on business performance – especially in the retail, construction and hospitality sectors that have borne the brunt of failures to date. However, amid these soaring temperatures it’s important to recognise that this likely represents a period of reprieve for businesses, rather than a turning point. “Consumer confidence remains fragile, and the one-two punch of contracting GDP in May and growing inflation in June will do little to assuage concerns over what the next six months will hold for struggling businesses. Indeed, with many industries dialing back hiring plans – in part due to the influence of employment taxes and the impact of AI – the much-needed uptick in consumer demand is unlikely to materialize, putting more firms at risk.” Businesses are still in “tough” times, despite the drop in insolvencies in June, cautions David Hudson, restructuring advisory partner at FRP. Hudson says: “The slight fall in insolvencies this month offers a glimmer of relief – especially for hospitality and retail businesses, which are now reaping the benefits of record hot weather. However, we’re still in tough territory. Consumer confidence remains stubbornly low, growth is stuttering – with GDP dipping again in May. June’s unexpected jump in inflation will only serve to continue eroding profit margins and consumer demand. “This environment is forcing businesses to fight on multiple fronts. Many will likely only be experiencing breathing space after dramatically paring back costs. Until demand shows a more sustained recovery and input costs ease further, there’s a risk that this reprieve is just a pause rather than a turning point.” Just in: the number of companies in England and Wales falling into insolvency dropped last month. The Insolvency Service has reported that there were 2,043 registered company insolvencies in England and Wales in June, 8% lower than in May 2025 (2,230) and 16% lower than in June 2024, when 2,430 companies failed. That could ease some concerns over the health of the UK economy, as companies tackle rising inflation and higher taxes. Despite the drop, monthly company insolvency numbers in the first six months of 2025 were slightly higher than the second half of 2024, but remain lower than the 30-year annual high seen in 2023. The Insolvency Service says: Company insolvencies in June 2025 consisted of 332 compulsory liquidations, 1,585 creditors’ voluntary liquidations (CVLs), 111 administrations and 15 company voluntary arrangements (CVAs). There were no receivership appointments. Goldman Sachs has predicted the Bank of England will take a slightly slower approach to cutting interest rates, following this week’s data. Goldman still expect a rate cut in August (from 4.25% to 4%), even though inflation rose in June and private sector pay growth in March-May was higher than expected. But they have now dropped their forecast for a September cut. Sven Jari Stehn, Goldman’s chief European economist, told clients: While the hurdle for speeding up cuts in September looks higher after this week’s data, we now expect sequential cuts from November until reaching a 3% terminal rate in March 2026 (versus February before). That is, we now expect a total of five cuts this year (previously six) and two next year (previously one). That would mean rate cuts in August, November and December this year, and February and March 2026. The Bank has already cut rates twice this year, at its meetings in February and May. Shares in pharmaceuticals firm GSK have dropped over 6% in early trading, after its blood cancer drug Blenrep hit a regulatory hurdle in the US. Yesterday, the US FDA’s panel of independent advisers recommended against Blenrep, citing earlier concerns over eye-related side effects. GSK told the City that it remains confident in the benefit/risk profile of Blenrep and said it will continue to work closely with the FDA as they complete their review of the drug. The final decision on whether to approve a drug rests with the FDA, which will consider the view of its Oncologic Drugs Advisory Committee (ODAC), which voted 5-3 against Blenrep. The company added that Blenrep combinations are approved for refractory multiple myeloma (cancer that does not respond to treatment) in several markets including the UK and Japan, and that applications in other markets including the EU and China are being reviewed. The European Union has announced the approval of a fresh sanctions package on Russia over its war against Ukraine, which includes a revised oil price cap and new banking restrictions. EU member states gave the package the green light this morning after Slovakia lifted its veto. Kaja Kallas, the EU’s High Representative for Foreign Affairs and Security Policy, says the sanctions package – the EU’s 18th – is one of the strongest put together against Russia so far. It includes a ban on more Russian banks accessing the SWIFT international payments system, sanctions on the Nord Stream gas pipelines, and a lower cap on Russian oil sales. Diplomat have told Reuters that the package will lower the G7’s price cap for crude oil to $47.6 per barrel. Bloomberg reports that the new price cap, which is currently set at $60 per barrel, will now be set “dynamically” at $15 below market rates. This follows criticism that Europe has been spending tens of billion on Russian energy since the Ukraine war began, exceeding the cost of it support for Kviv. Energy news: BP has continued its push to pivot back to oil and gas, by agreeing a deal to sell its US onshore wind business to LS Power. The wind business operates nine onshore wind energy assets across seven US states, and are grid-connected and are providing power to customers. William Lin, bp’s executive vice president for gas &amp;amp; low carbon energy, says: “We have been clear that while low carbon energy has a role to play in a simpler, more focused bp, we will continue to rationalize and optimize our portfolio to generate value. The onshore US wind business has great assets and fantastic people, but we have concluded we are no longer the best owners to take it forward. The price of the deal hasn’t been revealed; BP says it is part of its $20bn divestment program to simplify and focus its business. In the City of London, consumer goods maker Reckitt Benckiser has agreed to sell a majority stake in its Cillit Bang and Calgon arm to private equity firm Advent International. The deal is worth up to £3.6bn, and will see Reckitt retain a 30% stake in the essential home business - also including brands such as Air Wick, Woolite, Resolve, Sole and Easy-Off Kris Licht, Reckitt’s chief executive, says: “We are executing our strategic plan at pace. The divestment of Essential Home represents a significant step forward in unlocking the substantial value in our business. This moves Reckitt towards becoming a simpler, more effective world-class consumer health and hygiene company and it will enable us to focus on a core portfolio of high-growth, high-margin powerbrands.” Shares in Reckitt have risen 1.5% at the start of trading, putting it among the FTSE 100 top risers. Katsunobu Kato’s criticism of US tariffs come after Japan’s exports to the United States fell for the third straight month. Data released on Thursday showed that the value of shipments fell 11.4 percent in yen terms in June, compared with the same month last year. The car sector was hit hard, with exports were down 26.7%. The number of vehicles was up, but their average price was down nearly 30%. That could be a sign that automakers are cutting prices or shipping cheaper models to offset the tariffs. Donald Trump’s trade war has loomed over the meeting of G20 finance ministers in South Africa this week. Japan told the gathering of advanced economies in Durban that tariffs aren’t the right way to fix trade imbalances. Finance minister Katsunobu Kato told reporters at the G20: “Japan said that tariffs aren’t really the right tool to fix excessive current accounts imbalances.” Kato argued that countries facing such situations need to address them through domestic efforts, rather than slapping new levies on imports. The US’s trade balance (rarely the healthiest) has actually worsened this year, as American companies raced to import goods before tariffs were imposed. However, US Treasury secretary Scott Bessent won’t have heard Kato’s message as he’s not attending the G20. A finance ministry official accompanying Kato explained that many G20 members argued that market stresses appear to have eased somewhat, Bloomberg reports, as the world economy hasn’t suffered as much as expected from the trade war [although, of course, some of Trump’s new tariffs now don’t start until 1 August]. Good morning and welcome to our rolling coverage of business, the financial markets and the world economy. Relations between the US and China appear to have warmed, slightly, after chipmaker Nvidia was given a green light by Washington to resume sales of its H20 AI chip to Chinese companies. Nvidia’s CEO, Jensen Huang, revealed earlier this week that the US government has assured his company that licences for H20 chip sales to China would be granted, and that deliveries could start soon. That reverses a restriction announced in April, when the White House announced tighter controls on exports of computer chips used for artificial intelligence. And today, Beijing has welcomed this change of heart, confirming that the US has ‘taken initiatives” to approve H20 sales to China again. China’s Commerce Ministry said in a statement that “win-win cooperation” was the right path to go down, and that it hopes the two countries can “meet each other half way” and work together. The ministry also urged the US to abandon its “zero-sum mentality” and cancel ‘unreasonable’ trade restrictions on China, warning that “suppression” will not lead to solutions. The H20 graphics processing unit, or GPU, is an advanced chip for use in AI systems. But it’s less powerful than Nvidia’s top semiconductors today, as it was designed to comply with US restrictions for exports of AI chips to China. Earlier this week, commerce secretary Howard Lutnick revealed that the renewed sale of H20 chips to China was linked to a rare earths magnet deal. He also claimed Nvidia would only be selling China its “fourth best” chip. Even so, the prospect of more sales to China pushed Nvidia’s shares to record highs this week. Orders from Chinese companies for H20 chips need to be sent by Nvidia to the U.S. government for approval. The agenda 9.30am BST: UK insolvency data 10am BST: Eurozone construction output data for May 1.30pm BST: US housing starts data for June 3pm BST: University of Michigan consumer confidence report</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>There were 2,043 registered company insolvencies in England and Wales in June. That is 8% lower than in May 2025 (2,230) and 16% less than in June 2024. Consumer confidence across the US has inched up this month, according to the latest data.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Barclays has been fined £42m over “poor handling” of financial crime risks linked to two clients, including a gold bullion business run by James Stunt, the former son-in-law of Formula One tycoon Bernie Ecclestone. The Financial Conduct Authority (FCA) said the bulk of the penalties, about £39.3m, related to Barclays’ failure to properly screen Stunt’s business – Stunt &amp;amp; Co – and its relationship with Fowler Oldfield, a Bradford jeweller now infamously linked to a large money-laundering operation. The failures spanned 2015 to 2021, and Stunt &amp;amp; Co ultimately received £46.8m from Fowler Oldfield. Barclays was made aware of the fact that Fowler Oldfield was the subject of a criminal investigation involving potential money laundering in August 2016. But the bank only started to review its exposure to the company five years later, when a court fined NatWest more than £264m over its relationship with the purported jeweller, in a case brought by the FCA. The case gained widespread press attention, given the extraordinary details, including that staff had been depositing “big black bin liners” full of cash at a NatWest branch that overwhelmed its floor-to-ceiling safes. The FCA said on Wednesday that Barclays “did not gather enough information at the start of the relationship or carry out proper ongoing monitoring”. In March, two directors for Fowler Oldfield were convicted of money laundering and sentenced to more than a decade in prison each. Stunt was cleared at Leeds crown court of any money-laundering charges in relations to funds received from the purported jeweller. Barclays was also fined £3.1m on Wednesday for failing to check it had enough information to understand the money-laundering risk before opening a client money account for the now-collapsed wealth management firm WealthTek. The FCA in December charged WealthTek’s former head partner John Dance with fraud and laundering more than £64m from the firm’s client accounts. Dance is due to face a criminal trial at Southwark crown court in September 2027. Commenting on the fines, the FCA’s joint executive director of enforcement and market oversight, Therese Chambers, said: “The consequences of poor financial crime controls are very real – they allow criminals to launder the proceeds of their crimes, and they allow fraudsters to defraud consumers. “Banks need to take responsibility and act promptly, particularly when obvious risks are brought to their attention. In the first of these cases, Barclays secured a significant reduction in its fine through its extensive cooperation with our investigation and through making a voluntary payment to affected consumers at our request.” Barclays said the bank remained “deeply committed to the fight against financial crime and fraud”. It added: “The FCA’s investigation relating to Stunt &amp;amp; Co was centred around historical money-laundering activity and made no findings that the bank had breached money-laundering regulations. “As acknowledged by the FCA, Barclays undertook an extensive review and self-reported its findings to the FCA. Barclays fully cooperated with both investigations and has further strengthened its financial crime and other control capabilities.” • This article was amended on 17 July 2025. It was a court that fined NatWest more than £264m, not the FCA; however, the case was prosecuted by the FCA.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Barclays has been fined £42m over 'poor handling' of financial crime risks. Bank failed to properly screen James Stunt's business and relationship with Fowler Oldfield, a Bradford jeweller now linked to a large money-laundering operation. Barclays was also fined £3.1m for failing to check it had enough information to understand the money- laundering risk.</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Time to wrap up…. Britain’s blue-chip stock index has risen through the 9,000-point mark to touch a new high today, before falling back. The FTSE 100 share index hit 9,016.98 points in early trading on Tuesday, taking its gains during 2025 to more than 10%. Analysts said the London stock market had benefited from a range of factors this year, including a move by some investors to diversify away from US shares because of concerns about Donald Trump’s economic policies. The US president’s trade war has also helped UK stocks, as Britain is one of the few countries to have reached a trade deal guaranteeing lower tariffs Inflation shot up in June as the impacts of Donald Trump’s tariffs slowly started to show in US prices. Business leaders have said for months that the high, volatile rates of Trump’s tariffs will force companies to raise consumer prices. Prices remained stable in the spring, particularly as many of Trump’s highest tariffs were paused; however, they started increasing in May and have continued to rise in June. Annual inflation rose to 2.7% in June, up from 2.4% in May, according to the Consumer Price Index (CPI), which tracks the prices of a basket of goods and services each month. Core CPI, which leaves out energy and food prices, ticked up slightly to 2.9%, compared with 2.8% in May. The prices of appliances, furniture and toys, products typically manufactured outside the US, all rose. Food prices increased by 3%, with the price of beef rising by more than 2% over the month, coffee up 2.2% and citrus fruit prices rising 2.3%. While the price of eggs has been dropping over the last few months, a dozen eggs are still 27% more expensive than last year… China’s economy grew more strongly than expected in the second quarter as it proved resilient in the face of Donald Trump’s trade war. China’s gross domestic product (GDP) grew 5.2% in April to June compared with a year earlier, slowing from 5.4% in the first quarter, but just ahead of analysts’ expectations for a rise of 5.1%. Rachel Reeves has unveiled a package of City changes meant to cut “unnecessary” red tape and encourage more financial risk-taking by companies and consumers in the hopes of spurring economic growth. In a financial services strategy dubbed the Leeds Reforms, the chancellor outlined initiatives designed to boost the financial services sector, including plans to cut “unnecessary costs” related to accountability rules for senior bankers, and to launch an advertising campaign to get consumers investing cash savings in stocks. Thames Water has said it could collapse into temporary nationalisation if emergency talks with creditors fail, as it slumped to a £1.6bn annual loss. The loss for the 12 months to 31 March comes after a profit of £154m the previous year, even though revenues climbed by 8.7% to £2.7bn. It had net debt of £16.8bn, up from £15.2bn the year before. Thames’ top management were also warned they could be held in contempt of Parliament if they continue to refuse to hand over board minutes related to the takeover approach from KKR, which collapsed last month. The Footsie’s historic day has ended with a whimper, not a bang. After breaching the tape on the 9,000-point mark in early trading, the FTSE 100 has slipped back during the day. The index of blue-chip shares has just closed down almost 60 points, or 0.66%, at 8938 points, after the jump in US inflation dampened hopes of early interest rate cuts in America. That’s lower than yesterday’s closing high of 8998 points, as well as (obviously) lower than the new intraday high of 9016.98 points set this morning. But the mood in the City is still upbeat. Here’s Neil Wilson, UK investor strategist at Saxo: Overall, I’d say the FTSE has attraction from a value, income and defensive perspective given the volatility we have seen and changed macro backdrop and assumptions about US exceptionalism. a) it’s offering some relative shelter with defensive names, b) benefitting from flow dynamics as investors look beyond the US, c) is enticing value-focused investors with relatively low multiples when growth is at a premium, d) offers a good dividend income yield and e) may be picking up a little juice from the government’s capital investment plans for defence/energy/houses. 10,000 here we come. The US dollar has pushed higher since June’s inflation report was released. The dollar index is now up almost 0.5% against a basket of currencies, probably a sign that hopes of early US interest rates cuts have been hit by the jump in the CPI rate last month. This has pushed the pound down by a third of a cent, to $1.339. Stocks are now lower on Wall Street too, where the Dow Jones industrial average is down 248 points or 0.56% at 44,210. Bank of England interest rate-setter Catherine Mann has said today that UK inflation pressures remained a challenge despite a fall in the pace of pay growth in recent months, Reuters reports. Mann, usually one of the hawkish members of the Bank’s Monetary Policy Committee, told Business in Wales: “We have seen wage rates come down, so people are getting wage increases, but not at the rate in the past. “And we’ve seen price inflation come down quite a bit, but it’s still a challenge because it’s still well above our 2% objective.” We get the next UK inflation report tomorrow morning, followed by new labour market statistics on Thursday…. Donald Trump has repeated his call for sharp cuts to US interest rates. Posting on his Truth Social account, he says: Fed should cut Rates by 3 Points. Very Low Inflation. One Trillion Dollars a year would be saved!!! A three percentage point cut to the Fed Funds rate, as Trump calls for, would lower the Fed’s target rate from 4.25%-4.5% to 1.25%-1.5%. That would be a truly dramatic move for a central bank that likes to move in quarter-point or half-point change (when it moves at all!). For example, in the run-up to the financial crisis the Fed lowered the Federal Funds rate from 4.5% at the end of 2007 to 2% at the start of September 2008. Following the collapse of Lehman Brothers, it accelerated its cuts, and brought the target rate down to 0 to 25 basis points by the end of the year. Digging into the US inflation report, there are some indications that imported goods prices jumped in June. In food, for example, the cost of ‘oranges including tangerines’ rose by 4.7% in June. Instant coffee prices were up 5.1% in the month And among goods, nonelectric cookware and tableware prices rose 4.0% in June, with Audio equipment 2.9% more expensive. Ding ding! The opening bell of Wall Street has been rung, and shares are moving higher despite today’s rise in US inflation. The S&amp;amp;P 500 share index has risen by 32 points, or 0.5% to 6,300 at the start of trading, although the narrower Dow Jones industrial average is only 0.02% higher. The tech-focused Nasdaq index is up almost 1%. Investors seem relieved that core inflation rose by less than expected in June (although the annual rate of core CPI did rise, to 2.9% from 2.8%. Scott Helfstein, Global X‘s head of investment strategy, says: This is kind of a perfect inflation report for the Fed, just hot enough to justify their policy of holding rates steady, but not reflective of runaway prices. The question now is whether the labor market holds up throughout summer, and it probably will. If we see strong corporate earnings for the second quarter, growth forecasts for the US may be revised higher. The financial markets are treating the US inflation report as ‘benign’, reports Kathleen Brooks, research director at XTB: Today’s June US inflation report revealed early signs of tariff-led price increases, though not yet large enough to meaningfully move the headline, reports Atakan Bakiskan, US economist at Berenberg: With more tariff damage ahead, the Fed will certainly not feel content with today’s report, especially as core goods excluding used cars rose 0.3% mom in June -- the highest monthly increase since March 2023. Thames Water’s CEO has confirmed the company appealed to the government to let the company off up to £1bn in fines to avoid special administration. This was previously revealed by my colleagues Anna Isaac and John Collingridge, but now it has been confirmed by the CEO. Chris Weston told the Efra committee this morning that ministers and the regulators need to have a “recognition of the reality of the situation”, namely that they can’t both pay fines for polluting waterways with sewage and financially turn around the company. He added: We have talked to Ofwat about it, we have talked to the Environment Agency about it and we have talked to Defra about it. Chair of Thames Sir Adrian Montague added that they had been talking to the Treasury about the issue. The Treasury is reportedly pressuring Defra to avoid special administration because of an upfront cost of over £3bn. Weston claimed that this does not mean Thames is asking for “special circumstances” even though other companies are expected to pay their environmental fines. He added: I don’t think we are pleading special circumstances just for Thames. I think there are shortcomings in the regulatory regime, and part of what the regulatory regime needs is a structure which allows companies like Thames to turn themselves around for the benefit of customers and the environment. We are suggesting a reset because there isn’t really an alternative. He said that if the fines are upheld that Thames will probably collapse and go into SAR: We are trying to find a pragmatic solution, if we don’t find a solution to this, we will be looking at going into SAR. If any creditor came to Thames they would have to be prepared to accept those penalties and fines, they would have to be prepared to do that, I would imagine they would find that a disincentive to invest in and support Thames, and they wouldn’t do it. Britons should worry about the rising level of government debt, according to the Treasury’s independent watchdog, which warned that it may be difficult to cope with the next crisis without significant reforms to the public finances. Richard Hughes, the boss of the Office for Budget Responsibility, said there were three reasons why a government is financially vulnerable and the UK fails each test. The exposure to shocks is high, the ability to cut spending or raise taxes to provide a buffer is limited, and borrowing is becoming more difficult as traditional lenders, particularly UK pension funds, continue to decline, Hughes explains, saying: In all three of those areas there are reasons for the UK to worry. We are a country that is very exposed to shocks and has been particularly hard hit by the last three shocks the world has faced - the finacial crisis, Covid and then the energy price shock. We have already raised taxes quite a bit, And the size of the state is near a post-war high. And as we highlight in our fiscal risks report, there are concerns around the demand for UK debt and how that demand is going to wane over time, raising the cost of financing it. Back in the UK, new Institute for Fiscal Studies boss Helen Miller made one of her first public appearances in the job this morning, at the Institute for Government, in a discussion about whether Labour is (still?) a mission-driven government. It would be an understatement to say that Rachel Reeves’s team at the Treasury were not fans of her outspoken predecessor, Paul Johnson. But there was little sign from this event that Miller is going to give the chancellor an easier ride. She argued that Labour had failed to make the case for radical reform of tax and spend, either in the general election campaign or afterwards. “So they come into power, they have this ‘bring out the bodies’ event where you say, “Oh, we found a black hole”. Then you have a kind of one and done budget: “We found a black hole, we fixed a black hole”...That was always far too narrow,” Miller argued, adding: “It ignored the massive set of risks that were coming down the road. It didn’t really make room, not just for more spending potentially, it didn’t make room for that broader debate about, ‘we need to reform things, we need to be bold’”. Miller also suggested it wasn’t clear from Labour’s actions since that it is really prioritising its first mission, of growth - despite Reeves’s rhetoric. “I think we should be throwing the kitchen sink at it. It doesn’t feel to me like this is driving through everything, and everyone’s trying to work out, ‘how do we get that growth?’ and everyone’s pushing in the same direction. It feels like, ‘we’re trying some things on the plus side, we’re doing some things on the negative side’ It really doesn’t feel like a driving force.” Miller, who is a tax expert, repeatedly made the case for big bang tax reforms - including replacing vehicle excise duty with road charging and reforming stamp duty on housing transactions, for example. We can expect to hear a lot more about issues like these in the run-up to the crunch autumn budget. Neil Birrell, chief investment officer at Premier Miton Investors, reckons today’s inflation report could help clear the way for a cut in US interest rates in September: There have been a lot of hopes pinned on US CPI coming in lower than expected. June’s data was much as expected, but core inflation undershot, just, for the fifth month on the trot. Obviously, the Fed will be looking at this, but they will want to see the PCE behaving itself before moving policy. However, there is no doubt inflation is OK for now and a September cut in rates is likely. David Rees, head of global economics at Schroders, has spotted some signs in today’s inflation report that the Trump trade war is pushing prices in US shops: “Tariffs loomed large over today’s rise in US inflation, helped up in part by the cost of core goods. For example, household furnishing rose by 1% month-on-month in June. Elsewhere, goods prices were relatively contained, but heightened challenges could be on the horizon if all the Trump administration’s tariff threats are enacted on 1st August. “If they were to happen, we estimate the effective US import tariff rate could jump to 24%, potentially adding more than 1% to inflation - on top of our CPI forecast for average inflation of 3.1% through to the end of 2026 - and cutting GDP by more than 0.5%. “While markets appear to assume President Trump will soften his stance, the risk of stagflation in the US is real - especially if rising goods and services prices feed through to a tight labour market.” Donald Trump will be pleased that today’s US inflation report shows a fall in egg prices. Earlier this year, the US president insisted that egg prices are tumbling. And we can now see that in June, egg prices fell by 7.4% month-on-month. However, a rise in beef prices means that overall index for meats, poultry, fish, and eggs only dropped by 0.1% in June. But on an annual basis, the egg picture is less pleasing. The meats, poultry, fish, and eggs index has risen by 5.6% over the last 12 months, driven by a 27.3% increase in egg prices over the year. Still, that’s better than in February when eggs cost 59% more than a year ago. Newsflash: Consumer price inflation across the United States has accelerated, rather undermining Donald Trump’s claim that there is no inflation in the US. The US CPI index increased by 2.7% in the year to June, new data from the US Bureau of Labor Statistics shows. That’s up from 2.4% in May. Food prices rose by 3.0% over the year, while energy prices were 0.8% lower than a year ago. Core inflation, which strips out food and energy, rose by 2.9% over the last 12 months, up from 2.8% in the year to May, but lower than expected. The BLS says: Indexes that increased over the month include household furnishings and operations, medical care, recreation, apparel, and personal care. The indexes for used cars and trucks, new vehicles, and airline fares were among the major indexes that decreased in June. There has been a big debate at parliament today over whether or not it is appropriate, or legal, for Thames Water to be paying bonuses worth 300% of salary to 21 senior executives, my colleague Helena Horton reports. During the select committee hearing, Ian Pearson, a former Labour minister who now chairs the remuneration committee at Thames, gave a novel explanation. He said: “We all have husbands and wives back at home who ask questions, why don’t you go and work for somebody else that will pay you more”. The bonuses appear to have been constructed to get around environment secretary Steve Reed’s water (special measures) act. This is because the act bans specifically performance related bonuses to the CEO and CFO of a company. These are retention payments, paid regardless of employee performance. Thames says it can still pay these out, though they are currently on pause. The first tranche was paid in April of this year. Pearson explained: “We thought it was best to pause the plan and reflect on guidance that was coming from Ofwat. No decision has been made on restarting. I think we should always reserve the right to do things. What we are trying to do here is retain senior staff and we are trying to do so and reconcile that with the framework thats been set by Defra and by Ofwat. The payments that were made in April were to senior people in the organisation, they are not in any way related to Ofwat’s PRPP prohibition bill or to the water (special measures) act. “ They even believed that under the ban, they could pay CEO Chris Weston 300% of his salary in a retention payment. Weston declined the bonus. He said: “I decided that I wouldn’t participate. I was pleased the board expressed the confidence in me that they would offer it to me, but I felt that would be too much of a distraction and my number one priority was to address the stability in my team.” Sir Adrian Montague, the chair of Thames, said that they disagree with Reed on whether the bonuses can be paid: “We believed and continue to believe that the special measures act does not affect these bonuses. We don’t want to rest on that position, the secretary of state has made his views quite clear. I hope the secretary of state realises the interest we have in retaining our staff. We have not had a conversation with the department or the SoS about our dilemma. We need to retain these staff to see this restructuring through.” The Trump White House has given America’s top central banker another nudge to consider his future. US treasury secretary Scott Bessent said a “formal process” is already starting to identify a potential successor to the Federal Reserve chairman Jerome Powell. Bessent told Bloomberg TV: Well, look, there’s a formal process that’s already starting. There are a lot of great candidates, and we’ll see how rapidly it progresses. It’s President Trump’s decision, and it will move at his speed. Powell’s term as Fed chair expires next May, but there have been repeated chatter that Trump might try to fire him, and install a Fed chair more likely to cut interest rates. Technically, Powell could remain on the Fed board until his tenure as a governor expires in January 2028. But Bessent (who’s been reported to be a potential candidate!) also argued it would be “confusing” for Powell to remain at the Fed after his term as chair ends. Traditionally, the Fed chair also steps down as a governor, and there’s been a lot of talk of a shadow Fed chair causing confusion in advance of his or her nomination. And I can tell you, I think it’d be very confusing for the market for a former Fed chair to stay on. Just in: the boss of banking giant JP Morgan has warned that trade war uncertainty is looming over the US economy, after reporting a drop in profits. JP Morgan has kicked off the US bank reporting season by revealing a 17% drop in net income in April-June, to $15bn. Net revenue fell 10% to $45.7bn. However, these measures are distorted because last year, JP Morgan gained $8bn through an exchange of shares in credit card giant Visa. Income at its consumer &amp;amp; community banking arm was up 23%, while commercial &amp;amp; investment bank income rose 13%. Dimon says: The US economy remained resilient in the quarter. The finalization of tax reform and potential deregulation are positive for the economic outlook, however, significant risks persist – including from tariffs and trade uncertainty, worsening geopolitical conditions, high fiscal deficits and elevated asset prices. As always, we hope for the best but prepare the Firm for a wide range of scenarios. Thames Water’s top management have been warned they could be held in contempt of parliament if they continue to refuse to hand over board minutes related to their proposed rescue deal with KKR, which collapsed last month. The Efra (environment, food and rural affairs) committee want to know why Thames plumped for KKR as its preferred partner, only to see the US private equity giant walk away in June, and also want to know why the KKR approach failed. Efra committee chair Alistair Carmichael tells Thames at this morning’s hearing: Can I just be quite clear about this? In the event that we invoke the formal powers that parliament has given us, not to provide these minutes will be a contempt of parliament. Is that understood? Thames chair Sir Adrian Montague says the company “understand and respect the committee’s powers”, before arguing that it is inappropriate at this juncture to give these minutes, for several reasons. First, they contain confidential information concerning all the bidders; Thames are subject to confidentiality undertakings with regard to information. Second, he says, the company is subjected to market abuse regulations which control the dissemination of material, non-public information. The most important point, Montague argues, is that discussions over Thames’s future are at a “a very sensitive stage”. Right now, it will be “really difficult to really counterproductive” to release these documents, he insists. Montague also describes KKR’s bid as’ ‘exceptional’, adding that they didn’t give many reasons when they withdrew, but that KKR said they saw no financial or operational reason why they should not have been able to continue. The government’s battle against red tape means it is proposing changes to rules brought in after the financial crisis to hold senior bankers to account. The Treasury says it is consulting on reforms to the Senior Managers &amp;amp; Certification Regime, with the aim of “streamlining the regime to support growth and competitiveness”. The SM&amp;amp;CR was brought in to hold senior managers accountable, following the disastrous decisions that led to the worst financial crisis since 1929, almost 20 years ago. Today, though, the UK’s financial watchdogs – the Financial Conduct Authority (FCA) and Prudential Regulation Authority (PRA) – want to change it to drive growth in financial services. The proposals include: Give firms more time and flexibility to submit applications for approving new senior managers when there has been an unexpected or temporary change. Strip out duplication where the same individuals are certified for separate functions, which would reduce the number of certification roles by 15%. Provide guidance on how to streamline the annual checks firms need to undertake to certify individuals are ‘fit and proper’ to do their role. Allow more time for firms to report updates to senior manager responsibilities. Increase how long criminal record checks for senior manager applications are valid for, prior to application submission. Help firms to better understand the definition of certain SMF roles. Give firms more time to update the directory, which lists certified staff. This streamlining may sound sensible. But, those who lived through the financial crisis of 2007-08 could be concerned that regulators are backsliding. Indeed, the Treasury has launched a consultation about potentially developing a more proportionate replacement for the Certification Regime; significantly reducing the number of roles requiring regulatory pre-approval; and further streamlining the assessment process. Sam Woods, chief executive of the PRA and deputy governor for prudential regulation at the Bank of England, suggests the new rules will still ensure ‘high standards’, saying: High standards of accountability are important for maintaining confidence in our financial services industry. Today’s changes will reduce the burden of the Senior Managers and Certification Regime without diluting accountability, and we will work with the government on further reforms. Alistair Carmichael then asks Thames about its lamentable record on pollution, with incidents up in the last year (see 7.59am post). Carmichael points out that this morning’s annual report indicates that there was too much rain leading to overflows, shortly before Thames announced hose pipe bans! Thames Water CEO Chris Weston says “I’m sorry about that”, before insisting that the weather is a reason, not an excuse. He says: Last winter, before we came into this spring, we had the second wettest winter on record. There were some months like last September, where the rainfall was more than double the normal monthly rainfall, and our system, I’m afraid, was never intended to deal with that. We are taking huge steps to improve our position around pollutions. We are cleaning the network more than we ever have, and we are investing more than we ever have in our sewage treatment works, but it is going to take a while. Weston then suggess that turning around and transforming Thames “is going to take Between five and 10 years. Maybe a bit more.” This morning, he said this task could take at least a decade. Over in parliament, the chair of Thames Water has apologised to MPs after the company was recalled before the Environment, Food and Rural Affairs Committee. Sir Adrian Montague kicked off this morning’s session in a penitent manner, telling committee chair Alistair Carmichael MP: I’m making an apology. It’s rare, as you said yourself, for water companies or any company to be recalled to the committee. We regret that we have made that necessary. We have tried to be as forthcoming as we can with our disclosures. We will no doubt go into some of the reasons behind the actions we’ve taken. But I just wanted to say before we start, honestly, you’re all busy people. I’m sorry that we are taking up your time again. Carmichael had begun the session by telling Montague, CEO Chris Weston and non-executive director Ian Pearson, that Thames had been recalled after a ‘quite extraordinary session’ back in May. Carmichael says the recall was triggered by Montague telling the committee he had “mis-spoken” in the first hearing, which Carmichael says came to light after an inquiry from the Guardian. [Reminder: Montague told the committee that large bonuses for senior bosses which were to be paid from an emergency £3bn loan were insisted upon by creditors. We then reported that sources and court documents suggest the bonuses were agreed to by the creditors but not necessarily proposed by them.] Carmichael says Thames have since provided “significant amounts of information”, which he thinks could have been handed over earlier if the company was committed to transparency. He then accuses Thames of “quite a bit of gameplaying”, saying the committee only recieved a list of its senior creditors at 5.20pm yesterday, and pointing out that its annual report has been filed today, the last possible day. The Treasury also point to the Bank of England’s decision, last week, to relax mortgage lending rules. They say: First-time buyers will be supported to get on the housing ladder, with the Bank of England allowing more lending at over 4.5 times a buyer’s income – which could help 36,000 more people buy a home over its first year and are helping Nationwide support an additional 10,000 first-time buyers by lowering income thresholds for its popular ‘Helping Hand’ mortgage from tomorrow. Simplified mortgage lending rules being considered by the Financial Conduct Authority will also make it easier for existing borrowers to remortgage, while the introduction of a permanent government-backed Mortgage Guarantee Scheme will secure the availability of high loan-to-value mortgage products in times of economic uncertainty. The new guidelines announced by the Bank of England last week mean that individual banks and building societies can offer more high loan-to-income (LTI) mortgages, which are equal to, or worth more than, 4.5 times a borrower’s annual earnings. Rachel Reeves is also pledging to cut red tape, in a push to attract investment and drive growth. Under the ‘Leeds’ reforms just announced, “unnecessary financial red tape” will be “drastically cut”, the Treasury says. They add: A new concierge service within the Office for Investment will harness UK networks globally to actively court international financial services companies, creating a one-stop-shop to promote the UK and provide tailored support to help businesses plan where to invest based on their needs – better harnessing specialist clusters across the country from asset management in Edinburgh, to Fintech in Leeds and Cardiff, and insurance in Norwich and Norfolk. A key part of the new ‘Leeds’ financial services reforms is a push to encourage people to invest more. The Treasury says the UK has the lowest level of retail investment among G7 countries – that deprives businsses of capital, and means savers may miss out on returns. So, there is going to be a new ‘industry-led ad campaign’ to explain the benefits of investing to the public (which feels slightly odd, as investment firms do this anyway). From next April, the Financial Conduct Authority will allow banks to alert customers about specific investment opportunities to consider shifting money from a low-return current accounts to higher-performing stocks and shares investments. There’s also going to be a review of risk warnings on investment products, “to make sure they help people to accurately judge risk levels”. There has been speculation in recent weeks that Rachel Reeves could cut the amount of cash people could save in an Isa (a tax-free investment and savings account), to encourage people to put money into stocks and shares instead and boost the economy. That idea has been paused, though, after a backlash from the industry. Instead, the government says it will “continue to consider reforms to Isas and savings” to achieve the right balance between cash savings and investment. But as a first step, saves will be allowed to hold Long Term Asset Funds in Stocks &amp;amp; Shares Isas next year. This, they say, will help people to invest in assets such as innovative businesses and infrastructure – which could drive growth, and “can also deliver better returns”. There’s an investing mantra that people should only put money into the markets which they’re prepared to risk. The Treasury, though, is hailing the potential benefits of investing, saying: Stocks and shares have performed significantly better than cash savings accounts in recent decades. According to some industry estimates, more than 29 million adults across the UK have cash sitting in a low-interest rate account offering around 1% - while the average return for stocks and shares over the last 10 years is around 9%. If those savers invested £2000 today, they could have £12,000 in 20 years’ time. This compares to £2,700 if they held this money in a cash account offering 1.5% at the current interest rate, making them over £9,000 better off. This is a timely point, with the FTSE 100 share index at its record high today… Over in Leeds, Chancellor Rachel Reeves is setting out “the biggest reforms to financial services for much more than a decade”. Setting out the “Leeds reforms” in the West Yorkshire city, she says the government is aiming to “really invigorate our financial services sector”, and thus reinvigorate the whole economy. PA Media report that Reeves told finance chiefs in Leeds: We are fundamentally reforming the regulatory system, freeing up firms to take risks and to drive growth. Second, we’re providing certainty for banks operating in the UK, and ensuring that UK banks have the ability to compete internationally and drive economic growth. Third, we’re doubling down on making the UK an innovation capital and the place of choice for fintechs to start up, to scale up and to list in the UK. Fourth, we’re seizing opportunities in areas where we are already world leading, including asset management, sustainable finance and specialty insurance. And fifth, we are delivering prosperity by increasing the firepower of our capital markets and boosting retail in</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>The FTSE 100 share index hit 9,016.98 points in early trading on Tuesday. Analysts said the London stock market had benefited from a range of factors this year, including a move by some investors to diversify away from US shares. Inflation shot up in June as the impacts of Donald Trump’s tariffs slowly started to show in US prices.</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Time to recap… The pound dropped to a three-week low after the governor of the Bank of England said it could make bigger cuts to interest rates if the job market slows too quickly. Andrew Bailey said “slack” was opening up in the UK economy, as higher taxes have squeezed employers. He told the Times: “I really do believe the path is downward” for interest rates. The bank rate stands at 4.25%, after four quarter-point cuts in the last year, and the Bank is next scheduled to make another decision on 7 August. Bailey said: “If we saw the slack opening up much more quickly, that would lead us to a different conclusion. “I think the path [for interest rates] is down. I really do believe the path is downward but we continue to use the words ‘gradual and careful’ because … some people say to me: ‘Why are you cutting when inflation’s above target?’” The market-implied probability of a UK interest rate cut in August jumped to over 88% following Bailey’s comments. European markets have weakened after Donald Trump announced a 30% tariff on EU imports – a threat described as “absolutely unacceptable and unjustified” by Denmark’s foreign minister today. Germany’s DAX is down 0.8% today, with France’s CAC 40 index losing 0.5%. The EU’s lead negotiator with the US, Maroš Šefčovič, warned that a tariff of 30% or more would have a huge impact, making it “almost impossible to continue” current transatlantic trade, which is worth €4.4bn (£3.8bn) a day. Ministers are to consider handing over ownership of the Post Office to its operators after the Horizon IT scandal. A water company serving 3.9 million customers in London and south-east England has doubled the pay of its chief executive, despite the regulator saying it had “elevated concern” over its financial situation. There’s a mixed start to trading in the US market today, as investors ponder President Donald Trump’s latest tariff threats against the EU and Mexico. The Dow Jones industrial average is slightly in the red, down 17 points or 0.04% at 44,354 points. The broader S&amp;amp;P 500 index has slipped by almost 0.2%. Over in Wall Street, shares in aerospace manufacturer Boeing rose 2% at the start of trading, after an early report into the Air India disaster did not recommend action against the company. On Friday, the preliminary report found that fuel to both engines of the plane that crashed and killed 260 people last month appears to have been cut off seconds after the flight took off. The U.S. Federal Aviation Administration and Boeing have privately issued notifications that the fuel switch locks on Boeing planes are safe, according to a document seen by Reuters. EU’s trade chief Maroš Šefčovič is also speaking the briefing in Brussels, and says he echoes Rasmussen’s comments. Šefčovič tells reporters in Brussels that the EU has approached the talks with United States constructively, and in good faith. Šefčovič says the EU needs to focus on four areas, both in the run-up to the new deadline of August 1 and also beyond. On negotiations. Šefčovič says the EU remain convinced that the transatlantic relationship deserves a negotiated resolution, one that leads to renewed stability and cooperation. Šefčovič says he will continue talks with his US counterparts later today, insisting the EU “never walks away without genuine effort”. Šefčovič says “it takes two hands to clap”, so the EU must also prepare “well-considered, proportionate measures” to restore balance to the transatlantic relationship. He explains that the European Commission has drawn up a proposal for a second list of US imports, totalling €72bn, which could be subject to counter-tariffs. Member states now have a chance to discuss this list, he explains. [Reminder: the EU has decided to postpone its first set of retaliatory countertariffs on €21bn of US goods, in the hope of agreeing a trade deal] Over in Brussels now, the EU are holding a press conference following a Foreign Affairs Council meeting on trade. Lars Løkke Rasmussen, Minister of Foreign Affairs of Denmark, opens by explaining that ministers discussed the state of play and prospects for EU US trade relations, including possible EU countermeasures. Rasmussen adds that ministers also discussed President Trump’s announcement over the weekend of 30% general tariffs on the EU from 1 August, adding that “member states find [Trump’s announcement'] absolutely unacceptable and unjustified.” Rasmussen declares: We are committed to continuing working with the US on a negotiated outcome. It has to be a mutually beneficial agreement on terms that are acceptable to both sides. He adds that the EU is “prepared for all possible scenarios”. If no satisfactory solutions can be found, the EU remains ready to react, and that includes robust and proportionate countermeasures if required. Rasmussen says there was a “strong feeling of unity” in the room today. You can watch the briefing here: The big picture today is that markets remain calm despite the growing risks of tariffs, says Gabriele Foa, portfolio manager at Algebris Investments: “A broad set of new tariffs and threats were announced last week, targeting a wide range of countries and sectors, with rates reaching up to 200% on pharmaceuticals. However, markets are not fully reflecting the scale of these tariff threats, particularly given how aggressive some of the proposed rates are. European markets opened a bit soft on Monday, with no major moves. The copper market shows some divergence, with the London–US prices’ spread implying roughly a 50% probability of the copper tariff being implemented. In Brazil, where a 50% tariff is set to be imposed on exports, USDBRL and local rates initially sold off on the announcement but quickly reversed. More broadly, rates markets are not pricing in any growth disruption these measures could cause. Equity markets remain resilient and appear to be underestimating the potential inflation spike and demand hit that could follow. We see risks skewed to the downside.” Germany’s DAX index is still leading the losses across Europe today, down almost 0.9%. Carmakers are among the fallers, such as BMW (-2%) and Mercedes-Benz (-1.7%). Online retailer Zalando (-5%) is the top fallers, after Morgan Stanley lowered its price target and warned of growing disruption from TikTok Shop’s expansion into Europe. White House National Economic Council director Kevin Hassett has told reporters at the White House this morning that trade talks are still under way between the US and the European Union, Canada and Mexico. Asked about his expectations of talks with the EU, Hassett said: “We’ll see ... we’ve got a few weeks left.” The owner of McVitie’s has announced plans to inject £68m into its British operations in a bid to “supercharge” the growth of its brands. Turkish-owned snacking giant Pladis said investment funds will be used to boost manufacturing capacity and productivity across its factories. The London-based company, which also owns the Jacob’s and Godiva brands, added that it has “earmarked the bulk of the cash” to pump into sites across the north-west of England. The plans will include a £33 million overhaul of its Liverpool Aintree site, where it bakes Jacob’s cream crackers. It will have a comprehensive refurbishment which will include the installation of new ovens and infrastructure. Back in the markets, France’s long-term borrowing costs have hit their highest level since the eurozone debt crisis almost 14 years ago. French 30-year bond yields have risen by 3 basis points (0.03 percentage points) to 4.23% this morning. That’s the highest level since November 2011, when the eurozone was gripped by political instability and political turmoil, reflecting some anxiety about the US-EU trade situation. Bond yields rise when bond prices fall, and are a gauge of the cost of issuing new debt. French 10-year bond yields are flat on the day, right now, and still below levels hit in March this year… Water news: Households in several English counties have just been hit by a hosepipe ban. Thames Water has announced that a hosepipe ban across Swindon, Gloucestershire, Oxfordshire, Berkshire and Wiltshire will kick in at one minute past midnight on Tuesday 22 July. The ban will apply to all OX, GL, SN, RG4,RG8 and RG9 postcodes. Thames explains that the current heatwave has hit water supplies to these areas, saying: Water for much of this area is supplied by Farmoor Reservoir. Farmoor is fed by pumping water from the River Thames. The amount of water we can pump is dependent on the amount of flow in the river. We must leave enough flow remaining to protect the environment and maintain navigation. The very dry and warm weather we’ve had means that the flow in the river is low. This therefore impacts the amount of water we can pump into Farmoor Reservoir. Some homes in Oxford had an, umm, dry run of water disruption last week – some homes and businesses in the city were left with no water or low pressure due to a burst pipe (including my excellent local pub!). MP’s will hear from Thames Water chairman Sir Adrian Montague, CEO Chris Weston, and non-executive director Ian Pearson tomorrow morning, to discuss the company’s financial problems. The spot price of silver has hit its highest level since 2011 this morning. Silver traded as high as $39.09 per ounce, a 14-year high. Rostro’s chief market analyst, Joshua Mahony, says the jump in silver is an example of “resurgent demand for non-fiat assets” (see also bitcoin), adding: Notably, the rise in US debt coupled with higher stimulative spending does provide the basis for a more optimistic outlook for silver given its industrial use cases. Another factor could be Donald Trump’s surprise 50% tariff on copper, which could spur higher demand for silver imports, just in case…. Bloomberg reports that increased demand is leading to tighter physical supply of silver. Germany’s exporters have grown less competitive in recent years, leading to a fall in thir market share, the country’s central bank is warning today. The Bundesbank has calculated that more than three-quarters of the losses in export market shares between 2021 and 2023 were due to a deterioration in the competitiveness of German exporters. In a new report into “the sustained decline in German export market shares”, the Bundesbank says: The weak performance of German exports in recent years has been accompanied by significant market share losses for the German export industry. German export market shares have been contracting since 2017 and have increasingly fallen behind those of other advanced economies since 2021. As a result, the losses in market share have contributed significantly to the sluggish growth of the German economy. The Bundesbank has concluded that this decline is due to supply-side problems within Germany’s economy, which have affected some of its largest sector. It says: The machinery industry, electrical industry and energy-intensive sectors such as the chemical industry were the biggest contributors to the drop in competitiveness. The sectoral profile and timing of the losses in competitiveness suggest that supply chain problems and energy price increases weighed particularly heavily. Bloomberg have spotted that options traders are turning against the pound. They explain: One-month risk reversals — which show the difference in demand for bullish and bearish options — reflect the most negative outlook for the pound since February. The measure spans the next Bank of England and Federal Reserve decisions, as well as President Donald Trump’s 1 August tariff deadline. UK government ministers are to consider handing ownership of the Post Office to post office operators in the wake of the Horizon IT scandal, my colleague Mark Sweney reports. The Department for Business and Trade (DBT) has published a green paper starting the first major review of the scandal-plagued organisation in 15 years. The review, which will run until the 6th of October, follows the publication last week of the first part of the two-year public inquiry into the Horizon IT scandal. Ministers said that part of the review will include looking at ownership of the Post Office, which is ultimately controlled by the government, including the possibility of mutualisation. Ministers have previously met with representatives of post office operators to discuss the possibility of handing ownership to the network branch managers who run its 11,500 outlets. “This green paper marks the start of an honest conversation about what people want and need from their Post Office in the years ahead,” said Gareth Thomas, the post office minister, adding: “Post Offices continue to be a central part of our high streets and communities across the country. However, after 15 years without a proper review, and in the aftermath of the Horizon scandal, it’s clear we need a fresh vision for the future.” Wall Street is set to open lower in a little over four hour’s time, following Europe’s lead. The Dow Jones industrial average, the S&amp;amp;P 500 and the tech-focused Nasdaq are all down 0.3% in pre-market trading. Joshua Mahony, chief market analyst at Rostro, says: Donald Trump has once again done his best to dampen market sentiment, with mainland European stocks in the red and their US counterparts likely to follow suit. This comes after Trump’s tariffs letters reached the EU (30%) and Mexico (30%), building on the 35% tax announced for Canadian imports last week. We now have less than three-weeks until the 1 August deadline comes into play, and the EU are already warning of a prospective 21 billion euros worth of goods that they would target in return. Nonetheless, there is a clear desire to strike a deal, even if that means keeping the 10% tariff and seeking concessions on the sector specific taxes on the likes of the auto sector. Donald Trump’s deadline of 1 August for trade deals, or new high tariffs, could create market turbulence this summer. Henry Allen, economist and strategist at Deutsche Bank says investors should beware the end of this month…. Last year, the late-July/early August period set the stage for the worst market turmoil of 2024. This year, that week looks seriously problematic again from a market perspective. First, there’s the new August 1 tariff deadline. Markets are clearly not pricing in these higher tariffs, and we may only know the outcome in the final hours, offering the potential for a sharp market reaction and heightened volatility. Second, it’s the US jobs report that same day, and last year demonstrated that even a modest downside surprise can cause a big selloff, if investors are already jittery. Third, long-end bond yields are going into this period at higher levels today, meaning it would take less of a jump before we move into problematic territory that re-ignites fears around fiscal policy. This means the market narrative could suddenly shift in a more negative direction. If the tariffs snap back higher on August 1, and we then get an underwhelming jobs report, that would easily resurrect fears around a US recession. Despite Donald Trump’s tariff threats, Berenberg economist Salomon Fiedler believes the general US tariff rate on EU imports will end up “far below 30%”. Fiedler says there are several reasons for optimism that a deal will be reached: Trump has multiple times staked out extreme initial positions as a negotiation tool to be able to later “compromise” at a point still closer to his position. For example, on “Liberation Day” Trump initially announced a 20% tariff on the EU which he then rolled back to 10%. Since then, the EU seems to have accepted this 10% rate as the new baseline against which it will not retaliate. The fact that Trump only threatened the new 30% rate for 1 August, instead of implementing it more quickly, suggests he is still looking to negotiate. Inflation is unpopular. Over the summer, firms will increasingly pass on higher import costs to US consumers as the inventories they built up in anticipation of Trump’s tariffs empty out. Rising inflation (and the prospect of Fed rate cuts becoming ever more remote) may give Trump second thoughts about adding yet even more tariffs. Possibly, part of Trump’s motivation for the high tariff threat now was to shift the public debate in the US back towards more familiar ground (and away from, e.g., the Epstein files debacle). But Fiedler adds there are several reasons for pessimism, which could lead to the Trump tariff on the EU ending up rather higher than 10%: The tariffs alone will not fix the US’ trade deficits, which will thus remain a sore spot for the remainder of Trump’s term. Trump is not only using tariffs as a trade policy tool but also as a source of revenues to plug at least part of the gaping hole in the federal budget. Recent comments from his administration suggest that they rely even more on tariff income than we previously assumed – and that they thus may be tempted to collect even more money by raising rates. The always remote hope of a good negotiation outcome – the bilateral removal of all tariffs and some other trade barriers between the EU and the US – has all but disappeared from view by now A Bank of England interest rate cut next month is looking more likely, according to the latest city pricing. The money markets are indicating there’s now an 85% chance that the Bank cuts interest rates at its next meeting on 7 August, up from 76% at the end of last week. This follows BoE governor Andrew Bailey’s suggestion that the Bank is ready to make larger cuts to interest rates if the jobs market shows signs of a pronounced slowdown (see opening post). The City is expecting a quarter-point reduction, lowering Bank rate from 4.25% to 4%. Victoria Scholar, head of investment at interactive investor, points out that the next UK inflation report, on Wednesday, will be crucial too: Scholar writes: Friday’s disappointing GDP figures, combined with these weak jobs figures boost the case for the Bank of England to cut interest rates in August. The central bank’s governor Andrew Bailey told The Times ‘slack’ was opening up in the labour market, and he believes ‘the path is downward’ for interest rates. All eyes are on Wednesday’s inflation report with CPI expected to remain at remain around 3.4% in June, roughly unchanged for the third consecutive month.” Britain’s major stock market index is shrugging off trade war jitters. The FTSE 100 share index has risen by 15 points, or 0.18%, to 8956 points, towards the record highs set last week. Donald Trump’s threat to impose a 30% on European Union imports from next month is weighing on European stock markets this morning. Most of Europe’s markets have dropped at the start of trading, pulling the pan-European Stoxx 600 index down by 0.6%. Germany’s DAX has dropped by 0.95%, while France’s CAC 40 has lost 0.8%, Italy’s FTSE MIB index is almost 0.9% lower, and Spain’s IBEX is off 0.7%. Investors will be assessing the chances of the two sides reaching a deal by 1 August, and noting EU trade commissioner Maroš Šefčovič’s suggestion that the two sides are approaching a good outcome (see 8.06am). Richard Hunter, head of markets at interactive investor, says Trump’s tariff threats “show no signs of abating”, adding: Inadvertently or otherwise the President is testing the market’s patience. At a time when investors had seemingly brushed aside the likelihood of the base line of tariffs settling at 10%, the new pronouncements suggest a level of between 15% and 20% being the norm, with additionally punitive numbers on the likes of Canada at 35% adding to the uncertainty. The so-called “TACO” trade will therefore be tested again, with markets drifting in the US on Friday and futures currently suggesting a similar fall today. In addition, and as the new 1 August extension approaches, nerves are likely to jangle. The pound is slipping lower against the dollar – it’s now down almost half a cent at $1.3457 (still a three-week low). Jefferies’ Mohit Kumare says Bank of England governor Andrew Bailey “was on the dovish side” in his interview with The Times, “suggesting that the path of rates is downwards”. EU trade commissioner Maroš Šefčovič has claimed the European Union and United States are approaching a good outcome in their trade talks. Despite Donald Trump announcing 30% tariffs on EU exports on Saturday, Šefčovič struck an upbeat tone this morning, saying: “The feeling on our side was that we are very close to an agreement.” Šefčovič also warned that the 30% tariff threatened by Trump would practically eliminate trade, Reuters reports. He was speaking before European trade ministers meet in Brussels to discuss the situation. Some economists also believe that the US and EU will reach an agreement Mohit Kumar of investment bank Jefferies says: We see the 30% tariffs announcement as an opening move and eventual tariffs are likely to set lower in the 10-15% range. The announcement of higher tariffs is a negotiation tactic which should encourage EU and other countries to make a deal quickly. However, the recent tariff announcements over last week also highlight the uncertainty around tariffs and that uncertainty has probably moved up a notch. Trade data released this morning shows that China’s exports regained some momentum in June. China’s exports rose 5.8% in June from a year earlier to $325bn, while imports rose 1.1% to grow, according to data from the General Administration of Customs. Shipments to the US fell 16.1% from a year earlier, a smaller decline than the 34% fall recorded in May. That may show that the trade agreement hammered out by Washington and Beijing in Geneva, and London, this year has helped smooth trade flows. Bitcoin has surged to a new record high this morning, clearing the $120,000 point for the first time. The world’s largest crypto currency is now trading at $122,571, amid interest from institutional investors and the Trump White House’s pro-crypto atmosphere. It has now gained 30% so far this year (and roughly 1,200% over the last five years). Tony Sycamore, market analyst at IG, reports that money has been pouring into exchange traded funds which give exposure to Bitcoin, explaining: Its gains have been driven by strong inflows into ETFs, including BlackRock’s Bitcoin ETF IBIT, which, after receiving $1.7bn in inflows last week, now manages $84bn in FUM (funds under management). Ipek Ozkardeskaya, senior analyst at Swissquote Bank, suggests that bitcoin is “now back in overbought territory”, which could mean it slips back to the $105K–$110K range, adding: Still, the rally is underpinned by a crypto-friendly US policy shift and growing emerging market adoption — both remain intact. Update: that policy stance could turn even more friendly soon. It’s ‘crypto week’ in Congress, where US lawmakers will be considering a number of bills aimed at creating clearer regulatory frameworks for digital assets. European stock markets are on track to open lower, following Donald Trump’s threatened 30% tariff on EU imports. The EUROSTOXX 50 index of large European companies is down 0.72% in futures trading, while DAX futures (the German stock market) are down 0.84%, Reuters reports. The euro is also weakening this morning, after Donald Trump announced that goods imported from the European Union will face a 30% US tariff rate from 1 August. Trump’s latest trade war bombshell has disappointed the EU, as the two sides had been negotiating for weeks. Europe had hoped Trump would agree to a bare bones deal similar to the UK’s pact, that would have lowered tariffs on car exports and steel. But instead, the US president has decided to impose higher costs for US importers who buy goods from the EU. In response, the EU has decided to delay, again, its own retaliatory tariffs on US exports, European Commission president Ursula von der Leyen said yesterday: “The United States has sent us a letter with measures that would come into effect unless there is a negotiated solution, so we will therefore also extend the suspension of our countermeasures until early August. “At the same time, we will continue to prepare for the countermeasures so we’re fully prepared.” Given Trump’s track record, the planned August tariff increases aren’t guaranteed… That may be why the market reaction is modest, so far, with the euro down 0.17% at $1.1669. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. The pound has dropped to a three-week low this morning, after the governor of the Bank of England said it could make larger cuts to interest rates if the jobs market slows quickly. Andrew Bailey told The Times that “slack” was opening up in the UK economy, following the increase to employers’ national insurance contributions. That slack should create downward pressure on inflation. Bailey insisted: “I really do believe the path is downward” for interest rates. Bank rate is currently 4.25%, following four quarter-point cuts in the last year, with the Bank next scheduled to set rates on 7 August, Bailey added: “If we saw the slack opening up much more quickly, that would lead us to a different conclusion.” “I think the path [for interest rates] is down. I really do believe the path is downward but we continue to use the words ‘gradual and careful’ because … some people say to me, ‘Why are you cutting when inflation’s above target?’” Governor Bailey also pointed to Rachel Reeves’s decision to hike taxes on employers, saying companies were: “adjusting employment and hours and also having pay rises that are possibly less than they would have been if the NICs change hadn’t happened”. Last week, the Guardian revealed that the National Trust is to cut at least 550 jobs in efforts to save £26m after changes made in Reeves’s debut budget pushed up labour costs. Hospitality firms have repeatedly warned that higher NICS will force them to cut jobs. And indeed, new data this morning shows that the number of people hunting for jobs has surged at the fastest rate since the height of the Covid pandemic. Following Bailey’s rate cut hint, the pound has dropped by 0.2% this morning to $1.3467. That’s its lowest level since 23 June, three weeks ago, extending its recent losses.</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Andrew Bailey said “slack’ was opening up in the UK economy. He said higher taxes have squeezed employers. The bank rate stands at 4.25%, after four quarter-point cuts in the last year.</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>And finally… After a strong day’s trading in London, the FTSE 100 share index has ended the day at a new closing high. The blue-chip share index has closed up 108.64 points, or 1.23%, at a new end-of-day peak of 8975.66 points. Earlier in the session, the Footsie pushed its new intraday high record even higher, to 8979 points. Mining stocks led the rally, with Glencore (+39%), Rio Tinto (+3.9%) and Anglo American (+3.7%) at the top of the list of risers, along with equipment rental firm Ashtead (+3.8%). “It’s hard to think it was only last year that London’s blue-chip index climbed above the psychologically important 8,000 mark and stayed there. It had managed to briefly scale that peak a year earlier but quickly fell back, so watching the FTSE 100 creep closer and closer to 9,000 feels a little surreal,” says AJ Bell head of financial analysis Danni Hewson. She adds: “London based mining stocks have surged today, helping to bolster an index which has been on the front foot for most of the year, if you excuse its post Liberation Day rout. Investors have had a chance to digest Donald Trump’s copper tariffs and the surge in prices has certainly created opportunities, at least in the short term. “It’s going to take years for the US to increase its copper mining and smelting capacity, and considering how vital it is in manufacturing EVs and mobile phones, not to mention its importance in the power grid, US demand is unlikely to fall back in any measurable way. That means copper importers are stuck between a rock and a hard place, and it will be the US consumer who will ultimately pay the price. “But the current price surge reflects shifting policy. The sector had been anticipating tariffs on copper – even if they have come in much higher than expected – and stockpiles have been built up, so the price premium is expected to fall back in the near term. “What is unknown is where prices will settle once they’ve had a bit of time to bed in, and how that will affect global trade, especially if economic growth slows across the world as it’s predicted to because of all the uncertainty. “Generally, investors seem to have been rather dismissive of Donald Trump’s latest tariff tangos, believing that ultimately the US president will back off if negotiations don’t go his way. The crunch point is likely to be if a US-EU deal can’t get over the line, but even then the assumption seems to be that the new deadline, just like the last, is soft.” And on that note, goodnight! GW JPMorgan Chase CEO Jamie Dimon has warned that markets are complacent, in the wake of U.S. President Donald Trump’s tariff announcements, Reuters reports. Dimon told an event at Ireland’s foreign ministry: “Unfortunately I think there is complacency in markets” Although shares in London have had a strong day, the pound has been weakening. Sterling has slipped by a third of a cent today to $1.355, with the US dollar strengthening a little following the drop in jobless claims reported today. Back in the UK, Mulberry has raised £20m from its key shareholders, Challice and Frasers Group, to boost growth amid falling sales and widening losses at the British luxury handbag maker. The group said it would also raise up to £1.2m from other shareholders after it revealed sales fell 21% to £120.4m in the year to the end of March while underlying losses widened to almost £24m from just under £23m a year before. It said the new funds would enable it to make “targeted investments to accelerate its future growth and meet its stated medium term financial targets.” The latest fundraising comes less than a year after Mulberry raise £10.35m, before expenses to strengthen its balance sheet and provide “financial flexibility” amid a slowdown in the global luxury market. The group also slashed a quarter of staff at its headquarters in Somerset late last year after rejecting an £111m bid from Frasers, Sports Direct founder Mike Ashley’s retail business. Challice, a group controlled by the Singaporean entrepreneur Christina Ong and her husband, was quick to rebuff the proposal, saying it had no interest in selling its shares. Challice’s 56% stake means it can block any deal. The New York stock market isn’t matching the sizzling performance in London today. The S&amp;amp;P 500 share index has dipped by 2.5 points, or -0.04%, to 6,260 points in early trading. Airline stocks are rising, led by Delta Air (+11%) which told investors today that demand trends have “stabilised”. Just in: US job losses remain low, new data shows, despite trade war uncertainty. The number of Americans filing new claims for unemployment support fell by 5,000 last week, to 227,000, the Department of Labor has reported. Following the four arrests, an M&amp;amp;S spokesperson says: “We welcome this development and thank the NCA for its diligent work on this incident.” Four young people have been arrested for their suspected involvement in the damaging cyber-attacks against Marks &amp;amp; Spencer, the Co-op and Harrods, PA Media reports. The National Crime Agency (NCA) said the individuals were arrested early on Thursday morning on suspicion of blackmail, money laundering, offences linked to the Computer Misuse Act and participating in the activities of an organised crime group. The arrests included a 17-year-old British man from the West Midlands, 19-year-old Latvian man from the West Midlands, 19-year-old British man from London and 20-year-old British woman from Staffordshire. All four were arrested from their home addresses and remain in custody. It comes after investigations by NCA into attacks against the three retailers, where hackers sought ransom payments after breaking into their IT systems. Paul Foster, head of the NCA’s National Cyber Crime Unit, said: “Since these attacks took place, specialist NCA cybercrime investigators have been working at pace and the investigation remains one of the agency’s highest priorities. “Today’s arrests are a significant step in that investigation but our work continues, alongside partners in the UK and overseas, to ensure those responsible are identified and brought to justice.” Earlier this week, the chair of Marks &amp;amp; Spencer claimed two hacks involving “large British companies” had gone unreported in recent months. M&amp;amp;S’s cyber-attack is expected to knock around £300m hit to profits, as its online ordering system was offline for around six weeks. Back in the energy sector, a former boss of Virgin Money has been lined up to chair Britain’s fourth-biggest home energy supplier. Sky News are reporting that Dame Jayne-Anne Gadhia will become independent chair of Ovo as part of a boardroom shake-up at its parent company, succeeding Justin King, the former J Sainsbury chief. Gadhia’s appointment comes as Ovo holds merger talks with Scottish Power, one of its largest rivals. The EU and the US are no closer to announcing a deal after a phone call between EU trade commissioner Maros Sefcovic and the US trade representative Jamieson Greer, my colleague Lisa O’Carroll in Brussels writes. The agreement in principle is expected to be a three page document outlining headline reductions in tariffs for cars, medical devices and possibly steel, in exchange for a baseline 10% import duty on all imports from the bloc and some simplification of paperwork on food imports. Sources say the agreement is just waiting for Trump’s sign off and that did not happen last night so the call with Greer could never have delivered the deal. It could yet come later today but the EU is blind on Trump’s announcement intentions. The European Commission has the power to accept the deal as it is not legally binding as it is an agreement in principle, meaning there is no need for the type of showbusiness moment granted to UK prime minister Keir Starmer when he took a call from Trump while visiting Jaguar Land Rover’s factory in England. The FTSE 100 is now up more than 1% at a new record high, up 106 points or +1.1% at 8973 points. Victoria E Scholar, head of investment at interactive investor, says: UK indices, from large cap to small are catching a bid alongside European bourses like the CAC 40 and the DAX, which also at an all-time high. Positive sentiment from a strong session on Wall Street with the Nasdaq closing higher by nearly 1% has carried forward to this morning’s European session. Leading the gains on the UK blue chip index are the miners with Anglo American up over 5%, closely followed by Glencore and Rio Tinto. Commodities are fuelling the gains for the FTSE 100 with copper in the green and gold catching a bid on the back of a weaker US dollar. WPP is also helping drive the index higher as investors cheer the appointment of its new tech-savvy CEO. Optimism over the chances of a US-EU trade deal are also cheering markets, reports Susannah Streeter, head of money and markets at Hargreaves Lansdown: ‘’The Footsie is footloose, shrugging off trade worries to dance to an all-time high. Even a fresh volley of tariff letters from President Trump has failed to knock investors sentiment. The President’s latest moves are seen as posturing, and there is high expectation that there will be plenty of negotiations to head off higher duties in the weeks ahead. Indications that the EU is edging closer to a deal with the US, with an agreement thought to be possible in a few days, has added to the positive vibes. So, hopes are riding high that the effects on global growth won’t be as onerous as feared. Less encouragingly, almost 9% of European companies are in financial distress, according to the bi-annual Alvarez &amp;amp; Marsal Distress Alert. The survey also found that 32% of European companies (more than 2,500 corporates) have “fragile balance” sheets, the highest level since 2021, due to high interest rates and the struggle to generate enough operating cashflow to service debt. Alvarez &amp;amp; Marsal, the professional services firm, explains: In the UK, levels of corporate distress have fallen to 8.9% from 9.8% the year before, equating to around 250 companies. However, this remains one of the highest percentages among countries analysed. In line with the wider European trend, the proportion of UK companies lacking balance sheet robustness has been steadily growing over the last four years, now reaching nearly one in three, or around 870 of companies analysed. This demonstrates the impact of higher interest rates and slower economic growth on companies’ ability to service their debt. Elsewhere, Germany continues to be the most distressed market, at 11.5%, the highest level since the pandemic. The country has experienced minimal growth in recent years and is more exposed to struggling sectors like the automotive and chemicals industries. France recorded the sharpest increase in distress levels in 2024, to 10.5% from 8.1% the year before, driven by sluggish economic growth and political and fiscal challenges. Kathleen Brooks, research director at XTB, points out that most markets are rallying today, saying: Risk sentiment is buoyant on Thursday, with the exception of Brazilian markets, Europe’s main stocks indices are higher, the dollar is lower, and bond markets are clam, with UK Gilts outperforming. The FTSE 100 reached a fresh record high and is now up more than 16% since April’s low. US stock index futures are down slightly on Thursday but have picked up from their lows as risk sentiment gathers momentum. The FTSE 100 is being led higher by miners, and the materials sector is higher by more than 3% on Thursday. Healthcare stocks are also strong across Europe. This may sound counterintuitive, President Trump has just announced tariffs on copper, and is threatening a 200% levy on pharma imports, so why are these sectors rallying? The reason is that there has been very little concrete details about how tariffs will be applied, which is why we are seeing these sectors steal the spotlight: investors expect Trump to back-track. Thus, after heavy declines for Brazilian stocks on Wednesday they may also recover later today. The stock market is not the real economy, of course. Out in the real world, more people are facing a cost of living squeeze. New data from the Office for National Statistics shows that in June, 26% of adults reported that they would be unable to afford an unexpected, but necessary expense of £850. That’s the highest proportion reported since September 2024. The UK stock market is continues to flex its muscles and show strength, says Dan Coatsworth, investment analyst at AJ Bell, pushing the FTSE 100 to its record highs. Investors lapped up shares in the mining, oil and pharmaceutical sectors, showing a risk-on mood. “European markets in general continue to shrug off Donald Trump’s daily tariff updates, perhaps seeing them as noise and not facts. Trump is throwing out numbers left, right and centre, and investors have begun to dismiss anything that isn’t set in stone. “So many of Trump’s decisions have either been rolled back, forgotten about, or kicked down the road. For investors, that means a shift in focus back to economic data and corporate news flow as key drivers for markets. Rising stock markets can encourage the US administration to do ‘dumb stuff’, warns Dario Perkins, economist at City consultancy TS Lombard. Stock markets might be jolted out of their trade war complacency when the damage starts showing up in economic data. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, says: Newswires remain hectic. It’s all tariffs, tension, and chaos — but markets have an extraordinary capacity to adapt. Trade developments are quickly becoming the new normal; they no longer hammer sentiment the way they once did. What could jolt markets is when all this starts showing up in the data — through slower growth or higher inflation. Until then, the music plays on. The current stock market rally is somewhat surprising, given the uncertainty gripping the global economy. You might remember that shares tanked in early April after Donald Trump announced sweeping tariffs on US trading partners, only to start recovering once they were delayed for 90 days. That deadline has now been kicked on to 1 August, a deadline which the president insists won’t slip again (watch this space…), as it reimposes high tariffs on a swathe of countries. And yet, shares keep rising. Mohit Kumar of investment bank Jefferies says Trump’s announcements of additional tariffs on some countries was “largely ignored by the markets”. Jefferies’s prediction is that risky assets (such as shares) will “grind higher”. Kumar explains: Our view remains that tariffs do cause volatility and uncertainty but should not have much of a market impact medium term. We see eventual tariffs ending between 10-15% on average. While a negative from a macro perspective, the world can live with 10-15% tariffs. We also remain of the view that tariff revenue will be used to justify the extension of tax cuts. The negative impact from a tariff perspective, would be balanced to some extent by tax cuts. Germany’s major stock index has also hit a record high this morning! The DAX, which tracks the 40 largest companies listed in Frankfurt, is up 0.3% at 24,619 points. The DAX has rallied by a blistering 23% so far this year, lifted by Berlin’s plans to boost government spending on areas such as defence. The ‘Footsie’ is continuing to hit new highs this morning! It’s now up almost 1% at 8952 points, up 85 points today. Miners such as Anglo American (+4.6%), Glencore (+3.5%) and Antofagasta (+2.8%) are driving it higher. Boardroom news: Advertising giant WPP has turned to Microsoft executive Cindy Rose to lead its turnaround. WPP, which disappointed the City with a profit warning yesterday, says Rose will succeed outgoing chief executive Mark Read on 1 September. She is currently MS’s chief operating officer for Global Enterprise. Shares in WPP have risen 2.5% as investors welcome Rose’s appointment, helping to push the FTSE 100 to a record high this morning. WPP, which is under pressure from AI-generated campaigns, is touting Rose’s artificial intelligence nous. She’s also sat on the WPP board as a non-executive director since 2019. Philip Jansen, chair of WPP, says: “Cindy is an outstanding and inspirational business leader with extensive experience at some of the world’s most recognised companies and a track record of growing large-scale businesses. She has led multi-billion-dollar operations across the UK, EMEA and globally, built enduring client relationships and delivered growth in both enterprise and consumer environments. “Cindy has supported the digital transformation of large enterprises around the world - including embracing AI to create new customer experiences, business models and revenue streams. Her expertise in this landscape will be hugely valuable to WPP as the industry navigates fundamental changes and macroeconomic uncertainty. Cindy’s appointment follows a thorough selection process that considered both internal and external candidates. As an existing Board member she understands our business and the needs of our clients, and we look forward to working with her in her new role as CEO. Newsflash: Britain’s blue-chip stock index has hit a new alltime high, as investors shrug off the threat of Donald Trump’s trade wars. Update: The FTSE 100 index has risen by as much as 80 points, or 0.9%, to a fresh record peak of 8947.84 points, over the previous record of 8908.82 set in March. Mining stocks are leading the rally today, signalling that traders are not worried that Trump’s blizzard of tariffs will cause a global recession, despite new tariffs such as the 50% imposed on US copper imports and on imports from Brazil. Chris Beauchamp, chief market analyst at IG, says investors are in an “ebullient summer mood”, adding: Perhaps most notable is the market’s apparent indifference to escalating trade tensions. Trump’s 50 percent tariff on copper imports and threats toward Brazil triggered little reaction. Many now view such announcements as political posturing, summed up by TACO: Trump Always Chickens Out. So far this year, the FTSE 100 index has surged by over 9%. It has benefitted from a range of factors this year, including the rotation out of US assets as investors have feared that Donald Trump’s trade war would hurt America’s economy. Relief that the UK struck an early trade deal with the US has also helped make the London market attractive. Precious metals producer Fresnillo has been the top-performing FTSE 100 stock so far this year; it has more than doubled (+140% since 1 January), as the prices of both gold and silver have risen. British defence companies Babcock (+117% year-to-date)and BAE Systems (+63% ytd) have also both risen sharply this year, helped by expectations of a surge in defence spending as the Russia-Ukraine war has continued. Engineering firm Rolls-Royce (+73% ytd) has also had a strong 2025. From post to energy…. and the UK government has confirmed it will not introduce “zonal pricing”, under which southern electricity users would have been charged more than those in Scotland. The government says it has decided to retain a single national wholesale price (as the Guardian reported earlier this week) and also reform the existing national pricing system rather than split the country into different zones. Energy Secretary Ed Miliband said: “Building clean power at pace and scale is the only way to get Britain off the rollercoaster of fossil fuel markets and protect families and businesses for good. “As we embark on this new era of clean electricity, a reformed system of national pricing is the best way to deliver an electricity system that is fairer, more affordable, and more secure, at less risk to vital investment in clean energy than other alternatives. “Our package of reforms will protect consumers and secure investment as we drive to deliver our clean power mission through our Plan for Change.” Zonal pricing has split the energy industry – advocates argued it would encourage heavy energy users to relocate to areas where power is generated, cutting billions of pound off the cost of renewing and updating the electricity grid. Critics, though, said it would create a ‘postcode lottery’ for energy prices. Royal Mail has welcomed Ofcom’s decision to relax the universal service obligation (perhaps unsurprising, at it could save the company £425m!). Martin Seidenberg, group chief executive officer at International Distribution Services, says: “It is good news for customers across the UK as it supports the delivery of a reliable, efficient and financially sustainable Universal Service. “It follows extensive consultation with thousands of people and businesses to ensure that the postal service better reflects their needs and the realities of how customers send and receive mail today.” Ofcom needs to hold Royal Mail to account to improve postal deliveries, says Tom MacInnes, director of policy at Citizens Advice. MacInnes explains: “Royal Mail has a woeful track record of failing to meet delivery targets, all the while ramping up postage costs. Today, Ofcom missed a major opportunity to bring about meaningful change. “Pushing ahead with plans to slash services and relax delivery targets in the name of savings won’t automatically make letter deliveries more reliable or improve standards. “While Ofcom says it recognises the importance of affordability and reliability for consumers, we need to see those words backed by action, forcing Royal Mail to do what it should’ve been doing all along - giving paying customers a service that delivers.” Ofcom has also launched a review of pricing and affordability of the postal service. This will look at concerns over stamp prices, which have been steadily climbing. Natalie Black, Ofcom’s Group Director for Networks and Communications, explains: “As part of this process, we’ve been listening to concerns about increases in stamp prices. So we’ve launched a review of affordability and plan to publicly consult on this next year.” Back in April, Royal Mail increased the cost of first- and second-class stamps for the sixth time in just over three years. That raised the price of a first-class stamp by 5p, or 3%, to £1.70. The cost of the second-class service rose by 2p, or 2.4%, to 87p. This graphic shows how the changes to second-class letter post will affect deliveries across the UK: Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Britain’s postal operator is being relieved of the obligation to deliver second-class letters six days a week, as part of reforms to the service that will also relax its delivery targets. Regulator Ofcom has announced that from 28 July, it will allow Royal Mail to deliver Second Class letters on alternate weekdays, but no longer on Saturdays – but still within three working days of collection. Ofcom says it is making the change to allow the UK’s universal postal service – guaranteeing delivery to anywhere in the country at a fixed price - “to survive”. It points out that, since 2011, Royal Mail has been required under the universal service obligation to deliver First and Second Class letters six days a week. But the number of letters sent each year has more than halved over that time. Natalie Black, Ofcom’s Group Director for Networks and Communications, said: “These changes are in the best interests of consumers and businesses, as urgent reform of the postal service is necessary to give it the best chance of survival. “But changing Royal Mail’s obligations alone won’t guarantee a better service – the company now has to play its part and implement this effectively. We’ll be making sure Royal Mail is clear with its customers about what’s happening, and passes the benefits of these changes on to them. Royal Mail is now owned by Czech billionaire Daniel Křetínský, who took over its parent company International Distribution Services (IDS) last December. Ofcom estimates that changing second-class delivery days could create annual net cost savings of between £250m and £425m, allowing Royal Mail to “invest more in improving its delivery performance.” It will still be required to deliver First Class letters the next working day, Monday to Saturday, and there will continue to be a cap on the price of a Second Class stamp. In another fillip for Royal Mail, though, Ofcom is making its delivery targets less demanding. It will now only have to deliver 90% of First Class mail on the next day, down from 93%. The Second Class mail target is being weakened too, from 98.5% to 95% of letters delivered within three days. Removing Saturday from the roster of delivery days means some letters will take longer to arrive. Ofcom inists these new targets are high by international standards, pointing out that Germany’s three-day target is 95%, Spain’s is 93%, and Norway’s and Poland’s are 85%. The old targets have certainly proved tricky for Royal Mail – it has been repeatedly fined for missing them, with almost a quarter of first-class mail arriving late in the year to March. The agenda 8am BST: ECB board member Piero Cipollone lecture on the digital euro 1.30pm BST: US weekly jobless claims</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>The blue-chip share index has closed up 108.64 points, or 1.23%, at a new end-of-day peak of 8975.66 points. Earlier in the session, the Footsie pushed its new intraday high record even higher, to 8979 points. Mining stocks led the rally, with Glencore (+39%), Rio Tinto (+3.9%) and Anglo American (+ 3.7%) at the top of the list of risers.</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Time to recap: The Bank of England has rolled out looser mortgage rules that policymakers hope will help 36,000 more first-time buyers on to the housing ladder each year. New guidelines announced by the UK’s central bank mean that individual banks and building societies can offer more high loan-to-income (LTI) mortgages, which are equal to, or worth more than, 4.5 times a borrower’s annual earnings. While high LTI loans are usually considered more risky, the Bank said most banks were not taking advantage of their individual caps, meaning there were fewer available to borrowers than hoped. Sam Woods, the chief executive of the Bank’s regulatory arm, the Prudential Regulation Authority, said the changes should benefit tens of thousands of first-time buyers. In its latest financial stability report, the Bank also warned that US tariffs will hurt global growth, while governor Andrew Bailey suggested the recent increase in UK borrowing costs was part of a wider rise in bond yields. Nvidia has become the first company to ever hit $4 trillion in market value, solidifying its position as one of Wall Street’s most-favored stocks to tap in the ongoing surge in demand for artificial intelligence technologies. The CEO of X, Elon Musk’s social network, has announced she would step down after two years in the role. The maker of London’s black cabs has said it will cut 180 jobs at its factory in Coventry, blaming a declining UK market for taxis. Copper prices hit a record high in the US after Donald Trump announced he would impose a 50% tariff on the industrial metal, in the latest escalation of his trade war. Donald Trump has said there would be more trade-related announcements today… our US politics blog is tracking the latest developments: The maker of London’s black cabs has said it will cut 180 jobs at its factory in Coventry, blaming a declining UK market for taxis. The London EV Company, owned by Chinese car conglomerate Geely, said that the number of cabbies is falling across the capital and the rest of the UK, denting demand for its hybrid electric cars, which combine a battery with a smaller petrol engine. London’s black cabs are tightly regulated by Transport for London, with requirements such as a turning circle tight enough for the small roundabout outside the Savoy hotel. Since 2018 only “zero-emissions capable” vehicles have been eligible for first-time licences. However, that market has been largely satisfied, with over 60% of the capital’s taxi fleet made up of electrified LEVC TX models, with around 9,000 operating within the city. LEVC’s efforts to sell more cabs outside of London, and to sell van versions of the car, have not resulted in a large pick-up in sales, in part because of stiff competition. Some people close to Geely have suggested the company, which also owns the struggling Lotus sportscar brand in the UK, might consider basing a new pure electric taxi on vehicles made in China, with final assembly carried out in the UK. Government statistics show that the number of taxi-only driver licences fell by 7% in 2024 compared with a year earlier. At the same time, the number of private hire vehicle drivers jumped by 14%. LEVC’s vehicles do not tend to be used by many private hire vehicle drivers, such as those who drive for taxi apps Uber and Bolt, and who are thought to make up a large proportion of the overall increase in drivers. Alex Nan, LEVC’s chief executive, said: With the UK taxi market continuing to experience significant challenges, LEVC has reluctantly made the decision to reduce its TX manufacturing output, resulting in a round of compulsory redundancies. LEVC will of course provide full support for its customers as normal and there is no impact on the sales or aftersales of new or used TX. LEVC firmly believes in the future of the UK taxi industry and we remain committed to our vision of being a leading provider of green mobility solutions. Despite the temporary challenges the taxi sector is facing, we are dedicated to safeguarding the iconic London black cab and are actively discussing with regulators the requirements to support the development of an all-new TX. Newsflash: Linda Yaccarino, the CEO of Elon Musk’s social media platform X, has announced she’s stepping down. Yaccarino, previously an advertising executive, was appointed two years ago after Musk bought, and then rebranded, Twitter. During her tenure, some advertisers boycotted X due to concerns about extreme content running on the site. Posting on X, she says: After two incredible years, I’ve decided to step down as CEO of 𝕏. When @elonmusk and I first spoke of his vision for X, I knew it would be the opportunity of a lifetime to carry out the extraordinary mission of this company. I’m immensely grateful to him for entrusting me with the responsibility of protecting free speech, turning the company around, and transforming X into the Everything App. I’m incredibly proud of the X team - the historic business turn around we have accomplished together has been nothing short of remarkable. We started with the critical early work necessary to prioritize the safety of our users—especially children, and to restore advertiser confidence. This team has worked relentlessly from groundbreaking innovations like Community Notes, and, soon, X Money to bringing the most iconic voices and content to the platform. Now, the best is yet to come as X enters a new chapter with @xai. X is truly a digital town square for all voices and the world’s most powerful culture signal. We couldn’t have achieved that without the support of our users, business partners, and the most innovative team in the world. I’ll be cheering you all on as you continue to change the world. As always, I’ll see you on 𝕏 Wall Street has opened higher, as the Trump trade war fails to alarm investors. The S&amp;amp;P 500 index is up 0.6%, gaining 37 points to reach 6,263 points. The tech-focused Nasdaq has gained 201 points, or almost 1%, to 20,619 points. Another day, another plea from Donald Trump for lower interest rates. Posting on his Truth Social platform, the US president claims that US interest rates should be at least three percentage points lower, claiming there is “no inflation”. He also labels Fed chair Jerome Powell as “Too Late” again, writing: Our Fed Rate is AT LEAST 3 Points too high. “Too Late” is costing the U.S. 360 Billion Dollars a Point, PER YEAR, in refinancing costs. No Inflation, COMPANIES POURING INTO AMERICA. “The hottest Country in the World!” LOWER THE RATE!!! Fact check: The annual rate of US inflation was 2.4% in May, above the Fed’s 2% target, with prices rising by 0.1% on a monthly basis. The Fed’s current target rate is 4.25%-4.5%. Trump is suggesting that this should be 1.25%-1.5%, which would be the lowest since early 2022, before the Ukraine war drove up inflation. Ironically, Trump’s decision to shift the deadline for trade deals to 1 August makes it harder for the Fed to justify a rate cut this month, as it creates more uncertainty. Newsflash: chipmaker Nvidia has become the first listed company to be worth $4tn. Nvidia has hit this peak at the start of Wall Street trading, pushed up by continued investor excitement about artificial intelligence. Nvidia’s shares, which are up 2.7% in early trading, have gained 22% so far this year as the tech sector has largely shrugged off concerns about Donald Trump’s trade wars. Nvidia semiconductors, such as its “Blackwell” chip, have been in heavy demand as artificial intelligence companies have scrambled to build high-powered systems to train their AI models on. Last month, Nvidia’s CEO Jenson Huang cheered investors at the company’s annual shareholders meeting, telling them: “We have many growth opportunities across our company, with AI and robotics the two largest, representing a multitrillion-dollar growth opportunity.” The Bank of England has fined payment systems firm Vocalink Limited £11.9m for failing to operate adequate risk management and governance arrangement. Vocalink, which is owned by US payment processor Mastercard, designs, builds and operates bank account-based payment systems in Britain. Sarah Breeden, deputy governor for Financial Stability, says: “Vocalink fell short of its obligation to have adequate risk management and governance arrangements when responding to the Bank’s Direction. Its failure to comply with that Direction in full has resulted in a significant fine.” The Bank’s investigation identified the root cause of Vocalink’s non-compliance was the failure to have in place a sufficiently integrated risk management framework for the remediation programme. This would have ensured that risks facing the programme could be properly understood, monitored and shared amongst the three lines of defence (and external assurance providers). It also found there were failures to escalate key risks and information to senior committees, which undermined the firm’s ability to fully comply with the Direction. The Bank considers Vocalink’s governance arrangements fell below the standards expected of a financial market infrastructure firm. Daimler Truck Holding expects US orders to remain at “extremely” low levels until uncertainty over President Donald Trump’s trade policies subsides and freight volumes begin to recover. Chief financial officer Eva Scherer said logistics companies have cut back on truck purchases amid a drop in shipments of tariff-hit goods such as steel and aluminum. Scherer told Bloomberg: “We’re in a situation where it’s very difficult to predict from a CFO perspective. Scenario planning is more important than ever.” Over in the US, the Trump immigration crackdown is hitting the labour supply, reports Paul Ashworth, chief North America economist at Capital Economics. He writes: After stemming the inflow of unauthorised immigration over the Southwest border, the Trump administration now appears to be gradually ramping up the number of detentions and removals. This crackdown is beginning to have a more marked impact on labour supply, with the foreign-born labour force shrinking by more than one million people in the last four months. Despite all the trade war uncertainty, the UK stock market is rising towards its highest ever levels. The FTSE 100 is up 14 points (+0.16%) so far today at 8868 points, only around 16 points shy of its all-time closing high of 8,884 points set last month. Lenders can apply for a waiver from today to increase the amount of high loan-to-income mortgages they issue, says BoE deputy governor Sam Woods. Woods insists that today’s changes (outlined here) are ‘more than a tweak’. The Bank estimates that the unused capacity of high LTI mortgages that are not being issued at the moment is equivalent to “another 36,000 high LTI first-time buyer mortgages per year in the UK”. There are other constraits on first-time buyers, such as the need for a deposit (see here), Woods adds. He also predicts that the Bank may need to ‘put the brakes on’, if there is a surge in high LTI lending that takes the industry total up to the overall 15% of loans limit. BoE governor Andrew Bailey then calls for reforms to the UK pension system, but opposes the suggestion that funds should be forced to buy UK assets. Q: what’s your view on the possibility that the government will mandate how much invest pension funds should invest in UK assets? Bailey replies that the UK only has a low level of pension fund investment in “the real economy in this country”, and that structural changes to the pension fund industry (consolidating funds) would be helpful. However, he says: I do not support mandating. I don’t think that’s appropriate. He adds that the current government is taking the same approach as its predecessor on this issue, adding I think reforming the pension system does, to be honest, require a lot of heavy lifting, but it needs to be done. It will take a bit of time, but it needs to be done for these structural reasons. I don’t support mandating, but I do hope that we can reach a point where there is a natural ability to tackle this problem. Earlier this year, chancellor Rachel Reeves said she would create a “backstop” power to force large pension funds to back British assets, if necessary, to drive up investment. Q: Will a global trade war lead to UK job losses? BoE governor Bailey replies that there’s been a big increase in uncertainty around trade and tariffs, pointing out: Fragmenting the world economy is bad for activity in the world economy. That’s fairly simple trade theory. That fragmentation is bad for economic activity, and is therefore bad for employment, he adds: “Obviously, in that sense, there is a consequence. So we have to watch that very carefully.” Bailey adds that it was a “very good thing” that the UK government was first to negotiate a trade agreement with the US. Q: Your report warns that a weak IPO market is resulting in fewer exit opportunities for private equity backed firms. How concerned are you about the lack of buoyant public markets, including in London? (my colleague Kalyeena Makortoff asks). BoE governor Andrew Bailey replies that firms are telling the Bank that they are delaying investment decisions due to the higher level of uncertainty in the world economy. That can include decisiont on whether to raise capital, and in which market to raise it. Bailey adds: It’s not surprising, because economics and economic theory tells us this, that since investment decisions are typically irreversible. Once you take them, once you start them, you’ve got to go on, as it were. You usually can’t turn back. Then if uncertainty increases, then the option value of delaying goes up. And so you do see delayed investment, and I think we are seeing that at the moment. Q: What does the bond market reaction to the chancellor’s tears (last week) say about the fragility of the bond market? Andrew Bailey replies that there have been “broadly similar” movements in global government bond markets. Bailey says: We’ve seen steepening of yield curves globally. So I think it’s important to start in that context. There’s nothing, I would say, particularly UK focused about that. That steepening pattern is a global trend which the UK market has been part of. Bailey points out that the rise in UK bond yields last week did reverse (they fell back after Keir Starmer backed chancellor Rachel Reeves, easing concerns of a change of chancellor). That, he adds, is further evidence that we are in a period of more volatile markets, and one where there is also “fast reversion”. Andrew Bailey then explains that the BoE is putting its recommendation that lenders should offer more high loan-to-income mortgages into place from today. BoE governor Andrew Bailey then warns that another bout of trade war market turbulence could hurt the UK economy. He reminds reporters in London about the market slump in early April after Donald Trump announced new tariffs, in which risky asset prices fell and the US dollar weakened. Bailey says core government bond markets remained orderly during this stressful period, but warns that conditions might have become more strained if the episode of volatility had lasted for longer. Risk sentiment in some markets then recovered after president Trump paused these tariffs, Bailey reminds us – before warning that the risksk of another selloff remain high. He says: There has been a notable change in the usual correlation patterns between the dollar and other US assets, including equities and government bond yields. And given these developments, the risk of sharp falls in risky asset prices, abrupt shifts in asset allocation and a more prolonged breakdown in historical correlations remains high, and vulnerabilities in market based finance could amplify such moves which could impact the availability and cost of credit here in the UK. Bank of England governor Andrew Bailey has warned that the UK is particularly exposed to geopolitical risks, as it is an open economy with a large financial sector. Briefing journalists in London about today’s financial stability report, he says: Risks and uncertainty associated with geopolitical tensions, global fragmentation of trade and financial markets and pressures on sovereign debt markets are still elevated. Some geopolitical risks have crystallized and material uncertainty around the global macroeconomic outlook persists. The Bank of England is also warning that over three and half million mortgage holders are on track to pay higher payments by 2028. That’s because around 30% of mortgage holders have not yet refixed their mortage deals since interest rates started to rise at the end of 2021. This means the full impact of higher interest rates has not yet passed through to all mortgagors, the Bank says. However, another 2.5 mortgage holders can look forward to a drop in payments. That’s because rates peaked at 5.25% in August 2023 and were held for 12 months, followed by four quarter-point cuts over the last year. Donald Trump’s trade war has created uncertainty that will hurt growth in the global economy, the Bank of England warns. It’s new Financial Stability Report (FRS) also singles out the Middle East crisis as a factor making it hard to forecast inflation. The BoE says: Since the November FSR, the US announced increased tariffs, and in response some other jurisdictions announced changes to their own trade policies. Negotiations between the US and China led to a partial reversal of tariff increases in May, with further agreement subsequently reached, and a trade deal has been agreed between the US and the UK. There remains, however, considerable unpredictability about the near-term evolution of global trade policies with negotiations continuing between the US and a number of its trading partners. These developments are expected to weigh on world growth, driven both by the direct impact of higher tariff barriers and by the dampening effect of trade policy uncertainty on firms’ investment decisions. There is a high degree of economic uncertainty around the outlook, and there are downside risks to global growth in the near term, for example in the event of significant global supply chain disruption or further escalation of conflict in the Middle East leading to higher energy prices. These factors also contribute to uncertainty around the future path of inflation. The Bank of England’s financial policy committee also points out that accumulating a sufficient deposit continues to be the main barrier to owning a home. Its new financial stability report, just released, shows that almost 80% of prospective first-time buyers (FTB) do not have sufficient savings to cover a 5% deposit on a median-priced property typically purchased by an FTB in their area. Another 6% are restrained by lenders’ affordability assessments, and loan to income (LTI) ratio caps. A further 1% would not meet other requirements lenders set to manage their high-LTI lending (such as rules around minimum salary), leaving just 15% of prospective first-time buyers who can actually (potentially) buy a typical appropriate property in their area! Newsflash: The Bank of England is recommending that lending rules are relaxed so that banks and building societies can issue more mortgages at high loan-to-income levels. The BoE’s Financial Policy Committee is recommending that individual lenders should be allowed to increase their share of lending at high LTIs to above the current limit of 15%. This could make it easier for borrowers to stretch themselves to afford a more expensive property. High loan-to-income loans are defined as those at a ratio above 4.5. Loans above this level are riskier, as borrowers could struggle to meet mortgage payments if their incomes fell, or if interest rates rose. Announcing the plan, the FPC says: The Committee noted its role in supporting the Government’s priority to make home ownership more accessible and discussed the UK housing market and the role of regulatory mortgage policies. It wants the overall lending market to restrict high LTI loans to 15% of total demand, while allowing individual lenders to exceed it. The loan-to-income lending limit was introduced in 2014, as part of a package to cool the housing market. The FPC says: The Committee noted that the original policy intent of the LTI flow limit recommendation was to ensure the flow of new residential mortgages at high LTIs did not exceed 15% of total new mortgages in aggregate. The FPC judged that the aggregate 15 per cent limit continued to strike the right balance between providing appropriate protection from the increased risk to economic growth of large cuts to consumption associated with an over-indebted household sector, while providing sufficient capacity for otherwise creditworthy households to borrow at higher LTIs. As such, it has recommended the Prudential Regulation Authority (PRA) and the FCA amend implementation of its LTI flow limit to allow individual lenders to increase their share of lending at high LTIs while aiming to ensure the aggregate flow remained consistent with the limit of 15%. Here’s our news story about the jump in the US copper price: The oil price has hit its highest level in two weeks, after a cargo ship attacked in the Red Sea sank. The Eternity C cargo ship sank in the Red Sea following an attack on Monday, blamed on Yemen-Houthi militants, which killed at least four crew members. Brent crude has risen by 0.6% today to $70.71 per barrel, the highest since 23 June. Tom Bailey, head of research at HANetf, has warned that the threat of copper tariffs is leading to more of the metal becoming ‘trapped’ in warehouses, rather than being used. Bailey explains that this could distort prices for this vital metal: Copper sits at the centre of a looming supply-demand crunch. On one side is surging demand driven by grid upgrades, the rapid buildout of AI data centres, and the ongoing urbanisation of emerging markets. On the other is a supply base that is ageing, expensive, and increasingly unreliable. Ore grades are declining, discoveries are rare, and new mines take over a decade to come online. “However, tariffs mean that a new dynamic is potentially emerging: trapped copper. With tariffs looming, US buyers have rushed to bring in copper ahead of schedule. But much of this metal is not being consumed. Instead, it is sitting in warehouses or locked in financing agreements. Due to high US premiums, it is uneconomical to export. In practice, this copper is being stranded inside the US, unavailable to the rest of the world. The result could be distorted physical markets, with those outside the US forced to compete for a shrinking pool of freely available copper. German chancellor Friedrich Merz is optimistic that the European Union can agree a trade deal with the United States by the end of this month at the latest. Merz told lawmakers on Wednesday: “Our goal is to reach a trade agreement with the United States of America as quickly as possible that links mutual trade between America and the European Union with the lowest possible customs duties.” Merz added that he is in close contact with US president Donald Trump and the European Commission. Shares in some European pharma companies have dropped this morningn, after Donald Trump threatened to implement up to 200% tariffs on imported pharmaceuticals. The falls are modest, though, after Trump also said he would give drugmakers about one year “to get their act together”. In London, AstraZeneca’s shares have dipped by 0.77%. Switzerland’s Novartis has lost 0.8%, while Belgium’s UCB has dropped by 1.75%. Dan Coatsworth, investment analyst at AJ Bell, says: “The pressure is now on for drug companies to expand US production facilities so they are effectively on the doorstep of American customers. Boosting the manufacturing sector and creating more jobs is central to Trump’s tariff strategy, and the likes of AstraZeneca already have plans in motion to expand their US footprint. Carsten Menke, Head of Next Generation Research at Julius Baer, says the copper tariffs will be inflationary domestically in the US and deflationary internationally – which matches the price action we’ve seen since last night. Menke also points out that the jump in US copper prices (13% yesterday) is less than the 50% tariff, implying traders expect some imports will be exempt, saying: President Trump announced the imposition of 50% import tariffs at a cabinet meeting yesterday. While US-traded futures jumped on the news, the price differential is well below the tariff level, pointing to expectations of exemptions for key suppliers or expectations of different demand dynamics. As already mentioned, we remain of the conviction that the tariffs will be inflationary domestically in the US and deflationary internationally. Generally, we do not see a supply-constrained market, but we want to wait for the dust to settle before reassessing our outlook. Donald Trump’s trade war has helped nudge Malaysia’s central bank into cutting interest rates. The Monetary Policy Committee (MPC) of Bank Negara Malaysia has cut its policy rate by a quarter of one percentage point, to 2.75%, today. Malaysia’s MPC cited “tariff developments” (Trump announced a 30% tariff on imports from Malaysia this week), saying: The latest indicators point towards continued expansion in global growth, supported by sustained consumer spending and to some extent, front-loading activities. The global growth outlook would remain supported by positive labour market conditions, less restrictive monetary policy and fiscal stimulus. This outlook is weighed down by uncertainties surrounding tariff developments, as well as geopolitical tensions. Such uncertainties could also lead to greater volatility in the global financial markets and commodity prices. The European Union is working closely with Donald Trump’s administration to reach a trade deal, but Brussels is getting ready for all scenarios, European Commission President Ursula von der Leyen has told the European Parliament this morning. Von der Leyen said: “We stick to our principles, we defend our interests, we continue to the work in good faith, and we get ready for all scenarios.” Yesterday, Trump said the EU were now being “very nice to us”, and indicated that the US was “probably two days off” from sending Europe a letter on tariffs. In the short term, copper prices are expected to remain volatile as markets adjust to the new tariff landscape, predicts Daniela Sabin Hathorn, senior market analyst at Capital.com, who explains: Factors contributing to this volatility include potential shifts in global supply chains, as exporters may redirect copper shipments to other markets, and the possibility of retaliatory measures from affected countries. Additionally, the U.S.’s limited domestic smelting capacity could influence price dynamics, as the country currently imports about half of its copper needs. Ultimately, the dramatic rally in copper was triggered by a policy shift that caught the market off guard. The U.S. government’s move to impose steeper-than-expected tariffs has introduced a new layer of uncertainty into an already sensitive commodities landscape. With President Trump’s trade strategy known for sudden pivots, traders would be wise to stay alert for further developments that could reshape the outlook once again. Shares in advertising giant WPP have slumped by 13%, after it slashed its forecast for revenues and profits this year and blamed a “challenging economic backdrop”. WPP warned that “continued macro uncertainty” was weighing on client spend and leading to weaker net new business than originally anticipated. The company now expects its like-for-like revenue, excluding fees paid to suppliers, will fall by between 4.2% to 4.5% in the first half of this financial year. Mark Read, chief executive officer of WPP – whose departure was announced a month ago – says June was tougher than expected: “Since the start of the year, we have faced a challenging trading environment with macro pressures intensifying and lower net new business. While we expected the second quarter to be similar to the first quarter, performance in June was worse than anticipated and we expect this pattern of trading in the first half to continue into the second half. “As a result, we are updating our guidance for the full year and reducing our expectations on LFL revenue less pass-through costs growth to -3% to -5% (from flat to -2%) with a year-on-year decline in headline operating profit margin of 50 to 175 bps (vs. around flat previously). Shares in copper producer Antofagasta have dropped by over 3% at the start of trading in London. Other miners are also weakening, with Glencore (-2.2%) and Anglo American (-1.8%) among the FTSE 100 fallers. Analysts at investment bank Jefferies have warned that the new 50% tariff on copper will drive up costs in the US economy, saying: “The US does not have nearly enough mine/smelter/refinery capacity to be self-sufficient in copper. “As a result, import tariffs are likely to lead to continued significant price premiums in the US relative to other regions.” Tony Sycamore, market analyst at IG, questioned whether the Trump administration can easily make the US self-sufficient in copper: The aim of the new copper levy is to encourage domestic copper production, which is a challenging objective given the complexities of relocating a copper mine. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, says the latest trade news from Trump was not reassuring: First, hopes of an extension to the current tariff pause—which ends today—were dashed after Donald Trump threatened that the August 1st deadline will be final, with no further extensions. Second, he slapped a 50% tariff on copper and announced that pharmaceuticals will face 200% tariffs within a year. The news sent COMEX copper futures to a record high, while copper prices on other platforms like India’s MCX dropped, on expectations that surplus supply would shift to alternative markets. Donald Trump is expected to send more letters to countries, informing them of new tariff rates or announcing trade deals, today. Last night on his Truth Social site, the US president wrote: We will be releasing a minimum of 7 Countries having to do with trade, tomorrow morning, with an additional number of Countries being released in the afternoon. Thank you for your attention to this matter! In a separate post, Trump also insisted that his new deadline of 1 August to reach trade deals would not slip, writing: As per letters sent to various countries yesterday, in addition to letters that will be sent today, tomorrow, and for the next short period of time, TARIFFS WILL START BEING PAID ON AUGUST 1, 2025. There has been no change to this date, and there will be no change. In other words, all money will be due and payable starting AUGUST 1, 2025 - No extensions will be granted. Thank you for your attention to this matter! Copper prices outside the US have fallen, following Trump’s threat of a 50% tariff on imports. On the London Metal Exchange, the metal slid as much as 2.4% at the open, before easing to change hands at $9,653 a ton, 1.4% lower, Bloomberg reports. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. There’s turmoil in the copper market after it became the latest frontline in Donald Trump’s trade war The copper price has hit a record high in the US, and fallen in other markets, after Donald Trump announced he would impose a 50% tariff on imported copper. During a cabinet meeting at the White House, Trump revealed “Today, we’re doing copper,” adding: “I believe the tariff on copper, we’re going to make it 50%.” Copper is a critical element in electric vehicles, the power grid, military hardware and many consumer goods. It’s known as “Dr Copper” in the financial markets, because its price is a gauge of the health of the world economy. Investors’ reaction to Trump’s annoucement was swift – copper futures traded in the US jumped by over 10% to $5.682 per pound, closing at an all-time high. That’s the biggest jump on records stretching to 1969, the Financial Times reported. More expensive domestic copper, and a 50% tariff on imports of the metal, will add to inflationary pressures on US businesses and consumers. Trump also said he would soon introduce levies on semiconductors and pharmaceuticals – two shoes which investors have been waiting to drop for months. Pharmaceutical imports are also “going to be tariffed at a very, very high rate”, the president said. “Like 200%.” “We’re going to be announcing pharmaceuticals, chips and various couple of oth</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Bank of England has rolled out looser mortgage rules that policymakers hope will help 36,000 more first-time buyers on to the housing ladder each year. The maker of London’s black cabs has said it will cut 180 jobs at its factory in Coventry, blaming a declining UK market for taxis. Nvidia has become the first company to ever hit $4 trillion in market value.</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Time to wrap up Investors around the globe are gripped by Donald Trump’s trade war, as the deadline for the US to agree deals with trading partners moves closer. The EU has revealed that European Commission president Ursula von der Leyen had a “good exchange” with Donald Trump on Sunday, raising hopes of a deal by Wednesday. Olof Gill, the EU trade spokesperson, said: “We’re fully geared up to get an agreement in principle by Wednesday, and we’re firing on all cylinders to that effect.” The 90-day pause to the tariffs annouced by Trump in early April expires on 9 July, leaving little time for agreements to be reached. Trump posted online that he plans to start announcing deals, and letters announcing new tariffs on countries without a deal, from noon Washington time, or 5pm UK time. Those new tariffs will kick in on 1 August, US commerce secretary Howard Lutnick indicated. Treasury secretary Scott Bessent has hinted that announcements are close, He told CNBC: “We’ve had a lot of people change their tune in terms of negotiations. So my mailbox was full last night with a lot of new offers, a lot of new proposals. So it’s going to be a busy couple of days.” British steelmakers face a nervous wait to discover if they will be hit by US tariffs, after the UK government said it was trying to complete a deal to protect the industry from Donald Trump’s trade war. Stocks have dropped on Wall Street on nervousness over the trade war, while in London the FTSE 100 index has slipped by eight points (-0.1%). Our US Politics blog is tracking the latest trade war developments: British steelmakers are facing a nervous wait to discover if they will be hit by US tariffs, after the UK government said it was trying to complete a deal to protect the industry from Donald Trump’s trade war. The US has set a 50% tariff on foreign steel and aluminium imports. While the UK has brokered a reduced rate of 25% and is trying to bring it down to zero, a deal has not yet been completed. On Monday, Downing Street refused to confirm it was confident it could eliminate US tariffs on UK steel before Trump’s deadline on 9 July. A spokesperson for No 10 said: “Our work with the US continues to get this deal implemented as soon as possible. “That will remove the 25% tariff on UK steel and aluminium, making us the only country in the world to have tariffs removed on these products. “The US agreed to remove tariffs on these products as part of our agreement on 8 May. It reiterated that again at the G7 last month. The discussions continue, and will continue to do so.” Ding Ding! The opening bell of Wall Street has just been rung, and the main US share indices are slightly lower. The Dow Jones industrial average, which tracks 30 large US companies, dipped by 70 points at the open to 44,757, a fall of 0.16%. Traders are digesting Trump’s threat of new tariffs on Brics countries, Scott Bessent’s hints that some trade deals are imminent ahead of the 9 July deadline, and the new three-week delay until new tariffs come in, on 1 August. The broader S&amp;amp;P 500 index dipped by 19.70 points, a 0.3% fall, while the tech-focused Nasdaq is down 0.5%. Treasury secretary Scott Bessent has also hinted that the US will make several trade announcements in the next 48 hours. He told CNBC: “We’ve had a lot of people change their tune in terms of negotiations. So my mailbox was full last night with a lot of new offers, a lot of new proposals. So it’s going to be a busy couple of days.” More here: US treasury secretary Scott Bessent has said that he expected to meet with his Chinese counterpart in the coming weeks, to advance discussions on trade and other issues. Speaking to CNBC, Bessent said: “I’m going to be meeting with my Chinese counterpart at sometime in the next couple of weeks. We had good meetings in Geneva, in London. We both approached it with great respect. “I think there are things for us to do together if the Chinese want to do it, so we will discuss whether we are able to move beyond trade into other areas.” The London meeting, last month, led to a framework deal covering export restrictions on rare earths and semiconductors, building on the truce agreed in Geneva in May. European Commission president Ursula von der Leyen is expected to phone EU leaders today to take soundings on a draft framework deal with the US on tariffs, details of which have not been disclosed. “We’re fully geared up to get an agreement in principle by Wednesday, and we’re firing on all cylinders to that effect,” Olof Gill, the EU trade spokesperson, added. The deal is expected to include an agreement on reducing the current 27.5% tariff on car exports, something Germany badly wants, but also a potential standstill clause on tariffs on sectors including pharma and semi-conductors, while negotiations on a wider deal take place. Chemicals producer Dow has announced plans to shut three upstream plants in Europe, including one in the UK, and cut around 800 jobs. Dow blamed the closures on structural challenges in the region, and said it planned to remove higher-cost, energy-intensive portions of its European portfolio, Reuters reports. Under the plan, a Basics siloxanes plant in Barry, UK is set to close by the middle of 2026. Two plants in Germany – an Ethylene cracker in Böhlen, and a Chlor-alkali &amp;amp; vinyl (CAV) assets in Schkopau – are to close by the fourth quarter of 2027. CEO Jim Fitterling said: “Our industry in Europe continues to face difficult market dynamics, as well as an ongoing challenging cost and demand landscape.” The 800 roles affect are on top of the 1,500 job cuts announced in January, through a $1bn cost-cutting programme. Back in April, the Unite union warned that almost three hundred jobs were at risk at the Basics area of Dow’s plant in Barry, Vale of Glamorgan. The goal posts are shifting again on the trade and tariff issue, reports Brad Bechtel, global head of FX at Jefferies. Bechtel explains: President Trump has indicated countries will have until Aug 1 before new tariffs kick-in as they rush to complete trade deals with countries around the world. July 9 had been the working deadline and the administration is indicating that a slew of deals is in the hopper for this week, but the new quasi-extension was thrown out there this past weekend. Trump also indicated that trade deals will be announced today at 12pm. The EU and Japan are two of the larger deals to be resolved and EU officials claimed they were still working towards the Wednesday deadline to come to a conclusion. Trump indicating he will ‘have a deal or letter with most nations done by July 9’ but will start announcing deals today. He also threw in an extra 10% tariff for anyone ‘aligning’ with BRICS, whatever that means. Bangladesh’s interim government is anticipating a favorable resolution in trade negotiations with the US. “We’ve had at least seven rounds of negotiations, both virtual and in-person, and we expect a positive outcome,” commerce secretary Mahbubur Rahman said in an interview on Monday, Bloomberg reports. Rahman also said the US has hinted at creating two separate trade bands — one for least developed countries or LDCs, a group that includes Bangladesh, and the other for the remaining trading partners. Bangladesh was one of the countries hardest hit by Donald Trump’s trade war announcement of early April; it faced a new tariff of 37% on its imports to the US. European Commission president Ursula von der Leyen and Donald Trump had a “good exchange” on Sunday, raising hopes of a deal by Wednesday, the US president’s self-imposed deadline for trade deals. Olof Gill, the EU trade spokesperson, told reporters during a daily press briefing that: “We want to reach a deal with the U.S. We want to avoid tariffs. We believe they cause pain. We want to achieve win-win outcomes, not lose-lose outcomes”. As covered in our introduction, the Trump administration has said letters would go out from today notifying trading partners who don’t have a deal by 9 July of the higher tariffs that would take effect on August 1. The EU is demanding immediate relief from tariffs on cars, which currently stand at 29.5% and reduction of tariffs in steel, as part of a UK-style framework deal that is being negotiated. Both sides were locked in talks over the weekend after a high level delegation led by trade commission Maros Šefčovič to Washington last week. Among those he met were treasury secretary Scott Bessent who remarked over the weekend that “good progress” had been made with the EU after and initial impasse. Incidentally, our Europe Blog has all the main developments from across the continent: “Time is money” when it comes to tariff negotiations between the European Union and the United States, a German government spokesperson has said. The spokesperson says: “Time is money in the truest sense of the word.” They added that German Chancellor Friedrich Merz had discussed the matter with EU Commission President Ursula von der Leyen and the leaders of France and Italy at the weekend, explaining: “In this respect, we should give ourselves another 24 or 48 hours to come to a decision.” The Kremlin has insisted that the BRICS group of nations had never been working to undermine other countries. Kremlin spokesman Dmitry Peskov said the Kremlin had taken note of Donald Trump’s threat to impose a 10% tariff on those aligning themselves with its “anti-American policies”. Peskov added: “We have indeed seen such statements by President Trump, but it is very important to note here that the uniqueness of a group like BRICS is that it is a group of countries that share common approaches and a common world view on how to cooperate based on their own interests. “And this cooperation within BRICS has never been and will never be directed against any third countries”. The US-Vietnam trade deal announced last week “raises hopes” for agreements with other emerging markets (EMs), says Jon Harrison of City firm TS Lombard. Harrison told clients: The US administration has indicated that deals are close to completion for 10 major trading partners. Most larger and mid-sized EM are among the major trading partners, but are aiming for a tariff of less than the 20% agreed with Vietnam, while few will be prepared to allow the zero tariff access to all US products granted by Vietnam. At the same time, however, most EM have more to offer in terms of delivering investment and jobs to the US as well as being potentially larger markets for US exports. Our base case remains that for most EM there will either be phase one deals, or sufficient progress made to justify a delay in threatened tariffs. There are nonetheless risks to this scenario as the deadline approaches, with lack of progress and potential sticking points in a number of countries, including India, South Korea and Taiwan, meaning that one or more countries could face punitive tariffs, even if only temporarily. South Korea, for example, has asked to delay the deadline, although Trump has previously said that in general there would be no delays The indications that new US tariffs could kick in on 1 August, rather than this week, could bring some relief to markets. But that’s probably countered by Donald Trump’s threat of a new 10% tariff on imports from BRICS-aligned countries. This has left the Stoxx 600 up 0.16% in early trading, with Germany’s DAX index gaining 0.6%. Joshua Mahony, chief market analyst at Rostro, explains: A mixed affair for European equities this morning, with traders weighing up the implications of Donald Trump’s decision to delay the reciprocal tariffs (against) set against the threat of a 10% BRICS tax. Whether it is a case of him chickening out, he clearly does not want to implement the reciprocal tariffs in their original format, and thus what started as April, pushed to July, and now turns to August. There will be many that see this as weakening his hand as nations note his unwillingness to follow through on his threats. Nonetheless, this once again provides markets with a breather, bringing over three-weeks longer until tariffs kick in. After last week’s gyrations, the UK bond market is looking calmer this morning. The prices on UK short and long-term government bonds have risen slightly, which has pulled down yields (the effective interest rate on the debt) a little. The yield on 10-year gilts is hovering around 4.538%, down two basis points from Friday night’s close of 4.552%. That’s lower than the 4.633% hit last Wednesday, when uncertainty over chancellor Rachel Reeves’s future hit the bond market. But it’s still higher than the 4.498% set at the end of June, before worries about change at the top of the Treasury pushed up borrowing costs. Dean Turner, economist at UBS, suggests gilts could be attractive at current levels, telling clients: We learned last week that any attempt to curb spending is going to prove almost impossible for this government, even with such a large majority. This inevitably means taxes are going up. The sooner the government is honest with the public and gets the deed done, the better. For investors in the gilt market, the volatility is likely here to stay for the time being. But this does not mean gilts do not look attractive, especially relative to cash, as interest rates will be much lower by the time the government’s second anniversary comes around. Despite the uncertainty over tariffs, investor sentiment in the eurozone has hit its highest level in over three years. The Sentix index, which tracks euro area investor morale, has risen to 4.5 points this month, a rise of 4.4 points, its highest reading since February 2022. A measure of the current economic situation rose, but remained in negative territory, while a gauge of economic expectations also increased. Sentix says: Overall, the global upturn is gaining in breadth. The US economy in particular is making up ground. After the weak previous months, the US economy showed the greatest growth in July. The regions of Japan and Asia ex Japan are also providing growth impetus. Oof! Tesla’s shares are down over 7% in pre-market trading in New York, as investors react to Elon Musk’s launch of the new America party. That, by my maths, knocks around $70bn of Tesla’s market value, pulling it below the $1tn level to around $945bn. Victoria Scholar, head of investment at interactive investor, says: Much to the dismay of Tesla’s shareholders, after a brief political hiatus, it looks like Musk is renewing his focus on Washington once again, meaning he’ll have less time to spend on the electric vehicle giant. There is a distant idea that Musk garnering great political influence could mean a bounce back in interest in the green energy transition and a boost to green subsidies which would help Tesla. However, the more realistic, shorter-term likelihood is that Musk’s political shift is negative for Tesla since it comes at a time when the company’s performance is lagging, which necessitates a more hands-on approach from its boss. It looks like shares in Tesla will open lower today on Wall Street, with its Frankfurt listed shares in the red this morning. The stock is already down around 17% this year, sharply underperforming most mega cap tech names and the wider US stock market. Its latest figures revealed that Tesla is struggling amid Musk’s political focus and increased competition from EV rivals. The company suffered a 13.5% drop in quarterly deliveries in April to June, falling short of Wall Street’s estimates. It looks like there’s a long, bumpy, uphill drive ahead for Tesla.” The co-head of Japan’s opposition Japan Innovation Party has called on Tokyo to diversify its trade ties beyond the US market, and focus on countries favouring free trade. Hirofumi Yoshimura warned that Donald Trump’s tariffs show that the US is a source of uncertainty that could hurt its economy. Citing Europe as an example, he told Reuters: “Japan should expand trade ties with countries that focus on free trade.” “Instead of standing on just one, big pillar like the U.S., Japan should stand on, say, five to 10 smaller pillars. That’s a better approach to avoid its roof from falling off.” China opposes tariffs being used as a tool to coerce others, the Chinese foreign ministry said on Monday, after Donald Trump threatened an extra 10% tariffs on countries aligning themselves with the BRICS group of developing nations. The use of tariffs serves no one, said Mao Ning, spokesperson of the ministry, at a regular press conference, Reuters reports. Over in Frankfurt, shares in Tesla are sliding as the row between Elon Musk and Donald Trump escalates. Telsa have fallen 3% in early trading, an indication that they could fall when Wall Street trading begins later today, as investors react to Musk’s plan to launch a new US political party called the America party. Trump called the idea “ridiculous”, and claimed Musk had gone completely ‘off the rails’. Veteran tech analyst Dan Ives of Wedbush said Musk was Tesla’s “biggest asset” and his decision to dive deeper into politics could hurt the car maker’s share price. Ives wrote: “Tesla needs Musk as CEO and its biggest asset and not heading down the political route yet again...while at the same time getting on Trump’s bad side. “It would also not shock us if the Tesla board gets involved at some point given the political nature of this endeavour depending on how far Musk takes it.” London’s stock market has slipped very slightly at the start of trading. The FTSE 100 index of blue-chip shares has dropped by 9 points, or 0.1%. Shell are the top faller, down 1.8%, after lowering its forecast for gas output and natural gas production this morning, and predicting that trading and optimisation at its integrated gas division in the last quarter will be significantly lower than in Q1. Standard Chartered (+1.4%), the Asia-Pacific focused bank, are the top riser. UK house prices stagnated last month, new data from lender Halifax shows. Halifax reports that house prices were effectively unchanged month-on-month in June with the average price of a property sold coming in at £296,665, compared to £296,782 in May. This pulled the annual rate of house price inflation down to 2.5% from 2.6% in May. Northern Ireland has by far the strongest annual price growth in the UK, with prices up by +9.6% over the past year. But, growth was much more subdued in the South West of England, and London, with prices rising by just +0.5% and +0.6% respectively. Amanda Bryden, head of mortgages at Halifax, said the UK housing market “remained steady in June”, adding: “The market’s resilience continues to stand out and, after a brief slowdown following the spring stamp duty changes, mortgage approvals and property transactions have both picked up, with more buyers returning to the market. That’s being helped by a few key factors: wages are still rising, which is easing some of the pressure on affordability, and interest rates have stabilised in recent months, giving people more confidence to plan ahead. Bryden pointed out that affordability is still stretched, particularly for those coming to the end of fixed-rate deals, explaining: The economic backdrop also remains uncertain; while inflation has eased, it’s still above target, and there are signs the jobs market may be softening. Most Asia-Pacific markets are in the red today. Japan’s Nikkei 225 index has dropped by 0.55%, Hong Kong’s Hang Seng is down 0.4%, Australia’s S&amp;amp;P/ASX is off 0.15%, and India’s Sensex has slipped by 0.1% Jim Reid, market strategist at Deutsche Bank, says: “Asian equity markets are a little nervous this morning, perhaps on Trump’s BRICs comments.” Some BRICS currencies have also dipped this morning. South Africa’s rand has fallen 1%, to 17.75/$ from 17.57/$ on Friday night. India’s rupee has slipped by 0.5% against the dollar, to 85.8 rupees/$ down from 85.3925/$ at the end of last week. China’s yuan has slipped by 0.1%, while Brazil’s real and Russia’s rouble are both flat. Many currencies are slipping against the US dollar this morning, as traders await news of the tariff ‘deals and letters’ which Donald Trump says he will issue later today. The euro has slipped by 0.15% against the dollar to $1.176, not too far from the near-four-year high touched last week. The Australian dollar has lost 0.7%, while New Zealand’s dollar has dropped by 0.95%. The British pound is also weakening a little, down 0.35% at just over $1.36. So far, only the UK, China and Vietnam have reached any kind of trade agreements with the US in the last 90 days…. Good morning, and welcome to our rolling coverage of business, the financial markets, and the world economy. Donald Trump has targeted the BRICS group of developing nations in the latest salvo of his ongoing trade war, as the deadline to agree deals before the president’s 90-day tariff pause looms. Trump has warned overnight that he will impose a new 10% tariff on any country that aligns itself with the BRICS group, claiming they are “anti-American”. Writing on his Truth Social site, Trump declared: Any Country aligning themselves with the Anti-American policies of BRICS, will be charged an ADDITIONAL 10% Tariff. There will be no exceptions to this policy. Thank you for your attention to this matter! Trump’s attack comes after the Brics group — which was originally made up of Brazil, Russia, India, China and South Africa but now includes other nations — met in Brazil at the weekend. Brazil’s president Luiz Inacio Lula da Silva, told the meeting in Rio de Janeiro that BRICS was the heir to the “Non-Aligned Movement” – the bloc of countries who declined to ally with either side in the Cold War. Lula criticised the move (driven by Trump) towards increased spending on the military rather than on international development, pointing out: “It is always easier to invest in war than in peace”. He told leaders they were witnessing “the unparalleled collapse of multilateralism”, before warning: “If international governance does not reflect the new multipolar reality of the 21st century, it is up to BRICS to help bring it up to date.” The BRICS group also condemned US and Israeli attacks on Iran and urged “just and lasting” solutions to conflicts across the Middle East. All of which appears to have stirred Trump into another tariff threat. There’s also confusion this morning about the status of the original ‘liberation day’ tariffs which Trump announced at the start of April, and then paused for 90 days after the markets slumped. The president told reporters on Sunday that his administration plans to start sending letters later today to US trade partners dictating new tariffs. But there’s confusion about when these levies would kick in. Trump implied they would start on Wednesday, saying “I think we’ll have most countries done by July 9, yeah. Either a letter or a deal.” But commerce secretary Howard Lutnick then weighed in to explain: “But they go into effect on August 1. Tariffs go into effect August 1, but the president is setting the rates and the deals right now.” Trump has subsequently posted that “TARIFF Letters, and/or Deals” will be delivered from 12:00 PM (Eastern)“ today, (that’s 5pm BST) The agenda 7am BST: Halifax house price index for June 2pm BST: Eurogroup ministers meeting in Brussels</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>EU trade spokesperson: “We’re fully geared up to get an agreement in principle by Wednesday.” 90-day pause to the tariffs annouced by Trump in early April expires on 9 July. Trump posted online that he plans to start announcing deals, and letters announcing new tariffs.</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Time to recap… Donald Trump is preparing to send letters to trading partners, setting out tariff rates that countries will have to pay from the beginning of next month. The US president has said he will send out about “10 or 12” letters on Friday, with further letters over the next few days, as the 90-day pause on his “reciprocal tariffs” comes to an end. Trade tensions are bubbling at the second biggest economy in the world too. China announced new tariffs of up to 35% on brandy from the European Union, condemned as ‘unfair’ by an EU spokesperson. The Chinese tariffs will range from 27.7% to 34.9% and will be effective from Saturday, lasting five years. The Chinese commerce ministry said the decision follows a probe launched last year, which linked European cognac imports to threats against its domestic brandy industry. However, the duties include exemptions for some major cognac makers, including Remy Cointreau, Pernod Ricard and LVMH’s Hennessy. The EU imposed tariffs on Chinese electric vehicles last year, and Beijing has launched similar anti-dumping probes into European dairy and pork. The new tariffs could set a difficult tone for a China-EU summit that is scheduled to be held later this month in Beijing. Meanwhile in the UK, a former Bank of England deputy has said Rachel Reeves has to ‘neurotically fine tune taxes’ because of her decision to opt for fiscal rules that give her little wiggle room. Charlie Bean, who is also a former member of the OBR’s budget responsibility committee, told Radio 4’s Today programme: About £10 billion - that’s a very small number in the context of overall public spending. Government spending is about about one and a quarter trillion so £10 billion is a small number … and it is a small number in the context of typical forecasting errors. …She should aim to operate with a larger margin of headroom, so previous chancellors have typically operated with headroom of the order of £30 billion. Because she has chosen about a third of that … it is very easy for numbers to go in the wrong direction and she finds she has to neurotically fine tune taxes to control the OBR forecast that is several years ahead. The original sin is that she should not have chosen to operate with such a tight margin of error. Tesla sales in the UK rebounded in June, according to the latest figures for monthly new car registrations, following the launch of its new Model Y. The company, which is led by the billionaire Elon Musk, sold 7,719 cars in the UK last month, up 14% compared with June last year. However registrations still remain 1.3% lower in the year to date. Tesla has been struggling with weak sales in some of its international markets, as it has faced a consumer backlash against Musk’s politics, as well as stiff competition from Chinese rivals such as BYD. Overall the company delivered 384,122 vehicles in the second quarter, down 13.5% from 443,956 units a year ago. The end of a 90-day pause on Trump’s “reciprocal tariffs” looms next week on 9th July, with many countries racing to hammer out a deal before they are hit with the president’s levies. Indonesia has offered to cut duties on key imports from the US to “near zero” and to buy $500m worth of American wheat, as part of its trade talks with Washington, its lead negotiator has said. Jakarta is facing a tariff rate of 32% in the US market if it does not reach an agreement. Chief economics minister Airlangga Hartarto said the Indonesian government has offered to cut tariffs on key American exports, including agricultural products, to near zero, compared with current rates that vary between 0% and 5%. He said: It will be near zero … but it will depend as well on how much the tariffs we get from the US. Airlangga also said that the state carrier Garuda Indonesia would buy more Boeing planes as part of a $34 billion deal with business partners to boost purchases from the US. Elsewhere in the world of trade, tensions are simmering between the EU and China, after Beijing announced it would place new tariffs of up to 35% on brandy from the bloc. Olof Gill, a spokesperson for the EU, said: We believe that China’s measures are unfair. We believe they are unjustified. We believe they are inconsistent with the applicable international rules and are thus unfounded. The Chinese tariffs will range from 27.7% to 34.9% and will be effective from Saturday, lasting five years. The Chinese commerce ministry said the decision follows a probe launched last year, which linked European cognac imports to threats against its domestic brandy industry. However, the duties include exemptions for some major cognac makers, including Remy Cointreau, Pernod Ricard and LVMH’s Hennessy. The EU imposed tariffs on Chinese electric vehicles last year, and Beijing has launched similar anti-dumping probes into European dairy and pork. The announcement comes as the Chinese foreign minister Wang Yi tours Europe to discuss trade. Wang is set to meet his French counterpart, Jean-Noël Barrot, later today in Paris. A China-EU summit is planned to be held later this month in Beijing. The boss of Ryanair has said that he is hopeful that trade tariffs between the US and the European Union would not apply to commercial aircrafts, as it would disrupt complex supply chains. Ryanair chief executive Michael O’Leary told Ireland’s RTE radio: Commercial aircraft have always been exempt under previous tariffs ... We think that’s likely to be restored even if there are tariffs applied. The comments come as investors await the EU to finalise a trade deal with the US ahead of Trump’s deadline on 9 July. The Stoxx Europe 600 index, which tracks the performance of some of the biggest companies on the continent, is down by 0.65%. The EU and the US are closing in on a high-levle “framework” trade deal that would mean that the bloc could avert 50% tariffs on all its exports next Wednesday. The downturn in UK construction is starting to ease, according to new data released this morning. The S&amp;amp;P Global UK Construction Purchasing Managers’ Index rose to 48.8 from 47.9 in May, reaching a six-month high. It is still below the 50 threshold which represents growth in the market. The survey painted a mixed picture across the industry, with housing activity expanding for the first time since September, but the commercial sector contracting at the fastest rate since mid 2020. Gareth Belsham, of Bloom Building Consultancy, said: Yes the overall contraction in industry workloads continues to ease, and housebuilders even saw output rise in June. That’s the good news. But on the other side of the ledger, commercial sector workloads fell sharply, declining at their fastest level since May 2020 - a month when Britain was in the teeth of the Covid pandemic. Infrastructure and civil engineering work contracted even more rapidly. But the real cause for alarm is the continued decline in new orders - as they are the key to where the industry goes from here. Builders’ order books have got progressively thinner every single month in 2025 so far, and this is taking a severe toll on construction industry sentiment. The inability of Britain’s government to make cuts to its welfare sending has underscored the “formidable” challenge it faces in shoring up its finances, analysts at the credit rating agency S&amp;amp;P Global have said. This week Sir Keir Starmer was forced to gut his controversial welfare bill following strong opposition from Labour MPs, abandoning approximately £5bn in potential savings for the government. Analysts at S&amp;amp;P wrote: We consider the inability to make modest cuts to welfare spending, which has ballooned in the UK since the 2020 pandemic, underscores the UK government’s very limited budgetary room for manoeuvre. Turning back to the UK, house builders are among the worst performers across the FTSE this morning. MJ Gleeson, which has been struggling with high costs and planning delays, said it now expects its pre-tax profit to be at or around £24.5m, at the lower end of what the market had been expecting. The update has sent its shares down 5.4%. Rival Vistry has followed it down 3.1%, while in the FTSE 100 Berkeley and Barratt Redrow are both down by 2% and 1.7% respectively. Trump’s flagship tax bill steals from the sick, elgerly and hungry, and gives to billionaires and jackboots, writes Moira Donegan. The budget reconciliation bill that passed the US House of Representatives on Thursday and was promptly to be signed into law by Donald Trump represents the particular perversity of national politics in America: seemingly no one wants it, everyone hates it, and it is widely agreed to be devastating for staggering numbers of Americans. And yet, the bill felt inevitable: it was a foregone conclusion that this massive, malignant measure was something that everyone dreaded and no one had the capacity to stop. They didn’t really even try. In the Senate, a few conservative Republicans made noise about the bill’s dramatic costs: the congressional budget office estimates that the bill will add $3.3 tn to the deficit over the coming decade, and the senator Rand Paul, a budget hawk from Kentucky, declined to vote for it for this reason. But other Republicans, who used to style themselves as fiscally responsible guardians against excessive government spending, engaged in a bit of freelance creative accounting in order to produce an estimate that falsely claimed the cost of the bill would be lower. Most of them quickly found themselves on board. Elsewhere, the government has set out a roadmap for reviving the onshore wind industry in England, after Labour lifted the de facto ban last year which was put in place by the Conservatives. The Onshore Wind Industry Taskforce has set out more than 40 steps to help development in the sector, including planning reforms, re-powering old turbines and exploring plans to expand the clean industry bonus for onshore wind. Energy secretary Ed Miliband said in a report: As one of the cheapest and fastest-to-build sources of power we have, onshore wind will play a critical role in boosting our energy independence with clean power by 2030. The reality is that every turbine we build helps protect families, businesses and the public finances from future fossil fuel shocks. The government is planning to almost double onshore wind across England by 2030, taking its capacity from 14.8GW to 27 to 29GW. It has claimed the strategy will support the creation of up to 45,000 skilled jobs by the end of the decade. It is a rather weak open for stock markets in Europe this morning. In the UK, the blue chip FTSE 100 index has slipped 0.3% in early trading. The German Dax index slipped 0.5%, while the French Cac 40 index dropped by 0.8%, as the European Union tries to finalise a new trade deal with the US. Susannah Streeter, head of money and markets at the investment broker Hargreaves Lansdown, said that optimism is starting to evaporate at the end of the week as the US tariff deadline looms on 9 July. There’s a distinct lack of Friday fizz for the FTSE 100, as investors mull repercussions for the global economy. Investors are also assessing the implications of the passing of Trump’s big tax cut bill which will add to the mountain of US debt. Streeter added the US stock market has been riding high on signals that so far Trump’s trade policies have not weakened the economy. The closely watched US jobs report for June signalled much more strength in the labour market than expected. Although it’s wiped out hopes of an interest rate cut this month, it didn’t hit sentiment, which appears more focused on the resilience of the world’s largest economy. Markets are closed for the July 4th holiday but more caution is set to creep into sentiment and show up when trading resumes on Monday. Rachel Reeves has not given herself enough fiscal headroom to manage public finances, Charlie Bean, the former deputy of the Bank of England has said, and has to “neurotically fine tune taxes”. Bean, who is also a former member of the OBR’s budget responsibility committee, told Radio 4’s Today programme the chancellor had chosen fiscal rules that give her a “very small margin” of headroom. About £10 billion - that’s a very small number in the context of overall public spending. Government spending is about about one and a quarter trillion so £10 billion is a small number … and it is a small number in the context of typical forecasting errors. You can’t forecast the future perfectly both because you can’t forecast the economy and you can’t forecast all the elements of public finances …. the forecasts are imprecise and there is no way you can avoid that. That is a fact of life. She should aim to operate with a larger margin of headroom, so previous chancellors have typically operated with headroom of the order of £30 billion. Because she has chosen about a third of that … it is very easy for numbers to go in the wrong direction and she finds she has to neurotically fine tune taxes to control the OBR forecast that is several years ahead. The original sin is that she should not have chosen to operate with such a tight margin of error. Reeves has been under intense public pressure, after the government’s concessions to Labour MPs over plans to change welfare payments have wiped out plans for £5bn savings a year. Oil futures have slipped after the Iranian foreign minister Abbas Araqchi said Tehran remains committed to the nuclear Non-Proliferation Treaty. Brent crude futures dropped by 0.51% to $68.45 a barrel, while US West Texas Intermediate crude dropped 0.37% to $66.75. Vandana Hari, founder of oil market analysis provider Vanda Insights, said: Thursday’s news that the U.S. is preparing to resume nuclear talks with Iran, and Araqchi’s clarification that cooperation with the U.N. atomic agency has not been halted considerably eases the threat of a fresh outbreak of hostilities. This week Tehran enacted a law suspending cooperation with the UN nuclear watchdog, the International Atomic Energy Agency. However Hari added that the oil price correction “may have to wait till Monday”, when the US returns from a long weekend and reacts to an Opec+ decision on Sunday. Opec+, the world’s biggest group of oil producers, is expected to announce an increase of 411,000 barrels per day in production for August. Meanwhile in the UK, British electric car sales rose by a third in the first half of 2025 after the strongest June for overall car sales since before the Covid pandemic. The number of battery electric car sales rose 34.6% to 224,838 units in the first six months of the year, according to preliminary data from the Society of Motor Manufacturers and Traders (SMMT), a lobby group. New car sales rose 6.8% year-on-year in June to 191,200 units, the best sales figures for the month since 2019. A quarter of all June sales, or nearly 47,400, were electric. The figures come amid a difficult period for the the UK car industry, which has struggled to increase sales to pre-pandemic levels as potential buyers have been hit by the cost of living crisis after Russia’s full-scale invasion of Ukraine. British car factories have also had to contend with a major slowdown in response to extra US tariffs of 25% announced by Donald Trump in March. Last month UK car production fell to its lowest level for May since 1949 as manufacturers cut back shipments. You can read the full story from my colleague Jasper Jolly here. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. President Donald Trump has secured passage of his controversial flagship tax and spending bill, after the House of Representatives approved the bill late on Thursday. The 218-to-214 vote sends the legislation to Trump, who has said he plans to sign the bill on Friday as the US celebrates Independence Day. Speaking to supporters at the Iowa State Fairground, he said “there could be no better birthday present for America”. There could be no better birthday present for America than the phenomenal victory we achieved just hours ago, when Congress passed the “One Big Beautiful Bill” to make America great again…one-hundred-and-sixty-five days into the Trump administration, America is on a winning streak like, frankly, nobody has ever seen before in the history of the presidency.” Meanwhile, the president’s trade war rattles on. Trump told reporters late on Thursday that his administration will start sending out letters on Friday setting unilateral tariff rates, which countries would have to begin paying on 1 August. Trump said “10 or 12” letters would go out on Friday, with additional letters coming “over the next few days”. The higher import duties will range in value from “maybe 60 or 70% tariffs to 10 and 20% tariffs”, he said. The top tier of that range would be higher than any of the levies the president first outlined during his Liberation Day rollout in April. He did not provide any detail on which countries might receive such high tariffs. The UK is one of a few countries that has reached a trade agreement with Trump, including Vietnam. Many trading partners such as the European Union, Japan and South Korea are still trying to finalise trade deals. Trump has threatened that if countries fail to reach deals by 9 July, he could simply impose tariff rates on them. The agenda 9:00am BST: UK SMMT car market figures for the first half of the year 9:30am BST: UK PMI construction data US market closed for Independence Day</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>China announced new tariffs of up to 35% on brandy from the EU. The Chinese tariffs will range from 27.7% to 34.9% and will be effective from Saturday, lasting five years. The EU imposed tariffs on Chinese electric vehicles last year, and Beijing has launched similar anti-dumping probes into European dairy and pork.</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Time to recap… The US economy added 147,000 jobs in June, a sign of continuing strength in the labor market amid Donald Trump’s trade war. The number of jobs added surpassed expectations, as economists largely anticipated a drop in openings. In another boost, the unemployment rate decreased to 4.1%, down from 4.2% in May. Job gains were seen in state government and healthcare, which saw increases of 47,000 and 39,000 jobs, respectively. Meanwhile, federal government job losses continued, with another 7,000 roles down in May, as the Trump administration continues to cut jobs. The total job loss in the federal government has been 69,000 since January. Economists said the data cut the chances of an early interest rate cut from the US Federal Reserve. The dollar strengthened, while US bond prices fell, pushing up yields, and Wall Street hit a record high. UK government bonds have rallied after Keir Starmer backed Rachel Reeves to remain as chancellor for “a very long time” despite lingering investor concerns over a multibillion-pound hole in Britain’s public finances. The yield – in effect the interest rate – on British 10-year government bonds, also known as gilts, fell on Thursday morning to trade close to 4.5%, reversing much of the rise on Wednesday sparked by feverish speculation over Reeves’s future. The pound rose against other leading currencies, while a closely watched business survey showed that Britain’s dominant service sector recorded its fastest rate of growth in 10 months. But….some of the gains were later pegged back after the release of the stronger-than-anticipated US job market figures, which fuelled a rise in US government borrowing costs as investors bet the Federal Reserve may delay cutting interest rates. The boss of Currys, the UK’s biggest electrical goods retailer, has urged the government not to increases taxes on retailers this year, saying it would damage investment and force prices to rise. The EU and US are closing in on a high-level “framework” deal that would avert 50% tariffs on all exports from the bloc next Wednesday, Donald Trump’s self-imposed deadline. Richard Branson’s hopes of returning Virgin trains to the west coast mainline have been dashed after the UK rail regulator rejected its application amid concerns over delays and cancelled journeys. The boss of P&amp;amp;O Ferries was paid £683,000 in the financial year after the cross-Channel operator outraged the public and parliament by dismissing almost 800 mainly British workers. The London stock market has closed at its highest level for two weeks, lifted by UK-focused companies. The FTSE 100 index of blue-chip shares has ended the day 48 points higher at 8823 points. Top risers included banks NatWest (+3.2%) and Lloyds (+3.2%) and Tesco (+2.3%), while mining companies were among the fallers. AJ Bell head of financial analysis Danni Hewson says: “Borrowing costs, which shot up yesterday as investors priced in her potential departure from Number 11, have reversed course today, with a number of big names openly stating that they added to their gilt stash in a bet the turmoil would be short-lived. “There has also been better news from the UK service sector as the latest PMI figures came in hotter than expected, with both businesses and consumers feeling a little more confident about spending. “For once London’s blue-chip index was dominated by improved domestic sentiment – banks, retailers and housebuilders all made gains whilst global mining stocks slumped. “It was a similar story on the FTSE 250. External issues pulled down companies like Watches of Switzerland which is already seeing US retailers pushing through price hikes on its products. “The deadline for tariff talks is fast approaching and with the White House laser focused on getting that ‘big, beautiful bill’ signed into law investors might be nervous that the clock will run out before deals can be struck. In the world of trade, the EU and US are closing in on a high-level “framework” deal that would avert 50% tariffs on all exports from the bloc next Wednesday, Donald Trump’s self-imposed deadline. Talks in Washington could go down to the wire, but diplomats and officials said the EU was willing to accept Trump’s 10% blanket tariffs. Negotiators will only accept this, however, in exchange for an extension in talks and possible concessions on a 25% car tariff, which is hurting the German car industry, sources said. European Commission president, Ursula von der Leyen, has pointed out today that it is “impossible” to agree a final EU-US trade deal before July 9… A permanent risk premium could be attached to UK bonds following yesterday’s sell-off, warns Kathleen Brooks, research director at XTB: In the UK, the bond market is recovering on Thursday after Wednesday’s sell off. The Prime Minister has confirmed that Rachel Reeves will remain in place as Chancellor, however, bond yields have not fallen back to the levels that we saw before bonds started to sell off 24 hours ago. The 10-year yield had been down 10bps at one stage, however, this has been eroded, and yields are only down 5bps at the time of writing. A sharp rise in US yields is dragging UK yields higher as we move through Thursday. This suggests 2 things: 1: highly indebted western economies can see their sovereign debt markets move in unison, which is bad news for those who hoped there could be a full reversal in UK bond yields today. 2: there could be a permanent premium attached to UK yields as we move through the summer months to October’s budget. The premium this time is linked to Labour’s left having increasing control over Kier Starmer and pushing him for ever greater levels of public spending. If the government wants to avoid an embarrassing and devastating fiscal crisis, they need the guts to cut public spending to more reasonable levels. The bond vigilantes are circling, and Labour could be forced to U-turn on the U-turns. Back on Wall Street, Nvidia is on track to become the most valuable company in history. The chipmaker’s market capitalization has risen to $3.915trn today, after its shares rose 2% in early trading, lifted by continued optimism about demand for high-performance chips to power artificial intelligence systems. Tht gives it a slightly higher market capitalization than Apple’s record closing value of around $3.915trn on December 26, 2024, Reuters reports. The US Department of Labor has given Donald Trump the credit for June’s solid jobs numbers: The president has reposted this message on his Truth Social site, so I guess we can conclude it was the Trump economy in June rather than the Biden economy (which took the blame for GDP shrinking in January-March) Today has been a rough day for some airline passengers in the UK. Low-cost airlines Ryanair and easyJet both cancelled hundreds of flights due to French air traffic control strikes. Ryanair said it was forced to make 170 cancellations on Thursday and Friday as the strikes affect flights to and from France – and also flights over the country to destinations such as the UK, Greece, Spain and Ireland – impacting more than 30,000 passengers. Luton-based rival easyJet said it had cancelled 124 flights today and was scrapping 150 tomorrow due to the industrial action. Ryanair chief executive Michael O’Leary renewed calls on EU Commission President Ursula von der Leyen to take “urgent action” to reform European Union air traffic control (ATC) services in light of the disruption, which comes at the start of the European summer holidays. O’Leary said: “Once again, European families are held to ransom by French air traffic controllers going on strike. “It is not acceptable that overflights over French airspace en route to their destination are being cancelled/delayed as a result of yet another French ATC strike. “It makes no sense and is abundantly unfair on EU passengers and families going on holidays.” Analysts at ING predict that Donald Trump will have to wait until September for a cut to US interest rates. Following today’s stronger-than-expected jobs report, they say: The June US jobs report shows nonfarm payrolls rising 147,000 versus the 106,000 consensus with 16,000 of upward revisions to the past two months of data. Meanwhile, the unemployment rate surprisingly fell to 4.1% from 4.2% while the market was solidly backing the view that unemployment would actually tick higher to 4.3%. President Trump has been calling for the Federal Reserve to cut the policy rate 200-300bp immediately and two of his appointees (Chris Waller and Michelle Bowman) had suggested that they could vote for a rate cut as soon as this month’s FOMC meeting. But the rest of the FOMC is far more cautious and today’s data indicates there will be no rate cut before the September FOMC meeting, especially with tariffs set to push inflation higher over the next few months. Wall Street has hit fresh record highs, as investors hail today’s stronger-than-expected jobs report. The news that the US economy added 147,000 new jobs in June helped the S&amp;amp;P 500 share index and the Nasdaq to both open at fresh record highs. The Dow Jones Industrial Average rose 81.3 points, or 0.18%, at the open to 44565.75 points. The S&amp;amp;P 500 gained 0.3%, and the Nasdaq Composite rose by 0.5%. In other economic news… America’s trade deficit has widened again. The US trade deficit surged by 18.7% in May to $71.5bn, new data from the US Census Bureau and the US Bureau of Economic Analysis shows, up from $60bn in April. The increase was driven by a 4% drop in US exports during the month, while imports were flat. The report also shows that the US trade deficit with China shrank by over a quarter in May, after the US imposed high tariffs on Chinese imports. The deficit with China decreased $5.7bn to $14.0bn in May, with exports down $1.7bn to $6.9bn and imports down $7.4bn to $20.9bn. The report shows that in May the US also recorded deficits with the European Union ($22.5bn), Mexico ($17.1bn), Vietnam ($14.9bn), Ireland ($11.8bn), Taiwan ($11.5bn), Germany ($6.8bn), Japan ($5.8bn), South Korea ($5.4bn), India ($5.1bn), Canada ($2.8bn), Italy ($2.6bn), Malaysia ($2.4bn), and France ($0.5bn). The US ran a trade surplus with the Netherlands ($4.8bn), Hong Kong ($3.6bn), South and Central America ($3.3bn), Switzerland ($3.3bn), the United Kingdom ($3.0bn), Australia ($1.5bn), Brazil ($0.5bn), Saudi Arabia ($0.5bn), Belgium ($0.4bn), Singapore ($0.3bn), and Israel ($0.1bn). The jump in US bond yields today is feeding through to other markets, undermining the recovery in UK government debt earlier today. Although UK 10 and 30-year bond yields are still down, they’re only around 3 basis points lower, which means only some of yesterday’s jump has been wiped out. Today’s US jobs report shows that the labour market remains healthy, says Bradley Saunders, North America economist at Capital Economics. The 147,000 gain in non-farm payrolls in June was reassuring after the fall in the ADP measure of employment reported yesterday. A deeper dive shows the strength was again concentrated in government and health care employment, reflecting the increasing narrowness of the labour market’s strength. Nevertheless, with the unemployment rate edging lower again, the report was better than expected and will give the more hawkish members of the FOMC reason to push back against expectations for imminent interest rate cuts. The 147,000 gain in non-farm payrolls in June and slight upward revisions to earlier months’ data mean the three-month average rate now sits at a healthy 150,000. Glassdoor’s lead economist Daniel Zhao says June’s job gains were ‘moderate’: “The June jobs report feels more like a sparkler than a fireworks show—steady and slow-burning. While the labor market continues its gradual cooling, this report likely doesn’t reflect the full impact of upcoming tariffs, which could add pressure to hiring in the months ahead.” Isaac Stell, investment manager at Wealth Club, argues the US economy remains as solid as a rock, adding: It’s difficult to imagine what could cause the US economy to crack given tariff turmoil has done little to shake the foundations. As a result, hopes for a rate cut from the Fed in July have all but disappeared. All thoughts will now turn to the next inflation report on July 15th. If inflation remains some way above the Fed’s 2% target, there will start to be questions about whether rates get cut at all this year. Today’s numbers will not help that case and this in turn will likely do nothing to appease an already agitated President. However, as demonstrated at the last Fed meeting, the President’s unstoppable wave of political pressure is likely to do nothing to the immovable object of the central bank’s resolve. Unless an early Fed chair nomination changes the picture that is . . .” The US dollar is rallying, on the back of today’s better-than-expected jobs report. The dollar index has gained 0.6%, as the greenback strengthens against a basket of rival currencies, amid declining hopes of early cuts to US interest rates. This has knocked the pound lower; it’s now down 0.2% today at $1.3613, wiping out its small recovery this morning. Here are more details of the US jobs report, from Liz Ann Sonders, chief investment strategist at Charles Schwab. US bond prices are dropping, pushing up borrowing costs, as traders bet that an early interest rate cut is unlikely. This has pushed up the yield, or interest rate, on two-year US Treasury bonds by 9 basis points. Investors may be calculating that the Federal Reserve will be less inclined to cut borrowing costs soon, given job creation continued at a pretty robust rate last month. Around half the 147,000 new jobs created last month were in the US public sector, specifically education. Today’s jobs report shows that government employment rose by 73,000 in June, adding: Employment in state government increased by 47,000, largely in education (+40,000). Employment in local government education continued to trend up (+23,000). But, there were 7,000 job cuts in June in the federal government – where employment is down by 69,000 since reaching a recent peak in January. (Employees on paid leave or receiving ongoing severance pay are counted as employed in the establishment survey, the BLS points out, which makes it harder to see the impact of DOGE job cuts). Health care added 39,000 jobs in June, including 16,000 in hospitals and 14,000 in nursing and residential care facilities Social assistance employment rose by 19,000. However, there was little change in employment in other major industries. Newsflash: The US economy added more new jobs than expected last month, a sign that economic growth wasn’t chilled by Donald Trump’s trade wars. The US non-farm payroll, the closely-watched measure of America’s jobs market, rose by 147,000 in June, better than the 110,000 new hires expected. The unemployment rate has dipped to 4.1%, down from 4.2% recorded last month – and lower than the 4.3% which economist had forecast. The U.S. Bureau of Labor Statistics reported that “Job gains occurred in state government and health care. Federal government continued to lose jobs.” In another encouraging signs, the two previous month’s jobs report have been revised higher too. April was revised up by 11,000, from +147,000 to +158,000, and the change for May was revised up by 5,000, from +139,000 to +144,000. Economists predict that today’s US jobs report, due in about 30 minutes, will show that America’s labour market slowed in June. The consensus forecast is that the US non-farm payroll rose by 110,000 jobs last month, which would be a slowdown on the 139,000 new hires recorded in May. The US unemployment rate is forecast to rise to 4.3%, from 4.2%. Today’s rally in London has helped to push global stock markets to record levels. MSCI’s main index of global shares has touched a new record high today, as investors await the latest US jobs report in just under an hour’s time. News that the US and Vietnam have reached a trade deal has lifted the mood in the markets – under it, Americans will pay a 20% tariffs on imports from Vietnam, while the US will get tariff-free access into Vietnam’s markets. The UK stock market is higher today too. The FTSE 100 index of blue-chip shares is up 33 points, or 0.4%, at 8807 points. The smaller FTSE 250 index of medium-sized companies has gained 0.6%. Joshua Mahony, chief market analyst at Rostro, explains: European markets are on the rise today with the FTSE 100 attempting to regain lost ground as a sharp rise in borrowing costs raised fear of another Truss/Kwarteng moment yesterday. The watered-down version of the Labour welfare reforms does mean we are staring at a fiscal black hole which like means greater tax hikes, with the pop in UK bond yields highlighting the fear of financial instability in the UK. With Reeves known to follow the premise that all day-to-day spending must be covered by tax revenues, the prospect of her losing her post had initially spooked markets. However, Starmer’s efforts to calm markets appears to have paid off, with the PM pledging that she will “be the chancellor into the next election and for many years afterwards”. Today’s recovery in UK bond prices will be profitable for investors who bought gilts yesterday, after prices tumbled. According to the Financial Times, those winners include BlackRock and Schroders, who both bought UK debt during Wednesday’s sell-off. Both firms bet that the uncertainty over Rachel Reeves’ future would not trigger a deeper rout in UK government debt. Simon Blundell, co-head of BlackRock’s European active fixed-income team, has explained: “We are overweight the gilt market, we did add to that yesterday afternoon.” Because bond yield rise when prices fall, gilts bought yesterday will provide a higher rate of return than if you were to buy them today (as prices have recovered). A UK interest rate cut next month is looking slightly more likely, City predictions suggest. An August rate cut is now seen as an 81% probability, according to the money markets this morning. That’s up from around 75% earlier this week. Rachel Reeves has just spoken at an event to launch the UK’s new 10-year health plan. My colleague Andrew Sparrow reports that Reeves is smiling a lot as she says the plan will get the NHS “back on its feet”. And she says she has only been able to invest in public services by sticking to her fiscal rules. She does not refer to what happened in the Commons yesterday at PMQs. Health secretary Wes Streeting praised Reeves at the event too, saying she has put an extra £29bn into the NHS. Streeting said: It is thanks to her leadership that we’ve seen interest rates in our country fall four times. It’s thanks to her leadership that we see wages finally rising faster than the cost of living. And it’s thanks to her leadership we have the fastest growing economy in the G7. Andy’s Politics Live blog has all the action: The UK government is more likely to raise taxes in the autumn budget than attempt spending cuts, predicts Morgan Stanley economist Bruna Skarica. Skarica told clients this morning that the UK could potentially face a £30bn miss versus their fiscal framework in the autumn – £1bn from u-turning on winter fuel payments, £5bn from the delay to welfare reform, plus a potential £20bn hit if the Office for Budget Responsibility lowers its growth forecasts. Skarica points out that “to govern is to choose”, and suggests three options: Find alternative spending cuts. This, we think, would be challenging. Indeed, in our mid-year outlook we noted that our “our main concern going into the autumn is...that the existing departmental spending plans look very tight...It seems almost inevitable that current spending will be topped up”; Raise taxes. Hiking income, corporation or value-added taxes would breach Labour’s manifesto commitments, but we estimate it would be challenging to amass revenues of more than £10bn from increasing other levies and surcharges. In our mid-year outlook, we noted that the effective rate of income tax in the UK looks relatively low for median earners, implying that reversing the recently cut employee NICs could be one option for the Treasury to consider. Fiscal rules could be altered. The rising risks of this option, we think, is what drove the adverse market action [on Wednesday]. UK fiscal rules are self-imposed and can be adjusted by the Treasury. Elsewhere in the economy, demand for mortgages appears to be weakening. British lenders expect demand for mortgages will fall over the coming three months, according to new data from the Bank of England. The BoE’s quarterly Credit Conditions Survey shows that more lenders expect a drop in secured lending in the next three months. Uk 10-year bond yields have also recovered quite a lot of yesterday’s jump, as this post from Mohamed El-Erian (who we heard from earlier) shows: Prime minister Keir Starmer has “brought a sense of calm to markets” by backing Rachel Reeves, says Dan Coatsworth, investment analyst at AJ Bell. Coatsworth explains: “Starmer declaring his support for the chancellor has led to gilt yields pulling back and sterling rebounding after yesterday’s slump against the dollar. The initial sell-off in gilts and the pound was the market’s way of saying it was losing faith in the economic outlook and political stability. “It was an electric shock for investors but today’s rebound suggests that crisis has been averted, at least for now. UK economically sensitive assets were in relief mode, including a rally in housebuilders and banks. Newsflash: Britain’s services sector has grown at its fastest pace in 10 months, in a boost to the UK government. Data firm S&amp;amp;P Global has reported that UK service providers have reported “a sustained expansion of business activity in June”. Activity grew at the fastest rate since August 2024, lifted by growing improvement in order books, according to the latest poll of purchasing managers at UK services firms. This lifted S&amp;amp;P Global’s UK Services PMI to 52.8 in June, up from 50.9 in May and the highest for 10 months. Any reading over 50 shows a rise in activity. Companies attributed the pick-up to “generally improving business and consumer spending”, despite “subdued UK economic conditions, the impact of US tariffs and adverse geopolitical factors”, the report says. Tim Moore, economics director at S&amp;amp;P Global Market Intelligence, explains: “June data highlighted a modest rebound in UK service sector growth, fuelled by a turnaround in domestic business and consumer spending after a soft patch during the spring. Business activity expansion was slightly stronger than the earlier ‘flash’ estimate for June and the fastest seen since August 2024. While total new work picked up in June, shrinking export sales were a constraint on service sector growth. Survey respondents cited headwinds from US tariffs and geopolitical tensions, which resulted in subdued demand conditions across global markets. Britain’s 30-year bonds have almost recovered to their levels before yesterday’s sharp sell-off. The yield, or interest rate, on 30-year debt has now dropped by almost 10 basis points (0.1 percentage point) to 5.31%, down from 5.4% last night. At noon yesterday, they were trading at 5.29%, before worries over Rachel Reeves’s future sparked a bond selloff, pushing up yields (which rise when price fall). The boss of Currys, the UK’s biggest electrical goods retailer has urged the government not to increases taxes for retailers this year, warning it would “further dampen investment and increase prices.” Reporting a 37% jump in pre-tax profit to £162m in the year to 3 May and the revival of dividend payment to shareholders after two years as sales rose 3% to £8.7bn, Alex Baldock, the chief executive of Currys said: “We urge government not to make a further contribution to the tax burden as that would further dampen investment and increase prices in an inflationary way. I would urge government ot think very carefully before making the situation worse.” He said that Currys had increased sales at established stores by 6% in the UK, helped by a 12% surge in sales of services including repairs, financing and mobile subscriptions. Baldock said the wider electrical goods market had been flat in the UK and there were concerns about cheap electrical goods being dumped in the UK via online marketplaces amid new taxes on imports of such goods to the US and planned changes in the EU. Baldock said he welcomed the government’s promise that it would look at the so-called de minimus rules, which allow tax breaks on low value goods worth sent directly to consumers, but would “urge some urgency” on making changes. In the UK, the threshold for import duty is £135, while items valued at £39 or less also do not attract import VAT. UK gilts are “firming up this morning along with the pound” after the PM gave his chancellor much more vigorous backing, says Neil Wilson, UK investor strategist at Saxo Markets. He says Reeves is probably the “the most market-friendly chancellor Labour could field”. But, the government has a deeper problem – the market is getting nervous about its ability to make the sums add up whether Reeves is ‘market-friendly’ or not. Wilson adds: Despite the backing from the PM, or perhaps because of it, the question for investors right now is: will she leave? The market reaction should proclaim that she is required at No11 to avert a market response that delivers a death blow to the government; the prime minister is now giving her his full backing. The PM can’t control his backbenchers, but maybe the bond market can. The reaction could keep her in the job. But doubts remain and we might see continued pressure on gilts as we head into the autumn. And often when a PM has to constantly state his backing for a minister the writing is on the wall. The market’s attention is now turning to whether Chancellor Rachel Reeves is really as safe as Prime Minister Keir Starmer has suggested, says Kallum Pickering, chief economist at UK investment bank Peel Hunt. Pickering suggests there are three possible outcomes, writing: Reeves stays because Starmer realises that markets see her as less bad than the alternatives and because, put plainly, history shows that Prime Ministers who sack their Chancellors rarely last long either; Reeves is replaced by a presumed safe pair of hands (such as Pat McFadden) once markets have settled – but to restore credibility her replacement will need to stare down and win a budget fight with the far-left fringe of the Labour Party, which now appears to be the tail that wags the dog on fiscal policy; or Starmer may brief against Reeves to suggest she is the reason Labour promised not to raise the big three taxes (income tax, VAT and employee NI) before forcing her to raise one of them at the budget to get the finances on track, then sack her and let her to take the blame for the fiscal failures during the first 18 months in office. Pickering also warns that the next few days and weeks may be choppy in the run-up to 9 July, when the pause on Donald Trump’s ‘Liberation Day’ tariffs is due to end. The drop in yields on shorter-term UK bonds will be a relief to households looking to take out a mortgage (or remortgage). As the BBC’s Faisal Islam points out, those products are priced off the cost of UK government borrowing: Rachel Reeves has the backing of the bond market, argues Kathleen Brooks, research director at XTB. Brooks says yesterday bond market sell-off reflected concerns about what may come in the autumn budget; and is also a reminder to “the hard left of the Labour party that the UK economy cannot afford its benefits bill”. Brooks writes: After the watered down welfare reform bill, the focus was on the need to raise taxes and to potentially issue more borrowing to cover the cost of Labour’s plans. However, the bond market revolt suggests that these two options are not viable when national debt is so high and the economy is so weak. The bond market is telling the Chancellor to get on with the job of reducing unsustainable levels of public sector spending, but will she listen? The pound is pushing higher too! Sterling has now gained a third of a cent against the US dollar, up to $1.366. That means it has recovered roughly a third of yesterday’s tumble. The bond market is looking calmer this morning, as traders welcome Keir Starmer’s endorsement of Rachel Reeves. The prices on UK government debt are rising in early trading, which pulls down the yield (or interest rate) on the bonds. The yield on UK 30-year bonds has dipped by 0.8% in early trading, to 5.361%. Yesterday it had surged to 5.408%, from 5.234%. UK 10-year bond yields have also dipped by around three basis points, to 4.55% from 4.58% last night. These moves suggests the bond markets are relieved that Starmer is standing by Reeves, easing concerns that a new chancellor might be less committed to the fiscal rules, so might look to borrow more. But while today’s recovery eases some of the pressure on the government, it doesn’t wipe out all of Wednesday’s jump in borrowing costs – traders will be wondering how the government will patch up the multi-billion pound black hole in the public finances. Shorter-dated two-year and five-year bond yields have also slipped back, as prices recover some ground. The jump in UK borrowing costs yesterday will have added to Rachel Reeves’s fiscal problems, unless it reverses. Mohamed El-Erian, chief economic advisor to insurance giant Allianz, has calculated that Wednesday’s rise in bond yields would add £1.8bn to government spending each year, “if it sticks”. He told Radio 4’s Today programme that it’s “very hard” to take a risk premium out of markets, explaining: The minute you put a risk premium in the marketplace, it’s very hard to take out. I suspect that we will see some moderation, but we will not go back to where we were 24 hours ago. El-Erian says investors have been reminded that the UK’s fiscal problem is “deep”; without growth, we face a “vicious cycle where every action you try to take is either economically problematic or politically problematic,” he adds. He then warns that Reeves’s fiscal headroom of about £10bn (the margin before she breaks her fiscal rules) is “essentially gone”. That means she must find at least £10bn of measures in autumn’s budget, and that bill will go up if growth slows or borrowing costs rise further. And that money may have to come from taxes. El-Erian explains: So the area left are the two taxes that the Labour government ruled out in the election, income tax and VAT. They are your major sources of tax revenue. No one likes them, but in a world like this, they will become better than the alternatives. After a tough day yesterday, the pound is calmer in early trading. Sterling is marginally higher (+0.08%) against the US dollar today, at $1.3646, having dropped by a cent yesterday. The calm follows backing for Rachel Reeves from Keir Starmer. He told the BBC that the Chancellor has done a “fantastic job”, adding: “She and I work together, we think together. In the past, there have been examples – I won’t give any specific – of chancellors and prime ministers who weren’t in lockstep. We’re in lockstep.” That may reassure investsors worried that Reeves could be replaced, and that a new chancellor would be less enthusiastic about controlling borrowing. Simon French, chief economist at investment bank Panmure Liberum, argues that “almost all other Chancellor options from within the parliamentary Labour Party” are less market friendly options. French told clients: Recent weeks have shown that large parts of the parliamentary Labour Party in the UK do not have the stomach for the tough fiscal choices required in a normalised interest rate environment, amidst sluggish productivity growth, with the tax burden at an eight-decade high, and with a deteriorating demographic profile. The lack of a working majority for its economic plans leaves the Labour government with an intractable problem - its credibility with financial markets hinges on adherence to a set of fiscal rules that are incompatible with its manifesto tax commitments, and the plans outlined at the recent Spending Review. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. All eyes are on UK bonds, and the pound, after both fell sharply yesterday amid speculation over the future of chancellor Rachel Reeves. Wednesday was a turbulent day for the UK bond market; prices of British government debt fell heavily as investors were gripped by concerns of change at </t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>The US economy added 147,000 jobs in June, a sign of continuing strength in the labor market amid Donald Trump’s trade war. UK government bonds have rallied after Keir Starmer backed Rachel Reeves to remain as chancellor for “a very long time” The London stock market has closed at its highest level for two weeks, lifted by UK-focused companies.</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>The UK’s financial watchdog is expanding bullying and harassment rules to more than 37,000 City firms, in an effort to crack down on “rolling bad apples” who avoid consequences by hopping from firm to firm. It means that “serious, substantiated cases of poor personal behaviour” by senior managers at a range of firms including hedge funds, insurers and pension firms will have to be reported to the Financial Conduct Authority (FCA), as well as future employers who are assessing whether new hires are fit and proper for the job. Previously, only banks were required to report bad behaviour to the watchdog. The rules will now apply to tens of thousands of other firms across the City that are bound by the so-called senior managers and certification regime (SM&amp;amp;CR) that is meant to hold senior bosses accountable for wrongdoing at their firms. The regulator said the expanded rules would help “prevent ‘rolling bad apples’ – people moving from firm to firm without appropriate action being taken or without past serious non-financial misconduct being disclosed”. Sarah Pritchard, the FCA’s deputy chief executive, said: “Too often when we see problems in the market, there are cultural failings in firms. Behaviour like bullying or harassment going unchallenged is one of the reddest flags – a culture where this occurs can raise questions about a firm’s decision-making and risk management. “Our new rules will help drive consistency across industry and support the vast majority of firms that want to do the right thing to deepen trust in financial services.” The expanded rules on non-financial misconduct, which also cover racism, sexual harassment and violence and intimidation, will come into force on 1 September 2026. However, they will not apply to payments and e-money firms, regulated investment exchanges or credit ratings agencies, none of which are subject to SM&amp;amp;CR rules. The FCA recently won a tribunal challenge brought by the former Barclays boss Jes Staley, with judges upholding a lifetime ban against the former chief executive for misleading the regulator over the nature of his relationship with the convicted child sexual abuse offender Jeffrey Epstein and their last point of contact. The new rules come despite the FCA and fellow regulators facing mounting pressure from the government to slash red tape for businesses.</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>The Financial Conduct Authority is expanding bullying and harassment rules. Previously, only banks were required to report bad behaviour to the watchdog. The rules will now apply to tens of thousands of other firms across the City.</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Time to wrap up…. The chair of the Federal Reserve, Jerome Powell, has blamed Donald Trump’s tariffs for preventing the immediate interest rate cuts the president has demanded. Trump has repeatedly urged Powell to reduce borrowing costs in the US economy, and on Monday posted a hand-scrawled note on his Truth Social platform saying: “You have cost the USA a fortune – and continue to do so – you should lower the rate by a lot!” But Powell told an event hosted by the European Central Bank (ECB) in Portugal on Tuesday that the Fed was waiting to assess the inflationary impact of the president’s trade policies. Speaking on a panel of central bankers in Sintra, he said: “In effect we went on hold when we saw the size of the tariffs. “Essentially all inflation forecasts for the United States went up materially as a consequence of the tariffs. We didn’t overreact, in fact we didn’t react at all. We’re simply taking some time.” Shortly after Powell’s comments in Sintra, Trump claimed that “anyone” could do a better job as Fed chair. In other news… UK house prices fell in June, as the rise in stamp duty tax deterred buyers The governor of the Bank of England has warned that the UK economy, and the jobs market, are softening – which may clear the way for further cuts to UK interest rates The downturn in UK manufacturing eased last month, but the sector is still shrinking Eurozone inflation has risen to 2% EU trade commissioner Maroš Šefčovič is preparing for crunch talks over tariffs with US trade representative Jamieson Greer Marks &amp;amp; Spencer’s online business should be running “fully” within the next four weeks, its boss has said, as the retailer recovers from a damaging cyber-attack. Over at ‘Alligator Alcatraz’, a detention facility in Florida, Donald Trump has taken another bite at Jerome Powell. Our US Politics Live blog reports that Trump was asked if he intends to announce his pick for the next Fed chair’. In response, the US president gestured to Florida governor Ron DeSantis and US Secretary of Homeland Security Kristi Noem to imply they would both be good candidates, before adding: Anybody would be better than J Powell. He’s costing us a fortune because he keeps the rate way up. There’s an amusing moment at the ECB’s central bank forum, where Christine Lagarde declines to offer any advice to her eventual successor. Lagarde resists, telling the event in Sintra that she remembers being told by her predecessor that “it would be a walk in the park”. Lagarde became ECB president in November 2019, shortly before the Covid-19 pandemic struck the world economy, posing unprecedented challenges for central bankers. Top central bankers in Sintra are also asked what keeps them awake at night. European Central Bank president Christine Lagards says she is worried about “the truth”. Lagarde reveals she is “more and more concerned about the role that artificial intelligence is going to play”, about how things can be distorted, and how public opinion can be manipulated. That extends to fears that the data which the ECB relies on could be changed, she adds, saying: I do have this fear that things can be distorted, and we can fall prey to that. That is of great concern to me. Jerome Powell says that he is kept awake by the challenge of handing on a strong US economy to his successor. Powell explains that he has around 10 months of his term as chair left. All I want, and all anyone at the Fed wants, is to deliver an economy that has price stability, maximum employment, financial stability. What keeps me awake at night is how we get that done, and are we on a path to do that. I want to hand over to my successor an economy in good shape. Korea’s Rhee says he is worried about the perception gap between how fast the economy can grow, and how fast people think it should grow. Andrew Bailey explains that he want to deliver UK inflation sustainably at target. He became chair of the Financial Stability Board (an important watchdog) today, so that creates more vulnerabilities to keep him awake. Federal Reserve chair Jerome Powell also reassured the ECB’s conference today that the Fed isn’t planning to change how it offers dollar liquidity to other centra banks. Powell explained that the Fed’s dollar swap lines are “a big contribution” to global financial stability, and doesn’t plan to change that, saying: “We still have the same authorities, and we’re still prepared to use them in situations where it’s within our legal authorities and where we think it makes sense.” Powell was responding to Bank of Korea Governor Governor Rhee Chang-yong. who noted that countries such as South Korea need to build up dollar reserves in case they are needed. Fed dollar swap lines offer loans to eligible central banks to ensure dollar liquidity is not an issue for the global financial system and have been heavily used in times of crisis. The Financial Times reported last week that central banks are concerned the US could turn off this flow of dollars. Andrew Bailey then calls for policymakers to look at the causes of the problems of the world economy that have led to trade wars and threaten to lead to fragmentation. Christine Lagarde then offers Jerome Powell her support, insisting that all the panel would have acted exactly the same as the Fed chair this year. “Right?” she directs the Bank of Korea’s Rhee Chang Yong, firmly. “Yes,” replies Rhee, who worked under Lagarde at the IMF. Jerome Powell also refuses to respond to the outpouring of criticism from the White House. Bloomberg’s Francine Lacqua, who is moderating today’s session: Q: You get attacked by the president a lot on a personal basis. Does it make your job harder?” Powell insists that he is “very focused on just doing my job”. Sticking to the Fed’s mandate, Powell says: The things that matter are using our tools to achieve the goals that Congress have given us – maximum employment, price stability, financial stability. That’s what we focus on, 100%. At this point, Powell wins a supportive round of applause from the audience in Sintra, and from his fellow panelists – BoE governor Andrew Bailey, ECB president Christine Lagarde, Bank of Japan governor Kazuo Ueda, and Bank of Korea governor Rhee Chang Yong. Asked later if he would remain at the Fed after his term as Chair expires next May, Powell said: “I have nothing for you on that today.” Jerome Powell has also warned that America’s fiscal path is not “sustainable”, even though the current level of debt is sustainable. Andrew Bailey then fends off a cheeky question about how low the Bank of England could cut rates: Q: Will interest rates be closer to 3% or 4% at the end of the easing cycle? BoE governor Bailey says there is huge uncertainty about what the neutral rate of interest (r*) is. The more important thing to realise, Bailey argues, is that UK monetary policy is currently restrictive, and will continue to remain restrictive, but that level of restrictive-ness will come down. Fed chair Jerome Powell weighs in too, saying he thinks US interest rates are “modestly restrictive” at their current levels'; it doesn’t feel that the US economy is suffering from very tight policy. South Korea’s central bank chief fears that an escalation of the Trump trade wars would have a serious impact on its economy. Speaking on the ECB’s panel, alongside Jerome Powell, Rhee Chang-yong explains that global fragmentation has a serious impact on Korea’s economy as it is export-driven. That includes the direct impact of US tariffs, but also indirect impacts through the China, Mexico and Canada. Rhee explains that the Bank of Korea is watching for what happens when Trump’s 90-day tariff pause expires: It really depends what happens on July 9th… We don’t know what’s going to happen. He explains that if Trump reimposes the 26% retaliatory tariff announced on 2 April, added to sectoral tariffs on aluminium, steel, and cars, the impact could easily be more than 1% of Korea’s GDP. Jerome Powell says he can’t say whether the Fed could cut interest rates as soon as this month. It all depends on the data, he insists, adding that the Fed is going ‘meeting by meeting’. Christine Lagarde declines to comment on the strength of the euro, beyond suggesting that it is a reflection on the state of the eurozone economy. She suggests that there are two factors – the depreciation of the US dollar (which had its worst first half to a year since 1973), and an appreciation of the euro. Looking ahead, Jerome Powell says economic data will determine whether US interest rates are cut this year (as Trump has been loudly demanding). Powell explains that “a solid majority” of members of the rate-setting FOMC committee think it will be appropriate to reduce rates later this year (there are still four FOMC meetings scheduled]. But, Powell adds, this will depend on the incoming data, so the Fed will be monitoring the inflation data slowly, as well as the labour market. Kazuo Ueda, governor of the Bank of Japan, resists commenting directly on Donald Trump’s threat to impose more tariffs on Japanese imports. Ueda says the issus is being negotiated by the relevant minister, so he is “yrying to avoid making any specific comments on this.” Trump claimed it was unfair that Japan doesn’t buy US rice (it does, though, as CNN shows here) despite having a massive rice shortage, and hinted the White House will simply sent Toyko a letter laying out the tariffs it will face. Andrew Bailey, governor of the Bank of England, tells the ECB’s forum in Sintra that he is seeing some “softening” in the UK economy and “softening in the labour market”. That means Bailey believes “the direction of UK interest rates continues to be downwards.” Bailey agrees it’s too early to see the price effects from recent action on tariffs; endorsing Jerome Powell’s explanation for not having cut US interest rates this year. The top US central banker has indicated that Donald Trump’s trade war has prevented the cuts to interest rates which the president has been demanding. Jerome Powell, who has been repeatedly criticised by Trump for the Federal Reserve’s failure to cut interest rates this year, has told an audience in Portugal that uncertainty over the impact of Trump’s tariffs prevented the Fed from cutting rates. Powell explains that the US economy is “healthy” and in a good position, with inflation down to 2.3%, core inflation is at 2.7%, and an unemployment rate is 4.2%. Powell explains that “if you ignore tariffs”, inflation is behaving as the Fed expected and hoped. He says: We haven’t seen effects much from tariffs, and we didn’t expect to by now. We’ve always said the timing, amount and persistence of the inflation would be highly uncertain and it’s certainly proved that. We’re watching. We expect to see over the summer some higher readings, but we’re prepared to learn that it can be higher, or lower, or later or sooner than we’d expected. Q: Would the Fed have cut more by now if it wasn’t for the tariffs? Powell replies that “I think that’s right”, before explaining that the Fed is waiting until it knows the impact of the Trump trade war. He explains: In effect we went on hold when we saw the size of the tariffs. Essentially all inflation forecasts for the United States went up materially as a consequence of the tariffs. We didn’t overreact, in fact we didn’t react at all, We’re simply taking some time. Powell concludes by explaining that “the prudent thing to do” is to wait and see the impact of imposing tariffs on US imports, given the US economy is “in solid shape”. Trump has repeatedly accused Powell of being ‘too late’ to cutting rates, pointing out that other major central banks have lowered rates more quickly. The Fed hasn’t cut rates since last December. On Monday, Trump produced a hand-written note showing how US interest rates are much higher than many other countries. Trump wrote that the Fed “should be ashamed of themselves for allowing this to happen to the United States”, and claimed they had “cost the USA a fortune” by not lowering borrowing costs. The session in Sintra begins with Christine Lagarde welcoming this morning’s news that eurozone inflation rose to 2% in June, from 1.9% in May. Lagarde reminds her audience that 2% inflation, in the medium term, is the European Central Bank’s target. I am not saying ‘mission accomplished’, but I say ‘target reached’, OK. The ECB president then warns that “we are facing a lot of uncertainty”, including the risks of fragmentation, and worrying geopolitical developments that are causing a ‘two-sided risk to inflation’. We have to continue to be extremely vigilant, and remain committed to delivering on the inflation target, Lagarde says, insisting: We are well-equipped to navigate the tormented waters that we should anticipate. EU member states have been advised there could be four options emanating from this week crunch talks between trade commissioner Maroš Šefčovič and US trade representative Jamieson Greer over tariffs. One option is no deal but another more likely scenario of the three remaining is a deal in which both signs are aligned “in broad brush strokes” but centre, like the UK’s deal, on a limited number of sectors such as cars and steel. This would leave the threat of future tariffs on other sectors open, risking new crises emerging without warning during the remainder of the Trump term. A third option is a delay, extending talks beyond 9 July. This carries the risk of Donald Trump’s threatened 50% unilateral tariffs being imposed on all imports from the EU from 10 July. And a fourth option is an “imbalanced deal”, the type that would favour the US, something Emmanuel Macron last week said he would not accept. Details of the negotiations were not shared in the 45 minute briefing given by Ursula von der Leyen’s head of cabinet Bjoern Siebart and Sabine Weyand, director general of the trade commission, best known in the UK as Michel Barnier’s right hand woman during Brexit negotiations. EU ambassadors gave also been warned that the 10% blanket tariff may remain but that if they cannot secure a reduction then they will try and extract duty free exemptions in some sectors. A delegation headed by trade adviser Thomas Baert flew to Washington on Monday for technical talks with Šefčovič joining them tomorrow for talks with trade representative Jamieson Greer. He is likely to return to brief member states on Thursday with a possible further of ambassadors meeting on Friday ahead of next week’s deadline. The UK government has just published the timetable for the implementation of its big workers’ rights package, which UK employers will have to get their heads around in the coming months. Some business groups had been lobbying for a longer implementation period, but Labour is keen to press ahead. A new Fair Work Agency, to enforce the rules, will be up and running next year, ministers said. Some changes - such as the repeal of the Tories’ strike-busting minimum service levels legislation, will come into force as soon as the Employment Rights bill gets Royal Assent, expected to be later in the summer. Next April (2026) will mark the end of the two-day wait for statutory sick pay, and stronger protection for whistleblowers; new regulations to set up a fair pay agreement for the social care sector will follow next October. Another slew of changes are expected to come into force in 2027, including new rights to bereavement leave, and day one rights to unfair dismissal. Deputy prime minister Angela Rayner said: “these landmark reforms will kick in within months, demonstrating our commitment to making work pay for millions of workers across the country and delivering real change.” Over in Sintra, Portugal, some of the world’s top central bankers are about to discuss monetary policy and the state of the global economy. The central bank chiefs of the UK, the eurozone, the US, Japan and Korea are all appearing on a panel organised by the European Central Bank, at its Forum on Central Banking 2025. The session is titled: Adapting to change, macroeconomic shifts and policy responses. On the panel, we have: Andrew Bailey, Governor, Bank of England Christine Lagarde, President, European Central Bank Jerome Powell, Chair, Board of Governors of the Federal Reserve System Chang Yong Rhee, Governor, Bank of Korea Kazuo Ueda, Governor, Bank of Japan Elon Musk and Donald Trump are continuing to trade barbs. Trump has told reporters at the White House that he would look into deporting Musk, when asked about the billionaire’s vocal criticism of Trump’s tax and spending legislation. Trump then repeated his threat to unleash the Department of Government Efficency on Musk’s empire, saying: “We might have to put DOGE on Elon. DOGE is the monster that might have to go back and eat Elon. Wouldn’t that be terrible?” In response, Musk has posted enigmatically… So tempting to escalate this. So, so tempting. But I will refrain for now. The row is continuing to hurt Tesla’s shares, they’re now down over 6% in pre-market trading. Speaking of trade deals… US Treasury Secretary Scott Bessent has said America is hopeful China will do more to ease the export of rare earth magnets after last month’s deal between the two countries. Bessent told Fox News that flows had still not returned to levels seen in early April, despite the agreement which the two sides hammered out in London last month. Bessent said: “We are hoping that they will flow at a faster rate. “Rare earth magnets are flowing. They are not flowing as they did before April 4, but we are confident that the Chinese will live up to their side of the deal.” Here’s Susannah Streeter, head of money and markets at Hargreaves Lansdown, on M&amp;amp;S’s recovery from its cyber-attack: “Marks and Spencer is halfway there, but there’s still a lot to get back online before the company can put the cyber attack behind it. 50% of online operations are back up and running, but its popular click and collect services remain suspended. At the company’s AGM, CEO Stuart Machin put the latest timeline on a recovery at four weeks. This should mean the retailer will hit August firing on all cylinders once again. Management have previously estimated that it could cost as much as £300 million in lost sales and operational disruption, although it’s likely that this will be mitigated by insurance claims and cost efficiencies made elsewhere. While services have been suspended the company is believed to have used the opportunity to speed up part of its digital transformation plan, as well as ensuring that its IT systems are robust enough to withstand a future attack. “There will be high hopes that M&amp;amp;S can put this unfortunate chapter behind it, and the early signs are that there is pent up demand, particularly for its summer styles, with many of the popular products sold out online. Its strong set of annual results showed the retailer was in a resilient position before the cyber attackers infiltrated systems. Sales growth in the fashion and home &amp;amp; beauty division reflected improved customer perceptions of value, quality, and style. Demand for M&amp;amp;S food remains robust, with increased volumes driving growth. So, with the underlying performance remaining solid, it bodes well for M&amp;amp;S ahead, but until everything’s back up and running, it’s likely to weigh on investor sentiment. Although shares have been in positive territory today, they remain around 13% lower than the level in mid-April, before the cyber attack took hold.’’ European trade commissioner Maroš Šefčovič will travel to Washington tomorrow hoping to strike a tariff agreement in principle with Donald Trump’s team, my colleague Lisa O’Carroll reports from Brussels. He will meet trade representative Jamieson Greer with hopes rising they will have enough in the coming days to agree the basics ahead of 4 July Independence Day negotiations. At the same time they recognise the volatility on the US side and are working to avert any further threats of tariffs that Trump may like to announce to extract more concessions from the EU. He recently warned tariffs on pharma were coming “very soon”. If an agreement in principle is struck, talks would then continue, possibly beyond 9 July to work out the detail. This would follow the pattern in the UK which took more than a month to get to a final text. Yesterday Šefčovič revealed it was a good time get down to “drafting” an agreement and “drafts of proposals for the eventual agreement in principle”, a significant change of language which suggests they close to settling differences on major issues. EU sources confirm the European Commission is now putting all its efforts into a “quick deal” rather than hold out for a deep and wide one covering up to 1,000 product lines. This follows criticism by German chancellor Friedrich Merz last week that the EU was too complicated. Germany’s priority is get the 27.5% tariffs reduced or eliminated on car exports and the same for steel exports which are facing 25% tariffs. The Baltic states, in particular, area also keen to build on the humouring of Donald Trump at last week’s NATO summit and want to ensure everything is done to keep him on board with weapons supply in Ukraine. Sources say the EU is more or less resigned to a 10% blanket tariff on exports to the US remaining and may offer more imports on semi-conductors to sweeten the deal. However there remain worries that Trump could yet announce tariff on pharma exports as part of his negotiation tactics to extract more from the EU. An EU technical delegation flew to Washington on Monday, ahead of Šefčovič ’s visit with expected meetings with commerce secretary Howard Lutnick, who looks after sectoral deals, and with Greer. With the clock ticking down towards Trump’s self-imposed deadline for a deal of 9 July, there is still plenty of room for a change of mood in the Oval Office. Overnight Trump expressed frustration over Japan trade negotiations on Monday with treasury secretary Scott Bessent warning that countries could be notified of sharply higher tariffs as a July 9 deadline approaches despite good-faith negotiations. Speaking on Monday in Brussels, Šefčovič said “The 9th of July is around the corner. So for me, it’s always a good sign when we kind of move from, I would say, exchange of views, into the drafting process.” “As you know, we received first drafts of proposals for the for the eventual agreement in principle we are working on that,” he told reporters in Brussels. He added the EU was pushing for a deal that “was fair for both sides”. UK retailer Marks &amp;amp; Spencer is optimistic that the worst of its recent cyber attack will be behind it by August. M&amp;amp;S’s chief executive Stuart Machin told shareholders at the retailer’s annual general meeting today that the company Machin explained that the half of M&amp;amp;S’s online store which is not yet open – including its click and collect service – will be fully restored within the next four weeks, and other systems which are currently being rebuilt will be operating by August. He told shareholders: “I have previously highlighted that it would take all of June and all of July, maybe into August but definitely by July. “During the incident we chose to shut things down because we didn’t want the risk of things going wrong. “Currently, half of online is open but not areas like click and collect. Within the next four weeks we are hoping for the whole of online to be fully on. “Then our focus will be getting the Donington site back and running. We’re hoping that by August we will have the vast majority of this behind us and people can see the true M&amp;amp;S.” Last month Marks &amp;amp; Spencer reopened its website to shoppers, six weeks after it was forced to halt online orders after the cyber-attack. Shares in Tesla are set to fall when Wall Street opens, after relation between CEO Elon Musk and US president Donald Trump deteriorated. Tesla’s shares are down 4.5% in pre-market trading. Over the weekend, Musk claimed that Trump’s tax and spending bill was “utterly insane and destructive,” claiming the latest draft of the bill would destroy millions of jobs in America and cause immense strategic harm. Musk also claimed: “It gives handouts to industries of the past while severely damaging industries of the future.” Musk later vowed to unseat lawmakers who support the budget bill: Trump has now hit back, threatening to clamp down on the government subsidies received by Musk’s businesses using The Department of Government Efficiency department which the billionaire used to helm. Trump posted on his Truth Social site: Elon Musk knew, long before he so strongly Endorsed me for President, that I was strongly against the EV Mandate. It is ridiculous, and was always a major part of my campaign. Electric cars are fine, but not everyone should be forced to own one. Elon may get more subsidy than any human being in history, by far, and without subsidies, Elon would probably have to close up shop and head back home to South Africa. No more Rocket launches, Satellites, or Electric Car Production, and our Country would save a FORTUNE. Perhaps we should have DOGE take a good, hard, look at this? BIG MONEY TO BE SAVED!!! The London has moved gingerly into the second half of the year. The FTSE 100 index of blue-chip shares has dropped by 17 points, or 0.2%, to 8743 points. Mining stocks are leading the risers, reflecting optimism that the US may agree more trade deals soon. But housing stocks, and banks, are among the fallers following this morning’s news that UK house prices fell by 0.8% in June. The small pick-up in eurozone inflation last month makes it likely the ECB will leave interest rates on hold at its meeting later this month. Richard Flax, chief investment officer at Moneyfarm, says policymakers will be worried that energy prices could pick up again. Eurozone inflation rose slightly from 1.9% in May to 2.0% YoY in June, aligning with the ECB’s target. The increase was driven by higher energy costs and persistent service sector inflation, which continues to be the main source of upward pressure. Core inflation is expected to remain unchanged, suggesting that underlying price dynamics are stable for now. Energy markets remain a key risk. Prices surged in June due to geopolitical tensions, though a recent ceasefire in the Middle East has helped ease some of the pressure. Still, the potential for renewed volatility could complicate the inflation outlook in the months ahead. With inflation near target and no major surprises in core data, the ECB is expected to hold rates steady at its July meeting. Markets are looking to September for the next potential move, depending on how inflation evolves. Diego Iscaro, head of European economics at S&amp;amp;P Global Market Intelligence, also sees a September cut as more likely: “Inflation edged upwards in June, just as markets expected. The modest increase in inflation is not particularly worrying, given it was mainly driven by a lower fall in energy prices, but the somewhat stronger rise in service price inflation will not be welcome news. “We do not think June’s inflation print will give ammunition to either doves or hawks on the ECB’s governing council. With trade policy-related uncertainty still clouding the picture, there is a risk that the economic outlook may look quite different when the ECB meets later this month. We still expect interest rates to remain unchanged this month, but we see the door opening for a last 25bp cut in September as subdued activity and a stronger euro push underlying inflationary pressures down.” Newsflash: Inflation across the eurozone has risen back to target. Consumer price across the euro area rose by 2.0% in the year to June, statistics body Eurostat reports, up from 1.9% in May. That means inflation is back to the European Central Bank’s 2% target. The increase was partly due to changes in energy prices. Energy inflation rose to -2.7% in June, up from -3.6% in May, following the increase in oil prices last month driven by the crisis in the Middle East. Service sector inflation rose to 3.3%, up from 3.2%, while food, alcohol &amp;amp; tobacco inflatoin dipped to 3.1%, fromh 3.2% in May. Goods inflation slowed to 0.5%, from 0.6% in May. During his interview with CNBC, Andrew Bailey also warned that UK companies are delaying investments due to economic uncertainty. He says: “That increase in uncertainty and predictability is definitely coming through in terms of activity and growth. “When I go around the country talking to businesses, which I do a lot, what they tell me is that they are putting off investment decisions.” The downturn in UK manufacturing has eased last month, new data shows, as output, new orders and employment fell at slower rates than in May. The latest survey of purchasing managers at British factories has also found that business optimism improved to a four-month high in June. This lifted the UK manufacturing PMI to 47.7 in June, its highest reading in five months, but still below the 50-point level separating expansion from contraction. The report found that manufacturers cut output due to weak market conditions, lower demand from clients, trade war uncertainty and geopolitical tensions. Tariffs continued to hit demand, and client confidence, with new export business falling for the forty-first month in a row amid reports of reduced demand from the US, Europe and China, S&amp;amp;P Global says. Manufacturers also cut jobs, for the eighth month running, with the steepest reductions at large-scale producers, despite the UK securing its trade deal with the US last month. Rob Dobson, director at S&amp;amp;P Global Market Intelligence, says: “Although the downturn in UK manufacturing continued in June, the latest PMI survey provides signs of conditions stabilising. Production, new orders and employment all fell at slower rates, while business optimism picked up to a four-month high. The orders-to-inventory ratio, a reliable bellwether of future production trends, also climbed sharply to its highest since August 2024. Inflation of both input costs and selling prices meanwhile nudged lower to hint at a softening inflation trend. “That said, any hoped for stabilisation remains fragile and subject to potential headwinds that could severely impact demand, supply chain reliability and future growth prospects, as manufacturers continue to caution their optimism with concerns about heightened geopolitical tensions, weak global markets, tariff uncertainties and fears over the direction of future government policy.” Sainsbury’s has recorded its strongest growth since last summer after its Argos chain recorded a big step up in sales as shoppers sought out paddling pools and fans during recent hot weather. The retail group said Argos, its catalogue shop, was able to achieve growth of 4.4% in the three months to 21 June, up from 1.9% in the previous quarter. Comparable group sales, excluding fuel, rose 4.7% on a year earlier. The group’s total sales rose 4.9%, helped by the strong trading at Argos and a rise in clothing sales as shoppers snapped up shorts and swimsuits, as well as healthy demand for its premium food ranges. That excludes fuel, where sales fell partly because of price decreases. The retailer said it had achieved the strong sales despite a “subdued, highly competitive and deflationary general merchandise market” as it booked rapid growth in online sales and via its app. Sales in stores declined, partly because of further closures as many Argos sites move from high streets into Sainsbury’s supermarkets. Over in the eurozone, the manufacturing sector has shrunk again but at a slower rate. Data provider S&amp;amp;P Global has reported that its eurozone manufacturing PMI has risen to 49.5, up from 49.4 in May. That’s a 34-month high, but still below the 50-point mark that shows stagnation. Dr. Cyrus de la Rubia, chief economist at Hamburg Commercial Bank, reports that there are signs of stabilization in Europe’s manufacturing sector. Companies have now expanded production slightly for the fourth month in a row, order intake has ceased to fall, and slightly longer delivery times also indicate that demand is picking up a bit. Against the backdrop of numerous uncertainties - US tariffs, the crisis in the Middle East, and Russia’s ongoing war against Ukraine - this can certainly be seen as a sign of resilience. However, it also has to do with the fact that, after years of recession, the economic cycle usually turns at some point because old machines need to be replaced, cars can no longer be repaired, and the necessary modernization of factory buildings can’t be postponed any further. Bank of Engla</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Jerome Powell says the Fed is waiting to assess the inflationary impact of the president’s trade policies. Trump claims that “anyone” could do a better job as Fed chair. Christine Lagarde declines to offer any advice to her eventual successor.</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>A wage increase for low-paid workers, changes to superannuation and significant reforms to the pension are part of sweeping changes being made on 1 July. The end of the financial year is typically when state and federal governments change a range of legislation, implementing new policies. This year there is a lot happening so let’s take a look at the big-ticket items. Minimum wage rise Good news for those on the bottom income line, the minimum wage will increase by 3.5%, to $948 per week or $24.95 per hour, based on a 38-hour work week. The changes are expected to impact 2.6 million and will apply from the first full pay after July 1. Superannuation guarantee increases The minimum amount of superannuation employers must contribute is also set to rise from 11.5% to 12%. This will be the final increase in a five-year series of rises to the amount employers have to pay and will mean a 30-year-old earning $100,000 will have an additional $125,000 when they retire. In addition to cutting 20% off student loan debts for 3 million Australians, the government will also increase the amount that people can earn before they are required to start paying back their loans to $67,000, subject to the passage of legislation. Changes to the NDIS The national disability insurance scheme will introduce a number of changes from 1 July as part of its annual pricing review. The changes will mean that the maximum rates providers can charge some NDIS participants will be lowered after the review found some limits were “inflated” or “out of step with broader market rates”. For example, physiotherapy sessions have been reduced by $10 to $183.99 per hour. Maximum rates will also be made nationally consistent meaning some providers in jurisdictions will be increased – prices for psychology sessions have been standardised at $223.99 across all states and territories. Other changes will include removing an establishment fee providers once charged participants for setting up their services. Sector advocacy groups have criticised the changes, warning they will result in fewer services being available for participants in regional and rural areas. In brighter news, disability support workers will get a 3.95% pay boost from July. Aged pension rate increases The pension rate is not going up but increased income and asset thresholds mean thousands more will be entitled to benefits and bigger payments. From 1 July the thresholds will be adjusted to better keep up with inflation, with every couple who are asset-tested getting a $34.50 fortnight increase, with singles getting $22.50. The asset cut-off point when the pension starts to be reduced has also been increased from $470,000 for couples and $314,000 for singles to $481,500 per couple and $321,500 for singles. Centrelink indexation Around 2.4 million Centrelink recipients will also see a small increase to their payments, as the regular indexation is applied to their income. This means that payments and thresholds will increase by 2.4%. While any increase to the bottom line will be welcomed by those on the payments, advocates routinely say the high cost of living, including soaring rent, far outpaces the extra money. Better parental leave There is good news for parents and carers born in the new financial year with the number of paid parental leave (PPL) paydays lifting from 110 to 120, or 24 weeks. Parents will be able to claim the leave up to three months before their child “enters their care”. This is a series of increases to the scheme which will see it progressively expand until it hits 26 weeks by 2026. Changes to road rules AI-powered surveillance cameras, that will be able to detect when drivers are holding or using their mobile phones, will now be used across the country. There are also state-based changes. In NSW, for example, there will be harsher penalties if someone is found not wearing a seatbelt, as fines rise in line with the CPI increase of 3.2%. The state will start trialling average speed cameras for cars and motorcycles in two locations. In Queensland, speed limits will be reduced in selected areas and traffic fines will increase by 3.5%. Drivers in Victoria will now have to slow to 40kmh when passing roadside assistance vehicles, tow trucks or emergency response vehicles that are flashing their lights. In South Australia, this will be lowered to 25kmh on some roads. Drivers in Western Australia will now face fines up to $700 for mobile phone use and over $1,600 for excessive speeding. Cheaper home batteries program Households that are looking to install battery systems will be in a better position as the cheaper home batteries program offering a 30% discount on the purchase and installation kicks in. Paid practical placements Paid practical placements will start for some tertiary students studying teaching, nursing, midwifery, and social work. Eligible students will be able to access $319.50 per week while they’re undertaking a placement. Cystic fibrosis drug price slashed Affordable access to life-changing treatment for cystic fibrosis will be expanded to more Australians with a change to the Pharmaceutical Benefits Scheme. People living with rarer types of cystic fibrosis will pay a fraction of the price to access life-changing treatment under an expansion of the scheme. People will now pay a maximum of $31.60 per script, or $7.70 if they hold a concession card. • This article was amended on 30 June 2025. An earlier version said that the asset cut-off point had been decreased from $481,500 to $470,000 for couples, and from $321,500 to $314,000 for singles. In fact it has been increased from $470,000 to $481,500 for couples, and from $314,000 to $321,500 for singles.</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>The minimum wage will increase by 3.5%, to $948 per week or $24.95 per hour. The minimum amount of superannuation employers must contribute is also set to rise from 11.5% to 12%. This will be the final increase in a five-year series of rises to the amount employers have to pay. A 30-year-old earning $100,000 will have an additional $125,000 when they retire.</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>Time to wrap up…. US stock markets have hit record highs after America reached an agreement with China to speed up rare-earth shipments. The S&amp;amp;P 500 index, and the Nasdaq, both hit new peaks amid news of wider efforts to end the trade wars between the US and the world’s biggest economies. Donald Trump said on Thursday that the US had signed a deal with China the previous day, without providing additional details, and that there might be a separate deal coming up that would “open up” India. China confirmed the details of the deal on Friday, and reiterated that it will continue to approve the export permits of controlled items. European markets also rose, with the FTSE 100 closing at its highest level in over a week. Asia-Pacific markets hit three-year highs. There were signs that the trade war has hurt the UK auto sector, with shipments to the US halving in May. Nike has said it expects costs to increase by about $1bn (£728m) as a result of Donald Trump’s tariff war as the sportswear company looks to reduce its manufacturing in China. The European pharmaceutical industry has urged Brussels not to retaliate if Donald Trump brings in threatened tariffs on imported drugs, amid fears he could impose the levies as early as next week. There was relief in London after the US announced it plans to drop the ‘revenge tax’ section of Donald Trump’s new tax and spending bill. In other news… An increase in demand for weight loss drugs, including Mounjaro and Wegovy, as well as demand among its generation Alpha customer base for beauty products is driving expansion at Superdrug. Barclays and its former chief executive Jes Staley are facing a class action lawsuit in the US over claims they defrauded and misled investors over Staley’s relationship with the child sex offender Jeffrey Epstein. The police criminal inquiry into the Post Office Horizon IT scandal is investigating more than 45 individuals, with seven formally identified as main suspects. London’s stock market has ended the day at its highest closing level in over a week. The FTSE 100 index of blue-chip shares has closed 63 points higher at 8799 points, up 0.7% today. That’s its highest close since 18 June. Hopes that the US and EU will reach some form of a trade agreement before the 9 July deadline expires are also lifting markets. Bloomberg reports that European Commission President Ursula von der Leyen told EU leaders at a summit yesterday that she was confident a deal could be reached before the deadline to avoid an economically damaging escalation, according to people familiar with the matter. The boss of Barclays bank has welcomed the news that the White House wants to drop the ‘revenge taxes’ proposal, Section 899, from Donald Trump’s tax and spending bill. Barclays CEO C.S. Venkatakrishnan told Reuters: “The developments on 899 are welcome progress and a significant outcome for a great many UK companies like Barclays that invest in the US and support economic growth in both countries.” The Nasdaq is on track to enter a new bull market today, Reuters reports, adding: The tech-heavy index was last up 0.4% at 20,243 points, surpassing its record high of 20,204 on December 16. It had tumbled 26.8% from its previous peak, marking a bear market days after Trump’s “Liberation Day” reciprocal tariffs on April 2. Sportswear brand Nike are the top riser on the S&amp;amp;P 500 in early trading. Nike’s shares have jumped 15%, driven by hopes that its turnaround plan may be working, despite the company reporting a drop in profits for the last quarter yesterday. As reported earlier, Nike told analysts last night that the US tariffs on Chinese-made goods will cost it $1bn, and it plans to take steps including moving manufacturing out of China. Elior Manier, market analyst at OANDA’s MarketPulse, says the US-China trade deal breakthrough announced overnight has lifted markets. Stocks have also rallied through the week, on relief that the Israel-Iran ceasefire has held. Manier writes that stock markets have been “on a frenzy” this week, adding: “Markets are awaiting and getting a few good news on the US trade deals – The latest is the White House announcing that the July 9 is in the end not too important, and Trump mentioning the completion of a Deal with China, however the details are still missing. “Taking a step back to the daily chart highlights just how volatile equities have been in the first half of 2025. “One of the key emerging themes is the market’s increasingly muted reaction to Trump-related developments — especially now that the Israel-Iran conflict is fading from the headlines. Boom! America’s stock market has hit a new record high, as hopes of trade deal progress lift shares. The S&amp;amp;P 500 has just touched an intraday record high at the start of trading in New York. It gained 0.2% to 6,153.55 points, surpassing the previous peak set in mid-February. This milestone underlines that the markets have recovered from their slump in early April, when Donald Trump’s trade wars sparked a heavy selloff (before recovering when the president delayed his tariffs for 9o days). The tech-focused Nasdaq index has also hit a new record high, as optimism around artificial intelligence and hopes of interest rate cuts lifted technology stocks. The overnight comments from US commerce secretary Howard Lutnick, who said the White House has imminent plans to reach agreements with a set of 10 major trading partners, may be cheering Wall Street today. The future of UK bank TSB is growing closer to being resolved. Santander and Barclays are the main contenders left in the race to acquire TSB from its current owner, Sabadell, Bloomberg reports. The two banks are said to be the only ones in the data room, analysing a possible bid. Earlier this month, Sabadell said it has received interest from prospective buyers. The 0.4% decline in nominal US incomes last month “is not quite as bad as it looks”, reports Harry Chambers, assistant economist at Capital Economics, who tells clients: It was mainly due to a drop back in social security payments, which were boosted in April by changes in the Social Security Fairness Act. Chambers also points out that the 0.1% drop in consumer spending was due to a “huge drag from spending on motor vehicles and parts”. Just in: US personal incomes fell last month, just as the Federal Reserve’s preferred inflation measure rose. Personal income decreased by 0.4% in May, according to estimates released today by the US Bureau of Economic Analysis. This data measures the income which Americans receive from wages and salaries, Social Security and other government benefits, dividends and interest, business ownership, and other sources. Personal consumption, a measure of spending, dipped by 0.1% in the month. The BEA also reported that the PCE price index rose by 2.3% in the year to May, up from 2.2% in April. Core PCE inflation (which strips out food and energy) rose to 2.7% from 2.6%. This combination of falling incomes, weakening spending and rising prices may alarm the Fed, which is under pressure from Donald Trump to cut interest rates despite its concerns about inflation. China’s central bank has warned that its economy still faces “difficulties and challenges” such as weak domestic demand and persistently low inflation. In a statement following its quarterly monetary policy meeting, the People’s Bank of China (PBOC) also points to global challenges, saying: “The external environment has grown increasingly complex and challenging, with weakening momentum in global economic growth, rising trade barriers, and diverging economic performance among major economies.” Heathrow Airport has warned that the US travel market is becoming “more challenging”, dut to rising economic uncertainty across North America. In its latest investor report, released this morning, Heathrow says it is seeing “some early signs of softness on business-heavy routes”, a trend that appears linked to economic uncertainty than geopolitical reasons. Heathrow cautions: Transatlantic travel remains a core strength in our network however, we acknowledge the overhanging uncertainty in this market and we continue to monitor airline and passenger behaviour closely as the summer progresses. There’s relief today that the White House are dropping Donald Trump’s ‘revenge tax’, which could have hurt UK businesses. Last night, US treasury secretary Scott Bessent announced he was asking Congress to remove the Section 899 protective measure from Trump’s “One, Big, Beautiful Bill”, which is currently being debated. Section 899 would have allowed the US to impose retaliatory taxes on any company from a country that imposed unfair taxes on US companies. This could have hurt many FTSE 100 companies who have significant operations across the Atlantic. Bessent says the US has reached an agreement with the G20 that US companies will not be subject to the new OECD global minimum tax regime. He says: OECD Pillar 2 taxes will not apply to U.S. companies, and we will work cooperatively to implement this agreement across the OECD-G20 Inclusive Framework in coming weeks and months. Pillar 2 set a minimum global tax rate of 15%, and was designed to ensure large multinational enterprises pay a minimum level of tax on the income arising in each jurisdiction where they operate. The Section 899 breakthrough follows talks between the UK government and the Trump administration about exempting British companies from these “revenge taxes”. An HM Treasury spokesperson says: “The removal of Section 899 is welcome news for British businesses and comes after the Chancellor raised concerns directly with her G7 counterparts on behalf of those businesses. “This work will continue with global partners to ensure the international tax system provides a level-playing field, while combatting aggressive tax planning and avoidance.” Rachel Reeves has welcomed Bessent’s “important action”, adding: Look forward to further work with global partners to ensure a level playing field on tax. We are breaking down barriers and delivering in Britain’s national interest. After hitting its lowest levels since 2022 yesterday, the US dollar has not really taken much comfort from today’s trade deal optimism. The dollar is up just 0.08% against a basket of currencies. Raffi Boyadjian, lead market analyst at Trading Point, explains: The US dollar hovered near three-year lows at the start of European trading on Friday, putting its index against a basket of currencies on course for weekly losses of 1.5%. The receding crisis in the Middle East that had rekindled the US currency’s safe-haven appeal, combined with growing expectations of more than two Fed rate cuts this year have scuppered the dollar’s recovery prospects. Not even the headlines overnight about the White House finalizing the trade truce agreement with China and plans for 10 new deals have been able to inject much life into the flagging greenback. As things stand, the dollar, at best, is only able to halt the selloff, with a little help from some not-so-bad data. Trade deal optimism has pushed up shares in European carmakers too. Porsche (+2.7%), Daimler Trucks (+2.5%) and BMW (+2%) are among the risers on Germany’s stock market this morning. This has helped to lift Europe’s Stoxx Automobiles and Parts index by around 2% this morning. Stocks are rallying in London this morning. The FTSE 100 blue-chip index has gained 50 points, or 0.55%, to 8785 points, with banks among the risers. The smaller FTSE 250 index of medium-sized companies is up 0.65%, to a 10-month high. Neil Wilson, UK investor strategist at Saxo Markets, says the market mood today is very much optimistic. Markets are ignoring the noise – looking ahead to rate cuts from the Fed, fiscal stimulus in Europe, deregulation for banks on Wall Street, lower inflation and trade deals – hardly the negative environment everyone has been shouting about. But watch out for July 9th [when Donald Trump’s 90-day tariff pause expires]. And the big beautiful tax bill, on which a vote could happen this weekend...is that going to be dollar-negative but lift animal spirits? Czech billionaire Daniel Křetínský has been appointed chairman of Royal Mail, after his EP Group completed its £3.6bn takeover of the company. EP Group also announced it has issued a golden share to the UK Government, as agreed under the deal. That golden share should give the government the power to block the movement of Royal Mail’s headquarters abroad, of a shift in where the company pays its taxes. Křetínský’s appointment comes a week after the chief executive of Royal Mail left after just over a year in post, as the Guardian reported last Friday, Sportswear brand Nike has estimated that the US tariffs on Chinese imports will add $1bn to its costs, and warned that its industry is facing geopolitical volatility and tariff uncertainty. It revealed the figure on a call with analysts last night, calling these tariffs “a new and meaningful cost headwind”. Nike intends to respond by shifting some production out of China. Currently, 16% of its imports into the US are made at Chinese factories; it intends to cut this to single figures by the end of the 2026 financial year. Nike is also raising US prices, and will consider internal cost-cutting too. The company reported a 12% drop in revenues in the last quarter, but shares jumped in after-hours trading on hopes that its turnaround plan is starting to work. Mamta Valechha, consumer discretionary analyst at Quilter Cheviot, explains: “Nike continues to slump, with its fourth quarter the worst in at least two decades. Sales were down 12%, while its operating margin was a meagre 2.9%. The sales themselves had actually come in ahead of really low expectations, producing an earnings beat. “These troubling numbers, though, suggest that Nike may nearly be at rock bottom. The share price rallied strongly in after market trading as investors are beginning to expect a positive rate of change going forward. It has been a difficult period for Nike following the pandemic, and the threat of tariffs simply is not helping the situation for the company. UK car production has slumped to a 76-year low, as Donald Trump’s trade war hurt the British auto industry. Shipments to the US fell by 55.4% last month, according to new data from the Society of Motor Manufacturers and Traders. The SMMT says: This was primarily due to the imposition by the US administration of a supplementary 25% Section 232 tariffs on cars from March which depressed demand instantly forcing many manufacturers to stop shipments. However, with the trade agreement negotiated by government due to come into effect before the end of June, this should hopefully be a short-lived constraint. There was weakness elsewhere too, though. Shipments to the EU fell by 22.5%, while output for the UK domestic market tumbled by 42%. Overall, UK car and commercial vehicle production fell by 32.8% in May. That’s the lowest performance for the month since 1949, if you exclude 2020, when Covid lockdowns forced factories to shut or cut capacity. Data overnight has indicated the US trade war hurt earnings at China’s factories this year. China’s industrial profits plunged 9.1% in May, compared with a year earlier, and have fallen by 1.1% in the first five months of the year, according to the National Bureau of Statistics (NBS). NBS statistician Yu Weining attributed the fall to: “insufficient effective demand, declining prices of industrial products and fluctuations in short-term factors.” China has said it has further confirmed details of a trade framework with the US in recent days, Bloomberg reports. A spokesperson for the Chinese Commerce Ministry made the announcement in a statement today, while reiterating that it will continue to approve export permits of controlled items. In the statement, the Chinese Commerce Ministry said Beijing will “review and approve eligible applications for export of controlled items in accordance with the law,” and the US side will cancel restrictive measures, which it didn’t specify. Shares across Asia-Pacific markets have hit their highest level in more than three years today, as optimism builds in the markets. MSCI’s broadest index of Asia-Pacific shares outside Japan has climbed to its highest level since November 2021. The rally was driven by strong gains in Japan, where the Nikkei 225 index jumped by 1.4%. The yen, typically a safe-haven, weakened amid hopes for progress in tariff negotiations between the US and other countries. China’s markets were mixed, though, with the CSI300 index dipping by 0.5%. Jim Reid, market strategist at Deutsche Bank, suggests markets are in a ‘sweet spot’: The continued positive momentum in equities was impressive. We seem to be in a sweet spot post Middle Eastern calm and pre the July 9th reciprocal tariff extension deadline. This will start to come into view soon, and headlines are starting to bubble up. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Hopes are building that the US may be close to announcing more trade deals, and avoid imposing punishing new tariffs that would disrupt the global economy. Overnight, Donald Trump announced that China and the US had signed a deal, without providing details, declaring: “We just signed with China yesterday.” It later emerged that the agreement will expedite rare earth shipments to the US, building on the progress negotiators made in Switzerland last month. A White House official explained: “The administration and China agreed to an additional understanding for a framework to implement the Geneva agreement……how we can implement expediting rare earths shipments to the US again.” The US, and its trading partners, have less than two weeks until Trump’s 90-day trade war pause expires. US Commerce Secretary Howard Lutnick has claimed that progress is being made, and hinted that the White House has imminent plans to reach agreements with 10 major trading partners. Lutnick told Bloomberg Television: “We’re going to do top 10 deals, put them in the right category, and then these other countries will fit behind.” Trump has previously indicated he could send letters to countries announcing their new tariff rates, if deals aren’t agreed in time. Lutnick has indicated that countries will be sorted into “proper buckets” on 9 July, although there might be flexibility for further negotiations…. He says: “Those who have deals will have deals, and everybody else that is negotiating with us, they’ll get a response from us and then they’ll go into that package. If people want to come back and negotiate further, they’re entitled to, but that tariff rate will be set and off we’ll go.” The agenda 10am BST: EU consumer and business confidence stats 1.30pm BST: US PCE inflation report for May 3pm BST: University of Michigan’s US consumer confidence index</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B29" t="inlineStr">
         <is>
           <t>S&amp;amp;P 500 index, and the Nasdaq, both hit new peaks. European markets also rose, with the FTSE 100 closing at its highest level in over a week. There was relief in London after the US announced it plans to drop the ‘revenge tax’ section of Donald Trump’s new tax and spending bill.</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Economic and Market Volatility</t>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Movement of oil tankers in the Strait of Hormuz remains largely unchanged despite the US attack on Iran over the weekend and the treat of closing the channel, critical to the world’s energy supplies. The Joint Maritime Information Centre which issues daily alerts to the shipping industry in the region based on naval information, said the threat level was “elevated” with “severe consequences for shipping” the the Iranian parliament’s threat to close the Strait is carried out. In Monday afternoon’s alert it said there were “persistently higher levels of electronic interference” from the southern Iranian port of Bandar Abbas and in the Arabian Gulf which “seems to be excessively affected”. It noted that 67 vessels travelled eastward on Sunday and 50 westward, higher than the June average of 114 vessels daily sailing through the Strait but consistent wth last Monday’s traffic of 65 vessels heading out of the Arabian Gulf and 53 vessels entering. Time to wrap up… The financial markets have reacted pretty calmly to the US attacks on Iran’s nuclear facilities. Although oil did spike by 5% when trading began today, that jump quickly unwound. Indeed, crude oil prices are now down around 1% today, after US president Donald Trump called for cheaper prices, saying: EVERYONE, KEEP OIL PRICES DOWN. I’M WATCHING! YOU’RE PLAYING RIGHT INTO THE HANDS OF THE ENEMY. DON’T DO IT! Trump also stepped up his call for the US to increase its oil production, writing: “To the Department of Energy: DRILL, BABY, DRILL!!!” And I mean NOW!!!” Economists have warned that oil prices could jump if supplies from the gulf region were disruped. Goldman Sachs estimated that disruptions to shipping through the strait of Hormuz could push the price of Brent crude over $100 per barrel, up from $76 per barrel today. Jim Reid of Deutsche Bank warned that maintaining the accessibility of the Strait of Hormuz is “pivotal to the global economic outlook”, explaining: Despite being just 21 nautical miles wide at its broadest point, the strait handles a significant share of Middle Eastern oil exports. It features two narrow 2-mile-wide shipping lanes, separated by a 2-mile buffer zone. The head of the International Monetary Fund warned that US strikes on Iran could damage global economic growth. Director Kristalina Georgieva told Bloomberg TV that the IMF was watching energy prices closely, warning a rise in oil prices could have a ripple effect throughout the global economy. She explained: “There could be secondary and tertiary impacts. Let’s say there is more turbulence that goes into hitting growth prospects in large economies – then you have a trigger impact of downward revisions in prospects for global growth.” Wall Street is up in morning trading, as investors in New York digest the latest developments in the Middle East. The Dow Jones industrial average has gained 125 points, or 0.3%, to 42,331 points. The broader S&amp;amp;P 500 index is up 0.5%, led by Tesla whose shares have surged 9% after it launched its robotaxi service in Austin, Texas. The oil price has fallen, since president Trump issued his call for cheaper oil. Brent crude is now down 1.1% today at $76.13 per barrel. Fawad Razaqzada, market analyst at City Index, says “all eyes” are on how Tehran responds to the US bombing attack on its nuclear facilities, adding: Thus far, Iran’s has not responded in a meaningful way, but that could shift at any moment. Should Iran escalate—whether through direct strikes on US assets, attacks by proxies like Hezbollah, or sabotage of oil infrastructure in the Gulf—the market will react swiftly. The Strait of Hormuz is the wildcard. Roughly 20% of the world’s oil passes through this narrow choke point daily. Iran’s parliament has signalled its intent to close the strait in response to US actions, though the final decision rests with the national security council. A full blockade would hurt Iran as well, given its dependency on crude exports to Asia—but asymmetric attacks on ships or terminals remain a very real possibility. The current price moves, then, are best seen as a risk premium. There’s been no disruption to supply—yet. But the market knows all too well how quickly that could change. Elsewhere in the energy sector, the hot weather is hampering output at a nuclear power plant near Lyon. High water temperatures on the Rhone river in eastern France are expected to affect electricity production at the 2.6 gigawatt (GW) Saint-Alban nuclear plant from 1 July, nuclear operator EDF said in a notice on Monday. This is the second notice for high river temperatures after the Bugey nuclear plant was flagged last week, Reuters points out. Nuclear stations use a large amount of water to cool their systems, which they return back to rivers, lakes or the sea afterwards. Problems occur when the water intake is too warm to cool the plant, and when the hot water being returned to the river or sea kills fish and other wildlife. Donald Trump is also urging America’s energy department to encourage more oil and gas extraction across the US (a familiar Trump mantra). He posts: To The Department of Energy: DRILL, BABY, DRILL!!! And I mean NOW!!! Fresh from launching his bombing attack at Iran, president Donald Trump has urged ‘everyone’ to keep oil prices down. Posting on his Truth Social site a moment ago, the US president says: EVERYONE, KEEP OIL PRICES DOWN. I’M WATCHING! YOU’RE PLAYING RIGHT INTO THE HANDS OF THE ENEMY. DON’T DO IT! At pixel time, oil prices are broadly flat today, with Brent crude up 0.2% at $77.17 per barrel. Christine Lagarde also points out to MEPs that support for the euro has reached an all-time high, showing them a chart to prove it: She tells the European Parliament: Now is the time to make the euro area economy more productive, competitive and resilient. We need to see targeted fiscal and structural policies and strategic investments. Lagarde also calls for a legislative framework to pave the way for the potential introduction of a digital euro to be put in place rapidly, adding: By making the right policy choices, we can leverage the current momentum to boost the economic perspectives for Europe and its citizens. Over in Brussels, the head of the European Central Bank is warning that geopolitical risks could hurt eurozone growth. ECB president Christine Lagarde told the European Parliament’s Committee on Economic and Monetary Affairs that higher tariffs and a stronger euro are expected to dampen exports, with high uncertainty delaying investment decisions. Lagarde says: Risks to the growth outlook remain tilted to the downside, however. In particular, growth could slow in the event of a further escalation in global trade tensions and the associated uncertainties, deteriorating financial market sentiment and continued geopolitical tensions. That being said, a swift resolution to trade and geopolitical tensions or a further increase in defence and infrastructure spending could spur activity by more than expected. Lagarde also tells MEPs that the outlook for euro area inflation is more uncertain than usual; frictions in global trade present both upside and downside risks. She says: Upside risks include a possible fragmentation of global supply chains, while downside risks include lower demand for euro area exports and countries with overcapacity rerouting their exports to the euro area. The Green Party have also criticised Reform’s new “Britannia Card”, calling it a wheeze to prop up the super wealthy. They cite data suggesting that giving wealthy foreigners and returning British expats a bespoke tax regime in exchange for a one-off payment of £250,000 would cost tens of billions in lost tax. Green Party co-leader Adrian Ramsay MP says: “Nigel Farage’s latest wheeze to prop up the super wealthy, dressed up as helping the poorest, would result in an estimated loss of a whopping £34bn to the Treasury [1]. Rather than enabling the super-rich to buy their way out of paying UK tax, the Green Party would tax investment income as equivalent to earned income and introduce a wealth tax based on assets. This is the way to fix our public services to benefit everyone. “This is another reminder that Reform UK is a Party run by multi-millionaires out to look after their own and with net zero interest in the rest of us. There’s nothing patriotic about a “Britannia card” that would let the ultra-wealthy avoid paying taxes and contributing to society.” The £34bn figure was calculated by tax expert Dan Neidle, based on the revenue that would be lost from the current regime for non-doms. Detail of bigger commitments, such as Northern Powerhouse Rail, continue to be merely teased in today’s UK Industrial Strategy, but there are a couple of firm and specific pledges of interest to the railway. First, an East Coast mainline at Tempsford, Bedfordshire - a village that is destined to become a major new town. And secondly, an attempt to resolve that perennial trouble - train wifi. Two years after the Department for Transport was considering telling operators to simply give up on the substandard service, the government is now turning to space to solve the problem, spending £41m to introduce low-earth-orbit satellite connectivity on all mainline trains. The government says it will “significantly improve both the availability and internet connection speeds for wi-fi connected passengers, in turn enabling a better-integrated transport network.” Rachel Reeves has gleefully laid into Nigel Farage’s plan for a £250,000 flat-rate fee for wealthy foreigners - which some have compared to Donald Trump’s “golden visa”. Reform’s “Britannia Card” would allow returning expats and rich new arrivals lower taxes, in return for the levy - promising to spend the proceeds on low-income workers. However, the chancellor insisted the plan was “worse than a gimmick”. “Basically, it’s a massive tax cut for foreign billionaires,” she said, speaking to reporters in Nuneaton as Labour launched its industrial strategy. “It takes you back to a system that is even more generous than what the Tories had under Rishi Sunak. We tightened up the rules to bring in more than £33bn in tax revenue by ensuring that if people make Britain their home, they pay their taxes here, That’s what Labour’s ensuring. She added: “This opens up serious questions about what taxes will have to go up on working people and what public services, including the NHS, would have to be cut to afford a giveaway for foreign billionaires. If this is their first proper policy, then, you know, this is going to unravel pretty quickly.” The chancellor was also challenged about Friday’s public finances data, which showed the deficit for May running ahead of the Office for Budget Responsibility’s projections, prompting predictions of tax rises in the autumn. “That’s just one month’s worth of public finance data. It came in slightly higher than the OBR, but slightly lower than market expectations and obviously these numbers are all subject to revisions. So I wouldn’t read too much into one month’s data,” she said. The majority of Iran’s oil exports are directed to China, with the remainder primarily going to other Asia-Pacific nations, new analysis from Deutsche Bank shows. Their market strategist Jim Reid explains: Most of these shipments pass through the Strait of Hormuz—a critical chokepoint for global energy markets. Despite being just 21 nautical miles wide at its broadest point, the strait handles a significant share of Middle Eastern oil exports. It features two narrow 2-mile-wide shipping lanes, separated by a 2-mile buffer zone. Given these constraints, the continued accessibility of the Strait of Hormuz is pivotal to the global economic outlook—especially following U.S. involvement in the regional conflict over the weekend. As the chart suggests, China is likely to play a key role in influencing Iran’s strategic choices. European gas prices have risen today, as traders assess the risks of supply disruption. The benchmark Dutch front-month contract has gained 2% today to €41.50 per megawatt hour (MWh) this morning. That would be its highest closing level since the start of April. Jess Ralston, head of energy at the Energy and Climate Intelligence Unit (ECIU) says: “Oil and gas are commodities that are particularly vulnerable to price spikes as a result of conflicts and geopolitical events; this has always been the case and always will be. The UK is particularly exposed to increases in gas prices as we are reliant on the fuel for around 30% of our power generation and 85% of our home heating, which resulted in us being the worst hit by the gas crisis in western Europe, according to the International Monetary Fund. Three empty oil and chemical tankers have diverted away from the Strait of Hormuz and changed course, according to Marine Traffic ship tracking data reported by Reuters. The Marie C and Red Ruby, which were in ballast rather than carrying cargo and previously sailing towards the Strait, dropped anchor near Fujairah off the United Arab Emirates coast. The Kohzan Maru was sailing in the Gulf of Oman close to Omani waters, according to data on the MarineTraffic platform. Chancellor Rachel Reeves has told reporters that the government is following developments in the Middle East very closely. Asked about the potential impact on oil prices of closing shipping lanes that are crucial to global supplies, Reeves said: “We want de-escalation because it’s the right thing for the Middle East, but we also want de-escalation because of the ramifications of conflict in the Middle East for the rest of the world including the UK. “We have seen increases in oil prices in recent days and weeks, which of course will have an impact on the UK economy. We recognise the challenge that businesses and families face with energy costs. “Of course, higher oil prices will have implications for the UK economy. One of the reasons we want de-escalation is to ensure that oil continues to flow and to ensure that that key route, both for oil and for wider trade – the Strait of Hormuz – continues to be open.” At the end of May, before tensions between Israel and Iran soared, Brent crude was trading at $64/barrel, around 20% below its current levels. The pound is continuing to lose ground in the financial markets against the dollar. Sterling has lost almost three-quarters of a cent today to $1.3380, its lowest since 21 May. Potential geopolitical dangers, such as Iran’s threats to close the Strait of Hormuz, are providing support for the dollar. George Vessey, lead FX &amp;amp; macro strategist at foreign exchange payments firm Convera, explains: Over the weekend, President Trump launched airstrikes on three Iranian nuclear facilities — a move that not only bolstered Israel’s campaign to dismantle Iran’s nuclear program but also drew the U.S. further into the regional conflict. The decision surprised many. Trump had previously campaigned on an anti-interventionist platform, advocating against deeper U.S. entanglement in the Middle East. And as recently as late last week, he appeared willing to give diplomacy a two-week window before resorting to military action. That posture changed swiftly. In the lead-up to the strikes, markets were pricing in diplomatic progress: the euro strengthened, the dollar softened, safe havens were muted, and oil dropped nearly 3% on Friday — signaling a partial return to the pre-conflict playbook. But the U.S. intervention has now reversed that momentum. While the broader bias still leans toward structural dollar weakness, escalating Middle East tensions are injecting support for the greenback via the commodity channel. That channel will remain central in the days ahead, as Iran — according to state-run TV — has vowed to retaliate by closing the Strait of Hormuz, a critical artery through which about one-fifth of global oil flows. Although any such action would require approval from Supreme Leader Ayatollah Ali Khamenei, it would mark a first in the Islamic Republic’s nearly five-decade history. As such, even the threat alone is enough to keep the dollar bid, with positioning set to adjust as investors begin to unwind their bearish US dollar bets. This map, from LSEG, shows just how busy the Strait of Hormuz is today. It is 33km wide at its narrowest point, with the shipping lane just 3km wide. Members of the Organization of the Petroleum Exporting Countries (OPEC) – Saudi Arabia, Iran, the United Arab Emirates, Kuwait and Iraq – export most of their crude via the strait, mainly to Asia. Tim Gould, chief energy economist at the International Energy Agency, has said greater geopolitical uncertainty will be an “important driver” of change in the clean energy transition. Speaking at the Net Zero Delivery Summit in London this morning, Gould said an uptick in clean energy spending had happened “in particular since Russia’s invasion of Ukraine in 2022” and also “with intensifying conflict in the Middle East”. It has been “an important driver for the deployment of clean technologies”, he said, adding: “That may sound a little bit counterintuitive because you sometimes hear the view that if you are interested in energy security you invest in fossil fuels, if you are interested in emissions reductions you invest in renewables. But the reality is significantly more complicated.” While there are a range of motivators behind the decision to transition to clean energy, he said, “energy security” is an important reason to bring new technology into the system. “That was a big theme that we picked up during a recent summit held jointly with the UK government on the future of energy security. “Since 2022 we have seen a very rapid pick up in the pace of spending on energy transition and in today’s insecure, low trust world I think that preference for homegrown energy, particularly in fuel importing countries and regions, will continue to be an important driver of change.” A report by the IEA earlier this month found that global energy investment is set to increase in 2025 to a record $3.3trn, with clean energy technologies attracting twice as much capital as fossil fuels. Investment in clean technologies such as renewables, nuclear, grids, storage, low-emissions fuels, efficiency and electrification, is on course to hit a record $2.2trn this year, the IEA found. Investment in oil, natural gas and coal is on track to hit $1.1trn. Although the oil price’s early spike last night didn’t last, economists predict energy prices would soar if there was significant disruption to supplies from the Middle East. Goldman Sachs have predicted that disruptions to shipping through the Strait of Hormuz could push the price of Brent crude over $100 per barrel. That would be its highest level since August 2022, and almost a third higher than its current level of $77/barrel, pushing up transport costs, lifting inflation and hurting growth. Bloomberg explains: If oil flows through the Strait of Hormuz were to drop by half for a month, and remained 10% lower for another 11, Brent would spike briefly to as much as $110 a barrel, analysts including Daan Struyven said in a note. Should Iranian supply fall by 1.75 million barrels a day, Brent would peak at $90. However, Goldman’s baseline assumption is that that physical disruptions to Iran supply and regional oil and gas production and shipping are avoided; in that scenario, Brent crude falls to $60/barrel by the end of the year. As we reported last night, Iran’s parliament has voted to shut down the vital Hormuz shipping channel in retaliation against Donald Trump’s attack on the country. Goldman analysts argue that there are strong incentives to avoid disruption to the Strait of Hormuz, which carries a fifth of global oil. They say: “The economic incentives, including for the US and China, to try to prevent a sustained and very large disruption of the Strait of Hormuz would be strong.” Professor Costas Milas, of the Management School at the University of Liverpool, tells us: Following Trump’s direct intervention in the Israel-Iran war, geopolitical risk is on the rise and oil prices are expected to stay higher than previously thought. What are the implications for the UK economy and UK interest rates? The good news first: As I discussed in an LSE Business Review Blog (jointly with Michael Ellington from Liverpool University), the adverse impact of geopolitical risk and inflation on the UK economy has diminished over time. The bad news next: Higher oil prices are expected to increase inflation for up to four quarters. The negative impact of inflation on UK growth will take up to three quarters to show up. Geopolitical risk is expected to depress output for two to three quarters. The BoE’s monetary policymakers will have to make a judgement on whether the negative impact on GDP growth outweighs the inflationary impact. If so, Bank Rate will be cut in early August, if not earlier (through an unscheduled meeting in July). The UK’s industrial strategy also has a damning verdict on the role of the state, saying: For too long Britain has had a state which, paradoxically, both stands back and interferes too much. When our industries were at the mercy of change, too many people and communities were left to fend for themselves, with government uninterested in providing a bridge to the future. Yet equally, when new opportunities present themselves, Britain often finds itself too regulated to take advantage, or too cautious to change course. The result is a state that is both over-bearing and feeble, poorly serving an economy that has become too reliant on one place, too exposed to global volatility and too sluggish to take advantage of transitions. The UK government is attracting praise, and criticism, after outlining its new industrial strategy to support the British economy. Dubbed the ‘modern industrial strategy’, the plan (which you can read here) aims to increase business investment and grow the industries of the future. It focuses on eight important sectors: advanced manufacturing, creative industries, life sciences, clean energy, defence, digital and technologies, professional and business services, and financial services. The ‘growth mission’ breaks down into ten parts: Tackling high industrial electricity costs, including slashing green levies on thousands of businesses to bring down bills, and investing in the electricity grid so companies can get ‘timely grid connections’ Promoting free and fair trade through strong international partnerships, including securing new and improved trading arrangements with a pragmatic, agile, smart and fair approach to navigating a fragmented, geopolitically volatile, and tech-driven world. Strengthen the UK’s economic security through the uplift in defence spending Expanding access to finance, by giving the British Business Bank additional capital and expanding the mandate of the National Wealth Fund Driving innovation, underpinned by an £86bn investment into UK R&amp;amp;D Treating UK data as an economic asset Reforming the skills and employment support system to create a strong pipeline of skilled workers, Reducing regulatory burdens and cutting the administrative costs of regulation for business by 25%. Removing planning barriers, and fast-tracking decisions on critical projects in the planning system. Ensuring the tax system supports growth and high-growth sectors Ministers say they are offering investors political stability in this uncertain world, saying: Business-as-usual will not work. We need a new relationship between business and government, where government provides the strategic certainty that allows businesses to do what they do best: create wealth. This requires a more muscular approach to government: one prepared to back British businesses, invest in our comparative advantage, and take punts in pursuit of growth and productivity. And this government understands the importance of agility and enterprise; to relentlessly ask whether regulations are blocking the conditions for Britain to thrive. Recruitment and Employment Confederation (REC) chief executive Neil Carberry is pleased that Professional and Business Services is one of the eight high-growth sectors identified. Carberry says: “Firms need stable foundations from the state to deliver business investment and productivity growth. That’s what will increase prosperity and tackle the shortfall in the public finances. This Industrial Strategy is an important chance to finally make progress on this over the long term, forming a new partnership between business and government. The test now is whether the strategy can be delivered, not just by the Department for Business, but at the core of all government policy. The hospitality sector, though, is disappointed to miss out on any new support. Kate Nicholls, chief executive of UKHospitality, argues that the strategy ignores much of the economy: “This is not an industrial strategy that will deliver growth equally across the UK. In fact, by ignoring 70% of the economy it is at odds with the Government’s ambition to create jobs and help people into work. “Once again, growth will be distributed unevenly and centred around small industrial clusters that have high barriers to access – hardly a recipe for driving social mobility. “We were desperate to see a plan for hospitality and the high street, which together employs over 7 million people. We were disappointed. “How can national renewal be properly delivered if 70% of the economy is excluded from the Government’s flagship plan for growth? Oil has slipped back from its earlier highs, and is now slightly down this session. Brent crude is now trading at $76.85 per barrel, down 0.25% today (it closed at $77.01/barrel on Friday night). Its early spike to $81.50 per barrel, a five-month high, has not lasted long. AJ Bell investment director Russ Mould says: “The markets are not yet reacting with any degree of panic to the US airstrike on Iran’s nuclear facilities as they await to see how Tehran responds. The promised two-week hiatus as the US weighed its decision didn’t materialise as the Trump administration acted on Saturday. After briefly spiking above $80 per barrel when the market opened in Asia on Monday, Brent pared those gains to trade modestly higher. Growth across UK businesses accelerated slightly this month, but remains weak. The latest poll of purchasing managers at British companies shows that output picked up this month, as the private sector recovered from a drop in April. The services sector expanded, while manufacturing shrank again. Some companies reported a pick-up in order books, and client confidence, after the US rolled back its tariff announcements. But, global trade tensions and “rising geopolitical uncertainty” were cited as headwinds to growth, particularly in manufacturing. Overall, the flash UK PMI composite output interest rose to 50.7 this month, from 50.3 in May, showing the fastest growth in three months. S&amp;amp;P Global, which produces the report, says it is consistent with economic growth of around 0.1% in the April-June period. Chris Williamson, chief business economist at S&amp;amp;P Global Market Intelligence, says: “The UK economy remained in a sluggish state at the end of the second quarter, according to the early PMI survey data. “Although business conditions have continued to improve since April’s downturn, quelling recession fears, growth of business activity remains disappointingly lacklustre.” Airlines are weighing up how long to suspend Middle East flights, after the conflict in the region entered a new phase with the US attacs on Iran, Reuters reports. Leading Asian carrier Singapore Airlines, which described the situation as “fluid”, moved to cancel flights to Dubai through to Tuesday, having previously cancelled only its Sunday service. IAG group member Iberia cancelled Sunday’s and Monday’s Doha flights after making its own assessment, a spokesperson said. It has not made a decision regarding later flights. Air France KLM cancelled flights to and from Dubai and Riyadh on Sunday and Monday, and Finnair cancelled flights from Doha until at least Tuesday. Kazakhstan’s Air Astana cancelled flights to Dubai on Monday. More here: Airlines weigh Middle East cancellations after US strikes in Iran Over at Heathrow, a BA flight to Dubai that was due to leave at 12.50pm today has been cancelled, as has a 1.45pm Doha flight (although a 9.25pm flight to Doha is still shown to be operating…) The eurozone economy has continued to flirt with stagnation this month, with little growth in its key sectors. The latest survey of purchasing managers across the euro area, just released by S&amp;amp;P Global, shows that the eurozone services sector is stalling this month, while factory growth slowed. Firms reported another drop in new orders but, more encouragingly, business confidence improved to the strongest since the start of 2025. German business activity returned to growth in June, but French output fell further during the month. This has left the HCOB flash eurozone composite PMI output index unchanged at 50.2 (any reading over 50 shows growth). Dr. Cyrus de la Rubia, chief economist at Hamburg Commercial Bank, says: “The eurozone economy is struggling to gain momentum. For six months now, growth has been minimal, with activity in the service sector stagnating and manufacturing output rising only moderately. In Germany, there are signs of a cautious improvement in the situation, but France continues to drag its feet. The momentum evident in the official growth figure of 0.6 percent for the first quarter is unlikely to have carried over into the second quarter, especially since special factors such as Ireland’s unusual jump in growth inflated this figure. However, there is no reason to be resigned, as the outlook has brightened according to the survey and companies are keeping employment roughly constant. Japan’s currency has weakened today, as traders suspect that higher oil prices would hurt its economy. The yen has lost 0.8% against the US dollar, dropping to ¥147.24/$ from ¥146.07/$ on Friday night, extending its recent losses. Lee Hardman, senior currency analyst at MUFG, explains: Yen weakness could initially reflect investor concerns that Japan’s economy would be hit harder by higher oil prices given its reliance on energy imports from the region, and the potential for inflationary fears to lift yields more outside of Japan. The flight to quality bid in response to US missile strikes on Iran has not been sufficient to reverse the yen weakening trend that has been in place recently which has been encouraged as well by BoJ caution over raising rates given elevated uncertainty related to trade policy and geopolitical risks in the Middle East. European stock markets are also down in early trading. France’s CAC has lost 0.65%, Spain’s IBEX is down 0.6%, and Germany’s DAX lost 0.55% at the open. That’s a fairly muted reaction to the US bombing of Iran over the weekend. Mohit Kumar of investment bank Jefferies says the markets are waiting to see how Iran reacts, adding: Current market open suggests that base case is for a token response which will allow Iran to claim a counter-attack but with the aim of de-escalation. Key would be whether Iran would (or could) close the strait of Hormuz and disrupt global oil supply. With US and Israel planes reported to have almost clear access to Iran’s airspace, the closure of the strait would be practically impossible. Jefferies’ base case scenario is that we now enter a period of uncertainty lasting a few weeks, but without a sharp escalation. Kumar cautions that Jefferies are not “fully convinced” by the market’s sanguine reaction, explaining: We would advise using the limited reaction to reduce risk exposure in equities and credit. We are not geo-political experts. While we agree that Iran’s retaliatory capabilities may be significantly reduced, it could still use drones and smaller weapons to maintain a heightened level of uncertainty for some time. We don’t see a closure of the Hormuz strait but see possibility of disruption. Any attacks on US interests in the Gulf region could also escalate tensions further. The UK stock market has dropped at the start of trading, as traders weigh up the situation in the Middle East. Airline shares are down, with easyJet (-2.1%) and British Airways parent company IAG (-2.2%) leading the fallers on the FTSE 100 share index. Higher oil prices push up their costs, while the crisis could also lead to flight cancellations. Update: Yesterday, BA cancelled flights from London to Dubai and Doha. BP (+1.7%) and Shell (+1%) are leading the risers. Overall, the FTSE 100 index is down </t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Movement of oil tankers in the Strait of Hormuz remains largely unchanged despite the US attack on Iran. Iran’s parliament has signalled its intent to close the strait in response to US actions. The final decision rests with the national security council. Crude oil prices are now down around 1% after US president Donald Trump called for cheaper prices.</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Time for a recap. Donald Trump has turned up the temperature in his trade war, by criticizing the European Union and claiming Japan was being “tough” in negotiations. Trump claimed that the EU was failing to offer the US a favourable deal, telling reporters: “We’re talking, but I don’t feel that they’re offering a fair deal yet. They’re either going to make a good deal, or they’ll just pay whatever we say they have to pay.” Speaking after leading the G7 leaders’ meeting early, Trump also indicated talks with Tokyo were challenging, saying: “They’re tough, the Japanese are tough, but ultimately you have to understand we’re just going to send a letter saying ‘this is what you’re going to pay, otherwise you don’t have to do business with us’. But there’s a chance.” The White House has until 8 July to reach trade deals before its 90-day tariff pause ends. Trade data from Ireland has shown how pharmaceuticals exports surged this year, in an attempt to front-run new tariffs. While US retail sales fell in May. Rachel Reeves has argued that the UK is an “oasis of stability” at a time of global political and economic turmoil. She told a conference today: “In the age of insecurity we live in today, I hope that people are increasingly looking at Britain and seeing an oasis of stability where we have a sustainable politics, a stable economy and also tough, robust fiscal rules.” She was speaking just hours after Keir Starmer and president Trump signed off a UK-US trade deal at the G7 summit in Canada. The Israel-Iran crisis has gripped markets again today. Shares fell across Europe, and on Wall Street, while the oil price is now up almost 3% today. The cost of shipping oil from the Middle East to Asia has jumped in recent days…. …as has the cost of insuring shipping in the region. Raphael Olszyna-Marzys, international economist at J. Safra Sarasin Sustainable Asset Management, says: The Israel-Iran military conflict has pushed oil prices higher, though markets doubt that it will spark a global economic shock. The main risk for the world economy lies in a potential oil supply disruption that could drive prices sharply higher. Yet the oil market is currently not tight. A severe escalation, such as Iran targeting Gulf infrastructure or blocking the Strait of Hormuz, remains unlikely at this stage. Still, geopolitical uncertainty is likely to keep a risk premium embedded in oil prices, particularly as Israel appears set on inflicting long-lasting damage on Iran’s nuclear programme, a move that may not be feasible without America’s backing. And.. the UK government will not be recommended to turn water companies into not-for-profit companies under its “root and branch review” of the sector, review author Sir Jon Cunliffe has said, disappointing campaigners. It was also a day of losses on other European exchange. Germany’s DAX fell by 1%, France’s CAC lost 0.75%, Italy’s FTSE MIB shed 1.36% and Spain’s IBEX closed 1.4% lower. The Israel-Iran conflict continues to occupy investors’ minds, but hasn’t (yet) provoked a severe reaction. City consultancy Capital Economics say: Despite the further escalation in the Israel-Iran conflict over the weekend, the impact on major financial markets has remained relatively limited. Unless there is actual (not just feared) disruption to energy export infrastructure, the economic and financial impact of the conflict globally will probably remain limited. The London stock market has closed at its lowest level in over a week. The FTSE 1000 share index has ended the day down 41 points, or 0.46%, at 8834 points – its lowest close since 9 June. The rise in the oil price hit shares in airline operators IAG (-4.4%) and easyJet (-2.7%), but lifted BP (+1.65%) and Shell (+1.4%). Oil has continued to climb, putting Brent crude on track for its highest close in four months. Brent is now up almost 3%, at $75.48 per barrel; it hasn’t ended a session that high since 20 February (however, it was higher during trading on Monday, and last Friday). Fawad Razaqzada, market analyst at City Index, says: Markets were slightly rattled after Trump called for the evacuation of the Iranian capital—remarks that injected a measure of alarm into an already volatile geopolitical situation. Oil prices rose again and down went stocks and future. Meanwhile, Israel pressed on with its bombardment of Iran, prompting a forceful response from Tehran in the form of missile and drone strikes. War risk insurance premiums for shipments to Israel are as much as three time higher than a week ago as the war between Israel and Iran entered its fifth day, industry sources have told Reuters. The cost of a seven-day voyage to Israeli ports was quoted between 0.7% to 1.0% of the value of a ship versus around 0.2% a week ago, they said. Individual underwriters will price risk differently, but this will add tens of thousands of dollars per day for every voyage. The genetic testing company 23andMe has been fined more than £2.3m for failing to protect the personal information of more than 150,000 UK residents after a large-scale cyberattack in 2023. Family trees, health reports, names and postcodes were among the sensitive data hacked from the California-based company. It only confirmed the breach months after the infiltration started and once an employee saw the stolen data advertised for sale on the social media platform Reddit, according to the UK Information Commissioner’s Office – which levied the fine. The information commissioner, John Edwards, called the months-long incident across the summer of 2023 a “profoundly damaging breach”. The compromise of UK data was just a fraction of the wider losses, with the data of 7 million people affected. Today’s US retail sales report also shows that spending at restaurants and bars slumped in May by the most in more than two years. Sales at food services &amp;amp; drinking places fell by 0.9% last month, the report shows, the most since February 2023. That, as Bloomberg points out, indicates tariffs and geopolitical tensions are making consumers nervous about their finances. The recent increases in the oil price are starting to be felt by UK motoriests. Pump prices have increased marginally today, now averaging 132.2p for petrol and 138.3p for diesel, the AA reports. Both are up 0.2p from their low-points last week. Wholesale costs for both are largely static today, reports the AA, which suspects some retailers will raise their prices sooner than others. Wall Street has opened lower, as the Israel-Iran conflict weighs on markets. The Dow Jones industrial average, which tracks 30 large US companies, is down 129 points in early trading, a drop of 0.3%, at 42,385. The broader S&amp;amp;P 500 index is down 0.35%. In another sign that the US economy is slowing, industrial production fell 0.2% in May, the Federal Reserve has reported. That’s the second decline in three months, and a sign that the burst of activity in the first quarter of 2025 has cooled. The drop was slightly steeper than the 0.1% drop forecast by economists. Meanwhile in UK retail, Poundland is to shut 68 shops and two distribution centres and aims to close at least 80 more stores, putting more than 2,000 jobs at risk. The British company, which was sold last week to the US investment group Gordon Brothers for £1, has more than 800 outlets in the UK and the Republic of Ireland employing about 16,000 people. It said it planned to reduce this estate eventually to no more than 650 outlets. It also wants landlords to cut rents to zero on up to 180 stores – putting the future of those outlets in doubt – while also seeking rent reductions of between 15% and 75% on dozens more stores as part of a restructuring process that it will put to creditors in August. Poundland is also stopping selling online, ditching its Perks loyalty app, ceasing to sell frozen foods and reducing its range of chilled foods to those elements that make up its £3 meal deals – such as sandwiches – and essentials including milk. This will lead to the closure of Poundland’s frozen and digital distribution centre at Darton, South Yorkshire, later this year and its national distribution centre at Springvale in Bilston, West Midlands, in early 2026. Two other existing distribution centres in Wigan and Harlow will continue to operate. More here: The drop in US retail sales in May could be due to consumers having rushed to buy items earlier in the year, to avoid Donald Trump’s new tariffs on imports. Here’s Patrick O’Donnell, chief investment strategist at Omnis Investments, explains: The headline measure of retail sales came in below expectations in May. This was likely driven by the unwind of frontloaded purchases of autos and durable goods ahead of tariffs. Further weakness is probably in order as more of the tariff-related increase in costs are duly passed onto consumers, weighing on real incomes. However other measures of consumption have been holding up ok. As a result, the FOMC will need to see a steady trend of weaker data before there is any change to their communication, which amounts to a strategy of wait-and-see. Kathleen Brooks, research director at XTB, says: Newsflash: US retail sales fell last month, and by more than expected, in a sign that consumers may be cutting back. Retail trade sales were down 0.9% month-on-month in May, new data from the US Census Bureau shows. Sales at motor vehicle &amp;amp; parts dealers fell by 3.5% in May, the report shows, while takings at building material &amp;amp; garden equipment &amp;amp; supplies dealers were down 2.7%. The government will not be recommended to turn water companies into not-for-profit companies under its “root and branch review” of the sector, review author Sir Jon Cunliffe has said. At the launch of the Cunliffe review, the Department for Environment Food and Rural Affairs said that all options - except nationalisation - were on the table, and that a non-profit model such as that used in Wales was being considered. But Cunliffe has now said the ownership structure is not the problem causing sewage spills, financial mismanagement and water shortages created by a lack of investment, my colleague Helena Horton reports. He told parliament’s Environment, Food and Rural Affairs committee in Parliament today that the review will not be recommending one ownership structure for the industry. Cunliffe said: “If the question is whether we will recommend a wholesale transfer to another [ownership] model, what we won’t do is say we will move the whole sector to a different model. I’m not sure how you get there without spending a very large amount of public money to buy the assets and that’s outside my terms of reference”. Feargal Sharkey, former Undertones frontman turned water campaigner, said in response: “I had absolutely no expectations for this commission whatsoever and so far I am yet to be disappointed. “I fail to comprehend how the interpretation of a root and branch review of the water industry is to completely exclude the issue at the heart of the industry which is ownership of the industry and the financial abuse of the water companies. “Sir John is refusing to look at this because the government has told him not to.” When asked by MPs if his report was going to be “tinkering” if it was not recommending an overhaul of how water companies are owned, Cunliffe said: “It’s not tinkering, it’s trying to be evidence based. I don’t think looking at the models, the evidence we have, it’s not a big data set but I don’t think the conclusive evidence is there to make a big change like that.” He added that the terms of reference set by Defra secretary Steve Reed rule out using public money to nationalise water companies. Cunliffe said that in the review he will “think about the investors, how they want to take their money out, are they prepared to put more equity in as investment goes up, are they looking for capital gain, are they looking for a stream of dividends over time?” and added he will “look at how do we set rules around that”, adding “it looks maybe weak but I don’t think it is.” The review will also not make any recommendations on large bonuses and renumeration for water company CEOs: “I don’t have a problem with there being bonuses for the financial performance provided they are not at the expense of the public good. We are not going to make recommendations on particular renumeration packages for chief executives. There is a tension here between people taking pay packages they don’t deserve and recruiting and retaining. These are pretty big companies, the penalties for failure are pretty enormous. What we won’t get into is whether this [pay] is excessive.” The US stock market is set to fall when trading begins in under two hours. The main three stock indices are all in the red in the futures markets, as Reuters reports: At 7:04 a.m. ET (12.04pm BST), Dow E-minis were down 221 points, or 0.52%, S&amp;amp;P 500 E-minis were down 30.75 points, or 0.51%, and Nasdaq 100 E-minis were down 120 points, or 0.55%. Brad Bechtel of investment bank Jefferies explains that the Middle East crisis is dominating investors’ attention: The overnight news flow remains robust with plenty of headlines on Iran / Israel, the G7 meeting, which Trump exited early, and other events like the BoJ [it left Japan’s interest rates on hold]. The G7 statement contains a call for peace in the Middle East along with a clarifying statement indicating the G7 agrees that Iran should never have a nuclear weapon. Trump exited the G7 meeting rather quickly as he felt compelled to return to Washington as quickly as possible. The situation in Iran is still quite fluid with both sides still lobbing attacks but Israel claiming aerial superiority. The question on the media’s mind is around whether the US will provide bunker busters to target the nuclear facilities more aggressively, seemingly a red line for Iran with regard to negotiations. So far the view is that this attack by Israel will be a quick ‘operation’ but we heard the same on Gaza and Ukraine. Iran by far the toughest opponent in the Middle East, so we will see. Rachel Reeves has said she hopes global investors will see Britain as an “oasis of stability,” in an unstable world. Speaking at the FT Global Borrowers and Bond Investors Forum in London, the chancellor said she hoped her “non-negotiable” fiscal rules, had helped create confidence. Reeves said: “In a very uncertain world, the sort of age of insecurity we live in today, I hope that people are increasingly looking at Britain and seeing a sort of oasis of stability, where we have stable politics, a stable economy, and also tough, robust fiscal rules which this government is determined to stick to, as well as a government that’s squarely focused on growing the economy.” Being interviewed by the FT’s Chris Giles, the chancellor also made clear she hopes the independent Office for Budget Responsibility (OBR) will give the government credit for some of its pro-growth policies, when it makes its autumn budget forecasts. The OBR is widely expected to revise down its GDP forecasts, given that it is currently more optimistic than almost every other forecaster on productivity. But Reeves pointed to pro-growth factors. Reminding the audience that the OBR increased its GDP forecast by £6.8bn as a result of the government’s planning changes, she said more was to come, including the government’s planning and infrastructure bill, now going through parliament. “We are hopeful that will have a bigger impact on the ability to get stuff built in Britain,” she said. She also pointed to the government’s recent trade deals with the US and with India, and the controversial welfare reforms announced in the Spring statement. “We’ll work with the OBR over the summer, but I think there are things in both directions,” she said. Reeves also defended the government’s decision to cut the aid budget to fund defence - but appeared to suggest that decisions about higher defence spending would be for the next parliament. The new Irish pharma export data (see previous post) will add to Trump’s concerns about the trading imbalance with Ireland fuelled by big pharma which last year exported €72bn (£60bn) to the US, with taxes paid in Ireland on drugs consumed in the US. “The Irish are smart, yes, smart people,” Trump told the taoiseach Micheál Martin in the Oval Office in March, adding: “You took our pharmaceutical companies and other companies … This beautiful island of 5 million people has got the entire US pharmaceutical industry in its grasps.” While pharma exports to the US rocketed, today’s Central Statistics Office data shows that overall imports from the US fell 33% in April compared to March and by a similar level, 32%, year on year representing a drop in value of US goods brought into Ireland of €574bn year on year. Ireland’s pharmaceutical industry’s exports to the US rocketed in the first four months of the year as multinationals from Pfizer to Johnson &amp;amp; Johnson rushed to beat Donald Trump’s threatened tariffs. New data published by the government agency, the Central Statistics Office, this morning showed that exports of medical and pharmaceutical products represented more than 60% of all exports from the country. They also show that the big push to get medicines across the Atlantic peaked in March, my colleague Lisa O’Carroll in Dublin writes. CSO statistician Jane Burmanje said the overall increase in exports of pharma for the first four months of the year was more than double the value of exports for the same period of 2024, up from €30.8bn (£26.3) in January-April 2024 to €66.9bn in the first four months of this year. Exports of pharmaceuticals were down 54% in April compared to March but they were still much higher than in 2024, suggesting continuing efforts to escape import duties which Trump has repeatedly threatened. Between March and April this year, pharma exports were down €12.8bn (£10.92bn) or by 54% but exports overall were still up €2.1bn (23.6%) to €10.9bn in April 2025 compared to €8.8bn in 2024. The figures seem to confirm that efforts to beat tariffs were the root cause of a huge spike in Ireland’s economic output data for the first three months of the year. CSO data earlier this month showed gross domestic product soared by 9.7% as exports to the US ramped up. Trump has already imposed a 10% tariff on all exports from the EU to the US but the pharma industry is bracing itself for a further stacking of import duties with sectoral taxes threatened on medicines. As we reported at 10.42am, Trump says those pharmaceutical tariffs are coming “very soon”. He said: “We’re going to be doing pharmaceuticals very soon. That’s going to bring all the companies back into America. It’s going to bring most of them back into, at least partially back in.” The Iran-Israel conflict has hit risk sentiment yet again today, report Kathleen Brooks, research director at XTB. It is difficult to sum up the general mood in the markets on Tuesday. European stocks are extending losses as we move through the European morning session, and US equity market futures also point to a lower open. The oil price is also extending gains towards $74.50, as risk aversion takes hold once more. However, the gold price is only moderately higher. Headline risk from the Iran/ Israel conflict is once again impacting financial markets, after taking a reprieve on Monday. Stocks are lower after Donald Trump’s abrupt departure from the G7 to monitor events in the Middle East from the White House. This suggests that things could be about escalate in this conflict. The French President initially said that President Trump was leaving due to a ceasefire between Iran and Israel, but that was rebuffed by President Trump. This has spooked financial markets on Tuesday morning. Despite trade war uncertainty, global growth pessimism is fading, according to the latest European Fund Manager Survey from Bank of America. A net 46% of survey participants think that the global economy is set to weaken over the coming year, down from 59% last month and a record 82% in April, on the back of “a fading tariff threat”, BofA reports. A soft landing for the global economy is once more becoming consensus, with 66% of investors believing this is the most likely outcome, up from 37% in April. Investors regard a strong US consumer as the biggest upside risk for global growth, while the Trump policy mix is seen as the largest downside risk. A trade war that triggers a global recession is considered the biggest tail-risk by around half of the respondents and close to two-thirds think only very little of the tariff shock is already in the price, BofA adds. On the issue of pharmacautical tariffs, Trump told reporters: “We’re going to be doing pharmaceuticals very soon. That’s going to bring all the companies back into America. It’s going to bring most of them back into, at least partially back in.” US president Donald Trump has said the European Union was not yet offering a fair deal in trade talks between the United States and the 27-nation bloc. Seaking to reporters on Air Force One, as he returned early from the G7 summit, Trump explained: “We’re talking, but I don’t feel that they’re offering a fair deal yet. They’re either going to make a good deal or they’ll just pay whatever we say they have to pay.” Trump also said there was a chance of a trade deal with Japan, but said Tokyo was being “tough”, Reuters reports. Trump added that pharmaceutical tariffs were coming very soon and noted that Canada would pay to be part of his “golden dome” project. Trump has also told reporters on the flight that he wants “a real end” to the nuclear problem with Iran. White House Press Secretary Karoline Leavitt has posted that the briefing is a sign that Trump is the “most transparent President in history”: Reminder: The 90-day pause on new tariffs, which Trump announced in April after the markets slumped, ends on 8 July – giving the White House less than a month to strike scores of trade deals. Europe has been taking a relatively hardball strategy to secure a US trade deal – pitching itself between ‘rollover UK’ (who secured an early deal with the US) and ‘retaliatory China’ (who ended up in a full-blown tit-for-tat tariff war before a peace deal was agreed). German investor morale rose more than expected in June, according to new data from the ZEW economic research institute. ZEW’s economic sentiment index has jumped to 47.5 points, up from from 25.2 points in May, a larger rise than expected. The survey was conducted between 6 and 16 July (ie yesterday), so it covered the period when the US and China were striking a trade deal in London, as well as the Israel-Iran crisis, and began just after the European Central Bank cut interest rates on 5 June. ZEW president Achim Wambach says: “Confidence is picking up.” In the banking world, Spain’s Sabadell has said it has received interest from prospective buyers of its UK division TSB, and said it would assess any firm offers it may receive. Sabadell wants to sell TSB as it battles to fend off an €11bn (£9.4bn) hostile approach from its Spanish rival BBVA. The Catalonia-based lender said it had received “preliminary non-binding expressions of interest” for TSB from unnamed bidders, and would examine any potential binding offer. TSB, which has 175 branches in the UK, has more than 5 million customers and 5,000 staff. Two tankers have collided in waters off the United Arab Emirates and caught fire in the early hours this morning. The United Arab Emirates coast guard says it evacuated 24 people from oil tanker ADALYNN following a collision between two ships in the Gulf of Oman, near the Strait of Hormuz. British maritime security firm Ambrey has said the cause of the incident was not security-related. Daniel Smith, an analyst at Ambrey, said (via Bloomberg): “At the time of writing, we can only confirm that it is not a security incident. We continue to investigate the cause.” Global oil supply is set to increase “far” faster than demand in the coming years, the International Energy Agency has predicted. In a new report, the IEA argues that oil markets are undergoing structural changes as the key drivers of supply and demand growth of the past 15 years start to fade. The IEA estimates that global oil demand is forecast to increase by 2.5 million barrels per day (mb/d) between 2024 and 2030, reaching a plateau of around 105.5 mb/d by the end of the decade. At the same time, global oil production capacity is forecast to rise by more than 5 mb/d to 114.7 mb/d by 2030, due to increased output from the US, Canada, Brazil, Guyana and Argentina, and the unwinding of production cuts by the Opec+ group. The IEA says: This growth is set to be dominated by robust gains in natural gas liquids (NGLs) and other non-crude liquids. The strategic shift towards higher non-crude capacity is driven by strong global demand for petrochemical feedstocks and the development of liquid‑rich gas resources. Anxiety that the Israel-Iran crisis could escalate is pushing European markets down, and the oil price up (see 8.56am), analysts say. Shares in oil producers such as BP (+1.5%) and Shell (+0.7%) are rising again today, while airlines such as IAG (-2.1%) are falling. Here’s the situation: UK’s FTSE 100: -46 points or -0.5% at 8828 points German DAX: down 267 points or -1.1% at 23,430 points French CAC: down 61 points or -0.8% at 7,680 points Neil Wilson, UK investor strategist at Saxo Markets, reports that markets are very “headline driven” right now, reacting to the latest news from the Middle East. He explains: After rallying on Monday on hopes that the Israel and Iran conflict would remain contained, stock markets have lurched lower again on Tuesday after US President Trump left early from the G-7 summit in Banff and told Iran to evacuate Tehran, signalling potential escalation of the conflict. Trump said he left the summit early due to something “much bigger” than discussing a ceasefire. Israel and Iran meanwhile traded strikes for a fifth day. Reports have indicated that Tehran is willing to negotiate, but it takes two to tango and Israel won’t stop until it feels like it’s done enough. Diplomatic sources in Iran have reportedly pushed for a cease-fire, but Israeli PM Netanyahu said on Monday his country was “not backing down” from eliminating Iran’s nuclear programme. That brief fall in the oil price (see 7.52am) didn’t last long. Brent crude is now up 1.5% today at $74.36 per barrel, wiping out yesterday’s dip. Oil is rising as the Israel-Iran conflict enters its fifth day, with attacks between the two countries continuing. Earlier today, sirens sounded in several areas across Israel following the identification of missiles launched from Iran, according to Agence France-Presse (AFP). AFP also reported that two explosions were heard on Tuesday in Iran’s northwestern city of Tabriz. The UK is aiming to have energy costs that are competitive with Europe, business minister Sarah Jones has said ahead of the imminent launch of government’s industrial strategy. Jones said that the cost of energy is one of the top three concerns for businesses, who are hoping for aid in the long-awaited strategy. Her comments came as she announced the first £250m in funding for the Aerospace Technology Institute, which administers research grants. The government had already said it expects to spend £975m on research programmes up to 2030. The funding will support hydrogen-powered flight, 3D printing and using laser beams for large-scale manufacturing of aeroplane parts, the government said. Jones was speaking in the rarified surroundings of a gold-leaf salon of the Napoleonic-era residence of Britain’s ambassador to France during the Paris air show, a biannual gathering of the global aerospace and defence industries. She told the Guardian: “Whether you’re a company wanting to invest in the UK or whether you’re an existing company in the UK, energy prices is a challenge. The fact that we’re not competitive with it, with Europe, is the challenge.” As well as hurting existing industry, high energy prices relative to rivals have made it harder for the UK to attract new industries. That includes so-called sustainable aviation fuel (SAF), made either using biological matter or from hydrogen made using green electricity. “You’ve got to make sure you have the right environment in place for SAF, and obviously there are other countries that can produce certain things cheaper,” said Jones. “I think there can be a SAF industry in the UK. There are certain industries that are very interested in coming and that’s what we’re trying to work towards.” Overnight, Keir Starmer and Donald Trump have signed off a UK-US trade deal at the G7 summit in Canada, with the US president saying Britain would have protection against future tariffs “because I like them”. This means tariffs for UK carmakers will be reduced to 10% from 27.5% (25% being the recently introduced new tariff, and 2.5% existing duty). Mike Hawes, chief executive of the Society of Motor Manufacturers &amp;amp; Traders, said industry hopes the new 10% tariff rate will start “in the next few days”, speaking on BBC Radio 4’s Today programme. The UK-US trade pact had been negotiated in early May, “but we’ve been waiting for it to be implemented so manufacturers can start shipping without being subject to those punitive tariffs,” he said. He added that “a lot less” had been shipped to the US in the meantime, with some UK manufacturers shipping “a handful” while “a lot had to pause, waiting”. (British luxury carmakers Jaguar Land Rover and Bentley halted shipments, for example.) Hawes says: “They’ve been pausing because their customers – they’ve got shrewd customers – were going to wait and see what was going to happen from when the deal was announced. You could see that the cost to the ultimate consumer was going to come down because of the reduction in the tariff, but you just didn’t know when.” He expressed confidence that the new tariffs will be in place for some time, saying that “it’s been long negotiated and as the president says, he likes the UK”. He noted that UK exports have never been a threat to the US, as they tend to be small volume, high value manufactured goods, “not the type that are made in the US”. Over in Tokyo, Japan’s central bank chief has warned that the jump in the oil price, if maintained, could push up inflation. Speaking after the BoJ left interest rates on hold today, governor Kazuo Ueda told reporters: “Coupled with already rising food prices, such moves in oil prices caused by tensions in Iran and Israel, if persist, could risk affecting inflation expectations and underlying inflation. So we must scrutinise developments carefully.” Ueda also touched on trade war concerns, warning that manufacturers could be forced into cost-cutting if their profits were hit. He also warned that the economic outlook was clouded by trade war worries, saying: “Even if developments surrounding U.S. trade policy stabilise toward a certain direction, there’s very high uncertainty on how that could affect the economy…. For the time being, there is extremely high uncertainty over each country’s trade policy. As such, there is bigger downside risk for both Japan’s economy and prices.” The pan-European Stoxx 600 index has fallen to a three week low this morning. It’s down 0.9% today, with all the major European indices in the red. European stock markets have opened in the red. In London, the FTSE 100 index of blue-chip shares has dropped by 45 points, or 0.5%, to 8830 points. Germany’s DAX dropped almost 1%. Traders will be watching the Middle East, after US president Donald Trump told Iranians to “immediately evacuate” the capital. In a post on his Truth Social site, Trump says: Iran should have signed the “deal” I told them to sign. What a shame, and waste of human life. Simply stated, IRAN CAN NOT HAVE A NUCLEAR WEAPON. I said it over and over again! Everyone should immediately evacuate Tehran! Jim Reid, market strategist at Deutsche Bank, says investors are in “a bit of a limbo” as to whether anything substantive came out of the G7 summit before Trump’s early departure from the gatherering of world leaders. Reid adds: There are still big questions as to whether Israel would be receptive to a ceasefire, given that it is seeking to destroy Iran’s nuclear program. Moreover, the public rhetoric hasn’t leant that way either, and Iran’s Mehr News Agency cited a senior security official saying that it is prepared to deliver a “major blow” to Israel after its strikes. So there is maybe diplomatic movement behind the scenes but not yet in the open. The oi</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>FTSE closes at its lowest level in over a week. Shares fell across Europe, and on Wall Street, while the oil price is now up almost 3% today. The Israel-Iran conflict continues to occupy investors’ minds, but hasn’t (yet) provoked a severe reaction.</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>With European markets closed, that’s all for today. Our Middle East liveblog has the latest on the Israel-Iran conflict: Here’s our explainer on how the crisis could affect the oil price, and the knock-on impacts: And here’s more of today’s news: Wall Street remains in the green too; the Dow Jones industrial average is now up 363 points, or 0.86%, at 42,561 points. “‘Resilient’ could be the word of the day today, with markets on both sides of the Atlantic putting on a decent show despite the backdrop of global instability,” says AJ Bell head of financial analysis Danni Hewson. “The fact that so far key oil infrastructure hasn’t been targeted in the escalating conflict between Israel and Iran has been notable, and the oil price has been pared back today. But Brent Crude is still trading significantly up on where it was at the start of the month and that’s already raising the spectre of another cost-of-living crisis in the UK. “Households now have a keen understanding of what conflict in another part of the world can mean for bills back home. Inflation was already going to be in focus this week as we get May’s data on Wednesday morning followed by the latest decision by the Bank of England on where interest rates will go next a day later. “Markets are now pricing in a slim chance that the MPC will make a move on Thursday after disappointing jobs and growth data coupled with concerns that economic conditions could deteriorate later in the year if the oil price remains under pressure. “The black stuff lubricates the wheels of our lives, providing energy to create, ship and package goods. If it becomes more expensive then that will impact prices in all sorts of areas.” The FTSE 100 has crept closer to a new closing high today, but fallen just short, as investors’ anxiety over the Middle East crisis faded today. London’s index of leading blue-chip shares has ended the day up 24.5 points, or 0.28%, at 8875 points. That leaves the FTSE 100 slightly short of the record closing high, 8884.92, set last week. Stocks rose in the City amid a wider rally, following reports that Iran is seeking an end to hostilities with Israel and resumption of talks over its nuclear programme. Airline operator IAG (+1.5%) was among the top risers, along with financial stocks such as Standard Chartered (+3%), Barclays (+1.97%) and M&amp;amp;G (+1.9%). Other European markets also strengthened; Germany’s DAX and France’s CAC were both up around 0.8% in late trading. Stocks pushed higher after the Wall Street Journal reported that Iran has been urgently signaling that it seeks an end to hostilities and resumption of talks over its nuclear programs. Reuters has been told that Iran has asked Qatar, Saudi Arabia and Oman to press US President Donald Trump to use his influence on Israel for an immediate ceasefire in return for Tehran’s flexibility in talks about its nuclear program. That also pushed down the oil price; Brent crude is down 3.2% at $71.79 per barrel, having jumped around 7% last Friday after Israel launched an attack on Iran, hitting 100 major targets, including nuclear facilities and missile sites, and killing senior military commanders and scientists. UK prime minister Keir Starmer has declared that Britain and the United States should “very soon” finalise the implementation of a trade deal agreed last month. Speaking to reporters in Canada, on the sidelines of a Group of Seven (G7) meeting, Starmer said: “I’m certainly seeing President Trump today, and I’m going to discuss with him our trade deal. “I’m very pleased that we made that trade deal, and we’re in the final stages now of implementation, and I expect that to be completed very soon.” Once finalised, that deal should lower the tariffs on UK-made cars, steel and aluminium. Shares have jumped higher in New York, and the oil price is sliding faster, following a report that Iran has signalled it wants to de-escalate hostilities with Israel and negotiate. The Wall Stret Journal is reporting that Iran has been urgently signaling that it seeks an end to hostilities and resumption of talks over its nuclear programs, sending messages to Israel and the United States via Arab intermediaries. This is pushing equities up on Wall Street, where the S&amp;amp;P 500 share index is now up 69 points or 1.1% at 6,046 points. Oil has weakened, though – with Brent crude having now fallen by 3.4% today to $71.70 per barrel. That wipes out about half of its jump on Friday. With a little over an hour’s trading to go, London’s stock market is flirting with a new record high. The FTSE 100 index of blue-chip shares has now risen to 8881 points, up 0.35% today. That puts the Footsie just 3 points away from the record closing high of 8,884 points set last week [the alltime intraday high, of 8,908 points, is a little further away]. Over in New York, the stock market has opened higher as geopolitical anxiety appears to ease. The Dow Jones industrial average has risen by 265 points, or 0.6%, in early trading to 42,463 points. The broader S&amp;amp;P 500 share index has gained 0.6%. David Morrison, senior market analyst at fintech and financial services provider Trade Nation, reports that traders have been snapping up shares following the drop in values since Friday morning. Morrison says: The selling continued as markets reopened late on Sunday. But traders then bought into the dip, increasing their long side exposure once again. Time will tell if this is short-term opportunism, or a more general uptick in risk appetite. Hostilities between Israel and Iran continued over the weekend. Despite this, it appears that market participants are less concerned about the possibility of the violence spreading throughout the region than they were last week. It appears that most of the airstrikes and missiles have avoided the most significant parts of Iran’s energy infrastructure. But there are fears that this could change. In addition, Iran has threatened to disrupt, or even shut down, the Strait of Hormuz, through which around 20% of global oil is transported. But some analysts think that this is unlikely, given that this is an important route for Iranian oil to China, its major customer. Israel’s government bonds are also rallying today. Reuters reports that an Israeli bond maturing in 2054 has risen by more than 1% today. Israel’s currency is on track for its best day against the US dollar since the 2008 financial crisis. The shekel has gained around 3% today, rising to 3.51 to the dollar, up from 3.61 on Friday. The shekel had weakened last Friday after Israel launched its attack on Iran, on fears that its economy could be hurt if the conflict escalated. Analysts also suggested that the clashes could push back the timeline for monetary easing by the Bank of Israel; higher interest rates tend to support a currency. Oof! Business activity continued to decline in New York State in June, new data shows. The latest Empire State Manufacturing Survey, just released, indicates that business conditions in the state declined again this month, Firms reported that new orders and shipments declined, and supply availability worsened – possibly a sign that Donald Trump’s trade war continues to hurt the US economy. Overall, the Empire State headline general business conditions index fell seven points to -16.0, from -9 in May, weaker than expected. In brighter news, though, the survey also found that firms have turned optimistic about the outlook, with the future general business conditions index rising above zero for the first time since March. The survey was conducted between 2 and 9 June, after the US and China agreed their trade war truce in Geneva last month, but before their latest meeting in London last week had concluded. The Israel-Iran conflict, and its impact on oil prices, looms over central banks such as the Bank of England, which is scheduled to set interest rates on Thursday. The BoE is expected to leave borrowing costs unchanged this week, with a cut possible at its August or September meetings. Professor Costas Milas, of the University of Liverpool’s Management School, tells us: As the war between Israel and Iran continues, the outlook for oil prices is bound to become extremely uncertain. Notice that the Bank of England’s latest (in May) Monetary Policy Report assumes (Brent) oil prices of $64 per barrel for both 2025 and 2026. This is much lower than today’s oil price of $74.60. If the conflict continues, there are clear, and adverse, implications for (UK) inflation and GDP growth. It looks certain that the MPC will keep interest rates unchanged this week. The next decision is in early August. Nevertheless, if the war escalates, the MPC can still run an unscheduled meeting in July to deal with potentially hugely adverse effects on inflation and growth. European natural gas prices have risen today, as the energy markets continue to be influenced by events in the Middle East. Bloomberg has the details: Benchmark futures rose as much as 3.4% on Monday to the highest since early April, after jumping 4.8% on Friday. Open hostilities between Israel and Iran entered a fourth day with no sign of easing, stoking fears of a broader conflict in the energy-rich region. For gas traders, the biggest concern is that a further escalation could disrupt shipments through the Strait of Hormuz, a key waterway for seaborne supplies. While physical delivery of liquefied natural gas doesn’t currently appear to be affected, any interruption would strain the market at a crucial time in Europe’s stockpiling season. “If the narrow passage is closed, it would have a severe impact on markets,” said Arne Lohmann Rasmussen, chief analyst at Global Risk Management in Copenhagen. “We are seeing a growing risk that the market may become concerned about storage levels as winter approaches.” The dip in the oil price today is lifting shares in some airlines. IAG, which owns British Airways, are up 2.5% today, with Germany’s Lufthansa up 1.4%. Encouraging news: Businesses have grown less pessimistic about the world economy’s near-term outlook. That’s according to Oxford Economics’ June Global Risk Survey, which shows that the de-escalation of tensions between the US and China have lifted growth expectations. The Risk Survey found that businesses are confident that recession risks have declined. Respondents see less than a 15% chance of global recession this year, compared with more than 25% in April. However, sentiment remains weaker than earlier in the year, before Donald Trump’s ‘liberation day’ tariff hike announcements at the start of April. European shares are “surprisingly resilient” today against a backdrop of uncertainty,” says Russ Mould, investment director at AJ Bell. That resilience has helped to push the major European stock markets higher this morning, as they recover from Friday’s wobble. Mould points out that despite a weekend of violence between Israel and Iran, investors show no signs of panicking; future prices imply a positive day for Wall Street when US markets open later on. Mould writes: “The gold price is often a measure of investor sentiment, going up when people are worried and going down when they’re optimistic. The precious metal slipped 0.6% to $3,432 per ounce which indicates that investors remain alert to ongoing geopolitical tensions but they’re not reaching for their tin hats. “The Middle East conflict remains a fluid situation and there is the potential for markets to still experience sudden jolts if the tension escalates further.” But as things stand, the UK’s FTSE 100 index is now up 0.5% or 42 points, at 8,893 – closing in on its alltime high. Germany’s DAX is 0.3% higher, while France’s CAC has gained 0.7%. With shares up this morning, and the oil price now down, investors will be pondering how much weight to put on geopolitical issues. According to a new research note from Deutshe Bank, geopolitics historically onla has a wider market impact when it affects macro variables like growth and inflation. Deutsche Bank’s Henry Allen writes: So for markets, the geopolitical events that mattered were the stagflation shocks, like the 1970s oil crises, the Gulf War in 1990, and Russia’s invasion of Ukraine in 2022. Today, we haven’t seen a shock on that scale so far. Brent crude oil prices are still beneath their 2024 average of around $80/bbl. So this isn’t causing wider inflationary problems yet. Clearly, a larger price spike would evoke the 2022 scenario where central banks hiked rates to clamp down on inflation. But so far at least, we’re yet to see that. If anything, the extent of the market’s resilience to repeated shocks in 2025 has been a significant story in itself. The risk-off sentiment that gripped financial markets on Friday appears to be fading, even though Israel and Iran have continued to launch attacks at each other. After rising in early trading, the oil price has now dipped by almost 1% today, with Brent crude back down below $74/barrel. That still leaves it up over 6% since Thursday night, just before Israel launched its attack on Iran. Achilleas Georgolopoulos, senior market analyst at Trading Point, reports: Risk appetite appears to be improving slightly today, with the dollar losing a bit of ground, both oil and gold surrendering a decent portion of their recent gains, and bitcoin climbing to the $106k area again. However, this risk-on reaction could quickly reverse, especially if Iran openly threatens to block the Hormuz Straits. Over at the Paris Air Show, a row has broken out after four Israeli company stands at the trade fair were shut down. According to Reuters, French authorities ordered that the four stands should be closed for “displaying offensive weapons”, after not complying with an order from a French security agency to remove offensive or kinetic weapons from the stands. Israel’s defence ministry said it had categorically rejected the order to remove some weapons systems from displays, and that the show’s organisers had responded by erecting a black wall to block off the company stands. In a statement, the ministry said: “This outrageous and unprecedented decision reeks of policy-driven and commercial considerations. “The French are hiding behind supposedly political considerations to exclude Israeli offensive weapons from an international exhibition - weapons that compete with French industries.” Three smaller Israeli stands, which didn’t have hardware on display, and an Israeli Ministry of Defence stand, remain open, Reuters adds. While the markets are calmer today than last Friday, investors are still trying to evaluate the risks from the Middle East. That’s a difficult task, as Daniela Sabin Hathorn, senior market analyst at Capital.com, explains: Whereas economic metrics allow for at least some predictive modelling, geopolitical instability—especially when involving major powers such as the U.S. and Iran—introduces a layer of uncertainty that resists quantification. This latest conflict has direct implications for energy markets. The strikes targeted Iranian nuclear infrastructure, allegedly in response to Iran nearing the capability to produce a nuclear weapon. In retaliation, Iran has threatened to close the Strait of Hormuz—a key global shipping route. Meanwhile, Israeli forces have reportedly targeted Iranian gas and oil refineries, raising concerns over a major supply disruption. Although Iranian oil has technically been sanctioned for years, a substantial volume has continued to reach global markets through circumventive channels. Therefore, any credible threat to halt this flow could have profound effects—both as a supply shock and a trigger for inflationary pressures worldwide. Global investors are taking a more positive view of UK assets, investment bank Peel Hunt reports. In its latest financial results, Peel Hunt points says Europe is benefiting from the ‘rotation out of US assets’ in recent months (driven, it seems, by concerns over Donald Trump’s policy agenda). Peel Hunt says: Following the challenging market conditions of February and March, FY26 has started more positively, with the Trump administration agreeing a number of trade deals, including with the UK, and with interest rates having been cut by the Bank of England. We are seeing a rotation out of US assets into Europe and greater institutional positivity towards the UK. ECM [equity capital market] activity in the UK remains generally subdued but could gain traction should macroeconomic conditions continue to stabilise. Meanwhile our M&amp;amp;A franchise remains highly active with a strong pipeline of transactions. The interest in UK assets has led to more companies being taken over by overseas rivals this year. Peel Hunt points out: The increasing rate at which companies are exiting the London market presents a significant challenge for the UK economy. The FTSE 250 index of medium-sized companies is also rising this morning, up 38 points (+0.2%) at 21,212 points. Lender Metro Bank are the top riser, up 8.5%, after Sky News reported that it had received a takeover approach from Pollen Street Capital. Metro, which became the UK’s first new high street bank in a century in 2010, has been through a troubled time – a major accounting blunder in 2019 led to its near-collapse, and it was fined nearly £17m by the UK’s financial watchdog in 2024 for money-laundering control failures. But its fortunes have recently improved, after it returned to profitability; could it now join the exodus of companies from the London Stock Exchange? Oil prices are pushing a little higher – Brent crude is now up almost 1% at $74.90 per barrel. European stock markets have begun the new week with modest gains, despite the attacks between Iran and Israel continuing. In London, the FTSE 100 share index is 17 points (+0.2) higher at 8868 points. Oil companies BP (+1.4%) and Shell (+1.4%) are among the FTSE 100 risers, tracking the rise in crude prices. Mining companies are also higher. Betting firm Entain has jumped 6% after lifting its forecasts for revenues and profits from its US joint venture, BetMGM, this morning. In Germany, the DAX index gained 0.08%, while France’s CAC has jumped 0.3%. Jochen Stanzl, chief market analyst at CMC Markets, reports that there is caution in the markets: Investors are exercising caution following a weekend marked by mutual attacks between Israel and Iran. However, a complete sell-off has not materialized. The market currently anticipates a limited conflict, though there is little indication that hostilities will end quickly. It is expected that fighting will continue unabated this week, albeit on a limited scale. Investors should not harbor hopes for a quick resolution to the situation in the coming days. Uncertainty in the market typically leads to increased volatility because planning becomes more challenging. The risk of an escalation beyond localized retaliatory actions remains; this includes the possibility of Iran targeting energy facilities, which could result in a sharp rise in oil prices. If oil prices surge past $100 per barrel again, Germany could face the threat of recession once more. UK drivers could soon feel the impact of escalating tensions in the Middle East at the petrol station. Brent crude oil has risen from below $64/barrel at the end of last month to around $74.50 this morning, which typically leads to higher fuel prices. Thomas Pugh, economist at leading audit, tax and consulting firm RSM UK explains: “Just as tensions and uncertainty around global trade and tariffs seemed to be easing with a deal between the US and China on tariffs, the Israel/Iran escalation represents a new source of geopolitical tension. The main way this will impact UK businesses and the economy is through higher oil and natural gas prices. Indeed, oil prices have risen by about $10 per barrel (pb) in the last week. The most immediate impact will be on prices at the pump. A $10pb rise in oil prices will probably result in a 5p increase in pump prices over the next couple of months. “A rough rule of thumb is that a $10pb rise in the price of a barrel of oil eventually adds 0.1% to inflation as higher fuel prices make their way through the system. Natural gas prices have also risen, but by a slightly smaller amount. “However, to put this into context. This time last year oil prices were around $85pb and they are still way off their 2022 peaks of over $120pb. If oil prices stay at around these levels, it’s unlikely to make much of a difference to the Bank of England and the path for interest rates or economic growth this year. The price of gold, a classic safe-haven asset, has dropped back today – perhaps a sign that market anxiety is easing. As we blogged on Friday, gold jumped immediately after Israel launched its attack on Iran, as investors dashed into safer assets. That move has slightly unwound today, wih gold down 0.5% at $3,415 per ounce. It feels significant that gold remains below its alltime high, $3,500. Should it rise over that point, it will be a sign that the relative calm in the markets has fizzled out. As things stand… the oil price rally remains “limited” today amid mounting Middle East tensions, reports Ipek Ozkardeskaya, senior analyst at Swissquote Bank. Ozkardeskaya explains: Headlines were busy over the weekend as hostilities between Iran and Israel continued. An Iranian gas field in the Persian Gulf was hit on Saturday, fueling concerns that the escalation could spill over into global energy markets. While the damage appears limited to Iran’s domestic supply, the targeted gas processing facilities are linked to offshore oil production sites, potentially threatening broader energy flows. US crude opened the week above $76 per barrel, and Brent crude briefly pushed above $84 per barrel. However, both benchmarks quickly gave back gains. Natural gas also spiked at the open, breaking above its 100-day moving average, before retreating. The US dollar edged higher on haven flows, while gold, which opened at record levels, is also paring gains. The early trading reaction points to a surprisingly muted response from markets despite intensifying Middle East tensions. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. With the oil price rising again today, as attacks between Israel and Iran continue, economists are warning that the global economy faces an adverse shock, at an already difficult time for growth. Oil prices have risen this morning, up around 1%, as the conflict between the two countries enters a fourth day. Fears of disruption to supplies – a risk, if the Strait of Hormuz was to be closed – are making the oil price volatile. After a 7% surge on Friday, Brent crude is up another 0.5% on Monday morning at $74.60 per barrel, towards the five-month high touched early last Friday. Iran accounts for about 3% of global oil supplies, while roughly 20% of global oil and LNG flows through the Strait of Hormuz, making it a crucial artery for the global economy. Traders have noted that an Iranian gas field in the Persian Gulf was hit on Saturday, prompting Iran’s foreign minister to accuse Israel of seeking to expand the war beyond Iran. Mohamed El-Erian, economic advisor to insurance giant Allianz, says the conflict risks causing slower global growth, increased inflationary pressure, reduced “policy flexibility” for central banks, and “further gradual erosion of the global order”. He warned yesterday: Two days into intensifying hostilities, both the probability and potential severity of these four effects have risen, confirming the notion that, in economic terms, this constitutes an adverse shock to an already fragile global economy. Stock markets are, so far, showing some resilience on Monday. Japan’s Nikkei 225 index has gained over 1% today, while China’s markets are a little hgher. Wall Street is set to open a little higher too; Tony Sycamore, analyst at IG, explains: While the situation in the Middle East remains fluid, US S&amp;amp;P500 equity futures are trading about 0.95% higher this morning at 6036, likely buoyed by Israel’s early success in targeting Iran’s nuclear facilities, air defences, missile production, and military leaders to cripple strategic capabilities. Additionally, while Israel has targeted Iranian energy infrastructure used domestically, it has refrained from targeting key Iranian oil export infrastructure. The agenda All day: Paris Air Show 1.30pm BST: NY Empire State manufacturing index</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>The FTSE 100 has crept closer to a new closing high, but fallen just short. London’s index of leading blue-chip shares has ended the day up 24.5 points, or 0.28%, at 8875 points. Wall Street remains in the green too; the Dow Jones industrial average is now up 363 points. UK prime minister Keir Starmer has declared that Britain and the United States should ‘very soon’ finalise the implementation of a trade deal.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Time to wrap up. The price of oil and gold has soared and stock markets have fallen after Israel’s strikes against targets in Iran. The escalation of the conflict in the Middle East, the focal point of global oil production, prompted a sharp increase in prices. Brent crude initially jumped by more than 10%. But in late trading, it has slipped slightly – still up 5.7% today at $73.29 per barrel, on track for its biggest daily rise since April 2023. Mohamed El-Erian, economic advisor to Allianz, warned that rising oil risks creating a ‘stagflationary shock’. He says: For the average consumer, they will be looking at more income uncertainty. They will be looking at higher petrol prices, and in the UK, they’re probably looking now at higher risk of taxation in October. Matt Gertken, chief geopolitical strategist at BCA Research, says tonight: These attacks on Iran are most likely the first steps toward all-out conflict in the Middle East – but there is still a 25% chance of a diplomatic resolution and de-escalation. “We’ve already seen a minor oil price spike, yet Israel has not finished its campaign and Iran has not fully retaliated. In the worst-case scenario, which now has 45% odds, we could see Iran retaliate, the US enter the fray, and oil prices double as Iran strikes regional oil supply. “Any oil supply shock would have global implications, reminding the world of the US’s inherent advantages, weighing on European and Chinese economies, and playing into Russia’s hands in Ukraine. Shares in airlines fell sharply today, as the rising oil price pushes up their fuel costs. Gold rose closer to its recent record high, and there was a small flight to safety into the US dollar. But equity markets fell, with the UK’s FTSE 100 losing 0.4% and most other European markets down over 1%. Here’s the full story: Back on Wall Street, the US stock market has recovered some of its earlier losses. The Dow Jones industrial average is now down 0.9%, or 401 points, at 42,566. The S&amp;amp;P 500 is 0.44% lower. European market have also ended the day in the red. Both France’s CAC and Germany’s DAX lost a little over 1%, with Italy’s FTSE MIB and Spain’s IBEX down around 1.3%. Britain’s stock market has closed for the week, with many share prices hit by the conflict in the Middle East. The FTSE 100 index of blue-chip shares ended the day down 34 points at 8850, 0.4% below yesterday’s record closing high. IAG, parent company of British Airways, was the top faller, down 3.7%, with budget airline easyJet (-2.7%), investment firms Schroders (-3.4%) and International Capital Group (-2.5%) also losing ground. Bucking the selloff were precious metal producers Endeavour Mining (+2.9%) and Fresnillo (+2.2%), who benefitted from the rising golf price today, and defence companies BAE Systems (+2.8%) and Babcock (+1.9%). “This is a dangerous situation,” said Francois Savary, chief investment officer at Genvil Wealth Management in Geneva, summing up why shares have fallen today, while oil has jumped. “This is one of those situations where everything is under control and then everything is not under control.” US defence stocks are climbing in morning trading in New York, as geopolitical risks rise. Lockheed Martin are up 3.3%, RTX Corporation has gained 2.2%, and Northrop Grumman has risen 3.2%. Italian bank UniCredit have suggested oil prices could surge toward $130 per barrel, if the Israel-Iran crisis leads to a prolonged blockade of the Strait of Hormuz, the world’s most important oil artery. UniCredit’s says: In our risk scenario, Brent prices would move towards and above $100/bbl. How much above, depends on how lasting and serious the damage to global oil supply is. In the worst-case scenario, especially if there is a prolonged blockade of the Strait of Hormuz, Brent prices might jump to wards $130/bbl. But in UniCredit’s baseline scenario, where there are no major disruptions to the oil market, Brent crude stabilises at $75-$80 – up from its previous forecast of $65/bbl. In March 2022, after Russia’s invasion of Ukraine, Brent briefly jumped over $130/barrel, before falling back. It hasn’t traded over $100/barrel since August 2022. Travel companies are among the big fallers on Wall Street. Cruise operator Carnival (-4.7%), United Airlines (-4.4%) and Delta Air Lines (-4%) are among the top fallers on the S&amp;amp;P 500 share index. The New York stock market has dropped at the start of trading, following losses in Europe and Asia-Pacific markets. The news that Israel attacked Iran overnight has sparked a wave of selling, pushing the main indices into the red. Dow Jones industrial average: down 480 points or 1.1% at 42,487 points S&amp;amp;P 500: down 41 points or 0.7% at 6,003 points Nasdaq Composite: down 156 points or 0.8% at 19,505 points. As in the UK, airline stocks are falling sharply, but oil company shares are higher, tracking the rise in crude oil prices today. The surge in the oil price (currently up 8% today) means crude prices are on track for their 19th largest weekly rise since 1988, according to Deutsche Bank’s Jim Reid. He’s kindly created this chart, putting this week’s rise in the oil price in context: Reid writes: There were previous direct attacks between Iran and Israel in April and October of 2024, but this is much bigger in scale, with several senior Iranian military officials widely reportedly to have been killed. For markets, the focus is now turning to how the situation might escalate, given that Iran have pledged to retaliate, and President Trump has said that without a deal “it will only get worse!” This is raising genuine fears about a wider conflict, with the risk that the United States is also dragged in. From a market point of view, this is highly significant, although as the chart shows, the oil move today doesn’t look quite as big in historic terms. On a weekly basis, Brent crude is on track for the 19th largest climb since 1988 and as it stands is hovering around the top 50 in terms of single-day moves over the same period. Although at just before 4am London time we were at the 12th biggest daily jump. In a year of shocks, high volatility, but very strong performance in many areas (especially for non-US equities), it’s another curveball to throw into the mix. It’s probably yet another weekend to keep an eye on the news! As I type, Brent crude is changing hands at $74.90 per barrel, up from $66.47 at the end of last week. Greece and Britain have advised their merchant shipping fleets to avoid sailing through the Gulf of Aden and to log all voyages through the Strait of Hormuz after Israel’s large-scale attacks on Iran on Friday, documents seen by Reuters showed. Greek ship owners were urged to send details of their vessels sailing through the Strait of Hormuz to Greece’s maritime ministry, according to one of the documents issued by Greece’s shipping association, which was sent on Friday. It says: “Due to developments in the Middle East and the escalation of military actions in the wider region, the (Greek) Ministry of Shipping ... urgently calls on shipping companies to send ... the details of Greek-owned ships that are sailing in the maritime area of the Strait of Hormuz”. All UK-flagged vessels, which include the Gibraltar, Bermuda and Isle of Man ‘red ensign’ registries, were advised to avoid sailing through the southern Red Sea and the Gulf of Aden, a separate document issued by the UK’s transport ministry said. If transiting these areas, vessels must adhere to their highest level of security measures and limit the number of crew on deck during transits, said the advisory, seen by Reuters. Airlines were the worst-performing sector in Europe, after several countries in the Middle East close their airspace to commercial flights today. In Europe, Air France-KLM (-4.5%), Deutsche Lufthansa (-3.4%) and British Airways parent IAG (-4.2%) are all among the big fallers today. In Asia, Japan Airlines Co. dropped 3.7%. Turkish Airlines has dropped over 6% in Istanbul. Prices of copper and other industrial metals have fallen today, as investors sold risky assets after Israel’s attack on Iran. Benchmark three-month copper on the London Metal Exchange shed 1.3% to $9,575 a metric ton this morning, the weakest since 3 June, Reuters reports. A rising oil price could make it harder for central banks to cut interest rates this year, warns Kathleen Brooks, research director at XTB: “If the oil price continues to climb towards $100 in the coming days, then we could see the interest rate futures market price out rate cuts from the US and Europe, which may add to downside pressure on stocks. “However, if there is no nuclear escalation, then we think we could see oil prices settle back around $70 per barrel.” Goldman Sachs is sticking with its assumption that there will not be disruption to oil supplies in the Middle East. The Wall Street bank says that its adjusted summer 2025 forecasts include “a higher geopolitical risk premium”; even so, it still forecasts that strong supply growth outside US shale will lower oil prices. Goldman forecasts that Brent crude will fall to $59 per barrel in the fourth quarter of this year, and average $56/barrel in 2026. But, prices would be higher if oil supplies from Iran were disrupted. Goldman explains: While our base case is that the geopolitical risk premium will decline if oil supply is unaffected, geopolitical risks have risen sharply, and we estimate the upside price risk in alternative scenarios. The first scenario assumes that any potential damage to Iran’s export infrastructure reduces Iran supply by 1.75mb/d during 6 months before gradually recovering. Making the additional assumption that extra core OPEC+ production makes up half of the peak Iranian shortfall, we estimate that Brent jumps to a peak just over $90/bbl but declines back to the $60s in 2026 as Iran supply recovers. [Although the US currently imposes sanctions on Iran’s oil industry, it still exports crude to countries such as China]. The oil price remains sharply higher today, as tensions in the Middle East alarm investors. Brent crude is currently up 9% today at $75.55 per barrel, on track to close at its highest level since February. US crude is also up 9% at $74.32 per barrel. Tamas Varga, analyst at oil broker PVM (which is part of interdealer broker TP ICAP), says it is impossible to predict how the Israel-Iran conflict will develop. Only a list of possible events can be drawn up. Iran pledged to retaliate but is it capable of effectively doing so and if it is, will it also target US bases? Will regional oil supply and transport routes, namely the Strait of Hormuz, which 20 million bbls of oil sails through a day, be affected? Will the US and Western powers intervene to de-escalate? Will regional Arab powers get involved? There are many questions without satisfactory answers, therefore it would take a bold man to bet on the reversal of the overnight price jump ahead of the weekend. Donald Trump is urging Iran to “make a deal”, warning that further attacks “even more brutal” than last night’s move by Israel have already been planned. Posting on his Truth Social social network, the US president warns Tehran it must act before it is too late, saying: I gave Iran chance after chance to make a deal. I told them, in the strongest of words, to “just do it,” but no matter how hard they tried, no matter how close they got, they just couldn’t get it done. I told them it would be much worse than anything they know, anticipated, or were told, that the United States makes the best and most lethal military equipment anywhere in the World, BY FAR, and that Israel has a lot of it, with much more to come - And they know how to use it. Certain Iranian hardliner’s spoke bravely, but they didn’t know what was about to happen. They are all DEAD now, and it will only get worse! There has already been great death and destruction, but there is still time to make this slaughter, with the next already planned attacks being even more brutal, come to an end. Iran must make a deal, before there is nothing left, and save what was once known as the Iranian Empire. No more death, no more destruction, JUST DO IT, BEFORE IT IS TOO LATE. God Bless You All! The rush for safe-haven assets today has pushed up the US dollar, lifting it from Thursday’s three-year low. The dollar index has gained 0.4% today, as the US currency gained against a basket of currencies. The pound has dropped by over half a cent, to $1.355. Lee Hardman, senior currency analyst at banking group MUFG, says the Swiss franc, the yen and US dollar have all benefitted from the flight to safety. Hardman adds: The developments could provide a timely test of the US dollar’s traditional safe haven appeal after it hit fresh year to date lows yesterday prior to Israel’s military strikes. On the other hand the flare up in geopolitical tensions in the Middle East and heightened risk of an oil price shock has triggered a reversal lower for high yielding carry currencies such as the Hungarian forint, South African rand and Mexican peso which have benefitted recently from the reduction in financial market volatility. The more growth sensitive commodity currencies of the Australian and New Zealand dollars have been hit the hardest amongst G10 currencies. Consultancy firm TS Lombard have predicted that the surge in the oil price will fade, unless the US is dragged into the Israel-Iran conflict. They told clients this morning: Although it is too soon to tell if Iran will go further from its drone retaliation, it is clear that the US will not involve itself at this time, unless US assets are targeted. This alienates any “boots on the ground” scenarios which likely makes this recent escalation a transient episode. We expect the geopolitical risk premium added to Oil today to fade if escalation remains contained. Marco Rubio, Trump’s secretary of state and national security adviser, has stressed that Israel’s strikes were unilateral, while saying the U.S. had known attacks would occur. British gas producer Energean has temporarily suspended the production and activities of its power floating production storage and offloading (FPSO) located offshore Northern Israel, following the attack on Iran overnight. Energean told the City of London this morning that it had received a notice from Israel’s Ministry of Energy and Infrastructure ordering the suspension, “following the recent geopolitical escalation in the region.” It adds: The safety of Energean’s staff is our top priority. All production activities have now been temporarily suspended and notices have been issued to Energean’s customers and other stakeholders. Energean maintains a close dialogue with the Ministry of Energy and Infrastructure and other relevant stakeholders to facilitate the safe resumption of production as soon as possible. Energean’s shares have dropped by over 6%, the top faller on the FTSE 250 index of medium-sized companies. A conflict between Israel and Iran could dampen the outlook for the German economy if it leads to an increase in oil prices, the economic institute DIW Berlin has predicted. DIW chief economist Geraldine Dany-Knedlik says: “If a noticeable increase in oil prices were to result from this, they would be significant dampening factors that come at an unfavourable time.” Dany-Knedlik points out that consumer sentiment would be hit by a surge in fuel costs: “Private households are less influenced by the announcements of the European Central Bank and more by the gasoline and diesel prices they perceive daily.” The US stock market is set to fall when when trading begins, in a little over five hour's time. The futures market indicates the Dow Jones industrial average, and the broader S&amp;amp;P 500 share index, could both drop by 1.2%. Richard Hunter, head of markets at interactive investor, says: “Global markets are being rattled by an escalation of Middle East tensions as Israel attacked Iran’s nuclear programme overnight. The news came after the close on Wall Street on what was otherwise a positive day, but even at this early stage Dow Futures are heading south in response to the attack. There was an inevitable rush to haven assets such as gold following the assault, while the oil price itself gained by more than 7% overnight, all but wiping out its losses for the year. Of particular concern is the likelihood of retaliatory measures which, if aimed at the Strait of Hormuz where around 20% of global flows are handled, would further potentially constrict supply. Budget airline Wizz, whose shares are down almost 5% today, says it has suspended flights to Tel Aviv and re-routed flights affected by closed airspace in the region for the next 72 hours. The jump in the oil price today, following Israel’s attack on Iran, is a “bad shock for the global economy at a bad time”. That’s the warning from Mohamed El-Erian, President of Queens’ College, Cambridge, and advisor to insurance giant Allianz. Speaking to Radio 4’s Today programme, El-Erian explains that a higher oil price can lead to a “classic stagflationary shock”, undermining economic growth and fuelling inflation. El-Erian says: For the average consumer, they will be looking at more income uncertainty. They will be looking at higher petrol prices, and in the UK, they’re probably looking now at higher risk of taxation in October. [reminder: economists are already warning that Rachel Reeves may need to raise taxes in the autumn budget, to keep within her fiscal rules] He also suggest that the probability of interest rate cuts has fallen, which will disappoint president Trump who has been demanding lower borrowing costs. The fact the US says it was not involved in Israel’s attacks means they are “another shock to the stability of the US-led the global economic order”, which was already facing questions, El-Erian adds, saying: So whatever way you look at it, it’s negative short term, it’s negative longer term. European stock markets have joined the global selloff, as the overnight escalation in the Middle East has triggered a wave of risk-off sentiment. Here’s now the main indices have fallen: Germany’s DAX: -1.35% France’s CAC: -1.2% Italy’s FTSE MIB: -1.45% Spain’s IBEX: -1.55% Jochen Stanzl, chief market analyst at CMC Markets, says the markets are dominated by a single issue: Israel’s attack on Iran. This alarming escalation in the Middle East has likely caught many investors off guard. Those who have been looking for an opportunity to sell stocks and take profits are now becoming active. It seems the DAX has seen its yearly high from just over a week ago for the time being. Oil prices are skyrocketing as fears grow not only regarding the disruption of Iran’s recent strengthened oil exports but also the potential targeting of other oil production facilities in the region, should this conflict escalate further. Additionally, the transportation of oil through the Strait of Hormuz is now at risk. While the oil price is not as critical for the German economy as it was one or two decades ago, a rapid surge in prices can still affect the recent strength of the euro, which can no longer compensate for lower import prices under such circumstances. Investors are now grappling with the prospect of two wars and an ongoing trade conflict, prompting a reassessment of risks. Gold prices are heading towards record highs, equities are under pressure, and the dollar is rising once again. The events of the past few hours have sparked a broad risk-off movement among investors. In recent weeks, the U.S. has repeatedly tried to deter Israel from such an attack, but as we learned today, those efforts have been unsuccessful. News regarding the enrichment of weapon-grade uranium marked a turning point. The situation now hinges on Iran’s response. No one wants a wider conflagration in the Middle East, but the risk has noticeably increased due to the recent developments.” Shares in oil companies BP (+2%) and Shell (+2.1%) have jumped, following the surge in the oil price overnight. But the top riser on London’s FTSE 100 is weapons producer BAE Systems (+2.8%), reflecting concerns that the Israel-Iran conflict could escalate. Britain’s stock market has dropped at the start of tading, with most blue-chip shares in the red. The FTSE 100 share index, which finished Thursday at a record closing high, has dipped by 48 points or 0.56%, to 8837 points. Airline shares are falling sharply – British Airways parent company, IAG, has lost 5.6%, followed by easyJet which is down 4.6%. There is a “strong risk-off move” in several asset classes today, with the focus now shifting to what form Iran’s retaliation might take, reports Jim Reid, market strategist at Deutsche Bank. He says: There’ve been huge developments in the Middle East overnight, as Israel has carried out air strikes against Iran’s nuclear and military facilities. We still await further details, but press reports have said that explosions were heard in Tehran and Natanz, which is where one of Iran’s nuclear plants is. Iranian state TV has reported that Hossein Salami, the head of the Revolutionary Guards, was killed, along with armed forces chief of staff Mohammad Bagheri. Israeli PM Netanyahu has said the operation “will continue for as many days as it takes to remove this threat”, although US Secretary of State Marco Rubio has said the US weren’t involved in the strikes. The news has led to significant fears about an escalation and a wider regional conflict. For instance, Iran’s armed forces spokesperson said that Israel and the US will receive a “harsh blow” in response, and Iran’s Supreme Leader said Israel “should expect a severe punishment”. In turn, oil prices have surged on the news. Gold is heading towards a record high, as investors seek out safe-haven assets. The spot price of gold has jumped 1% to $3,418 per ounce, towards the all-time peak of $3,500/oz set in April. Derren Nathan, head of equity research at Hargreaves Lansdown, says: Safe haven assets are back in demand with gold prices at seven-week highs at over $3,400 per ounce. Diminishing risk appetite, as well as the potential for lower interest rates on cash paint, a positive picture for investors in the yellow metal. European shares are set to open sharply lower in under 30 minutes time. Reuters has the details: Euro STOXX 50 futures, which track blue-chip euro zone stocks, dropped 1.4%, with contracts on the German and French benchmarks each down over 1%. Futures on Britain’s oil- heavy FTSE fell 0.4%. Shares across Asia-Pacific stock markets fell sharply after Israel launched its military operation at Iran’s nuclear facilities. Japan’s Nikkei dropped 1%, South Korea’s KOSPI has lost 0.85% and China’s CSI300 is down 0.66%. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Stock markets are sliding, and the oil price has surged, after Israel launched an attack on Iran overnight, targeting nuclear facilities, military commanders and Iranian scientists. The attacks, a major escalation of tensions in the Middle East, have sent investors dashing into safe-haven assets, fearing it could spiral into a wider conflict. Brent crude oil surged by over 10% when news of the attacks broke, reaching its highest level since January. It’s now up 8% at $73.52 per barrel, which would be the biggest daily rise since 2022. Oil was driven higher by worries that supplies from the region could be disrupted, if the conflict escalates. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, suggests that oil could push higher, perhaps to $90–$100 per barrel, in that scenario, saying: Oil jumped as much as 13% after Israel launched a major and unprecedented attack on Iran, targeting nuclear and military facilities. While the news isn’t entirely surprising—there had been reports of Israel preparing action and the U.S. ordered Americans to leave the region earlier this week—the Israeli strikes could mark the beginning of wider regional tensions. If Israel continues operations beyond its borders, the Middle East could heat up fast. Latest: Israel says Iran’s nuclear programme poses an existential threat and vows that its operation will continue for as long as necessary. Iran has already launched hundreds of drones in retaliation and could go further. But how much further? Benjamin Netanyahu has indicated that the Israeli operation will take “many days”, and warned that “Israeli citizens may have to remain in sheltered areas for lengthy periods of time.” The agenda 3pm BST: US consumer confidence report</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Brent crude initially jumped by more than 10%. But in late trading, it has slipped slightly – still up 5.7%. On track for its biggest daily rise since April 2023. Mohamed El-Erian, economic advisor to Allianz, warned that rising oil risks creating a ‘stagflationary shock’</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Time to recap… Donald Trump has endorsed the US-China trade deal struck in London that will ramp up supplies of rare earth minerals and magnets needed for the automotive industry, saying it will take total tariffs on Beijing to 55%. Acknowledging that his Chinese counterpart, Xi Jinping, still needed to give his final approval on the terms agreed late on Tuesday night at Lancaster House, the US president disclosed the pact would also facilitate Chinese students’ access to US colleges. Posting on his Truth Social site, Trump says: OUR DEAL WITH CHINA IS DONE, SUBJECT TO FINAL APPROVAL WITH PRESIDENT XI AND ME. FULL MAGNETS, AND ANY NECESSARY RARE EARTHS, WILL BE SUPPLIED, UP FRONT, BY CHINA. LIKEWISE, WE WILL PROVIDE TO CHINA WHAT WAS AGREED TO, INCLUDING CHINESE STUDENTS USING OUR COLLEGES AND UNIVERSITIES (WHICH HAS ALWAYS BEEN GOOD WITH ME!). WE ARE GETTING A TOTAL OF 55% TARIFFS, CHINA IS GETTING 10%. RELATIONSHIP IS EXCELLENT! THANK YOU FOR YOUR ATTENTION TO THIS MATTER! The 55% tariff total appears at first glance to be a hike from the 30% rate agreed in the truce struck early last month when both sides slashed triple-digit rates. However, a White House official said it merely reflected Trump’s worldwide 10% baseline “reciprocal” tariff on imports, the 20% fentanyl trafficking levy and a 25% pre-existing tariff on China. Trump also posted that he and president Xi will “work closely together to open up China to American Trade”. Trump was speaking (or posting) after the US and China extended the truce in their trade war after two days of talks in London that resulted in a “framework” deal over export restrictions on rare earths and semiconductors. But, there are reports tonight that China is putting a six-month limit on rare-earth export licenses for U.S. automakers and manufacturers. US prices continued to rise in May as companies and consumers grappled with Donald Trump’s tariffs. The president has repeatedly pledged to lower costs across the economy. Annualized inflation ticked higher to 2.4% in May, up from 2.3% in April. On a month-to-month basis, the consumer price index rose by 0.1%, down from 0.2% the previous month. The readings were softer than expected. Economists had expected a headline CPI reading for 2.5% in May, amid widespread uncertainty over the direction of the US economy. Core inflation, which measures price increases outside of food and gas, went up 0.1% on the month, down from 0.2% in April, according to the Bureau of Labor Statistics. In other news… The FTSE 100 has ended the day close to its record closing high. Chancellor Rachel Reeves has outlined the UK government’s spending plans for the next three years The Wall Street Journal is reporting that China is putting a six-month limit on rare-earth export licenses for U.S. automakers and manufacturers, according to people familiar with the matter. This will give Beijing leverage if trade tensions flare up again, but also creates lingering uncertainty for American industry. The WSJ reports: Chinese negotiators agreed to the temporary restorations of the licenses after the latest round of talks with their American counterparts in London after two days of intense talks, aimed at upholding an interim agreement forged in Geneva last month. In exchange, the people said, the U.S. negotiators agreed to relax some recent restrictions on the sale to China of products such as jet engines and related parts as well as ethane, a component of natural gas important in manufacturing plastics. Details of the framework are still being worked out, the people said. The White House declined to comment. Beijing wants to keep its chokehold on the supply of such critical commodities for future negotiations, according to people who consult with senior Chinese officials. In other trade news…. the White House has welcomed a federal appeals court ruling earlier this week that allows President Donald Trump‘s most sweeping tariffs to remain in effect. The decision by the U.S. Court of Appeals for the Federal Circuit in Washington, D.C. means Trump may continue to enforce, for now, his “Liberation Day” tariffs on imports from most U.S. trading partners, as well as a separate set of tariffs levied on Canada, China and Mexico. The tariffs will remain in effect while the Court reviews a lower-court decision blocking them on grounds that he had exceeded his authority by imposing them. White House spokesman Kush Desai said in a statement: “The Trump administration is legally using the powers granted to the executive branch by the Constitution and Congress to address our country’s national emergencies of persistent goods trade deficits and drug trafficking. The US Circuit Court of Appeals’ stay order is a welcome development, and we look forward to ultimately prevailing in court.” Donald Trump has renewed his calls for the US Federal Reserve to lower interest rates dramatically. Posting on his Truth Social site, Trump urges the Fed to cut rates by a whole percentage point – a call he also made last Friday. Welcoming the small rise in US inflation, Trump says: CPI JUST OUT. GREAT NUMBERS! FED SHOULD LOWER ONE FULL POINT. WOULD PAY MUCH LESS INTEREST ON DEBT COMING DUE. SO IMPORTANT!!! Britain’s blue-chip share index has risen closer to its record closing high tonight. The FTSE 100 has closed at 8864 points, up 0.13% or 11 points today, as it closes in on the previous record close of 8871.31 points set on 3 March. Housebuilders helped to lift the Footsie, after UK chancellor Rachel Reeves announced a surge in funding for affordable housing (see our Politics Live blog for details) AJ Bell head of financial analysis Danni Hewson, says: “The FTSE 100 has returned over 10% so far this year, a heady performance which might just be the green shoots of a revival in the UK equity market. It’s early days, but a sustained period of strong performance could see investors reappraise the prospects for UK stocks, and create a virtuous circle whereby more money starts to flow into UK plc, boosting performance even further. “Housebuilders had a rather splendid day, after the Chancellor confirmed £39 billion of investment in affordable and social housing, which she claims is the biggest cash injection in fifty years. This comes on top of existing plans to remove red tape around planning permission to make it easier for housebuilders to develop new homes and flats. There is a clear tailwind for the housebuilding sector and the cherry on top would be a further decline in interest rates so more people can afford to get on the housing ladder. When the FTSE 100 finally hits its record high, it will cap off a recovery in stocks over the last two months, as markets rebounded after crashing in early April. Back on 9 April, the FTSE 100 closed at 7,679 points, before recovering through April and May as Trump backed down over some of his tariff threats. UK and Scottish ministers are scrabbling to save around 400 jobs at one of the UK’s largest electric bus manufacturers, Alexander Dennis, after its owners announced a consultation on the closure of two Scottish sites. The company’s owners, NFI, said midway through the Chancellor’s spending review statement at Westminster they wanted to consolidate all manufacturing to Scarborough because of the intense competition from Chinese electric bus makers, our Scotland editor Severin Carrell reports. The closures raise fresh questions about the UK’s transition to net zero, which the Chancellor prioritised in her statement. Alexander Dennis’ factories are in Falkirk and Larbert, close to Grangemouth oil refinery which has recently closed with the loss of 400 jobs. Ian Murray, the Scottish secretary, said he was “a bit surprised” at the timing of NFI’s announcement given ministers in both governments were in talks about a deal to protect those jobs. He said that could include putting the workforce on furlough to “buy a little time”. Murray blamed the Scottish government for failing to give the firm enough orders. Andy Burnham, the mayor of Manchester, had placed an order for 200 of its EV buses while the Scottish government had only bought 44: “The Scottish government hasn’t ordered enough buses from their indigenous bus company, and we need to try and find a way through that. “Obviously it’s a huge shock to the workforce, a huge shock to the local area, but the 45 day notification period on this allows us to get a bit of time to see if there’s ways in which we can help.” Kate Forbes, Scotland’s deputy first minister, said they had “engaged extensively” with the company to “ensure that every possible avenue is explored to mitigate the need for redundancies.” Stocks have risen on Wall Street in morning trading, as investors welcome the US-China trade accord. The news that inflation rose by less than expected last month has also cheered traders. The Dow Jones industrial average, which contains 30 large US companies, has risen by. 167 points or 0.4% to 43,034 today. The broader S&amp;amp;P 500 share index is rising towards its recent record high; it’s up 0.3% at 6,056 points. John Lloyd, global head of multi sector credit at Janus Henderson Investors, says today’s inflation report should reassure policymakers: However, this report will provide the Fed with comfort that we are on the correct pathway with regards to underlying inflation. The path for policy rates over the next year is certainly more difficult to forecast as the economy and markets will be impacted by governmental policy decisions in the US and around the world. There are currently 50 bps of cumulative cuts to the Fed Funds rate priced in for the year. This report gives us more confidence that we will realise at least two cuts before year end. Today’s inflation report suggests that the Trump trade war has not, yet, had much impact on US prices. Alexandra Wilson-Elizondo, global co-CIO of multi-asset solutions in Goldman Sachs Asset Management, explains: “Inflation in May was lower than anticipated, suggesting the tariffs aren’t having a large immediate impact because companies have been using existing inventories or slowly adjusting prices due to uncertain demand. While we might see some price increases on goods later, service prices are expected to remain stable, suggesting any rise in inflation is likely to be temporary. As we wait for the 90-day tariff pause to pass, the market will be caught between inflation and job prints. If inflation stays under control or the job market weakens, the Federal Reserve will likely consider cutting interest rates down the road. We expect the Fed to remain on hold at next week’s meeting, but we see a path to a rate cut later in the year.” Donald Trump’s statement that “WE ARE GETTING A TOTAL OF 55% TARIFFS” from China has caused some confusion, as the truce agreed last month in Geneva had lowered tariffs to 30%. But, this 55% total also includes pre-existing trade levies, it seems. A White House official has told Reuters said the agreement allows the U.S. to charge a 55% tariff on imported Chinese goods. This includes a 10% baseline “reciprocal” tariff, a 20% tariff for fentanyl trafficking and a 25% tariff reflecting pre-existing tariffs. China would charge a 10% tariff on U.S. imports, the official said. More here. Trump’s claim that the US is ‘getting’ the tariffs is questionable, as they will be paid by US companies when they import goods from China (despite claims that the country shipping the goods pays them). Donald Trump will be pleased to learn that eggs prices fell last month. The US president has repeatedly claimed that egg prices, which surged after a bird flu outbreak last year, have fallen on his watch (a claim which CNN dubbed a lie in April) Today’s inflation report shows that egg prices fell by 2.7% in May, helping to pull the index for meats, poultry, fish, and eggs down by 0.4%. But over the last 12 months, egg prices have increased by 41.5%, hitting US households hard in the pocket. Trump recently claimed that egg prices were down 400% (implausible, as that would mean retailers paying shoppers to take them away…). On a monthly basis, the US consumer prices index rose by 0.1% in May, lower than the 0.2% rise expected. More expensive housing pushed up the cost of living; the index for shelter rose 0.3% in May. Food prices rose by 0.3%, while energy prices fell 1% thanks to cheaper gasoline. Newsflash: Annual inflation across the US rose in May, but not as much as expected. The consumer prices index rose by 2.4% over the last 12 months, the US Bureau of Labor Statistics has reported. That’s up from 2.3% in the year to April, but lower than the 2.5% which economists had predicted. Energy prices decreased by 3.5% over the last year, while the food index increased 2.9% over the last year. Core inflation (which strips out food and energy) rose 2.8% over the last year, matching April’s reading. Newsflash: Donald Trump has announced that the US trade deal with China is “done”, following the talks in London this week. He explains that the US will get the access to Chinese rare earth minerals, and magnets, which his officials had been pushing for at Lancaster House on Monday and Tuesday. In a post on his Truth Social site, Trump also declares that the relationship with China is “excellent” (previously he has claimed that negotiating with Beijing was ‘not easy’). Today, he writes: OUR DEAL WITH CHINA IS DONE, SUBJECT TO FINAL APPROVAL WITH PRESIDENT XI AND ME. FULL MAGNETS, AND ANY NECESSARY RARE EARTHS, WILL BE SUPPLIED, UP FRONT, BY CHINA. LIKEWISE, WE WILL PROVIDE TO CHINA WHAT WAS AGREED TO, INCLUDING CHINESE STUDENTS USING OUR COLLEGES AND UNIVERSITIES (WHICH HAS ALWAYS BEEN GOOD WITH ME!). WE ARE GETTING A TOTAL OF 55% TARIFFS, CHINA IS GETTING 10%. RELATIONSHIP IS EXCELLENT! THANK YOU FOR YOUR ATTENTION TO THIS MATTER! Over in parliament, Rachel Reeves will soon begin delivering the government’s spending review to MPs, outlining spending plans for the next few years. We’re live-blogging it here: The review will not be a “game changer” for the markets, predicts Fawad Razaqzada, market analyst at City Index. In the UK, Chancellor Rachel Reeves will unveil her Spending Review—but expectations are low. The headline takeaway is simple: the coffers are tight. Departmental spending is set to grow by just 1% in real terms annually over the next three years, with most of that going to health, defence, and education. This isn’t a full Budget, and with no Office for Budget Responsibility forecast alongside it, there’s not much scope for headline-grabbing fiscal moves. Don’t expect fireworks in gilts or the pound as a result. UK pub chain Fuller has pledged to take a cautious approach to increasing prices, as it juggles rising costs. CEO Simon Emeny said this morning: “Like everybody in the sector, we have had to raise prices during April to help us navigate this extra cost burden placed on us by the chancellor, but we’ve kept those as low as possible,.” That cost budgen includes the rise in employers’ social security contributions and the minimum wage. This led Fuller’s to hike the price of a pint of beer by abut 15p across its bars after being hit with £8 million in extra staff costs. Emeny was speaking after Fuller reported that pre-tax profits more than doubled in the last year, to £33.8m, from £14.4m. China has welcomed the progress made at its trade talks with the US in London this week. Chinese vice premier He Lifeng, who led Beijing’s delegation, has said the US should resolve trade disputes with China through equal dialogue and mutually beneficial cooperation, the Xinhua newswire reports. In a statement published by state broadcaster China Central Television (via Bloomberg), He explained: “As a next step, the two sides should follow the important consensus and requirements reached by the two heads of state on the phone call, further play a good role in the China-US economic and trade consultation mechanism.” Back in the City of London, shares in UK housebuilders are rising as investors anticipate higher government spending slowing into the sector. Rachel Reeves is expected to announce a near-doubling of spending on affordable housing in today’s spending review, in an attempt to hit the government’s house-buildinng targets. The chancellor will announce nearly £40bn worth of grants to be spent over 10 years for local authorities, private developers and housing associations – a major increase on the previous programme. Shares in Persimmon and in Barratt Redrow, two of the UK’s largest housebuilders, have jumped around 1.8%, putting them in the list of top risers on the FTSE 100 this morning. Smaller rivals Vistry (+8.4%) and Crest Nicholson (+5.9%) are among the top risers on the FTSE 250 index of medium-sized companies. Vistry is focused on social housing. Richard Beresford, chief executive of the National Federation of Builders (NFB), has welcomed the plan, saying: “Rachel Reeves is backing up her planning reforms with the funding required to build the social and affordable homes the nation so desperately needs. This is a significant step in the right direction and demonstrates that both the Prime Minister and Chancellor have a long-term plan to fix the housing crisis and are not afraid to share the limelight for the good of the nation.” Elon Musk’s admission of regret rather undermines the theory that his attacks on Donald Trump were part of a ‘grand strategy’. Earlier this week, Morgan Stanley analysts suggested that Musk might have been executing a cunning plan to focus attention on the US national debt. (which will be pushed higher by the tax cuts in Trump’s spending bill). Shares in Tesla are set to rally in New York later today, after Elon Musk attempted to patch up relations with Donald Trump. Tesla’s shares are up 2.5% in premarket trading at $334.28, as traders react to Musk’s expression of regret over his criticism of Trump last week. Sources close to Musk had said his anger has started to subside, and that they believe he may want to repair his relationship with Trump, Reuters reports. Elon Musk has said he “regrets” some of his posts about Donald Trump, in an apparent attempt to patch up relations with the US president. In a post on X, Musk has written: I regret some of my posts about President @realDonaldTrump last week. They went too far. This abrupt U-turn comes almost a week after the world’s richest man launched a fierce attack on Trump, calling his “big, beautiful bill” a “disgusting abomination”. Musk also alleged, without supplying evidence, that Trump was implicated in the Jeffrey Epstein files, a claim denied by Epstein’s former attorney [Musk appears to have subsequently deleted this post]. Trump hit back at Musk last week, claiming the Tesla CEO had “lost his mind” and threatening to cancel Musk’s US government contracts and subsidies. The row hit Tesla’s share price last week, and had a significant impact on Musk’s wealth – according to the Bloomberg Billionaires Index, he has lost approximately $90bn of his fortune. Richard Hunter, head of markets at interactive investor, says this week’s talks in London between the US and China “represent progress”, despite the lack of detail about what was agreed: “Apparently constructive talks between the US and China have put markets on a firmer footing, as investors hope that the worst of the tariff turbulence may have passed. Details of the framework which has been agreed in principle were patchy and in any event yet to be signed off by both Presidents. Chinese exports of rare earth minerals are likely to have been high on the agenda, although at this stage it has not become apparent what China may have negotiated in return. Even so, the two days of talks represent progress and the hope is now that the more conciliatory momentum can be maintained. European stock markets have opened higher, as the US-China trade framework agreement lifts the mood. In London, the FTSE 100 share index has gained 22 points, or 0.25% to 8,875 points. That takes the index towards its record high of 8,908 points, set in March before trade war turmoil hit the markets. Prudential (+2.3%) and Standard Chartered (+2%), which are both focused on Asia-Pacific markets, are leading the risers. Mining stocks are also rising, reflecting hopes that a damaging trade war that would hurt demand for commodities can be avoided. France’s CAC and Germany’s DAX share indices are both up around 0.2%. Charu Chanana, chief investment strategist at Saxo in Singapore, says: “Markets will likely welcome the shift in tone from confrontation to coordination. But with no further meetings scheduled, we’re not out of the woods yet. The next step depends on Trump and Xi endorsing and enforcing the proposed framework. “It’s important not to mistake this tactical de-escalation for a full reversal of strategic decoupling. The underlying competition around technology, supply chains, and national security remains very much intact. New issues can always emerge, and the real test will be how far this “new old deal” is implemented.” Shares have risen in China, as traders appear to welcome the trade framework agreed in London last night. The CSI 300 index, which tracks the largest stocks on the Shanghai and Shenzhen, is up around 0.8% in late trading. Hong Kong’s Hang Seng index is up 1%, while South Korea’s KOSPI has gained 1.3%. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, reports that “Risk sentiment across Asian markets is broadly positive”, as “trade headlines are striking an optimistic tone this week”. Josh Lipsky, senior director of the Atlantic Council’s GeoEconomics Center in Washington, fears that the US and China are still a long way from a wide-ranging trade deal. Lipsky posted on X: When you step back and think about the announcement in London we’ve gone from a trade war to an export control skirmish but never resolved the trade piece. Now there’s a truce on export controls but the idea of a broader trade agreement in August seems further away than ever. The US and Mexico may be close to a breakthrough in negotiations over steel tariffs. Reuters are reporting that the two countries are negotiating a deal to reduce or eliminate President Donald Trump’s 50% steel tariffs. An industry source familiar with the talks said that a likely outcome would include a quota arrangement, under which a specified volume from Mexico could enter duty free or at a reduced rate and any imports above that level would be charged the full 50% tariff. Reuters add that it’s unclear whether the deal would eliminate tariffs altogether for in-quota steel import volumes from Mexico or reduce them to a lower level, and that the specific volume level of the quota also was not yet determined. Reaction to the US-China agreement is flooding in this morning, as analysts digest the overnight news that a ‘framework’ has been agreed. Jim Reid, strategist at Deutsche Bank, says there is “perhaps a little disappointment” that we don’t have more details of the agreement, telling clients: The main details came from Commerce Secretary Lutnick, who said that “We do absolutely expect that the topic of rare earth minerals and magnets” will be resolved and that export controls implemented by the US should come down as China approves relevant export licenses. China’s trade representative Li Chenggang said that the US and Chinese delegations will now take the proposal back to their respective leaders, with Lutnick noting that “once the presidents approve it, we will then seek to implement it”. At the same time, there was no evidence of progress on topics such as the fentanyl-related 20% tariffs on China that the US has implemented since February. So while the mood music has stayed positive, investors may be wary of the pattern that emerged during the previous US-China trade talks in 2018-19, when apparently constructive in person meetings seemed to take a step back as the negotiating teams returned to their capitals. So there’s perhaps a little disappointment this morning that we haven’t yet got a bigger announcement, even though there’s time to hear the full conclusions of the meeting. Chris Weston, head of research at brokerage Pepperstone, agrees that “the devil will be in the details”, adding: “The details matter, especially around the degree of rare earths bound for the US, and the subsequent freedom for US produced chips to head East, but for now as long as the headlines of talks between the two parties remain constructive, risk assets should remain supported.” Lin Gengwei, CEO of Rain Tree Partners in Singapore, called the agreement a “temporary achievement”, adding: “The U.S. will not completely remove restrictions on chip exports to China, but may relax the curbs in response to pressure from both Beijing and the domestic semiconductor sector.” Zeng Wenkai, chief investment officer at Shengqi Asset Management in Hong Kong, suggests more countries should stand up to the US in trade discussions: “The market likely anticipated this — Trump is just TACO (Trump always chickens out).” “Look at how countries are negotiating with the U.S. these days; it’s no longer like how Vietnam approached things early on. Japan and South Korea are taking a tougher stance. People have realised that kneeling gets you nowhere — in fact, it only invites more bullying.” Tony Sycamore, market analyst at IG, says the US and China have found a way to quell trade tensions which risked spiralling out of control last week. “If we keep the terms of the Geneva Agreement, we’re looking at US tariffs on Chinese goods staying at 30% for a period of time and Chinese tariffs on US goods at 10%. So that’s down from 145% and 125% respectively. That would be fantastic. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. “Jaw, jaw is better than war, war,” as Harold Macmillan once remarked. And after two days of talking in London, the US and China have managed to patch up their trade conflict truce. Just before midnight last night the two countries agreed a framework that, it is hoped, will ease tensions between the two economic superpowers. It will reinforce their initial agreement made in Geneva a month ago, once presidents Donald Trump and Xi Jinping have approved it. Speaking at Lancaster House last night, US commerce scretary Howard Lutnick said the trade framework and implementation plan agreed with China in London should result in restrictions on rare earths and magents being resolved. That had been a key demand for the US side, worried that American companies were being starved of vital supplies. Lutnick told reporters the US negotiating team will take the framework back to Trump to get his approval, and then hope to implement it. China’s vice commerce minister Li Chenggang described the talks as “rational and candid”, telling reporters: “The two sides have, in principle, reached a framework for implementing the consensus reached by the two heads of state during the phone call on June 5th and the consensus reached at the Geneva meeting.” The talks, which began on Monday morning, took longer than expected – with the two sides sustained by deliveries from restaurant chain Ottolenghi, McDonald’s, Burger King and KFC. Investors are now waiting for details of the agreement, and confirmation that it will satisfy Xi and Trump. Traders are also anticipating the latest US inflation report, which may show that the trade war has driven up prices in the shops. Economists predict the US CPI index will have risen to 2.5%, from 2.3%. While in London, chancellor Rachel Reeves will deliver the government’s spending review, outlining day-to-day departmental spending for the next three years. The agenda 12pm BST: US weekly mortgage applications data 12.30pm BST: Chancellor Rachel Reeves to deliver UK spending review 1.30pm BST: US inflation report for May</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Donald Trump has endorsed the US-China trade deal struck in London that will ramp up supplies of rare earth minerals and magnets. The US president disclosed the pact would also facilitate Chinese students’ access to US colleges. Trump also posted that he and president Xi will “work closely together to open up China to American Trade”</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>With the US-China trade talks at Lancaster House set to run into the evening, it's time for a round-up of today’s main stories: Brietbart’s John Carney reports that trade talks are on a break, and will resume in two and a quarter hours…. US sources have confirmed that talks are ongoing at Lancaster House. Treasury Secretary Scott Bessent has to return to Washington to give testimony tomorrow so they will wrap later tonight but as yet it is not clear, after more than 12 hours of talks, whether resolution has been struck on any issues on the table. Hopes of more interest rates cuts this year also pushed the FTSE 100 higher today, reports AJ Bell head of financial analysis Danni Hewson: “Hopes that lacklustre jobs data might give rate setters the ammunition they need to deliver further cuts helped to propel London’s blue-chip index to within a whisker of a fresh record close. “The last time the FTSE 100 displayed this kind of form was back in March, before Donald Trump’s White House whiteboard moment and when the UK economy was still delivering growth, even it if was looking a little sluggish. “It was no shock to see UK housebuilders storming away as expectation that mortgage rates could become more affordable fuelled investor appetites. Those expectations were fuelled by this morning’s weak jobs data, showing a drop in employees on payrolls and a rise in unemployment. Newsflash: Britain’s blue-chip share index has ended the day close to its all-time closing high. The FTSE 100 index has closed at 8853 points, up 20 points or 0.24% today. That take the ‘Footsie’ close to its previous alltime closing high, of 8871 points, set in early March. Housebuilders led today’s rally, such as Persimmon (+5.95%) and Barratt Redrow (+5.6%), after rival Bellway reported strong sales numbers this morning and raised its forecast for the number of homes it expects to build this financial year Retailer Marks &amp;amp; Spencer (+3.8%) had a good day too, after resuming orders on its website after weeks of disruption caused by a cyber attack. The FTSE 100 has made a strong recovery over the last two months, after slumping in early April after Donald Trump announced steep tariffs on US trading partners. At its recent low, on 9 April, the FTSE 100 closed at 7,679 points. As Trump rowed back, shares recovered. It’s not a completely clear picture, however, as a US Treasury spokesman has said the trade talks are still ongoing…. The United States and China have concluded trade talks in London, a U.S. official told Reuters on Tuesday. That follows two days of negotiations in the UK, as both countries seek a breakthrough on export controls. We may not get a closing high on the Footsie today, I fear. With around 40 minutes trading to go, the FTSE 100 is now trading at 8857 points – up 0.3% today. Although that’s a gain of 25 points, it leaves the share index almost 15 points shy of its previous closing high, of 8871 points, set three months ago. As the talks continue, here’s a snap from Lancaster House of US and China flags pictured together Kenya’s central bank has lowered its growth forecast for this year today, underlining the impact of the US trade war. The bank has revised down its 2025 economic growth forecast to 5.2% from a 5.4% forecast given at its last policy meeting in April “on account of higher tariffs on trade“. It also lowered interest rates for the sixth time in a row, cutting Central Bank Rate by 25 basis points (a quarter of one percentage point) to 9.75%. Bond trading giant PIMCO has released its five-year outlook on the global economy today, warning that investors must navigate a new global order. PIMCO say: The traditional world order – in which economics shaped politics – has been turned on its head, with politics now driving economics. Sharp policy shifts are transforming long-standing trade, security, and economic alliances, with the effects set to reverberate for years. One consequence, they say, is that demand for US assets compared to those of other countries could drop in a “multipolar world” of changing trade dynamics and policy priorities. They suggest that the US dollar could weaken further, but argue it is “almost impossible” the dollar could lose its global reserve currency status over the next five years, given the lack of realistic alternatives. Just in: The World Bank has slashed its global growth forecast for 2025 by 0.4 percentage point to 2.3%, blaming higher tariffs and heightened uncertainty. In its twice-yearly Global Economic Prospects report, the World Bank warned that trade tensions are a “significant headwind” for nearly all economies. It has lowered its forecasts for nearly 70% of all economies - including the United States, China and Europe, as well as six emerging market regions - from the levels it projected just six months ago. Worryingly, the World Bank reckons the 2020s are on course to be the weakest decade for the global economy since the 1960s. Here’s the full story: The US stock market has risen slightly at the start of trading, as investors hope for progress at the trade talks in London. The S&amp;amp;P 500 share index is up 7 points, or 0.12%, at 6,012.95 points. However, the Dow Jones Industrial Average, which contains 30 large US companies, is down 0.02%. Fawad Razaqzada, market analyst at City Index and FOREX.com, says market sentiment has been improved by the US-China trade talks: Investors appear cautiously optimistic that the US and China may be on the brink of putting some of their longstanding differences aside, with high-level trade talks taking place in London. This comes after last week’s “very positive” phone call between Presidents Trump and Xi. With equity markets remaining largely in a “buy-the-dip” mode, investors may soon start trimming their exposure to haven assets like gold… With talks underway again after lunch, here’s Associated Press’s latest take on the trade talks in London: The U.S. and China held a second day of talks Tuesday in London aimed at easing their trade dispute , after President Donald Trump said China is “not easy” but the U.S. was “doing well” at the negotiations. A Chinese delegation led by Vice Premier He Lifeng met U.S. Commerce Secretary Howard Lutnick, Treasury Secretary Scott Bessent and Trade Representative Jamieson Greer for several hours on Monday at Lancaster House, an ornate 200-year-old mansion near Buckingham Palace. Wang Wentao, China’s commerce minister, and trade negotiator Li Chenggang are also in Beijing’s delegation. Lutnick said as he arrived Tuesday morning that the talks were “going well,” and he expected them to continue all day. Asked late Monday how the negotiations were going, Trump told reporters: “We are doing well with China. China’s not easy.” The two sides are trying to build on negotiations in Geneva last month that agreed to a 90-day suspension of most of the 100%-plus tariffs they had imposed on each other in an escalating trade war that had sparked fears of recession . Since the Geneva talks, the U.S. and China have exchanged angry words over advanced semiconductors that power artificial intelligence, visas for Chinese students at American universities and rare earth minerals that are vital to carmakers and other industries. Trump spoke at length with Chinese leader Xi Jinping by phone last Thursday in an attempt to put relations back on track. Trump announced on social media the following day that the trade talks would resume in London. China, the world’s biggest producer of rare earths, has signaled it may ease export restrictions it placed on the elements in April, alarming automakers around the world who rely on them. Beijing, in turn, wants the U.S. to lift restrictions on Chinese access to the technology used to make advanced semiconductors. Trump said that he wants to “open up China,” the world’s dominant manufacturer, to U.S. products. “If we don’t open up China, maybe we won’t do anything,” Trump said at the White House. “But we want to open up China.” The London stock market continues to close in on its previous record high. The FTSE 100 is now up 48 points, or 0.55%, at 8880 points – which puts it above its previous closing high, and not far from the intraday high of 8,908 points set in March. Housebuilders, M&amp;amp;S and oil producers continue to dominate the risers. The trade talks at Lancaster House appear to have paused for lunch. Chinese vice premier He Lifeng left the talks a few minutes ago. Bloomberg’s Daniel Flatley reports that he is having lunch offsite, and will return around 2pm UK time. European leaders promised last month a “massive” increase in sanctions against Russia if Vladimir Putin refused a ceasefire. A few weeks on as the deadly bombardment of Ukraine continues, the European Commission will outline its response. European Commission president Ursula von der Leyen and EU foreign policy chief Kaja Kallas are later on Tuesday expected to present the EU’s 18th round of sanctions against Russia since the full-scale invasion of February 2022. Most of the measures, which have been trailed by von der Leyen, target Russia’s banking and energy sectors, as well as tightening up measures against the shadow-fleet, hundreds of old and poorly-maintained tankers that enable Russia to export oil to countries such as India, above the western price cap of $60. One week ahead of the meeting of the G7, the Commission proposes lowering the price cap to $45 per barrel. The current price cap was agreed through the G7 during Joe Biden’s presidency. For the first time EU sanctions are also targeted at the captain of a shadow fleet tanker, an Indian national. Officials hope this will have a chilling effect, discouraging others from manning these tankers that fly under a flag of convenience. Other proposals include: Sanctions on 70 other shadow fleet vessels, bringing the total under designation to more than 400. A ban on doing business with Nordstream I and II in order to prevent any future gas flows through these pipelines connecting Russia to the EU. Adding 42 names (9 people and 33 entities) to the sanctions list, taking the total of people and organisations subject to asset freezes and travel bans subject to more than 2,500. Banning 22 more banks from transacting with EU counterparts, including five China-based entities. Hopes of success at the US-China trade talks today may be pushing the oil price higher. Brent crude, the international benchmark, has risen by 0.5% today, or 36 cents per barrel, to $67.40 per barrel. Harry Tchilinguirian, group head of research at Onyx Capital Group, explains: “There’s a sense of optimism around these trade talks, the market is waiting to see what this will produce and that is supporting prices.” Economic uncertainty is set to drag on Spain’s economy this year. The Spanish central bank has predicted that Spain’s GDP will grow at the slowest pace in almost two years this quarter, a blow to one of the eurozone’s faster-growing members in recent years. Bloomberg has the details: Gross domestic product will rise by 0.5%-0.6%, the Bank of Spain said Tuesday. While still “relatively high,” it could point to the start of a slowdown, it said. GDP increased by the upper end of that range in the first three months — the smallest advance since 2023. “Consumer confidence has been declining markedly since the start of the year,” Chief Economist Angel Gavilan said. US small-business confidence improved last month, as bosses welcomed the de-escalation in trade tensions between Washington and China. The National Federation of Independent Business has reported that its Small Business Optimism Index increased three points to 98.8 last month, rising for the first time since December. The improvement was driven by a pick-up in business conditions and sales expectations. NFIB chief economist Bill Dunkelberg says: Although optimism recovered slightly in May, uncertainty is still high among small business owners. While the economy will continue to stumble along until the major sources of uncertainty are resolved, owners reported more positive expectations on business conditions and sales growth. The commerce ministers of the US and China have both arrived for day two of their trade talks: US commerce secretary Howard Lutnick has told reporters that trade talks with China that are taking place in London were going well, Reuters reports. Lutnick also indicated that the meeting at Lancaster House is expected to last all day today. Reminder: the two sides talked for over six hours yesterday, with Monday’s deliberations fuelled by a supper from one of Yotam Ottolenghi’s restaurants: Back in the City, Marks &amp;amp; Spencer is helping to push the FTSE 100 share index towards a new record high. M&amp;amp;S shares are among the top risers this morning, up 3.7%, after it resumed online orders after its recent cyberattack. But rival Next is pulling the index the other way! Next’s shares are down 2%, making it the top faller – traders may be concluding that its short-term sales boost from M&amp;amp;S’s disruption is now over… Chinese and US leaders have resumed talks at London’s historic Lancaster House for a second day to try and resolve the trade dispute triggered by Donald Trump’s imposition of tariffs on all imports from the country. Select outlets including Fox News, Chinese TV, the BBC and Bloomberg but not the Guardian, Sky News or LBC, have been allowed inside the security perimeter, to record any press briefing that may take place later today. There are expectations there may be some sort of truce in relation to China’s export restrictions on rare earths and the US’s restrictions on the export of semi-conductors from the US to China, but not an overall deal on the 145% tariffs imposed by the US [currently lowered to 10% under the temporary truce agreed last month]. China, like 60 other countries, is currently in “negotiations” on tariff deals but rare earths and critical raw materials crucial for military, auto and medical sectors across the world are just one of Trump’s challenges. He is also seeking to control the import of cheap Chinese steel and aluminium products with critics warning the reduction in supply is already hitting manufacturing in the US. Most European markets have edged high this morning as investors patiently waited for news on US/China trade talks,” says Russ Mould, investment director at AJ Bell. “Where there is still a sense of cautiousness around how to position portfolios for the longer term, there were enough corporate news flow to spur trading in a range of stocks. “UK housebuilders were at the top of the wish list for many investors after Bellway reported ‘robust’ spring trading. It was enough to drive a rally in the sector, putting the likes of Persimmon, Barratt Redrow and Taylor Wimpey at the top of the FTSE 100 risers’ list. “The blue-chip UK index moved 0.4% higher to 8,868, helped by strength in energy producers Shell and BP amid oil price resilience, and Rolls-Royce moving up on success with its nuclear operations.” The UK stock market rally is also being driven by bargain-hunting investors. “UK stocks are among the cheapest in Europe,” said Georges Debbas, head of European equity derivatives strategy at BNP Paribas Markets 360 (via Bloomberg). Debbas added: “The country is also the most friendly to the US, as it’s the only one to have a firm trade agreement in place. That allows you to have a more constructive view on the market.” US-China trade talks are the main focus for investors as they continue in London after a “fruitful” session on Monday, reports Neil Wilson,UK investor strategist at Saxo Markets: It’s hoped that the deal with see the US ease export restrictions of chips while China will release its rare earth minerals. A good outcome could send Wall Street to a fresh record high, with the S&amp;amp;P 500 finishing marginally higher on Monday a few points above the 6k level. Apparent concessions for Western automakers last week suggest a deal is in the offing. In the City, the London stock market is heading back towards its alltime high. The FTSE 100 share index has gained 41 points, or nearly 0.5%, in early trading to 8874 points – slightly above its previous record closing high. The Footsie’s record intraday high, 8,908.8 points, was set in early March, before trade war fears send shares tumbling. Shares have recovered since slumping in early April (when the index fell as low as 7544 points), as Donald Trump cheered traders by pausing or reversing aspects of his trade war. Housebuilders are leading the risers this morning, after Bellway reported “robust trading through the spring selling season” this morning. Bellway raised its outlook for volume output and average selling price this year Jason Honeyman, Bellway’s chief executive, says: “Bellway has delivered a solid trading performance, and we are on track to deliver strong growth in volume output and profits in the full financial year. We have a healthy forward order book and outlet opening programme, which will serve as a platform for further growth in FY26. I remain confident that, supported by the Group’s operational strengths, land bank depth and an increased focus on cash generation and capital efficiency, Bellway can capitalise on the positive fundamentals of our industry and deliver volume growth, improved returns and ongoing value creation for shareholders.” In other trade news, China has extended a high-profile investigation into imported pork from the European Union by six months. The extension comes just days before the probe, which began a year earlier, was due to wrap up. China has decided to extend the investigation period to December 16 due to the “complexity” of the case, the country’s commerce ministry said in a statement on its website. The probe began last summer, after the EU imposed provisional tariffs on Chinese EV imports coming into the bloc. Minister for employment Alison McGovern has insisted that the government is making progress in helping people into work: “Six months after we launched Get Britain Working, we are already seeing the benefits with economic activity at a record high, with 500,000 more people in employment since we entered office and real wages growing more since July than in the decade after 2010. “People all over the country are benefiting from increased training opportunities and the newly launched Jobs and Careers Service will allow us to test new and innovative approaches to personalise employment support.” But, shadow business secretary Andrew Griffith blamed the increase in companies’ national insurance payments for the rise in joblessness: “It is disappointing but no surprise that unemployment is up again. “Businesses are still absorbing a £25 billion jobs tax but things are about to get even worse as Labour’s £5 billion unemployment bill hits businesses with higher regulation.” Liberal Democrat treasury spokeswoman Daisy Cooper also criticised the rise in employers’ NICs payments: “These figures could not be a clearer signal to the Chancellor ahead of the spending review that the Government must change course. “The Chancellor’s pig’s ear of a jobs tax is crushing the growth potential of our high streets and small businesses, pushing people out of work, and ramping up the benefits bill. “This week, instead of pursuing another round of devastating departmental cuts, the Government needs to take the handbrake off our economy and go for growth.” Elsewhere in UK retail, Mark Ashley’s Frasers Group has confirmed that it is in the race to buy Revolution Beauty and is considering a cash-only offer for the struggling beauty firm, which put itself up for sale last month. Revolution Beauty said on Monday that Frasers is “one of a number of parties conducting due diligence as part of the formal sale process announced on 21 May”. Frasers put out a statement today, confirming its participation in the sale process, but adding that there can be no certainty that an offer will be made. In mid-May, Revolution Beauty warned that it was reviewing funding options before its £32m credit facility runs out in October, pushing shares to a record low. Sales have been weaker than expected in March and April amid worsening consumer confidence affecting its performance in the US. Revolution was set up in 2014 to launch a vast affordable makeup range aimed at young people and priced from £1. It has struggled on the AIM junior market since floating in July 2021 with valuation of almost £500m. Frasers, which owns Sports Direct, has snapped up stakes in several retailers in recent years, including THP, Boohoo, Asos and Mulberry. Government borrowing costs are also dipping as bond prices rise, with traders calculating that today’s weak jobs report makes UK interest rate cuts more likely. Sterling is weakening on the foreign exchange markets, as investors digest the rise in UK unemployment and the drop in payrolls. The pound has dropped by almost a cent against a generally stronger US dollar, to $1.346, its lowest level since the end of May. The drop in the number of payrolled employees in the UK will help to “cement” an interest rate cut in August, argues ING Bank. James Smith, ING’s developed markets economist, told clients this morning: The cooling in the UK jobs market is gathering pace. Wage growth is slowing, too. While the bar for the Bank of England to speed up rate cuts seems to be set fairly high, this data helps cement cuts in August and November. The UK jobs market might be turning a corner – and not in a good way. What stands out from the latest hiring numbers is a sharp 109,000 fall in payrolled employees in May. That is the largest monthly fall outside of the Covid-19 pandemic, since the data began in 2014. However, there’s a fairly significant caveat, which is that this data has a habit of being revised up later on. Back in March, we saw a 78,000 fall, which was later revised up to a drop of 35,000. We’ll have to reserve full judgment until next month. Marks &amp;amp; Spencer has reopened its website to shoppers, six weeks after it was forced to halt online orders after a cyber-attack. The retailer said on its website that customers “can now place online orders with standard delivery to England, Scotland and Wales”. Deliveries to Northern Ireland “will resume in the coming weeks”. “We will resume click and collect, next-day delivery, nominated-day delivery and international ordering in the coming weeks,” it said. Wage growth slowed over the last quarter – which could be another sign of a weakening UK jobs market. Average regular pay rose by 5.2%, in the February-April quarter, compared with a year earlier. That’s down from 5.8% in the previous quarter. Annual growth in total pay (including bonuses), slowed to 5.3%, down from 5.7% in November-January. Once you adjust for CPI inflation, regular pay growth slowed to 2.1% while total pay was up 2.3%. Monica George Michail, associate economist at the NIESR economic research body, explains: Annual regular wage growth remains strong at 5.2% in the three months to April 2025 amidst the rise in national minimum/living wage, according to today’s ONS figures. High service sector earnings growth is contributing to persistent core inflation, which continues to exceed 3%. Unemployment continues to rise, which is expected to ease wage pressures moving forward. However, if wage inflation remains elevated in the coming months, there would be even less room for interest rate cuts by the Bank of England”. The number of vacancies across the UK has fallen, again, making it harder for unemployed people to find a new job. Vacancies fell by 63,000 in the March-May quarter, to 736,000 – the 35th consecutive quarterly decline in a row. There are now 150,000 fewer vacancies than a year ago – lifting the ratio of unemployed people per vacancy to 2.2 in February to April, up from 1.9 in the previous quarter. Unemployment across the UK rose in the last quarter, today’s labour market data shows. The UK unemployment rate rose to 4.6% in the February to April quarter, which is the highest rate recorded since the summer of 2021. That’s a rise from 4.5% in January-March, and also up from 4.4% in the previous quarter. But…. the employment rate has also risen, up 0.1 percentage point over the quarter to 75.1%. How can employment and unemployment both go up? Because the number of people classed as economically inactive (neither in work, nor looking for a job) has dropped – pulling the UK economic inactivity rate down by 0.2 percentage points over the quarter to 21.3%. Newsflash: The number of people on payrolls across the UK has fallen notably, in a sign that the jobs market is weakening. The latest labour force statistics, just released, show that payrolled employment decreased by 109,000 employees (0.4%) in May, compared with April. On an annual basis, there were 274,000 fewer employees last month, compared with May 2024, pulling total payrolls down to 30.2 million. The Office for National Statistics does caution that these estimates are more uncertain than usual; if they’re accurate, though, it indicates that demand for workers at British firms is cooling. The largest decrease was in the accommodation and food service activities sector, a fall of 124,000 employees in the last year, while health and social work added 62,000 employees. ONS director of economic statistics Liz McKeown says: “There continues to be weakening in the labour market, with the number of people on payroll falling notably. Feedback from our vacancies survey suggests some firms may be holding back from recruiting new workers or replacing people when they move on. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Trade talks between the US and China are set to resume in London today, as officials push for a breakthrough over shipments of technology and rare earth elements. After more than six hours of talks on Monday, negotations will resume at Lancaster House later this morning. Investors are hopeful of a breakthrough that could continue to ease tensions between the two economic superpowers. President Donald Trump has indicated that the first day of talks were encouraging. He told reporters that “We are doing well with China. China’s not easy….I’m only getting good reports.” The US are unhappy that China has not released crucial rare earth minerals, and magnets, as rapidly as hoped since the two countries agreed an initial trade pact in Geneva a month ago. Treasury secretary Scott Bessent told reporters in London they had a “good meeting”, Bloomberg reports, while commerce secretary Howard Lutnick called the discussions “fruitful.” The agenda 7am BST: UK labour market report 10.15am BST: FCA CEO Nikhil Rathi and FCA chair Ashley Adler testify to Treasury Committee 2.30pm BST: World Bank to release latest economic forecasts</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Britain's blue-chip share index has ended the day close to its all-time closing high. The FTSE 100 index has closed at 8853 points, up 20 points or 0.24% today. Housebuilders led today’s rally, such as Persimmon (+5.95%) and Barratt Redrow (-5.6%) Kenya's central bank has lowered its growth forecast for this year.</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>There were early signs that the March GDP figures were not going to be good. To start with, the Bureau of Statistics’ new measure of household spending that covers about two-thirds of all household spending had already revealed that spending for the quarter was flat compared with a 1.6% jump in December quarter last year. So household spending was worse. Then last week the private capital expenditure figures revealed a 0.1% fall in investment in buildings and engineering, compared with a 0.2% rise in the December 2024 quarter. So private investment was worse. On Tuesday, the balance of payments revealed that trade in the first three months of this year was expected to “detract 0.1%pts from the March quarter” compared with adding 0.2%pts in December. So trade was worse. Just to top it off, on Tuesday the figures for government spending and investment showed that public demand fell in the March quarter and would also detract 0.1%pts from GDP growth compared with it adding 0.2%pts to GDP growth last December. So the impact of the public sector was worse. To be honest, once you take away households, private investment, trade and government spending, you really are not left with much. So it came to be. In the March quarter of this year, GDP growth was just 0.2%, down from 0.6% in the December quarter. The only good news is the March quarter last year was pretty dire as well, so all up it meant annual growth remained steady at a still extremely weak 1.3%. If the graph does not display click here This weak growth meant that per capita GDP fell again – the ninth quarter out of the past 11. This is not a good state of affairs, and certainly does not accord with the views of the Reserve Bank back in April when it looked at the first three months of this year and suggested that “the limited information available about activity in early 2025 suggested that the pick-up in GDP growth had been sustained”. Ahh well, at least they can say they were not wrong for long? Well no. In the minutes of the May board meeting released this week the RBA now suggested that “GDP growth had increased in the December quarter 2024 and year-ended growth looked to have picked up a little further in the March quarter”. Going from 1.3% growth in December to 1.3% growth in March is hardly “picked up”. The May Statement on Monetary Policy also predicted annual GDP growth in June of 1.8%. To get to that level, the economy would need to grow in April, May and June by 0.7% – the strongest quarter growth for three years. Here’s hoping … So what drove the growth that was there? Households were the biggest contributor to growth – although as in all things the context is key. Their contribution to the growth of the economy in the March quarter was about half what you would normally expect. If the graph does not display click here And a big reason for the increase in consumption was a jump in spending on electricity, gas and other fuels – due to the ending of some of the state government energy rebates (which also had an impact on inflation). That is not the type of spending you want to see driving households. All up the level of household consumption is well down on what would have been expected before the pandemic. The Reserve Bank’s interest rate rises did their job – they snuffed out spending. Clearly more rate cuts are needed to undo that damage and it is quite extraordinary that the RBA is so sanguine about it all: If the graph does not display click here The overall level of household spending and private-sector investment quickly rules out the use of the phrase “strong” when searching for a term to describe what is going on: If the graph does not display click here And that’s not surprising because while home loan rates have come down, the average discounted rate is still more than 300 basis point higher than it was at the start of 2022. But for small business owners taking out an overdraft loan, things are even worse – the rate is 400 basis point higher: If the graph does not display click here But let us not be too negative. One very good piece of news is that household living standards are on the rise. After two years, finally household disposable income per capita is above the level it was in March 2020: If the graph does not display click here One reason for this was there was a very slight decline in the level of mortgage repayments, due to the rate cut in February. This cut actually helped increased living standards in the first three months of this year. But that was a very small repair, given since March 2022 mortgage repayments have contributed about 63% of the fall in living standards: If the graph does not display click here That’s a sizeable chunk and it reinforces the damage that is done when the RBA so badly misreads the economy as it has. These figures highlight that not only should the Reserve Bank have cut rates in April but having made that error it compounded it by not cutting rates by at least 50 basis points last month. So far this year the RBA has kept misreading the economic situation and erred on the side of caution. Let us hope these weak figures spur it to cut rates when it meets next month and not suggest it still needs more time to see what is going on. Greg Jericho is a Guardian columnist and policy director at the Centre for Future Work</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>In the March quarter of this year, GDP growth was just 0.2%, down from 0.6% in the December quarter. The Reserve Bank’s interest rate rises did their job – they snuffed out spending. Clearly more rate cuts are needed to undo that damage and it is quite extraordinary that the RBA is so sanguine about it all.</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Time to recap. Global policymakers continue to count the cost of Donald Trump’s trade wars. The governor of the Bank of England has told MPs that the global trade system has been ‘blown up’, and that fragmenting the world trading system is negative for world growth and world activity. Andrew Bailey told MPs: “The overall picture on trade now I’m afraid is one where the rules-based system is sort of dead. That has very serious consequences for the global economy.” Bailey also warned that the future path of UK interest rate cuts was shrouded in a lot more uncertainty. The OECD has warned that global economic growth is slowing more than expected, as the trade war weighs on the world economy. It now expects global growth will slow from 3.3% last year to 2.9% in 2025 and 2026. The OECD also downgraded its expectations for the UK economy this year and next from a forecast made in March, pushing down UK growth from 1.4% to 1.3% in 2025 and from 1.2% to 1% next year. China’s factory output fell last month, as manufacturers were hit by falling orders and weaker export demand. The US private equity group KKR has pulled out of a deal to inject fresh equity into Thames Water, leaving the troubled supplier’s future in doubt and increasing the prospects of a temporary nationalisation. A review of the water industry in England and Wales has found that its “deep-rooted, systemic” problems are the fault of companies, the government and industry regulators. UK ministers could give the go-ahead to the new Sizewell C nuclear power plant in Suffolk within weeks, according to reports. Wall Street trading has begun with little drama, as tariff fears continue to weigh on the New York stock market. The Dow Jones industrial average is up 13 points, or 0.033%, at 42,319 points. The broader S&amp;amp;P 500 index is 0.03% higher. Traders are looking for signs of progress in trade talks between the US and its trading partners, and also digesting this morning’s growth forecast downgrade from the OECD. Cyber hackers have claimed two more corporate victims. Fashion brand The North Face and luxury jeweller Cartier have become the latest retailers to report having customer data stolen in cyber attacks. The North Face has told some customers that it suffered “a small-scale credential stuffing attack” on 23 April, in which attackers used email addresses, usernames or passwords stolen from another company to long into its users’ accounts. Cartier has told its customers that “an unauthorized party gained temporary access to our system and obtained limited client information.” Back at parliament, Bank of England governor Andrew Bailey has told MPs that the rules-based, multilateral trade system that has underpinned the global economy has been ‘blown up’ by Donald Trump’s trade wars. During his testimony to the Treasury committee this morning, Bailey explained how the overall picture of global trade has been significantly disrupted over the last few months. This will have serious implications, he argues, unless policymakers can rebuild that rules-based system. Bailey explained that over recent decades, a pattern of world trade agreements had been build up which led to a lowering of tariffs. It was initally based, after the second world war, on the GATT which became the World Trade Organisation. Govenor Bailey warned: I’m afraid that system has now, really been blown up to a considerable degree by all of this. That has very serious consequences for the world economy, he continued, while also acknowledging that some of the Trump administration’s criticism of that system are well-founded. As Bailey put it: We can’t say the US administration is just wrong-headed. There are things that have gone on in this whole trade picture which, I think, do point to the stress that that system has been under. But he adds, there will be “very serious implications for the world economy” if policymakers abandon that system and say it’s never coming back. He cites the example of ‘most-favoured nation status’, which means that a country offer the same trade terms to all trading partners. [The unilateral tariffs which Donald Trump announced would be imposed on US trading partners in early April were clearly at odds with the concept of MFN status, before he paused them for 90 days]. Bailey says: That has now gone, it just isn’t part of the current picture. That has very serious implciations. He argues that policymakers need to “come back to the multilateral table”, admit there were problems with the old system, and work very hard to fix those problems, adding: If we abandon it, we’re into a much more difficult world. Concerns over Thames Water’s future continue to mount, after potential rescuer KKR walked away from a deal to inject fresh equity (see early morning post). Lena Swedlow, campaigns manager of cross-party campaign group Compass, say’s KKR’s about-turn is a victory for Thames’s customers, arguing that the company should be under public ownership: “KKR pulling out of negotiations with Thames Water is a victory for the people of the region for whom it is an essential resource. It’s a victory for the work of the Thames Water Emergency Board in bringing together households, workers, local government reps, environmental groups, and experts who should be included in decisions about the future of water companies. But it shouldn’t be a sigh of relief. A company with their record should never have been an option to take over a vital resource for millions of us. “The Government proved that taking essential industries into direct control was possible with Scunthorpe Steelworks back in April. Thames Water are in crisis as a direct result of private investment - public ownership is the only option.” Union UNISON’s head of environment Donna Rowe-Merriman says ministers must be decisive, saying: “The situation at Thames Water can’t go on. Customers and staff are being failed at every turn and deserve better. With the options running out, the government must take decisive action sooner rather than later. The company’s been saddled with billions of pounds of debt by private equity firms after huge payouts to shareholders and bosses. Thames Water staff need certainty about the firm’s future and billpayers need assurances about soaring prices. The Cunliffe Review highlights once again that the water industry is broken. Failure to fund regulators properly, and give them the powers they need, has left the sector mired in financial turmoil and sewage spills. Only sustained investment will ensure a clean and safe water supply, safeguard the environment and protect customers.” The European Commission’s vice president Maroš Šefčovič is to meet US trade representative Jamieson Greer tomorrow morning in Paris as efforts to achieve a breakthrough on the threatened trade war intensify, my colleague in Brussels Lisa O’Carroll reports. The world is currently holding its breath to find out whether Donald Trump will back down on his decision to double tariffs as of tomorrow on steel and aluminium products to the US to 50%. But sources indicate it is unlikely that the EU will retaliate immediately given the delicacy of talks around the wider 20% reciprocal tariff plus tariffs on auto imports from the US. The EU has the power to bring forward a €21bn package already agreed in April on the initial tariffs imposed by Trump on steel and aluminium. However it has also agreed to try and find a swift path to settling their differences following Trump’s “good call” with European Commission president Ursula von der Leyen on 26 May. At the time she emphasised the bloc’s readiness to act “swiftly and decisively”but said the EU would need until July 9 to finalise a deal. It is understood they agreed to allow two weeks to play out from that call before taking any other steps, fuelling expectations that the EU would not retaliate against any new steel tariff tomorrow. Turning to trade deals, BoE governor Andrew Bailey says that it’s “really good” to see the trade deal between the UK and India agreed in early May. But, he warns, it will take time to see the economic benefits, as trade patterns adjust. He reminds MPs that in the short-term, Brexit will have a negative effect on the UK economy by making it less open, but that damage can be reduced through trade deals. Bailey adds that it would be a “good thing” if the UK can “rebuild trade with the EU, our largest trading partner” (echoing points he made last week). Asked whether the dollar’s safe-haven status is under threat, BoE governor Andrew Bailey says non-US investors have been reassessing how much risk they want to take. But, he suggests, many investors were probably ‘overweight’ on US risk in the past, due to an optimistic view of the US economy. They’re reassessing that. And they will do that, and go on doing that I’m sure as this story unfolds. But… Bailey says he doesn’t see the US dollar losing its reserve currency status. That status means US assets have a strong “embedded position” in the financial infrastructure, such as the way Treasuries (government debt) are used as a risk-free assets, “it would take a lot to change that,” Bailey points out. Andrew Bailey then warns MPs that stock markets could suffer falls if trade war tensions flare up again. He is asked about the recent recovery in share prices: Q: Does the “dramatic recovery” in equity markets in recent weeks back up the hypotheses of the Taco trade – that the damage caused by president Trump is overstated because Trump always chickens out and is terrified of the bond markets? Bailey says he won’t get into the question of the “taco thing’, telling MPs: That’s a euphemism that people in markets have come up with. I don’t think the president particularly likes it. Indeed…. Bailey agrees there has been a lot of volatility in the markets recently. He is most concerned when you see rising bond yields, falling currencies and falling equity markets. That became quite acute on two occasions after Liberation Day, and on both occasions the administration did respond – with a 90-day period to negotiate trade agreements with other countries, and with reassurance about the position of Fed chair Jerome Powell, Bailey says. He cautions that policymakers need to watch this very carefully, as the equity markets are obviously discounting views of the future. Bailey tells the Treasury committee: They appear to be discounting a more optimistic view about how this will come out. We need to bear in mind, therefore, that their view is conditioned on that and if things change they will respond. He adds that fortunately, we have not seen a real threat to financial stability from trade tensions. BoE policymaker Swati Dhingra is hopeful that the UK will avoid a repeat of the recent inflation shock in the next few years, thanks to signs that trade war tensions is eased. Dhingra tells the Treasury commitee that she is encouraged that prices will remain under control. She is hopeful that the world will avoid fragmenting into multipolar trade blocks, as could have happened if Europe had retaliated against the US with similar tariffs, sparking a full-blown trade war. Instead, given the way policy developments have panned out, Dhingra is ‘somewhat reassured’ that the impact of trade tensions will be milder than the worst case scenarios, and even some less severe scenarios. However… BoE policymaker Catherine Mann warns that supply chain disruption can potentially lead to an environment of higher volatility in inflation, which can require higher interest rates to control prices. Andrew Bailey adds that there is “a lot more uncertainty and unpredictability” about the global trading system, and the global economy more widely. Bailey tells MPs that the Bank must make two judgements: 1) what are the policies going to be. 2) what’s the impact of those policies. The challenge with the first judgement is that the Bank needs to “stop the music” when it takes its decisions, Bailey says. But the question of the impact is more important. Bailey tells the Treasury committee: The impact of fragmenting the world trade system is negative for world growth and world activity. It obviously increases uncertainty, Bailey adds, saying he’s heard this message as he goes round the country meeting businesses. That uncertainty causes delays to investment decisions. These are one-off decisions, and the appeal of waiting has gone up in the current climate, Bailey says. He adds that the impact of trade tensions on prices is more ambiguous. One argument is that it will lower world activity, which lowers world export prices which lowers inflation. That is ‘quite open to question’, though, the Bank of England governor argues. But if supply chains are disrupted, it could have the opposite effect and create upward pressures on inflation. "At the moment it’s frankly too soon to tell, Bailey concludes -- which backs up his earlier point about the uncertainty that is shrouding the path of UK interest rates. Bank of England governor Andrew Bailey has warned that the path of UK interest rates ‘is ‘shrouded’ in uncertainty, due to the turmoil created by trade conflict. Testifying to the Treasury committee this morning, Bailey declines to predict how he might vote at the Bank’s next meeting, in late June. Bailey believes that the path of UK interest rates, which were cut to 4.25% last month, is still lower. But, he warns, that process is harder to predict. Bailey tells MPs: “I think the path remains downwards, but how far and how quickly is now shrouded in a lot more uncertainty, frankly.” He says the “the external situation” is relevent, reminding the commitee that the Bank has adjusted the language it uses to describe the economic environment, saying: We’ve added the word ‘unpredictable’ to ‘uncertain’ , because of the sheer nature of what we’re dealing with. [Reminder, the OECD cut its forecast for global economic growth in 2025 and 2026 this morning, due to the turmoil caused by Donald Trump’s trade wars.] Policymaker Catherine Mann agrees with Bailey that the glide path for UK interest rates is downwards. But, Mann cautions that it’s not possible to predict by what steps that journey will happen, or over what timeframe. Deputy governor Sarah Breeden also believes the path for interest rates is lower, but tells MPs “there is uncertainty about how far, how fast.” Bank of England governor Andrew Bailey has denied that there is a culture of “group think” on its Monetary Policy Committee. He point out that chief economist Huw Pill voted to hold interest rates last month, while other Bank officials voted for a cut. Deputy governor Sarah Breeden, who has voted with the majority at every meeting she’s attended so far, also pushes back against ‘group think’ accusations. She says those majorities have often been a ‘broad church’, saying she has had a different interpretation of the economic outlook than colleagues (even if they voted the same way). [the overall MPC did look rather disunited last month, with nine policymakers split 5-2-2 between a small rate cut, a large one, and no cut at all]. Here’s a live feed of the Bank of England’s appearance before the Treasury committee: Treasury committee chair Dame Meg Hillier MP reminds Bank of England policymaker Swati Dhingra that she has now been outvoted at 16 of the 21 MPC meetings she’s attended. Dhingra has been a persistently dovish member of the committee, and argues that interest rates could have peaked at a lower level (they hit 5.25% in August 2023, and were kept there until August 2024). Last month, she voted for a half-point cut in rates, to 4%, while a majority voted for a smaller cut to 4.25% (and two policymakers, including Catherine Mann, wanted no change). Dhingra tells MPs today that “keeping policy gradual is a good thing”. But the problem is that if interest rate policy has been held too tightly for too long, at some point that starts to “really play a role”. Hinting that she could vote for larger rate cuts than in the past, Dhingra says: “I now need to start thinking about ‘do I increase the decrements for which I’ve been voting, or not?’” Bank of England governor Andrew Bailey is confident that UK pay growth will slow this year. Bailey takes issue with Catherine Mann’s argument (see last post) that the labour market hasn’t weakened this year, telling MPs that the UK labour market “has loosened somewhat” since February. Governor Bailey points to recent data showing pay growth has slowed faster than expected, as he explains why he voted for a quarter-point cut to interest rates last month. Although wages have been rising faster than is consistent with the Bank’s 2% inflation target, Bailey says the Bank believes pay growth will come down this year, based on what it is seeing in the data, and what firms around the country are telling the BoE. He is sticking with his policy of taking a “gradual and careful” approach to interest rate cuts. Deputy governor Sarah Breeden says he also favoured the quarter-point cut in Bank rate, “even absent” international developments (ie, trade wars). She says the persistence of inflation will depend on pay growth, citing predictions from the Bank’s agents that pay rise settlements will slow to 3.7% by the end of this year, more than a percentage point lower than where we are today. Bank of England policymaker Catherine Mann has pointed to recent easing in financial market conditions to explain why she has switched her position on interest rate cuts twice this year. Mann, who had been traditionally seen as a hawkish member of the BoE’s monetary policy committee, is in the spotlight after flipping to a dovish position in February when she voted for a half-point cut in interest rates (when most colleagues favoured a quarter-point cut). Then in May she flipped back, and was in the minority voting to leave rates on hold (when the MPC plumped for another quarter-point cut, in a three-way split). Today, she tells MPs that the two votes have to be looked at in the context of economic and financial market conditions. In February, Mann explains, she was looking at the prospects for the UK labour market to “loosen in a non-linear way”, as increases to the minimum wage and employers’ national insurance contributions hit the jobs market. At that stage, she says, a 50bp cut was needed as financial conditions were not consistent with those risks. But by May, things had changed. Partly because the labour market had not loosened as much as she had feared. Consumption was no weaker than expected, she tells the Treasury commmitee, and inflation was not decelerating in a way consistent with hitting 2% target, with goods prices rising not falling. But most importantly, from February to May, financial markets had eased quite dramatically [thanks to Donald Trump’s trade war spooking investors]. That, Mann says, actually delivered more of an easing than the 50bp which she voted for in February, she insists. Incidentally, FT Alphaville recently worked out that Catherine Mann now holds the silver and bronze medals for rapid vote shifts. Over in parliament, the Treasury committee is holding a session with Bank of England policymakers. They’re hearing from governor Andrew Bailey, the Deputy Governor for Financial Stability, Sarah Breeden, and external members Dr Catherine Mann and Dr Swati Dhingra. They’ll discuss the Bank’s decision to reduce the Bank Rate by 0.25 percentage points to 4.25% in early May, as well as the increase in inflation in April and the impact of US tariff policy. The cost of living squeeze across the eurozone has eased last month, potentially smoothing the way for cuts to interest rates. The Eurozone inflation rate fell to 1.9% in May, down from 2.2% in April according to a flash estimate from statistics body Eurostat. That takes euroozone inflation below the European Central Bank’s 2% target, for the first time since September 2024. The decline was driven by cheaper energy prices – energy prices fell by 3.6% across the eurozone, having been flat in April. Food, alcohol &amp;amp; tobacco is expected to have the highest annual inflation rate in May, at 3.3% (up from 3.0% in April), followed by services (3.2%, compared with 4.0% in April), non-energy industrial goods (0.6%, stable compared with April) and energy (-3.6%, stable compared with April). Diego Iscaro, head of European Economics at S&amp;amp;P Global Market Intelligence, says: “This easing inflation is good news for households, as it will help to offset some of the headwinds on consumption stemming from a highly uncertain economic environment. “May’s inflation print, coupled with the moderation in wage growth during the first quarter, suggests that the ECB will almost certainly cut rates by 25bp later this week. We expect a disinflationary environment will drive further monetary policy easing during the second half of the year, with the deposit rate likely to reach a low of 1.5% during the third quarter.” European stock markets are in the red this morning, as investors digest the OECD’s downgrade growth forecasts (see here) and the weak manufacturing data from China (see here). Germany’s DAX has dipped by 0.2%, while France’s CAC has lost 0.35%. The UK’s FTSE 100 share index has lost 26 points, or 0.3%, to 8747 points. Mining companies are among the fallers, following a drop in commodity prices after China’s factory output fell at its fastest rate since September 2022. The futures market indicates Wall Street will open lower too. Russ Mould, investment director at AJ Bell, says investors are showing signs of nervousness around tariffs and the economic outlook. “The OECD has downgraded its forecast for global economic growth as the effects of the trade war start to be felt. It’s only a small revision – from 3.1% to 2.9% for 2025 – but it’s still enough to cause investors some indigestion as they consume their morning news. The downgrade weighed on the mining sector as the market fears it could mean reduced demand for commodities, and therefore a potential knock to the price of metals and minerals. “The 90-day pause on tariffs has just over a month before expiration, meaning the pressure is on countries to do deals with the Trump administration. Reports suggest that Trump wants best offers on trade negotiations by Wednesday, perhaps to avoid any last-minute rush or stalemate situations.” Alistair Carmichael MP, who chairs the UK parliament’s EFRA Committee, fears that Thames Waater is now in a ‘perilous position,’ now that KKR has walked away. Carmichael, whose committee has been examining the water industry, says: “In our evidence session with Thames Water bosses in May we raised serious concerns that Thames had only pursued one bidder at an early stage for its takeover bid, against the wishes of Ofwat, and highlighted the risks this could pose if KKR chose not to proceed. Unfortunately, our concerns have been realised, putting Thames in a perilous position. “The Government has shied away from acknowledging the potential impact of this scenario on the public finances and must ensure that any takeover is in the public interest and does not line the pockets of financial institutions further to the detriment of customers and operational performance”. The OECD’s new economic forecasts were released as it begins a Ministerial Council Meeting in Paris today. The UK’s trade secretary, Jonathan Reynolds, is attending, and is due to meet his US counterpart to try to agree a timeline to exempt Britain from America’s steel and aluminium tariffs. Reynolds is expected to meet his US counterpart, Jamieson Greer, at the OECD meeting in Paris next week to discuss tariffs. Last weekend, a UK government spokesperson said: “The UK was the first country to secure a trade deal with the US earlier this month and we remain committed to protecting British business and jobs across key sectors, including steel.” “We are engaging with the US on the implications of the latest tariff announcement and to provide clarity for industry.” Last week, Trump unexpectedly doubled the tariffs on steel and aluminium imports to 50%; those levies are due to come into effect on Wednesday. Clean water campaigner Feargal Sharkey is calling for the UK government to end the ‘debacle’ at Thames Water and put it into special administration, after KKR dropped out of the rescue deal (see earlier post). Back in the water industry, some of Thames Water’s bond prices have slumped to record lows this morning after private equity firm KKR dropped out of the rescue deal for the utility firm. Reuters has the details: KKR’s withdrawal sent Thames’ 2040 bond down 4 pence in the pound to 69 pence, while its euro-denominated April 2027 bond dropped 2 euro cents to just under 68 cents. US commerce secretary Howard Lutnick has declared that he is “very optimistic” of reaching a trade deal with India soon. Speaking at the annual summit of the US-India Strategic Partnership Forum in Washington last night, Lutnick said: “You should expect a deal between the United States and India in the not-too-distant future because I think we found a place that really works for both countries.” The OECD also show how the United States’s effective tariff rate had risen to 15.4% by mid-May, up from just over 2% in 2024. That’s the highest rate since 1938, after the Great Depression, when the Smoot-Hawley Tariff Act had significantly raised tariffs on imported goods in the US, in a failed attempt to support domestic industry. The OECD explain: The US tariffs, together with retaliatory action by China, as well as more limited action by Canada, means that trade equivalent to over 2% of world GDP is now directly facing higher tariffs, pointing to much greater disruption than during the US-China trade tensions in 2018-19. If current applied tariffs are sustained, effective tariff rates are likely to fall over time, as trade in more heavily-tariffed goods is likely to slow. This chart, from the OECD’s new economic forecasts, show how trade policy uncertainty has surged this year: US economic growth is expected to slow markedly to 1.6% in 2025 and 1.5% in 2026, the OECD says. That’s relatively weak growth by recent standard, and slower than the “robust” growth of 2.8% recorded in 2024. The OECD says the slowdown is due to the “substantial increase” in the US effective tariff rate on imports, and the impact of retaliation from some trading partners. It also cites “high economic policy uncertainty, a significant slowdown in net immigration, and a sizeable reduction in the federal workforce”, a nod to Donald Trump’s clampdown on workers entering the US and Elon Musk’s DOGE cost-cutting drive, The OECD adds: Annual headline inflation is set to pick up to 3.9% by end-2025 due to higher import prices but is expected to ease throughout 2026, aided by moderate GDP growth and higher unemployment. Risks to the growth projection are skewed to the downside, including a more substantial slowing of economic activity in the face of policy uncertainty, greater-than-expected upward pressure on prices from tariff increases, and large financial market corrections. The OECD has also cut its forecast for UK growth in 2025 and 2026, due to the damage caused by Donald Trump’s tariff war. It has downgraded its expectations for this year and next from a forecast made in March; UK GDP growth is now projected to be 1.3% in 2025 before slowing to 1.0% in 2026. Constraints on Whitehall spending and higher than expected inflation also played a part in a downgrade, the OECD said. More here: Newsflash: Global growth will slow this year as Donald Trump’s trade wars hit the world economy, a new report says. The Organisation of Economic Cooperation and Development (OECD) has cut its forecasts for growth in 2025 and 2026, and warned that the global outlook is becoming “increasingly challenging”. The OECD now predicts that global GDP growth will slow from 3.3% in 2024 to 2.9% this year and in 2026, “on the technical assumption that tariff rates as of mid-May are sustained despite ongoing legal challenges”. In its latest global economic outlook, just released, the Paris-based thinktank explains: The slowdown is concentrated in the United States, Canada and Mexico, with China and other economies expected to see smaller downward adjustments. Back in March, the OECD had predicted that global GDP growth would slow to 3.1% in 2025, and then to 3.0% in 2026. Today, it warns that global trade growth is likely to slow substantially over the next two years, after a burst of activity earlier this year as firms tried to stock up on goods ahead of tariff increases. It says: Substantial increases in barriers to trade, tighter financial conditions, weaker business and consumer confidence and heightened policy uncertainty will all have marked adverse effects on growth prospects if they persist. Higher trade costs, especially in countries raising tariffs, will also push up inflation, although their impact will be offset partially by weaker commodity prices. Here are the OECD’s latest growth forecasts: Uncertainty is expected to hold back business investment, the OECD adds. It fears that further increases or swift changes in trade barriers could intensify the growth slowdown and trigger significant disruptions in cross-border supply chains, and that the tariffs could push up inflation expectations, leading to higher interest rates and lower growth. But on the upside, a reversal of the increase in trade barriers would support growth and reduce inflation, the OECD adds. Thames Water don’t disclose why KKR chose to walk away from talks to inject desperately needed fresh equity into the company. Two weeks ago, Bloomberg reported that KKR’s proposal involved slashing about £8bn of Thames Water’s debt. The US investment group had been chosen by Thames to lead the company’s turnaround after it offered to put £4bn into the company. Negotiations with regulator Ofwat had been expected to run throughout June, so today’s news that KKR have walked away is a surprise…. The slump in China’s manufacturing PMI (see opening post) is “a canary in the trade war coal mine,” says Stephen Innes, managing partner at SPI Asset Management. The poor bird’s feathers have been “scorched by tariffs and global uncertainty”, Innes reports, explaining: The Caixin Manufacturing PMI’s plunge to 48.3 isn’t just a weak print—it’s a body blow to the backbone of China’s economy: small and mid-sized exporters now caught in a brutal vice grip between faltering global demand and a Washington-led tariff regime that’s more carrot-and-stick diplomacy than ceasefire. Elsewhere in the water industry, a new report has warned that the water sector in England and Wales needs a “fundamental reset”. In an interim report published on Tuesday, the Independent Water Commission says the water sector has been beset by “deep-rooted, systemic” failures. The Commission says wide-ranging and fundamental change is needed in five areas – including clearer direction from government, stronger regulation of water companies, bringing decisions on water systems closer to local communities, and greater focus on responsible, long-term investors. The report also singles out regulation, saying that Ofwat needs to embrace a “supervisory approach”, so it can intervene early before problems arise. The current model relies heavily on ‘comparability’ – benchmarking companies against one another to assess efficiency and justify customer bills, the Commission says. Independent Water Commission chairman Sir Jon Cunliffe said he had heard a “strong and powerful consensus” that the system was not working for everyone. Cunliffe: “There is no simple, single change, no matter how radical, that will deliver the fundamental reset that is needed for the water sector.” “We have heard of deep-rooted, systemic and interlocking failures over the years – failure in Government’s strategy and planning for the future, failure in regulation to protect both the billpayer and the environment and failure by some water companies and their owners to act in the public, as well as their private, interest. “My view is that all of these issues need to be tackled to rebuild public trust and make the system fit for the future. We anticipate that this will require new legislation.” Newsflash: Thames Water’s efforts to avoid nationalisation have taken a blow. US investment firm KKR has walked away from the chance to take a stake in the troubled water utility, putting its future in fresh doubt. Thames had selected KKR as a “preferred partner” at the end of March, as it looked for a partner to take a stake in its business. But today, Thames told the City that KKR has indicated that it will not be in a posi</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Bank of England governor Andrew Bailey told MPs that the global trade system has been ‘blown up’ by Donald Trump’s trade wars. He warned that fragmenting the world trading system is negative for world growth and world activity. Bailey also warned that the future path of UK interest rate cuts was shrouded in more uncertainty.</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Time to wrap up… US factory activity has contracted for a third consecutive month, as American firms warn that tariffs are disrupting their businesses. The latest PMI survey from the ISM has found that new orders and backlogs contracted in May, as production and employment contracted. China has accused the US of “seriously violating” the fragile US-China detente that has been in place for less than a month since the two countries agreed to pause the trade war that risked upending the global economy. China’s commerce ministry said on Monday: “The US has successively introduced a number of discriminatory restrictive measures against China, including issuing export control guidelines for AI chips, stopping the sale of chip design software to China, and announcing the revocation of Chinese student visas.” Trade war worries have knocked the US dollar today, sending the pound towards a three-year high. Stocks have fallen on Wall Street, after a sell-off in parts of Asia. But in London, shares in defence companies have rallied as the UK government lays out plans for new investment. In the UK property sector, mortgage approvals fell to the lowest in over a year in April. But prices recovered in May, according to lender Nationwide. The surprise decline in the ISM manufacturing index in May (see earlier post) indicates that tariffs continue to weigh significantly on the sector, says Alexandra Brown, North America economist at Capital Economics. Brown explains: While the May data is less gloomy than initially appears, as a sharp decline in inventories offset a strengthening in the other components of the index, its low level points to manufacturing output stagnating at best. The headline index edged lower to 48.5 last month, from 48.7. This was driven by inventories, which fell 4.1 points, as firms drew down on their large inventories previously stockpiled to avoid tariffs. The production and new orders indices both rose, although a decline in the new export orders indicates that the latter was driven by domestic demand. Here are more comments from US manufacturers bemoaning the impact of tariffs on their businesses, from today’s ISM PMI report. “The administration’s tariffs alone have created supply chain disruptions rivaling that of COVID-19.” [Electrical Equipment, Appliances &amp;amp; Components] “We have entered the waiting portion of the wait and see, it seems. Business activity is slower and smaller this month. Chaos does not bode well for anyone, especially when it impacts pricing.” [Primary Metals] “Tariff whiplash continues while the easing of tariff rates between the U.S. and China in May was welcome news, the question is what happens in 90 days. We are doing extensive work to make contingency plans, which is hugely distracting from strategic work, plus it is also very hard to know what plans we should actually implement. The 10-percent tariff on other countries is impactful as well, and it is unclear if/when deals will be made.” [Miscellaneous Manufacturing] Oof! Economic activity in the US manufacturing sector contracted in May for the third consecutive month, as factories were hit by a slump in export orders. In a sign of the economic damage caused by Donald Trump’s trade war, US manufacturers have reported that new orders, and backlogs of work, fell last month, while production and employment levels contracted. That’s according to the latest poll of purchasing managers by the Institute of Supply Management (ISM), which shows that US manufacturing activity slipped further into contraction last month. Worryingly, 57% of the sector’s gross domestic product (GDP) contracted in May, up from 41% in April, the ISM say. Several firms surveyed by the ISM reported that trade war turmoil is causing disruption. That’s a turnaround on earlier this year, when there was a jump in demand for manufacturered goods to front-run tariffs. “Most suppliers are passing through tariffs at full value to us,” reported a chemicals producer, adding: “The position being communicated is that the supplier considers it a tax, and taxes always get passed through to the customer. Very few are absorbing any portion of the tariffs.” It has been hard for US manufacturers to keep up with the twists and turns in the trade war. In recent weeks, Trump has all but halted tariffs on Canada and Mexico, while steep individual tariffs calculated for a string of trading partners were reduced to 10%, and a 145% tariff on Chinese goods was drastically cut in a truce that may already be unravelling. A fabricated metal products maker said that “Tariff uncertainty is impacting new international orders. Tariffs are also the main reason our Asia customers are requesting delayed shipments.” And a paper producer warned: “Uncertainty due to the recent tariffs continue to weigh on profitability and service. An unresolved (trade deal with) China will result in empty shelves at retail for many do-it-yourself and professional goods.” Overall, the Manufacturing PMI dropped to 48.5% in May, down from 48.7% in April, which indicates a faster contraction. An index of export orders fell, while ISM’s “Imports Index” plunged into extreme contraction in May; it dropped to 39.9%, 7.2 percentage points lower than April’s reading of 47.1%. Oil prices have jumped by over 3% today, after the Opec+ group decided to raise output in July at the same rate as in May and June. Opec+ decided last weekend to raise output by 411,000 barrels per day. Brent crude has jumped to $64.74 per barrel, up around $2, on relief that the producers didn’t agree a larger increase in output. Shares in some US steel companies are rallying, as traders react to Donald Trump’s decision to lift tariffs on imported steel to 50%. Nucor Corporation, the steel producer based in Charlotte, North Carolina, has jumped by 13%. Cleveland-Cliffs, the steel manufacturer based in Cleveland, Ohio, is up 21%. Both companies could benefit from higher tariffs on overseas competitors; it could allow them to undercut rivalls, or pump up their own profit margins. Stocks have opened lower on Wall Street, as investors weigh up the risks that the US trade war flares up again. The main indices are all lower at the start of the first trading day of June, with the Dow Jones industrial average shedding 158 points, or 0.4%, to 42,111. The S&amp;amp;P 500 index dropped by 0.3%, while the tech-focused Nasdaq dipped by 0.25%, as traders digest the tit-for-tat accusations between the US and China (with each accusing the other of violating their trade truce). Fawad Razaqzada, market analyst at City Index and FOREX.com, reckons June is shaping up to be a trickier month than May, adding: Between fresh trade war fears and looming political fights over tax and spending in the US, there’s plenty for markets to digest. And with the debt ceiling drama simmering in the background, expect volatility to make a comeback. For the gold forecast, this backdrop of risk aversion and fiscal uncertainty couldn’t be more favourable. Here’s a chart showing how the pound has risen close to a three-year high against the US dollar today (but it still a little lower than last week) The dollar has begun June with a “significant decline” due to the renewed escalation in trade tensions, reports Hani Abu Akleh, senior market analyst at XTB MENA. The dollar’s decline came after US President Donald Trump announced a 50% tariff on steel and aluminum imports, effective June 4, a move that further heightened global trade tensions. Meanwhile, trade disputes with China escalated after Beijing rejected Washington’s accusations that it had violated the Geneva agreement signed last May. While US officials criticized what they described as China’s failure to commit to removing non-tariff barriers, Beijing demanded that the United States roll back trade restrictions it described as discriminatory. The pound is approaching a three-year high against the US dollar, as trade tensions grip the markets. The dollar has continued to lose ground against other currencies, after China hit back against the US today, and accused Washington of “seriously violating” their trade pact. Sterling gained almost a cent today, trading as high as $1.3557, its highest level since 27 May – when the pound hit a three-year peak. Concerns that the US trade war might be flaring up again are hurting the dollar; the euro has hit its highest level since April, at $1.143. Against a basket of currencies, the dollar is down over 0,5% today, hitting a five-week low this morning. Dean Turner, chief eurozone &amp;amp; UK economist at UBS Global Wealth Management, says a combination of policy uncertainty and ongoing trade and budget deficits points to more weakness in the coming quarters: He told clients: “Nobody can know for sure if the ‘dollar unwind’ is over or whether it has only just begun. When thinking about the outlook for the USD, we should acknowledge that one important thing has changed. In recent years, periods of uncertainty have benefited the USD as investors flocked to what was perceived to be a safe-haven currency. In today’s world, with the US increasingly the source of uncertainty, its safe-haven appeal is dwindling. A high level delegation from the EU is on the way to Washington DC today for urgent talks to avert a doubling of Donald Trump’s tariffs on steel exports on Wednesday. With the new 50% tariff entering into force in two days time, the talks take on a new sense of urgency, my colleague Lisa O’Carroll reports. They will take place in parallel with talks between European Commission vice president Maros Sefcovic in Paris and US commerce secretary Howard Lutnick on the margins of the OECD council meeting in Paris tomorrow. Trump’s surprise announcement over the weekend was described as “yet another body blow” by UK Steel which had been promised the existing 25% tariff would be reduced to 0% as part of Keir Starmer’s highly publicised deal with Trump last month. It is now a race against time for the UK and the EU, which has also been exposed to tariffs on cars and a future blanket tariffs on all exports from the bloc. A team of around half a dozen, headed by Tomas Baert, trade adviser to European Commission president Ursula von der Leyen will be in the US, aiming for a breakthrough on steel before Wednesday but also a long tariff and potential mini trade deal. Sefcovic has a number of bilaterals in Paris including the US and China where Trump’s decision to double import duties to 50% on steel will be very much on the agenda. He is also meeting representatives from Australia and Thailand tomorrow and a delegation from India today. In the auto sector, Tesla’s sales slump has not abated, in France at least. Tesla’s new-vehicle registrations fell by 67% in France in May, according to French industry association Plateforme Automobile, to 721 cars. Tesla’s registrations were the lowest since July 2022, despite the company rolling out a redesigned version of its most popular vehicle, the Model Y, Bloomberg reports. Data last week showed that Tesla’s sales in Europe fell 49% in April, year-on-year, despite hopes that the refreshed Model Y would spur a sales boost. Back in the City, shares in defence companies are pushing higher on expectations of a spending boost from the UK government. Babcock are now up around 8.5%, leading the FTSE 100 risers, whle BAE Systems are up 2% to a record high. Loredana Muharremi, equity analyst at Morningstar, says the UK’s strategic defence review is “unequivocally positive for the sector”. Key beneficiaries of this announcement include BAE Systems, which is well-positioned across all priority areas (such as submarines, munitions, cyber via its Digital Intelligence division, and long-range weapons), and Rolls-Royce, through its role in naval nuclear propulsion. Also, a broader network of Tier 2 and Tier 3 suppliers in the UK industrial base should benefit from the localisation of munitions and components. It’s all change at Royal Mail’s parent company, International Distribution Services, today, following its takeover by Czech billionaire Daniel Křetínský. Firstly, its boardroom has become much emptier. Keith Williams, Sarah Hogg, Maria de Cunha, Michael Findlay, Lynne Peacock, Shashi Verma, Jourik Hooghe and Ingrid Ebner have all stepped down as non-executive directors of IDS today. But while they leave, former UK government minister Greg Hands is joining Křetínský’s EP Group, as a full time Strategic Adviser. According to a post on LinkedIn, Hands will have a current special focus on the UK and Germany. It says: In his new role, reporting directly to Chairman and CEO Daniel Křetínský, Mr Hands will be based primarily in the UK, with additional activities in Germany. He will provide strategic counsel to EP Group’s executive leadership, focusing on regulatory and market developments in the UK and Germany. His insights will support EP Group’s efforts to expand its portfolio across both countries, aligning with the company’s commitment to secure and sustainable energy solutions. The shake-up comes as IDS’s stock market listing in London is officially cancelled today, after the takeover by EG Group was completed earlier this year. Shares in advertising companies have just taken a hit, following a report that social-media company Meta is aiming to let brands fully create and target ads using artificial intelligence by the end of next year. According to the Wall Street Journal, Meta is aiming to help brands create advertising concepts from scratch. Meta’s ad platform already offers some AI tools that can generate variations of existing ads and make minor changes to them before targeting the ads to users on Facebook and Instagram, and now plans to expand this. The WSJ reports: AI-powered advertising is part of Meta Chief Mark Zuckerberg’s grand vision for his company’s evolution. Advertising makes up the bulk of Meta’s business—it brought in more than 97% of overall revenue in 2024—and funds its multibillion-dollar investments in AI chips and data centers, and for training cutting-edge AI models. Using the ad tools Meta is developing, a brand could present an image of the product it wants to promote along with a budgetary goal, and AI would create the entire ad, including imagery, video and text. The system would then decide which Instagram and Facebook users to target and offer suggestions on budget, people familiar with the matter said. Meta also plans to enable advertisers to personalize ads using AI, so that users see different versions of the same ad in real time, based on factors such as geolocation, the people said. A person seeing an advertisement for a car in a snowy place, for example, might see the car driving up a mountain, whereas a person seeing an ad for that same car in an urban area would see it driving on a city street. Investors are calculating that a surge in AI adverts would dent revenues and profits at advertising companies – shares in WPP are down 4.1%, while Publicis Group have fallen 3%. Although the US dollar has fallen against most currencies, it has risen against the Russian rouble today. The rouble has dropped by 1.7% this morning to ₽78.8 to the $, reversing a recovery last week that pushed Russia’s currency to a two-year high. The losses come as Ukrainian and Russian negotiators prepare to meet later today in Istanbul to hold peace talks. The meeting follows a major Ukrainian drone attack on Russian military bombers in Siberia yesterday, and attacks by Russia on Ukraine earlier today, which could dampen hopes of a breakthrough in Turkey. The rouble could also be under pressure from speculation that Russia’s central bank might cut interest rates soon, to stimulate economic growth. The highest paid director at Monzo made £12m last year, the bank’s latest accounts show. Monzo, the digital bank best known for its coral pink debit cards, has become one of the most popular and fastest growing banks in the UK. Its success has also meant its top paid director has seen their total compensation package rise to £12m in its financial year ended in March, compared with £1.7m last year. Just over £11m of the package this year came from share-based payments. It makes the director, who was not named in the report but is thought to be its chief executive TS Anil, among the best paid in the banking sector. Last year the boss of Lloyds Bank, Charlie Nunn, took home a total package of £5.6m, while the chief executive of Barclays, C.S. Venkatakrishnan, was paid a package worth £8.7m, excluding the impact of share price appreciation. At digital rival Starling Bank, its latest annual report showed its top paid director’s package was worth £1.7m. Monzo, which has been led by Anil since 2020, also reported a bumper set of numbers for its 2025 financial year. Its revenue grew by 48% to surpass £1bn for the first time, and pre-tax profit more than quadrupled to £60.5m. The bank now has 12.2m customers, up 25% compared with last year. UK mortgage approvals have fallen to their lowest level in a year, as the end of a tax break on stamp duty cooled demand. Net mortgage approvals for house purchases, decreased for the fourth consecutive month in April, falling by 3,100 to 60,500, according to data from the Bank of England. That’s the lowest number of monthly mortgage approvals since February 2024. The drop follows a rush to agree house sales earlier this year, before changes to stamp duty at the start of April which pushed up the cost of buying a new home in England and Northern Ireland. The BoE’s data also shows that net borrowing of mortgage debt decreased sharply by £13.7bn to -£800m in April. This followed an increase in net borrowing by £9.7bn to £13.0bn in March. Simon Gammon, managing partner at Knight Frank Finance, says: “There was a significant drop in net borrowing in April because so many deals were squeezed through in March to beat the stamp duty deadline. Approvals for house purchase are a much better barometer of the health of the market as they reflect buyer intent at an earlier phase. “On that front, the market looks solid but unspectacular. Approvals are tracking about 10% below the 2019 average and are unlikely to improve markedly without further, sustained falls in mortgage rates. That looks unlikely at the moment - hotter-than-expected inflation figures published earlier this month prompted a repricing among the high street’s larger lenders. Leading fixed rates are now only a whisker below 4%. “Whether that proves to be a sustained move higher will depend on a combination of domestic UK inflation data and the day-to-day whipsawing of US trade policy.” Today’s UK PMI report (see 9.52am) also shows that business confidence at British factories remained ‘subdued’ last month. Manufacturers continued to raise concerns that turbulent trade conditions, the weak economic outlook and rising cost burdens will make market conditions tough during the year ahead. Only 49% of firms surveyed expect production volumes to grow over the next 12 months, compared to 13% expecting a contraction. Confidence levels at small-scale producers fell to a near-record low. Britain’s factory sector may have “turned a corner” last month, despite another fall in manufacturing output and new orders. The latest survey of purchasing managers at UK manufacturers found that the sector contracted again in May, but not by as much as initially feared. S&amp;amp;P Global’s PMI index has risen to 46.4 in May, a three-month high, up from 45.4 in April and above the earlier flash estimate of 45.1. Any reading below 50 shows a fall in activity, and the PMI report shows operating performance has deteriorated for the past eight months. Total new business volumes decreased for the eighth month running, amid reports of a general reluctance among clients to commit to new contracts. The report says: Weak global market conditions, trade uncertainty, low customer confidence and cost pressures resulting from recent increases to UK employer NICs and minimum wages also contributed to clients’ reluctance to spend. That said, a recent bout of good weather did boost sales at some manufacturers. The survey reports “some tentative signs” that the sector may have turned a corner; indices monitoring trends in output and new business rose for the second month in a row. Rob Dobson, director at S&amp;amp;P Global Market Intelligence, explains: “May PMI data indicate that UK manufacturing faces major challenges, including turbulent market conditions, trade uncertainties, low client confidence and rising tax-related wage costs. Downturns in output, new orders and new export business have continued, and business optimism has stayed subdued by the historical standards of the survey. “Smaller manufacturers are experiencing the sharpest pinch, registering the steepest retrenchments in output and demand and seeing their confidence slump to a near record low. Job losses are also rising across manufacturing, with the rate of decline in employment gathering pace. “There are some signs of manufacturing turning a corner though. PMI indices tracking output and new orders have moved higher in each of the past two months, suggesting the downturn is easing, and came in better than the earlier flash estimates for May. That said, trading conditions remain turbulent both at home and abroad, making either a return to stabilisation or a sink back into deeper contraction likely during the coming months.” The euro has now hit its highest level against the US dollar since late April, as trade war jitters hit the foreign exchange markets. The single currency hit $1.1436 this morning, a five-week high, up almost a cent. Derek Halpenny, FX expert at MUFG bank, reports that increased tensions between the US and China are weighing on the dollar. The flip-flopping on trade policy looks set to continue and it appears the uncertainty this creates does not bother President Trump at all. That is likely to give investors the reason to renew selling of the US dollar. The DXY index is back below the 99-level today and within 1% of the intra-day low on 21st April. Certainly if the Trump-Xi meeting goes badly or if it doesn’t take place at all, that low-point for the dollar could well be breached this week, taking us to levels not seen since March 2022. Salzgitter, Germany’s second-biggest steelmaker, has warned that Washington’s tariff policy was dealing a severe blow to European industry, Reuters reports. Reacting to Donald Trump’s plan to double steel import levies to 50%, Gunnar Groebler, Salzgitter’s CEO, says: “An increase in steel import duties in the USA to 50% should prompt the EU Commission to accelerate its efforts to implement the measures under the Steel and Metals Action Plan.” Shares in UK-listed weapons makers are rising this morning, as the UK launches its new defence review. Babcock, who are one of the Ministry of Defence’s largest contractors, are leading the FTSE 100 risers, up 3.8%. BAE Systems, which makes combat vehicles, artillery systems, missile launchers, fighter jets and submarines, are up 1%. Defence technology company Qinetiq (+3%) are leading the risers on the smaller FTSE 250 index. Prime minister Keir Starmer is launching the review today. It calls for the UK to move to “war-fighting readiness” to deter Russian aggression in Europe and to increase its stockpiles of arms and support equipment, to make Britain ready to fight a war in Europe or the Atlantic. Dr Alexander Gilder, associate professor of International Law and Security at the University of Reading, explains: “The Strategic Defence Review’s expected recommendation that the UK ready its armed forces for warfighting will allow the UK to play a key leadership role in NATO. “It is plausible that, were there to be peace in Ukraine in the short term, Russia could be capable of mounting small incursions into other neighbouring states. For instance, Narva in eastern Estonia has been much discussed in recent years. This would trigger Article 5 and require NATO to be prepared to defend its member state. “The Government’s investment in AI and drones is a direct result of these technologies being used prolifically in the Ukraine war. The Russian Air Force has played a small role. Similarly, in any future conflict, the UK would not want to risk much more expensive fighter jets and their pilots unless necessary. “The UK and its allies are seeking to show Russia that they are capable of rapid military action in the event a NATO member is invaded. Increased naval power is an important part of this. Long-range weapons are expected to feature heavily in any modern conflict between global powers as they seek to destroy each other’s logistics.” European stock markets have dropped in early trading, as investors assess the latest trade war developments. Germany’s DAX has dropped by 0.25%, while France’s CAC index is down by almost 0.5%. The mood is downbeat in London, too, where the FTSE 100 index is down 23 points, ro 0.27%, at 8748 points, following those earlier losses in Asia. Investors are trimming their risk exposure amid the renewed flare-up in U.S.-China tensions, reports Stephen Innes, managing partner at SPI Asset Management, adding: What started as posturing is now veering dangerously close to a breakdown in the fragile truce announced on May 12. Beijing’s counteraccusation highlights new U.S. measures on AI chip export controls, expanded restrictions on tech sales, and the abrupt cancellation of several Chinese student visas. The tit-for-tat narrative has sharpened, and with both sides digging in, the political tone is growing more adversarial by the hour. This isn’t just diplomatic shadowboxing anymore—it’s bleeding into market sentiment. Trade war fears don’t seem to have hurt the UK housing market last month. Lender Nationwide has reported that the average house price rose by 0.5% duing May, reversing most of the 0.6% fall recorded in April. This lifted annual house price inflation to 3.5%, with the average property now costing £273,427. Robert Gardner, Nationwide’s chief economist, says: “Despite wider economic uncertainties in the global economy, underlying conditions for potential home buyers in the UK remain supportive. “Unemployment remains low, earnings are rising at a healthy pace (even after accounting for inflation), household balance sheets are strong and borrowing costs are likely to moderate a little if Bank Rate is lowered further in the coming quarters as we, and most other analysts, expect. Treasury Secretary Scott Bessent suggested yesterday that the US and China were in dispute over critical minerals. Bessent told CBS’s “Face the Nation”: “What China is doing is they are holding back products that are essential for the industrial supply chains of India, of Europe. And that is not what a reliable partner does.” Share prices in Hong Kong have weakened today, pulling the Hang Seng index down by 1.5%. In Japan, the Topix share index has lost 0.9%. Jim Reid, market strategist at Deutsche Bank, points out that “it’s hard to see past trade at the moment,” adding: It is really hard to keep up or predict what’s going to happen on trade at the moment, and that’s before we factor in the full ramifications from the court ruling last Thursday night, and then subsequent brief stay of execution for them on appeal. For now it seems likely that the tariff uncertainty will linger for a long time ahead even if we’re still likely past the peak aggressiveness of US policy. [Update: Mainland China markets were closed today]. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Trade war tensions are on the rise again, as relations between China and the US deteriorate. Beijing has hit back this morning against Washington, accusing the US of “seriously violating” the trade truce which the two powers agreed in Zurich last month. China’s commerce ministry also promised to take forceful measures to safeguard its interests, rejecting a claim from Donald Trump last week that China has ‘totally violated’ its trade agreement with the US. In a statement, the ministry said: “The U.S. government has unilaterally and repeatedly provoked new economic and trade frictions, exacerbating uncertainty and instability in bilateral economic and trade relations.” Beijing accused the US of unilaterally introducing new discriminatory restrictions, including new guidelines on AI chip export controls, curbs on chip design software sales to China and the revocation of Chinese student visas, Bloomberg reports. Stock markets across the Asia-Pacific region have dropped today, as investors fret that the détente between the two sides is fraying. Last Friday, the US president – perhaps stung by jibes that Trump Always Chickens Out – declared that China “HAS TOTALLY VIOLATED ITS AGREEMENT WITH US.”, raising fears that the trade war will continue to rattle the global economy. This latest uncertainty is hurting the US dollar. It has slipped against a basket of currencies, with the pound up almost half a cent at $1.35, and the euro gaining a third of a cent to $1.138. The legality of Trump’s trade war was also thown into doubt last week, when a US federal court ruled that his “liberation day” tariff plan is illegal, only for a federal appeals court to temporarily reinstate the tariffs while the case progresses. The agenda 9am BST: Eurozone manufacturing PMI for May 9.30am BST: UK manufacturing PMI for May 9.30am BST: Bank of England mortgage approvals and credit conditions data 3pm BST: US manufacturing PMI for May</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>US factory activity has contracted for a third consecutive month. New orders and backlogs contracted in May, as production and employment contracted. China has accused the US of “seriously violating” the fragile US-China detente. Trade war worries have knocked the US dollar today, sending the pound towards a three-year high.</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Time to wrap up…. The IMF has upgraded its forecast for the UK economy this year after strong growth in recent months. The Fund now forecasts UK GDP will increase by 1.2% this year, up from a forecast of 1.1% last month. Following its annual assessment of the UK, the IMF says: An economic recovery is underway. Growth is projected at 1.2 percent in 2025 and will gain momentum next year, although weak productivity continues to weigh on medium-term growth prospects. The authorities’ fiscal plans strike a good balance between supporting growth and safeguarding fiscal sustainability. It will be important to stay the course and deliver the planned deficit reduction over the next five years to stabilize net debt and reduce vulnerability to gilt market pressures. Further refinements of the fiscal framework could help minimize the frequency of fiscal policy changes. In the longer term, the UK will face difficult choices to align spending with available resources, given ageing-related expenditure pressures. The IMF also recommended that Rachel Reeves should refine her fiscal rules to prevent the need for emergency spending cuts. This would help the chancellor avoid making short-term savings when there is a downturn in economic forecasts. Stock markets in the UK and the US have rallied, as trading resumes after a long weekend on both sides of the Atlantic. Share prices jumped on relief that Donald Trump has delayed planned 50% tariffs on European goods until July, sending the FTSE 100 to its highest since early March. Germany’s DAX hit a record high. The US president has posted today that the EU has “called to quickly establish meeting dates”. In other news: Africa’s growth forecast for the year have been cut, due to tariff uncertainty UK retailers are gloomier about business prospects, after reporting a drop in sales Sales of Tesla cars across Europe have fallen sharply again, down around 50% in April. Food inflation across the UK has risen again US companies vulnerable to a trade war are among the top risers on Wall Street today. Nike (which makes almost all its products in Asia) are up 3%, as are chipmaker Nvidia. The US stock market is extending its early gains, with the Dow Jones industrial average now up 1%, and the Nasdaq gaining 2%. Analysts at ABN Amro are hopeful that we may be past the worst with tariffs. In a note to clients today, they say: The US-China trade truce shows that there are limits in how far the Trump administration is prepared go in implementing its radical trade agenda We expect significant tariffs to remain in place, and this will weigh on growth in the near term However, the trough in growth is likely to be shallower, and the downside risks significantly reduced Donald Trump has claimed that his threat last Friday to impose 50% tariffs on European Union imports has had an effect. Posting on his Truth Social site this morning, the US president says the EU has been in touch to agree dates for a meeting to discuss a trade deal. Trump says: I was extremely satisfied with the 50% Tariff allotment on the European Union, especially since they were “slow walking (to put it mildly!), our negotiations with them. Remember, I am empowered to “SET A DEAL” for Trade into the United States if we are unable to make a deal, or are treated unfairly. I have just been informed that the E.U. has called to quickly establish meeting dates. This is a positive event, and I hope that they will, FINALLY, like my same demand to China, open up the European Nations for Trade with the United States of America. They will BOTH be very happy, and successful, if they do!!! Stocks have jumped in New York as trading resumes after yesterday’s Memorial Day holiday. Investors appear relieved that Donald Trump has agreed to delay his threatened 50% tariffs on EU goods until July 9, while trade negotiations take place. The Dow Jones industrial average, which tracks 30 large US companies, has risen by 0.8% at the start of trading, up 333 points at 41,936 points. The broader S&amp;amp;P 500 index is up 0.95%, and the tech-focused Nasdaq has gained 1.3%. Wall Street (like the City of London this morning) is catching up with yesterday’s gains across many European markets yesterday, as Bob Savage, head of markets macro strategy at BNY, explains: Risk sentiment steadies after the long weekend in the U.S. and U.K., with tariffs, long-end yields and lower inflation driving equities higher. On Sunday, President Trump delayed his 50% tariffs on the EU until July 9. The EU, in turn, gave “fast-track” status to trade negotiations. This action led to a relief rally in shares on Monday… Donald Trump’s trade war is expected to hurt Africa’s economic growth this year. The African Development Bank has cut its forecast for growth across the continent to 3.9% this year, down from an earlier estimate of 4.1%. That would still be stronger growth than in 2024, when the region grew by 3.3%. The African Development Bank also cut its initial 2026 growth forecast by 0.4 percentage points to 4.0%, citing trade tariff uncertainty. In its latest African Economic Outlook report, it says: “Since January 2025, the world has experienced additional shocks, exacerbating an already complex global macroeconomic landscape. “These shocks include a plethora of new tariffs imposed by the United States and retaliatory measures announced and implemented by its trading partners.” Over in the US, meanwhile, demand for durable goods has dropped amid the economic uncertainty caused by the Trump trade wars. Orders for durable goods — items meant to last at least three years — fell 6.3% in April, driven by weaker demand for commercial aircraft. Core capital goods orders- which strip out volatile items such as aircraft orders - decreased by 1.3% last month, new data from the US commerce department shows. Despite lifting its forecast for UK growth a little for 2025, from 1.1% to 1.2%, the IMF also warns that growth risks “remain to the downside”. One reason is the US trade war. The IMF says: Tighter-than-expected financial conditions, combined with rising precautionary saving by households, would hinder the rebound in private consumption and slow the recovery. Persistent global trade uncertainty could further weigh on UK growth, by weakening global economic activity, disrupting supply chains, and undermining private investment. In today’s assessment of the UK economy, the IMF also suggest further tax rises may be needed to balance the books. The Fund argues that it is important to “stay the course and reduce fiscal deficits as planned over the medium term.” Risks to that strategy include high global uncertainty, volatile financial market conditions, and the challenge of containing day-to-day spending, they say, and warn: Materialization of these risks could result in market pressures, put debt on an upward path, and make it harder to meet the fiscal rules, given limited headroom. To this end, staff recommends adhering to the current plans, and implementing additional revenue or expenditure measures as needed if shocks arise, to maintain compliance with the rules. The UK also gets a hat-tip from the IMF for the trade deals announced in the last few weeks. The Fund says: Policy stability is critical to support business confidence in an increasingly uncertainty global environment. In this context, recent efforts to strike trade agreements with key partners, including the EU, India, and the US, demonstrate the authorities’ commitment to finding common ground and establishing a more predictable environment for UK exporters. On monetary policy, the IMF recommends that the Bank of England continues to ease interest rates “gradually”, while remaining flexible due to elevated levels of uncertainty. The Fund says: The pickup in inflation that began in 2024 is expected to last through the second half of this year, with a return to target later in 2026 as underlying inflationary pressures continue to recede. Although monetary policy calibration has become more difficult due to still-weak growth, the temporary rise in inflation and high long-term interest rates, staff sees the BoE’s gradual pace of easing as appropriate. Given the elevated uncertainty, the MPC is encouraged to retain flexibility to adjust the monetary stance in either direction if needed. The IMF also applauds Rachel Reeves’s recent changes to the fiscal rules, saying they “enhance its credibility and effectiveness”. But… the Fund also suggests the chancellor could “promote further policy stability” by having only one Office for Budget Responsibility assessment of her self-imposed fiscal rules each year, at the time of the Budget, rather than the current twice-yearly review. The Financial Times reports that this idea is under discussion in the Treasury, “according to several well-placed officials”. In what looks like a significant intervention, the International Monetary Fund is recomending that Rachel Reeves loosens her fiscal rules to prevent the need for emergency spending cuts. Adding to the clamour from backbench Labour MPs incensed by the government’s welfare cuts, the Washington-based organisation said the chancellor should examine ways to avoid making short-term savings when there is a downturn in economic forecasts, my colleague Phillip Inman reports. An easing of to the fiscal rules would potentially give the chancellor more breathing space on potential spending cuts. The IMF said the current system inherited from the previous Conservative government of twice-yearly assessments of the public finances by the Office for Budget Responsibility (OBR) was ripe for an overhaul. It said: “There is still significant pressure for frequent fiscal policy changes, given that small revisions to the economic outlook can erode the headroom within the rules, which is the subject of intense market and media scrutiny.” The IMF said Reeves could downgrade the significance of spring OBR report, give a broader outlook for the public finances – “de-emphasising” the single cash figure for spending headroom – or “establish a formal process so that small rule breaches do not trigger corrective fiscal action outside of the single fiscal event”. More here. The Chancellor of the Exchequer, Rachel Reeves, has responded to the IMF’s upgraded growth forecast for 2025, saying: “The UK was the fastest growing economy in the G7 for the first three months of this year and today the IMF has upgraded our growth forecast. We’re getting results for working people through our Plan for Change – with three new trade deals protecting jobs, boosting investment and cutting prices, a pay rise for three million workers through the National Living Wage, and wages beating inflation by £1,000 over the past year.” Newsflash: The International Monetary Fund has lifted its forecast for UK economic growth this year. Following an annual check-up on the British economy, the IMF has upgraded the UK’s expected growth rate this year to 1.2% from 1.1%, and reassured us that an “economic recovery is under way”. This reverse some of the IMF’s downgrade last month, when it cut the UK’s predicted growth this year from 1.6% to 1.1%. It follows the UK economy’s decent start to 2025, with growth of 0.7% recorded in the January-March quarter. Luc Eyraud, the IMF’s mission chief to the United Kingdom, told reporters in London this morning: “These revisions reflect the strong GDP performance in the first quarter, reflecting the resilience of the UK economy despite the complex external environment.” However, looking ahead, the IMF also warns that trade tensions linked to US tariff plans will reduce UK economic growth next year. It expects global trade tensions will wipe 0.3 percentage points off growth for the year, but is still predicting growth will increase to 1.4% in 2026. Trade tensions will weigh on growth through “persistent uncertainty, slower activity in UK trading partners, and the direct impact of remaining US tariffs on the UK”, the IMF warns. Ouch. Confidence among British retailers has fallen at the sharpest pace in five years. The latest healthcheck on UK retailing from the CBI shows that a decline in sales volumes gathered pace this month, and that stores expect conditions to worsen. The CBI’s quarterly gauge of business sentiment has dropped at its fastest rate since May 2020 this month. A net balance of -29% of firms expect their business situation to worsen over the coming three months, compared with -19% in February. The CBI’s monthly gauge of how retail sales compared with a year earlier fell to -27 this month - the lowest since March - from -8 in April, which had been its highest since October. A measure of expected sales for June fell to -37, the lowest since February 2024. Ben Jones, lead economist at the CBI, says: “This was a fairly downbeat survey and highlights some of the challenges facing the retail and wider distribution sector. In contrast to other recent retail data, this survey suggests parts of the sector are still struggling with fragile consumer demand, though online sales seem to be holding up better.” However, the official retail sales figures from the Office for National Statistics have been more optimistic laterly – they’ve shown a rise in sales volumes in recent months, helped by sunny weather. Economic sentiment across Europe has risen this month, the latest data from the European Commission shows. The EC’s economic sentiment indicator (ESI) has improved in both the EU (+0.6 points to 95.2) and the euro area (+1.0 points to 94.8). That’s an encouraging pick-up, following two months of declines, but both gauges are still below their long-term average. The EC reports that: The rise in the ESI for the EU was primarily driven by a partial rebound of confidence in the retail trade sector and among consumers, with a moderate contribution also from the construction sector. Confidence in both the industry and services sectors remained broadly stable. Among the largest EU economies, the ESI increased in Italy (+2.8) and in Germany (+1.5), but fell in France (-3.5), the Netherlands (-0.8), Poland (-0.6), and Spain (-0.4). Relief that trade tensions between the US and Europe have abated is pushing down the gold price. Gold has fallen by 1.3% to $3,297 per ounce, away from the record highs touched earlier this year. Relief that Donald Trump has delayed new higher tariffs on EU imports has pushed Germany’s DAX share index up to a new record high! The DAX has touched a new peak of 24,161 points this morning, up around 0.5%. It’s now up around 21% so far this year, outpacing other markets. Boom! Britain’s FTSE 100 share index has hit its highest level since early March. The UK’s blue-chip share index has risen over the 8,800 point mark for the first time in two and a half months, up 86 points or almost 1%. Ouch! Germany’s economy is on track for its worst performance in post-war history, a new report shows. The German Chamber of Commerce and Industry (DIHK) predicted this morning that Europe’s largest economy will contract by 0.3% this year, Reuters reports. That would be the third annual contraction in a row, although not as bad as the 0.5% fall in GDP which the DIHK predicted back in February. The DIHK also warned that the risk of recession persists, even though growth in the first quarter of the year was boosted by a scramble to pre-empt the US trade war. The DIHK forecasts German exports will decline by 2.5% in 2025, with 29% of companies surveyed expecting exports to fall over the next 12 months, while only 19% expect a rise. The London stock market is being pushed higher by “positive trade vibes”, reports Susannah Streeter, head of money and markets at Hargreaves Lansdown: “A mood of cautious relief is spreading after the long weekend, amid hopes for more fruitful trade negotiations between the United States and its global partners. There are no post bank holiday blues for the London market, with the Footsie in striking distance of the record high reached in February. More positive vibes are pulsing about the outlook for the global economy, with hopes that more scores can be etched on the doors of trade talks. “US futures point to a higher open on indices, as optimism spreads after the holiday break. Trump once again has pressed the pause button, this time on proposed 50% tariffs on imports from the European Union, which caused nervousness at the end of last week. But while the FTSE 100 is still up almost 1%, European markets – which rallied yesterday – are more subdued. Germany’s DAX has gained another 0.3%, while France’s CAC is 0.15% higher. The UK government is pledging to create tens of thousands of apprenticeships and training opportunities, as part of its push to increase workers’ skills and cut net migration. Ministers have promised a total of 120,000 new training opportunities for construction workers, engineers, healthcare staff and other trades in England before the next general election. Up to 45,000 training places will be funded by hiking the charge paid by employers for bringing in foreign workers by a third. Announcing the push, education secretary Bridget Phillipson said: “A skilled workforce is the key to steering the economy forward, and today we’re backing the next generation by giving young people more opportunities to learn a trade, earn a wage and achieve and thrive. When we invest in skills for young people, we invest in a shared, stronger economic future - creating opportunities as part of our plan for change. But everyone has a role to play in a thriving economy, and we’re taking our responsibility seriously providing more routes into employment, it’s now the responsibility of young people to take them.” European bond prices are rising this morning, pulling down government borrowing costs. The yield, or interest rate, on German 10-year bonds has dropped by four basis points (0.04 percentage points) to 2.519%. UK 10-year gilts are down almost 8 basis points, at 4.6%, while shorter-dated two-year gilt yields are down four basis points at 3.96%, the lowest in over two weeks. This follows a recovery in US Treasury prices this morning. Over the last couple of weeks, bond yields had been rising as prices fell amid a global debt sell-off. The Financial Times is reporting this morning that the UK government is shifting to shorter-term borrowing to lower its interest bill, and to lift some of the pressure on its tax and spending plans. Jessica Pulay, head of the UK’s Debt Management Office, told the FT that the DMO is softening Britain’s reliance on long-term borrowing. Short-term borrowing is typically cheaper than issuing longer-term debt, but it also means a country has to return to the markets more often. Stocks have jumped in London as trading resumes after the Bank Holiday weekend. City investors are relieved that Donald Trump has delayed his threatened hike on EU tariffs to 50% until July, cooling trade war fears. The FTSE 100 index of blue-chip shares is up 75 points, or 0.85%, to 8792 points, close to a two-month high. Engineering group Melrose (+3.8%) are the top FTSE 100 riser, followed by technology firm DCC (+2.4%) and Rolls-Royce (+2%). Food inflation in the UK has risen for the fourth month in a row, figures show, driven by increases in the cost of fresh produce, including steak. The annual rate of food price rises hit 2.8% this month, after a 2.6% rise in April, according to the latest shop price data from the British Retail Consortium (BRC). However, prices overall remained in deflation – 0.1% cheaper than a year ago and unchanged from last month – with the cost of non-food goods falling, particularly for electricals as retailers cut prices to drum up business before a potential hit from Donald Trump’s tariffs. Last night the EU’s trade commissioner Maros Šefčovič signalled that the bloc was “fully committed” to reaching a trade agreement with the United States. Šefčovič posted on X last night that he had had “good calls” with US commerce secretary Howard Lutnick and US trade representative Jamieson Greer, and that the European commission “remains fully committed to constructive and focused efforts at pace” towards an EU-US deal. More car news: Japanese manufacturer Toyota is moving some production of its GR Corolla sports car to Britain. According to Reuters, Toyota will spend around $56m on a dedicated production line at its Burnaston plant in Derbyshire, to produce 10,000 cars annually for export to North America from the middle of 2026. Reuters reports: By shifting some production from Japan, Toyota aims to use excess capacity in Britain to help it cut delivery wait times for the car, said the people, who spoke on condition of anonymity. The move was not in reaction to U.S. President Donald Trump’s tariffs on automobile imports, they said. Reuters adds that the Burnaston site has suffered a decline in production since Brexit. The news should cheer the UK government, as it There’s a sense of relief in the financial markets after Donald Trump delayed his threatened 50% tariffs on all European Union imports into the US. Trump had shocked investors last Friday when he announced he planned a 50% tariff on EU imports from the start of June. But following a call with European Commission president Ursula von der Leyen, that hike in levies has been delayed until 9 July, to give both sides more time to negotiate. Stocks are set to rally in London today, with Wall Street also set to rise, as trading resumes after the bank holiday break Yesterday, France’s CAC index rose by 1.2% while Germany’s DAX gained 1.7%, and the euro hit a one-month high against the US dollar. Tony Sycamore, market analyst at IG, reports that “risk sentiment improved” after Trump announced the delay to his 50% tariffs on the EU. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, cautions that market rallies are on “thin ice”. She explains: European markets are flirting with ATH [all time high] levels, US futures were also up yesterday — but the reality is that with every piece of incoming information, the collective welfare deteriorates. Today, we are in a worse position than we were a month ago. And a month ago, we were in a worse position than we were three months ago. The global trade negotiation period was supposed to last 90 days—and now, it ends all of a sudden. The tariffs won’t be brought below the 10% ‘universal’ level and market rallies are triggered not by good news, but by the least bad of the options — once Trump or his administration softens a previously crazy stance. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Tesla’s sales across Europe halved last month, as the backlash against Elon Musk continues to hurt his electric car company. The latest sales figures from industry body ACEA, released this morning, show that sales of Tesla cars fell by 52% year-on-year in the European Union in April, down to 5,475 units, from 11,540 a year before. They fell 49% in the wider “EU + EFTA + UK” area. The decline follows falls in Tesla sales in Europe in January, February and March, suggesting Musk’s controversial politics and association with the Trump White House are hurting the brand’s popularity, as anti-Musk protests have popped up at Tesla showrooms this year. The overall EU car market grew slightly in April, ACEA reports, with new car registrations rising by 1.3% year-on-year, “despite the ongoing unpredictable global economic environment”. So far this year, new battery-electric car sales have grown by 26.4%, to 558,262 units, capturing 15.3% of the total EU market share. Sigrid de Vries, ACEA’s director general, says: “The share of battery-electric vehicles is slowly gaining momentum, but growth remains incremental and uneven across EU countries.” Tesla’s sales in Europe this year have been disrupted by model changes, as it refreshed its offer with a new Model Y vehicle. But it also faces tough competition from China’s BYD, which sold more EVs than Tesla in Europe for the first time last month, according to market researcher Jato Dynamics. After several months shaking up US bureaucracy through the DOGE initiative, Musk appears to be refocusing on his day job. Last weekend Musk posted that he was “back to spending 24/7 at work and sleeping in conference/server/factory rooms”, as he became “super focused” on his social media company X, artificial intelligence initiative xAI, Tesla and SpaceX. The agenda 10am BST: Eurozone economic sentiment report 11am BST: CBI distributive trades survey of UK retailing 1.30pm BST: US durable goods orders data 2pm BST: US house sales</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>The IMF has upgraded its forecast for the UK economy this year. The Fund now forecasts UK GDP will increase by 1.2% this year, up from a forecast of 1.1% last month. Stock markets in the UK and the US have rallied, as trading resumes after a long weekend. Share prices jumped on relief that Donald Trump has delayed planned 50% tariffs on European goods until July.</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Time to wrap up… Britain’s private sector is shrinking for the second month running as factory output falls at the fastest rate in a year and a half, a new survey shows. The latest poll of purchasing managers at UK companies found that private sector output is decreasing in May, although at a slower rate than in April. The slowdown came as UK government borrowing rose last month to over £20bn, larger than expected. Economists said Britain’s high borrowing was creating pressure for more tax rises in the next budget. In other news… Britain’s factory downturn has continued, with manufacturers reporting a sharp fall in orders and output this month, US jobless claims fell last week, as America’s labour market remained solid Stocks have fallen in London, where the FTSE 100 share index is now down 78 points at 8708 points. Manchester United’s shares have fallen 8%, after they lost to Spurs in last night’s Europa League final Bond yields have risen too, as US debt fears worry investors The rise of weight loss drugs could dampen demand for cocoa, analysts at Rabobank have predicted in a new report. The rise of weight loss drugs could dampen demand for cocoa, analysts at Rabobank have predicted in a new report. Rabobank believe cocoa prices will go through a bumpy ride in the coming year, having soared in 2024, before dropping in early 2025 and then recovering in recent weeks. This turbulence has led to a fall in cocoa consumption this year, they say, as elevated cocoa prices will lead to higher retail prices. Manufacturers have also employed “shrinkflation and skimpflation strategies” – shrinking their chocolate products or putting less cocoa into them. Oran van Dort, commodity analyst for RaboResearch, says: “As a result, familiar chocolate products may become smaller and more expensive, with innovations focusing on minimizing cocoa use. Ingredients like wafers, nuts, dairy, cocoa butter equivalents, and sugar will become more prevalent, altering the consumer experience and potentially reducing chocolate’s presence in supermarket aisles.” Rabobank also suggests that a health-conscious consumer environment and increased use of weight-loss drugs also contribute to reduced demand. As flagged earlier, Manchester United’s share price has taken a tumble (-8%) as investors react to last night’s Europa League defeat… The selloff in UK shares is gathering pace. The FTSE 100 shares index is now down over 1%, having dropped by 95 points to 8691 points today. That’s despite a cautious open on Wall Street, where the Dow Jones industrial average is falt in early trading and the S&amp;amp;P 500 up 0.25%. US debt fears are causing ripples of worry in the markets, after yesterday’s poor auction of US government debt, reports Susannah Streeter, head of money and markets at Hargreaves Lansdown, adding: ’The growing mountain of US debt is causing ripples of worry across financial markets, with signs investors are baulking at financing the Trump administration. These concerns have hit sentiment in Europe, given the repercussions that financial difficulties in the world’s largest economy would have on the global economy Finance ministers and central bank governors from the Group of Seven nations pledged to address “excessive imbalances” in the global economy, according to a draft communique seen by Bloomberg News. G7 finance ministers and central bank chiefs have been meeting in Alberta, Canada, in the last few days, with the meeting to wrap up later today. According to Bloomberg, the draft communique – which summarises three days of meetings between the US, UK, Canada, France, Germany, Italy and Japan – says a common understanding of how “non-market policies and practices” undermine international economic security is needed. The draft calls for an analysis of “market concentration and international supply chain resilience,” and that officials agreed “on the importance of a level playing field and taking a broadly coordinated approach to address the harm caused by those who do not abide by the same rules and lack transparency.” More here. We have confirmation today that Mexico avoided falling into recession earlier this year. Mexico’s statistics body has reported this morning that Mexican GDP rose by 0.2% in the first quarter of this year, in line with its initial estimate. That follows a 0.6% contraction in October-December 2024. The takeover of regional news publisher National World by marketing business Media Concierge has been approved by a High Court judge. Media Concierge, which owns a number of Irish publications, already has 27.8% of National World’s shares, and made its buyout proposal last November. London-listed National World acquired the parent company of the Scotsman, Yorkshire Post and more than 100 titles, including the Sunderland Echo and Sheffield Star, for just £10m in 2020. America’s jobs market continues to shrug off the uncertainty caused by Donald Trump’s trade wars. The number of Americans filing new claims for unemployment support fell last week, by 2,000 people, new data shows. That pulled the weekly total of initial claims down to 227,000, suggesting US companies are still holding onto workers despite concerns that tariffs will demand and economic growth. Back in the bond markets, Britain’s long-term borrowing costs have hit their highest level in six weeks. The yield, or interest rate, on 30-year UK gilts has risen by 6 basis points to 5.56%, its highest level since 10 April. Neil Wilson, UK Investor Strategist at Saxo Markets, reports: Investors are pushing back against the tax and spending plans by the US administration – the bond vigilantes are only ever sleeping lightly. This is not just a US problem – we have seen incredibly weak bond auctions in Japan this week too. And in the UK we have the same problem – figures today show borrowing was £20.2bn, up £1bn from April last year and the fourth-highest April borrowing figure since monthly records began in 1993. Gilt yields ticked up. Financing domestic bliss and neverending entitlements cannot be sustained forever... Shares in Manchester United have fallen in pre-market trading, after the club were defeated by Tottenham Hotspur last night in the Europa League final in Bilbao. Manchester United’s stock is on track to fall around 5.5% when trading begins, having yesterday (before the game) hit its highest level in eleven weeks. Last night’s game (high on tension, but not a classic) has been dubbed the £100m showdown, and shareholders will be disappointed that Manchester United have missed out on the lucrative place in next seaason’s Champions League. Participation in the Champions League leads to earnings from tickets, broadcast money, and sponsor bonuses. Instead, Manchester United won’t play in European competition at all next season, which will damage the club’s revenues and profits for 2025-2026 as a rebuild gets underway…. Ooof. British factories have reported a sharp fall in orders and output this month, underlining how the economy appears to be stumbling. The CBI’s latest Industrial Trends report, just released, shows that manufacturing output volumes fell in the three months to May, at the joint-steepest pace since August 2020. Factory bosses are pessimistic about the short-term outlook too, with output expected to fall further over the three months to August. The CBI explains: Total order books weakened marginally in May, relative to April, while export order books improved from a sharply negative reading last month. But both total and export order books remain well below their long-run averages. Manufacturing firms reported that stock adequacy for finished goods was largely unchanged from last month, with the balance standing close to the long-run average. The CBI suggests that rising domestic business costs and US tariff uncertainty are hitting confidence. UK property firm British Land has declared that the “return to the office is in full swing”. In its latest financial results, British Land reports that mid-week occupancy at its offices is back to pre-pandemic levels, and that “value and multi-channel retailers are competing aggressively for space on our retail parks”. British Land’s CEO, Simon Carter, has told the FT that demand for high-end London offices is starting to “trickle down” to older buildings because of sky-high rents, fewer people working from home and a shortage of new properties. The jump in UK government borrowing last month (see opening post) is prompting predictions that the government will increase taxes in the autumn budget. Thomas Pugh, economist at leading audit, tax and consulting firm RSM UK, explains: Public sector net borrowing excluding Banks was £20.2bn in April, £1bn higher than in April last year. The good news was that borrowing in the 24/25 fiscal year was revised down to £148.3bn, meaning the overshoot compared to the OBR forecast was £11bn. With the public finances in a pretty dire state going into what is likely to be a much tougher Q2 and second half of the year for the economy, some fiscal consolidation in October, probably in the form of higher taxes, looks likely. “On the details, total government receipts rose by £5.1bn compared to April 2024 with the increase in NICs meant that compulsory social payments rose by £1.7bn. At the same time, expenditure rose by £4.2bn as inflation and pay rises raised pressure on government spending. “Looking ahead to the budget in October, the persistent over borrowing and under performance of the economy means some sort of fiscal consolidation is starting to look inevitable. Given the recent indications that there will be some sort of a U-turn on the cuts to winter fuel payments and the difficulty the government has had in getting even tiny reductions in welfare spending through parliament, it feels like any fiscal consolidation will come from higher taxes rather lower spending. Indeed, we expect a combination of higher taxes and slightly higher borrowing at the next budget. “The good news is that with interest rates likely to be around 4% at the time of the budget there is plenty of scope for the Bank of England to cut rates to offset the impact of any fiscal consolidation on the economy.” Britain’s private sector is shrinking for the second month running as factory output falls at the fastest rate in a year and a half, a new survey shows. The latest poll of purchasing managers at UK companies found that private sector output is decreasing in May, although at a slower rate than in April. Manufacturing production fell at the fastest rate since October 2023, although this was moderated by a “fractional rise” in service sector output. UK firms reported that clients were cautious this month, due to business uncertainty, leading to a drop in new orders. However, worries about US tariffs have dropped this month, after Donald Trump delayed tariffs on America’s trading partners and agreed a trade deal with the UK. Export orders fell this month, which manufacturers blamed on the new US 10% tariff on UK imports, and on wider uncertainty about global trade condititions. Worryingly, manufacturers reported that they cut jobs at the fastest pace in five years, through redundancies, restructurings, hiring freezes, and the non-replacement of departing staff. This was blamed on subdued demand, and higher payroll costs – following the increase in national insurance contributions at the start of April. Overall, the UK PMI composite index rose to 49.4, up from April’s 48.5, but still below the 50-point mark that separates expansion from contraction. Ouch. Private sector output across the eurozone has fallen for the first time in five months, as the sector slides into contraction. The latest poll of purchasing managers across the euro area shows that new orders continued to decrease, led by a slump in output in the services sector. Output in Germany, meaning Europe’s largest economy joined France in contraction territory. The rest of the euro area continued to outperform the largest two economies, although there was a slowdown here. Data firm S&amp;amp;P Global also reports that business confidence in the eurozone fell to a 19-month low. Its HCOB Flash Eurozone Composite PMI output index, which tracks activity, has fallen to a six-month low of 49.5 this month, down from 50.4 in April. Dr. Cyrus de la Rubia, chief economist at Hamburg Commercial Bank, said: “The eurozone economy just cannot seem to find its footing. Since January, the overall PMI has shown only the slightest hint of growth and in May, the private sector actually slipped into contraction. Do not blame US tariffs for this one. In fact, efforts to get ahead of those tariffs might partly explain why manufacturing has held up a bit better lately. Manufacturers have now increased production for the third straight month, and for the first time since April 2022, new orders did not decline. On the flip side, service providers, who are generally less exposed to US trade policy, except in areas like international logistics, are seeing business activity shrink for the first time since November 2024. While foreign demand for services is softening, it is the sluggish domestic demand that seems to be dragging the sector down. The share price of the FTSE 250’s Johnson Matthey has soared by 30% after it announced the £1.8bn sale of part of its business making catalysts for the chemical industry. Johnson Matthey announced the all-cash deal with US conglomerate Honeywell this morning. The UK company, which has been under pressure to increase cash generation from American activist investor Standard Investments, said it will return most of the money to shareholders, after costs of £200m for the transaction. The share price rose as high as £18.66 on Thursday morning, its highest in more than a year and well above the £13.89 closing price on Wednesday. However, it remains far short of the price above £32 in 2021 before it abandoned an effort to make electric car batteries. The British manufacturer has one of the most venerable histories on the London Stock Exchange, stretching back to a business testing precious metals in 1817, and spending years as a member of the FTSE 100 index of blue-chip companies. However, it has struggled in recent years as investors questioned what would replace its reliable earnings from catalytic converters on petrol and diesel cars after the electric vehicle transition. Liam Condon, Johnson Matthey’s chief executive, said that the Honeywell deal would realise 80% of the British company’s market value in return for only 20% of the company. “It’s quite an exceptional valuation.” Johnson Matthey will be left as a company selling catalytic converters to the car industry, and refining and recovering platinum group metals, plus a longer-term bet - yet to reach profitability - on growth in demand for green hydrogen made with renewable electricity. Condon insisted that the company was not abandoning its history of chemicals innovation, and said it would benefit from the transition away from fossil fuels because of demand for platinum group metals in hydrogen fuel cells, plus industries such as defence and pharmaceuticals. Condon also argued that investors had overestimated the pace of the transition away from petrol and diesel cars. Catalytic converters, which cause reactions that prevent harmful pollutants from being emitted into the air, will be “around for a long, long time”, Condon said. “The long-term outlook has improved versus three years ago because the electrification outlook has changed dramatically.” On hydrogen, Condon said that the technology was “taking longer than anybody thought” to become mainstream, and that there was “definitely an overhype” on its introduction. However, said that he expected the hydrogen bet to take off after five to 10 years. In the meantime, catalytic converter sales would continue to generate cash. “We can afford to wait now for the market to grow. We have a very big cash machine, with a free growth optionality on top.” The oil price has fallen by 1% this morning, on reports that the Opec+ group could lift crude output sharply again this summer. According to Bloomberg, Opec+ are considing increasing output by 411,000 barrels per day in July. That’s triple the amount initially planned, and would match previous increases agreed for in May and June. This has knocked Brent crude down to $64.25 per barrel, its lowest level in nearly a week. Shares in Bloomsbury, the book publisher behind the Harry Potter series, have dropped by about 15% this morning after a sharp fall in its pre-tax profit. The publisher’s pre-tax profit fell 22%, from £41.5m to £32.5m, in its latest financial year, which ended in February. Organic revenue, which strips out the contribution from its recent acquisition of academic publisher Rowman &amp;amp; Littlefield, was broadly flat at £341.2m. The company, which also publishes the fantasy A Court of Thorn and Roses series by Sarah J. Maas, said it remained “cognisant of the uncertain macroeconomic backdrop”, although noted that books remain exempt from US trade tariffs. The drop in Bloomsbury’s share price has put it at the bottom of the FTSE 250 today. However, it follows a strong few weeks for the stock, which had risen by about a tenth from the start of April up until yesterday. Market strategist Bill Blain of Wind Shift Capital is “increasingly convinced” a debt crisis is approaching. Writing after last night’s weak auction of US debt, Blain says: Global markets are increasingly nervous on the US debt-quantum – while it seeks to increase the fiscal deficit as rates rise, the dollar is no longer directing the proceeds of global trade into Treasuries, and confidence in American politics declines. Doh! It feels like we’re approaching the end game of this cycle – decades of financialisation, rising inequality (its apparently fine the bottom 10% of Americans will lose out to give the top 10% of Americans bigger tax breaks – and no one blinks), and the debilitating cold treacle of political meh. As that happens, markets are become less global and more insular – it will be Japanese investors that fund Japanese debt, meaning they aren’t going to fund the US. All of which spells crisis as the USA will be looking for investors to fund the deficit as a time when Trump has managed to offend about everyone. It means higher and higher US yields – precipitating the debt crisis. More here: The UK government borrowed more than expected in April, underscoring the challenge for Rachel Reeves to fix public services and grow the economy while meeting her fiscal rules. With the chancellor under pressure on Labour’s tax plans, the Office for National Statistics (ONS) said public sector net borrowing rose to £20.2bn in April, £1bn more than the same month a year earlier. City economists had forecast borrowing of £17.9bn. More here: Stock markets are falling today, as investors fret about a worryingly weak auction of US government debt last night. In London, the FTSE 100 index fell 45 points at the open to 8741 points, away from the record high set in February. European markets are also in the red, with Germany’s DAX falling 0.4%, and France’s CAC down 0.5%. Stocks are weakening after investors shunned an auction of $16bn of 20-year US government bonds yesterday, forcing the Treasury Department to offer an interest rate, or yield, of over 5% to attract interest. That’s the highest rate on this type of bond since 2020, and may be a sign that demand for US assets is waning, less than a week after Moody’s downgraded the US credit rating from Aaa to Aa1. This prompted a selloff on Wall Street last night, as Jim Reid of Deutsche Bank explains: The soft 20yr auction was also a trigger for a broader market slump, with the S&amp;amp;P 500 falling from -0.2% on the day to -1.61% by the close, its worst day in the past month. This was a very broad-based decline with only 18 advancers in the whole index and the equal-weighted version of the S&amp;amp;P down -2.15%. Food ingredients firm Tate &amp;amp; Lyle has warned this morning that Donald Trump’s trade war will push up its costs and hurt sales. Tate &amp;amp; Lyle told shareholders that “tariffs and the associated uncertainty” have increased costs, mainly for products supplied between the US and China. With Washington and Beijing having agreed a 90-day truce earlier this month, Tate &amp;amp; Lyle are now awaiting “clarification on tariffs”. But in the meantime, it currently expects that revenue growth will only reach the bottom of its medium-term range, or slightly below it. Tate &amp;amp; Lyle also reported a 5% rise in revenues for the last financial year (to the end of March), although operating profits almost halved to £106m. The group sources raw foodstuffs from around the world, and creates ingredients designed to offer crunch or creaminess, add fibre, or a give a sweet taste to foodstuffs without the attendant calories. They originate from the likes of corn, tapioca, seaweed, stevia leaf and citrus peel. Chief Secretary to the Treasury, Darren Jones, has responded to April’s jump in borrowing, saying: “After years of economic instability crippling the public purse, we have taken the decisions to stabilise our public finances, which has helped deliver four interest rate cuts since August, cutting the cost of borrowing for businesses and working people. “We’re fixing the NHS, with three million more appointments to bring waiting lists down, rebuilding Britain with our landmark planning reforms and strengthening our borders, delivering on the priorities of the country through our Plan for Change.” Any night owls trying to browse the M&amp;amp;S website overnight would have been sorely disappointed. As of 6:20am this morning, visitors were still being greeted by a static landing page that simply read: “Sorry you can’t browse the site currently. We’re making some updates and will be back soon.” For now, the site seems up and running, though online orders are still paused. It’s not clear how long the outage ultimately lasted. When contacted this morning, M&amp;amp;S’ press office refused to say whether this was part of regular maintenance or linked to ongoing disruption from last month’s devastating cyber attack. M&amp;amp;S also refused to confirm whether customers should expect more website outages - cyber attack related or otherwise - in the coming weeks. M&amp;amp;S has been left with some empty shelves and been forced to halt online orders on its website after the hack on Easter weekend. The attack targeted customer personal data, which could have included names, email addresses, postal addresses and dates of birth. The company said on Wednesday that the attack had been caused by “human error”, and could end up costing the first around £300m. CEO chief executive Stuart Machin has said general disruption could last until July. The tax take from inheritance tax also rose last month. Figures from HMRC show that inheritance tax receipts rose by £97m year-on-year in April to around £800m. Shaun Moore, tax and financial planning expert at Quilter, predicts this upward trend will continue: With property prices remaining high and nil-rate bands still frozen until 2030, more families are being caught by IHT, many without realising until it’s too late. Upcoming changes to business and agricultural relief from 2026, and the inclusion of unused pensions in estates from 2027, mean this trend is unlikely to reverse any time soon. For those who are worried about IHT, gifting remains the best defence against it, but this should be weighed against your own needs. It’s not all bad news for Rachel Reeves, though. The Office for National Statistics has revised down its estimate for borrowing in the last financial year, to £148.3bn. That’s £3.7bn less than the initial estimate, but still £11bn more than had been forecast by the Office for Budget Responsibility (OBR). Today’s borrowing figures are “disappointing”, and highlight the Chancellor’s lack of wiggle room, says Ruth Gregory, deputy chief UK economist at Capital Economics. Gregory told clients: April’s public finances figures showed that despite the boost from the rise in employers’ National Insurance Contributions (NICs), the fiscal year got off to a poor start. This raises the chances that if the Chancellor wishes to stick to her fiscal rules, more tax hikes in the Autumn Budget will be required. Here’s a chart showing the details of today’s public finances: Good morning, and welcome to our rolling coverage of business, the financial markets and the eurozone. It’s a new financial year, but the same old story for the UK government, as borrowing rises faster than expected. The latest public finance figures, just released, show that the UK borrowed £20.2bn in April. That’s £1bn more than in April 2024 and the fourth-highest April borrowing since monthly records began in 1993. City economists had forecast a deficit of around £18bn, so the new financial year has not gott off to a great start for Rachel Reeves, at a time when the chancellor is under pressure to raise taxes to avoid cuts to welfare payments. The public finances report shows that central government’s current receipts rose by £5.1bn year-on-year, due to increased tax receipts – including £1.7 billion in Income Tax, £500m in Value Added Tax (VAT), £500m in tobacco duty, £400m in stamp duty (on land and property), and £200m in Corporation Tax receipts. However, spending rose too – central government’s current expenditure increased by £4.2bn, as pay rises and inflation pushed up the cost of goods and services, and some benefits increased in line with inflation. ONS deputy director for public sector finances Rob Doody says: “At £1 billion higher than the same time last year, this April’s borrowing was the fourth highest for the start of the financial year since monthly records began more than 30 years ago. “Receipts were up on last April, thanks partly to the higher rate of National Insurance contributions. However, this was outweighed by greater spending, due to rising public services’ running costs and increases in many benefits and state pensions.” Happily, though, the interest payable on central government debt fell by £500m to £9.0bn, due to lower payments on inflation-linked bonds. The agenda 7am BST: UK public finances for April 9am BST: Eurozone ‘flash’ PMI report for May 9am BST: IFO survey of eurozone business confidence 9.30am BST: UK ‘flash’ PMI report for May 11am BST: CBI industrial trends 1.30pm BST: US weekly jobless claims 1.30pm</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Britain’s private sector is shrinking for the second month running as factory output falls at the fastest rate in a year and a half. UK government borrowing rose last month to over £20bn, larger than expected. The rise of weight loss drugs could dampen demand for cocoa, analysts at Rabobank have predicted in a new report.</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Time to recap US consumer sentiment has fallen again as fears over tariffs drive up inflation expectations. The University of Michigan’s preliminary May sentiment index has declined to 50.8 from 52.2 a month earlier, weaker than forecast, as trade war fears hit the US economy. Economists are hopeful that sentiment will improve, though, now that the US and China have paused their trade war. In the UK, King Charles’s personal fortune increased to £640m in the past year, making him as wealthy as the former prime minister Rishi Sunak and his wife, Akshata Murty, according to the Sunday Times rich list. The 76-year-old monarch, who acceded to the throne in 2022, recorded a £30m increase in wealth and ranks joint 238th on the list of the UK’s wealthiest people and families. The estimate of the king’s wealth is based on personal assets, including the investment portfolio he inherited from his late mother and private estates at Sandringham and Balmoral, and does not include the crown estate. According to the list, there are 156 UK-based billionaires, down from 165 last year, marking the third year in a row the number has fallen. The fall was blamed on recent market turbulence, and the crackdown on non-doms. The biggest drop in wealth was felt by Sir Jim Ratcliffe, the founder of Ineos and a part-owner of Manchester United, whose fortune fell by about £6bn. There were protests in London today, calling for a wealth tax to help fund better public services. In other news: The eurozone’s trade surplus with the US has surged The CEO of Novo Nordisk boss is stepping down, under pressure over its falling share price Microsoft has offered to sell its Office product without Teams at a lower price than Office with Teams, to placate EU antitrust regulators Japan’s economy has shrunk for the first time in a year The UK stock market has ended the week in a sunnier mood. The FTSE 100 share index has closed 51 points higher at 8684 points, up 0.6% today, its highest closing level since the last week of March. Alexandra Brown, North America economist at Capital Economics, is hopeful that US consumer sentiment should soon rebound, now the US and China have paused their trade war. Brown explains: The weaker-than-expected May print of the University of Michigan consumer sentiment index was driven by a further increase in inflation expectations and suggests households remain wary about the tariff outlook. Nevertheless, given the recent big de-escalation with China, we expect a marked rebound in sentiment next month. Sentiment among US consumers has continued to deteriorate this month, as people worry that Donald Trump’s trade war will drive up prices. US consumer confidence has dropped again in May, according to the latest sentiment gauge from the University of Michigan. The survey found that inflation expectations have jumped and that Americans are concerned that their personal finances will suffer from weakening incomes. Here’s the details: The index of Consumer Sentiment: fell to 50.8 this month, down from 52.2 in April, and down 26% year-on-year A measure of Current Economic Conditions fell to 57.6, down from 59.8, and down 17.2% year-on-year The Index of Consumer Expectations fell to 46.5, down from 47.3, and down -32.4% year-on-year Surveys of Consumers director Joanne Hsu explains: Tariffs were spontaneously mentioned by nearly three-quarters of consumers, up from almost 60% in April; uncertainty over trade policy continues to dominate consumers’ thinking about the economy. Note that interviews for this release were conducted between April 22 and May 13, closing two days after the announcement of a pause on some tariffs on imports from China. Many survey measures showed some signs of improvement following the temporary reduction of China tariffs, but these initial upticks were too small to alter the overall picture – consumers continue to express somber views about the economy. Hsu adds: Year-ahead inflation expectations surged from 6.5% last month to 7.3% this month. This month’s rise was seen among Democrats and Republicans alike. Long-run inflation expectations lifted from 4.4% in April to 4.6% in May, reflecting a particularly large monthly jump among Republicans. Shares in space tourism firm Virgin Galactic have jumped by a quarter in early trading, as investors hail its latest results. Virgin Galactic reported last night that it is “keeping pace” with its plans to begin commercial spaceflight in 2026. The company reported: First spaceflight with new SpaceShip carrying research payloads planned for summer 2026. Private astronaut spaceflights planned for fall 2026. Midway through feasibility study to potentially develop second spaceport in Italy. Marketwatch reports that Virgin Galactic also suggested its ticket prices could be higher than expected: Speaking during a conference call to discuss the results, Virgin Galactic Chief Executive Michael Colglazier said that the company expects to open the first wave of spaceflight reservations in the first quarter of 2026. Specific pricing has not been set, according to Colglazier, although Virgin Galactic expects that this will increase relative to the company’s last price of $600,000. The company’s shares are up 26% at $4.29, which still leaves them down 98% over the last five years…. Over in New York, the stock market has opened a little higher, adding to this week’s gains. The S&amp;amp;P 500 share index is up 3 points, or 0.05%, at 5,920 points. It has gained almost 2% over the last five days, on relief after the US and China agreed a pause in their trade war that cut tariffs for 90 days. Just in: there are signs that Donald Trump’s flurry of tariffs may have cooled the US housing market. U.S. single-family homebuilding fell in April by 2.1%, new data shows, to an annual rate of 927,000. That may show that tariffs on imported materials dampened demand, along with high mortgage rates. Overall housing starts in April rose by 1.6%, though. But, applications for building permits – to allow future construction, dropped by 4.7% on a monthly basis in April, and were 3.2% lower than in April 2024. There’s drama in the pharmaceuticals world, where the boss of Denmark’s Novo Nordisk has unexpectedly resigned. Novo Nordisk, which produces the weight loss drug Wegovy and the diabetes medication Ozempic, says Lars Fruergaard Jørgensen is stepping down “as per mutual agreement” with the company’s board. Jørgensen appears to be leaving in response to rising competion in the weight loss drug market, which has led to Novo Nordisk’s share price more than halving over the last year. The company says that Novo Nordisk Foundation Board recently “initiated a dialogue with the Novo Nordisk Board on the merits of an accelerated CEO succession”, adding: Considering the recent market challenges, the share price decline, and the wish from the Novo Nordisk Foundation, the Novo Nordisk Board and Lars Fruergaard Jørgensen have jointly concluded that initiating a CEO succession is in the best interest of the company and its shareholders. Lars Fruergaard Jørgensen has agreed to continue as CEO for a period to support a smooth transition to new leadership. Just last week, Novo Nordisk cut its annual revenue and profit forecasts, as it faced rising competition from US rival Eli Lilly, which makes the diabetes and obesity drugs Mounjaro and Zepbound. Donald Trump’s trade war has taken another twist. The US president has revealed today that his administration will write to trading partners telling them their new tariff rates “over the next two to three weeks.” That’s something of a u-turn, given Trump has previously spoken about cutting new trade deals with other countries. He appears to have realised that agreeing over one hundred new deals in just a few months is not practical. Trump said today that Treasury Secretary Scott Bessent and Commerce Secretary Howard Lutnick “will be sending letters out essentially telling people” what “they’ll be paying to do business in the United States.” During a meeting with business executives in the United Arab Emirates, Trump said: “I think we’re going to be very fair. But it’s not possible to meet the number of people that want to see us.” Trump announced new tariffs on imports from a swathe of countries on 2 April, only to pause them for 90 days a week later after the financial markets tumbled. The US is now maintaining a new “baseline” 10% tariff on imports. Young people from the climate action group Green New Deal Rising have staged a protest outside White’s, the London private members club, today to call for new wealth taxes. Green New Deal Rising held the protest to promote their new PAY UP campaign – which calls for the super-rich and big corporations pay “their fair share” of tax - to fix rumbling services, fund real climate action, and create a fairer society. They are pushing for a 2% tax on the wealth of individuals such as the Duke of Westminster, Denise Coates and Jim Ratcliffe, who all feature highly on this year’s Rich List. Green New Deal Rising have also released a new poll, conducted by YouGov, which found: 58% of Brits believe this Government’s economic policies currently best serve wealthy individuals (40%) and large corporations (18%) compared to UK businesses (3%), the working population (3%), and ordinary British people (2%) It also found that 64% of Brits support introducing a cap on the amount individuals can donate to a political party each year and 73% believe young people today are worse off than their parents’ generation. Hannah Martin, co-director of Green New Deal Rising, says: “Every year, the Sunday Times Rich List exposes the huge wealth of Britain’s super-rich who have seen their fortunes explode over the last thirty years. Meanwhile, millions of us can’t heat our homes, pay our rent or get a doctor’s appointment. All whilst this Government claims there is no money to fund the climate action we desperately need to protect our futures. The British public clearly think that this government’s policies serve the wealthy and large corporations. But instead of taxing people like Jim Ratcliffe and Nick Candy fairly, Keir Starmer and Rachel Reeves want to impose even more cruel cuts to the most vulnerable. These are political choices and we want the Government to choose differently. It’s time for the people who lock themselves away in private luxury clubs like White’s to pay up for our schools, hospitals, homes and climate action.” Today’s Rich List should be a reality check for the government, argues Caitlin Boswell, head of advocacy and policy at Tax Justice UK. Just 350 ultra-rich individuals and families hold more wealth than the GDP of countries like Belgium, Argentina or Ireland. At the same time, record numbers of people are using food banks, too many people are waiting for healthcare appointments, schools don’t have enough money to teach our children well and local services are being slashed. The government is trying to balance the books by cutting support for disabled people while millions are already struggling to keep a roof over their head and put food on the table. The government must catch up and start taxing wealth to fix the country and improve people’s lives, so that all of our communities can flourish.” Microsoft has offered the European Union an olive branch over charges that it illegally linking chat and video app with Office 365 products. The US software giant has offered to sell its Office product without Teams at a lower price than Office with Teams, and offer rivals better interoperability access to its services and products, EU antitrust regulators said today. The European Commission said it was now going to seek feedback from rivals and customers before deciding whether to accept the offer. Microsoft’s Vice President for European Government Affairs Nanna-Louise Linde said in a blogpost that the proposal was a clear and complete resolution to concerns raised by rivals and would give Europeans more choice. Last June, the EC accused Microsoft of illegally linking its chat and video app Teams with its Office 365 suite of products including Word. The charges could potentially lead to a large fine. Donald Trump won’t like this! Europe’s trade surplus with the US has swelled, as the US president ratched up trade war tensions. Data provider eurostat has reported that the EU’s trade balance with the US swelled to €40.7bn in March, up from €16.7bn a year earlier. Exports to the US jumped by 59.5%. Overall, the EU posted a €35.3 bn surplus in trade in goods with the rest of the world in March 2025, compared with €22.3 bn in March 2024. The increase was driven by a jump in chemicals and related products. Data last week showed that the US trade deficit swelled in March as firms rushed to import goods such as pharmaceuticals, ahead of new tariffs being imposed. Shares in Future, the owner of magazines and websites including Marie Claire, TechRadar and GoCompare, have tumbled more than 6% after the publisher said it now expects revenues to decline this financial year due to “ongoing macroeconomic uncertainty”. The UK-based company revised its outlook after reporting a 3% fall in revenues and 4% decline in adjusted profits in the six months to the end of March. Future said it is adopting a “more cautious view” of the second half of its financial year and now expects a “low single digit” decline in full year revenues. The company, which closed a number of underperforming magazines and websites last year including Total Film, said that digital advertising in the US declined in March but returned to growth last month. It also said that foreign exchange rates represent a “headwind” based on current rates. Revenues at its GoCompare division fell 1% in the first half as the volume of car insurance quotes declined, however revenue from non-automotive insurance quotes climbed 10%. Kevin Li Ying, chief executive of Future, says: “Whilst the wider macroeconomic environment remains challenging, the quality of our content and intent-driven audience, and the uniqueness of our tech stack, underpinned by our strong financial characteristics, position us well to deliver long term growth in what is an ever-evolving media landscape.” Japan’s economy has shrunk for the first time in a year, helping to cement the UK’s position as the fastest growing member of the G7 so far this year. New data today shows that Japan’s real gross domestic product (GDP) contracted by 0.7% in annualised terms (or -0.2% during the quarter), a larger fall than expected. It’s the first quarterly contraction since January-March 2024. The decline was due to stagnant private consumption and falling exports, suggesting the economy was losing support from overseas demand even before Donald Trump announced sweeping “reciprocal” tariffs on 2 April. Sam Jochim, economist at EFG Asset Management, says: Japan’s GDP contracted by more than expected in Q1, falling 0.2% over the quarter. The contraction was the first in a year and reflected weakness in exports, likely due in part to the yen appreciation in the first three months of the year that would have impacted Japan’s export competitiveness. The partial offset, and main positive within the data was that domestic demand remained strong. In addition, Japan’s potential growth rate is estimated by BoJ staff at around 0.5% year-on-year. This equates to a quarterly growth rate of around 0.1%, which is lower than for many economies and means any deviations below this can easily result in a contraction. With only Canada yet to report Q1 GDP data, here’s how the G7 line up. UK: +0.7% growth in January-March Italy: +0.3% growth Germany: +0.2% growth France: +0.1% growth US: a -0.1% contraction Japan: a -0.2% contraction Alex Beard isn’t the only person to lose their billionaire status this year. The Sunday Times Rich List also shows that Suneil Setiya and Greg Skinner, who founded hedge fund Quadrature Capital, are now worth £980m each, a drop of £35m. Strive Masiyiwa, the telecommunications and technology entrepreneur who founded Econet, has also slipped out of the club – his wealth dropped sharply in the last year, down £538m to £968m. Malcolm Healey, the founder of Wren Kitchens, also had a bad year. Healey and his family’s net wealth has been cut by £600m this year to £901m, meaning they’re no longer Yorkshire’s richest family (a title now taken by Portakabin creaters the Shepherd family). Thor Bjorgolfsson, once Iceland’s first billionaire, has had his wealth more than halved! It’s dropped to £806m, down from £1.666bn in 2024. Igor and Dmitry Bukhman, the Russian-born brothers who founded mobile gaming company Playrix, top the list of the wealthiest people under the age of 40 in London. Playrix has produced popular mobile titles including Fishdom, Township, Homescapes and Gardenscapes. More than 100 million people play their games each month, giving the Bukhman brothers a combined wealth of £12.54bn – up over £6bn over the year – and 10th place on the main Rich List. Brewdog cofounder James Watt and reality TV star Georgia Toffolo appear on the Rich List this year, following their marriage. Watt, who created “punk” brewer BrewDog, and Toffolo, who appeared on “Made in Chelsea” and “I’m a Celebrity... Get Me Out of Here!” and now runs a talent-management agency and a dog food business, have a combined wealth of £425m. They married in March, despite Watt’s concerns that he might miss out on tax relief for investing in Toffolo’s dog food operation. Toffolo told the Sunday Times that the pair squeezed the honeymoon into two days between work commitments, explaining: I suppose I’ve always had a particular type: powerful, successful men. Because I’m so ambitious myself, I think I would be insufferable for someone who wasn’t at the top of their game themselves. And watching James’s devotion to work, to creating new things, is amazing. We talk about work constantly. When we sit down to supper we’ll talk about the intricacies of a board meeting he’s just had. I know that wouldn’t be for everyone, but I find it invigorating. The family owners of Bet365 swelled their estimated wealth by almost £2bn last year, as they weigh up a potential sale of their gambling empire. Denise, John and Peter Coates are now worth £9.44bn, today’s Rich List estimates, up £1.978bn over the last year, due to their ownership of Bet365. That value could soon be crystallised; earlier this month, the Guardian reported that the Coates family are weighing up a sale that could value the business – founded in a Portakabin in a Stoke car park- at £9bn. Pop star Dua Lipa is the youngest person to feature on this year’s Sunday Times 40 Under 40 Rich List. Dance The Night singer Lipa, 29, who has won several Brit Awards and three Grammys, is 34th on the list, with an estimated wealth of £115m. In 2024 she released her third studio album, Radical Optimism. She also headlined Glastonbury Festival’s Friday evening slot last year, in a set dubbed “an unequivocal success” by our own Alexis Petridis. Commodity giant Glencore’s former head of oil, Alex Beard, has lost his billionaire status due to stock market turbulence. Beard, a highly successful commodity trader, is now worth £991m according to the 2025 Rich List, a drop of £224m. Glencore’s shares have almost halved over the last year, as commodity prices were hit by fears that a global trade war would trigger recession. In August 2024, Beard was charged with bribery offences relating to the Swiss commodity trader’s operations in Africa. He is set to stand trial in a London court in 2027 having indicated he will plead not guilty. Luke Hildyard, Executive Director of the High Pay Centre, says today’s Rich List highlights the connection between the excess wealth of “Britain’s billionaire class” and the country’s low pay and poor public services. Hildyard explains: “The rich list is a useful annual reminder of the inefficiency of the UK economy. It shows a small fall in the value of oligarch assets this year, but over a longer period it illustrates how a tiny handful of very rich people have captured an increasing share of the country’s wealth. If the super-rich and the companies they own were taxed more effectively and paid the people that work for them a better wage, living standards in Britain would be much higher. Meanwhile the rich list entrants would still be extremely rich by any reasonable person’s definition and well rewarded for whatever success they have achieved. It’s naive to pretend that taxing or limiting billionaire wealth would be easy, but equally such extreme concentration of income and wealth is very obviously not sensible or efficient and policymakers should surely be a lot more energetic in trying to do something about it.” King Charles’s wealth has reportedly soared over the last year to £640m, matching former prime minister Rishi Sunak and his wife Akshata Murty, who have moved in the opposite direction. Today’s Rich List shows that the King’s personal wealth has jumped by £30m to £640m in the last year. That lifts him to joint 238th in the list of the UK’s 350 wealthiest people and families, up 20 places from 258th in 2024. The Sunday Times concedes that the magnitude of the King’s wealth divides opinion, as assets – such as the £15.5bn Crown Estate – are owned “in the right of the Crown”, and are not the King’s private property. But as they explain, Charles built up his wealth over the years by saving the profits he received from the duchies of Lancaster and Cornwall – two vast property empires that generate private income for the monarch and the monarch’s male heir respectively (corrected). Charles also inherited a large investment portfolio from Queen Elizabeth, which the Rich List says is worth about £125m, as well as valuable assets such as Sandringham and Balmoral. But his wealth exceeds £640m, by some measures. Back in 2023, the Guardian reported that King Charles’s private fortune was estimated at £1.8bn. At £640m, the King is now tied with Sunak and Murty, whose wealth has slipped to £640m from £651m, That’s due to a drop in the value of Murty’s stake in Infosys – the tech company founded by her father, which was hit by worries over US tariffs. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. The number of British billionaires has fallen, as the super-rich are hit by stock market turbulence and the end of tax breaks for non-doms. The Sunday Times’s annual totting-up of Britain’s richest people, just published shows that the number of billionaires slid to 156 this year from 165 in 2024. That’s the sharpest decline in the Rich List’s 37-year-history. The Sunday Times reports that “falling fortunes” have led many to drop off the list, while others are no longer eligible, having “fled Britain after Labour’s non-dom crackdown”. Robert Watts, compiler of the Rich List, says: “Our billionaire count is down and the combined wealth of those who feature in our research is falling. “We are also finding fewer of the world’s super rich are coming to live in the UK.” In March 2024, then-chancellor Jeremy Hunt announced plans to axe the UK’s tax breaks for non-doms, which allowed foreign nationals who live in the UK to avoid paying UK tax on their overseas income and gains. One London-based billionaire non-dom left the UK for good on the day of Hunt’s announcement, a tax advisor revealed. Rachel Reeves tightened the policy in her first budget, before then softening the changes in an attempt to woo the rich. The Sunday Times has calculated that the combined wealth of the 350 entries on the Rich List has dropped by 3% over the last year, to £772.8bn, the third consecutive drop in collective value. The entry level flatlines at £350m. For the fourth successive year, the list is topped by Indian-born industrialist Gopi Hinduja, 85, and family with a fortune of £35.3bn, down from £37.1bn in 2024 due to the drop in the value of their stock market-listed companies. Overall, the Hinduja’s companies operate in automotive, oil and speciality chemicals, banking and finance, IT, cybersecurity, healthcare, trading, infrastructure project development, media and entertainment, power, and real estate. David and Simon Reuben and family have risen to second place, with £26.8bn (up from £25bn last year) overtaking Sir Leonard Blavatnik, whose wealth has dropped to £25.725bn (from £29.2bn) due to a drop in his stake in Warner Music Group, There are some eye-catching fallers on the list too, including businessman Sir Jim Ratcliffe. He’s dropped from 4th to 7th, after his wealth declined to £17bn from £23,5bn in 2024. Britain’s billionaires will have gained wealth in the last few weeks as global stock markets recovered from their plunge in early April, when Donald Trump launched his global trade war. The agenda 9.30am BST: Hong Kong GDP report for Q1 2025 10am BST: Eurozone trade balance report for March 1.30pm BST: US building permits and housing starts data for April 3pm BST: University of Michigan survey of US consumer sentiment for May (flash estimate)</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>The University of Michigan’s preliminary May sentiment index has declined to 50.8 from 52.2 a month earlier, weaker than forecast. Economists are hopeful that sentiment will improve, though, now that the US and China have paused their trade war. King Charles's personal fortune increased to £640m in the past year, making him as wealthy as the former prime minister Rishi Sunak and his wife.</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Time to recap… The chair of Thames Water has admitted its finances were “hair raising”, as he said bosses were in line for “substantial” bonuses linked to an emergency £3bn loan. The UK’s biggest water company came within just five weeks of running out of money, Adrian Montague told MPs on Tuesday. “Thames in the last year has come very close to running out of money entirely,” he said. He added there were times where it only had weeks’ worth of cash left. “Running a £20bn corporation on five weeks’ liquidity, honestly, it’s hair raising,” he said. Montague also said some executives at the struggling water company were in line for payouts amounting to “50% of salary, very substantial bonuses” as part of the high-interest emergency debt package, which was approved by the high court in February. During the hearing, chief executive Chris Weston also warned that he couldn’t guarantee there wouldn’t be restrictions on water use this summer, but was confident that Thames wouldn’t run out of water. Weston said the crisis at Thames had been ‘decades in the making’, due in part to a lack of leadership and turnover in the boardroom. Montague insisted that the new team was committed to fixing the problems at Thames. Elsewhere today… Inflation in the US has dropped to a four-year low in April, the month that Donald Trump announced his sweeping “liberation day” tariffs on the US’s largest trading partners. The annual inflation rate was 2.3% in April, down from an annual rate of 2.4% March, according to a new inflation report from the Bureau of Labor Statistics (BLS). The unemployment rate in the UK has risen to its highest level in almost four years, according to official figures, as the jobs market continues to slow. The Office for National Statistics (ONS) said the rate was 4.5% in the first three months of this year, up 0.2% on the previous quarter and the highest reading since summer 2021. The ONS also reported that UK wage growth slowed, as firms reduced their vacancies and cut the number of staff on their payrolls. Wall Street has opened higher, as investors welcome the drop in US inflation today. The S&amp;amp;P 500 share index gained 0.64%, up 37 points at 5,881 points. The tech-focused Nasdaq has risen by over 1%. The drop in inflation may be reassuring traders that the Federal Reserve will have space to cut interest rates this, if it needs to stimulate the US econonomy. The Dow Jones industrial average is in the red, though, down 119 points at 42,290.86 points. It’s been dragged down by UnitedHealth (-13%), which today announced that CEO Andrew Witty was quitting immediately for “personal reasons” as it suspended its annual outlook. Starling Bank has been ordered to launch an external review and boost compliance training after CMA said it had concerns about an “underlying weakness” in the online lender’s procedures. The challenger bank’s breaches related to data it fed into customer satisfaction surveys, which it regularly tops. It was found to have excluded 17% of personal account customers from data handed to a market research company in both 2023 and 2024, and also overstated the total number of accounts held by customers to the competitions regulator between 2020-2023. It comes months after the bank was hit with a £29m fine by the Financial Conduct Authority in October 2024, over “shockingly lax” controls that the FCA said left the financial system “wide open to criminals”. That included failures in its automated screening system for individuals facing government sanctions. The CMA said on Tuesday that excluding a large number of customers from the data was a “material breach”, and while the impact on the rankings was likely “negligible”, it risked undermining consumer confidence in the survey results. The CMA said it was “concerned that there may be an underlying weakness in Starling Bank’s procedures.” It added: “The CMA has concerns that formal action may be necessary to prevent a recurrence. This is because Starling Bank has now breached the requirements to provide full data on current account holders twice and we are not convinced that Starling Bank is capable of preventing further breaches through the initiatives mentioned above.” Starling said that the exclusions were due to a lack of appropriate oversight, and that the over-reporting was a misunderstanding of the regulatory requirement. Starling itself notified the CMA of the breaches last year and was called into the regulator in November to discuss the matter. The bank has now been issued with directions that include hiring an external firm to carry out a review of its processes and procedures, and will now have to provide extra compliance training for staff. Starling said in a statement: “Last year we identified some reporting errors related to the CMA’s customer satisfaction surveys. We informed the CMA of our findings, we apologised, and we changed our processes to prevent a recurrence. We are pleased that the CMA has now determined that the impact on customers was ‘negligible’ and that the bank has overpaid rather than underpaid its dues. We will continue to work constructively with the CMA because we share their goal of ensuring that people can see which banks are listening to their customers and meeting their needs.” MPs also heard today that Thames Water’s senior executives will receive large “retention incentives” funded through the £3bn emergency loan it agreed recently. Chair Sir Adrian Montague told the EFRA committee that the deal “required” Thames to create a retention plan for its senior management team, which he called “our most precious resource”. That plan will pay out in three installments – when the first restructuring plan is agreed, then when the second restructuring is agreed, and then a larger amount at the end of the process. The first two installments are worth 50% of salary, which Montague agrees is “very substantial”. He reveals its the first time he’s encountered this sort of deal. And he denied that Thames was swayed to choose the funding offer from its A-class creditors, rather than a rival offer, at a lower interest rate but no such retention scheme, from B-class shareholders. Customers should take into account that they are not paying these bonuses, Montague insists: This amount will be funded by the lenders, and at the end of the day borne by the lenders. It’s hard to see much impact from Trump’s tariffs in today’s inflation report, says Heather Long, the Washington Post’s economics columnist. The drop in US inflation in April suggests that the tariffs are yet to feed through to inflation, says Seema Shah, chief global strategist at Principal Asset Management, adding: Yet, it is questionable whether or not today’s CPI print really moves the needle after the rollercoaster ride of the past month. After all, not only is the April CPI report unlikely to have fully captured the tariff impact post-Liberation Day, but inflation numbers will now be further whipsawed by the US/China trade truce announcement. An inflation impulse will likely come through during late Q2, but may be partially and quickly eroded if container traffic rapidly resumes in light of the drop in US/China tariffs. The implication is that a clear read on the inflation trend won’t be visible for several months yet. This prolonged inflation uncertainty likely implies a prolonged Fed pause. “ Donald Trump will be pleased to see inflation has managed to ease slightly in the US, says Lindsay James, investment strategist at Quilter. But the US is “far from out of the woods” when it comes to inflation, James adds: The first quarter of the year saw businesses ramp up their inventories as they looked to stockpile ahead of ‘Liberation Day’. As such, price rises are very much delayed, and we can still expect inflation in the US to spike because of these policies. This is, of course, why the Federal Reserve is reluctant to cut interest rates at this point. The reprieve for Chinese goods will likely lead to some more re-stocking before the end of the 90-day period. But while tariffs are much reduced since yesterday, they remain markedly higher than before the 2nd April. The ‘Art of the Deal’ means no-one knows how permanent these tariffs may become, if at all, or if they will be reintroduced in a less harsh form. However, businesses will become increasingly wary of the shifting sands beneath their feet as these deadlines approach. Given we are already almost at the halfway point of Trump’s 90 day pause for the ‘reciprocal tariffs’ on other nations, we may soon see them building in more margin through price rises to protect themselves from sudden changes in policy making. Tariffs are not the only thing weighing on inflation either, however, and there remain some other underlying factors that aren’t changing as quickly. Food prices in the US remain elevated despite Trump’s campaigning to lower those pressures for consumers. Today’s inflation figure may paint somewhat of a sanguine picture, but scratch lightly under the surface and it is clear the US faces a number of risks. With economic growth slowing at the same time, the Fed is left in a bind of where to go from here. Risk of policy misstep, therefore, is growing and as such market volatility remains very much on the table.” Newsflash: US inflation was lower than expected last month, despite fears that tariffs will push up costs. On an annual basis, US consumer price inflation fell to 2.3% in April, down from 2.4% in March, the lowest reading since February 2021. Economists had expected the rate would be unchanged. This might cheer Donald Trump, and bolster his claim that he is easing the price pressures hitting US households. The Bureau of Labor Statistics (BLS) reports that food prices rose by 2.8% over the year, while energy prices were 3.7% cheaper than a year ago. Shelter (housing costs) rose by 4% year-on-year. During the month, prices rise by 0.2% in April, having dropped by 0.1% in March. The BLS says: Indexes that increased over the month include household furnishings and operations, medical care, motor vehicle insurance, education, and personal care. The indexes for airline fares, used cars and trucks, communication, and apparel were among the major indexes that decreased in April. The Bank of England’s chief economist, Huw Pill, has underlined his concerns about wage growth, suggesting it might mean rates have to stay higher for longer. Speaking at a conference at the London School of Economics today, he said he was concerned about the upside risks to inflation, which might get stuck above the Bank’s 2% target. Pill said that could, “mean that the response of monetary policy, in order to ensure that we get back to our target within a reasonable cycle, needs to be somewhat more aggressive or more persistent in itself.” Jaguar Land Rover has welcomed the US-UK trade deal announced last week, after reporting its highest annual profit in 10 years. JLR posted a £2.5bn pre-tax profit in the year to 31 March, its highest profit in a decade. The company is pleased that the UK has negotiated down tariffs on cars exported to the US, saying: In April, at the start of the new financial year, we implemented a series of short-term actions to address the immediate impact of trade tariffs introduced by the US Administration on the global automotive sector. On 8 May 2025 we welcomed the positive announcement of a US-UK trade deal. This reduces US trade tariffs on UK auto exports to the US from 27.5% to 10%, within a quota of 100,000 vehicles. This deal brings greater certainty for our sector and stakeholders. We will continue to engage with the UK Government on the detail of the trade deal. Our priority is to ensure we deliver for our global clients and protect EBIT through delivery of transformation and efficiency initiatives. Thames Water’s CEO concedes that the company has run up “extremely high” costs on advisors, which total around £159m. That bill reflects the fact Thames is the “largest restructuring of a balance sheet in British history”, Chris Weston says. Life would be “extremely difficult for everyone” if Thames Water falls into a special administration regime (effectively nationalisation), its chair told MPs. Adrian Montague suggested that suppliers might wonder how much longer they wanted to work for Thames; senior management might also consider their position, and there would be a considerable burden on government, who could face £5bn of extra costs, and would need to eventually find a buyer for the business. Touching again on Thames’s cash squeeze, Sir Adrian Montague says the company’s liquidity was very tight when it was negotiating with lenders recently. Having only five weeks liquidity “is a nightmare” for a large company such as Thames, Montague says. But, he insists, Thames was in a “beggers can’t be choosers situation” when it was negotiating the deal to provide a £3bn lifeline. Montague adds: We were running along the edge of the precipice, and we had to secure the financial future of the company. MPs have also quizzed Thames Water’s top brass about its future ownership. Chief executive Chris Weston told the committee it was still a “very fluid situation”, despite investment firm KKR having been chosen as the sole bid to invest in the company. He says there is still a possibility that Thames could go back to other interest parties if “if the current process fails”. Other options are that creditors step in, and execute a debt-for-equity swap. Or, there is a possibility the company could still fall into public ownership. Weston says: “It’s a very fluid situation but those both are possibilities.” “There’s no guarantee we would not stay on a market-led solution as opposed to a special administration, but it is a very fluid situation and those are all possibilities.” Sir Adrian Montague then refuses to give a commitment to Helena Dollimore MP that the Thames Water top team at the committee hearing (him, CEO Chris Weston, and CFO Steve Buck) will remain in place through this parliament. We live in a competitive marketplace, Montague points out, adding: We have to live in the real world. No-one will give you a commitment that will be no change in the leadership team over five years. It is simply not possible. Q: So how can we have any faith in the commitments you are making? “We are the new kids on the block,” Montague declares, adding “We are making progress. We are here to try to put things right.” We won’t quit until the job is done, but it is not realistic to say there will be no changes in the team over 5 years. Q: Why would headhunters recruit from a failing company? “It’s not a failing company”, Montague fires back, “it’s a company in recovery”. We are making progress. This is a good team. You can see how the progress is starting to become apparent. Committee chair Alistair Carmichael seems unimpressed, asking: Q: If a 40% rise in pollution incidents is a sign of success, what does failure look like? Montague says “We must go back into those pollution incidents”. Thames Water chair Sir Adrian Montague then defends the company’s controversial decision to pay dividends, rather than investing in improving its infrastructure. Montague says Thames decided to pay the ‘intergroup’ dividend, of £157m, in October 2023 so it could keep discussions about future capital injections with then-shareholders alive. “In the event, that failed”, he admits. But at the time, Thames didn’t know it wouldn’t work. Helena Dollimore MP points out that a better use of that would have been to mend pipes, or to fund the 100 infrastructure projects that were delayed in summer 2023. UPDATE: Montague may have his dates mixed up here. The Guardian reported last June that this £150m dividend was agreed in March 2024, having already faced investigation for paying a £37.5m dividend in October 2023, for which it was fined. Thames CEO Chris Weston then feels more heat over his bonus payments. He reveals that Thames’s front-line staff can qualify for bonuses worth 3%-6% of their salary, while Weston can earn 156% of his salary in a bonus. Weston concedes that “it is a lot of money”, but argues that Thames must offer competitive packages to attract and retain the staff it needs. Labour MP Helena Dollimore says there is a “clear discrepancy” here, and that if Thames was truly committed to improving its infrastructure it would have more focus on the morale of front-line staff, and support them better. Thames Water’s chair has admitted to MP’s that the company came worryingly close to running out of money in the last year. Tackled over Thames’s decision to delay 100 vital infrastructure projects, to prevent storm overflows and pollution incidents, in August 2023, Sir Adrian Montague reveals He says: Thames in the last year has come very close to running out of money entirely. There were times in the last year when we had five weeks of liquidity. Running a £20bn corporation on five week’s liquidity is “hair-raising”, Montague says. He explains that the decision to delay those projects was the start of a process to fight a “funding crunch”, as “we felt we needed to conserve cash”. Montague denies that the money was used on bonuses, which he says are necessary to retain staff. Thames Water is taking steps to prepare for a possible drought this summer, its CEO insists (even though its desalination plant at Beckton is still out of action). Chris Weston tells MPs on the EFRA committee that Thames has four levels of drought awareness, and has just raised that level from zero to 1. That means: Thames is checking all its reservoirs are as full as can be – they are currently 94% full now, and the company is trying to top them up. it is going through all its plants to ensure all critical maintainance is done before the summer It will also start to communicate the importance of conserving water to customers. Weston says: At the moment, from what I can see, we have learned the lessons from the situation in 2022 and we are doing all that we need to at the moment to prepare for water shortage. I hope that is not necessary. Q: How confident are you that you won’t run out of water this summer? Weston replies that he is confident Thames won’t run out of water. But, he’s not confident that it won’t have to restrict usage, as that will depend on weather and rainfall. MPs then tackle Thames Water about the problems with its water desalination plant in Beckton, east London. CEO Chris Weston confirms that the plant, which is designed to turn salty seawater into fresh drinking water, will be out of action again this year, despite fears there could be a drought. Weston says the desalination plant, which cost £250m, is a big problem, and reveals he wonders why it was built (!). He tells the EFRA committee: It is not a good story, it was not a good investment. There are no excuses about it. Thames Water’s chairman, Sir Adrian Montague, tells MPs that there is a “vast amount to be done to bring performance up to scratch”. City grandee Montague, who was appointed in summer 2023, says: We know we are letting customers down. We know that pollution, spills, supply interruptions cause inconvenience and sometimes real hardship. He adds that a discussion about Thames’s turnaround plan should start by achnowledging that the company “haven’t always served our customers as well as we should, and through the committee apologising to them”. That turnaround is starting to yield “real progress”, Montague insists, saying that green shoots are there – citing improvements on supply interruptions, and water quality. It’s such a big business, you can’t hope to put everything right straight away. You’ve got to choose your targets, and little-by-little improve it overall. Q: Staff are worried about the future, because of the uncertainty over Thames’ ownership. Can you guarantee that their jobs, pay, terms and conditions will be maintained? CEO Chris Weston swerves away from the word “guarantee”, as he doesn’t know how things will change. But, he insists, he sees a growing employee base, over the last year and over the next five years. Staff should take comfort from that, he argues. However, it would be “more difficult” if Thames Water falls into a special administration regime – but even then, jobs should be protected as Thames must keep providing services. Weston goes on to criticise short-term decisions to cut staff in the past, which undermined its performance. He promises to fight for jobs, if Thames’s new owner pushes for efficiency savings, saying: I will fight for every job in Thames. MPs then turn to the BBC’s recent (revealing) documentary into the Thames Water crisis. Q: Why did CEO Chris Weston tell the BBC that “I won’t know how it got this way”, after 10 months at the company? What’s his analysis today? Weston replies that he has a pretty clear idea now, and was also pretty clear then, but questions the value of “talking about it publicly and pointing the finger” [in which case, why allow TV cameras into the company?!]. Weston tells the EFRA committee there are “many authors” responsible. He says: I’m clear how we got here. This has been decades in the making, the crisis we face at Thames. I think all actors had a role to play in this. Absolutely, the company and management has got something wrong. Five chief executives in five years is not a recipe for success, and I would argue consistency in leadership is a very important part of what we need to do now. But, Weston also takes aim at the UK’s regulatory regime, saying it is flawed. Regulators need to attract investment into the sector, and allow companies who are in trouble to turn around and improve – Weston argues that it doesn’t do that at the moment. Thames Water CEO Chris Weston is then tackled about his decision to accept a £190,000 bonus after three months at the company. Q: Was that a wise thing to do, given your focus on providing leadership? Weston says his remuneration was agreed with the board before he joined. By and large, he says, people do recognise the magnitute of his job. And he insists that he did “make a difference” in his first three months. Weston says he started to put a new organisation structure in place, and started to give Thames staff “confidence and reassurance” that they could take pride in their job. That helped to stabilise the company, and I think that was important. Thames Water chief executive Chris Weston has blamed “confusion” and a lack of direction from previous bosses for the problems that have beset the company. Testifying to the Environment, Food and Rural Affairs Committee this morning, Weston says he has been making progress since becoming CEO 16 months ago. He explains: “Where it had gone wrong is that Thames has lost direction a bit.” Weston tells the committee he was the 5th CEO appointed in five years, and that 26 members of the executive team had changed in that time. That churn has created “a confusion for people in the company,” Weston explains, insisting that Thames staff weren’t unwilling to do their job or take on accountability. He says he has provided clearer direction at the company, created a better organisation structure and a governance structure to allow him and the board to understand performance at the company,. Weston says: “I want the people in the company to feel that they have clear direction, they have the right resources and they are supported in what they do. My job is to make them feel supported and confident in what they are doing.” Weston also tells MPs he was “very impressed” with Thames’s performance when he joined the company: “2.6bn litres of clean water every day, 5bn litres of waste dealt with every day. I couldn’t help but be impressed, coming from outside the industry”. And he adds that he is “quite pleased with the progress we are making” at the company. (one which became notorious for sewage spills, a push for higher bills, and a debt pile that threatens its future). Weston cautions, though: It’s going to take a long time to turn Thames around. Over in parliament, MPs are digging into the crisis at Thames Water. The Environment, Food and Rural Affairs Select Committee (EFRA) are quizzing top brass at the water company – CEO Chris Weston, chair Sir Adrian Montague CBE, and CFO Steve Buck. You can watch it here. MPs are planning to cover the following issues… Leadership and culture at the company Recent court case and appeal Current ownership The future of Thames Water Thames Water’s selection of KKR as its preferred bidder Price review, performance, and penalties Returns to investors and profitability Executive pay and bonuses UK pub chain Marston’s has swung back to a profit in the first half of its financial year, thanks to a busy Christmas and Mother’s Day, as well as a tighter focus on costs. The pub owner reported a pre-tax profit of £19m in the 26 weeks ended on 29 March, compared with a loss of £0.2m in the comparable period in 2024. That was largely driven by a sharper focus on costs, as revenue was broadly flat at £427.4m. But more recent sales growth has been much stronger thanks to a busy Easter season: like-for-like sales in the 5 weeks since 29 March grew by 10.5%. Chief executive Justin Platt has said he is “excited for the summer months ahead”. Shares in Marston’s bounced by as much as 6.4% in early trading on Tuesday. Goldman Sachs has lowered its estimate for the likelihood that the US economy falls into recession in the next year, following an easing in trade war tensions. Economists at Goldman have cut the chances of a US recession in the next 12 months to 35%, down from 45%. The move follows the agreement reached by the US and China yesterday to sharply reduce tariffs for the next 90 days. That deal means US importers will only pay a 30% tariff on imports from China, down from 145%. Goldman now forecast the US economy will grow by 1% during 2025, twice as fast as the 0.5% previously forecast. The bank says: Their revised forecast reflects a combination of a lower effective tariff rate and the recent easing of financial conditions. A month ago, Goldman raised the odds of a US recession to 45% from 35%, after Donald Trump announced a swathe of tariffs on trading partners – which have all now been paused while trade negotiations take place. Goldman has also lifted its forecast for gains on the US stock market this year, saying: We raise our S&amp;amp;P 500 return and earnings forecasts to incorporate lower tariff rates, better economic growth, and less recession risk than we previously expected. Our new 3- and 12-month returns forecasts are +1% and +11%, indicating levels of 5900 and 6500 (previously 5700 and 6200). Warm weather in the UK has helped drive demand for DIY and gardening equipment, retailer Wickes has reported. Wickes reported a 9.6% rise in revenues in the 17 weeks to 26 April, which it partly credits to decent weather in recent weeks. Wickes tells the City: We have been well positioned to benefit from the warmer weather at the start of this year, which has supported the strong sales performance in Retail. For example, in the week of the early May bank holiday we had our biggest ever week for sales of compost and top soil. Wickes strikes a cautious note, though, adding that “the consumer outlook remains uncertain and the business faces significant cost headwinds”. Marks &amp;amp; Spencer has revealed that “some personal customer information” was taken during the cyber-attack which hit the retailer last month. In a statement on LinkedIn, M&amp;amp;S adds that there is “no need for customers to take any action”, as the information does not include usable card or payment details. The company has told the City: Today, we are writing to customers informing them that due to the sophisticated nature of the incident, some of their personal customer data has been taken. M&amp;amp;S says it will prompt online customers to reset their passwords when they next log in, adding: Everyone at M&amp;amp;S is working around the clock to get things back to normal for customers as quickly as possible, and we are very sorry for any inconvenience they have experienced. Our stores remain open as they have throughout. M&amp;amp;S has been battling the disruption caused its cyber-incident for more than three weeks. It was forced to halt all orders through its website and apps at the end of April. At the start of May, the Information Commissioner’s Office said it had received reports from Marks and Spencer, and also the Co-op Group, which was also hit by a cyber attack. The largest employment falls were seen in UK retail and hospitality in the last quarter, reports Stephen Evans, chief executive of Learning and Work Institute (L&amp;amp;W). Evans adds: Pay growth is fastest in those sectors as the rise in the minimum wage takes effect. That, along with rises in national insurance and other changes, may show the pressures employers are facing. Time will tell whether this is an indicator of a broader slowdown or a temporary effect.” According to the ONS, the number of employees in the accommodation and food services sector has fallen by 107,000 in the year to April, while there was an 87,000 rise in employees in the health and social work sector. The increased cost of hiring workers in the UK is continuing to dampen the job market, according to the Institute of Directors. Alex Hall-Chen, Principal Policy Advisor for Employment at the Institute of Directors, says: “Today’s figures indicate declining employer demand for labour in the UK job market, with the number of payrolled employees decreasing on the month by 0.1% and vacancies falling by 42,000 on the quarter. “The business case for hiring has been weakened by a perfect storm of last month’s increased employer National Insurance Contributions and above-inflation increases to the minimum wage, alongside a wave of measures in the Employment Rights Bill which will make hiring staff riskier and costlier. “If the government is to achieve its aim of an 80% employment rate, it must take urgent action to restore business confidence in hiring. We urge the government to support targeted changes to the Employment Rights Bill which would ensure that the Bill works for both businesses and employees.” Economists are concerned that the UK’s jobs market appears to have cooled in recent months, judging by today’s labour statistics. Suren Thiru, ICAEW economics director, fears the employment market is cooling, saying: “April’s drop in payrolled employment and unemployment rate increase suggests that cracks in the labour market are widening as the double whammy of rising National Insurance and National Living Wage hit employers, exacerbated by elevated global uncertainty. “While wage growth remains uncomfortably high, the downward pressure from a struggling economy, softening jobs market and rising employment costs should help put pay settlements on a firmer downward path. “Although more difficult times lie ahead for the jobs market with sinking business confidence and rising employment costs likely to drive a modest rise in unemployment, any increase should be limited by longstanding employer concerns over skills shortages. “This growing softness in the labour market is unlikely to be sufficient to persuade rate setters to depart from their current approach to gradually cutting interest rates, given lingering concerns over inflation and heightened global uncertainty.” Paige Tao, economist at PwC UK, suggests the weakening jobs market could spur the Bank of England towards further interest rate cuts: “If last month’s labour market data hinted at an early response to upcoming employer tax rises, this month’s figures confirm a clearer weakening. Unemployment ticked up for the first time in four months by 0.1 percentage point, payrolled employment fell by 33,000, and vacancies dropped further — staying below pre-pandemic levels for a second straight month. Heightened uncertainty around U.S. tariffs have likely added to the drag on business confidence. “Wage growth has cooled, with annual earnings including bonuses easing by 0.2 percentage points in March — suggesting fading inflationary pressures from pay in advance of April’s tax changes. As the Bank of England continues to balance inflation risks with growing weakness in the UK growth outlook, today’s figures may indicate a green light for another rate cut at next month’s MPC meeting.” Lindsay James, investment strategist at Quilter, fear today’s jobs report may be “the start of the expected slowdown”, adding: The unemployment rate ticked up slightly to 4.5% in January to March 2025, while payrolled employee numbers fell by 47,000 between February and March 2025 and by 63,000 between March 2024 and March 2025.</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Thames Water came within five weeks of running out of money last year. Chairman Adrian Montague said bosses were in line for ‘substantial’ bonuses. Chief executive Chris Weston said crisis had been ‘decades in the making’</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Time to wrap up…. Donald Trump has floated cutting tariffs on China from 145% to 80% before a weekend meeting as he looks to de-escalate the trade war. Top US officials are expected to meet a high-level Chinese delegation this weekend in Switzerland in the first significant talks between the two nations since Trump provoked a trade war with stiff tariffs on imports. The US president wrote “80% Tariff on China seems right! Up to Scott B” on his social media account on Friday morning, referring to Scott Bessent, the treasury secretary. Bessent and Jamieson Greer, the US trade representative, will meet their counterparts in Geneva in the most senior known conversations between the two countries in months, the Trump administration announced this week. It comes amid growing US market concern over the impact of the tariffs on the prices and supply of consumer goods. Stock markets in Europe have rallied on hopes of a thawing between the two sides. The latest trade data from China has shown that exports to the US, and imports the other way, both fell in April, as shipments to the rest of the world picked up. While in the UK, Bank of England governor Andrew Bailey has said the UK now needs to do everything it can to rebuild its long-term trade relationship with the European Union. He told the BBC: “Having a more open economy to trade with the European Union … would be beneficial, because there has been a fall-off in goods trade with the EU over recent years.” The Bank’s chief economist, Huw Pill, has predicted that US tariffs are not likely to have a “dramatic” effect on Britain’s economy. In a presentation today, Pill said: “The analysis in the baseline forecast does not suggest that there’s a dramatic shift in the behaviour of the UK economy on the back of these trade announcements and trade uncertainties.” Switzerland and the United States have agreed to accelerate their trade talks and are determined to reach an agreement quickly, Swiss President Karin Keller-Sutter has revealed. Keller-Sutter was speaking at a news conference after meeting US treasury secretary Scott Bessent and chief trade negotiator Jamieson Greer in Geneva, ahead of their talks with China this weekend. Wall Street has opened a little higher, as traders grasp onto hopes of progress in the US-China trade war. The main indices have all risen in early trading, as investors eye this weekend’s negotiations in Switzerland, and digest Donald Trump’s suggestion that China’s tariffs could be cut to 80%. Here are the early moves: Dow Jones industral average: up 123 points or 0.3% at 41,491 points S&amp;amp;P 500: up 25 points or 0.45% at 5,689 Nasdaq Composite: up 132 points or 0.75% at 18,060 That follows gains in Europe today, where Germany’s DAX index hit a new all-time high. Hopes of a thawing in US-China trade tensions are boosting stocks, reports Fawad Razaqzada, market analyst at City Index: Bullish momentum picked up for global stocks after reports emerged that the US is considering reducing tariffs on Chinese goods to below 60%, a significant pullback from the punitive 100%+ levies imposed earlier. However, Trump has posted on his social account that the levy could be reduced to only 80%, which “seems right” according to him, although that it is up Scott Bessant ahead of the weekend talks with Beijing. Meanwhile, China’s exports to the US have already taken a hit, with the latest data showing a marked slump. But the real damage from those tariffs is only just starting to show. Markets, though, are forward-looking—and any sign of easing tensions is enough to get investors back into risk assets, as we have seen in the last few weeks. Australia’s Macquarie Group has snapped up a UK smart meter rental business. Spain’s Iberdrola has agreed to sell its SP Smart Meters Assets – which it owns through Scottish Power – to Macquarie Group for almost £900m. The sale to Macquarie, whose previous investments include now-troubled Thames Water, is expected to complete in the third quarter of the year. Earlier today Macquarie also warned that global trade is under “the most intense pressure for decades”, as it reported a 5% increase in annual profits in the last year. Donald Trump’s suggestion that tariffs on China should be cut to 80% may have disappointed some investors. Earlier today, Bloomberg reported that the US had set a target of reducing tariffs below 60%, as a first step that they felt China may be prepared to match. Newsflash: Donald Trump has suggested that the US tariffs on Chinese goods should be 80%. Posting on his Truth Social site, the US president says: 80% Tariff on China seems right! Up to Scott B. Scott B is presumably Treasury secretary Bessent, who is due to meet with Chinese Vice Premier He Lifeng in Switzerland this weekend to discuss the trade war. An 80% tariff would be a notable reduction on the 145% which Trump imposed last month, but would still make it significantly more expensive for US companies to import goods from China than before the trade war began. Trump has also urged Beijing to open up its markets, posting: CHINA SHOULD OPEN UP ITS MARKET TO USA — WOULD BE SO GOOD FOR THEM!!! CLOSED MARKETS DON’T WORK ANYMORE!!! Reminder: trade data from China earlier today showed a drop in shipments to, and from, the US. European Commission President Ursula von der Leyen has suggested she could visit Washington to meet President Donald Trump to discuss trade negotiations – but, crucially, once a “concrete” trade package is on the table. Speaking in Brussels today, von der Leyen said: “If I go to the White House, I want to have a package we can discuss. It has to be concrete, and I want to have a solution that we both can agree on. That is the work we are doing right now.” More here. An index of fear in European stock markets has dropped to its lowest level since just before Donald Trump’s ‘Liberation Day’ tariff announcement at the start of April. The Euro Stoxx Volatility Index has fallen by 2% today to around 20 points, its lowest since 28 March. In the days after Trump kicked off his trade war the index had hit a three-year high over 50 points, before falling back after the US president paused his global tariffs for 90 days. Britain’s new trade deal with the US could lead to more foreign investment into the UK, explains Professor Costas Milas, of the University of Liverpool’s management school: However “incomplete” the new US-UK deal might look and be, it signals smooth long-term business relationships between the U.S. and the UK. In fact, foreign car companies and those involved in production of steel and aluminum might be tempted to increase foreign direct investments (FDIs) in the UK to get indirect access to the U.S. market. As I explained in a recent co-authored paper, additional FDIs will translate into higher wages and productivity in the UK. The US-UK deal is reasonably good news. Goldman Sachs are sticking with their view that the Bank of England will cut interest rates sharply in the second half of this year, and in early 2026. Following yesterday’s quarter-point rate cut to 4.25%, in a split decision, Goldman don’t expect another cut in June. But it then expects cuts at every meeting from August until next March, which would mean six reductions, reducing rates by 1.5 percentage points. Goldman says: Given today’s signals towards a continued quarterly pace of cuts, we no longer expect the MPC to cut Bank Rate at the June meeting, as this would likely require material downside surprises in the near-term data. That said, we maintain our view that a weaker economy—including softer growth, pay gains and inflation—will push the MPC into faster rate cuts in H2. We therefore now expect a pause in June but maintain our forecast for sequential 25bp rate cuts from August to an unchanged terminal rate of 2.75% in March 2026 (versus February before). German manufacturer Siemens Energy (+2.7%) is leading the risers on the DAX this morning. It’s followed by pharmaceuticals group Merck Group (+1.86%) and carmaker BMW (+1.8%), two companies exposed to the US trade war, who would benefit from an easing of tensions. Back in Reykjavík, Bank of England governor Andrew Bailey has pointed out that the US-UK trade deal still leaves tariffs on most British exports to the US higher than before April. Bailey also reiterated that the deal was good news, saying: “It’s good news in a world where it will leave the effective tariff rate higher than it was before all of this started.” Jochen Stanzl, chief market analyst at CMC Markets, has explained why Germany’s DAX share index has the potential to push higher, setting new record highs: The framework established by Trump’s London pact is essentially a loosely defined intention that primarily provides the U.S. president with an exit strategy: it allows him to claim later that he does not need to reactivate the reciprocal tariffs. The markets celebrate this agreement not because it shines in every detail but because this rough framework might be sufficient to maintain the temporary suspension of countersanctions permanently. The DAX continues its upward trend, with the record high tantalizingly close. With the Friedrich Merz government poised to unveil its Agenda 2030, it is a good moment to examine the current state of the DAX. Analysts anticipate an average earnings growth of six percent over the next twelve months, followed by almost thirteen percent in the subsequent year. The current price-to-earnings ratio (P/E ratio) of around 17 suggests that the index could rise to 24,700 points solely based on expected earnings growth over the next twelve months, eventually reaching 27,900 points in two years—assuming investors continue to accept a relatively high valuation level. From a political and economic standpoint, this potential arises in two ways: Firstly, the prospect of expansive fiscal programs—such as increased spending on infrastructure, energy, and defense—will drive revenues and profits for DAX-listed companies. Secondly, the gradual normalization of monetary policy following the inflation surge in recent years is likely to lower interest rates, further supporting stock prices. Andrew Bailey also warns that central bankers will continue to face a “challenging” and unpredictable environment, adding to the challenge of setting interest rates. He tells his audience in Reykjavík: We must learn the lessons from the difficulties we have faced as policymakers and forecasters over this period. Our models, infrastructure and analytical frameworks were challenged by the sheer scale and unpredictability of the shocks that hit us. Underlying issues were revealed under the stress of these big unforeseeable events. Forecasting became much more difficult, irrespective of the specific models and approaches used. We need no reminder that the global economic environment is likely to continue to be challenging – and less predictable – than it was in the past. So we need to adapt and develop to ensure that our processes are nimble and robust, and that our monetary policy decisions are communicated effectively, while ensuring that we continue to act methodically in response to inflationary pressures. Over in Iceland, Bank of England governor Andrew Bailey has insisted that the BoE is fully committed to its inflation target. Speaking to the Reykjavík Economic Conference, Bailey insists: Our commitment to the 2% inflation target is unwavering. Bailey is outlining the challenge of setting monetary policy in a world beset by major shocks, which drive up prices or hit demand. He reminds his audience: A sequence of unprecedented global shocks has created a very challenging environment for monetary policy. The largest pandemic in a century, the largest war in Europe since 1945, and now a trade war between the world’s two largest economies – these are not small and simple disturbances to aggregate demand, and they come against a backdrop of low productivity growth and ageing populations. While it remains to be seen how recent changes to global trade policies will play out and what the effects on our economies will be, the effects of the pandemic and Russia’s brutal war on the Ukrainian people are fresh in our minds. Our economies have suffered, inflation has surged. These have been hard times for businesses and households, not least those on lower incomes. Shares in BP have jumped 2.4% towards the top of the FTSE 100 leaderboard this morning, as takeover speculation continues to swirl around the UK oil company. The Financial Times has stirred the pot this morning, reporting that Shell, Chevron, ExxonMobil, TotalEnergies and Adnoc have all separately run the numbers on whether a bid would make sense. As the FT explains, BP does appear undervalued: A sum of the parts valuation suggests BP’s assets are worth in excess of £120bn, without including debt and liabilities, more than twice its current market capitalisation of £57bn, which follows a sharp slump in its shares over the past 12 months. “The continued underperformance of BP makes it open to a takeover,” said a person close to the activist investor Elliott Management, which has built a leading stake in the company. A week ago, Bloomberg reported that Shell had been eying up BP, a move that would create a major energy giant. Germany’s stock market has recovered all its losses following Donald Trump’s “Liberation Day” tariff shock five weeks ago. The Dax, which tracks the largest companies listed in Frankfurt, has risen over its previous record high – set in March – this morning. The rally comes amid a wider rise in European stocks this morning (see earlier post), due to hopes that the US-UK trade deal could be an encouraging signal for other negotiations. Neil Wilson, UK Investor Strategist at Saxo Markets, reports: Trade deal optimism seemed to be reflected in a positive move for equity markets, with European stock markets rising on Friday – the DAX hit a record high this morning at 23,500. Bloomberg reports that hopes of increased government spending, under new chancellor Friedrich Merz, has also supported stocks in Germany: The DAX, which had previously lost as much as 16% amid heightened market volatility due to Trump’s tariff announcements, has recovered as the new government commitment’s to significant fiscal stimulus is seen fueling economic growth. The German index has become so popular among investors that it’s now relatively expensive, trading at the highest premium against its European peers since 2009. Shares are rising in London in early trading as well. The FTSE 100 index of blue-chip shares has gained 32 points, or 0.4%, to 8564 points. Retailer JD Sports, whose US operations are vulnerable to US tariffs on goods made in China, are up 2%, among the top risers. Officials from the US and China are due to hold talks in Switzerland this weekend, which may be the first step toward resolving their trade war. The US-UK trade deal has also lifted sentiment in the City, reports Derren Nathan, head of equity research at Hargreaves Lansdown: “The diplomatic offensive presented conjointly by President Trump and Keir Starmer from Washington and Solihull has ignited a feint spark of optimism in equity markets. The coincidence with VE day commemorations seemed designed to underline the special relationship between the two allies. With details emerging late in the day it wasn’t enough to prevent a down day on the FTSE [yesterday] but sentiment has picked up this morning. There may be some disappointment that the baseline 10% tariffs remain in place but for certain industries the picture on trade restrictions are looking up. While pharmaceuticals have escaped the US Presidents wrath for now, UK companies in the sector and other knowledge-intensive areas have been promised preferential treatment. As yet, that’s not come at the expense of lifting the 2% Digital Services Tax Britain applied to the likes of YouTube and eBay, but with more talks to come on a separate digital services deal, it’s likely to form part of negotiations. European stock markets have opened higher, amid hopes of progress in the US trade wars. Germany’s DAX has jumped by 0.6% at the start of trading, with France’s CAC up 0.5%, with suggestions that the US-UK trade deal is a sign that other countries will be able to reach agreement with Washington too. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, says news of yesterday’s US-UK deal resonated positively across global financial markets – even though Trump hasn’t lifted his baseline 10% tariff on UK goods. Ozkardeskaya explains: Not only do we have a new pope this week, but we also have the first deal in Trump’s global trade war - between the UK and the US. Trump’s enthusiastic announcement, complete with a lot of CAPITAL LETTERS, helped inflate sentiment, making this US-UK deal feel bigger than it actually is. I mean, the fact that the two countries could agree on a few points is a good start, but the UK entered the negotiations with a tariff rate of 10% and left the table with... a tariff rate of 10%. Sure, the tariffs on cars were pulled lower from 27.5% to 10% — leading to an almost 14% jump in Aston Martin. Rolls Royce’s plane engines are exempt from tariffs in exchange for a pledge from British Airways to buy $10bn worth of Boeing planes — Rolls Royce jumped by more than 3.5%. The tariff on UK steel will be cut to zero, while British farmers will benefit from tariff-free quotas — just like their US counterparts. The two countries also agreed to keep working on a digital agreement. But again, the 10% tariffs remain. So yes, it’s a deal — but is it a big deal? One person at Axios even said that the UK was the “low-hanging fruit of trade deals” and that negotiations won’t be as simple with others. We’ll see. Yesterday, Donald Trump teased us by revealing that an unnamed UK company had bought $10bn of planes from Boeing. And this morning, British Airways’ parent company has revealed itself as the buyer. International Airlines Group (IAG) stated, in its latest financial results, that it has ordered 53 aircraft for its medium-term long-haul fleet requirements. The Group has ordered 21 Airbus A330-900neo aircraft and 32 Boeing 787-10 aircraft for delivery from 2028 to 2033. The aircraft are mainly for replacement, with around one third for growth in IAG’s core markets. Reports that the US will have a veto over Chinese investment in Britain as a result of the UK-US trade deal are “complete nonsense”, Treasury minister Darren Jones has insisted this morning. The Telegraph reported that such a veto is part the deal, but Treasury minister Mr Jones told Times Radio: “This story on the front page of the Telegraph is complete nonsense. I mean, I’m at a bit of a loss as to know where it’s come from. I think it was a Conservative Party criticism. “But as you said, we’ve not even published all of the documents yet, so I’m not quite sure how they were able to come up with that. “I can be completely categorical with you there is no such thing as a veto on Chinese investment in this trade deal, this is not what this trade deal is about. “It is a sectoral trade deal in relation to tariffs in key sectors, in the way that we’ve just been talking about. So I’d suggest the Conservative Party reads the documents and they maybe come back for a second go.” Our First Edition newsletter has kicked the tires on the US-UK trade deal, showing that it is far from comprehensive, but will help crucial British industries such as car-making. The broader economic impact may be limited, though. As our economics editor Heather Stewart put it: “It’s very important to have this piece of good news to take to the public and now that the Bank of England has cut interest rates they’re going to have positive headlines about people’s mortgages going down and this deal being done and that will help boost consumer and business confidence, But in terms of the broader economic impact this deal is really quite small.” The Governor of the Bank of England has called for Britain to “rebuild” its trade relationship with the European Union, as the UK celebrates yesterday’s trade deal with the US. Andrew Bailey has told the BBC that reversing the post Brexit hit to UK-EU trade would be “beneficial”. And while Bailey was keen not to take a view on Brexit, as a public official, he also argued that a closer relationship between the UK and the EU would help the economy and inflation. Bailey says: “It would be beneficial. Having a more open economy to trade with the European Union. Because there has been a fall-off in goods trade with the EU over recent years. “It is important we do everything we can to ensure that whatever decisions are taken on the Brexit front do not damage the long-term trade position. So I hope that we can use this to start to rebuild that relationship. That relationship could be improved later this month, when a crucial EU-UK summit is held. As we covered in yesterday’s blog, Bailey was also pleased that the US and UK had reached a trade deal, telling the Beeb: “It demonstrates that trade deals are important. Trade deals can be done, and the trade is important…honestly, it seems an unpromising landscape at times. But I hope that we can use these deals to rebuild the world trading system.” But while Donald Trump hailed that agreement yesterday, it still leaves the UK facing 10% tariffs on shipments to the US. Good morning, and welcome to our rolling coverage of business, the financial markets, and the world economy. Trade between the US and China cooled sharply last month, new data shows, as Donald Trump’s tariff war hit demand. The latest trade data from China shows that shipments to the US fell 21%, year-on-year, in April. That indicates the tariffs imposed on China by Trump, which rose to 145% during April, hurt trade. Shipments the other way fell too. China’s imports from the US fell by almost 14%, after Beijing’s tit-for-tat tariffing raised its tariffs on US goods to 125%. But… the broader picture is that China’s overall exports jumped by 8.1% in April, year-on-year, beating forecasts for a 1.9% rise, while imports dipped by 0.2%. Economists have suggested that countries around the world are scrambling to take advantage of Donald Trump’s 90-day pause to the tariffs he announced at the start of April (not including China, though). That is leading to stronger demand for China’s materials. Stephen Innes, managing partner at SPI Asset Management, says: The numbers just confirmed what markets already suspected: Trump’s tariff blitz is biting, and hard. Chinese exports to the U.S. cratered 21% in April, the sharpest drop in years, while exports to ASEAN, Africa, LatAm, and even the EU surged. The global supply chain is being rerouted in real time. On the surface, China’s overall April export growth held up—rising 8.1% YoY. But strip out the spin, and it’s clear the headline resilience masks a fundamental shift. The U.S. is no longer China’s growth engine. The manufacturing juggernaut is diverting flow wherever the tariff pain isn’t. Vietnam, Indonesia, and Thailand—still in the 90-day reciprocal tariff grace period—saw double-digit percentage surges in China-bound exports. These aren’t one-off distortions. This is structural repositioning. The agenda 9.40am BST: Bank of England governor Andrew Bailey to give keynote address at the Reykjavik economic conference 2025 12.15pm BST: Bank of England chief economist Huw Pill gives the national Monetary Policy Committee agency briefing</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Top US officials are expected to meet a high-level Chinese delegation this weekend in Switzerland. It is the first significant talks between the two nations since Trump provoked a trade war with stiff tariffs on imports. The US president wrote “80% Tariff on China seems right! Up to Scott B’ on Friday morning.</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Time to recap… A 17-month period of expansion in the UK’s services sector came to an abrupt end in April as uncertainty created by Donald Trump’s tariff war hit new orders and exports. A poll of purchasing managers in services businesses showed that the US president’s tariff campaign had sent a chill through the sector, which accounts for about three-quarters of the UK economy, hitting business confidence about the prospects for the years ahead. Service sector export sales were particularly subdued, with total new work from abroad decreasing at the fastest pace since February 2021, during the Covid pandemic. Smaller domestic services companies also said tax increases introduced by the chancellor, Rachel Reeves, were weighing on costs and had led to them laying off workers at a faster rate in April. At 49.0 in April, down from 52.5 in March, the headline seasonally adjusted S&amp;amp;P Global UK services PMI activity index was the lowest since January 2023. A score of more than 50.0 represents expansion. In other news… The US trade deficit has widened to a record level in March, as American companies scrambled to import goods before new tariffs came into effect. Britain and India have agreed a long-desired trade deal that ministers said would add £4.8bn a year to the UK economy by 2040. The deal promises a boon for the UK’s car and alcohol industries, which have suffered from the impact of Donald Trump’s tariffs in the US. India’s tariffs on British whisky and gin will be halved from 150% to 75% before reducing to 40% by the 10th year of the deal, according to the business department. UK car sales have dropped 10% in April, a decline blamed on “a fragile economic backdrop and weakened consumer confidence. Ford, Mattel and Ferrari have all warned that tariffs will eat into their profits. The Irish government revised down its economic outlook as global trade uncertainty caused by US President Donald Trump’s tariff tirade threatens growth. Canada is likely to fall into recession this year due to the US trade war, ratings agency Fitch warned. The UK stock market’s longest running winning streak on record just got a little longer! The FTSE 100 index of blue-chip shares in London has ended the day up one point, or 0.07%, at 8597 points. That means the Footsie has now risen for 16 sessions in a row, extending the record set at the end of last week. Gold miners led the FTSE 100 risers today, with Endeavour Mining up 5,2% and Fresnillo gaining 4.7%, followed by supermarket chain Sainsbury’s (3.4%). This rally means the FTSE 100 has recovered all the losses it suffered in early April, when it plunged to just 7,544 points in the market panic after Donald Trump’s “Liberation Day” tariff announcement. The recovery began when the president u-turned, and delayed most tariffs for 90 days. Treasury Secretary Scott Bessent has said today that the U.S. is in the midst of negotiations with 17 of the country’s largest trading partners, Fox Business report. In testimony to the House Appropriations Subcommittee on Financial Services and General Government, Bessent explained that the timing of trade deals “will be path dependent on our trade partners.” He added: “As I’ve said before, there are 18 very important trading relationships. We are currently negotiating with 17 of those trading partners. China we have not engaged in negotiations with as of yet.” “Approximately 97% or 98% of our trade deficit is with 15 countries, 18% of the countries are major trading partners, and I would be surprised if we don’t have more than 80% or 90% of those wrapped up by the end of the year.” With around 40 minutes trading to go, it’s nip-and-tuck whether the London stock market will extend its record-breaking run. The FTSE 100, which has risen for the last 15 sessions, is curently down 2 points today at 8593 points. So shortly after 4.30pm today, after the closing auction, we’ll know if the rally has faltered… Back in Frankfurt, stocks are recovering after Friedrich Merz won a second vote to become the next German chancellor, a few hours after dramatically losing the first vote. The DAX is now down just 0.4%. The euro has pushed a little higher too – now up half a cent against the US dollar at $1.136. UK lender Nationwide has announced cuts to its mortgage deals – perhaps anticipating the Bank of England lowering borrowing costs on Thursday. Nationwide is trimming up to 0.3 percentage points off some mortgage products, which means rates now start at 3.84%. The cuts mean Nationwide is now offering sub-4% first-time buyer rates for first time since September 2024. It’s lowest first-time buyer rate is 3.94% and available on a two-year fixed rate product at 60% loan-to-value (LTV) with a £1,499 fee. Ireland is bracing for a growth slowdown if Donald Trump maintains tariffs on the European Union. Ireland’s finance ministry has issued new forecasts, showing that growth in Ireland’s domestic economy is expected to slow to 2% this year if a 10% tariff on U.S. imports from the European Union remains in place or 2.5% if tariffs are removed. Wall Street has opened in the red, with the main indices all lower in early trading. Dow Jones industrial average: down 273 points, or 0.66%, at 40,945 points S&amp;amp;P 500: down 39 points, or 0.7%, at 5,611 points Nasdaq composite: down 160 points, or 0.9%, at 17,684 points Ratings agency Fitch is predicting that the trade war with the US will push Canada into recession this year, and push up unemployment. In a new report today, Fitch warns that “due to the impact of U.S. tariffs, we forecast a recession” – a blow to new prime minister Mark Carney. Fitch predicts that Canadian GDP will declining for three-quarters, starting in April-June this year, with annual average growth in 2025 of just 0.1%. The agency adds: The rapidly changing tariff and trade landscape in the U.S. will both directly affect Canadian exports and also indirectly via slower U.S. GDP growth. This will have an adverse effect on the labour market; Fitch expects the unemployment rate to rise to over 8%. Britain has secured its biggest trade agreement since Brexit, by agreeing a free trade deal with India. Britain’s business department says the deal, just announced, is a “huge economic win” for the UK, and will cut Indian tariffs on key products such as whisky, cosmetics and medical devices. The deal is expected to increase bilateral trade by £25.5bn “in the long run” (which I think means by 2040). Business and Trade Secretary Jonathan Reynolds says: “By striking a new trade deal with the fastest-growing economy in the world, we are delivering billions for the UK economy and wages every year and unlocking growth in every corner of the country, from advanced manufacturing in the North East to whisky distilleries in Scotland. “In times of global uncertainty, a pragmatic approach to global trade that provides businesses and consumers with stability is more important than ever.” Under the deal, India’s tariffs on UK whisky and gins will be halved from 150% to 75% before reducing to 40% by year ten of the deal, while automotive tariffs will go from over 100% to 10% under a quota. Other UK goods with reduced tariffs include cosmetics, aerospace, lamb, medical devices, salmon, electrical machinery, soft drinks, chocolate, and biscuits. In return, the UK will cut tariffs on Indian producs including clothes, footwear, and food products including frozen prawns. India’s prime minister Narendra Modi has also hailed the deal, saying: “These landmark agreements will further deepen our comprehensive strategic partnership, and catalyse trade, investment, growth, job creation, and innovation in both our economies.” Just in: New data confirms that the US trade deficit rose to a record level in March. America’s total goods and services deficit increased by $17.3bn to $140.5bn in March, up from $123.2 billion in February, the US censud bureau reports. The increase was due to a 4.4% rise in imports in March, to $419bn, while US exports were only 0.2% higher at $278.5bn. The increase in imports may be due to companies trying to stock up before the White House imposed new tariffs on goods from abroad in April. The report shows that imports of consumer goods increased by $22.5bn, while capital goods imports rose by $3.7bn, computer accessories were up $2bn and automotive vehicles, parts, and engine shipments increased by $2.6bn. The report also shows that the US achieved budget surpluses with Netherlands ($4.5bn), South and Central America ($3.2bn), Hong Kong ($1.9bn), United Kingdom ($1.2bn), Singapore ($500m), Brazil ($500m), and Saudi Arabia ($200m). But beficits were recorded with the European Union ($48.3bn), Ireland ($29.3bn), China ($24.8bn), Mexico ($16.8bn), Switzerland ($14.7bn), Vietnam ($14.1bn), Taiwan ($8.7bn), India ($7.7bn), Germany ($7.5bn), South Korea ($6.8bn), Japan ($5.8bn), Canada ($4.9bn), Italy ($4.4bn), France ($3.9bn), Malaysia ($3.2bn), Australia ($1.0bn), Israel ($1.0bn), and Belgium ($100m). Luxury car maker Ferrari has joined the pack of auto companies warning that the US trade war could hurt its earnings. Ferrari reported a 13% rise in revenues in the first three months of this year, with operating profit up 23%. “Another year is off to a great start” said Benedetto Vigna, CEO of Ferrari, explaining: “In the first quarter of 2025, with very few incremental shipments year on year, all key metrics recorded double-digit growth, underscoring a strong profitability driven by our product mix and continued demand for personalizations. Vigna added that Ferrari is “very excited about what lies ahead.” But that roadmap includes the threat of tariffs – and Ferrari warns that the introduction of import tariffs on EU cars into the USA could knock 50 basis points (half a percentage point) off its profitability percentage margins this year. Ian Plummer, commercial director of online vehicle marketplace Auto Trader, said “short-term turbulence” is most likely to blame for April’s drop in new car sales (see earlier post for details). He added: “We’re seeing new car visits on Auto Trader up 8% on 2024 and we’re confident this will convert to sales in the coming months.” Dan Caesar, chief executive of lobby group Electric Vehicles UK, said: “Month after month at least one in five new car buyers are now going battery electric. “As the industry demonstrates that battery electric vehicles are the cheaper and better option, more and more end-users will opt for all-electric vehicles.” Sales of new light commercial vehicles (LCVs) also fell last month in the UK. Van registrations dropped by -14.9% in April, with 20,332 vans, 4x4s and pick-ups sold, according to the latest figures published today by the Society of Motor Manufacturers and Traders (SMMT). Shares in Ford are set to fall when trading begins in New York in just under two hour’s time. Ford’s stock is down almost 2.5% in premarket trading, after it withdrew its financial guidance last night and indicated tariffs could wipe $1.5bn off its profits this year. The EU has launched a market surveillance of Chinese imports into the bloc amid fears that the trade war with the US is diverting goods to Europe, my colleague Lisa O’Carroll reports. It comes amid reports that discount online retailers Shein and Temu have upped their marketing spend in Europe after Donald Trump’s tariffs were introduced on all packages up to $800 in value on Saturday. Trade commissioner Maros Sefcovic has again warned that the existing tariffs on the automotive and steel sectors along with the threat of tariffs in six other areas is “unacceptable”. Speaking at the European parliament on Tuesday he again urged the US to cut a deal describing the EU as “by far the most important economic partner of the US”. He said if Trump carries through his various threats of tariffs in addition to existing import duties on cars and steel, its import taxes would jump from €7bn in 2024 to €100bn. He said: “This situation is not acceptable and we cannot afford to stay idle.” If the US doesn’t cut a deal, Europe is prepared for retaliatory tariffs and litigation, he warned. In the meantime the EU has started monitoring potential diversion of trade from China to the US to Europe with the first results of the survey anticipated in mid-May. “The aim is to protect the EU market from possible surges of imports from other countries that are also hit by US tariffs and which seek alternative markets. The first results of this work are anticipated in mid-May,” he said. The decline in the UK private sector last month adds to the pressure on the Bank of England to ease monetary policy. The BoE is widely expected to cut interest rates at its next meeting, on Thursday. The money markets indicate there’s a 92% chance of a quarter-point cut to Bank rate, to 4.25%, and an 8% possibility of a larger, half-point cut to 4%. Daniela Sabin Hathorn, senior market analyst at Capital.com, sets the scene: The Bank of England (BoE) is widely expected to deliver a rate cut at its upcoming meeting, as policymakers balance weak domestic growth with the inflationary risks stemming from global trade tensions. At its March meeting, the Monetary Policy Committee (MPC) voted 8-1 to keep the Bank Rate at 4.5%, with only external member Swati Dhingra advocating for a 25-basis-point cut. At that time, persistently high inflation was a key factor in maintaining the current rate. Headline CPI had climbed back to 3% in January, and the BoE projects it could rise further to 3.75% by summer. Geopolitical uncertainty and renewed U.S. tariff threats have also prompted a cautious stance, even as domestic data shows lacklustre growth and hiring plans, while wage pressures in services remain elevated. Governor Andrew Bailey reiterated the need for prudence, noting that while easing is on the table, it must be guided by “accumulating evidence that price pressures are easing,” and emphasizing that there is “no presumption about cuts at the next few meetings. Thursday’s rate decision will be released at 12.02pm, incidentally, rather than bang on noon, due to the two-minute silence to mark VE Day. Moody’s Ratings has cut its global growth forecast to 1.9% in 2025 and 2.3% in 2026, driven by tariff uncertainty and trade tensions. Moody’s updated forecasts now predict: Reduced UK real GDP growth of 0.8% in 2025 and 1.3% in 2026. US real GDP growth to fall to 1% in 2025 and 1.5% in 2026, with inflation to hit 3% this year. China’s real GDP growth to slow to 3.8% in 2025 and 3.9% in 2026. In the Eurozone - Germany’s real GDP growth is expected to be 0% in 2025 and 1.4% in 2026, with slowdowns in France (0.5% in 2025 and 1.2% in 2026) and Italy (0.5% in 2025 and 0.6% in 2026). Back in the City, the early stock market gains have vanished. The FTSE 100 index is now down 17 points, or 0.2%, at 8597, threatening to end its record-breaking run of 15 daily rises in a row. The slide comes as European markets drop, led by Germany’s DAX which has fallen by 1.9% today. Frankfurt traders are alarmed that Friedrich Merz has failed to get enough votes to become chancellor in the first vote today in the Bundestag. That’s quite a shock, as Merz had been expected to be rubber-stamped to succeed Olaf Sholz today. His CDU/CSU/SPD coalition nominally has 328 votes in the Bundestag – but he got only 310, six short of the majority required to confirm him as the next chancellor. It has prompted the far-right Alternative für Deutschland party calls for fresh elections in Germany. Sales of Tesla cars tumbled by over 60% last month, amid a wider backlash against Elon Musk. Just 512 new Tesla models were registered in April, the latest sales data from trade body the SMMT shows, down from 1,352 in April 2024. Tesla’s market share shrank to 0.43% in April, down from 1% a year ago, as sales of battery electric vehicles (BEV) increased 8.1%. Tesla’s sales have also been dropping across Europe this year, with some customer shunning the brand following Musk’s tilt to the political right. But last month’s sales drop may also be due to model changes at Tesla. Deliveries of its latest Model Y, codenamed “Juniper”, were expected to begin in May, so customers may have been waiting for it to arrive. In February, Tesla’s Model 3 and Model Y cars were the second and third most popular in the UK after the Mini Cooper. But both failed to make the top 10 in April, with Kia’s Sportage topping the list: Worryingly, UK business expectations for the year ahead fell sharply last month. This morning’s PMI report shows that service sector firms are bracing for an extended period of global economic turbulence and heightened recession risks. Some 22% of the survey panel predict an outright decline in business activity during the next 12 months, up from 14% in March and well above the post-election low of 6% in July 2024. Tim Moore, Economics Director at S&amp;amp;P Global Market Intelligence, says: “UK service sector output slipped into contraction for the first time in one-and-a-half years as heightened business uncertainty weighed on order books during April. Export conditions were particularly weak, with new business from abroad falling to the greatest extent since February 2021. Survey respondents often commented on the impact of global financial market turbulence in the wake of US tariff announcements. Businesses in the technology and financial service sectors noted rising risk aversion and delayed spending decisions among clients, especially in relation to major investment plans. Consumer service providers meanwhile cited subdued domestic economic conditions and challenges with passing on rising payroll costs, especially those in the hospitality and leisure sectors. Newsflash: Business activity across the UK has fallen for the first time in 18 months, as trade war fears batter the British economy. The latest poll of purchasing managers at UK service sector companies has found that business activity declined in April, ending a 17-month run of growth, and pulling the wider private sector into a contraction. New order books at services companies shrank last month, driven by the fastest decline in exports since February 2021, when the Covid-19 pandemic was hitting activity. Data provider S&amp;amp;P Global says that “survey respondents widely commented on risk aversion and delayed spending decisions among clients in response to rising global economic uncertainty.” This dragged the S&amp;amp;P Global UK Services PMI Business Activity Index down to 49.0 in April, down from 52.5 in March, which is the lowest reading since January 2023. Any reading below 50 signals a contraction. The PMI report says: While many firms continued to report unfavourable domestic demand conditions, the latest survey indicated a particularly marked decline in new work from overseas markets. The rate of contraction was the steepest for just over four years and mostly linked by survey respondents to the impact of rising global trade tensions. S&amp;amp;P Global also reports that the wider UK private sector also contracted last month. Its UK PMI Composite Output Index, which also tracks the manufacturing industry, fell to 48.5 in April, down from 51.5 in March and below the 50.0 no-change value for the first time in one-and-a-half years. Car sales across the UK fell by over 10% last month, compared to a year ago. New industry data shows that 120,331 new vehicles were registered in April, 10.4% fewer than in April 2024. The Society of Motor Manufacturers and Traders (SMMT) attributes “a fragile economic backdrop and weakened consumer confidence” for the sixth fall in the last seven months. The SMMT also blames increases in Vehicle Excise Duty (VED) which began at the start of April – and which let to a jump in sales during March. It says: In what is traditionally a quieter month following the March plate change, volumes were also impacted by the late timing of Easter, resulting in fewer working days. In addition, the implementation of VED changes affecting all new cars, including the Expensive Car Supplement which became applicable to many new EVs from 1 April, pushed transactions into March as shrewd buyers got ahead of the tax increases. The drop in sales last month was broad-based, with private sales down 7.9% and purchases by businesses dropping by around 11%. Battery electric vehicle sales jumped by 8.1% to 24,558 units, with a market share of 20.4%. Sales of plug-in hybrids (PHEV) jumped by 34.1%. But sales of hybrid electric vehicles (HEVs) fell -2.9%, with petrol sales down 22% and diesel plunging by 26.2%. Just in: growth across the eurozone private sector slowed last month. The HCOB Eurozone composite PMI output index, which tracks activity across the euro area, has dropped to 50.4 for April, down from 50.9 in March, showing a weaker expansion in business activity. The PMI index, based on data from purchasing managers at European firms, found that new orders fell last month, again, as demand weakened. France’s private sector contracted for the eighth month running, while Germany’s private sector output barely rose in April. Ireland recorded the strongest increase in activity, while Spain and Italy also expanded. Dr. Cyrus de la Rubia, chief economist at Hamburg Commercial Bank, says: “Eurozone economic growth slowed at the start of the second quarter, following a pick-up in the first three months of the year. The services sector, which is a major player, practically stagnated in April. Even though manufacturing output saw a surprising uptick, it wasn’t enough to prevent the overall slowdown in growth. In the services sector, cost pressures are still relatively high, though they have eased a bit over the past couple of months. Inflation is down for sales prices and continued to trend lower. Many members of the European Central Bank (ECB) have been hinting at another interest rate cut in June, and these latest figures seem to support their stance. Associated British Foods has confirmed it is in talks with the parent company of Hovis about selling its Allied Bakeries business. ABF’s shares have risen by 1% after telling the City “it is in discussions with Endless LLP regarding a potential transaction” for Allied Bakeries, whose brands include Kingsmill, Allinson’s and Sunblest. ABF told shareholders: Allied Bakeries continues to face a very challenging market. We are evaluating strategic options for Allied Bakeries against this backdrop and we remain committed to increasing long-term shareholder value. A further announcement will be made as and when appropriate. ABF, which also owns Primark, reported last week that sales at Allied Bakeries fell in the 24 weeks to 1 March. Britain’s blue-chip share index is on track to extend its record-breaking run of gains. The FTSE 100 share index has risen by 27 points, or 0.3%, in early trading, partly thanks to BP’s rally. The ‘Footsie’ has already risen for the last 15 sessions in a row, the longest run of gains since it was created in the 1980s. It has now recovered all its losses since 2 April, when Donald Trump announced a swathe of tariffs on trading partners: Richard Hunter, head of markets at interactive investor, explains why the FTSE 100 has been gaining ground in recent weeks: The FTSE100 remains something of a beacon of light compared to many of its global peers, with its suite of relatively stable and defensive sectors playing into investors’ desire for alternative investment destinations. Coupled with an undemanding valuation both historically and globally, alongside an average dividend yield of 3.5%, the index has added 5.6% this year, and at the open further resilience was in evidence. A broad mark up incorporated both defensive and cyclical sectors, the latter of which resulted in some strength in the likes of the retailers and the housebuilders.” Shares in energy giant BP have jumped by 3.3%, following reports that rival Shell has considered a takeover bid. BP’s shares rose to 361p at the start of trading, a one-week high, making it the top riser on the FTSE 100 share index. Shell’s shares are down 0.7%. City traders are responding to Bloomberg’s report last weekend that Shell has been discussing the feasibility and merits of a takeover of BP with its advisers in recent weeks. My colleague Lauren Almeida reported: If this were to happen, it would mark one of the biggest deals ever in the oil and gas industry. Speculation about a possible takeover comes as BP’s shares have suffered this year. They have fallen by more than 30% in the past 12 months as a turnaround plan under the chief executive, Murray Auchincloss, has failed to inspire investors and oil prices have fallen. Bloomberg also reported that Shell could decide to focus on share buybacks and bolt-on acquisitions rather than a megamerger, and that other large energy companies have also been analyzing whether they would want to bid for BP. The takeover of UK food-delivery platform Deliveroo by US rival DoorDash has been agreed. The two sides have reached agreement on DoorDash’s offer of 180p in case for each Deliveroo share, made last month. The deal values Deliveroo at £2.9bn, and is almost 30% higher than Deliveroo’s share price the day before the offer was made. It’s less than half the value at which Deliveroo was floated on the London stock market four years ago, though. Tony Xu, CEO and co-founder of DoorDash, says he has “long admired” Deliveroo’s team, including CEO Will Shu (who will pocket around £170m from the shares he owns): Like DoorDash, Deliveroo is obsessively focused on their customers - consumers, merchants, and riders. They work day in and day out to improve their consumer value proposition, bring new services to local businesses, and offer flexibility and support to riders. These efforts and attention to detail from Will and the team have had a tremendous positive impact in the communities where Deliveroo operates. American children face paying higher prices for Barbie dolls due to the Trump tariffs on imports. Mattel, the toy manufacturing giant, revealed last night that it plan to raise prices on American toys due to tariffs, and is also looking to move some manufacturing out of China. In its latest earning report, Mattel told shareholders it is taking “mitigating actions” to fully offset the potential incremental cost impact of tariffs on future performance. Those measures include: Accelerating diversification of its supply chain and further reducing reliance on China-sourced product, Optimizing product sourcing and product mix, and Where necessary, taking pricing action in its U.S. business. Chief financial officer Anthony DiSilvestro explained: Given the evolving tariff situation, we are taking mitigating actions designed to fully offset the potential incremental cost impact. Paying more for a new Barbie, or Ken, might highlight the impact of tariffs for US consumers. Donald Trump, though, argued last weekend that “a young lady” doesn’t need 37 dolls, and might be “very happy with two or three or four or five.”.. Dutch medical-technology firm Philips has lowered its outlook for profitability this financial year, blaming the US trade war. In its latest financial results, Philips trimmed its profitability outlook for the year, as it calculated “the assumed impact of currently announced tariffs”. Philips now expects an estimated net tariff impact of €250m to €300m “after substantial tariff mitigations”, and has lowered its forecast for its adjusted operating earnings margin by one percentage point, to 10.8% to 11.3%. Roy Jakobs, CEO of Royal Philips, explains: In an uncertain macro environment that has intensified due to the potential impact of tariffs, we are focused on what we can control. We are improving our supply chain agility, taking decisive cost actions to mitigate financial impact where possible, and ensuring we can continue to serve our customers and consumers. Philips makes medical devices such as MRI and CT scanners, and has been using artificial intelligence (AI) to speed up results: America’s car industry is calculating the cost of the trade wars. Overnight, Ford Motor suspended its annual guidance, due to “tariff-related uncertainty”, and estimated new tariffs would cost it about $1.5bn (£1.1bn) of profits this financial year. Ford CEO Jim Farley told analysts: “It’s still too early to fully understand our competitors’ responses to these tariffs,” “It’s clear, however, that in this new environment, automakers with the largest U.S. footprint will have a big advantage.” Last week, Donald Trump’s 25% import tax on engines, transmissions and other key car parts came into force, a move that will push up costs for automakers. Ford had previously predicted it would post earnings before interest and taxes of between $7bn and $8.5bn this financial year. But with uncertainty over how the trade war will play out, Ford told investors that guidance was now suspended, explaining: Given material near-term risks, especially the potential for industrywide supply chain disruption impacting production, the potential for future or increased tariffs in the U.S., changes in the implementation of tariffs including tariff offsets, retaliatory tariffs and other restrictions by other governments and the potential related market impacts, and finally policy uncertainties associated with tax and emissions policy, the company is suspending guidance. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Investors will be scrutinising the latest healthchecks on companies across the world today, for signs that the US-China trade war is hurting the global economy. And… the latest purchasing manager’s survey data has shown that China’s service sector activity growth has hit a seven-month low, as business confidence fell to the lowest since early in the Covid-19 pandemic. The Caixin China General Services Business Activity Index, released this morning, fell to 50.7 in April, down from 51.9 in March. That shows the slowest rise in activity since last September – but still above the 50-point mark that signals stagnation. China’s service sector firms reported a slowdown in new business, while business sentiment fell to the lowest level seen since February 2020, while companies continued to cut staffing levels. The report says: The slowdown in business activity growth reflected the trend seen for new business. Disruptions to goods trade amid fresh tariffs had negatively impacted some service providers in April, according to anecdotal evidence, and led to the slowest rise in overall new work for 28 months. New export business increased only fractionally, with some firms noting improved foreign demand amid rising tourism activity. Data yesterday showed that the US services sector’s growth picked up in April, while the prices paid by American firms for materials and services jumped, indicating that the tariffs announced by the Trump administration are fuelling inflation. The financial markets are looking for progress in trade talks between the US and its trading partners. Yesterday, treasury secretary Scott Bessent told CNBC that he believes the U.S. is “very close to some deals.” Bessent explained: “As President Trump said last night on Air Force One, maybe as early as this week.” He added that there could be “substantial progress in the coming weeks” with China; last week, Beijing signalled it was “assessing” potential trade talks with the U.S…. The agenda 9am BST: UK car sales data for April 9am BST: Eurozone services sector PMI report for April 9.30am BST: UK services sector PMI report for April 3.10pm BST: US RCM/TIPP Economic Optimism Index</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>US trade deficit widens to a record level in March as companies scramble to import goods before new tariffs came into effect. Britain and India have agreed a long-desired trade deal that ministers said would add £4.8bn a year to the UK economy by 2040. UK car sales have dropped 10% in April, a decline blamed on “a fragile economic backdrop and weakened consumer confidence”</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>You say you want a revolution, sang the Beatles back in 1968. And that seems to be the interpretation of electoral results across the industrialised world. From the seismic shifts in recent US and German elections to the rise of Reform and the Green party in the UK, electorates are signalling that they reject the status quo. As the song says: “We all wanna change the world.” And yet, there is an important caveat in the next few lines of the lyrics penned by Lennon and McCartney that are just as important almost 60 years later. “But when you talk about destruction, don’t you know that you can count me out.” As private wealth has accumulated since the 1950s, only the radical few have been prepared to see jobs disappear and their wealth diminished while they wait for the supposed benefits of political and economic upheaval. And no amount of pleading from leaders to wait for the good times will overcome that resistance. For several years now we have witnessed the call for revolution from those who consider themselves insulated from its effects, until that is, the level of destruction they voted for takes a toll on their own finances. That was the case with Brexit, and buyer’s remorse is now widespread. While it takes time for people to react, financial markets have become more sensitive. Over the past month we have seen the custodians of global wealth – fund managers and pension funds – react with almost palpable anger to Donald Trump’s attempts at revolution, just as they did when former prime minister Liz Truss embarked on a borrowing spree to revolutionise the UK’s economy. Andy Haldane, the former chief economist of the Bank of England and outgoing boss of the Royal Society for the Encouragement of Arts, Manufactures and Commerce (RSA), says financial markets have become a bulwark against leaders’ excesses. Writing in the Financial Times, he said the interconnectivity of world trade and the costs of tearing up supply chains sparked fears of a return to high inflation, spooking investors. “The excess sensitivity of financial markets [applies] a double-lock. By telescoping and amplifying these costs, they serve as a real-time disciplining device on politicians claiming they can weather the short-term pain. This makes capitulation speedier than in the past.” Last month the US president vented his anger at financial markets, accusing them of undermining his economic project with panic selling. Coining a new term, he said on his Truth Social platform: “Don’t be a PANICAN (A new party based on Weak and Stupid people!).” Haldane is not the only one to say that the loss of more than $6tn from global stock markets by the end of April, which wreaked pain on ordinary savers and undermined consumer confidence, helped halt the tariff scourge. As a senior fellow at the free-market American Enterprise Institute (AEI), Desmond Lachman analyses the subject from a different perspective, but comes to the same conclusion. He said US consumers will be next to put a block on Trump’s intentions. Despite his feisty rhetoric, Trump understands that he has less room for manoeuvre than he wanted. And his U-turns have had their reward. The stock market recovery this week is built on US officials saying they have approached Xi Jinping for talks over escalating tariffs. That humiliating climbdown comes after Trump’s claims that China had much more to lose from tariffs than the US. A resumption of Washington’s support for Ukraine’s war effort, after a deal to share the badly battered nation’s mineral wealth, has also calmed markets. Lower tariffs between the world’s two largest economies and a reassertion of the old international order, one that maintains Russian aggression breached international law, is good for business. Sensible policies have reasserted themselves and we have the markets to thank for that. Yet, while it might seem like a good outcome for those who gained from the old system, those who consider themselves losers are left with a festering anger. Politically, they might not achieve an electoral majority. Too many middle income households will support the old ways because that is what delivered them housing and pension assets they could only dream of 60 years ago. The poorer half of the income distribution – those who have seen their low incomes flatline for almost two decades – might still have some power, especially if they opt for social unrest. Lennon and McCartney wouldn’t have been surprised. They were writing the White Album while the 1968 student riots raged across Europe. Young people are one of the biggest losers from the 21st century economic lottery. They are voting green in the south and east and reform in the west and north in ever-greater numbers. What will they do when voting gets them nowhere?</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>From the seismic shifts in recent US and German elections to the rise of Reform and the Green party in the UK, electorates are signalling that they reject the status quo. As private wealth has accumulated since the 1950s, only the radical few have been prepared to see jobs disappear and their wealth diminished while they wait for the supposed benefits of political and economic upheaval.</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Time to recap. Amazon has denied that it planned to show the cost of new US tariffs on products on sale on its website, after being heavily criticised by the White House. An Amazon spokesperson has insisted that it never considered listing tariffs on its main retail site and nothing was implemented on any company site, saying: “The team that runs our ultra low cost Amazon Haul store considered the idea of listing import charges on certain products. This was never approved and (is) not going to happen.” Amazon commented after White House press secretary Karoline Leavitt claimed the plan to disclose tariff costs was “a hostile and political act by Amazon,” and “Another reason why Americans should buy American”. Leavitt responded to a question from the media about a report on Punchbowl News that claimed Amazon will soon display how much of an item’s cost is derived from tariffs. That report prompted president Trump to phone Jeff Bezos, Amazon’s founder, to complain, CNN reports. She was speaking at a press briefing today, where Treasury Secretary Scott Bessent warned that China risks losing millions of jobs unless it agrees a deal to cut tariffs soon. Bessent told reporters: “I think that over time we will see that the Chinese tariffs are unsustainable for China. I’ve seen some very large numbers over the past few days that show if these numbers stay on, Chinese could lose 10 million jobs very quickly. And even if there is a drop in the tariffs that they could lose 5 million jobs.” Bessent also said that negotations with India, South Korea and Japan are progressing well. But we’ve seen more signs today of the economic harm caused by Donald Trump’s trade war: The US trade in goods deficit has widened Firms have cut back on job vacancies US consumer confidence has hit a five-year low Companies have also been reporting the impact of new tariffs: HSBC raised its provisions for bad debts Adidas warned that the price of its goods in the US will rise UPS didn’t issue new financial guidance GM postponed a conference call with top management and investors until Thursday Electrolux cut its forecast for the US market this year Economics professor Justin Wolfers suggests, tongue-in-cheek, that the White House should show Amazon some gratitude! Here’s a video clip of White House press secretary Karoline Leavitt laying into Amazon: Back in London, the stock market has recorded its longest run of gains in over eight years. The FTSE 100 index of blue-chip shares rose by 46 points, or 0.55% today, to end at 84,63 points, its highest close in three weeks. This means the Footsie has now risen for 12 days in a row, beating the 11-day winning streak in December 2019 (when there was a rally after Boris Johnson’s Conservative Party won the general election). It’s the longest run since January 2017, when the FTSE 100 managed a 14-day run of gains. HOWEVER, this still leaves the Footsie down 1.3% in April – it hasn’t quite recovered all its losses earlier this month, when the trade war exploded. CNN’s White House reporter, Alayna Treene, has learned that president Trump phoned Jeff Bezos to complain that Amazon reportedly planned to show the cost of US tariffs on its site. That call was made shortly after Trump was made aware of the story on Punchbowl – and before Amazon insisted the plan was never considered for its main site. Amazon are insisting that while its Amazon Haul team considered the idea of listing import charges on certain products, this was “never approved and not going to happen.” A company spokesperson says: “The team that runs our ultra low cost Amazon Haul store considered the idea of listing import charges on certain products. This was never approved and is not going to happen.” Investors Observer has calculated that California is the state most exposed to the US-China trade war. California importing almost $123 billion worth of goods from China in 2024 – almost triple the amount imported by the next state, and 25% of imports to the state. It’s followed by Illinois, Texas and Tennessee. Meanwhile in Scotland, trade union leaders have accused the Scottish and UK governments of betraying thousands of oil and supply chain workers after PetroIneos announced on Tuesday that production at Scotland’s only oil refinery had ended. PetroIneos, jointly only by Jim Ratcliffe’s Ineos and PetroChina, announced late last year it was phasing out oil refining at Grangemouth, arguing the aged refinery, the oldest of six across the UK, was haemorrhaging money and no longer viable. It said the first phase of more than 400 direct job losses would take effect on 30 April, but the announcement that refining had totally ended on Tuesday morning surprised unions meeting in Dundee for the Scottish TUC’s annual congress. Roz Foyer, the STUC’s general secretary, told delegates the closure was symbolic of the failure by the UK’s governments to protect workers and the wider economy from the transition to a low carbon economy. She said John Swinney, Scotland’s first minister, and Anas Sarwar, the Scottish Labour leader, both of whom addressed this year’s congress, were full of “warm words and platitudes” yet seemed powerless. “The failure to keep the refinery open is an inexcusable and unforgiveable failure [that] cannot be ignored,” she said, to applause from delegates. PetroIneos has spent £50m on an expanded fuel terminal, importing petrol and diesel from other refineries, protecting around 70 jobs. Even so, the union Unite fears that around 2,822 jobs in the wider supply chain and amongst local businesses will be affected by the refinery’s closure. Scottish union leaders are angry that UK ministers intervened to stop British Steel’s Scunthorpe steel furnaces from being shut down, but failed to nationalise Grangemouth. Chris Hamilton, the Unite convenor at Grangemouth oil refinery, who was at the congress, said they knew refinery production would end around now. “It doesn’t make today any less devastating and any less emotional, because ultimately, what we’ve campaigned for for the last 18 months was to continue operations at the refinery, to then invest and then transition to future stuff. “18 months ago, when this announcement was first made, it certainly wasn’t inevitable. Look what’s happened at Scunthorpe: the closure of that site clearly wasn’t inevitable. So for us, if there was a will, there’d be a way. But ultimately for Grangemouth it looks like there’s not been a will, and therefore there has not been a way. And today Scotland loses its last refinery.” Global commodity prices are set to fall by 12% this year and continue declining in 2026, putting pressure on the finances of many developing countries, the World Bank warns today. The Bank’s experts expect the slowdown in global growth resulting from escalating trade tensions, to outweigh the inflationary impact of the tariffs. Oil prices are expected to drop particularly sharply, as the Opec+ producers’ cartel keeps output high in a bid to maintain market share. The Bank is predicting an average Brent Crude oil price of $64 a barrel for 2025 - down from the $73 it was predicting before the tariffs were introduced. The report’s authors point out that the downturn, induced by US policy, is only the latest shock to hit commodity markets in what they call, “a remarkably turbulent decade so far”. The Bank’s deputy chief economist, Ayhan Kose, warned that with many emerging economies already in debt distress, plunging commodity prices are likely to make life harder for those that depend heavily on exports. He said: “These countries already went through a series of shocks over the last five years. So in terms of having fiscal space, they are not in in a good shape.” The report also warns of what it calls, “marked downside risks to the outlook for global economic growth amid rising trade tensions, and therefore also to commodity demand”. To quantify these risks, the World Bank’s economists take the gloomiest 10% of growth forecasts from other experts. If things get this bad, it reckons, the Brent Crude oil price would drop another 7%, to $59 a barrel. Another economic blow today – Americans’ confidence in the economy slumped for the fifth straight month to the lowest level in five years. The Conference Board’s consumer confidence index fell 7.9 points in April to 86, its lowest reading since May 2020, early in the Covid-19 pandemic. Worryingly, the survey’s Expectations Index – which measures consumers’ short-term economic outlook – dropped to the lowest level since October 2011, to levels that usually signals a recession ahead. Amazon’s share price has recovered most of its early losses, after it denied planning to disclose the cost of tariffs on the goods it sells on its main site. Amazon’s stock is now down just 0.5% today – they were initially down 2.2% in premarket trading after the White House let rip. Back in the US economy, there are more worrying signs that America’s labor market may be weakening. The total number of job openings at US companies dropped last month to 7.192m, according to the latest JOLTS report, down from 7.48m in February, and almost 8.1m in March 2024. That suggests a slowdown in hiring in March, a month in which Donald Trump imposed tariffs on China, Canada and Mexico. You can read the original report that sparked the White House’s ire here, on Punchbowl News. It claimed: Amazon doesn’t want to shoulder the blame for the cost of President Donald Trump’s trade war. So the e-commerce giant will soon show how much Trump’s tariffs are adding to the price of each product, according to a person familiar with the plan. Heads-up: Amazon is denying that it planned to display tariff costs on its main website, reports Jeff Stein of The Washington Post. The retailer is saying that its Amazon Haul store, which sells low-cost items had considered listing import charges on “certain products”. “Nothing has been implemented on any Amazon properties,” the company added, shortly after the White House accused it of a ‘hostile and political’ act (see earlier post). It’s not hard to understand why the White House is cross with Amazon. Donald Trump has repeatedly claimed that the tariffs he imposes on imports are paid by other countries, despite economists pointing out that actually US businesses – and ultimately consumers – stump up the money when goods arrive. If consumers are seeing a ‘tariff cost’ on their Amazon orders, they might realise how the system works. Gavin Baker, CIO of investment firm Atreides Management, suggests other companies may adopt the same plan too: The White House’s attack on Amazon is a “significant” move which could alarm the financial markets, says Kathleen Brooks, research director at XTB. She writes that it’s a sign that the US administration is targeting comapnies who disagree with them – that means an increase in political risk. Brooks explains: The US administration has changed its tone towards tariffs yet again on Tuesday. The White House Press secretary and the Treasury Secretary accused Amazon of a ‘hostile political act’, after Amazon planned to expose the cost of tariffs to its consumers. This comes days before Amazon reports earnings on Thursday, and its stock price fell ahead of the US open and is down more than 2% so far. The US administration has mostly saved its ire for other countries that it believes gives the US a raw deal in global trade. Now it appears that the US administration is targeting US companies who question the logic of its moves. This is significant. Financial markets have been roiled by political interference in the global economy in recent weeks. Investors do not digest political risks well, so if the Trump administration is now publicly accusing US companies of hostile acts if they disagree with the President’s US economic policy then this could stop the recent recovery rally in risky assets. Political analyst Ian Bremmer isn’t convinced by the White House’s argument against Amazon. He suggests telling a customer the cost of tariffs on their goods is no different than flagging the sales tax on a receipt: Blimey. The surge of imports into the US last month are a sign that America’s economy probably contracted at the start of this year, consultancy Capital Economics suggest. Paul Ashworth, their chief North America economist, explains: The advance economic indicators revealed a massive surge in consumer goods imports in March, as firms raced to beat the imposition of reciprocal tariffs in early April. As a result, we now estimate that Q1 GDP contracted at a 2.0% annualised pace, down from our most recent estimate of a 0.1% gain. We’re expecting the first estimate of US GDP for the last quarter to be released tomorrow….. Shares in Amazon have dropped 1.3% at the start of trading, after the White House accused it of a ‘hostile’ act for showing consumers the cost of tariffs…. The Trump White House is furious with Amazon over reports that it plans to display the cost of tariffs on items it sells. Press secretary Karoline Leavitt has just given the company both barrels, at her briefing with the media today. Leavitt claims the move is “a hostile and political act by Amazon”, and asks why Amazon didn’t take a similar step when inflation hit 40-year highs under the Biden administration. She also adds that it’s “not a surprise”, citing a report (from 2021) that Amazon partnered with a Chinese propaganda arm. Leavitt argues: So this is another reason why Americans should buy American. It’s another reason why we are onshoring critical supply chains here at home, to shore up our own critical supply chain and boost our own manufacturing. Q: Is Jeff Bezos still a Trump supporter? Leavitt declines to comment on the president’s relationships with Jeff Bezos, but reiterates that “this is certainly a hostile and political action by Amazon”. America’s Asian trading partners and allies have been “the most forthcoming” in terms of doing trade deals, Treasury secretary Scott Bessent says. He adds that vice-president Vance made some very good progress during his trip to India last week, and that the contours of a deal with South Korea are coming together. Bessent then gives some “inside baseball” know-how in India, saying they are easier to negotiate with than many other countries because they have many very high tariffs. So it’s much easier to confront the direct tariffs…than the non-tariff trade barriers which can be much more insidious and also harder to detect. So a country like India, which has the posted and ready tariffs, it’s much easier to negotiate with them. So I think the India negotiations are moving well. In what may prove a hostage to fortune, Treasury secretary Scott Bessent says he doesn’t expect supply chain shocks due to the slowdown in shipments from China. Bessent says retailers have managed their inventory in front of this, explaining to the press pack: I speak to dozens of companies, sometimes daily, but definitely weekly. They know that President Trump is committed to fair trade and have planned accordingly. Scott Bessent is then asked why Donald Trump has decided to cushion the impact of his tariffs on US carmakers by easing some duties on foreign vehicle parts. The Treasury Secretary explains that Trump is committed to bringing back auto production to the US, so his administration wants to give automakers a path to do that “quickly, efficiently and create as many jobs as possible”. Over at the White House, Treasury secretary Scott Bessent is facing the press, and taking questions about the trade war. Quizzed about the situation with Beijing, Bessent argues that the Chinese tariffs are “unsustainable for China”, and could cost million of jobs very quickly [he may be citing a Goldman Sachs prediction that 16 million jobs are at risk]. Bessent says: Remember that we are the deficit country. They [China] sell almost five times more goods to us than we sell to them. So the onus will be on them to the take off these tariffs. They’re unsustainable for them. Bessent is also asked who the Trump administration is talking to Beijing specifically about tariffs, but he says he won’t talk about who’s talking to whom – joking that his role doesn’t include running the White House switchboard. Some snap reaction to the jump in the US trade deficit last month: Ouch! America’s trade in goods deficit has widened sharply last month, jumping by over 9%. The US trade deficit with the rest of the world rose to $162bn in March, up $14.1bn compared with February, when the deficit was $147.8bn. New data from the Census Bureau shows that US exports rose by $2.2bn to $180.8bn in March. But that was firmly outpaced by a surge in imports, which rose by $16.3bn during March to $342.7bn. That might indicate that US businesses and consumers raced to import goods last month before Donald Trump announced new tariffs on 2 April. In other trade war news, India is reportedly prepared to include a sweetener in trade talks with Washington that would “future-proof” a deal by ensuring no other trade partners could have superior terms. The “forward most-favoured-nation” clause, rarely granted by India in previous trade negotiations, would automatically apply to the U.S. any more-favourable tariff arrangements that might be agreed with other countries, two officials with direct knowledge of the matter told Reuters. One official explained: “This clause, in a sense, future-proofs the U.S. deal and is the only way to do so.” China has insisted that it will “never kneel down” in the trade war with the US, in a propaganda video that compares the US to “a small, stranded boat”. The video, released on social media today by Beijing’s foreign ministry, claims that China is standing up for the rest of the world against American “bullying”. The video suggests the current relative calm in the trade was is just “the eye of the storm”, declaring: Bowing to a bully is like drinking poison to quench thirst. It only deepens the crisis. The video then outlines how the US accused Japan of dumping semiconductors, forced Toykoto sign the Plaza Accord (to weaken the dollar against the yen), and forced the break-up of France’s Alstom. Pitching China bravely carrying a torch against US imperialism, the video says: History has proven compromise won’t earn you mercy. Kneeling only invites more bullying. China won’t kneel down because we know standing up for ourselves keeps the possibility of cooperation alive while compromise snuffs it out. China won’t back down, so the voices of the weak will be heard. Bullying will be stopped, and justice will not disappear from the world. All bullies are just paper tigers. Car giant General Motors is also struggling to get a grip on the economic outlook. GM has pulled its annual forecast, blaming uncertainty created by Donald Trump’s trade war. GM’s chief financial officer Paul Jacobson told a press call: “We believe the future impact of tariffs could be significant.” “We’re telling folks not to rely on the prior guidance, and we’ll update when we have more information around tariffs.” Jacobson was speaking after GM reported net income of $499m in the first three months of this year down from $536m for the quarter ending on 31 March, 2024. The company has also delayed a call with analysts that had been scheduled for today, until Thursday. GM says: Based on recent reports regarding updates to trade policy, GM Chair and CEO Mary Barra and GM Chief Financial Officer Paul Jacobson will now host a conference call for the investment community at 8:30 a.m. ET Thursday, May 1 instead of Tuesday, April 29 to discuss these results and GM’s updated 2025 full-year guidance. The company’s initial full year 2025 financial guidance does not contemplate the potential impact of tariffs. Donald Trump’s trade war is making it hard for delivery companies to assess their future prospects. Today, United Parcel Service (UPS) said the “current macro-economic uncertainty” means it is not updating its outlook for this year. UBS, which could be hit if shipments to US consumers fall, made the comments as it reported a 0.7% rise in revenues in the first three months fo this year, with operating profits up 3.3%. Ireland’s economy has grown for the third quarter running, driven by major international companies based in the Republic. Irelands’ Central Statistics Office has reported that Gross Domestic Product (GDP) increased by 3.2% in the first quarter of 2025. Enda Behan, Statistician in the National Accounts Integration Division, said: “In today’s release, GDP is estimated to have expanded by 3.2% in January, February and March (Q1) 2025 in volume terms when compared with Q4 2024. This was driven by an increase in the multinational dominated sectors in Q1 2025 with a more modest increase in the domestic sectors. GDP is estimated to have risen by 13.3% when compared with Q1 2024. The Bank of England’s stability watchdog has increased its scrutiny of Britain’s banks following the turmoil triggered by Donald Trump’s trade war, MPs have heard today. Sam Woods, head of the Prudential Regulation Authority, told the Treasury Committee this morning that the PRA has “stepped up” its monitoring of the firms, as is typical in such situations. Woods told MPs that “we consider ourselves still to be in the middle of this thing”, as he outlined the response to the jittery markets of recent weeks. He says the PRA is watching “very closely”, but has not taken its monitoring to the highest level of ‘daily liquidity monitoring’, as it doesn’t think that is necessary. Woods adds that the regulator is also watching for the “macro impact” of the trade war, reminding MPs that the IMF downgraded its growth forecasts last week. I think it would be interesting to see whether our banks in the next period, choose to provide more for a different economic environment, because they do forward looking provisions. That’s where our focus is now. Reminder: HSBC raised its expected credit losses by $200m to around $900m for the first quarter of 2025 this morning. Woods also told MPs that the PRA did not see any signs that the market turmoil after ‘Liberation Day’ had spread into bank funding, and that there was also no sign that customer behaviour was affected. But, he did flag the ‘very unusual move’ in the financial markets, which was the selloff in the US dollar and in US government debt. Woods says that was a worry: Normally we see the opposite in these risk off type of conditions. Normally we see a flight into those types of assets. So that was quite concerning. He added that it is “notable” that after this move, president Trump decided to announce his 90-day pause which settled the markets. Economic sentiment across Europe has weakened this month, as the Trump trade war hit financial markets. The European Commission’s Economic Sentiment Indicator, just released, declined by 1.4 points in both the European Union (to 94.4) and the euro area (to 93.6). A measure of employment expectations also fell across the EU. German sportswear group Adidas has warned today that Donald Trump’s tariffs will push up costs for American consumers. In its latest financial results, Adidas told shareholders that it faces increased uncertainty due to US tariffs and higher macroeconomic risks. It reported a 13% jump in sales, and increased operating profits. Adidas chief executive Bjørn Gulden would said that the uncertainty created by new tariffs imposed by the US had “put a top” to an upgrade to the company’s guidance this year. Gulden added: Although we had already reduced the China exports to the US to a minimum, we are somewhat exposed to those currently very high tariffs. What is even worse for us is the general increase in US tariffs from all other countries of origin. Since we currently cannot produce almost any of our products in the US, these higher tariffs will eventually cause higher costs for all our products for the US market. Given the uncertainty around the negotiations between the US and the different exporting countries, we do not know what the final tariffs will be. Therefore, we cannot make any ‘final’ decisions on what to do. Cost increases due to higher tariffs will eventually cause price increases, not only in our sector, but it is currently impossible to quantify these or to conclude what impact this could have on the consumer demand for our products. Primark-owner ABF is hoping that new tariffs on small shipments into America might encourage shoppers to visit its US stores. ABF currently has 29 Primark stores in the US, and hopes to raise that to 60 by the end of 2026. CEO George Weston has told Reuters today that the company remains committed to that plan, and suggests that the end of the ‘de minimis’ rule (under which packages worth less than $800 did not qualify for any taxes or tariffs) could help sales. Weston says: “De minimis imports in the U.S. are very, very large, they supply a lot of Americans who don’t know about Primark yet but are looking for value. “With prices going up from this part of the trade, I wonder if some Americans might start going back to shopping centres to find value there.” UK grocery inflation has edged up this month, as consumers are hit by rising food prices. Data provider Kantar has reported that supermarket prices rose by 3.8% per year in the four weeks to April 20, up from 3.5% a month earlier. Despite this squeeze, spending on Easter eggs was up 11% year-on-year. Fraser McKevitt, head of retail and consumer insight at Kantar, explains: “Chocolate confectionery prices rose by 17.4% this period, the fastest of any category, but that didn’t stop the British public treating themselves this Easter. The volume of chocolate eggs sold through supermarket tills still grew by 0.4% on last year, while at the dinner table lamb was the most popular fresh meat joint, followed by beef and pork. Some households chose to indulge in less seasonal fare as the sun came out and they dusted off the barbecue, with burger sales shooting up by 31% over the last month.” A separate report from the British Retail Consortium today has shown that food inflation increased to 2.6% year on year in April, up from 2.4% in March. ABF are also threatening to shut their UK bioethanol plant, Vivergo, unless the government relaxes regulations on the industry. ABF told the City this morning that Vivergo, located in the East Riding of Yorkshire, has cut its production levels in response to continued low prices for bioethanol, leading to lower sales and an operating loss in the first half of the financial year. The company says: The way in which regulations are being applied to bioethanol is undermining the commercial viability of our business. We are having constructive discussions with the UK Government to explore regulatory options to improve the position. There is no guarantee that these discussions will be successful, and we will either mothball or close the Vivergo plant if necessary. Groceries-to-clothing firm Associated British Foods has added its voice to the chorus of warnings about the economic outlook. ABF told shareholders this morning that the “geopolitical landscape continues to be fragile”, citing the Russian war in Ukraine as well as trade polic changes in the US. ABF flagged the risk of a US recession, saying: Consumer sentiment remains cautious and trading activity within elements of our shopper base has been weak. Sentiment is unlikely to improve as markets continue to face uncertainty and instability following recent tariff announcements by the US, retaliatory actions by China and the risk of further tariff trade wars. Consumer confidence could deteriorate further as a number of countries, including the US, face the risk of recession that could increase individuals’ debt problems. The impact on our businesses will depend on the extent of government intervention, the extent of increased taxation on individuals and businesses and the duration of any economic downturns. The company reported a 2% drop in revenues for the six months to 1 March, with pre-tax profits down 21%. CEO George Weston told shareholders he was “frustrated” with the results at its sugar business, which made an adjusted operating loss of £16m due to lower prices in Europe. ABF, which owns the clothing chain Primark, also warned that trading has been challenging in the UK, saying: The UK clothing retail market declined in the period, reflecting cautious consumer sentiment and a lack of seasonal purchasing catalyst in the autumn months due to mild weather. Shares in the company are down almost 9% this morning, the top faller on the FTSE 100 index. The architect of BP’s failed green energy agenda will leave the embattled oil company within months as it continues its retreat from low-carbon investments following this morning’s sharp fall in profits (see last post). The oil company said Giulia Chierchia, the executive in charge of BP’s sustainability ventures, would step back from her role from 1 June 2025 to “pursue other opportunities” outside the company. She will not be replaced. Oil giant BP has missed profit forecasts this morning, adding to the pressure on the company’s executives. BP reported an underlying profit of $1.38bn for the first quarter of 2025, missing forecasts of $1.53bn, and much weaker than the $2.7bn it earned in January-March 2024. The company blamed “weak” trading at its gas trading division – gas prices have fallen this year, on concerns that a global trade war will hurt demand for energy. Shares in BP have dropped by 2.3% in early trading. The company has been under growing pressure from activist investor Elliott Management this year to make spending cuts, to increase its free cash flow. Murray Auchincloss, BP’s chief executive officer, says: In February, we announced a fundamental reset of our strategy - to grow the upstream, focus the downstream and invest with discipline in the transition - and we have already made significant progress. So far this year we have started up three major projects, made six exploration discoveries and have progressed our divestment programme - all while delivering strong operational performance, with over 95% upstream plant reliability supporting the best operating efficiency* on record, and over 96% refining availability. We continue to monitor market volatility and changes and remain focused on moving at pace. I’m confident that our plans to strengthen the balance sheet, reduce costs, and improve cash flow and returns will grow long-term shareholder value and strengthen the resilience of bp. In what could be a nod to Elliott, BP says it will lower its planned spending for 2025 by $500m (£373m) to about $14.5bn this year. It also plans to divest between $3bn and $4bn of assets. Patrick Galey, Interim Head of Fossil Fuel investigations at Global Witness, is unimpressed, saying: “BP has spent the last year flip-flopping on its climate commitments, lurching back towards fossil fuels just as the world needs a clean energy transition.” “The fact that its returns are now dwindling and investors seem to be losing confidence shows BP’s climate u-turn is not only planet-wrecking but financially wrong-headed too.” “Now is the time for investors to change direction. Continuing to back fossil fuel giants as the world moves towards safer, cleaner, home-grown energy is a decision that could leave them empty-handed in the years ahead, with falling demand and billions’ worth of stranded assets.” Amazon is seeking steep discounts from suppliers and setting tough terms to protect its margins amid the Trump trade war, the Financial Times reports this morning. According to the FT, Amazon had sought low double-digit price cuts from the sellers of goods ranging from homeware to consumer electronics, according to three vendor consultants — who negotiate on behalf of multiple brands and suppliers. You can read the story here. German airline Lufthansa is sticking with its forecasts for this year, despite the rising trade tensions and tougher US immigration processes under Donald Trump. CEO of Lufthansa, Carsten Spohr, struck an upbeat tone this morning, telling investors: “Global demand for air travel continues to grow. Despite all the geopolitical uncertainties, we therefore remain on course for growth, are optimistic about the summer, and are sticking to our positive outlook for 2025. In the first quarter, our airlines were able to sell their expanded capacity at higher yields in the market. There have been reports in recent weeks that tourism to the US has fallen due to a backlash against Trump, and high-profile deportations and detentions at the border. Lufthansa, though, has seen an increase in transatlantic demand; Spohr</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Amazon has denied that it planned to show the cost of new US tariffs on its website, after being heavily criticised by the White House. White House press secretary Karoline Leavitt claimed the plan to disclose tariff costs was “a hostile and political act by Amazon,” and “Another reason why Americans should buy American” A company spokesperson says: “The team that runs our ultra low cost Amazon Haul store considered the idea of listing import charges on certain products. This was never approved and (is) not going to happen.”</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Time to wrap up: Donald Trump’s increasingly erratic trade war has triggered a slump in shipments to the US’s most important ports, amid the growing risk of a recession in the world’s largest economy. In the latest sign of the US president’s tariff policies rattling the economy, figures show the number of vessels scheduled to arrive at the Port of Los Angeles next week is down by almost a third on the same period a year earlier. According to the data compiled from ocean carrier manifest records by Port Optimizer, the number of arrivals this week is on track to be down by about 11% on the same week last year. Separate figures reported by the Financial Times from Vizion, a data provider, show container bookings from China to the US fell 45% by mid-April compared with a year earlier. Asset manager Apollo Global warned that the US trade with China was weakening, as America suffers a ‘stagflation shock’. Marks &amp;amp; Spencer has told hundreds of workers at its main online distribution centre in Leicestershire to stay at home as website orders remain on hold for the fourth day in a row. The retailer, which is battling the consequences of a cyber-attack that began a week ago and has affected stores as well as its online business, told 200 agency staff at the Castle Donington site they were not currently required. The move, first reported by Sky News, came after it halted all orders through its website and apps on Friday. The company has apologised to shoppers for “this inconvenience”, which will hit its online clothing and homeware sales, which amount to almost £3.8m a day on average. Shares in M&amp;amp;S fell over 2% at one stage, and have closed down 0.6%. The UK economy is set to slow sharply for the next two years as Donald Trump’s global tariff war weighs on consumer spending and business investment, a study by a leading forecaster has predicted. Manufacturing businesses in Texas have reported a slump in activity this month, as Trump’s tariffs caused economic disruption. Shares in Deliveroo have risen by 17% as investors reacted to a $3.6bn (£2.7bn) takeover offer by the rival food delivery app DoorDash that could net its founder more than £170m. The EU’s strategy to secure its own supply of microchips is “deeply disconnected from reality”, a damning report by the official European court of auditors (ECA) has found. Britain’s blue-chip share index had matched its best run of daily gains in eight years – just! The FTSE 100 ebbed in late trading, perhaps hurt by that weak economic data from the US. But it ended the day in positive territory, up 2 points or 0.02% at 8417 points. That means the FTSE 100 has risen for the last 11 days trading, matching the 11-day run recorded in December 2019. It hasn’t had a longer stretch since January 2017, when the index posted a 14-day rally. The FTSE 100 hasn’t recovered all its trade war losses, though – it had been trading over 8,600 points before Donald Trump announced his new tariffs on US trading partners at the start of April. Stocks have been rising as Trump backed away from a trade war, by pausing most of those tariffs for 90 days. Neil Wilson, UK investor strategist at Saxo Markets, points out that the FTSE 100 has “defensive characteristics” – many of its members are decent dividend payers. But, he adds: Markets appear way too complacent at this stage – tariffs are on pause, not cancelled. Markets are behaving like the latter. Certainly the direction of travel can be ascertained ‘at the moment’, but we don’t what happens next. Because this is not a game of chicken that Trump is losing right now. The early Wall Street rally has rather fizzled out, after investors learned of the downturn in Texas’s manufacturing sector this month. The Dow Jones industrial average is now flat, while the tech-focused Nasdaq has now dropped by 1%. Here’s some snap reation to the poor Dalles Fed manufacturing report: Just in: manufacturing activity in Texas has plunged at the fastest rate since the early months of the Covid-19 pandemic five years ago. Company bosses in the region are warning that Donald Trump’s trade war is hurting their businesses, with That’s according to the latest Texas Manufacturing Outlook Survey from the Federal Reserve Bank of Dallas. It has found that business conditions worsened in April, with a measure of general business activity index falling to its lowest reading since May 2020. A gauge of economic uncertainty jumped, as bosses’ view of the economic outlook also fell to a postpandemic low. An index of new orders plummeted, while an index of shipments index fell into negative territory for the first time this year. Helpfully, the Dallas Fed also released comments from survey respondents. One chemicals manufacturing firm said: “Tariff uncertainty and actual impact is likely to be significant for the business and ongoing projects”. A computer and electronics manufacturer also warned about the economic damage of a trade war, saying: There is really no way to predict anything accurately six months out or even six weeks out now for our industry due to the tariff and trade uncertainty. Carve-outs for large electronics businesses (cellphones and laptops) leaves small business burdened to deal with tariffs on our own, which are likely to cause delays, cancellations and early product obsolescence on existing products and orders. We have already had to turn around and refuse shipments because customers cannot afford the tariffs, delaying our ability to build, which will eventually lead to job losses. If this continues for any length of time, many small companies are likely to be significantly hurt or even gone. If we want to bring manufacturing back to the U.S., can we try not to kill the companies that can actually help do that before we get the chance? Maybe we can think about using a scalpel rather than a sledgehammer? The risk we face now is far greater and less understood than what we saw during the COVID shutdown. Consumers and businesses will limit investment and orders until there is some sense of stability, and we have already experienced this with smaller orders and delayed orders. It’s chaos right now. Food manufacturers also criticised trade uncertainty, with one saying: Tariffs and tariff uncertainty are wreaking havoc on our supply lines and capital spending plans. Travel companies are among the top risers on the S&amp;amp;P 500 in early trading, with Norwegian Cruise Line Holdings up 3.5%, and Southwest Airlines gaining 2,8%. The New York stock market has begun the week with some small gains. The Dow Jones industrial average has risen by 184 points, or 0.5%, to 40,297 points. The broader S&amp;amp;P 500 has gained a more modest 0.1%. Despite its recent recovery, the Dow is still down 3% over the last month. But even so, only Richard M. Nixon’s second term has offered a worse return from US equities, 100 days in, than Donald Trump’s second stint That’s according to AJ Bell investment director Russ Mould, who explains: As President Trump approaches 100 days in office, an 11% rally in America’s S&amp;amp;P 500 index from its closing low on 8 April may just stop his second term in office from offering investors the worst start of any post-war American leader, in terms of stock market returns. “The S&amp;amp;P 500 is down by 7.9% since Trump’s inauguration on 20 January and only Richard M. Nixon’s second term offered a tougher start for investors, as the index fell by 9.9% in the first 100 days of his second term back in 1973.” “The rough start to Trump’s second presidency, so far as share prices and the dollar is concerned, represents a remarkable shift in sentiment, given the rapturous welcome given to Trump’s election victory last November, when the S&amp;amp;P 500 (and the greenback) soared, while US Treasury yields remained stable. “The imposition of blanket tariffs, an escalation of tensions with China and then a flurry of sidesteps and backtracks, as additional reciprocal levies are delayed, exemptions are provided for technology hardware and tentative olive branches are offered to Beijing leave everyone confused and seem to be shaking markets’ prior strong faith in American exceptionalism. Despite all the anxiety about the economic damage of the US trade war, European markets are higher today. In London, the FTSE 100 index is now up 30 points or 0.36% at 8445 points, on track for its highest close in over three weeks. Germany’s DAX is 0.7% higher, while France’s CAC 40 index is up 1%. In Madrid, the stock market is still operating despite the massive power outage hitting Spain, and Portugal, with the Spanish IBEX up 0.6%. Tom Stevenson, investment director at Fidelity International, says markets are in limbo: “Investors are stuck in an uneasy place between optimism about the so-called Trump put and anxiety about what looks like an increasingly likely economic slowdown or recession. “The Trump put refers to the idea that there is a point at which the US President will respond to market weakness and reverse trade and tariff measures. Sharp rallies in both bond and equity markets in the past couple of weeks suggest that this put exists and that it will kick in at close to the recent market lows. “That’s the optimistic argument. It is supported by still reasonable earnings growth expectations (albeit slowing in future quarters) and valuations which have fallen from their recent highs. “The earnings picture will become clearer this week as a swathe of results emerge across a range of key sectors. Most important of all will be tech stock results from Meta, Microsoft and Amazon. At the same time, valuations of those Magnificent Seven shares have come back from elevated levels to more reasonable multiples. The Mag Seven as a whole is now priced at 25 times expected profits, compared with 40 only a few months ago. Germany’s Chancellor-in-waiting Friedrich Merz has declared today that he will urge Donald Trump to “go to zero” on all tariffs. Merz declared: “We will offer the United States of America that it would be best if we go to zero for all customs duties in the mutual exchange of goods.” He also suggested “the mutual recognition of technological standards” between Germany and the US, explaining: “What we have seen in recent years and decades are increasingly divergent technical barriers between the individual major trading nations of the world, which we must overcome, and this can also contribute to the sustainable reduction of bureaucracy.” Merz also announced some early cabinet picks – utility executive Katherina Reiche was named as his likely economy minister, and foreign policy expert Johann Wadephul, a former soldier and trained lawyer, gets the nod as foreign minister. M&amp;amp;S have confirmed that agency staff at its Castle Donington clothing and homewares logistics centre in the East Midlands were told not to come in today. Workers employed by M&amp;amp;S at the site are still working, PA Media reports. The retailer’s stores are still open and operating, and shoppers are still able to browse its website and app. Contactless payments are also back online in stores after these were originally impacted by the cyber issue. The company has taken action to protect its network and has also reported the incident to data protection supervisory authorities and the National Cyber Security Centre. The chief executive of Channel 4, Alex Mahon, is to step down after eight years and will leave the broadcaster in the summer. During her tenure Mahon, who joined in 2017 as the first female CEO in the broadcaster’s four-decade history, helped fight off two attempts to privatise Channel 4. The 51-year-old, who faced criticism when she took home the biggest pay packet of any chief executive in Channel 4 history, will be replaced on an interim basis by the chief operating officer, Jonathan Allan. “She has been one of the most impactful chief executives since Jeremy Isaacs’ founding of Channel 4 more than 42 years ago,” said Dawn Airey, interim chair at the broadcaster. Fast food chain Domino’s Pizza has reported a drop in US sales in the last quarter – a potentially worrying sign for the economy. Like-for-like store sales at Domino’s US outlets fell by 0.5% in the first three months of this year, the company reports, taking the shine off a 3.7% rise in international same store sales growth. Investec analyst Kate Calvert has pointed out that the longer it takes for online sales to resume, the worse the hit would be for M&amp;amp;S. She says: “There will be a short-term profit impact without a doubt.” The gold price is slipping away from its recent record high today. Bullion is down 0.85% at $3,290 per ounce, as investors favour riskier assets. Last Tuesday gold hit a new alltime high of $3,500 per ounce, but has eased back since as trade war anxiety in the markets has eased (despite signs that the conflict is causing economic harm). Achilleas Georgolopoulos, senior market analyst at Trading Point, says: It is a rather steady start to the trading week, as market participants are mostly preparing for what lies ahead. Risk appetite appears to be on the mend though, with US equity indices experiencing a rather positive performance last week and the US dollar erasing its early-week losses. The Nasdaq led the rally on the back of commentary, and partly wishful thinking, that the US-China trade war might gradually de-escalate, with technology products being the first beneficiaries of a lower tariff regime. The path, of course, towards a US-China agreement will not be straightforward, despite some positive commentary from both sides, mostly from US Treasury Secretary Bessent. Both governments are unwilling to make the first significant step and open the door to proper negotiations, as such a move might be seen as a sign of weakness, a perception President Trump is unlikely to accept. UK retailers have reported that sales volumes fell for the seventh month running in April, according to the CBI’s latest Distributive Trades report. A net balance of -8% of retailers reported that sales volumes fell this month, rather thn rising – an improvement on the -41% balance reported in March. However, retailers expect sales to fall at a quicker pace next month. Martin Sartorius, principal economist at the CBI, blames the tax rises announced in last year’s budget, which came into effect this month, saying: “Annual retail sales volumes fell more slowly in April, but firms remain pessimistic about the outlook due to the impact of Autumn Budget measures, persistently weak consumer sentiment, and global economic uncertainty. These themes were echoed in the wholesale sector, which reported one of the sharpest sales declines in the past four years. The CBI’s survey paints a more downbeat picture than the official retail sales report from the Office for National Statistics, which shows that sales rose in the first quarter of this year (on a seasonally-adjusted basis….) Oof! There’s a high risk that the global economy will slip into a recession this year, according to a majority of economists in a Reuters poll. Asked about the risk of a global recession this year, a 60% majority - 101 of 167 - said it was high or very high. Sixty-six said low including four who said very low. Many of the economists polled by Reuters also believe that Donald Trump’s tariffs have damaged business sentiment. Reuters explains: Showing an uncommon unanimity, none of the more than 300 economists polled April 1-28 said tariffs had a positive impact on business sentiment, with 92% saying negative. Only 8% said neutral, mostly from India and other emerging economies. Back in Beijing, China’s foreign ministry has said President Xi Jinping had not spoken to Donald Trump. The ministry also denied that the two administrations are in talks to strike a tariff deal, which contradicts a claim from Trump last week. Guo Jiakun, a ministry spokesperson, told a press conference: “As far as I know, the two heads of state have not called each other recently, “I would like to reiterate that China and the U.S. have not conducted consultations or negotiations on the tariffs issue. “If the U.S. really wants to solve the problem through dialogue and negotiation, it should stop threatening and blackmailing (China).” Last Friday, Time Magazine reported that Trump had told them last week that his administration is talking with China to strike a tariff deal and that Chinese President Xi Jinping had called him. Sky News are reporting that hundreds of agency staff at Marks &amp;amp; Spencer’s main clothing and home warehouse in the East Midlands have been told not to come in. That highlights the disruption being cause by the huge M&amp;amp;S cyber-attack, which has led to the suspension of online orders last week. Goldman Sachs analysts remain cautious about the outlook for shares, though. In a new research note today, Goldman say they “continue to see equities as in a bear market”, due to the likelihood of elevated trade uncertainty and weaker economic activity. The equity market is currently pricing a growth outlook above Goldman economists’ baseline forecast, they say, citing the recovery in the pan-European Stoxx 600 index: Despite the uncertainty, the STOXX 600 is up 3% year-to-date, having rebounded by 11% from its recent trough. Looking at the performance of Cyclicals versus Defensives, we find that the European equity market is currently pricing Euro area GDP growth of approximately 1.5%. This is higher than our economists’ forecast for Euro area real GDP growth of 0.7% in 2025. Britain’s stock market is on track to match its longest run of gains in eight years. The FTSE 100 index has risen by 20 points, or 0.25%, in early trading to 8436 points. That puts the blue-chip shares index on track for its 11th daily rise in a row, a record last set in December 2019 after Boris Johnson’s election win. The FTSE 100 last set a longer winning run from late-December 2016 to mid-January 2017, when it rose for 14 days on the trot. The recovery over the last few weeks has been helped by the US pausing many of its tariffs on trading partners (tho not China) These recent gains have not fully recovered the losses after Donald Trump’s announcement of new global tariffs, though, as this chart shows: For April as a whole, the FTSE 100 is still down 1.7%. Marks &amp;amp; Spencer are leading the FTSE 100 fallers this morning, as it reels from the damage caused by a cyber-attack. Shares in M&amp;amp;S are down 2.3% this morning at 376p, as traders digest the ongoing disruption at the company. On Friday it halted all orders through its website and apps, and encouraged customers to visit its stores instead. The cyber incident began a week ago, on Easter Monday, affecting contactless payments and click-and-collect orders in stores across the UK. M&amp;amp;S disclosed it on Tuesday, saying a “cyber incident” affected contactless payments and the pick up of online orders in its stores in recent days. Shares in M&amp;amp;S have dropped by over 8% since then, having closed at 411p before Easter. Susannah Streeter, head of money and markets at Hargreaves Lansdown, says the ongoing problems underline how difficult the breach has been to get a handle on. Streeter points out that the suspension of online orders will be hugely damaging for sales, adding: Marks and Spencer’s recent run of success has been partly down to how it been so efficient at managing its multi-channel operations with click and collect services particularly popular. It’s been reducing its store footprint focusing on smaller food stores where customers can swing buy and pick up products bought online. This ease of shopping and delivery has been upended. Even though stores are open, many simply don’t stock the popular ranges from online. Fashion sales are likely to take a big hit particularly as the attack has come during the spell of warm weather when summer ranges would ordinarily be piling up in virtual baskets. While other retailers have not been immune to IT breaches, the depth of Marks and Spencer’s problems in resolving the issue are worrying, and it may take some time to win back some more warier shoppers. Shares in food delivery group Deliveroo have jumped by 17% at the start of trading in London, after receiving a takeover approach from US rival DoorDash. On Friday night, the news broke that DoorDash had offered to buy Deliveroo for $3.6bn (£2.7bn). Deliveroo said that received an indicative proposal from DoorDash for a possible cash offer worth 180p per share, and that it would be “minded to recommend such an offer to Deliveroo shareholders”. Its shares have jumped to 170p this morning…. This morning, Deliveroo also announced that it has suspended its £100m share buyback programme, due to the approach from DoorDash. DoorDash’s interest comes four years after Deliveroo floated on the London stock market, in what has been called the City’s worst IPO ever. Deliveroo’s shares were priced at 390p each, but slumped by a quarter on the first day of trading – causing the firm to be dubbed “Flopperoo”. The Times points out today that if the DoorDash deal goes through at 180p, Deliveroo founder Will Shu would receive a payout of more than £172m, based upon his 5.9% stake The UK economy is set to slow sharply for the next two years as Donald Trump’s global tariff war weighs on consumer spending and business investment, a study by a leading forecaster has predicted. The EY Item Club is now forecasting that UK gross domestic product (GDP) will grow by 0.8% this year, down from a projection of 1% in February, and has cut its 2026 forecast from 1.6% to 0.9% as longer-term effects hit the UK. American customers of fast-fashion giant Shein are now feeling the impact of the trade war. Shein raised the US prices of a swathe of products on Friday, Bloomberg reported, in anticipation of new tariffs on small parcels. Over to Bloomberg for the details: The average price for the top 100 products in the beauty and health category increased by 51% from Thursday, with several of the items more than doubling in price. For home and kitchen products and toys, the average jump was more than 30%, led by a massive 377% increase in the price of a 10-piece set of kitchen towels. For women’s clothing the rise was 8%. This follows Donald Trump’s decision to end the “de minimis” exemption for small packages from mainland China and Hong Kong. which had meant that packages under $800 did not qualify for any taxes or tariffs. China’s policymakers are insisting today that they will hit this year’s growth targets, despite the impact of Donald Trump’s tariffs. The vice head of China’s state planner said on Monday he was “fully confident” that the world’s second-largest economy would achieve its economic growth target of around 5% for 2025. Zhao Chenxin, vice chair of the National Development and Reform Commission, told a press conference that new policies will be rolled out over the second quarter, based on changes in the economic situation. Zhao said: “The achievements of the first quarter have laid a solid foundation for the economic development of the whole year. No matter how the international situation changes, we will anchor our development goals, maintain strategic focus and concentrate on doing our own thing.” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Donald Trump’s trade war is weakening the US economy and causing a plunge in trade with China, economists and logistics firms are warning. Nearly four week’s after Trump’s ‘Liberation Day’ announcement of higher tariffs triggered a trade war with Beijing, evidence is mounting that businesses and consumers are cutting back. Torsten Sløk, chief executive at asset manager Apollo Global Management, explains: For companies, new orders are falling, capex plans are declining, inventories were rising before tariffs took effect, and firms are revising down earnings expectations. For households, consumer confidence is at record-low levels, consumers were front-loading purchases before tariffs began, and tourism is slowing, in particular international travel. Sløk has pulled together a chartbook highlighting the damage to company earnings… …on new orders… …and notably on trade with China. A trade war is a “stagflation shock”, Sløk fears. He explains that it typically takes between 20 and 40 days for a sea container to travel from China to the US. That means that the slowdown in container departures from China to the US which started in early April will be felt at US ports in early and mid-May. That would hit demand for trucking from mid-May, leading to empty shelves and layoffs in trucking and retail industry, causing what Sløk dubs “The Voluntary Trade Reset Recession”. Sløk warned on Friday: In May, we will begin to see significant layoffs in trucking, logistics, and retail — particularly in small businesses such as your independent toy store, your independent hardware store, and your independent men’s clothing store. With 9 million people working in trucking-related jobs and 16 million people working in the retail sector, the downside risks to the economy are significant. There are signs today that this trade slowdown is underway, due to the 145% tariff imposed on Chinese imports to the US. The Financial Times reports this morning that the Port of Los Angeles, the main route of entry for goods from China, expects scheduled arrivals in the week starting 4 May to be a third lower than a year before. The new higher tariffs announced on other countries are currently paused, of course, while the US negotiates new trade deals. Trump has claimed to Time Magazine that he’s made 200 deals. But this appears to be, well, an exaggeration. US Treasury secretary Scott Bessent told ABC News he believes Trump is “referring to sub deals within the negotiations we’re doing.” Bessent insisted, though, that progress is being made, arguing: If there are 180 countries, there are 18 important trading partners, let’s put China to the side, because that’s a special negotiation, there’s 17 important trading partners, and we have a process in place, over the next 90 days, to negotiate with them. Some of those are moving along very well, especially with the Asian countries. Last week, shipping giant Hapag-Lloyd reported that its customers have cancelled 30% of shipments to the United States from China….and there has been a “massive increase” in demand for consignments from Thailand, Cambodia and Vietnam instead. The agenda 11am BST: CBI’s distributive trades survey of UK retailing 11am BST: France’s unemployment data for March 3.30pm BST: Dallas Fed manufacturing index for April</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Number of vessels scheduled to arrive at Port of Los Angeles down by a third. Shipments from China to the US fell 45% by mid-April compared with a year earlier. UK economy set to slow sharply for the next two years due to trade war.</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>With the London stock market closed, it’s time to wrap up for the day, and the week! A brisk recap: US consumer sentiment has fallen to one of the lowest readings on record, as Americans fear that Donald Trump’s trade war will drive up prices and slow the economy. China has denied it is in talks with the US about a trade deal… after Donald Trump claimed the two sides were negotiating. But there are also signals that Beijing is lifting some tariffs, to de-escalate the situation. Top policymakers in Beijing also pledged to support firms and workers most affected by the impact of new US tariffs. In London, the FTSE 100 index has posted its longest winning streak in over five years. Our US Politics blog will be tracking the action: Here’s our economics editor Heather Stewart’s take on this week’s Spring Meeting of the IMF in Washington. And here’s a flavour: Kristalina Georgieva’s favourite film, the International Monetary Fund boss told the audience at a packed panel event in Washington on Thursday, is Tom Hanks’s cold war romp Bridge of Spies. In one of the stranger digressions in a frequently strange week, Georgieva recalled the moment when Hanks’s character, a US lawyer, tells the Soviet spy he has been appointed to defend that he will probably be executed. “You don’t seem alarmed,” Hanks says to him; to which the spy – played by Mark Rylance – replies, “Would it help?” Georgieva mentioned the vignette to underline the fact that this week’s spring meetings of the IMF and World Bank were not swept up in panic, despite the mayhem emanating from the Trump administration. Britain’s stock market has just posted its longest run of daily gains in over five years. The FTSE 100 index of blue-chip shares has closed almost 8 points higher tonight at 8415 points, a rise of 0.09%. That means it has now risen for 10 sessions in a row, having climbed from 7679 points on 9 April. That’s the longest winning run since 2019, when Boris Johnson’s election win sparked a relief rally. Neil Wilson, UK investor strategist at Saxo Markets, says the UK market has benefitted from a broad relief rally, but there’s more to it than that… Wilson writes: The news flow on tariffs has been incrementally more positive, while the Fed has hinted at being ready to cut rates in the coming months. But it’s also the case that the FTSE has a lot of defensive characteristics - we’ve noted earlier that there are plenty of stocks with hefty dividend yields that can be viewed as a place of relative shelter from instability and volatile markets. It should be noted that when markets are stressed, capital preservation becomes even more important and some big dividend payers could be attractive. The relative shelter from volatility is highlighted by the fact that in the period since April 9th, while the FTSE has made slow and steady progress, the S&amp;amp;P 500 has seen one daily decline of almost 3.5%, and two more in excess of 2%. The FTSE 100 may be like an old blanket that you can wrap yourself in when times are tough and the shiny stuff breaks. It may also be that the UK is benefiting from a broad reallocation of global capital from the US to elsewhere. It’s noteworthy that in the same two-week period from April 9th closing low, sterling has gained about 4.5% against the dollar. In dollar terms the FTSE is up about 15% since the lows after recovered its pre-liberation day equilibrium. Back in Washington, Bank of England policymaker Megan Greene has predicted that Donald Trump’s tariffs are likely to lead to lower rather than higher inflation in the UK. Greene told a discussion with the Atlantic Council think tank on the sidelines of the International Monetary Fund’s spring meeting that: “We have tariffs, and none of us have any idea what they’ll look like when the dust finally settles,” “In my mind, the risk space has changed a little bit. So I think the risk is now on the disinflationary side. So I think that tariffs on the UK would, on net, be more disinflationary than they are inflationary.” Greene, one of the hawkish members of the Bank’s monetary policy committee, also said she was concerned about weak growth. Factcheck: Tariffs could be deflationary in two ways. First, a global trade war could dampen economic growth, leading to weaker demand. Second, companies hit by US tariffs could ship more goods to other countries, such as the UK, and cut prices to be competitive. On the other hand, if the UK retaliated with its own tariffs, then that would push price up. Ouch! US consumers’ economic expectations have slumped at the fastest rate since the 1990s recession. A closely-watched poll of consumer morale, from the University of Michigan, has found that economic expectations have fallen by a “precipitous” 32% since January, which they say is the biggest three-month drop since the economic downturn 35 years ago. The survy also found that consumer sentiment fell for the fourth straight month in April, plunging 8% from March, driven by a tumble in expectations. The final April sentiment index fell to 52.2 from 57 in March. That’s the fourth-lowest reading in data back to the late 1970s, Bloomberg reports. Sentiment is 32% lower than a year ago, the survey show. Surveys of Consumers director Joanne Hsu says: Expectations have fallen a precipitous 32% since January, the steepest three-month percentage decline seen since the 1990 recession While this month’s deterioration was particularly strong for middle-income families, expectations worsened for vast swaths of the population across age, education, income, and political affiliation. Consumers perceived risks to multiple aspects of the economy, in large part due to ongoing uncertainty around trade policy and the potential for a resurgence of inflation looming ahead. Labor market expectations remained bleak. Even more concerning for the path of the economy, consumers anticipated weaker income growth for themselves in the year ahead. Without reliably strong incomes, spending is unlikely to remain strong amid the numerous warnings signs perceived by consumers. The poll also found that Americans’ year-ahead inflation expectations surged from 5.0% last month to 6.5% this month, the highest reading since 1981. The University of Michigan also provided a handy chart, showing how inflation expectations evolved with major trade policy announcements this month. They say: After the April 9 partial pause in tariff increases, inflation expectations ebbed but remained substantially elevated relative to March. There’s a mixed start to trading on Wall Street today, as investors try to work out what’ happening in the trade war. The Dow Jones industrial average, of 30 large US companies, has dipped by 22 points or 0.05% to 40,070 points. The broader S&amp;amp;P 500 index is up 0.2%, though. Traders could take some comfort from signs earlier today that China is looking to de-escalate the situation, by removing some tariffs. However, they may be concerned that China has denied that it is in talks with the US about tariffs. A foreign ministry statement posted by the Chinese Embassy in the US says: “China and the US are not having any consultation or negotiation on tariffs. The US should stop creating confusion.” That rather undermines Donald Trump’s claim to Time Magazine that his administration is in active talks with the Chinese to strike a deal. Oooh! Back in the London stock markets, shares in Marks &amp;amp; Spencer have dropped by 4% after it announced it is pausing taking online orders in the UK and Ireland due to a recent ‘cyber incident’. M&amp;amp;S told the City: As part of our proactive management of the incident, we have made the decision to pause taking orders via our UK &amp;amp; Ireland websites and apps and some M&amp;amp;S International operated websites. The M&amp;amp;S product range is available to browse online, and our stores remain open and ready to welcome and serve customers. We continue to manage the incident proactively and the M&amp;amp;S team - supported by leading experts - is working extremely hard to restore online operations and continue to serve customers well. Earlier this week, M&amp;amp;S apologised to customers after a “cyber incident” affected contactless payments and the pick up of online orders in it stores in recent days. M&amp;amp;s says today that there is still no need for customers to take any action, which may indicate that personal data has not been accessed. The Bank of England is going to test how the City’s crucial financial plumbing would cope with a serious trade war. The Bank revealed today that this year’s test of central counterparties will involve a scenario involving a market panic about a trade war and a sovereign debt crisis. Central Counterparties (CCPs) act as an intermediary between buyers and sellers in financial transactions, and are the counterparty to both sides of the trade. The Bank will kick the tires on three – all three UK authorised CCPs – ICE Clear Europe Limited (ICEU), LCH Limited (LCH), and LME Clear Limited (LMEC). The Bank says: The Stress Test will be centred on a bespoke ‘Baseline Market Stress Scenario’, designed by the Bank. This scenario is an extreme but plausible hypothetical scenario, equivalent to a one in 3,500 event, in terms of where the scenario sits relative to the historic distribution. It is intended to represent extreme market moves over a period of two to five days in which there is escalating concern about fragmentation in global trade and sovereign debt risks. This results in a sharp decline in equity markets, rising interest rate expectations and mixed movements in commodities markets. The 2025 CCP Stress Test will use a reference date of end of day Wednesday 26 March – a week before Donald Trump’s “Liberation Day” tariff announcement, that led to turmoil in the markets…. Soybean prices have hit their highest level in two and a half months, helped by hopes of a de-escalation in the US-China trade war. The most-active soybean contract on the Chicago Board of Trade hit its highest since February 5 at $10.67-1/2 per bushel. Reuters has more details about what’s occuring in the soybean world: U.S. soybeans have not been mentioned so far in Chinese tariff exemptions and China is currently in a period where it mainly buys freshly-harvested Brazilian soybeans. However, moves to defuse trade tensions are seen as positive for U.S. exports beyond this season. Sentiment in the U.S. soybean market has also been boosted by brisk demand from Europe and a report that Japan is considering an increase in soybean imports from the United States as part of tariff negotiations. Just in: Donald Trump has denied that panic in the bond market forced him to temporarily lift his reciprocal tariffs for 90 days. He’s given a big interview to Time Magazine, to mark 100 days of the second Trump presidency, in which he insists that tariffs are necessary. Speaking about the 90-day pause to the ‘Liberation Day’ tariffs, Trump says: “The bond market was getting the yips, but I wasn’t.” Trump added that he would consider it a “total victory” if the U.S. still has tariffs as high as 50% on foreign imports a year from now. [Reminder, Trump announced the 90-day pause on 9 April, a week after announcing a swathe of new tariffs, following wild turbulence in the bond and stock markets] Trump also told Time that China’s President Xi Jinping has called him, and that his Administration is in active talks with the Chinese to strike a deal. He adds: “There’s a number at which they will feel comfortable. But you can’t let them make a trillion dollars on us.” Russia’s central bank has warned that trade conflict could push up domestic inflation, as it voted to leave interest rates on hold. The Bank of Russia fears that the rouble could weaken if oil price fall, or the global economy slows, which would make inports more expensive. After voting to leave interest rates on hold at 21%, the Bank said that the balance of inflation risks is still tilted to the upside in the medium term. It explained: The key proinflationary risks are associated with a longer upward deviation of the Russian economy from a balanced growth path and high inflation expectations, as well as with the deterioration in the terms of external trade. A further decrease in the growth rate of the global economy and oil prices in case of escalating trade tensions may have proinflationary effects through the ruble exchange rate dynamics. This chart from Cornwall Insight shows how its forecast for the price cap change in July has dropped in recent weeks, as wholesale energy prices have weakened. Dr Craig Lowrey , Principal Consultant at Cornwall Insight, strikes a cautious note, though: “While a fall in bills will always be welcomed by households, we mustn’t get ahead of ourselves. We have all seen markets go up as fast as they go down, and the very fact the market dropped so quickly shows how vulnerable it to geopolitical and market shifts. “It would be easy to conclude the fall in the market was due to the United States tariffs, but the reality is that the interactions within and across the energy market are complex - from energy storage requirements in Europe, to warmer weather, to global trade issues – and contribute to the volatility we have seen in recent weeks. “There is unfortunately no guarantee that any fall in prices will be sustained, and there is always the risk of the market rebounding. The only real way to protect households from this constant cycle of instability and insecurity is to reduce our dependence on international wholesale markets. That means continuing to focus on growing low carbon energy generation here in Great Britain and building a more secure, more sustainable energy future.” Energy bills across Great Britian are set to fall this summer, partly thanks to the disruption caused by Donald Trump’s trade war. Consultancy Cornwall Insight has predicted that the quarterly price cap set by regulator Ofgem will fall by almost 9% in July, due to a recent fall in wholesale energy prices. That would cut an average bill by £166 per year, bringing a typical household bill down to £1,683 from July, from £1,849 in April. Cornwall Insight explain: The recent decline in wholesale prices has been driven by a mix of geopolitical and market developments, including the United States’ decision to introduce tariffs – and the broader impact of these – and the impact of above average temperatures, which has reduced demand expectations and eased pressure on short-term prices. While falling prices may appear to be good news, they are also a sign of how volatile the market remains. There are many moving parts, and with the July cap still a month away from being finalised, it is too early to say whether these reductions will hold. The trick in the markets in recent weeks has been to “sell hubris, buy humiliation”, say analysts at Bank of America. They told clients this morning there has been a remarkable flip from “US exceptionalism” hubris to “US repudiation”, with 304 stocks in the S&amp;amp;P 500, and 58 in Nasdaq 100 now trading below their 2021-22 highs. They also point out that while many US stocks are now oversold, Spanish stocks are up 25% year to date in US dollar terms. That shows tht a “reallocation of global capital from US” has begun, “e.g. Latin American capital now heading to Madrid not Miami”. The US was becoming an increasingly important export market for the UK before Donald Trump’s tariffs, according to official figures. Highlighting the stakes in the escalating trade war, the latest snapshot for 2024 from the Office for National Statistics shows the UK exported £59.3bn of goods to the US market last year. Accounting for 16.2% of all of the UK’s goods exports worldwide, the ONS said the US had been growing in importance for British companies as a market to sell cars, pharmaceuticals and other manufactured goods. This is because the proportion of total goods exported to the US has been steadily rising in recent years, up from 13.8% of global exports in 2022. The ONS says this is “indicating that the US may be becoming a relatively more important export partner for the UK.” Machinery and transport equipment is the main export to the US, with shipments worth £29.1bn in 2024 - a £1.8bn (6.7%) increase on the previous year. This was followed by chemicals, worth £10.8bn - accounting for almost a fifth of the UK’s global chemicals exports. The data also show that the UK ran a small trade in goods surplus with the US, as it imported £57.1bn of goods from the United States last year. The details come as the chancellor, Rachel Reeves, is in Washington for the spring meetings of the International Monetary Fund and the World Bank, where she is also aiming to make progress towards a trade deal with US officials to exempt Britain from Trump’s blanket 10% tariff on imports. Cars - subject to 25% US tariffs - were the biggest single category of export, worth £9bn - accounting for 27.4% of all global car exports. This made the US the UK’s number one export partner for cars, with sales worth more than double the second-largest market - China. Exports of iron and steel - also subject to 25% US tariffs - were worth a relatively limited £400m, accounting for 8.4% of total global exports. The UK’s trade in services with the US was worth significantly more than the value of goods. In 2024, the UK imported £61.2bn of services and sold £137bn of services exports to the US - led by areas including research and development, professional and management consulting. American Chamber of Commerce in China president Michael Hart said companies in the pharmaceutical sector had reported that they had been able to import drugs to China in the past week with tariff exemptions, Reuters reports. He said he believed that the exemptions granted by China were drug-specific, not industry wide in nature. Back in China, top policymakers have pledged to support firms and workers most affected by the impact of new US tariffs. The ruling Communist Party’s Politburo held a top-level meeting today, and state media report that officials also reiterated plans to accelerate debt issuance and ease monetary policy. The state media Xinhua reports that president Xi Jinping presided over the meeting. Xinhua says: It was noted at the meeting that the country has seen its economy improve this year, with public confidence continuously boosted and solid progress made in high-quality development. However, the foundation for the country’s sustained economic recovery needs to be further consolidated, and the country faces increasing impact from external shocks, the meeting said. The meeting urged preparing for worst-case scenarios with sufficient planning, and taking concrete steps to do a good job in economic work. The UK stock market is on track to extend its longest winning run since the aftermath of Boris Johnson’s election victory over five years ago. The FTSE 100 has already risen for the last nine trading sessions, as trade war tensions have cooled, which is the best run since December 2019. A 10th rise today would match the “Boris Bounce” rally. Before that, I think you’ve got to look back to December 2016/January 2017, when the FTSE 100 posted a 14-day rally. European stock markets are rising this morning, amid hopes that China is relaxing some of its tariffs. In London, the FTSE 100 index is up 12 points or 0.13%, at 8417 points. Engineering companies are among the top risers, with aerospare manufacturers Melrose up 3.6%, and Rolls-Royce up 2%, after Safran reported that tariffs on aircraft parts have been lifted. Across Europe, Germany’s DAX is up 0.36% while France’s CAC is 0.6% higher. Now this is interesting… The head of French engine maker Safran has said that China has granted exemptions from import tariffs for some aircraft parts including engines. That’s a sign that, as rumoured earlier today, China is taking steps to remove tariffs from some imports. CEO Olivier Andries told reporters on first-quarter results call (via Reuters): “We learned last night that China has taken the decision not to tax engines or landing gear or nacelles - in other words a certain number of aerospace equipment parts.” “It demonstrates that the situation is very fluid.” Advertising group WPP has reported that its clients are waiting to see how the trade conflict unfolds. Mark Read, chief executive officer of WPP, told investors this morning: “While WPP is not itself directly affected by tariffs, they will impact a number of our clients as well as the broader economy. At this point we have not seen any significant change in client spending and we reiterate our full-year guidance which already reflected a challenging environment.” WPP also reported a 0.7% drop in like-for-like revenues in the first quarter of this year, which it says reflects “macroeconomic challenges”. Rachel Reeves used a brief speech to US investors at the British ambassador’s lavish residence in Washington last night, to acknowledge some of the downsides of globalisation, in a nod to Donald Trump’s stance. As she prepares to meet Treasury secretary Scott Bessent today, Reeves said China’s entry into the global trading system 25 years ago had created “huge benefits in terms of cheaper goods, more innovation and more opportunities to trade”. But she said there had also been “many more challenges”, reports our economics editor Heather Stewart. Drawing parallel between the frustrations that drove British voters to back Keir Starmer last July, and those of Trump’s supporters, she said, “in this country, but also back home in my country last year, people voted for change”. She added: “They voted for change because they didn’t think that the economy worked well enough for them and their families. They saw the erosion of good jobs that paid a decent wage. They saw industries that once powered their towns disappear. And as elected politicians we have to respond to that”. Reeves’s host, current British ambassador Lord Peter Mandelson, also highlighted the strong transatlantic relationship in his introductory remarks, with a typically colourful metaphor. Mandelson said: “Some may say that under this very consequential president we have at the moment, this is a rollercoaster period and therefore a challenge to us all. But we would say that a rollercoaster is fine, as long as we are rolling in the right direction.” City economists are encouraged that UK retail sales rose last month. Kris Hamer, director of insight at the British Retail Consortium, credits the warmer weather, which boosted demand for clothing and DIY equipment: “Sales continued to grow in March as the sunshine and warm weather encouraged people to spend more. Clothing and footwear performed well as consumers sought to take advantage of the good weather and prepare for summer. The sunny weather also gave a boost to garden supplies and DIY, as people spent more time outside. Sagar Shah, associate partner at McKinsey &amp;amp; Company, says consumers appear resilient: “Mother’s Day and the spring sunshine saw retail sales rise by 0.4% in March. A positive surprise given that Easter hopped over into April this year – meaning March didn’t benefit from the holiday lift. It also marks the largest three-month rise in sales volumes since July 2021 – a sign there is some underlying resilience in shopper behaviour and the big discounts in the early part of the quarter brought back consumers. Food sales saw a decline of 1.3%, likely due to people eating out and Easter not falling in March. But, we’d expect this to bounce back in April. Conversely, sales volumes in textiles, clothing, and shoes jumped by 3.7%, as people started getting ready for the spring.” However…..there is a wrinkle, as these retail sales are seasonally adjusted to smooth out one-off factors, such as the timing of Easter. Jacqueline Windsor, head of retail at PwC UK, explains: “March’s retail sales should be read with care as the ONS adjusts for the impact of Easter and school holidays falling in April this year. Continuing February’s improving trend, seasonally-adjusted retail sales rose again month-on-month, for the third consecutive month in volume terms. Excluding petrol, retail sales volumes rose by a respectable 3.3%, which translated into 3.8% more pounds in the till compared with this time last year. In the event, the sunniest March since records began particularly helped seasonal fashion retailers, which grew sales volumes on an annual basis for the first time in six months. In fact, all product categories showed positive sales growth, with only grocery retail showing a slight decline in volume terms, no doubt due to the later Easter holidays. The oil price is inching higher today, amid hopes of a de-escalation in US-China trade conflicts. Brent crude, the international benchmark, has risen by 0.5% to $66.86 per barrel. Back in Britain, retail sales grew faster than expected last month – in an encouraging sign for growth this year. Retail sales volumes across Great Britain rose by 0.4% in March, the Office for National Statistics reports, surprising economists who had expected a 0.4% fall. Clothing and outdoor retailers reported that good weather boosted sales, the ONS reports. However, that was partly offset by falls in supermarket sales. March’s growth follows a rise of 0.7% in February (revised down from a first estimate of 1.0%). The broader picture is that retail sales volumes grew by 1.6% rise in the first three months of 2025, comped with October-December 2024. That’s the largest three-monthly rise since July 2021, suggesting consumer spending is holding up quite well this year. The US-China trade conflict is forcing companies to rethink their supply chains. Apple, for example, is reportedly pivoting away from China, which would be a major change to its supply chain. The Financial Times reports this morning that Apple plans to shift the assembly of all US-sold iPhones to India by as soon as the end of 2026. That would mean doubling the iPhone output in India. The FT explains: Apple has in recent years been steadily building capacity in India with contract manufacturers Tata Electronics and Foxconn, though it still assembles most of its smartphones in China. iPhone assembly is the last step in the production process, bringing together hundreds of components for which Apple is still heavily reliant on Chinese suppliers. Stock markets across the Asia-Pacific region are higher today, following those reports that China is considering suspending its 125% tariff on some US imports, Hong Kong’s Hang Seng index has rallied by 1%, as has South Korea’s KOSPI. Japan’s Nikkei index has jumped by 1.8%, while China’s CSI 300 share index is up a more modest 0.2%. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, reports that signs of de-escalation of trade tensions are lifting optimism. Yesterday allowed global risk investors to take a deeper breath. Dovish comments from Federal Reserve (Fed) members, and de-escalation of trade tensions between the US and China allowed a further recovery in global equities. Optimism was backed today by the Chinese announcement that it is considering easing tariffs on some US imports, further signalling de-escalation of trade tensions and supporting earlier comments from the Trump administration that triple-digit tariffs could come ‘substantially’ down. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Hope is swirling this morning that China might relax some of the tariffs it has imposed on US goods as part of Donald Trump’s trade wars. With the economic costs of the tit-for-tat trade war hurting Chinese companies, Beijing appears to be seeking to mitigate the economic fallout from the conflict. According to Bloomberg, this means China’s government is considering suspending its 125% tariff on some US imports – a sign that policymakers are worried about the damage caused by its trade war with Washington. Bloomberg say: Authorities are considering removing the additional levies for medical equipment and some industrial chemicals like ethane, the people said, asking not to be identified discussing private deliberations. Officials are also discussing waiving the tariff for plane leases, the people said. Like many airlines, Chinese carriers don’t own all of their aircraft and pay leasing fees to third-party companies to use some jets — payments that would have become financially ruinous with the additional tariff. This potential easing in the US-China trade conflict comes after Donald Trump revealed yesterday that the world’s two largest economies had held talks to help resolve the trade war. The US president told reporters: “We may reveal it later, but they had meetings this morning, and we’ve been meeting with China.” Reuters is also reporting that China is considering exempting some U.S. imports from its 125% tariffs and is asking businesses to identify goods that could be eligible. A Ministry of Commerce taskforce is collecting lists of items that could be exempted from tariffs and is asking companies to submit their own requests, Reuters adds, citing a source. Signs of de-escalation in the trade war will cheer investors, after a bruising few weeks since Trump announced his tariffs on trading partners. It could also reassure politicians and central bankers around the world, who fear the consequences of a slowdown in world trade. As the Bank of England’s governor, Andrew Bailey, warned on Thursday, the UK economy faces a “growth shock” as a result of Trump’s trade policies. The agenda 7am BST: UK retail sales report for March 9.30am BST: UK trade data for Q4 2024 3pm BST: University of Michigan’s survey of US consumer confidence 3pm BST: IMF holds press conference on the economic outlook for Europe</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>US consumer sentiment has fallen to one of the lowest readings on record. China has denied it is in talks with the US about a trade deal. But there are also signals that Beijing is lifting some tariffs. In London, the FTSE 100 index has posted its longest winning streak in over five years.</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Time for a recap… Anxiety over Donald Trump’s trade wars continues to grip policymakers. The International Monetary Fund has urged global leaders to resolve trade tensions rapidly. Speaking at the IMF’s Spring Meeting in Washington, managing director Kristalina Georgieva said “the first and most urgent priority” is “for countries to work constructively to resolve trade tensions as swiftly as possible, preserving openness and removing uncertainty”. She added: A trade policy settlement among the main players is essential, and we are urging them to do it swiftly, because uncertainty is very costly. Georgieva, who described the mood at the Spring Meeting as “anxious”, also urged Beijing to “pull back from too much intervention”, and rebalance its economy towards more domestic consumption. However, China has instead squashed hopes of an immiment breakthough. Beijing said that the US should “completely cancel all unilateral tariff measures” if it wants trade talks. China also insisted that reports of ongoing US tariff talks were ‘baseless’. He Yadong, a spokesperson for China’s ministry of commerce, said: There are currently no economic and trade negotiations between China and the United States. Any claims about progress in China-US economic and trade negotiations are baseless rumors without factual evidence. In her latest global policy agenda, Georgieva also warned that trade tensions could test the economic and financial stability of individual countries and the world economy, and the resilience of the International Monetary System (IMS). Germany’s government highlighted those risks today, by cutting its growth forecast for this year to zero. Companies are lining up to report the damage from tariffs. Unilever and Nestlé have raised prices for consumers – and indicated further increases could be on the way amid cost inflation and Donald Trump’s tariff war. Pepsico cut its profit guidance for the year, while consumer goods maker Procter &amp;amp; Gamble lowered its sales and profit forecast. In the financial markets, Wall Street is rallying today, but London’s FTSE 100 only closed a little higher. The dollar has dipped against a basket of rival currencies, with Deutsche Bank warning that we could be facing a ‘structural dollar downtrend’. Back in the City, the UK’s blue-chip share index has ended the day pretty much where it started. The FTSE 100 index has closed 4 points higher at 8407 points, up 0.05% today. Although a small gain, that’s the Footsie’s 9th daily rise in a row, as it claws back its losses after the trade war blew up. Bank of England governor Andrew Bailey has said he is focused on the shock to economic growth that is likely to be caused by US president Donald Trump’s import tariffs, and retaliatory measures taken by other countries. Bailey has been speaking to CNBC on the sidelines of the IMF’s Spring Meeting in Washington, where he said: “We are certainly quite focused on the growth shock” Bailey explained that the BoE’s focus had been on balancing weak growth against domestic supply constraints that put upward pressure on inflation, adding: “We’ve got to balance those two. But I think the trade issue is the new part of that story.” He said weak surveys of businesses published earlier this week reflected uncertainty among companies although recent official gross domestic product data had been quite encouraging and he did not think the UK economy was close to a recession. Wall Street is pushing higher. After its early dip, the Dow Jones industrial average is now up 0.5%. The S&amp;amp;P 500 share index is now up 1.2%, while the tech-focused Nasdaq is 1.7% higher. Fox Business’s Charles Gasparino is reporting that people inside the Trump White House are alerting Wall Street executives they are nearing an agreement in principle on trade with India. The proposed deal could include “agreed upon goals” and a deadline for the fully-baked trade pact, according to Gasparino’s sources, and could be used as a template for a deal with Japan, South Korea and Australia. We should be cautious about leaping on encouraging trade rumours from the White House, of course. But also, why are Wall Street big hitters getting early tipoffs?! Germany’s government has given up hopes of growing its economy this year. Germany’s economy is expected to post zero growth in 2025, outgoing Economy Minister Robert Habeck said today, as he laid the blame for this stagnation on Donald Trump’s trade policy. Habeck declared: “The US trade policy of threatening and imposing tariffs has a direct impact on the German economy, which is very export-oriented.” The German government had previously expected growth of 0.3% this year. Its new forecast, of 0% growth, matches the IMF’s new forecast, released on Tuesday. Consumer goods maker Procter &amp;amp; Gamble has cut its sales and profit forecast today, blaming a pullback in consumer behavior as uncertainty over tariffs and the economy hits confidence. P&amp;amp;G now expects flat sales for its current fiscal year after previously projecting growth of as much as four percent. The company also warned that it could be forced to raise prices – passing on the impact of tariffs on imports to its customers. CFO Andre Schulten told reporters on a call: “We will have to pull every lever we have in our arsenal to mitigate the impact of tariffs within our cost structure and P&amp;amp;L [profit and loss statement].” The Bank of England can learn lessons from the Covid-19 crisis about how to communicate issues around uncertainty, according to one of its top policymakers today. BoE deputy governor Claire Lombardelli argues that one of the biggest challenges facing the central bank – and the wider economics profession – is how to talk about economic uncertainty, and communicate with economic decision makers at businesses, households, and across the economy. Speaking at an event organised by the Peterson Institute for International Economics in Washington today, Lombardelli says the Bank is learning a lot of lessons, both from the economics profession and the academic literature, but also from a number of other disciplines. Lombardelli says: So we learnt a lot, for example, during Covid about communication and communication of uncertainty from health professionals and scientists. So I think there’s a real opportunity here for us to take those rigorous tools of economics and use them in a policy-making context that recognizes the uncertainty that we’re all trying to navigate through and helps economic agents navigate that uncertainty too. It’s a muted start to trading on Wall Street today. The Dow Jones industrial average has dropped by 0.4%, down 168 points to 39,437 points. It’s being dragged down by IBM, whose shares are down 8.5% after missing expectations with its latest financial results. But the broader S&amp;amp;P 500 index is up 0.24% at 5,388 points, up 12 points. Happily, trade war tensions have not led to a big increase in layoffs at US companies. The number of new claims for unemployment support rose by 6,000 last week to 222,000, new data shows, still a relatively low level. Q: What has been the mood of IMF members at this week’s Spring meeting? They are “anxious”, Kristalina Georgieva replies soberly, explaining: The membership is anxious because we were just about to step on the road to more stability after multiple shocks. Actually, she adds, the Fund had been worried that its forecast of 3.3% global growth this year was not high enough – before the Trump trade war forced it to cut that forecast eralier this week. Georgieva adds that IMF members are also recognizing the importance of “a rule based global economy” in which both government and the private sector can plan with some certainty. Turning to Argentina, Kristalina Georgieva says that the country has demonstrated that “this time it is different”, with a “decisiveness” to put the economy on a sound track. She cites falls in inflation, and a drop in poverty levels from over 50% to around 27% now. Georgieva says: It [poverty] is still very high, but going down. The state is stepping out from where it doesn’t belong, to allow more dynamism in the private sector. That’s quite an endorsement of Javier Milei’s harsh austerity measures, in which public spending was slashed in a “chainsaw” campaign of fiscal balance and deregulation. Asked about the outlook for Africa, Kristalina Georgieva says the continent has “so much to offer the world”. She explains: Obviously, they have the leaders, the natural resources, a young population. I think a more unified, more collaborative continent can go a long, long way to be an economic powerhouse. IMF chief Georgieva is then quizzed on why the Fund doesn’t believe the US will fall into a recession this year. Grabbing a bottle of Perrier, she fills her glass more than half-way up – to illustrate that the Fund sees a less than 40% risk of recession in America this year. She explains: My glass, when you look at it, it is more than 60% full. Well, that’s this is where we are. This is what it is. How can I call it empty? I can’t. When we look at the data, what we see is that for the United States, recession risks have increased now to 37%. We don’t see either in the labor market or indicators for the functions of the economy such a dramatic loss of economic activity that will push growth in United States all the way to below zero. Kristalina Georgieva also touches on yesterday’s stinging attack on the IMF by US Treasury secretary Scott Bessant. She says the Fund “greatly value” the voice of the US, who are its largest shareholder. During his speech yesterday, Bessent accused the IMF and World Bank of “mission creep”, and called on them to stop their “sprawling and unfocused agendas” on issues such as climate change and gender. Georgieva seems keen to sooth the US, saying she very much appreciated that Bessent reiterated the US’s commitment to the fund and to its role, saying: He raised a number of important issues and priorities for the institution that I look forward to discussing with us, authorities and the membership as a whole. Central bank independence is “critical” for their credibility, Kristalina Georgieva adds. She says central banks must strike a balance between supporting growth and containing inflation. To do so, they must not only adjust policy interest rates, but also rely on their credibility to anchor expectations, she points out. IMF chief Kristalina Georgieva is urging global leaders to resolve trade tensions rapidly. Speaking at a press conference to discuss her Global Policy Agenda, Georgieva warns that the world economy is facing “a new and major test”, at a time where its policy buffers are depleted after the shocks of recent years. That puts countries in a difficult position, Georgieva says, and also creates “urgency for action”. She says there are three “overarching priorities”, starting with ending the trade war that Donald Trump ignited this year. Georgieva says: First and most urgent [is] for countries to work constructively to resolve trade tensions as swiftly as possible, preserving openness and removing uncertainty. A trade policy settlement among the main players is essential, and we are urging them to do it swiftly, because uncertainty is very costly. Georgieva explains that businesses cannot invest if they do not have certainty, while households will save rather than spend. But in a nod of support to the White House, Georgieva says countries also need to address the imbalances that are fuelling today’s trade tensions. Some countries, like China, need to boost private consumption and embrace a shift to services. Others, like United States, need to reduce their fiscal deficit, she explains. Europe needs to complete the single market, banking union, capital market union, and remove internal barriers to intra EU trade, insists Georgieva (a former European commissioner herself). And all countries should seize this moment to lower their trade barriers, both tariff and non tariff, she added. Newsflash: the head of the International Monetary Fund is warning that trade war tensions could rock the stability of the world economy, and the International Monetary System. IMF managing director Kristalina Georgieva is releasing her latest global policy agenda now, which is aimed towards “anchoring stability and promoting balanced growth”. In it, Georgieva cautions that the economic landscape is “rapidly changing”, due to the US trade war, saying: Trade tensions have soared following the tariff announcements by the U.S. and responses to them, fueling a high level of uncertainty and market volatility, and threatening to stymie trade. These were in part driven by concerns about the uneven distribution of gains from economic integration, its impact on the international division of labor, supply chain security, and global imbalances. These trade tensions could test the economic and financial stability of individual countries and the world economy, and the resilience of the International Monetary System (IMS). The IMS is currently based around the idea that the US dollar is the global reserve currency, with the IMF sitting at the centre, and central banks around the world holding the system together. Over in Washington, UK chancellor Rachel Reeves is being interviewed by cable news channel Newsmax. She reiterating her confidence that a UK-US trade deal can be agreed. Update: Reeves told Newsmax: “We don’t always agree with the policy prescriptions and we’re seeking a deal that reduces the trade barriers between our countries.. “But I am confident that a deal can be done, that our strong relationship when it comes to defense, when it comes to security and when it comes to the economy and prosperity, means that we can strike a deal. Just in: Soft drinks and snacks group PepsiCo has abandoned hopes of growing its earnings this year, as new tariffs drive up its costs. In its latest financial results, PepsiCo told shareholders is now expects its core earnings per share to be “approximately even” this year, compared with 2024. It had previously expected mid-single-digit growth. Chairman and CEO Ramon Laguarta says PepsiCo are actively planning mitigation actions to address higher supply chain costs. Laguarta explains: “Our businesses remained resilient in the midst of increasingly dynamic and complex geopolitical and macroeconomic conditions in the first quarter. As we look ahead, we expect more volatility and uncertainty, particularly related to global trade developments, which we expect will increase our supply chain costs. At the same time, consumer conditions in many markets remain subdued and similarly have an uncertain outlook.” UK companies have been hit by a drop in export orders this month, as the Trump tariffs depress global trade. The CBI’s latest monthly balance for export orders sank to -41 this month from -29 in March. That’s the weakest since December 2020 with the exception of November 2024, and shows that more companies reported a drop in export orders. Ben Jones, lead economist at the CBI, says: “The recent downturn in manufacturing output appears to have eased, but manufacturers still seem gloomy about their prospects amid rising costs, an expected decline in new orders and heighted uncertainty around global economic conditions. “The combination of financial pressures, market instability and falling confidence is leading manufacturers to cut back employment and investment, with plans for spending on buildings, equipment, innovation and training all taking a hit. “The wider geopolitical environment is becoming increasingly challenging for exporters, with export optimism falling sharply for a second successive quarter and export order volumes now hovering around post-pandemic lows. “The government is right to make the case for global free trade, with the Chancellor in Washington this week at the IMF spring meeting reaffirming that commitment. The uncertainty around global economic conditions only increases the importance of getting it right in domestic economic policy. Wall Street is on track to drop when trading resumes in New York. The Dow Jones industrial average is expected to drop by 0.7%, or around 250 points, according to the futures markets. Similar-sized losses are expected on the S&amp;amp;P 500 and the Nasdaq. There’s anxiety after Donald Trump indicated last night that his administration could reimpose tariffs it paused on 9 April within “the next two, three weeks” if countries haven’t struck a deal – rather than maintaining the current 90-day pause. Speaking at the White House, the US president said: “In the end, I think what’s going to happen is, we’re going to have a great deals, and by the way, if we don’t have a deal with a company or a country, we’re going to set the tariff. I’d say over the next couple of weeks, wouldn’t you say? I think so. Over the next two, three weeks.” Our US Politics Live blog has full details: China has picked up the olive branch proffered by Donald Trump earlier this week, and bashed the US president with it. He Yadong, the Chinese Ministry of Commerce’s spokesman, has told reporters today that the US should revoke all the unilateral tariffs recently imposed, and also insisted there has not been any progress towards a trade deal. He told a press briefing: “The US should respond to rational voices in the international community and within its own borders and thoroughly remove all unilateral tariffs imposed on China, if it really wants to solve the problem.” Reminder: on Tuesday, Trump said high tariffs on goods from China will “come down substantially. He, though, has dismissed speculation that progress has been made in bilateral communications, saying “any reports on development in talks are groundless.” The US dollar is weakening today, down around 0.5% against a basket of currencies, wiping out some of yesterday’s gains. The euro has climbed 0.7% to $1.1383, towards the three-year highs of $1.15 set at the start of this week. Deutsche Bank has revamped its medium-term FX forecasts yesterday, and are now predicting a “structural dollar downtrend.” George Saravelos, global head of FX research at Deutsche Bank, gives a four-point explaination: What has changed since the start of the year? The list of superlatives is long – the largest shift in US trade policy in a century; the biggest pivot in German fiscal policy since re-unification; the most significant reassessment of US geopolitical leadership since World War II, to name a few. Our view on all these factors is that the pre-conditions are now in place for the beginning of a major dollar downtrend. Our forecasts foresee the end of a “higher for longer” dollar with EUR/USD appreciating closer to purchasing power parity of 1.30 over the remainder of the decade. At the core of the dollar bear market are three assessments: a reduced desire by the rest of the world to fund growing twin deficits in the US; by extension, a peak and gradual unwind in elevated US asset holdings ; and a greater willingness to deploy domestic fiscal space to support growth and consumption outside of the US. In a world of extreme uncertainty and rapidly shifting policy norms, the risk of market dislocations and regime breaks remains high. The stock market turmoil triggered by Donald Trump’s tariff announcements also hurt the world’s largest sovereign wealth fund. Norway’s wealth fund posted a near-$40bn loss for the first quarter of this year, a return of -0.6% (or -415bn kroner), caused by losses on its tech stock investements. The fund’s manager, Nicolai Tangen, said the quarter has been characterized by “large fluctuations in the market”, adding: Equity investments yielded negative returns, and it was mainly technology stocks that dragged down the result. Growth across the eurozone is likely to peter out in the second half of this year, Goldman Schs has predicted. Goldman analysts say they expect euro area growth to slow further, with flat GDP in the second half of 2025, telling clients: First, the ongoing trade tensions are likely to weigh materially on activity via weaker net trade and investment, despite President Trump’s 90-day pause on the country-specific reciprocal tariffs. Second, we expect weaker global growth to weigh on exports, given recent downgrades by our US and China teams. Third, financial conditions—with our Euro area FCI [financial conditions index] 50bp tighter since early March—point to a building headwind. Goldman predict eurozone growth of 0.7% in 2025 and 1% in 2026, which they add is “notably” below consensus, the ECB March staff projections and the latest IMF forecasts. Donald Trump’s tariffs will make it harder for Sir Jim Ratcliffe’s car division, Ineos Automotive, to reach its first profit. Ineos Automotive’s CEO, Lynn Calder, told Bloomberg that the US president’s 25% tariff on foreign cars will make it harder to hit the earnings target. Calder said: “For sure, this last week has put a dent in that and, for sure, delayed it,” Calder insisted, though, that Ratcliffe is still “absolutely, 100%” committed to cars, adding: “We’re stubborn as mules. We’re not easy to knock down.” The threat of a US trade war has driven UK consumer confidence down to its lowest level on record, the British Retail Consortium reports today. Its latest healthcheck on shoppers found that people were much more negative about the state of the UK economy, and of their own financial situation. The survey was conducted between the 4th and the 7th April, which covers the period immediately after Donald Trump announced new tariffs on US trading partners. It rather bolsters Andrew Bailey’s warning that the US trade war will hurt UK growth (see opening post). Helen Dickinson, chief executive of the British Retail Consortium, says: “With fieldwork completed just days after Donald Trump’s “Liberation Day” tariffs, it is unsurprising that consumer expectations for the economy plummeted to a record low. The original tariff schedule, since reduced for most countries, was expected to reduce growth in the UK and elsewhere. Yet despite this economic pessimism, expectations of retail spending rose slightly as the prospect of Easter shopping drew closer. Here’s the details: The state of the economy dropped significantly to -48 in April, down from -35 in March. Their personal financial situation worsened to -16 in April, down from -10 in March. Their personal spending on retail rose to +3 in April, up from 0 in March. Their personal spending overall fell slightly to +10 in April, down from +11 in March. Their personal saving rose slightly to -4 in April, up from -5 in March. The survey does not catch the reaction to Trump’s decision on 9 April to pause most tariffs for 90 days. Dickinson warns, though, that confidence is still weak despite that u-turn: “Even with a pause on many of the US tariffs, business and consumer confidence remains fragile. The risk of higher global prices is an unwanted addition to the £7bn in new costs hitting retailers this year from higher employer National Insurance, increased NLW, and a new packaging tax. Many retailers are also concerned about the risk of cheap Chinese products being diverted from the US to other destinations, including the UK. The London stock market has opened to little fanfare. After rallying yesterday to a near three-week high, the FTSE 100 has risen by just 2 points (or 0.03%) to 8405 points. UK brokerage AJ Bell has benefitted from recent market turbulence. It reports that there has been increased trading activity in April as customers respond to “changing market dynamics”, typically by snapping up shares whose values fell. AJ Bell told the City: The long-term investment outlook among customers is illustrated by the fact more than three-quarters of these trades were buys with the net investment totalling more than £300 million. Several UK-listed companies are telling investors this morning that they don’t expect major damage from the US’s new trade war. Unilever, the consumer goods giant, told the City that it expects a “limited and manageable” hit to its earnings from tariffs. Unilever, which owns Marmite, Dove and several ice cream brands, said it was sticking to its targets for 2025, but added: The direct impact of tariffs on our profitability is expected to be limited and manageable. All this being said, we are conscious that the macroeconomic environment, currency stability and consumer sentiment remain uncertain and we will be agile in adjusting our plans as necessary. Pizza maker Domino’s told shareholders that its initial assessment of newly introduced tariffs shows “minimal direct impact”, adding: We continue to assess any indirect impacts on our supply chain, monitor the broader environment going forward and our full year expectations remain unchanged.” Engineering firm Senior, which makes high technology components and systems, is taking a similar line. It told investors this morning: The direct impact of announced tariffs is limited and manageable. We remain mindful of the potential broader macroeconomic impact on the market sectors in which we operate and will continue to monitor the situation and respond appropriately. There are signs that some investors are looking to move money out of US assets and into Europe instead, fund manager Jupiter says this morning. Jupiter told shareholders that there was “elevated market volatility” across asset classes in April “as a result of trade policies” (a reference to the crash, and partial rebound, after Trump’s ‘Liberation Day’ tariff announcement). Jupiter says this will “undoubtedly have an impact on client risk appetite”, adding: We also see early-stage evidence of asset owners and other investors looking to reallocate away from the US and towards other markets, such as the UK, Europe and Asia Pacific. Volatility isn’t all bad, though – Jupiter reckon mispriced assets present an opportunity for active asset managers. It also reported a £1bn drop in assets under management in the last quarter, to £44.3bn, driven by net outflows of £500m and negative market movements of £500m. Donald Trump’s tariff flip-flopping is continuing this week, with reports that the US president is planning to spare carmakers from some of his most onerous tariffs. According to the Financial Times, the US is now planning to exempt car parts from the tariffs that Trump is imposing on imports from China to counter its role in fentanyl chemical exports, as well from those levied on steel and aluminium The u-turn comes after intense lobbying by industry executives over recent weeks, who have been warning the White House about the damage that tariffs will cause But it won’t spare the car industry completely from Trump’s trade war. As the FT explains: The exemptions would leave in place a 25 per cent tariff Trump imposed on all imports of foreign-made cars. A separate 25 per cent levy on parts would also remain and is due to take effect from May 3. More here (£). ACEA’s latest European car sales report shows a continued decline in demand for fossil fuel-powered vehicles. While new battery-electric car sales grew by 23.9% in the first three months of 2025, to 412,997 units, petrol car registrations saw a significant decline of 20.6%, with all major markets showing decreases. France experienced the steepest drop, ACEA reports, with petrol registrations plummeting by 34.1%, followed by Germany (-26.6%), Italy (-15.8%), and Spain (-9.5%). The diesel car market declined by 27.1%. Tesla’s share of the European car market has dropped again, following protests against the car maker’s CEO, Elon Musk. Tesla’s market share in the European Union, the UK and the EFTA trade zone (Iceland, Liechtenstein, Norway, and Switzerland) fell to 2% in March, down from 2.9% in March 2024. Total sales in the month fell to 28,502, down from 39,684 a year ago, new data from the European Automobile Manufacturers’ Association (ACEA) this morning show. During 2025 so far, Tesla’s market share in the EU/UK/EFTA has dropped to 1.6%, from 2.5% in January-March 2024. Its sales are down 37%, to 54,020 from 86,027 in Q1 2024. That’s despite a near-24% increase in overall battery-electric car sales in Europe so far this year. Overall, car sales across Europe dipped by 0.2% in March, and are down 1.9% so far this year. Earlier this week, Tesla reported a sharp tumble in profits and revenues in the first quarter of 2025 amid a backlash against his role in the Trump White House, where he has been driving cutbacks to federal services. Protests against Musk, and Tesla, have been taking place in the US and across Europe in recent weeks, prompting reports of a European consumer backlash by some Tesla owners and prospective buyers. Tesla’s recent sales decline has also been blamed on its ageing lineup of models (its Model Y has just been updated) and intense competition from rivals such as China’s BYD, as well as the backlash from Musk’s embrace of rightwing politics. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Fears are mounting that Donald Trump’s trade war will hurt the UK economy, even as the US president backtracks over some of his tougher measures. Even though Britain is getting off relatively lightly with a 10% tariff, new trade disruption is likely to damage economic growth. Andrew Bailey, the governor of the Bank of England, sounded the alarm in Washington last night, where the International Monetary Fund’s Spring Meeting is taking place. Bailey told an Institute of International Finance event that the UK’s open economy was vulnerable to a global trade war. Bailey explained: “It’s not just the relationship between the US and the UK, it’s the relationship between the US, the UK and the rest of the world that matters so because the UK is such an open economy. “We have to take very seriously the risk to growth. I’ve said a number of times, fragmenting the world economy will be bad for growth.” The Bank will release its latest economic forecasts in two weeks, when it is widely expected to cut UK interest rates. Earlier this week the IMF cut its forecast for UK growth this year to 1.1%, down from 1.6% predicted in January The UK government has been pushing for a trade deal with the US. But on Wednesday, chancellor Rachel Reeves dashed hopes of an early breakthrough in negotiations, stressing that the UK is “not going to rush” into a deal. Financial markets rallied yesterday after Trump said his tariffs on China would come down “substantially”, but not to zero. These hints that the US might de-escalate tensions with Beijing are lifting the “mood music” in the markets, reports Michael Brown, senior research strategist at brokerage Pepperstone. Brown adds: Isn’t it remarkable how the ‘Art of the Deal’ appears to simply be for Trump to negotiate with himself (aka fold like a cheap suit), then to end up jumping around claiming a ‘win’ anyway. The agenda 9am BST: IFO survey of Germany’s business climate 11am BST: CBI’s industrial trends survey of UK manufacturing 1pm BST: IMF to release Global Policy Agenda report 1.30pm BST: US weekly jobless claims data 1.30pm BST: US durable goods orders</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>The International Monetary Fund has urged global leaders to resolve trade tensions rapidly. IMF managing director Kristalina Georgieva said ‘the first and most urgent priority’ is “for countries to work constructively to resolvetrade tensions as swiftly as possible” China has instead squashed hopes of an immiment breakthough. Beijing said that the US should “completely cancel all unilateral tariff measures” if it wants trade talks.</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>The global financial system is coming under increasing strain as Donald Trump’s trade war rocks markets, the International Monetary Fund has warned. “Global financial stability risks have increased significantly,” the IMF said in its regular snapshot of the system, urging regulators to be on the alert for potential crises. It pointed to the “sharp repricing of risk assets” that has followed the US president’s tariff announcements since February – in particular his 2 April “liberation day” statement – and warned that there may be more to come. Published as finance ministers and central bankers gather in Washington for the IMF’s spring meetings – and as the IMF downgraded its forecasts for global growth amid tariff concerns – the Global Financial Stability Report identified what it called “forward-looking vulnerabilities” in markets. These include what it said were overstretched valuations for stocks and bonds in some areas, even after recent sell-offs; the highly leveraged state of some financial institutions, including hedge funds; and the vulnerability of some governments to volatility in sovereign bond markets. The IMF also warned economic policy and trade uncertainty were at an all-time high, “foreboding further shocks, corrections of asset prices, and tightening of financial conditions”. Governments in emerging economies could be hit especially hard by sudden increases in borrowing costs, the IMF warned, suggesting “investor concerns about public debt sustainability and other fragilities in the financial sector can worsen in a mutually reinforcing fashion”. Meanwhile, companies may find it more expensive to borrow, if volatile corporate bond markets drive up the cost of debt, it suggested – while households will be hit via “wealth effects”, if the value of their pensions and other investments continues to slide. The Washington-based lender expressed particular concern about the growing role of “nonbank” lenders, which are much less heavily regulated than banks, but can still pose risks to the wider financial system. The role of these lenders, which include pension and investment funds, has grown rapidly in recent years, after rules on banks were toughened up after the 2008 global financial crisis. The IMF warned of a “deepening nexus” between these nonbank lenders and traditional banks. It suggested they could be forced to divulge more information to regulators, which could then identify and rein in “poorly governed and excessive risk-taking institutions”. High levels of borrowing by these nonbank lenders also “imperils market functioning”, the IMF said, noting these investors had amplified a recent sell-off in US government bonds due to pressure to meet margin calls. This is when an investor must provide collateral to cover losses quickly. Borrowing by hedge funds could also “exacerbate losses” during periods of market turmoil, the IMF said. At the hedge funds that make big macroeconomic bets, leverage can be as high as 40 times the value of their assets, the report found. The institution also suggested big global banks could be underestimating the “true level of risk” attached to their business. Banks use the “average risk-weight”, or “RWA density”, as a metric to reflect the level of risk connected to its business. However, the IMF found that data from international banks, even those with similar models and overall risk profiles, showed “wide variation” by this measure. The IMF also urged governments to ensure there is sufficient capital and liquidity in the banking system to cope with a crisis – including by the “full, timely and consistent implementation” of the so-called Basel 3 rules, devised after the 2008 crisis. The Bank of England recently delayed the implementation of the final stage of these rules, known as Basel 3.1, by a year in the UK, as the chancellor, Rachel Reeves, pressed regulators to take a more pro-growth approach. The report also flagged potential contagion risk in the private credit fund system, which it said could “spread credit shocks across institutions and countries”. More companies are borrowing from private credit funds, it said, and big investors such as pension funds are increasingly backing foreign direct-lending funds. As the market becomes more complex and global, “the risk that credit shocks will propagate from one jurisdiction to others intensifies”, the report said. Separately on Tuesday, a member of the Bank’s rate-setting panel, Megan Greene, said US trade tariffs were more likely to push down UK inflation than to drive it up, but that there were risks on both sides. Greene told Bloomberg: “The tariffs represent more of a disinflationary risk than an inflationary risk.” However, she added: “There’s a ton of uncertainty around this, but there are both inflationary and disinflationary forces.” On Monday, Trump renewed his attack against the Federal Reserve chair, Jerome Powell, and the independence of the US central bank. Greene said that “credibility is the currency of central banks and I think independence is quite an important piece of that”. She said the Bank could credibly try to hit its targets because it was free to make its own decisions.</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>International Monetary Fund warns of 'sharp repricing' of risk assets. Warns of 'deepening nexus' between nonbank lenders and traditional banks. IMF downgrades forecasts for global growth amid tariff concerns.</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Keir Starmer and Rachel Reeves have underlined how much the world has changed after Donald Trump’s “liberation day”, with the UK prime minister even declaring an end to globalisation. But as the chancellor prepares to fly to Washington this week to meet her global counterparts at the International Monetary Fund meetings, Labour appears to see the risks purely in terms of the hit to international trade. While frantically negotiating with Washington over tariffs, the government is pressing ahead with plans to deregulate the City – just as global financial stability appears threatened by the chaos unleashed by the White House. Labour has taken a muscular approach to saving the steelworks in Scunthorpe, and Reeves has written of the need for a “strong, smart and agile state to support key industries”. Yet Labour’s stance on the UK’s highly globalised financial sector appears to remain the one set out in the chancellor’s Mansion House speech in November: that rules imposed after the 2008 crash have “gone too far”. The governor of the Bank of England, Andrew Bailey, appeared to raise a metaphorical eyebrow at that suggestion a couple of months later, when he used a speech to warn: “Memories disappear in the rear-view mirror. And those of us who lived through it, worked through it and had to deal with it, are left saying: ‘Just remember what we had to deal with.’” So far, little has changed, aside from regulators being hauled in repeatedly to explain themselves to the chancellor, and new remits issued, including to the Financial Conduct Authority, urging them to target growth. But Labour gives the sense of being intensely relaxed with the big beasts of high finance. Hosting the US investment company BlackRock’s chief executive, Larry Fink, in Downing Street last autumn, Starmer tweeted: “I’m determined to deliver growth, create wealth and put more money in people’s pockets. This can only be achieved by working in partnership with leading businesses, like BlackRock.” An edgy calm was restored to financial markets on both sides of the Atlantic last week, after a wrenching sell-off in US government debt prompted Trump to pause his “reciprocal” tariffs on 9 April. But the anxiety unleashed by wild moves in the market for Treasuries – US government debt – underlined the risks that Trump’s policy will not only reorder trade flows but could put global financial stability at risk. Trump’s open flirtation with trying to remove the Federal Reserve chair, Jerome Powell, is unlikely to help. Treasury yields are the benchmark against which interest rates across the world’s markets are priced; and the safe-as-houses collateral for a kaleidoscope of risky bets. If investors really are reassessing Treasuries’ value, as some analysts have suggested – because of what in an emerging economy would be called “political risk” – the consequences could rapidly be transmitted throughout the global economy. Such a shock would come at a time when global debt levels stand at more than three times GDP, according to the Washington-based Institute of International Finance – far higher than in the run-up to the 2008 crash. These include the hefty debts run up by governments as they stepped in to cushion their citizens from the worst effects of the Covid pandemic, but also household borrowing and the loans piled on to companies bought by the rampaging private equity sector. Much of this borrowing has not been issued by banks, which have been hemmed in more cautiously with regulation since the crisis – but by other, less-regulated “private” lenders. As a recent British Private Equity &amp;amp; Venture Capital Association (BVCA) update put it: “The global financial crisis was the catalyst for growth, as banks adopted more conservative lending practices and deleveraged their balance sheets.” And since the UK remains a leading global financial centre, this barely regulated, non-bank lending has exploded here – with fund managers holding $257.9bn (£194.7bn) of “private debt” by the end of 2023, according to the BVCA: a staggering sum, which it pointed out amounted to 64% of the European total. The Bank of England has been working hard to track how players in this shadow banking sector might respond in the event of a crisis – including by carrying out a fearsomely complex choose-your-own-adventure exercise it calls the “system-wide exploratory scenario”, launched after the Liz Truss market scare. Its results underlined how a fiendish spider’s web of financial interconnections could amplify a potential shock. The Bank, which keeps a much closer eye on financial stability these days, is confident it has the tools to respond, but the complexity of the system is reminiscent of the little-understood dependencies that bound the global financial system together before the 2008 crisis. Despite the size of the UK’s finance sector, it has not tended to generate a wall of cash flooding towards key national investment priorities, or growing UK businesses, which often complain they struggle to find funding. Labour are taking measures to encourage private sector investment into green projects and much-needed infrastructure – by consolidating pension funds, and through the new national wealth fund, for example. Yet this more activist approach sits alongside an intention to cut back regulation rather than, say, bring shadow banking under firmer control (aside from buy now, pay later lending, where Labour have rightly pressed ahead with Tory plans to regulate – although not until 2026). Starmer and Reeves are right to rethink globalisation. But they would be wise to remember that it is not only steelworkers in Scunthorpe who are exposed to its unforgiving forces. If a crisis hits the hyperglobalised financial system – which includes the private equity companies that have gleefully gobbled up care homes and nurseries across the UK – we are all at risk.</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Labour has taken a muscular approach to saving the steelworks in Scunthorpe. But the government is pressing ahead with plans to deregulate the City. Global financial stability appears threatened by the chaos unleashed by the White House.</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Time for a recap. Global financial markets are on edge as investors await Donald Trump’s widely-trailed announcement on new tariffs on America’s trading partners. White House aides have reportedly drafted plans for 20% tariffs on most goods imported to the United States, which would have a significant negative impact on global trade. A new report has shown that if Trump imposed 25% tariffs, triggering retaliatory action, up to $1.4rn could cause a $1.4tn hit to the world economy. Jun Du, a professor of economics at Aston University who co-wrote the report, said this would have similar effects to the 1930 trade war that deepened the Great Depression. “These findings align with historical precedents like the Smoot-Hawley tariffs and modern trade conflicts, illustrating how protectionism erodes competitiveness, disrupts supply chains, and imposes disproportionate costs on consumers.” The UK government is expecting to be hit by new tariffs tomorrow. Business secretary Jonathan Reynolds told the BBC: “It appears tomorrow there’ll be no country in the world exempt from the initial announcements”. Reynolds has also denied that the issue of free speech has featured in tariff negotiations: The UK is also hoping that it can reach a deal with the US eventually to avoid Trump’s new tariffs. But even if that happens, Britain’s economy could still be hit by the shockwaves of a global trade war. Goldman Sachs has trimmed its forecast for UK growth this year and in 2026. The head of the European Commission, Ursula von der Leyen, has said the EU has a “strong plan” to retaliate against tariffs imposed by Donald Trump but would prefer to negotiate. Europe’s financal markets have closed higher tonight… …while gold hit a record high in early trading. Uncertainty over tariffs has hit factory output in the UK, new data shows, and in the US. Across Europe, stock market trading has ended for the day, with shares higher as investors await tomorrow’s announcement from Donald Trump on tariffs. In London, the FTSE 100 share index has closed 52 points higher at 8634 points, up 0.6% today. Germany’s DAX was up almost 1.7% at the closing bell, while Frances’s CAC was 1% higher. Traders are weighing up whether this is a buy the dip opportunity or part of a longer standing period of uncertainty that will weigh on stocks, reports Joshua Mahony, analyst at Scope Markets. Mahony adds: While countries such as the UK might stand in a good position to strike a deal, there is a risk that tomorrow marks the beginning of a tit-for-tat trade war that brings yet more uncertainty and concern for markets. The expected retaliation from Canada, the eurozone, China, Japan, and Korea does signal that it could get worse before it gets better. The slowdown in production at American factories last month (see earlier post) shows that tariffs are failing to give US manufacturing a lift, reports ING. They told clients: Today’s US data are in general softer than hoped. The ISM manufacturing index for March dropped to 49.0 from 50.3, lower than the 49.5 consensus and back in contraction territory. This is broadly in line with regional manufacturing indicators released in recent days. The details show big drops in employment (44.7 from 47.6) and new orders (45.2 from 48.6) with production down at 48.3 versus 50.7. Remember 50 is the break-even level so anything above is expansion and the further below 50 the deeper the downturn. This suggests that tariff fears (impact on supply chains and potential reciprocal action from foreign trading partners) are hurting the sector right now. Note too the big rise in prices paid to 69.4 from 62.4, which suggests pre-emptive moves ahead of the imposition of tariffs with the threat of higher prices for consumers looking very real. Below is a chart of manufacturing production growth (YoY%) versus the ISM production index. This underscores how the stagnation in the sector over recent years looks set to continue despite tariffs supposedly being a tool to reinvigorate manufacturing. After 90 minutes trading on Wall Street, the S&amp;amp;P 500 has recovered its early dip and is now flat. Investors are bracing for Donald Trump’s announcement on tariffs, expected at 4pm3pm in Washington DC tomorrow (9pm8pm BST). “Investors are on the sidelines because it’s impossible to get any kind of clear compass reading on the direction of the economy until these tariffs are finalized,” said Peter Andersen, founder of Andersen Capital Management. “The market is going to sway back and forth, but with a bias to the negative side, because this is making it very difficult for CEOs of companies to make any kind of estimates.” Production at US factories declined last month as order book growth slowed due to tariff uncertainty, new data shows. The latest healthcheck on American manufacturing shows that growth stalled in March. with production falling and order books only expanding modestly. S&amp;amp;P Global’s poll of purchasing managers also found that confidence in the outlook for business activity “softened”, amid “some uncertainty over the impact of federal government policies”. This pulled S&amp;amp;P Global’s US Manufacturing PMI down to 50.2 in March, down from 52.7 in February, only just above the level showing stagnation. Manufacturers are worried that trade tensions will lead to lower orders, explainsChris Williamson, chief business economist at S&amp;amp;P Global Market Intelligence: “The strong start to the year for US manufacturers has faltered in March. A combination of improved optimism surrounding the new administration and the need to front-run tariffs had buoyed the goods-producing sector in the first two months of the year, but cracks are now starting to appear. Production fell for the first time in three months in March, and order books are becoming increasingly depleted. While business confidence about the outlook remains relatively elevated by standards seen over the past three years, this is based on companies hoping that the nearterm disruption caused by tariffs and other policies will be superseded as longer-term benefits from the policies of the new administration accrue. However, March has seen more producers question this belief. Business optimism about the year ahead has deteriorated further from January’s near threeyear high, and has dropped sharply over the past two months, causing firms to stop raising payroll counts for the first time since October. A key concern among manufacturers is the degree to which heightened uncertainty resulting from government policy changes, notably in relation to tariffs, causes customers to cancel or delay spending, and the extent to which costs are rising and supply chains deteriorating in this environment. Tariffs were the most cited cause of factory input costs rising in March, and at a rate not seen since mid-2022 during the pandemic-related supply shock. Supply chains are also suffering to a degree not seen since October 2022 as delivery delays become more widespread. European countries will be presenting themselves as safe havens for investors in the wake of a tariff war that is already spooking the stock markets, my colleague Lisa O’Carroll reports from Dublin. “On the eve of such a significant day in the history of the world,” Ireland’s finance minister has said there were three potential brighter spots people across the EU should remember including record employment levels and political and economic stability compared to the US. “I do think investors at the moment are re evaluating the EU and investing in the European Union, I think there’s a growing appreciation of the value of predictability and order on the global stage,” Paschal Donohoe told reporters on Tuesday. Donohoe, who is also president of the Eurogroup of finance ministers in countries using the euro, said the EU will act calmly in the event of “an economic shock” but warned there could be a slow down in Ireland’s growth. “We are in an atmosphere of high uncertainty”. So far this year, the pan-European Stoxx 600 index has gained 6%, while the US S&amp;amp;P 500 index has lost 5%. Experts have been warning today that tomorrow’s tariffs announcement could lead to increased job cuts in the UK. Matt Swannell, chief economic advisor to the EY Item Club, said: “US tariffs on goods imports from the UK could rise tomorrow, with survey respondents indicating that the possibility of higher tariffs is already weighing on demand for exported goods.” He said the prospect of tariffs, coupled with weak domestic demand, is “seeing the sector cut jobs”. Myron Jobson, senior personal finance analyst for Interactive Investor, has warned that the UK will be affected by the trade war, even if it manages to dodge direct tariffs: “President Donald Trump’s tariffs war could have far-reaching consequences for Britons, even if the UK manages to escape direct levies. “If tariffs contribute to higher inflation, central banks may be forced to tighten monetary policy, which can weigh on bonds and borrowing costs. “This could impact everything from mortgage rates to corporate investment, potentially slowing economic growth. “For investors with exposure to US equities – either directly or through pension funds and ISAs – this could translate into market turbulence.” Over in New York, shares have fallen at the start of trading. After a late rally yesterday, the Dow Jones Industrial average has dropped by 0.6% or 261 points today to 41,740 points. The S&amp;amp;P 500, which also finished yesterday’s volatile session higher, is down 0.4%. Traders will be digesting today’s report that the White House is preparing new 20% tariffs on most imports to the US, for Donald Trump to announce on Wednesday. Fawad Razaqzada, market analyst at City Index and FOREX.com, reports that market sentiment remains fragile ahead of “Liberation Day” (as Trump dubs it) tomorrow. All eyes are on Trump’s next move—a sweeping set of new tariffs, set to be unveiled on Wednesday, which he has proudly dubbed “Liberation Day.” The premise? That hiking tariffs will boost domestic industry and create jobs. The reality? Investors fear it could stoke inflation while simultaneously weighing on economic growth—a toxic mix for an already shaky market. Investors have been catching their breath today after a volatile first three months of the year. The first quarter of 2025 was “historical” in several ways, say analysts at Deutsche Bank. As well as the launch of Donald Trump’s tariffs, there was a “huge fiscal regime shift” in Europe with Germany taking steps to boost borrowing and spending, and the launch of new AI models by China’s DeepSeek. Amid the volatility, virtually all global assets were positive in return terms, outside of US equities. Here’s the details: Gold prices (+19.0%) saw their strongest quarterly gain since 1986. That’s partly due to concerns around inflation, with the US 1yr inflation swap (+72bps) rising to 3.25%. At the other end, US tech stocks had a very rough time, with the Magnificent 7 (-16.0%) posting its biggest quarterly decline since Q2 2022, back when the Fed pivoted towards 75bp rate hikes to deal with inflation. Similarly, the NASDAQ fell -10.3%. In Europe, equities saw a much brighter performance given the fiscal shift, even if they gave up some of those gains in the second half of March. For instance, the DAX surged by +16.3% in Q1 in US dollar terms, which got some help thanks to the +4.5% appreciation of the Euro against the US Dollar in the quarter. That said, Euro sovereign bonds struggled, and March 5 saw the 10yr bund yield post its biggest daily jump since German reunification, with an astonishing +29.8bps move. Over the quarter as a whole, it was up +37bps to 2.74%. With investors moving out of US assets, the US Dollar weakened against other major currencies, with the dollar index down -3.9% over the quarter. In fact, the dollar weakened against every other G10 currency apart from the Canadian dollar in Q1, which faced the impact of US tariffs. Donald Trump doubled his wealth last year, Forbes reports, partly thanks to his dabbling in crypto. Forbes’s latest Annual Billionaires List shows that Elon Musk is the world’s richest person again, having overtaken French luxury goods titan Bernard Arnault. Musk’s net worth grew by 75% in 2024 to an estimated $342bn, due to higher valuations of xAI and SpaceX, and a 12-month rise in Tesla stock, despite the recent selloff. Musk is the first person to reach the $300 billion mark. President Donald Trump more than doubled his net worth to an estimated $5.1bn, thanks to his shares of Trump Media &amp;amp; Technology Group and “big cash inflows from his recent crypto ventures”, such as the $Trump meme coin launched earlier this. Here are more highlights from the report, via Forbes: Newcomers: The 2025 ranking features 288 newcomers, including musician Bruce Springsteen, Chipotle founder Steve Ells, Alphabet/Google CEO Sundar Pichai, actor and former CA governor Arnold Schwarzenegger and Scale AI cofounder Alexandr Wang, the youngest self-made billionaire in the world, at age 28. Globally: The United States has more billionaires than any other country, now boasting a record 902 on the list, worth a combined $6.75 trillion. China follows, with 450 billionaires, while India comes in third, with 205. The $100 Billion Club: A record 15 people worldwide now have 12-figure fortunes, up from 14 last year and zero in 2017. This elite group is worth $2.4 trillion in all, meaning just 0.5% of the world’s 3,028 billionaires hold approximately 15% of all billionaire wealth. Drop-offs: 107 people dropped off the list this year, including Hermès heir Nicolas Puech and Hobby Lobby’s David Green, among others. An additional 32 billionaires died. OBR chair Richard Hughes is not the only one concerned about the work of the Office for National Statistics (ONS). The cabinet office has launched an independent inquiry into the Newport-based number-crunchers, underlining the concern in government about the reliability of its data. Chaired by former DWP permanent secretary, Sir Robert Devereux, the review will report by the summer. Its findings will be handed to cabinet office permanent secretary, Cat Little, and another Sir Robert (Chote, in this case), chair of the UK Statistics Authority. A Cabinet Office spokesperson said: “in light of some specific concerns, the UK Statistics Authority and the Cabinet Office are commissioning an independent review into the ONS and how we can best support its staff and the timeliness and accuracy of the UK’s official statistics.” The chief executive of Channel 4 has said that artificial intelligence companies are “scraping the value” out of the UK’s £125bn creative industries, and the government must not allow them to continue to do so without paid permission. Alex Mahon said that if the government pursues its proposed plan, to give AI companies access to creative works unless the copyright holder opts out, it would put the UK creative industries in a “dangerous position”. “AI is clearly absolutely critical to the future of our industry, and many industries,” she said, speaking at the House of Commons culture select committee of MPs on Tuesday. “The debate of the day is we need very clear terms. UK copyright law is are very, very clear. And what is happening at the moment is the scraping of value from our creative industries.” Critics of the government’s opt-out proposal, issued in a consultation that closed in February, argue that it is unfair and impractical. Generative AI models, the term for technology that underpins powerful tools such as CharGPT, are trained on vast amounts of data to generate highly realistic responses. Mahon said that allowing large language models (LLMs) to continue to freely scrape data poses a major threat to the creative industry, which generates £125bn in gross value added (GVA), a measure of how much value companies add through the goods and services they produce. “The creative industries account for 6% of the UK’s GVA and is growing 1.5 times faster than other sectors,” she said. “If we continue in a world where LLMs can scrape and use that data without paying for it properly we are in a dangerous position for the industry.” Mahon said that Channel 4 is “very clear” that the copyright regime should be “opt-in”. “The burden should be on them, not us,” she said. “We are very clear we think that LLMs need to licence what they use and pay properly for it. We can’t have automated scraping, we need a proper payment and licensing regime.” Goldman Sachs have cut their forecast for UK growth this year, due to the economic damage that new US tariffs will cause, even if Britain ultimately avoids them. In a new research note today, Goldman say they assume that the US does impose duties on critical goods imports from the UK, but also that the UK ultimately avoids reciprocal tariffs given the balanced trade between the two countries (which could happen if a trade deal is agreed). Even so, though, Goldman have trimmed 0.1 percentage point off their forecast for UK growth this year, and in 2026, saying: However, our updated global baseline now assumes notably larger US tariffs on other economies including the EU. We have consequently downgraded our 2025 growth forecasts for both the US and the Euro area, implying greater spillovers to the UK. As such, we now see a larger total hit to UK GDP from trade tensions even if the UK does avoid a reciprocal tariff. We therefore lower our UK growth forecast for 2025 to 0.8% (from 0.9%) and for 2026 to 1.2% (from 1.3%). White House aides have drafted a proposal to impose tariffs of around 20% on most imports to the United States, the Washington Post is reporting. U.S. President Donald Trump’s team is mulling using trillions of dollars in new import revenue for a tax dividend or refund, the report said, citing sources. If the US were to maintain tariffs at 20% or 25% on the UK for five years it would “knock out all the headroom the Government currently has”, the UK’s fiscal watchdog has warned. Giving evidence to the Treasury Committee on the spring statement, OBR member David Miles said: “If tariffs at 20, 25% were put on the UK and maintained for five years, our assessment of what that does is that it will knock out all the headroom that the Government currently has. “Had we made that a central forecast, and had the Government not changed policy at all knowing that we were going to take that as our central forecast, then the headroom would have pretty much all gone. “Of course that would have been in some ways, a very extreme assumption. Because not only would that be as bad as people might expect in the very near term, but it would have been maintained for five years, which is beyond the next presidential election in the US.” Rachel Reeves maintained her headroom to hit her debt targets in last week’s spring statement, by announcing new cuts to welfare spending. Miles also suggested that a “very limited tariff war” could be “mildly” beneficial for the UK economy, if we kept out of it! He explained: “There’s a bit of trade that will get diverted to the UK, and some of the exports from China, for example, that would have gone to the US, they’ll be looking for a home for them in the rest of the world. “And stuff would be available in the UK a bit cheaper than otherwise would have been. So there is one, not central scenario at all, which is very, very mildly potentially positive to the UK. All the other ones which involve the UK facing tariffs are negative, and they’re negative to very different extents.” Tomorrow could bring “trepidation not liberation” says Rupert Thompson, chief economist at IBOSS (part of financial services group Kingswood). On Trump’s “Liberation Day” he writes: The range and size of the tariff increases remains quite uncertain, not least because of the complexity of the issue and the sheer difficulty in assessing the appropriate tariff for differing goods/countries. That said, the tariff hikes are looking likely to be significantly higher than was generally expected a couple of months ago. As with all his proclamations on tariffs, it is impossible to know whether and for how long they will actually be implemented. And on the recession risks to the US, he adds: The hit to US growth over the coming year looks likely to be of the order of 1% or so depending on the size of the tariff hikes. However, we continue to believe a fall into recession is unlikely. The economy proved unexpectedly resilient to Fed jacking up rates in 2022. And with the consumer and the corporate sector still in pretty good shape, it is well placed to withstand the self-harm now being inflicted. As Office for Budget Responsibility chair Richard Hughes continues his evidence to MPs on the cross-party treasury select committee, he has underlined the challenges of forecasting at the moment, on the basis of shonky data from the Office for National Statistics (ONS). Hughes said the OBR currently receives “an incomplete picture from different points in time,” from the ONS - with GDP and jobs market data updated on different timescales. He says: “Waiting for either the numerator or the denominator to be updated when you’re either looking at one or the other is not a good place to be; and so I think quality, timeliness and consistency of the main economic data sets are the things that are most important to us as forecasters.” Hughes’s colleague David Miles also gave an alarming insight into the importance of hard-to-estimate productivity growth, on the overall forecast. If productivity growth does not recover as the OBR expects, from “dismal” rates in the last two years, by the end of the five year forecast, “that would mean that the current deficit is something like £50bn,” instead of the £10bn surplus in last week’s projections, Miles warned, adding, “it’s absolutely enormous.” Bank of England interest rate setter Megan Greene has warned that the US dollar’s status as the global reserve currency could be hurt by trade war uncertainty. Greene said she thought a trade war involving retaliatory tariffs would probably be disinflationary for Britain’s economy. Exchange rates were likely to be a key way the effect of trade wars would be transmitted across economies, Greene explained, adding: “It’s also possible that the dollar’s role as a global reserve currency could be undermined a little bit by all of the uncertainty that we’re seeing, and so we don’t know how the exchange rate will behave.” The EU will react strongly to any reciprocal tariffs the US may impose on its exports, Ursula von der Leyen, European Commission president has warned. Von der Leyen says in a speech on Tuesday: “Europe has not started this confrontation. We do not necessarily want to retaliate, but we have a strong plan to retaliate if necessary. Our objective is a negotiated solution. But of course, if need be, we will protect our interests, our people, and our companies.” “Our objective is a negotiated solution. But of course, if need be, we will protect our interests, our people and our companies. I want to be very clear on the aim of our response. We think that this confrontation is in no one’s interest. The flow of goods and services between us is nearly balanced. We are willing to work on the trade balance of goods as well as services. This is the largest and most prosperous trade relation worldwide. We would all be better off if we could find a constructive solution.” Welcome news in the eurozone: inflation has ticked down to 2.2% in March, from 2.3% in February. The drop was due to lower energy prices – which fell by 0.7%, following a 0.2% rise in February. Services inflation slowed to 3.4%, from 3.7%, although food, alcohol &amp;amp; tobacco inflation picked up to 2.9%, from 2.7%, and goods prices rose by 0.6% having been unchanged in February. But a global trade war could have implications for prices in the eurozone, and beyond. ING economist Bert Colijn explains: Uncertainty around the short-term outlook for inflation remains very high. US tariffs could result in deflationary pressures on the eurozone market as they depress exports and therefore growth. Besides that, it also results in more supply in the eurozone market as the US increases barriers to access. Retaliatory measures from the European Commission will likely have an upward effect on eurozone inflation, though, as they are essentially a domestic tax that gets introduced and will be paid for by consumers to some extent. Elsewhere in the data world, the UK’s statistics regulator has criticised the Department for Work and Pensions for a misleading claim about the rise in people receiving disability benefits. The Office for Statistics Regulation says it was “entirely misleading” to claim in a recent press release that the number of people claiming disability elements of Universal Credit has increased by 383% in the last five years. Rob Kent-Smith, deputy head of the Office for Statistics Regulation, wrote in a letter to Sir Peter Schofield, Permanent Secretary at the DWP: The figure does not recognise that the majority of this increase is due to the process of migrating people from legacy benefits, such as Employment and Support Allowance, to Universal Credit over the last few years. When these people are accounted for, the actual increase in the number of people claiming disability elements of Universal Credit is 50%. After we raised concerns with DWP, the press release was amended on 27th March. The updated version of the press release includes some references to people moving from other benefits and acknowledges that the number of people with no requirement to look for work across Universal Credit health and other benefits since the pandemic has increased by 50%. However, we consider that these additions do not go far enough. Kent-Smith is asking the DWP to update the press release by Friday to remove references to the 383% figure, and not use the figure again. Over at parliament, Richard Hughes has told MPs that he has let the chancellor know that he would like to serve a second five year term as chair of the Office of Budget Responsibility. Appearing before MPs on the cross-party Treasury select committee to discuss last week’s spring statement, Hughes was asked whether he would like to stay in the post, after his first term ends on 3 October. He replied: “I have written to the chancellor, to the effect that I would be interested in serving a second and final term, earlier this year.” Asked whether he had heard back from Rachel Reeves, he said he hadn’t, but added: “I appreciate that the chancellor has a lot on her plate at the moment”. The OBR’s role in economic policymaking has come under intense scrutiny in recent weeks, as Reeves implemented spending cuts to ensure she is on course to meet her fiscal rules - including £500m of last minute welfare reforms, after the OBR rejected the government’s costing of its plans. Hughes also sought to reassure committee chair Meg Hillier that he did not believe leaks of aspects of the forecast before the spring statement had come from within the OBR. “I am satisfied that the OBR is not the source,” he said, adding that the Treasury had commenced its own leak inquiry. Rates for shipping containers from China to the United States are rising ahead of “tariff day” according to new figures from shipping analytics firm Xeneta. The cost of shipping goods to the east coast of the US is up by 9% ($322 for a forty-foot equivalent unit (FEU), a standard shipping container), while it has jumped 16% to the west coast of the US to $383/FEU, Xeneta data shows. “We live in a volatile market so, while the general direction of travel has been downward for spot rates from the Far East to the US since 1 January, we should expect some bumps in the road,” said Peter Sand, chief analyst at Xeneta. Average spot rates on container ship journeys from the Far East to the US are expected to increase by $300 - $600 per FEU as a result of General Rate Increases (GRI) by shipping firms. A GRI is the amount by which ocean carriers increase their base rate on certain trade routes, usually to cover rising operating costs and to make sure that shippers remain profitable on certain routes. Sand added: “Carriers will chance their arm and push GRIs during times of heightened uncertainty. Nervousness in the market means they can have some success too, even if it seems to defy the underlying balance of supply and demand.” The full-scale trade war outlined in Aston University’s report involves the US imposing extensive tariffs (25% across the board, except 10% on Canadian energy and an additional 20% on China) – and all affected countries retaliating equivalently. In that scenario, there will be “severe disruptions to global trade are observed”, leading to the $1.4tn of damage to the global economy. The report explains that this scenario would hurt US trade particularly badly: The US experiences substantial declines, with exports down 66.2%, imports down 46.3%, and significant welfare losses (-2.5%), alongside notable domestic price increases (5.5%). Canada and Mexico suffer pronounced trade contractions (exports falling by approximately 32.6% and 35.0%, respectively) and face substantial welfare reductions (Canada: -4.9%, Mexico: -6.6%). Major economies like Germany, China, Japan, and the UK also report reduced trade volumes, diminished domestic output, and welfare losses, though less severe compared to North America. The UK specifically sees exports down by 7.0%, imports down by 5.2%, and a welfare loss of 0.5%. These results underline the significant negative global economic consequences of comprehensive tariff escalations and retaliatory measures. Ireland could lose half its pharmaceutical sales to the US if tariffs of 20% are imposed by Donald Trump on exports from the EU, the government will be told today. It would leave a €29bn gap in the economy, my colleague Lisa O’Carroll reports from Dublin. “We don’t want to be in that space,” said Simon Harris, the deputy prime minister, as he arrived for a cabinet meeting this morning. Harris added: “Over a five year period, if the EU imposed a tariff of around 20% and the US imposed a tariff around 20% you could, over a five year period see a very significant reduction up to around half in the amount of pharmaceutical products we’re exporting.” Ireland is seen as particularly exposed to Trump’s attempt at shock therapy after its huge pharmaceutical sector was singled out as a target in his efforts to repatriate jobs and tax. Pharma and medical devices manufacturing are the backbone of US investment in Ireland, responsible for €58bn of the country’s €72bn exports to the US in 2024. Pfizer, Amgen, Johnson &amp;amp; Johnson, Merck Sharp and Dohme, Abbvie and Bristol Myers Squibb are among the owners of 90 pharma plants in Ireland. Harris said a trade war was “regrettable” and would fundamentally alter the EU and US relationship. A full-blown trade war between the US and its trading partners could cost $1.4tn, a new report shows. Economists at Aston Business School have modelled a range of potential scenarios, including the possibility that America it hit by full global retaliation after it announces new tariffs against other countries. That full-scale trade conflict could result in a $1.4 trillion global welfare loss, Aston has calculated. The report explains that tariff escalation leads to higher prices, reduced competitiveness, and fragmented supply chains, as we saw in 2018 in the US-China trade war. It says: Donald Trump’s 2025 return to power has unleashed a gale of protectionism, reshaping global trade within weeks. They outline six scenarios, from the first wave of tariffs already announced against Canada, Mexico and China to a full-blown trade war. Here are the key findings: US initial tariffs: US prices rise 2.7% and real GPD per capita declines 0.9%. Welfare declines in Canada by 3.2% and Mexico by 5%. Retaliation by Canada, Mexico and China: US loss deepens to 1.1%, welfare declines in Canada by 5.1% and Mexico by 7.1%. US imposes 25% tariffs on EU goods: Sharp transatlantic trade contraction, EU production disruptions, US welfare declines 1.5%. EU retaliates with 25% tariff on US goods: Prices rise across US and EU, mutual welfare losses and intensified negative outcomes for the US. UK experiences modest trade diversion benefits. US global tariff: Severe global trade contraction and substantial price hikes substantially affect North American welfare and UK trade volumes. Full global retaliation with reciprocal tariffs: Extensive global disruption and reduced trade flows, severe US welfare losses, $1.4 trillion global welfare l</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>FTSE 100 closes up 0.6%, DAX up 1.7%, CAC 1% as investors await Trump announcement. New report shows 25% tariffs could cause a $1.4tn hit to the world economy. UK government expecting to be hit by new tariffs tomorrow.</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Time to wrap up European stock markets have hit a two-week low, after Donald Trump announced a new 25% tariff on car imports to the US. Automakers’ shares have been hit, with BMW down 2% in late-afternoon trading and Volkswagen 1.3% lower. US manufacturers have fallen too – with General Motors falling 7%, as it will also face a tariff on cars manufactured outside the US and on imports of components. UK chancellor Rachel Reeves has suggested Britain does not want to retaliate. She told Sky News: “We’re not at the moment in a position where we want to do anything to escalate these trade wars. “We are looking to secure a better trading relationship with the United States,” British Steel plans to close its two blast furnaces and steelmaking operations in Scunthorpe, putting up to 2,700 jobs at risk in a move unions called “devastating”. The company, which is owned by China’s Jingye, said it would immediately start consultations with its workforce and unions on redundancies stemming from the planned closures alongside a reduction of steel rolling-mill capacity. The closures affect between 2,000 and 2,700 workers out of a workforce of about 3,500, British Steel said, and will bring an end to steelmaking in Scunthorpe after 160 years of production. Lower-income households are on track to become £500 a year poorer by the end of the decade as a result of the UK chancellor’s spring statement, according to analysis by a leading thinktank. The Resolution Foundation said a combination of weak economic growth over the next five years and benefit cuts that fell disproportionately on lower-income households would result in an average annual loss of £500 in 2030 for those in the poorest half of the population. Some pharmaceuticals firms are sending more medicines by air to the US than usual, in an attempt to front-run President Donald Trump’s 2 April tariffs announcement. Two European-headquartered drugmakers told Reuters this week they are sending as much of their medicines across the Atlantic as possible over the past several weeks and heard other pharmaceuticals companies were doing the same. Gaurav Ganguly, senior director for economic research at Moody’s Analytics, warns that the consequences of the new US car tariffs are significant: “A number of European countries are in the immediate firing line, including Sweden and Germany. If the policy remains in place, the consequences for consumer confidence and employment in the auto sector and beyond are severe. European, Japanese, South Korean and Chinese manufacturers all face plummeting demand from U.S. buyers. While the stated intention is to use tariffs to raise revenue for tax cuts, this is unlikely to happen if U.S. consumers don’t buy tariffed products. For automakers, offering deep discounts to these consumers might offer some short-term relief but is clearly unsustainable, while this degree of policy volatility makes it harder to shift production to the U.S. with confidence.” Jess Ralston, analyst at the Energy and Climate Intelligence Unit (ECIU) has argued that jobs didn’t have to be at risk in Scunthorpe: “Job losses are devastating for anyone, but particularly in a community like Scunthorpe that relies heavily on the steelmaking industry. It did not have to be this way. While steel production in the UK has been declining since the 1970s, long before climate commitments, China has been ramping up its production and undercutting other manufacturers across the world. A phased transition to the steel industry of the future, including hydrogen, could have kept these jobs in communities that need them. Clearly, we cannot afford to stick to the status quo. The EU recently published its Steel Action Plan and countries like the US are making moves to ensure they have a steel industry thats able to go green as the rest of the economy does. Many in Scunthorpe will be worried about their jobs, wondering what our long-term plan is, and whether we’ll be able to compete with the rest of the world for this industry of the future.“ Trade Secretary Jonathan Reynolds has declined to rule out changing taxes on major tech firms in exchange for exemptions from US tariffs, but insisted they would pay “a fair amount of tax”. Speaking at a trade conference hosted by Chatham House, Mr Reynolds suggested ministers were willing to discuss the digital services tax (DST) with their US counterparts. Reynolds explained: “We have always been of the view as a country that this has to be something ideally agreed on an international basis, but it’s not that DST has been put in place as something that can never change or we can never have a conversation about it.” Last night’s announcment about US car tariffs has also hurt the Mexican peso. The Mexican peso has weakened by around 0.9% to around 20.29 per U.S. dollar. In other moves, the Canadian dollar fell 0.31% to C$1.43 per dollar. Airline travel between Canada and the US is “collapsing” amid Donald Trump’s tariff war, with flight bookings between the two countries down by over 70%, newly released data suggests. According to data from the aviation analytics company OAG, airline capacity between Canada and the US has been reduced through October 2025, with the biggest cuts occurring between the months of July and August, which is considered peak travel season. Passenger bookings on Canada to US routes are currently down by over 70% compared to the same period last year. Comparing the available bookings from March 2024 to March 2025, OAG looked at how many people have booked trans-border flights in the six-month period between April through September. It found that the number of tickets booked is down anywhere from 71% to 76%. Over on Wall Street, US auto makers have joined the global selloff in car companies. General Motors has dropped 6.3% in early trading, the worst-performing company on the S&amp;amp;P 500 index, while Ford are down 2.5%. That follows losses in Europe earlier today, where Stellantis (whose brands include Jeep and Dodge, alongside Fiat and Citreon) have fallen 5.7% today, and BMW has lost 3%. Traders are concluding that the new 25% tariff on cars, and imported auto parts, will hurt the US car industry. GM, Ford, and Stellantis build vehicles in Canada, Mexico, and China, and would also face higher production costs due to tariffs’ effect on the auto supply chain. Jobs are also at risk at Sky. The broadcast is cutting about 2,000 jobs, in a push to replace more of its traditional call centre roles with online and AI-guided services. Sky is to close three of its 10 customer service sites — in Stockport, Sheffield and Leeds — and scale back two others. Downing Street said the Government had made a “generous offer” to British Steel, ahead of its decision to propose closing steelmaking in Scunthorpe. The Prime Minister’s official spokesman said: “We’ve made a generous offer to British Steel designed to deliver a sustainable future for staff, industry and the local community… we’ve got a two and half billion pound plan to rebuild the sector. “We will continue to work with British Steel and with the company’s owners to secure its future and deliver on a good outcome. “But we’ve made that offer and that’s obviously up to the company involved.” As flagged earlier, there are reports that Jingye Group turned down a £500m offer of support. Mexico faces the biggest economic impact from Donald Trump’s car tariffs, according to analysis from consultancy Capital Economics. They have examined which countries export most autos to the US as a share of their own GDP. Mexico and Slovakia appear very heavily exposed, with these exports accounting for 4 to 6% of GDP. Shares for Korea, Canada and Japan are 1 or 2%. However, to get a better picture, they’ve also examined the “domestic value added dependent on exports of autos and parts to the US”, which strips out the impact of components bought overseas (eg, if a German carmaker used parts imported from Slovakia, the value added by Slovakia should be excluded) On this basis, Mexico is still most vulnerable, but with a smaller 1.6% of its GDP at risk, followed by Slovakia, Korea, Hungary, Japan, Canada and Germany. Capital Economics also suggest the tariffs could benfit the US auto sector, or they might simply hurt demand. US vehicle sales totalled 16 million in 2024, of which about eight million were imported. The low level of US capacity utilisation in the vehicle sector suggests that there is scope for domestic production to rise to offset lower imports. If capacity utilisation returned to its prior peaks, that would be consistent with a rise in vehicle assemblies of three million. That said, the big risk is that higher prices will cause consumers to reduce demand rather than switch to domestic suppliers, and there will be other constraints on production in the short term such as a lack of workers. We also have confirmation that Donald Trump inherited a solidly growing economy. US GDP rose by 2.4%, on an annualised basis, in October-December, new data shows, slightly higher than the previous estimate of 2.3%. This equates to growth of 0.7% in the quarter, faster than the eurozone (which grew by 0.2%) and the UK (which grew by 0.1%). The yield, or interest rate, on UK government bonds has risen today as investors digest yesterday’s Spring Statement. 10-year gilt yields are up 6 basis points, or 0.06%, to 4.784%, towards the 16-year high over 4.92% set in January. Long-dated 30-year gilt yields are up too, at 4.362%. Yields rise when bond price fall, and measure the government’s cost of borrowing. US government bond yields are also up today, but European borrowing costs are lower. The fiscal plans outlined yesterday showed borrowing would be higher than previously forecast over the next five years: Rising bond yields adds to the UK’s fiscal challenges, as it pushes up the cost of borrowing. And if the UK’s economy performs worse than expected (perhaps due a trade war), tax receipts could be lower, meaning pressure to borrow more. Yesterday, the UK’s Debt Management Office (DMO) outlined how it will issue £299bn of gilts this financial year, to cover maturing debt and new borrowing. That’s slightly lower than the £305bn forecast. Evem so, analysts at Morgan Stanley have warned that “the path ahead looks fraught”, telling clients: The headroom was restored, the gilt remit was kept just under £300 billion, and the share of longs [longer-dated gilts] was lower than even our below-consensus forecast. And yet...the consolidation was back-loaded. Fiscal buffer is modest. Risks to growth are skewed to the downside. The path ahead looks fraught - although on current forecasts, it is a path of a meaningful fiscal consolidation. Business and trade secretary Jonathan Reynolds has been interrupted by pro-Palestinian protesters calling for an end to the sale of F35 jet parts to Israel, PA Media report. At the start of Mr Reynolds’ appearance at a conference on trade hosted by the think tank Chatham House, a demonstrated shouted: “This man and his government are complicit in genocide. “The F35s are massacring Palestinian children. They have not stopped the trade of F35s.” After the protester was removed from the event, Mr Reynolds said: “We have suspended arms exports to Israel. “We have not suspended F35s because they are integral to our national security and the defence of Ukraine, and people will know the supply chain for the F35 means they cannot be isolated to one country. “That decision was laid out very clearly in Parliament, so I’m quite happy if he wants to ask a question rather than jump on stage to have that engagement with him.” He was then interrupted by another protester waving a Palestinian flag and calling for an end to F35 exports, who was subsequently removed. The proposed closure of the Scunthorpe blast furnaces is another big issue in Jonathan Reynolds’s in-tray, as the business secretary also faces the threat of a US trade war. Reynolds has insisted today that he will work with British Steel’s owners, Jingye, over the plant’s future, saying: “I know this will be a deeply worrying time for staff and, while this is British Steel’s decision, we will continue working tirelessly to reach an agreement with the company’s owners to secure its future and protect taxpayers’ money. “We’ve been clear there’s a bright future for steelmaking in the UK. “We’ve committed up to £2.5 billion to rebuild the sector and will soon publish a plan for steel setting out how we can achieve a sustainable future for the workforce, industry and local communities.” Trade body UK Steel has warned that Britain’s national security would be threatened if steelmaking ceased in Scunthorpe. UK Steel Director General, Gareth Stace, said: “The proposal to close iron and steelmaking at Scunthorpe marks a heartbreaking and pivotal moment for our sector. It is a shocking blow to the 3,400 workers, our sector and to the whole community in Scunthorpe. This gut punch to UK steelmaking will have a profound impact, felt throughout the British economy. “All options should be on the table, and we need a secure future for our steel industry. The end of steelmaking at British Steel would mean we have a major gap in capacity to meet the future demand of the nation and will be an irreparable break in the armour of national security. “This devastating decision will cause untold disruption and damage to our supply chains, threatening jobs, businesses and the nation’s economic strengths. The steel industry is officially in a crisis. UK Steel has been sounding the alarm. Government must get back to the negotiating table to urgently stop the lifeblood draining from our sector and take action to rebuild the steel industry.” The Unite union have condemned British Steel’s proposal to close its Scunthorpe blast furnaces, accusing the company of trying to blackmail the government into providing more financial support. Unite general secretary Sharon Graham said: “This announcement of job losses is quite simply a disgrace. British Steel is guilty of trying to hold the government to ransom, while using its dedicated workforce as pawns. “In discussions with Unite, the government has clearly moved and has made an offer to invest heavily in British Steel (Jingye). This offer comes with long-term job guarantees, anything less would be a complete misuse of taxpayers’ money. British steel now needs to make the necessary commitments. “British Steel must now withdraw its job threats and work with the government and Unite on a sustainable way forward which is in the best interests of the workers, their communities and the wider economy. “The UK has the opportunity of becoming a leader in green steel and British Steel should be at the forefront of that transformation.” Newsflash: British Steel is proposing to close its steelmaking operations in Scunthorpe, with the loss of up to 2,700 jobs. It has just launched a consultation on the proposed closure of its Scunthorpe blast furnaces, rod mill and steelmaking operations in the Lincolnshire town. British Steel says it has not been able to reach an agreement with the UK government for support to keep the plant running, and to allow future investment in Electric Arc Furnace (EAF) technology, which is more environmentally friendly than traditional furnaces. Three options are under consideration: Closure of the blast furnaces, steelmaking operations and Scunthorpe Rod Mill by early June 2025 Closure of the blast furnaces and steelmaking operations in September 2025 Closure of the blast furnaces and steelmaking operations at a future point beyond September 2025 The proposed closures will impact between 2,000 and 2,700 jobs, says British Steel, which is owned by Chinese industriall group Jingye. British Steel CEO, Mr Zengwei An, says: “We understand this is an extremely difficult day for our staff, their families, and everyone associated with British Steel. “But we believe this is a necessary decision given the hugely challenging circumstances the business faces. “We remain committed to engaging with our workforce and unions, as well as our suppliers and customers during this time.” British Steel says it will continue to work with the UK Government to explore options for the future of the business. Sky News reported earlier this week that Jingye had rejected a £500m offer from the government, to help British Steel’s transition to green steel production. UK-based manufacturers might be able to pass on the impact of tariffs onto their wealthy customers, which would cushion the impact of the latest levies. My colleague Jasper Jolly looked at this issue in January, and reported: About 10% of UK car exports go to the US, although the majority go to the EU, according to the Society of Motor Manufacturers and Traders, a lobby group. One small silver lining for the UK may be that a large number of those exports from companies such as the Jaguar and Land Rover owner JLR, the BMW-owned Rolls-Royce or the Volkswagen-owned Bentley, are classed as luxury vehicles, with prices that can start at £100,000 and rise to multiples of that. Those companies should be able to pass on the cost of tariffs to wealthier customers without denting sales. The British Chambers of Commerce has warned that the new 25% tariff on car imports to the US will hurt business confidence. The BCC says the impact on the UK car sector “cannot be overstated”, given the importance of the US market for British manufacturers. William Bain, BCC head of trade policy, explains: “Businesses were already looking with trepidation towards next week’s planned reciprocal tariffs before this fresh upheaval was announced. “Around half of the cars purchased in the US are imported so this will pass through into much higher costs for US consumers. If fully extended to all components it will affect supply chains too. “The impact of this on the UK car industry cannot be overstated. Cars are the UK’s biggest goods export to the US, with £6.4bn in sales in 2023, led by iconic manufacturers such as Aston Martin, Jaguar, and Land Rover. “Piling these tariffs on top of the others already expected on 2 April, will sap business confidence and add further uncertainty for both UK and US firms. “We urge the UK Government and the US Administration to continue intensive dialogue over the coming days and weeks to reach a mutually beneficial agreement on technology and trade. “This needs to provide certainty for business and consumers alike on the future tariff landscape and remove unnecessary levies already in place.” Kathleen Brooks, research director at XTB, reports that tariffs are “dominating market sentiment”, as investors calculate the impact of the trade dispute: European stocks have opened sharply lower after President Trump announced a 25% levy on imports of cars and car parts coming into the US. This news has had an immediate effect on share prices, the US imports 8 million cars a year and untold car parts, which equates to $240bn in trade. Unsurprisingly, the biggest decliners on the Eurostoxx index include Ferrari, Volkswagen, BMW and Mercedez Benz Group. There’s also plenty of speculation today that Rachel Reeves may need to make tax rises in the autumn statement, if the UK’s fiscal position worsens. Goldman Sachs has warned there are “further fiscal pressures ahead” that could squeeze the chancellor’s headroom against her fiscal targets. Goldman analyst James Moberly told clients: We think that the OBR will ultimately downgrade its trend growth forecast by around 0.2pp, possibly in the Autumn, which could reduce headroom by around £14bn, and we expect increasing pressure for the government to raise defence spending above 2.5% in the current Parliament. If these pressures do materialise, we continue to think that tax changes are the most likely response. That said, we do think that lower interest rates could ease some of the pressure on the fiscal position as we expect the Bank of England to cut further than the market expects. Richard Hughes, head of the independent Office for Budget Responsibility, has warned that the car tariffs announced by Donald Trump will eat into Rachel Reeves’s fiscal headroom. Speaking to Radio 4’s Today programme, Hughes also flagged that a full-blown global trade war could eliminate that headroom altogether. He explained: “This represents the crystallisation of one of the risks that we highlighted around our central forecast, which was one of escalating global trade tensions.” “The UK exports, in terms of goods to the US, around 2% of GDP. Car exports are about 10% of that. “So that’s affecting directly UK goods exports of around 0.2% of GDP. So what Trump’s announced overnight is not the whole of that worst-case scenario, but it’s elements of it, and it’s the beginning of that risk side.” The OBR presented three trade war scenarios yesterday – the worst, where the UK and US hit each other with reciprocal tariffs, showed 1% would be wiped off UK GDP. We’re not there yet, though, with Reeves arguing against escalating the trade war this morning. Next has rung up £1bn in annual profits for the first time but warned of growing risks to the UK economy, saying big business could not afford to finance “excessive regulation” and government debt. The retailer said pre-tax profits rose 10% to just over £1bn, before one-off items including a £15m pension charge, in the year to January after sales rose 8.2% to £6.3bn, led by strong overseas growth and sales of other brands. Simon Wolfson, the chief executive of Next, said he now expected to make £1.06bn next year, £20m more than previously expected, as he said the first eight weeks of the new financial year had been “ahead of our expectations”. Wolfson, who is a Conservative peer, said: “We are as positive about the company today as we were [a year ago], albeit in an environment where the risks to the wider UK economy are growing. Next’s shares have jumped over 5%, to the top of the FTSE 100 leaderboard. Britain’s car sector is calling for more government support, after reporting another fall in output. UK car and commercial vehicle production declined by 11.6% in February, to 82,178 units, according to new data from the Society of Motor Manufacturers and Traders (SMMT). The SMMT blames a range of factors, including “soft markets at home and overseas, model changeovers and plant restructuring”. Mike Hawes, SMMT chief executive, said, “These are worrying times for UK vehicle makers with car production falling for 12 months in a row, rising trade tensions and weak demand. The market transition is not keeping pace with ambition and, while the industry can deliver growth – and green growth at that – it needs policies to deliver that reality. It was disappointing, therefore, to hear a Spring Statement that did nothing to alleviate the pressure on manufacturers and, moreover, confirms the introduction next month of additional fiscal measures which will actually dissuade consumers from investing. Without substantive regulatory easements our manufacturing viability remains at risk and the UK’s transition to zero emission mobility under threat.” And on the new auto tariffs, Hawes has urged the UK and US governments to “come together immediately and strike a deal that works for all”. European stock markets are sea of red in early trading, dragged down by the auto sector. Germany’s DAX index has dropped by 1.6%, with Mercedes-Benz (now -5.5%) and Porsche (-4.8%) leading the fallers. France’s CAC has lost 1.1%, dragged down by Stellantis (now -6%). The gloomy mood has also reached London, where the FTSE 100 index (which doesn’t contain any carmaker) is down 0.6%, or 52 points, at 8637 points. Mohit Kumar of investment bank Jefferies explains: Tariff concerns returned to the market with Trump imposing 25% tariffs on Auto imports and suggesting reciprocal tariffs to come. Comments from trading partners overnight suggest potential counter tariffs will be likely. Tech stocks were under pressure on reports that China would use energy efficiency rules to limit use of high-end imported chips. European car giant Stellantis’s shares have fallen over 5% in early trading. German carmakers are being rocked by the announcement of new auto tariffs at the US border too. Shares are being hit in early trading in Frankfurt, where BMW are down 4.2%, Volkswagen has lost 3.3%, and Mercedes-Benz has dropped 4.1% Jochen Stanzl, Chief Market Analyst at CMC Markets, says Donald Trump’s new tariffs will “significantly worsen the situation for German car manufacturers”, writing: The European Union is now tasked with negotiating preferences, whereby only the portion of each vehicle not manufactured in the U.S. will be subject to the tariff. However, not all manufacturers will succeed equally in these negotiations, and it’s quite possible that certain vehicles may no longer be available in the U.S. market due to lost competitiveness. Further complicating matters is the looming implementation of tariffs on auto parts in May, which will only exacerbate the challenges faced by automakers. The new tariffs will significantly worsen the situation for German car manufacturers, whose profits have already taken a substantial hit. The U.S. is a crucial trading partner; for instance, 80% of Volkswagen’s car sales in the U.S. are imports, while for Mercedes-Benz, this figure exceeds 60%, and for BMW, it is about 50%. One can only hope that Trump will use these tariffs as leverage to negotiate a better deal. Shares in UK luxury carmaker Aston Martin have tumbled over 6% at the start of trading in London, to what looks to be a record low. Rachel Reeves has declared that the UK is not planning “at the moment” to introduce retaliatory tariffs on the US, and does not want to escalate a trade war with Donald Trump. Speaking to broadcasters this morning, the chancellor said Britain is working intensely with Washington to secure an exemption from tariffs She told Sky News: “We are not at the moment in a position where we want to do anything to escalate these trade wars. Trade wars are no good for anyone.” Reeves has also told the BBC that an escalation of tariffs would be bad for Britain “but it would be bad for the U.S. as well, and that’s why we are working intensely these next few days to try and secure a good deal for Britain.” Keir Starmer’s government had hoped to avoid being entangled in a trade war with the US, as trade between the two countries appears broadly balanced. Yesterday, the Office for Budget Responsibility showed that a full-scale, tit-for-tat, trade war could knock 1% off the size of the UK economy. That would firmly upend the latest forecasts for UK growth, and borrowing. Shares in US carmakers fell in after-hours trading last night too, after Trump’s announcement. General Motors has fallen by 6.2%, and Ford has lost 4.7%. The new US tariffs will apply all cars made outside of the US, and certain car parts too, so they will have a wide impact on the auto sector, and could badly hurt profits. As Barrons explains: Estimates of cost increases from new tariffs are in the thousands of dollars per new car. Higher costs could turn into higher prices, destroying demand for new cars, or they could eat into profit margins. Any impact would be uneven, though. The Chevy Equinox is made in Mexico. The Toyota RAV4 is built in Ontario, Canada. The Ford Escape is made in Kentucky. It isn’t easy to untangle 30-plus years of free trade. Germany’s economy minister Robert Habeck has called for the European Union to deliver a firm response to Donald Trump’s new 25% tariff on imported cars. In a statement, Habeck says: “What counts now is to have a firm response to these tariffs from the EU. It needs to be clear that we will not take this lying down.” Shares in Asia-Pacific car companies have fallen after Donald Trump announced plans to impose sweeping 25% tariffs on cars from overseas last night. The latest eruption in the Trump Trade Wars has hit investor confidence, and angered US trading partners around the world. In Japan, shares in Toyota Motor have lost 2.04%, Honda Motor fell fell 2.48% while Nissan Motor slipped 1.68% – which all helped to pull the Nikkei index down 0.6% today. In South Korea, Hyundai Motor’s shares have fallen over 4% – just days after it tried to placate Trump by announcing a $21bn investment in the US. The European Commission president, Ursula von der Leyen, has described Trump’s move as “bad for businesses, worse for consumers”. Trump has also threatened further tariffs if the EU worked with Canada “in order to do economic harm to the USA”, which may fuel fears of a tit-for-tat trade conflict that would hurt the global economy. Writing on his own social media platform, Truth Social, he said if they did so, “large scale Tariffs, far larger than currently planned, will be placed on them both in order to protect the best friend that each of those two countries has ever had!” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. As the dust settles after yesterday’s spring statement, analysis shows that lower-income households are set to become £500 a year poorer over the current parliament. The Resolution Foundation has been crunching the data since Rachel Reeves updated us on the nation’s finances, and concluded that poorer households will be most affected by the various tax and benefit changes in this Parliament. Over the next five years, the average income across the poorest half of working age households is projected to decline by three per cent, or £500. That has only happened before during the early 1990s recession (1989 to 1994-95) and the financial crisis (2007-08 to 2012-13). Ruth Curtice, Chief Executive of the Resolution Foundation, says: “High debt servicing costs, weak tax receipts, and the need to reassure jittery markets, meant the Chancellor had to announce tax rises or spending cuts in her Spring Statement. “She chose to focus the bulk of her consolidation on welfare cuts. These cuts have been justified on the basis of getting people into work, but it is questionable how much of a jobs boost they’ll deliver. After all, the bulk of the cuts are to disability benefits which aren’t related to work, and the cuts take effect from 2026, three years before the Government’s employment support programme kicks into gear. “While the OBR’s outlook for growth today got gloomier, it is far more optimistic about Britain’s medium-term economic prospects. The Chancellor will hope that reality catches up with the OBR, rather than the OBR falling back to reality, otherwise more tough choices await. “The outlook for living standards remains bleak. Britain’s poor economic performance, combined with policies that bear down hardest on those on modest incomes, mean that 10 million working-age households across the bottom half of the income distribution are on track to get £500 a year poorer over the course of the Parliament.” Yesterday the chancellor announced welfare cuts of £4.8bn, with official figures showing that three million households could lose £1,720 a year in benefits. That could yet lead to a rebellion among Labour MPs when it comes to a vote… …especially as Resolution Foundation have calculated that the £4.8bn welfare savings are actually built on £8.1bn worth of cuts. They explain: The full scale of welfare cuts are far greater than the net £4.8 billion savings. After accounting for the £1.9 billion boost to the standard rate of Universal Credit (UC), and the ‘gain’ from not going ahead with scored-but-never-implemented changes to the Work Capability Assessment, cuts to ill-health, disability and carer’s benefits rise to £8.1 billion in 2029-30, and will continue to grow over time. Economists are also concerned that Reeves has not left herself very much headroom to hit her fiscal targets – any slippage could force her to consider tax rises. The risks to the economy were amply demonstated by Donald Trump last night, as he announced new 25% tariffs on cars from overseas. The agenda 8.30am GMT: Bank of England policymaker Swati Dhingra speaks on a panel in South Africa 9am GMT: Resolution Foundation event assessing the Spring Statement 10.30am GMT: Institute for Fiscal Studies press conference on the Spring Statement 12.30pm GMT: Updated US Q4 GDP report. 12.30pm GMT US weekly jobless claims</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>European stock markets have hit a two-week low, after Donald Trump announced a new 25% tariff on car imports to the US. Automakers’ shares have been hit, with BMW down 2% in late-afternoon trading and Volkswagen 1.3% lower. US manufacturers have fallen too – with General Motors falling 7%, as it will also face a tariff on cars manufactured outside the US and on imports of components.</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Here’s our breakdown fo the key points from today’s spring statement: Rachel Reeves blamed “global uncertainty” as she announced swingeing cuts to welfare and other public spending designed to plug a fiscal hole caused by soaring borrowing costs and sluggish economic growth. The chancellor told the Commons that the UK’s growth forecasts for this year had been halved from 2% to 1% by the Treasury watchdog, which concluded that the chancellor would have missed her goal of balancing the books if she did not act. Striking a defiant tone, Reeves set out measures in her spring statement she said would turn a predicted £4.1bn hole in the public finances back into a £9.9bn surplus within five years. This would restore “in full” the headroom against her self-imposed fiscal rules, she said. In a pointed message to her cabinet colleagues and Labour backbenchers who have privately argued for the fiscal rules to be revisited, Reeves said they were “non-negotiable” and “an embodiment of this government’s unwavering commitment to bring stability to our economy”. She suggested that abandoning those fiscal rules would be an irresponsible move akin to Liz Truss’s disastrous mini-budget. The chancellor said the cuts she announced would be offset by billions of pounds in long-term investment to grow the economy, with a particular focus on the building of millions of new homes and supporting higher spending on defence. It’s nearly time for Rachel Reeves to deliver the Spring Statement, with cuts to benefits and lower growth forecasts both expected. We’re live-blogging the action here: The British public’s expectations for inflation over the longer term have risen this month to their highest since October 2022, new data shows. A Citi/YouGov survey shows that the public’s longer-term inflation expectations have risen to 4.2% in March, from 3.9% in February. That’s the highest since the recent peak of inflation, when surging energy costs were driving up the cost of living. Year-ahead inflation expectations rose to their highest since October 2023 at 4.0%, up from 3.9%. Citi economists Callum McLaren-Stewart and Michel Nies explain: “For the (Bank of England) MPC, this survey will warrant continued caution with quarterly cuts the likely outcome for now.” Uk supermarket chain Morrisons has reported rising sales in the three months to January. The grocery giant said sales were 2.4% up over the quarter to January 26, hitting £4 billion, despite having announced hundreds of people are at risk of redundancy earlier this week. The company said it made £56m in savings during the period and hiked its long-term savings target from £700m to £1bn. Rami Baitiéh, chief executive, says: “Despite a challenging environment, Morrisons has made exceptional progress in a very short time and that is entirely down to the hard work, positivity, talent and customer focus of the colleagues in our stores, in our foodmaking sites and in our operations across the country.” Former chancellor George Osborne has told Bloomberg that today’s spring statement needs to be “a reset”. Osborne was speaking in Hong Kong, at a summit organised by HSBC, where he says there is “quite a negative sentiment about the UK”, which needs to be changed. Osborne argues that the government has not, until quite recently, given an “unabashedly pro-business or pro-enterprise” message. Instead it has been raising taxes on business and pushing entrepreneurial, wealthy people away, he adds. This morning’s UK February inflation report was a welcome gift to doves at the Bank of England, reports Achilleas Georgolopoulos, senior market analyst at XM. Both the headline and core inflation figures decelerated to 2.8% and 3.5%, respectively, bringing smiles to the BoE halls and supporting the chances of a May rate cut. The pound has not taken lightly the lower inflation prints, though, losing ground against both the euro and the dollar. Earlier this month the most dovish policymaker at the Bank, Swati Dhingta, was the only member of the Monetary Policy Committee to vote for a rate cut – her eight colleagues voted to leave rates on hold. The focus now shifts to the spring statement update, Georgolopoulos adds: Rachel Reeves is expected to avoid changing her fiscal rule and increasing taxes, and instead focus on spending cuts. Reports point to significant cuts in welfare spending and a leaner public sector, which sounds similar to what Musk’s DOGE is implementing in the US. These new measures will probably be begrudgingly accepted by the majority of voters and most Labour MPs, who are already upset about the fiscal policy mix implemented by the Labour government. Today’s inflation data is consistent with the Bank of England cutting by a further 25bps at May’s meeting, says Gabriella Dickens, G7 economist at AXA Investment Manager. Dickens points out, though, that we will see another CPI print (for March) before then. She tells clients: CPI inflation will tick up over the coming months, peaking at around 3.5% in Q3. Underlying pressures, though, should continue to ease, albeit with some volatility. We continue to see three 25bps cuts this year leaving Bank Rate at 3.75% by year end. There isn’t consensus on what the Bank of England will decide to do this year. The. National Institute of Economic and Social Research (NIESR) predict it will only manage one more interest rate cut this year. Monica George Michail, NIESR associate economist, explains: We forecast CPI inflation to remain above the Bank of England’s 2 per cent target throughout this year, driven by increased public spending, persistent wage growth and global trade fragmentation. We therefore think there will only be one more 25 basis point interest rate cut in 2025”. Profits at the UK housebuilder Vistry Group have slumped by more than a third in what it described as a “disappointing year” but it is pinning hopes of a turnaround on the government’s promise this week to inject £2bn into affordable homes. After three profit warnings last year, Vistry suspended dividend payouts to shareholders on Wednesday and its shares were the biggest faller on the FTSE 250 index, dropping by as much as 8% before easing back to 5.5% down. Greg Fitzgerald, Vistry’s chief executive, said 2024 had been challenging but welcomed the government’s affordable housing pledge, adding the builder would “be seeking to progress as quickly as possible with our partners to deliver quality new homes across the country”. We also have a healthcheck on the UK’s property sector, which show that rental growth slowed a little last month. The Office for National Statistics reports that average UK monthly private rents increased by 8.1%, to £1,326, in the 12 months to February 2025, down from 8.7% in January. The ONS says: Average rents increased to £1,381 (8.3%) in England, £785 (8.5%) in Wales, and £998 (5.8%) in Scotland, in the 12 months to February 2025. That means rents across the UK are rising faster than wages (total pay rose by 5.8% per year in the quarter to January), and around three times faster than the headline CPI inflation measure. The ONS also reports that UK house prices increased by 4.9% in the 12 months to January, lifting the average price to £269,000, up from 4.6% in the year to December 2024. It adds: Average house prices increased to £291,000 (4.8%) in England, £210,000 (6.0%) in Wales, and £187,000 (4.6%) in Scotland, in the 12 months to January 2025. The pound has weakened further against the US dollar this morning, and is now down half a cent at around $1.289. Dan Coatsworth, investment analyst at AJ Bell, says investors are bracing for the UK government’s Spring Statement (from 12.30pm today), as well as digesting this morning’s inflation data: “The OBR is widely expected to downgrade its economic forecast for the country. What really matters to investors is the extent of that downgrade and the omens look bad. “It could be a testing day for markets if chancellor Rachel Reeves delivers more bad news and is seen to be fighting a losing battle. However, the flipside of a weaker pound is that it benefits the army of dollar earners on the FTSE 100, hence why the UK index traded higher. Energy producers and miners were among the top risers. “Lower than expected inflation figures today and strong services PMI data earlier in the week will have been welcomed with open arms by Reeves. Sadly, these two data points are not enough to convince markets that everything is rosy with the UK. Investec economist Philip Shaw predicts the Bank of England will have lowered UK interest rates by three-quarters of a percentage point by the end of the year – implying three quarter-point cuts. Shaw writes: With the targeted [inflation] measure at 2.8%, the Bank of England’s February Monetary Policy Report short-term forecasts are back on track. We note that the Bank’s projections see inflation peaking at 3.7% in Q3 and with our own forecast at 3.2%, we are hopeful that the MPC will be amenable to cutting the Bank rate again through the course of this year. Of course the outlook for rates will also depend in no small measure on the committee’s assessment of labour market conditions, in particular the outlook for pay. But with the economy still struggling to gain positive momentum we stand by our view that the MPC will bring the Bank rate down to 3.75% by the end of the year from its current level of 4.50%. Responding to the inflation figures, Treasury chief secretary Darren Jones said: “Our number one mission is kickstarting growth to raise living standards for working people, that is why we are protecting working people’s payslips from higher taxes. “In a changing world, we’re focused on delivering economic stability to secure people’s finances – freezing fuel duty, protecting the triple lock and increasing the national living wage by £1,400 a year for full-time workers, while going further and faster to drive growth through our plan for change.” [that growth drive hasn’t got off to a great start this year, though – GDP fell by 0.1% in January]. Shadow chancellor Mel Stride has also responded: “Inflation remains higher than when Labour took office and the Bank of England expect it to rise over the coming year. “We left Labour with inflation bang on target. But since their no-strings-attached union payouts, record tax rises and borrowing splurge, they have pushed up the cost of living. “The Chancellor’s choices have saddled the country with higher inflation for longer. Unless she takes urgent action at her emergency budget today, working families will continue to pay the price.” [Stride is correct that inflation was 2% in June last year, just before Labour won the election. But CPI had also been over the UK’s target for most of the previous three years – peaking over 11% in October 2022]. Analysts at ING predict the Bank of England will cut interest rates three times this year – which is one more cut than the City currently prices in. They told clients this morning: We expect the current quarterly pace of rate cuts to continue through 2025 and into 2026, with a terminal rate of 3.25%. Bank rate is currently 4.5%, following three quarter-point cuts since last summer. Sanjay Raja’s, chief UK economist at Deutsche Bank Research, reckons a May interest rate cut is ‘more likely than not’. He writes: Ahead of the Spring Statement, today’s inflation data should give Chancellor Reeves some reprieve. Headline CPI fell back to 2.8% y/y – in line with the BoE’s forecast, and below our own expectations. Core CPI also ticked lower to 3.5% y/y – slipping below consensus expectations (as well as the Bank’s forecasts). Underneath the hood, however, there remain some concerns around services prices. Indeed, services CPI stayed put at 5% y/y. But underlying measures of services CPI ticked higher in February – underscoring continued price pressures in the services basket. With the NLW hike coming and the increase in employer NICs we think price over the next couple of months will be very important to watch. Make no mistake, inflation remains on a one-way journey: up. We see headline CPI rising to just under 4% y/y later this year. Inflation expectations have already risen on the back of rising headline prices, energy prices, and food prices. The MPC have taken notice – one reason they opened the door to a potential pause in May. The good news is that today’s data should provide the BoE a path to continue with its gradual dial down of restrictive policy. We continue to think a May rate cut is more likely than not. And we expect Bank Rate to fall to 3.25% next year as headline pressures recede and wage settlements fall back to a more target-consistent level of 3%. The odds of a cut to UK interest rates in May have risen this morning, following the drop in inflation from 3% to 2.8% in February. The money markets are now indicating there is a 55% chance of a cut at the Bank of England’s next monetary policy decision, scheduled for 8 May (which is turning into something of a nail-biter). Before the inflation data hit the wires, a cut in May was a 45% possibility according to money market pricing, with ‘no change’ at 55%. Those odds have now flipped. David Morrison, senior market analyst at Trade Nation, says: “UK inflation, as measured by the CPI, rose 2.8% in the 12 months leading up to February. This was lower than the 2.9% expected. This still remains above the Bank of England’s 2% target but brings some positive news ahead of Rachel Reeve’s spring budget announcement today. “There was an instant market reaction. Sterling fell against both the US dollar and the euro, while futures on the FTSE 100 stock index shot up. This dip in inflation increases the probability that the Bank of England may consider another rate cut over the coming months. Although members of the rate setting MPC are unlikely to react to a single piece of data and will want to see the numbers trend lower over time back towards their 2% target.” [The Bank will also be watching services inflation, which remained unchanged at 5.0% last month] Sarah Coles, head of personal finance at Hargreaves Lansdown, warns that today’s drop inflation could reverse in a month’s time: “Like an over-refreshed pub-goer after midnight, inflation has staggered uncertainly in a new direction again, falling from 3% to 2.8%. It’s not a major shift, but it’s not what markets were expecting. It’s expected to lurch back to growth again next month, and then keep rising in April once the price rises of Awful April kick in. There was no change to food inflation last month, but retailers are warning that prices will accelerate later this year as rising costs are passed onto consumers. Food and non-alcoholic beverages inflation was 3.3% in the year to February, matching January’s reading. Kris Hamer, director of insight of the British Retail Consortium, warns that “Headline inflation fell marginally in February, driven by marginal drops in housing and household services and clothing and footwear entering deflation. Despite continued cost pressures, namely energy price volatility, food inflation remained unchanged. There was good news as some dairy products such as milk, cheese and eggs all saw price drops on the month. Heavy clothing and footwear discounting continued into February, as fashion sales continue to suffer due to unseasonal weather throughout the month.” “Retail operates on tight margins and it would be impossible to absorb all £5bn of new costs which hit the industry in April. Food inflation has jumped significantly in recent months and is forecast to hit 5% by the end of 2025 as a result of the costs arising from the Budget. On top of this, retailers are still burdened by an outdated business rates system. It is vital that the government’s reform of business rates doesn’t impose additional costs onto retailers. Reform must leave no shop paying more.” Sterling is weakening a little, after UK inflation fell by more than expected this morning. The pound has lost nearly a third of a cent against the US dollar to $1.2915. Kathleen Brooks, research director at XTB, says: The market reaction to this data has been minimal, as the focus remains on the Spring Statement later today. The pound has dropped slightly, but GBP/USD is down less than 20 pips so far on Wednesday, the bond markets are not open, but we think that UK Gilts will also have a mild reaction to this data. Here’s a chart showing the various price changes that pulled UK inflation down to 2.8% last month. Core inflation has also slowed in February, despite prices rising steadily in the services sector. Core CPI (which excludes energy, food, alcohol and tobacco) rose by 3.5% in the 12 months to February 2025, down from 3.7% in the 12 months to January. The CPI goods annual rate slowed from 1.0% to 0.8%, while the CPI services annual rate was unchanged at 5.0%. Yael Selfin, chief economist at KPMG UK, says the UK’s central bankers will be cheered by the drop in core CPI: “The Bank of England will be reassured by today’s fall in underlying inflation, with core inflation easing. We expect underlying inflationary pressures to fall further over the coming months. That will hopefully allow the MPC to look through the expected near-term increase in headline inflation and resume cutting interest rates in the upcoming May meeting. “Goods inflation fell to 0.8% in February, however ongoing trade frictions could push prices higher. With the potential imposition of tariffs, the cost of imported goods could increase, creating additional cost pressures for both businesses and households. “Headline inflation eased to 2.8%, driven by a fall in the price of clothing. We expect headline inflation to rise over the coming months, driven by higher energy prices as well as a further increase in food prices.” ONS chief economist Grant Fitzner reports that alcoholic drinks prices have risen: “Inflation eased in February. Clothing prices, particularly for women’s clothes, was the biggest driver for this month’s fall. “This was only partially offset by small increases, for example, from alcoholic drinks.” Today’s UK inflation report shows that prices of alcohol and tobacco rose by 5.7% in the year to February, up from 4.9% in January. Cheaper clothing pulled the UK’s inflation rate down last month. Overall prices for clothing and footwear fell by 0.6% in the 12 months to February 2025, compared with a rise of 1.8% in the 12 months to January February’s figure was the first negative annual rate since October 2021, due to more discounting by retailers last month as they tried to shift stock. The inflation report explains: The easing in the annual rate was mainly the result of a large downward effect from garments for women, with small downward effects coming from a range of women’s clothing items. There were additional small downward effects from children’s clothing, and other clothing and clothing accessories, such as hats and women’s scarves. Newsflash: UK inflation has fallen back to 2.8%, in a boost to Rachel Reeves a few hours before she delivers her spring statement. The Office for National Statistics said annual inflation as measured by the consumer prices index cooled last month, dropping from 3% in January. That slightly lowers the cost of living pressure on families, but also means prices are still rising faster than the Bank of England’s 2% target. On a monthly basis, CPI rose by 0.4% in February 2025, compared with a rise of 0.6% in February 2024. The largest downward contribution came from clothing, the ONS reports. The Prospect union are urging the government to make sure the new funds for defence are spent in the UK, rather than on overseas weapons makers. Mike Clancy, General Secretary of Prospect, says: “The need to invest in defence becomes more obvious by the day, and this new money is an important down payment on this national priority. “New investment in the sector must go towards creating good, well-paid jobs in the UK’s world leading defence industry and not sending work abroad as has happened too often in the past. “Government must also go further in investing in skilled staff in the MOD in areas like procurement, to guarantee we have the expertise at the heart of government to ensure that extra money is spent well in the national interest.” You can get up to speed on the tricky economic picture facing the chancellor here: Rachel Reeves’s spring statement plans have suffered a last-minute shock. Britain’s fiscal watchdog, the Office for Budget Responsibility, has rejected the government’s estimate of savings from the changes announced last week, which will force the chancellor to make additional welfare cuts today to keep within her fiscal rules. Final estimates from the OBR suggested the changes announced by Liz Kendall, the work and pensions secretary, which included tightening the criteria for the personal independence payment (Pip), would not save the £5bn needed to keep within Reeves’s self-imposed borrowing limits. The chancellor is expected to announce an additional £500m in benefits cuts to make up part of the £1.6bn shortfall, first reported by the Times – with the rest of the gap filled by spending cuts elsewhere. Here’s the full story: According to Sky News, Reeves is now expected to announce that universal credit (UC) incapacity benefits for new claimants, which were halved under the original plan, will also be frozen until 2030 rather than rising in line with inflation. There will also be a small reduction in the basic rate of UC in 2029, with the new measures expected to raise £500m, they add. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. It’s a red letter day in the City of London, as investors await the latest UK inflation report, and then an update on the nation’s finances. On inflation, due at 7am, economists expect a small slowdown in the rising cost of living. The Consumer Prices Index is forecast to have risen by 2.9% in the year to February, down slightly on January’s 3%. That would still show prices rising faster than the Bank of England’s 2% target but would at least be a move in the right direction for strugging households. However, any relief may be short-lived, with many bills set to rise in April. The BoE predicts inflation will hit 3.75% this autumn. Economist Robert Wood and Elliott Jordan-Doak of Pantheon Macroeconomics predict: “February should be the calm before the storm of annual price resets, as Government-set price hikes and tax rises drive up headline CPI inflation to 3.5% in April. A drop in inflation would be welcome news for Chancellor Rachel Reeves, as she prepares to deliver her spring statement. This was initially intended to be a low-key update, but Reeves is now expected to announce spending cuts for some Government departments, and cuts to sickness and disability benefits which will be very unpopular with Labour MPs. Reeves is in a bind because government borrowing is running ahead of estimates, while growth has been disappointing. The Office for Budget Responsibility is expected to lower its growth forecasts, and could halve its growth projection for 2025 from 2% to near 1%. The rise in UK government borrowing costs since last October’s budget has also eaten into the chancellor’s limited headroom to keep within her debt limits. Reeves is expected to promise “security and national renewal”, alongside familiar pledges to kickstart economic growth and protect working people. She’ll also announce a further £2.2bn funding increase for defence from April, to keep the country safe. Reeves is expected to say she is proud of what has been delivered in the nine months since the general election: “Restoring stability to our public finances; giving the Bank of England the foundation to cut interest rates three times since the General Election; rebuilding our public services with record investment in our NHS and bringing down waiting lists for 5 months in a row; and increasing the National Living Wage to give 3 million people a pay rise from next week. The agenda 7am GMT: UK inflation report for February 9.30am GMT: UK house prices and rents report 12.30pm GMT: Rachel Reeves delivers the spring statement 1pm GMT (approx): Office for Budget Responsibility publishes its latest economic and fiscal outlook</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Rachel Reeves blamed ‘global uncertainty’ as she announced swingeing cuts to welfare and other public spending. UK’s growth forecasts for this year had been halved from 2% to 1% by the Treasury watchdog. Reeves said measures would turn predicted £4.1bn hole in the public finances back into a £9.9bn surplus within five years.</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Time to wrap up…. Activity across the UK’s private sector has accelerated this month, easing some pressure on chancellor Rachel Reeves ahead of the spring statement on Wednesday. The latest UK PMI Composite Output Index shows private sector growth is running at a six-month high in March, helped by strong growth in the services sector. But manufacturing contracted, as rising global economic uncertainty and fears of US tariffs hit demand for British goods. Donald Trump has calmed investors’ nerves, by suggesting he could take a targeted approach to the new tariffs inked in for 2 April. However, the US president has also surprised markets by announcing new ‘secondary tariffs’ on Venezuela’s oil and gas exports. The Irish government has warned that the country could lose up to 80,000 jobs if Donald Trump launches a trade war with the EU, and has hit back at accusations by the US that Ireland is operating a “tax scam”. In other news… Sales of new Tesla cars slumped in Europe last month in the latest indication of a potential buyer backlash over Elon Musk’s high profile and controversial behaviour since becoming a leading figure in Donald Trump’s administration. The UK’s transport secretary has said she would “struggle to sleep” if she had been running Heathrow airport, amid reports that its chief executive slept during the early hours of an unfolding crisis on Friday. Hundreds of hospitality companies have called on the UK’s competition watchdog to investigate the energy market amid fears that small businesses may have been overcharged. The oil price is up 1% this afternoon, as traders digest the new ‘secondary tariff’ on Venezuela’s energy exports announced by Donald Trump today. Brent crude has risen to $72.83 per barrel, the highest since 3 March. Traders will be calculating that Venezuela’s oil and gas customers may scramble to buy supplies from elsewhere, to avoid incurring a 25% tariff on their exports to the US. A looming trade dispute between the US and the EU is “extremely concerning”, the governor of the Central Bank of Ireland said, as he warned that the country is in a period of “significant change and volatility”. Gabriel Makhlouf said that forecasting in a time of “extreme uncertainty” is challenging, adding that he was reluctant to “speculate” on the impact of US tariffs on the Irish economy. He said on Monday that the views of the Central Bank are in line with those reflected in a report on the potential impact of tariffs from the Department of Finance and Ireland’s Economic and Social Research Institute (ESRI). It found that an intense trade dispute between the US and the EU would risk increased prices, fewer new jobs and slower growth in the economy. Makhlouf explained: “My overall sense is that we’re living in a period of significant change, significant volatility, and the most important thing that we can do is keep a clear head, understand exactly what is happening, and then make a decision on how to respond and start talking about what our view is as to its impact. “The last thing I’d want to do is to start speculating in a way that was just uncomfortable.” Trade data earlier this month shows that China was the largest market of Venezuela’s oil, receiving some 503,000 bpd, Reuters reported. The US was the second largest receiver with 239,000 bpd, followed by Europe with 69,200 bpd and India with 68,000 bpd. Venezuela’s political ally Cuba received some 42,000 bpd of crude and fuel. The US, though, has been cutting its links – and has ordered Chevron to wind down their activities in Venezuela. Newsflash: Donald Trump has announced a new “secondary tariff” on countries which buy oil and gas from Venezuela. In a post on his Truth Social site, the US president says he is imposing the levy because Venezuela has “purposefully and deceitfully” sent tens of thousands of criminals to the US. Trump writes: Among the gangs they sent to the United States, is Tren de Aragua, which has been given the designation of “Foreign Terrorist Organization.” We are in the process of returning them to Venezuela — It is a big task! In addition, Venezuela has been very hostile to the United States and the Freedoms which we espouse. Under Trump’s new ‘secondary tariff’, any country that purchases oil and/or gas from Venezuela will be forced to pay a tariff of 25% on all its imports to the US. All documentation will be signed and registered, and the Tariff will take place on 2 April, Trump adds, declaring it will be “LIBERATION DAY IN AMERICA”. [Reminder: tariffs are paid by the company or consumer importing goods, not by the exporter]. Heather Long of the Washington Post is alarmed by the drop in the US manufacturing PMI this month (see here). She fears it signals a potential manufacturing downturn/recession, posting: Yikes. US manufacturing is feeling the tariff pain. The US dollar is having a solid day, and has crept up to its highest level in over two weeks against a basket of major currencies. This has pulled the Japanese yen down to ¥150.0, its weakest level since 3 March, while the euro has dropped to $1.079, its lowest since 7 March. The pick-up in activity in the UK private sector this month (see earlier post) could take some pressure off the Bank of England to cut interest rates this year. This afternoon, the City money markets are only pricing in 43 basis points of cuts to Bank Rate this year. That implies fewer than two quarter-point cuts – last week, two cuts were still priced in. UK inflation is expected to fall to 2.9% per year on Wednesday, when the latest consumer prices data is released, down from 3% in January but still above the Bank’s 2% target. BoE poliicymakers were split 8-1 last week in favour of leaving rates on hold at 4.5%. The next meeting, at the start of May, looks like a coin-toss, with a 47% chance of a cut and 53% for no change again. Confidence among US businesses is falling this month, as companies grow increasingly cautious about the economic outlook, a new survey shows. The latest poll of purchasing managers across American companies has found that confidence in the outlook has deteriorated further this month. Business expectations for the year ahead have dropped to their second-lowest since October 2022, with companies reporting worries about customer demand and the impact of some of Donald Trump’s administration’s policies. The S&amp;amp;P Global Flash US PMI report shows that manufacturing output fell into decline this month with new orders growth coming close to stalling in the goods-producing sector. US factories also reported fewer instances of output having been boosted by the “front-running” of tariffs (where customers place more orders than usual, to avoid having to pay new levies if the US trade war escalates). The report says: However, export sales showed the smallest decline for nine months thanks to rising orders in particular from Canada, Germany and other EU countries, hinting at some further efforts to fulfil orders ahead of tariff implementation. But while manufacturing shrank, output growth in the services sector picked up – from a 15-month low in February. And that led to faster growth in the wider economy – the flash US PMI Composite Output Index has risen to a three-month high of 53.5, from February’s 51.6. That could calm fears that the US could be slipping into a recession. Chris Williamson, chief business economist at S&amp;amp;P Global Market Intelligence, says: “A welcome upturn in service sector activity in March has helped propel stronger economic growth at the end of the first quarter. However, the survey data are indicative of the economy growing at an annualized 1.9% rate in March and just 1.5% over the quarter as a whole, pointing to a slowing of GDP growth compared to the end of 2024. “Near-term risks also seem tilted to the downside. Growth is concentrated in the service sector as manufacturing fell back into decline after the frontrunning of tariffs had temporarily boosted factory output in the first two months of the year. Similarly, some of the March upturn in services was reportedly due to business picking up after adverse weather conditions had dampened activity across many states in January and February, which could prove a temporary bounce. Williamson also warned that business confidence in the outlook has “darkened”, mainly due to growing worries over negative impacts from recent policy initiatives from the Trump White House. he says: Most widely cited were concerns about the impact of Federal spending cuts and tariffs. A key concern over tariffs is the impact on inflation, with the March survey indicating a further sharp rise in costs as suppliers pass tariff-related price hikes on to US companies. Firms’ costs are now rising at the steepest rate for nearly two years, with factories increasingly passing these higher costs onto customers. Shares in Tesla have jumped 6.6% to $265.23, as Elon Musk’s electric car company recovers some of its recent losses. Ding ding! Stocks have opened higher in New York, as investors welcome signals that Donald Trump may take a more measured approach with his next flurry of tariffs. The Dow Jones Industrial Average has jumped by 441 points, or 1.05%, to 42,426 points, while the broader S&amp;amp;P 500 index is up 1.4%. The tech-focused Nasdaq Composite is 1.6% higher. As we covered in the introduction (see here), Trump has hinted that he could show flexibility when drawing up the new trade levies to be announced on 2 April, and take a more targeted approach than feared. Chinese auto giant BYD has overtaken Tesla for sales last year, as it continues to dominate the electric car markets. Shenzhen-based BYD revenue of 777bn yuan ($107bn) for the 12 months to 31 Deceber 2024, beating forecasts of 766m yuan. That means BYD brought in more sales than Tesla, which reported total revenues of $97.69bn for 2024. Bloomberg has more details: BYD also sells about the same number of EVs as Tesla — 1.76 million in 2024 versus 1.79 million — but, when all of its other passenger hybrid car sales are included, it’s much larger. BYD’s total deliveries last year climbed to 4.27 million, almost as much as Ford Motor Co. BYD has forecast it can sell between 5 million to 6 million vehicles this year. It’s already off to a strong start, with sales in the first two months of 2025 up 93% year-on-year to 623,300 units. For the last quarter of 2024, BYD reported a record net profit of 15bn yuan ($2.1bn). BYD has been making strides into Europe with its entry-level Dolphin and its more premium Seal car, having become China’s largest manufacturer of electric cars. BYD made a stir last week by reporting that it has developed a new charging system that would make it possible to charge an EV as quickly as it takes to refill with petrol. Back in the UK, houses across England and Wales have become less unaffordable than at the height of the pandemic. The Office for National Statistics has reported that housing affordability in England and Wales returned to its pre-pandemic levels last year. New data today shows that the median average home in England, at £290,000, cost 7.7 times the median average earnings of a full-time employee (£37,600) in 24. In Wales the average home (£201,000) was 5.9 times annual earnings (£34,300). The ONS explains: Affordability in England and Wales in 2024 has returned to its pre-coronavirus (COVID-19) pandemic levels after a sharp increase between 2020 and 2021 (worsening affordability); median house sales prices have increased by 1% since 2021, while average earnings have increased by 20%. The report also found: In 2024, 9% of local authorities (LAs) (27) had homes bought for less than five times workers’ earnings on average and were therefore deemed affordable; this is the highest proportion since 2015, but well below that at the start of the series in 1997 (88% of areas). Housing affordability improved in 289 of the 318 LAs in England and Wales (91%) and worsened in 28 (9%) since 2023. The most affordable LAs in 2024 were Blaenau Gwent (with a ratio of 3.8), Burnley (3.9) and Blackpool (3.9); the least affordable was Kensington and Chelsea (27.1, which was about seven times less affordable). Between 2019 and 2024, 4 of the 10 largest increases in affordability ratios (worsening affordability) were in the East Midlands, while the 10 largest decreases in affordability ratios have all occurred in LAs in London Sales of Tesla’s electric cars in Europe fell behind Volkswagen and the BMW group last month, data by research platform JATO Dynamics shows. In a report, JATO said that Elon Musk’s role in politics, rising competition in the EV market and the phasing out of the existing version of its best-selling vehicle, the Model Y, have all impacted sales. Felipe Munoz, Global Analyst at JATO Dynamics, explains: “Brands like Tesla, which have a relatively limited model lineup, are particularly vulnerable to registration declines when undertaking a model changeover.” Tesla’s battery-electric vehicle (BEV) registrations in 25 European Union markets, the UK, Norway and Switzerland fell on average by 44% from the same month of 2024, to under 16,000 cars sold in February, according to JATO. Its market share in the month fell to 9.6%, the lowest February reading in the last five years. By comparison, Volkswagen’s BEV sales were up 180% to under 20,000 cars, while the BMW brand and BMW-owned Mini, combined, sold almost 19,000 BEVs in February, the data showed. Here’s some expert reaction to this morning’s news that UK private sector growth has hit a six-month high this month. Ashley Webb, UK economist at Capital Economics: Despite the rise in the composite activity PMI in March, it’s still consistent with the near-stagnation in GDP in recent quarters continuing in Q1. More positive were signs that businesses intend to shed jobs by less than previously feared to cope with higher taxes. But with price pressures still elevated, the BoE will be concerned about the growing upside risks to inflation. Thomas Pugh, economist at audit, tax and consulting firm RSM UK: “The rise in the flash S&amp;amp;P Global UK Composite PMI for March to 52.0 suggests the domestic economy regained a little bit of momentum at the end of Q1, but the manufacturing sector is still suffering. However, this will offer little consolation to Rachel Reeves before her speech on Wednesday, where she will have to announce around £10bn of spending cuts. “The difference between the services and manufacturing sectors was even starker than usual in March. The manufacturing PMI dropped to 44.6, its lowest since September 2023, primarily driven by weak export sales as tariff uncertainty continues to weigh on the sector. Meanwhile, the services PMI rose to 53.2, its highest in almost a year. “The employment balance jumped to 47.4, which still suggests private sector employment is falling. Admittedly, the PMI is probably overstating the weakness in the jobs market. But a weak labour market combined with the input price balance dropping a little may give the Bank of England a bit more confidence to cut interest rates in May. “Overall, it seems like the domestic economy is now finding its feet after a stumble around the budget. But weak global growth and surging uncertainty about US tariff policy is hammering the external sector, especially manufacturing products, dragging on total growth.” Rhys Herbert, senior economist at Lloyds: “The uplift in business activity is testament to the hard work undertaken by businesses when faced with challenging economic and geopolitical conditions. This boost aligns with data from our latest Business Barometer, which shows that confidence rose to its highest level since August 2024, reflecting improved economic optimism and stronger trading prospects across sectors.” Novo Nordisk, the Danish drugmaker, has been unseated from its position as Europe’s most valuable company. The firm behind obesity and diabetes injections Wegovy and Ozempic has been overtaken by German software firm SAP for market capitalisation. Reuters has calculated that at 9am, SAP had a market cap of $340bn, slightly more than Novo Nordisk. SAP produces a range of business application software, and has benefitted from forecasts that its cloud business will benefit from the artificial intelligence boom. SAP’s shares are up 10% so far this year, and up almost 40% over the last 12 months. Novo Nordisk became Europe’s largest company in September 2023, due to strong demand for its weightloss drugs. But last August, Novo Nordisk cut its annual profit expectations after posting weaker-than-expected sales of Wegovy. It also faces the threat of tariffs, especially if Donald Trump continues his push to take control of Greenland from Denmark. The Bank of England has launched the 2025 Bank Capital Stress Test for the seven largest and most systemic UK banks and building societies. The stress test will assess whether UK banks have enough capital to survive a financial crisis. This year’s test will model a “severe global aggregate supply shock” that leads to deep recessions in both the UK and globally. This scenario includes: UK GDP falls by 5% in the early part of the scenario; World GDP falls by 2%; UK unemployment almost doubles to a peak rate of 8.5% in the third year of the scenario, similar to the peak level experienced in the global financial crisis. World trade falls by 20%; Oil and gas prices rise sharply; Inflation peaks at 10% before falling back to the 2% target by the end of the scenario; Bank Rate is increased to a peak of 8% and is then lowered over the scenario as inflation returns to the target; UK residential property prices fall by 28%. The results will be published in the fourth quarter of this year. The banking sector has generally passed previous stress tests. In 2023, the UK’s largest banks were strong enough to weather a £125bn financial hit during a severe economic downturn, while in 2021 the UK’s top eight banks could withstand a near tripling of national unemployment, a sharp fall in property prices and a large economic contraction. But back in 2014, the Co-operative Bank failed the test, while Lloyds Banking Group and Royal Bank of Scotland only just scraped through. Today’s UK PMI report also shows that business confidence remains shaky this month. Confidence among manufacturers was the weakest since November 2022. However, optimism among service providers edged up to a five-month high. The report says: Service sector firms noted a gradual improvement in sales opportunities and projections for organic growth, despite lingering concerns about constrained business investment and the impact of rising payroll costs on client demand. In the manufacturing sector, there were many concerns about US tariffs and gloomy forecasts for export sales due to volatility in global markets. UK companies are continuing to raise prices at a ‘robust’ rate this month, today’s poll of purchasing managers shows. Prices at the factory gate have accelerated to the fastest rate since April 2023, but this was balanced by a slight slowdown in price growth in the service sector. Thus, the overall rate of output charge inflation was unchanged compared with February. The PMI report says: Forthcoming increases to National Insurance contributions and the National Minium Wage were cited as the main reasons for higher output prices, but there were also sporadic reports of discounting to stimulate sales. UK private sector output growth has climbed to a six-month high. in March, in a pre-Spring Statement boost for chancellor Rachel Reeves. While British manufacturing output is sliding this month, the services sector is growing at a faster rate. This services rebound has lifted the UK PMI Composite Output Index, which tracks activity in the economy, up to 52.0, the highest since last September, up from 50.5 in February. S&amp;amp;P Global, which compiles the PMI report, says that service sector growth was bolstered by renewed improvements in both domestic and overseas sales. But manufacturers were hit by “severe headwinds”, including rising global economic uncertainty and potential US tariffs. The report says: Weak international demand resulted in the fastest decline in manufacturing export sales since August 2023. Moreover, manufacturers reported the steepest downturn in production volumes for nearly one-and-a half years. Here are the details: Flash UK PMI Composite Output Index: 52.0 (Feb: 50.5). 6-month high. Flash UK Services PMI Business Activity Index: 53.2 (Feb: 51.0). 7-month high. Flash UK Manufacturing Output Index: 44.6 (Feb: 47.3). 17-month low. Flash UK Manufacturing PMI: 44.6 (Feb: 46.9). 18- month low. The report also shows that private sector employment is fallling in March for the sixth month running. Companies cited business restructuring, investments in automation and the non-replacement of leavers in response to rising payroll costs – a sign that Reeves’s increase to employers’ national insurance rates, and the minimum wage, is hitting workforce levels. Chris Williamson, chief business economist at S&amp;amp;P Global Market Intelligence said: “An upturn in business activity in March brings some good news for the government ahead of the Chancellor’s Spring Statement, offering a respite from the recent flow of predominantly downbeat economic data. However, just as one swallow does not a summer make, one good PMI doesn’t signal a recovery. The signal from the flash PMI is an economy eking out a modest expansion in March, consistent with quarterly GDP growth of just 0.1%, but with employment continuing to be cut thanks to concern over costs and the uncertain outlook. Confidence is still running close to January’s two-year low. Williamson cautions that the improvement is also being driven by only small pockets of growth, notably in financial services, with consumer-facing business and manufacturers continuing to struggle against headwinds both at home and abroad. He adds: These headwinds include the additional costs imposed on businesses in the Budget, low confidence among businesses and households, and sluggish demand at home and abroad, the latter linked to heightened geopolitical uncertainty resulting from US tariff policies. Worryingly, these headwinds are likely to grow in force as higher National Insurance contributions come into effect in April, coinciding with the anticipated review of US tariff policy on 2nd April, the latter having the potential to further subdue global economic growth and dampen UK trade.” Happy news: the eurozone’s factory sector has returned to growth this month, perhaps thanks to a rush to beat new US tariffs. S&amp;amp;P Global’s poll of purchasing managers from across Europe’s private sector has found that manufacturing production has increased for the first time in two years, even though new orders fell again. Here’s the details (where any reading over 50 shows growth): HCOB Flash Eurozone Composite PMI Output Index at 50.4 (February: 50.2). 7-month high. HCOB Flash Eurozone Services PMI Business Activity Index at 50.4 (February: 50.6). 4-month low. HCOB Flash Eurozone Manufacturing PMI Output Index at 50.7 (February: 48.9). 34-month high. HCOB Flash Eurozone Manufacturing PMI at 48.7 (February: 47.6). 26-month high Dr. Cyrus de la Rubia, chief economist at Hamburg Commercial Bank, says: “Just in time with the beginning of spring we may see the first green shoots in manufacturing. While we should not be carried away by a single data point, it is noteworthy that manufacturers expanded their output for the first time since March 2023. It’s also encouraging, that the index output has risen for three months straight. This is complemented by a much softer fall in new orders and employment. One could pour some cold water on this development arguing that it’s the temporary tariff-related import boom from the US which has driven the improvement in manufacturing. However, given the will of Europe, to invest heavily in defense and infrastructure – in Germany a corresponding historical fiscal package has been approved only last week – hope for a more sustained recovery seems well founded. The price development in the services sector, which is very much under scrutiny of the ECB, will be well received by the doves of the monetary authority. Both input costs and selling prices are rising at a slower pace compared to recent months. Lower input cost inflation points to less pressure from wages which are a key ingredient of input costs in the labour intensive services sector. Meanwhile, in manufacturing, price increases for both selling and purchasing remain moderate, helped along by declining energy costs. Japan’s private sector output is falling this month for the first time since last October, a new poll has found, and at the fastest rate in three years. The latest poll of purchasing managers at Japanese companies shows that manufacturers were hit by worsening demand, while services companies suffered from labour constraints Overall new orders fell for the first time in nine months, while sales in March were notably also dampened by elevated prices. Investors are more concerned than three months ago about the threat from Donald Trump’s trade war, a new poll by Deutsche Bank has found. The survey of 400 people found that the perceived tariff risk has gone up so far this year. On a scale of 0 to 10, where 0 means ‘No additional tariffs’ and 10 means ‘An extreme tariff regime’, 38% of those who took part in the poll plumped for at least 7 – a level that would mean Trump delivering on his pledges during the election campaign. That’s up from 18% who chose 7, 8, 9 or 10 in December. It still means that 62% of respondents reckon Trump will put in sustained tariffs that are softer than his campaign pledges. Deutsche’s global markets survey polled financial professionals from around the world, and also found: European equities are aggressively favoured over the US over the next 12 months but over 5 years this flips back heavily in the US’s favour. So US exceptionalism is expect to return after a continued lull in 2025. Germany is expected to grow at 1.2% on average over the next 5 years with a peak 10yr Bund rate of 3.7% over this period. The US recession risk over the next 12 months is seen at 43% on average but the distribution of responses was very wide. A surprisingly huge majority think this US administration actively want a weaker dollar. Digital marketing group S4 has warned that concerns over tariffs are making its clients cautious. Sir Martin Sorrell, executive chairman of S4, told shareholders that the company is facing challenging global macroeconomic conditions and continued high interest rates. Sorrrell added: The macroeconomic environment in 2025 will remain challenging given significant volatility and uncertainty in global economic policy, particularly tariffs. In geopolitics, US/China relations, Russia/Ukraine and Iran remain volatile issues and therefore clients are likely to remain cautious. S4 reported an 11% fall in like-for-like net revenues for 2024. It has also taken a Non-cash impairment charge net of tax of £280m, due to “trading conditions in the second half of 2024 and the medium-term outlook”. That pushed it into a loss for the year of £306.9m, compared with a £14.3m loss in 2023. European stock markets are up across the board. Germany’s DAX has gained 0.85%, while France’s CAC is up 0.8% and Italy’s FTSE MIB is 0.66% higher. Stocks have opened higher in London, lifted by those hopes that Donald Trump will show flexibility when he announces new global tariffs next month. The FTSE 100 share index is up 0.5%, or 42 points, at 8688 points, which recovers most of Friday’s losses. Mining stocks are leading the rally, with Anglo American (+3.9%), Antofagasta (+3.3%), Glencore (+3%) and Rio Tinto (+2.5%), benefitting from hopes that ‘Liberation Day” might be less damaging to the world economy than feared. A sector upgrade by JP Morgan is also helping the miners. A war of words has broken out between Heathrow and National Grid over the fire which brought the London airport to a standstill on Friday. The chief executive of National Grid sparked the row by claiming that Heathrow Airport had enough power from other substations despite Friday’s shutdown. Following criticism that the power network lacked resilience to cope with the fire at one substation, at North Hyde, John Pettigrew has revealed that two other substations were “always available for the distribution network companies and Heathrow to take power”. Pettigrew told the Financial Times: “There was no lack of capacity from the substations. Each substation individually can provide enough power to Heathrow.” But Heathrow, which had more than 1,000 flights cancelled on Friday, insists it’s not as simple as that. A Heathrow spokesperson says: “As the National Grid’s chief executive, John Pettigrew, noted, he has never seen a transformer failure like this in his 30 years in the industry. His view confirms that this was an unprecedented incident and that it would not have been possible for Heathrow to operate uninterrupted. Hundreds of critical systems across the airport were required to be safely powered down and then safely and systematically rebooted. Given Heathrow’s size and operational complexity, safely restarting operations after a disruption of this magnitude was a significant challenge. In line with our airline partners, our objective was to reopen as soon as safely and practically possible after the fire. The emergency services and hundreds of airport colleagues worked tirelessly throughout Friday to ensure the safe reopening of the airport. Their success meant that over the weekend, we were able to focus on operating a full schedule of over 2500 flights and serving over 400,000 passengers. Lessons can and will be learned, which is why we fully support the independent investigation announced by the Government yesterday.” Keir Starmer has been warned against “appeasing” Donald Trump as he considers reducing a major tax for US tech companies while cutting disability benefits and public sector jobs. His chancellor, Rachel Reeves, confirmed on Sunday that there were “ongoing” discussions about the UK’s £1bn-a-year digital services tax that affects companies including Meta and Amazon. She expressed optimism that Trump’s 25% tariffs on British steel could be removed in any deal, but did not deny there could be changes to the digital services tax, which the US has lobbied against. “You’ve got to get the balance right,” she said. While any changes would not take place in this week’s spring statement, the Liberal Democrats warned Labour was “in danger of losing its moral compass” and it would be “tantamount to robbing disabled people to appease [Elon] Musk and Trump”. Even if the Trump White House takes a more ‘flexible’ and targeted approach, “Liberation Day’ is likely to bring in steep new trading barriers at the US border. Stephen Innes, managing partner at SPI Asset Management, explains: U.S. equity futures caught a bid in early Asia trading as markets latched onto signs that the next round of Trump-era tariffs may be more calibrated than initially feared. While the White House is still moving ahead with its April 2 “Liberation Day” deadline, the tone appears to be shifting—from a broad-based barrage to a more targeted, reciprocal framework. According to sources close to the matter, the administration now plans to narrow its focus. It will apply tariffs to a group of nations dubbed the “dirty 15”—countries with persistent trade imbalances that collectively represent the lion’s share of U.S. imports. These nations will bear the brunt of the tariff hikes, while others could be hit with more modest levies. The White House is reportedly easing back on industry-specific tariffs, such as those on autos, semiconductors, and pharmaceuticals. These tariffs had been expected to drop alongside the reciprocal action. For now, those sectoral tariffs may be shelved, although insiders note that planning remains fluid and subject to change. Nonetheless, the administration’s April 2 tariff salvo could lift duties on the U.S.’s largest trading partners to levels not seen in decades. According to sources familiar with the planning, countries landing on the “dirty 15” list should brace for sharply higher, potentially punitive tariff rates, marking a dramatic escalation in the push for trade “reciprocity.” The message from Washington is clear: imbalanced trade comes with a price tag—and it’s about to go up. Financial markets have made an optimistic start on Monday with U.S. stock futures rising and the dollar firm, Reuters reports. S&amp;amp;P 500 futures are up about 0.</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>US president announces new ‘secondary tariff’ on Venezuela’s oil and gas exports. Brent crude has risen to $72.83 per barrel, the highest since 3 March. Irish government warns country could lose up to 80,000 jobs if Donald Trump launches a trade war with the EU.</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Londoners might not bat an eyelid at paying £5 for a pint but the national average is poised to rise above that watermark for the first time, with publicans blaming tax rises introduced by the chancellor, Rachel Reeves. The sobering milestone is likely to be reached next month, according to research by Frontier Economics, with the average price of a pint of beer on course to hit £5.01, up from £4.80. The British Beer and Pub Association (BBPA), which commissioned the research, said landlords had been left with no choice but to raise prices to offset tax rises that are due to come into force in April. Pubs will face greater overheads due to an increase in the national minimum wage, a rise in national insurance rates and a decrease in the threshold at which they start paying out national insurance. Discounts on business rates paid by hospitality firms will also be cut from 75% to 40% from April. The net cost to the pubs sector of these measures, introduced in last October’s budget, will hit £650m in total, the trade body said. Last week the brewer Shepherd Neame, maker of ales including Spitfire and Bishops Finger, said it would raise its beer prices in response to rising taxes. Emma McClarkin, the chief executive of the BBPA, said: “The cumulative impact of these taxes and regulations is now plain to see and it is highly unfortunate that the only way many pubs can remain viable is to pass on the array of upcoming costs to consumers. “No one wants to see the cost of an average pint increase by a further 21p and break the £5 average pint barrier that will be required for pubs to maintain their punishingly slim profit margins.” Pubs and the wider hospitality sector have struggled to recover from the impact of enforced closures during the Covid-19 pandemic, which left many with crippling debt burdens. The sector’s budding recovery was then hampered by inflation and the accompanying cost of living crisis. The number of pubs fell below 39,000 for the first time in December 2024 after hundreds of closures, according to the property data company Altus Group. “It is more urgent than ever that government looks at ways to cap or reduce the costs of doing business so we can keep pubs open, preserve their community value and make sure the price of a pint remains affordable for all,” said McClarkin.</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Average price of a pint of beer on course to hit £5.01, up from £4.80. Pubs will face greater overheads due to an increase in the national minimum wage, a rise in national insurance rates and a decrease in the threshold at which they start paying out national insurance.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Time to wrap up… The European Commission has accused the US tech companies Google and Apple of breaking its digital rules, in a landmark action that could escalate transatlantic tension with Donald Trump. The US president has sought to exert pressure on the EU to back away from tougher regulation of American technology groups, warning that he could retaliate by imposing tariffs on foreign companies. But on Wednesday, the commission pressed ahead with enforcement action against Apple and Google’s parent company Alphabet, two of the world’s five largest companies by stock market value, accusing them of breaking the EU Digital Markets Act (DMA). Turkish assets have been rocked by the news that police have detained Istanbul’s mayor Ekrem İmamoğlu, the main political challenger to President Recep Tayyip Erdoğan. Turkey’s BIST 100 share index has slumped almost 9% by the close of trading, while the lira crashed to a record low – before recovering slightly; it’s now down 2.7%. The Bank of Japan has warned that tariffs and trade war threats are creating heightened uncertainty, as it left interest rates on hold today. Stocks are rallying on Wall Street, ahead of tonight’s interest rate decision by the US Federal Reserve. Bank Santander is to close 95 branches across the UK, with the loss of up to 750 jobs – here’s the list. The value of Elon Musk’s social media platform, X, has reportedly soared back to the $44bn he paid for it, in a dramatic reversal of fortunes since the billionaire became a key ally of Donald Trump. The EC has pressed on with action against Google and Apple, despite the risk of potential retaliation by the US, as Donald Trump has previously criticised European fines against American companies. As the FT explains: The US president is considering tariffs on countries that levy digital services taxes against American companies. According to a memo released last month, Trump said he would look into taxes and regulations or policies that “inhibit the growth” of US corporations operating abroad. Oliver Bethell, Google’s senior director for competition, has said “today’s findings now increase the risk of an even worse experience for Europeans.” The EU’s rulings haven’t hurt Apple and Alphabet’s stock. Both company’s shares are rising today, as Wall Street pushes higher ahead of the Federal Reserve interest rate decision later today. Apple are up 1.5%, while Alphabet are 1.1% higher. EU antitrust chief Teresa Ribera has defended the EC’s decision to push Apple to open up its operating systems more to connected devices, saying: “With these decision, we are simply implementing the law, and providing regulatory certainty both to Apple and to developers.” Apple has slammed the EU order, saying it would hurt users and help its rivals. It says: “Today’s decisions wrap us in red tape, slowing down Apple‘s ability to innovate for users in Europe and forcing us to give away our new features for free to companies who don’t have to play by the same rules.” The European Commission has accused Google and Apple of failing to meet its digital rules. In a double-whammy of action against US Big Tech, Brussels has hit Google’s parent company, Alphabet, with two charges of breaching the Digital Markets Act, and is also pushing Apple to open up its ecosystem to rivals. The EC has taken a “preliminary view” that Google Search treats Alphabet’s own services more favourably compared to rival ones, breaching the requirement to treat third-party services in a “transparent, fair and non-discriminatory” way. It says: Alphabet treats its own services, such as shopping, hotel booking, transport, or financial and sports results, more favourably in Google Search results than similar services offered by third parties It has also concluded that Google Play does not comply with the DMA, as developers who use the app marketplace are prevented from freely steering consumers to other channels for better offers. Alphabet can now respond to the Commission’s findings; if the preliminary views are ultimately confirmed, the Commission would conclude that the company is indeed not complying with the DMA. The DMA is designed to ensure fair competition and limit the power of large tech companies. It designated companies like Alphabet, Amazon, Apple, Meta, and Microsoft as “gatekeepers”, meaning they can face large fines for non-compliance. Apple has been ordered to open up its closed ecosystem to rivals, to help third parties develop products and services. Firstly, the EC wants Apple to give device manufacturers and app developers improved access to nine iOS connectivity features, which are mainly used for connected devices such as smartwatches, headphones or TVs. The EC says: As a result, connected devices of all brands will work better on iPhones. Device manufacturers will have new opportunities to bring innovative products to the market, improving the user experience for consumers based in Europe. The measures ensure that this innovation takes place in full respect of users’ privacy and security as well as the integrity of Apple’s operating systems. Second, it is telling Apple to “improves the transparency and effectiveness of the process” for developers who are interested in obtaining interoperability with iPhone and iPad features. The Commission explains: Developers will benefit from a fast and fair handling of their interoperability requests. The measures will accelerate their ability to offer a wider choice to European consumers of innovative services and hardware that interoperate with iPhones and iPads. The specification decisions are legally binding, it concludes. Chancellor Rachel Reeves has announced a new “strategic steer” for the UK’s National Wealth Fund. The tweak will send the Fund down a path towards higher risk projects, as part of the drive for faster economic growth, while also supporting clean energy and national security. The Treasury says clean energy, advanced manufacturing, digital technologies, and transport have been set a “new priority sectors” for the National Wealth Fund. This means money will be invested across the United Kingdom in projects like carbon capture, green hydrogen, gigafactories, green steel, and ports, they say, by using public money to attract private investment too. The National Wealth Fund’s economic capital limit is being increased from £4.5bn to £7bn, allowing it take on more risk. Reeves says: By directing tens of billions of pounds into the UK’s industrial strengths, we’ll deliver the high-skilled, high-paid jobs of the future in every corner of the country. The government is also looking for a new CEO for the Fund, as John Flint – who has been turning the UK Infrastructure Bank into the National Wealth Fund – is stepping down in the summer. Small investors did their bit for Britain last month, by buying the most gilts (government debt) on record. Financial services firm Hargreaves Lansdown reports that trading in gilts on its platform in February was 63% higher than in January (based on net buys). It’s the highest monthly trading value on direct gilts on the HL platform on record, suggesting that investors have been tempted by the relatively attractive yields on offer. Hargreaves adds: Values bought on platform year to date are nearly 60% of the total value traded throughout 2024 (net buys). There has been a 32% increase in the number of our clients that hold gilts compared to 12 months ago. Retail investor demand for gilts has been big enough to impact prices recently. Stocks have opened higher on Wall Street, ahead of the Federal Reserve’s interest rate decision in over four hour’s time. The S&amp;amp;P 500 has risen by 18 points or 0.33% to 5,633, bringing some relief to investors who have seen the share index fall into correction territory this month. Bloomberg are also reporting that Turkish lenders sold around $8bn this morning to support the lira after the currency plunged as much as 11% following the detention of Istanbul mayor Ekrem İmamoğlu. The intervention in the lira market was carried out through multiple lenders, they add. That would explain why the lira recovered, partially, from its earlier slump. The Turkish lira sell-off could be “a catalyst for major contagion” to other emerging markets, warns Robin Brooks, senior fellow at The Brookings Institution. Bloomberg reports that Turkey’s financial markets are sinking ‘the most in the world’ today: Turkey’s lira sank, an equity selloff triggered a trading halt, and government bond yields surged to the highest levels this year as investors dumped the nation’s assets after the arrest of a key rival to President Recep Tayyip Erdogan. The lira plunged more than 10% to new record lows on news of the arrest early on Wednesday, before paring losses to about 6% as of noon in Istanbul. The benchmark Borsa Istanbul 100 Index was also down 6%, with the banking sub-index dropping more than 9%. The declines were the worst in the world among respective asset classes. The sell-off on the Istanbul market is gathering speed, following the arrest of Istanbul’s mayor Ekrem İmamoğlu. The BIST 100 share index is now down over 8% in afternoon trading. Tomasz Wieladek, an analyst at T Rowe Price, has described the crackdown as “a wake-up call for everybody”, the FT reports. Wieladek added that “assets will probably continue to sell off further”, noting that Turkey’s central bank had limited firepower to defend the currency. The average US 30-year mortgage rate has risen for the first time since early January, dampening demand in America’s housing market. The contract rate on a 30-year mortgage climbed 5 basis points to 6.72% last week, up from the lowest level this year, according to data from the Mortgage Bankers Association. The rate on a 15-year fixed mortgage also rose. Rates rose as investors tried to assess whether trade conflict would push up US inflation, leading to higher borrowing costs. The Daily Mail reports that Topshop and Topman have “sent shoppers into meltdown with a bombshell announcement” five years after they vanished from the high street. Apparently, there’s a kerfuffle about a social media post showing a couple standing on an industrial rooftop below a huge Topshop sign. Cutting to black, a message says: ‘We missed you too’. Very touching, I’m sure you’ll agree. And the Mail insists that Brits have been sent “into a frenzy”, adding: ‘Topshop announcing they’re returning to the high street is a joy only millennial girlies will understand. We’ve missed you x,’ one person wrote on X. ‘I feel like my parents just got back together,’ another fan said on Instagram, while a second one joked: ‘Millennials everywhere are screaming, crying &amp;amp; throwing up… I’m one of them.’ Celebrating the news, another person on Instagram wrote: ‘My wardrobe and my life just fell back into place. Might start going out again.’ That’s the spirit! However…. sources at Asos, which owns a stake in Topshop, report that the advert is plugging a dedicated Topshop website – which we reported last year will be launched by next summer. So this doesn’t appear to be the grand return to the high street, yet anyway… Bentley sales fell by more than a fifth in 2024 amid weak Chinese demand, as the British luxury car brand braces for further disruption from Donald Trump’s trade wars. The manufacturer, based in Crewe, Cheshire, delivered 10,600 cars in 2024, down 21.5% from the 13,560 in 2023, according to figures published by its German parent company. Bentley’s boss, Frank-Steffen Walliser, had declined to share sales figures earlier this week. However, the sales were included in data published by Audi, the part of Germany’s Volkswagen that controls the Audi, Bentley and Lamborghini premium and luxury brands. Bentley blamed the decline in sales on weakness in China in particular. The Chinese economy has been hit by a persistent property crisis, which has weighed on demand for luxury products. Sales were down only 7% in the final quarter of 2024, suggesting that the slump may have eased towards the end of the year. However, Walliser warned this week that the outlook was clouded by the prospect of tariffs on cars threatened by Trump. Bentley will raise costs for consumers if tariffs are imposed. In the UK utility world, Southern Water has reportedly asked some of its creditors to write off part of their debt. Bloomberg says the request comes as owner Macquarie Asset Management injects fresh funds into the company, explaining: The company requested the concession from debt holders at the riskier, holding company level, the people said, asking not to be identified discussing a private matter. Total external debt at this level stood at £380m as of March 2024, the latest figures available. Creditors, however, are unhappy with the terms on offer and are pushing for better ones, they added. Southern will be keen to avoid falling into the sort of crisis that has engulfed Thames Water, which revealed yesterday it has received six takeover approaches. The Financial Times reports today that those potential bidders include Stonepeak, the US infrastructure investor, and London-based fund FitzWalter Capital. Other interested in investing in Thames are US private equity firm KKR, Hong Kong infrastructure investor CKI, hedge fund Covalis Capital and Castle Water. Jenny Ross, money editor at consumer group Which?, has warned that Santander’s branch closures will “come as a real blow to many customers”. She said: “Schemes introduced by the banking industry to protect these services, such as banking hubs, are a good start in plugging gaps left by closing physical branches, but they must be rolled out much more quickly if consumers are to feel their benefits. “The government must hold banks’ feet to the fire to ensure the commitments they’ve made to set up 350 hubs by 2029 are met – and should be prepared to review the target upwards if necessary.” The cost of living squeeze in the eurozone has eased a little. The euro area annual inflation rate fell to 2.3% in February, down from 2.5% in January, statistics body Eurostat has reported. That’s lower than its ‘flash’ estimate of 2.4%, and should cheer policymakers at the European Central Bank who have already cut interest rates six times since last summer. Eurostat reports that the lowest annual rates were registered in France (0.9%), Ireland (1.4%) and Finland (1.5%). The highest annual rates were recorded in Hungary (5.7%), Romania (5.2%) and Estonia (5.1%). Services inflation dipped to 3.7% per year in February, while energy prices were just 0.2% higher than a year earlier, good prices were 0.6% higher, and food, alcohol and tobacco prices were up 2.7%. The Turkish lira has also fallen over 4% against the pound: Stocks are slightly lower in London this morning, where the FTSE 100 share index is down 10 points of 0.11% at 8695 points. Catering firm Compass (-3.5%) are the top faller, after BNP Paribas cut their recommendation to ‘underperform’ from ‘outperform’ . Tesco (-1.7%) are also in the fallers, as concerns linger that rival Asda might launch a price war: M&amp;amp;G are still leading the risers (+2.6%) after reporting a surprise rise in profits, followed by weapons maker BAE Systems (+2.5%) as investors continue to bet on higher defence spending. There’s turmoil in the Turkish financial markets today, after Istanbul mayor Ekrem Imamoğlu, a key rival of President Recep Tayyip Erdoğan. Imamoğlu was arrested as part of an investigation into alleged corruption and terror links, State media reported, with authorities also closing several roads around Istanbul and banned demonstrations in the city for four days in an apparent effort to prevent protests following the arrest. Imamoğlu’s arrest comes a few days before Turkey’s main opposition party, the Republican People’s Party (CHP), was due to hold a primary election in which Imamoğlu was expected to be chosen as its presidential candidate. CHP’s chairman,Özgür Özel, denounced Imamoğlu’s detention as a “coup”. The arrest has shocked investors, who had become used to increased stability in Turkey following the economic crisis of 2023. Stocks have tumbled on the Istanbul stock exchange, where the BIST 100 share index is down 5.7%. The Turkish lira has slumped by 5.6% to 38.6 lira to the US dollar – at one stage it was down over 14% (!) at almost 41 lira/$. The cost of insuring Turkish debt against default has also risen – a sign of investor jitters rising. Turkey’s 5-year credit default swaps has jumped by 23 basis points (0.23 percentage points) to 279 bps, the highest since October 2024, according to S&amp;amp;P Global Market Intelligence. That still shows a low risk of default, though. Superdrug is to open 25 new stores this year in a move that will create around 600 jobs, as the health and beauty retailer said it intends to invest more in beauty treatments and luxury fragrances. The company, which said that investing in larger stores drives its bricks and mortar strategy, currently has 780 shops in the UK and Ireland. “We can see from our sales last year that investing in and increasing the number of large format stores in our estate allows us to accelerate our bricks-and-mortar strategy,” said Nigel Duxbury, Superdrug property director. Superdrug, which said that investment is particularly focused on shopping destinations and retail parks, also plans to refurbish 65 stores this year, and expand multiple sites including in Luton and and Dundee. The company said that investment in its largest stores in recent years helped them deliver sales growth of 25%, and the retailer’s in-store beauty studios saw a 7% rise in sales in 2024. Duxbury says: “We want everyone who enters Superdrug to feel an elevated customer experience.” In January, the firm hailed its “best Christmas ever” after annual like-for-like sales increased by 5.1% in the final weeks of 2024. Santander’s branch closuse plans risk leaving more people strugging to get to a physical bank, rather than relying on electronic banking (when it works…) But… LINK, the ATM network, has just announced 19 new high street locations where it could soon open a shared banking hub. LINK says this “follows the announcement of the closure of 95 branches of Santander”. Banking hubs allow customers from various major banks to access services such as withdrawing or cashing in money, making bill payments or speaking to an adviser. The new earmarked locations are: Bexhill-on-Sea (East Sussex) Billericay (Essex) Dover (Kent) Droitwich (Worcestershire) Dunstable (Beds) East Grinstead (West Sussex) Holyhead (Isle of Anglesey) Ilkley (West Yorkshire) Larne (Antrim, NI) Maldon (Essex) Morley (West Yorkshire) North Walsham (Norfolk) Redcar (North Yorkshire) Saffron Walden (Essex) St Annes on Sea (Lancashire) Turriff (Aberdeenshire) Uckfield (East Sussex) Urmston (Great Manchester) LINK adds that it has now recommended 224 hubs as it continues to assess cash access across the country, and that 139 hubs are up and running as of this week. Here’s the details of the 95 Santander branches which are to be closed (see previous post) Aberdare 17 Victoria Square, Aberdare, Mid Glamorgan, CF44 7LH 24 June 2025 Arbroath 167 High Street, Arbroath, Angus, DD11 1DY 17 June 2025 Armagh 19 Upper English Street Armagh, County Armagh, BT61 7HG 01 July 2025 Blackwood 148 High Street, Blackwood, Gwent, NP12 1YZ 23 June 2025 Blyth 22 Regent Street, Blyth, Northumberland, NE24 1LB 05 August 2025 Bognor Regis 42 High Street, Bognor Regis, West Sussex, PO21 1SP 14 July 2025 Borehamwood 105-109 Shenley Road, Borehamwood, Hertfordshire, WD6 1AX 01 July 2025 Brecon 18 High Street, Brecon, Powys, LD3 7AL 25 June 2025 Brixton 498 Brixton Road, Brixton, London, SW9 8EX 11 August 2025 Caernarfon 1 Bridge Street, Caernarfon, Gwynedd, LL55 1AB 07 July 2025 Camborne 6 Trelowarren St, Camborne, Cornwall, TR14 8AA 07 July 2025 Canvey Island 28 Furtherwick Road, Canvey Island, Essex, SS8 7AF 05 August 2025 Clacton 9 Station Road, Clacton-On-Sea, Essex, CO15 1TD 16 June 2025 Cleveleys 98 Victoria Road West, Thornton, Cleveleys, Lancashire, FY5 1AG 23 June 2025 Colne 3 Church Street, Colne, Lancashire, BB8 0EB 14 July 2025 Colwyn Bay 16 Penrhyn Road, Colwyn Bay, Clwyd, LL29 8PR 24 July 2025 Crowborough 4 High Street, Crowborough, East Sussex, TN6 2PY 23 July 2025 Croydon 128 NE 128 North End, Croydon, Surrey, CR0 1UE 16 June 2025 Cumbernauld 40-42 Teviot Walk, Cumbernauld, Lanarkshire, G67 1NG 07 July 2025 Didsbury 712-716 Wilmslow Rd, Didsbury, Greater Manchester, M20 6DQ 08 July 2025 Downpatrick 49-51 Market Street, Downpatrick, County Down, BT30 6LP 06 August 2025 Dungannon 1 Market Square, Dungannon, County Tyrone, BT70 1AL 23 June 2025 Edgware Road 388-390 Edgware Road, St Johns Wood, London, W2 1DR 12 August 2025 Eltham 73 Eltham High Street, Eltham, London, SE9 1UW 23 June 2025 Exmouth 19 Rolle Street, Exmouth, Devon, EX8 1EZ 15 July 2025 Falmouth 13 Market Street, Falmouth, Cornwall, TR11 3AE 21 July 2025 Farnham 17 The Borough, Farnham, Surrey, GU9 7NG 29 July 2025 Felixstowe 61 Hamilton Road, Felixstowe, Suffolk, IP11 7BS 16 July 2025 Finchley 50 Ballards Lane, Finchley, London, N3 2DP 06 August 2025 Fleet 152 Fleet Road, Fleet, Hampshire, GU51 4BJ 30 June 2025 Formby 12 Chapel Lane, Formby, Merseyside, L37 4HU 11 August 2025 Gateshead Metro Metro Centre 63 The Galleria, Gateshead, Tyne &amp;amp; Wear, NE11 9YP 16 June 2025 Glasgow LDHQ Ground Floor 301 St Vincents St, Glasgow, Lanarkshire, G2 5HN 24 June 2025 Glasgow MX 7 The Avenue, Newton Mearns, Glasgow, Lanarkshire, G77 6EY 23 June 2025 Greenford 28 The Broadway, Greenford, Middlesex, UB6 9PT 24 June 2025 Hackney 392 Mare Street, Hackney, London, E8 1HP 15 July 2025 Hawick 56 High Street, Hawick, Roxburghshire, TD9 9HE 24 July 2025 Herne Bay 135 Mortimer St, Herne Bay, Kent, CT6 5EZ 08 July 2025 Hertford 20 Maidenhead St, Hertford, Hertfordshire, SG14 1EA 29 July 2025 Holloway 408 Holloway Road, Holloway, London, N7 6QF 14 July 2025 Holywell 69 High Street, Holywell, Clwyd, CH8 7TF 13 Aug 2025 Honiton 108 High Street, Honiton, Devon, EX14 1JW 14 July 2025 Kidderminster 2 Josiah Mason Mall, Rowland Hill, Kidderminster, Worcestershire, DY10 1EJ 18 June 2025 Kilburn 131-135 Kilburn High Rd, Kilburn, London, NW6 7HS 17 June 2025 Kirkby 4 St Chad’s Parade, Kirkby, Merseyside, L32 8ZQ 22 July 2025 Launceston 19-21 Broad Street, Launceston, Cornwall, PL15 8AB 16 June 2025 Louth 21 Market Place, Louth, Lincolnshire, LN11 9PD 17 June 2025 Magherafelt 9 Rainey Street Magherafelt, County Londonderry, BT45 5DA 24 June 2025 Malvern 22 Worcester Road, Malvern, Worcestershire, WR14 4QW 02 July 2025 Market Harborough 4 High Street, Market Harborough, Leicestershire, LE16 7NJ 01 July 2025 Musselburgh 123 High Street, Musselburgh, Midlothian, EH21 7EQ 30 June 2025 New Milton 120 Station Road, New Milton, Hampshire, BH25 6LL 28 July 2025 Peterhead 6 Marischal St, Peterhead, Aberdeenshire, AB42 1HU 16 June 2025 Plympton 2 St Stephens Place, Plympton, Devon, PL7 2ZN 14 August 2025 Portadown 24 Market Street, Portadown, County Armagh, BT62 3LD 30 June 2025 Pudsey 5 Lidget Hill, Pudsey, West Yorkshire, LS28 7LG 28 July 2025 Rawtenstall 15 Bank Street, Rawtenstall, Lancashire, BB4 6QS 15 July 2025 Ross-On-Wye 32 High Street, Ross-On-Wye, Herefordshire, HR9 5HD 30 July 2025 Ruislip 73 High Street, Ruislip, Middlesex, HA4 8JB 07 July 2025 Rustington 6 Ash Lane, Rustington, West Sussex, BN16 3BP 05 August 2025 Saltcoats 19 Chapelwell Street, Saltcoats, Ayrshire, KA21 5EB 21 July 2025 Seaford 28 Broad Street, Seaford, East Sussex, BN25 1NH 15 July 2025 Shaftesbury 53 High Street, Shaftesbury, Dorset, SP7 8JE 23 July 2025 Sidcup 39 Sidcup High Street, Sidcup, Kent, DA14 6ED 11 August 2025 St Austell 36-38 Fore Street, St Austell, Cornwall, PL25 5PA 08 July 2025 St Neots 56 Market Square, St Neots, Cambridgeshire, PE19 2HL 30 July 2025 Stokesley 48 High Street, Stokesley, Cleveland, TS9 5AX 31 July 2025 Strabane 64 Main Street, Strabane, County Tyrone, BT82 8AX 23 July 2025 Surrey Quays Unit 34 Surrey Quays Rtl. Cen., Redriff Road, Surrey Quays, London, SE16 7NB, 10 November 2025 Swadlincote 52 High Street, Swadlincote, Derbyshire, DE11 8HS 30 June 2025 Tenterden 32 High Street, Tenterden, Kent, TN30 6AW 07 July 2025 Torquay 41 Fleet Street, Torquay, Devon, TQ2 5DN 17 June 2025 Tottenham 472 High Road, Tottenham, London, N17 9JX 08 July 2025 Whitley Bay 269 Whitley Road, Whitley Bay, Tyne &amp;amp; Wear, NE26 2SS 06 August 2025 Willerby Unit 4 Willerby Shopping Park, Willerby, North Humberside, HU10 6EB 13 August 2025 Wimborne 8 High Street, Wimborne, Dorset, BH21 1HY 04 August 2025 Wishaw 2 Main Street, Wishaw, Lanarkshire, ML2 7AF 22 July 2025 In addition, a date has yet to be announced for when these sites will close: Bexhill 45 Devonshire Rd, Bexhill-On-Sea, East Sussex, TN40 1BD Billericay 97 High Street, Billericay, Essex, CM12 9BD Dover 24 Cannon Street, Dover, Kent, CT16 1ST Droitwich 15 Victoria Square, Droitwich, Worcestershire, WR9 8DE Dunstable 11 High Street North, Dunstable, Bedfordshire, LU6 1HY East Grinstead 56-58 London Road, East Grinstead, West Sussex, RH19 1BJ Holyhead 40 Market Street, Holyhead, Gwynedd, LL65 1UN Ilkley 7 The Grove, Ilkley, West Yorkshire, LS29 9LL Larne 54 Main Street, Larne, County Antrim, BT40 1SP Lytham St Annes 54 St Annes Rd West, Lytham St Annes, Lancashire, FY8 1RF Maldon 53 High Street, Maldon, Essex, CM9 5PT Morley 91 Queen Street, Morley, West Yorkshire, LS27 8EF North Walsham 6 Market Place, North Walsham, Norfolk, NR28 9BP Redcar 60 High Street, Redcar, Cleveland, TS10 3DR Saffron Walden 35 King Street, Saffron Walden, Essex, CB10 1EU Turriff 17 High Street, Turriff, Aberdeenshire, AB53 4ED Uckfield 15 High Street, Uckfield, East Sussex, TN22 1AG Urmston 6-8 Flixton Road, Urmston, Greater Manchester, M41 5AS Santander is to close a fifth of its branches in the UK as part of an overhaul of its network, putting 750 jobs at risk. The retail bank said it would shut 95 out of its 444 high street outlets, and reduce the services or hours at a further 50-plus branches, by June to “better serve the changing needs of customers”. The lender, which said in January that it was not planning any permanent closures this year, said it was also changing 18 branches to become “counter-free” and a further 36 would operate reduced hours. “Closing a branch is always a very difficult decision and we spend a great deal of time assessing where and when we do this and how to minimise the impact it may have on our customers,” a spokesperson for Santander UK said, adding: “As a business, we must move with customers and balance our investment across all the places where we interact with customers, to deliver the very best for them now and in the future.” Savings and investment firm M&amp;amp;G has warned this morning that it faces uncertain times. In its full year results for 2024, M&amp;amp;G points out that: Increased geopolitical uncertainty and market volatility continue to weigh on client sentiment and pose a significant challenge to financial institutions across the globe. Shares in M&amp;amp;G have jumped by 3.3% in early trading, to the top of the FTSE 100 leaderboard, after it susprised investors with a rise in annual profits. M&amp;amp;G’s total adjusted operating profit before tax for 2024 rose 5% to £837m, up from £797m, beating forecasts of a dip to £769m. That was due to a rise in income from asset management. In a week’s time, we’ll be bracing for Rachel Reeves’s spring statement, which may turn in to more of a mini-budget given speculation of possible spending cuts or tax rises to keep within the chancellor’s fiscal rules. But businesses are still getting to grips with the chances made in last autumn’s budget, such as the increase in employer national insurance contributions and the higher minimum wage, which both kick in next month. Shepherd Neame, which claims to be Britain’s oldest brewer, says these “new, and unwelcome, cost increases” will cost it £2.6m, which it plans to absorb through higher prices and cutting out costs. The Kent-based brewer, maker of Spitfire and Bishops Finger, told the City this morning: The Company has traded well in the first half and delivered strong profit growth. Like other operators in the sector, we face many cost headwinds that will impact us in the second half, following the recent Budget, notably the increase in national living wage and national insurance from April. We estimate that the annualised impact of these two items is £2.6m, with the incremental costs commencing in April and impacting the final quarter of the 2025 financial year. We plan to mitigate the majority of these costs over the next 18 months through price increases and cost efficiencies. Japan’s exports rose at a faster rate last month, suggesting that some customers overseas may have been increasing their orders ahead of a possible trade war. Exports measured by value rose by 11.4% year-on-year in February, Japan’s Ministry of Finance reported, while imports fell 0.7% That pulled Japan’s trade balance back into the black, with a surplus of ¥584.5bn. By region, shipments to the US rose 10.5% by value, though they did slip by 3.3% in terms of volume. Those to China increased 14.1%, probably due to a pick-up in demand after the Lunar New Year holiday ended, while exports to Europe fell 7.7%. The apparent rebound in the value of X comes at a see-saw moment for Elon Musk’s finances. The recent slump in the value of Tesla means that his vast stake in the electric car market is no longer his most valuable asset. Musk’s stake in SpaceX, his private rockets and satellites business, is now the billionaire tycoon’s largest asset for the first time in five years, according to Forbes, which still pegs his net worth at $323bn – more than anyone else in the world. The value of X has reportedly rebounded back to the level that Elon Musk paid for the social media platform back in October 2022. According to the Financial Times, investors valued X at $44bn when they bought a stake in the company earlier this month. That would be a rebound for Musk and the investors who helped him purchase Twitter (now renamed) three years ago. X’s value had tumbled under Musk’s early ownership, with some advertisers cutting their spending on X due to concerns that extreme content on the platform could damage their brands. At the start of 2024, mutual fund Fidelity revealed it had cut the value of its stake by 71%, which implied X’s value then had fallen to about $12.5bn. But today, the FT reports that while X’s revenues have dropped since Musk’s takeover, it made an adjusted EBITDA (ie underlying) profit of $1.2bn last year. They say: Investors valued the platform at $44bn in a so-called secondary deal earlier this month, in which they exchange existing stakes in the company, according to two people with knowledge of the matter. X was also working on raising fresh capital in a primary round, which would aim to raise about $2bn through selling new equity and be used to pay off more than $1bn of junior debt that Musk agreed to take on to finance his buyout of the company, then known as Twitter, in 2022, several people briefed on the situation said. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. These are difficult times for central bankers, as the threat of a global trade war and fears of a US recession grip economies and the markets. And this morning, the Bank of Japan has put its finger on the problem – policymakers simply can’t predict what will happen next. Speaking to reporters, BoJ governor Kazuo Ueda explained: “In the past month or so, there have been rapid changes in the scope and speed of U.S. tariffs. However, there are aspects we may not know even beyond April, so uncertainty remains high. We will scrutinise how the U.S. trade policy unfolds, how it affects the U.S. and other global economies, and how that all impacts Japan’s economic and price outlook.” Ueda also cautioned that “overseas uncertainty has heightened sharply lately”, and that it is hard to quantify the risks at this stage. Ueda was speaking after the BoJ decided to leave Japan’s interest rates on hold at 0.5%, even though Japan’s annual wholesale inflation rate hit 4.0% in February. In the weeks leading up to today’s meeting, president Trump has imposed 25% tariffs on steel and aluminium imports to the US and pledged to bring in ‘reciprocal and sectoral’ tariffs on 2 April, to balance out any imbalances. But he has also pulled back from his trade war with Canada and Mexico by temporarily delaying tariffs on many goods from the two countries, adding to the trade policy uncertainty</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>The European Commission has accused Google and Apple of failing to meet its digital rules. In a double-whammy of action against US Big Tech, Brussels has hit Google’s parent company, Alphabet, with two charges of breaching the Digital Markets Act. The EC is also pushing Apple to open up its ecosystem to rivals. Apple has slammed the EU order, saying it would hurt users and help its rivals.</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Time to wrap up… Thames Water said it has received six takeover offers from potential suitors to buy the company, and that talks are ongoing. The company hopes to agree a deal by the end of June, and complete it by the end of September. Its appeal to lift customers bills by more than regulators allowed has been paused while talks continue, but the CMA will consider appeals by five other water companies. Geopolitical tensions have pushed the gold price to a new all-time high of $3,038 per ounce. Analysts said the weaker dollar, and fears of a global trade war, were fuelling a new gold rush. The dollar has recovered ground this afternoon, after slipping to a four-month low which saw the pound trade at $1.30 for the first time since November. Back on bosses’ earnings… the CEO of Centrica’s pay packet has almost halved. Chris O’Shea received £4.322m last year, the company’s annual report shows, down from £8.231m in 2023. The decline was due to a lower bonus – O’Shea’s variable remuneration declined to £3.376m, down from £7.328m last year. Two years ago, O’Shea admitted that a £4.5m pay packet was “impossible to justify”. Back in Berlin, Germany’s outgoing parliament has passed a massive increase in government borrowing, including a sweeping change to the country’s debt rules. The legislation now goes to the Bundesrat upper house, which represents Germany’s 16 states, and is set to vote on Friday. Robin Winkler, chief German economist at Deutsche Bank Research, says: “After much nail-biting over the last fortnight, Germany’s outgoing parliament today decided to reform the constitutional debt brake. In our view, this is a historic fiscal regime shift, arguably the largest since German reunification. Yet, as with reunification, a fiscal expansion does not guarantee success: the next government will need to deliver structural reforms to turn this fiscal package into sustainable growth.” Our Europe liveblog has all the action: Bosses at the publisher of the Mirror, Express and Star newspapers took home more than £2m in pay and bonuses last year, angering staff who were awarded a few hundred pounds each following a boost in profits last year. Jim Mullen, the chief executive of Reach, the owner of more than 100 news brands including the Manchester Evening News, the Birmingham Mail and the Liverpool Echo, received total remuneration of £1.25m last year. His pay packet was sweetened by a maximum bonus of £662,000 after the company boosted operating profit by 6% to £102m last year. According to Reach’s annual financial report Mullen was paid 35 times that of an employee in the 25th percentile, the lower end of the company’s pay structure. Darren Fisher, Reach’s finance chief, received £857,000 including a £378,000 bonus. Following deep cuts affecting more than 800 staff Reach struck a deal to boost employee pay by 5% last year, and a £600 bonus payment this month as part of the company’s profit share scheme. Management is currently in negotiations with the National Union of Journalists over a proposed 2% increase this year, while any increase in the base salary of Mullen and Fisher will be decided on 1 April. The NUJ said that in light of the publication of top executive pay Reach should reconsider its pay offer. “It is good news that the business has turned around its key digital revenues and has improved its operating profits out of which these bonuses will be paid,” said Reach’s NUJ chapel. “But this was done on the back of heroic efforts by employees to dramatically increase the number of stories going online and by those in print outperforming the market with threadbare resources thanks to significant redundancies.” Donald Trump appears to have triggered a stampede out of the US stock market. Bank of America’s March Global Fund Manager Survey has found there was a record rotation out of US stocks by fund managers this month, as investor sentiment was hit by fears of a trade war and possible US recession. BofA reports there has been a “bull crash” in fund manager sentiment this month, with March seeing the second biggest drop in global growth expectations ever, the biggest drop in US equity allocation ever, and the biggest jump in cash allocation since Marcn 2020. This is reflected in market prices this year – the S&amp;amp;P 500 share index is down 4.5% during 2025, while Europe’s Stoxx 600 has jumped 9%. Back in the financial markets, the US dollar has shaken off its earlier losses – pulling the pound down to $1.296. Gold, though, is undaunted, and has now touched a new all-time high of $3,038 per ounce, up 1% today, thanks to a cocktail of Middle East tensions, US trade war fears, and the ongoing scamper into safe-haven assets. The news that Thames Water has received six takeover proposals since last summer comes as regulator Ofwat asks the competition watchdog to consider requests from several other water companies to lift their bills even higher than has been allowed. Ofwat is referring redetermination requests from Anglian Water, Northumbrian Water, South East Water, Southern Water and Wessex Water to the Competition and Markets Authority (CMA). The five companies are all challenging Ofwat’s ruling last year about how they can raise their bills between 2025 and 2030, arguing that the increase – 36% on average across the industry – wasn’t enough to invest in pipes, drains, reservoirs and treatment works. Ofwat defends its decisions, saying: The increase in investment means that customers’ bills will increase from 1 April; many customers are already expressing concerns about the level of increase. While the companies have not yet set out the details of their reasons for appealing, their initial statements highlight the need for additional funding beyond the substantial increase already allowed. This would mean a further increase in bills for customers. Interestingly, the regulator has also agreed a request from Thames Water to defer its referal to the CMA for up to 18 weeks. That delay, Thames says, will give it time to potentially “unlock a market-led solution for the recapitalisation of the Company” (presumably through one of the six offers on the table). Thames Water has revealed it has received six approaches from potential suitors. The struggling utility, which has been on the verge of collapse for months, says it has received proposals from six parties in response to a fundraising process launched in 2024, and that it “has since been conducting a detailed assessment of each proposal”. Thames says that many of the proposals included its bond holders taking a hit: The proposals involve a range of potential valuations, structures and outcomes for stakeholders. Of the five proposals that provided financial metrics, all except one (from a Class B Creditor and with significant conditions attached) indicated a material impairment of the Class A debt. The sixth proposal was for minority equity, intended to partner with investors, and did not set out financial metrics. In certain of the contemplated proposals, relevant creditors would receive – in exchange for debt impairment – certain rights to share in future growth in the value of the Company, and/or will have the ability to co-invest in the business. Thames adds that most of the proposals are conditional on the company achieving various “regulatory support and accommodations” – a nod to its financial and operational problems, from a £19bn debt pile to crumbling infrastructure. It explains: Discussions with relevant parties are ongoing, although there is no certainty that a binding equity proposal will be forthcoming or that any such proposals will be capable of being implemented. As a result, certain senior creditors continue to progress in parallel alternative transaction structures to seek to recapitalise the business. Thames does not name any of its suitors. But in December, the company received a £5bn bid from infrastructure investor Covalis Capital. News of the six takeover approaches comes a day after the UK court of appeal has upheld an emergency debt package worth up to £3bn. That debt should keep Thames operating for a few months while efforts to recapitalise it are progressing. The Guardian reported last week that Thames Water is asking to be spared billions of pounds of costs and fines over the next five years and heap more on to bills so it can attract new investors. The company is hoping to persuade the regulator Ofwat to grant it significant leniency on penalties and extra costs, to help woo bidders. South Yorkshire has become the latest combined authority to announce it will take buses into public control. Mayor Oliver Coppard has followed his fellow metro mayors in the north in deciding to pursue bus franchising to improve local services. Today’s decision came after a public consultation in which the authority said nearly 90% of 7,800 respondents backed local authority control of buses. South Yorkshire will, like Greater Manchester, West Yorkshire and Liverpool, now take control of the bus network - including depots and vehicle fleets, and setting routes, timetables, ticketing and fares. Buses are expected to operate under the new system from September 2027. Coppard said the move was “turning back the tide on the failed experiment of the privatisation of our bus network that was started in the 1980s, putting the public back into public transport.” He added: “Over the last forty years we’ve seen public transport taken apart; fares go up, routes and passenger numbers go down, and our city centres, our high streets and our economy flatline. “I want us to build a bigger and better economy in South Yorkshire and we need a public transport system that allows people to get to where they want to go, when they want to go there. “The destination is a fully integrated transport system across Barnsley, Doncaster, Rotherham and Sheffield, one that works in the interests of our communities and our economy, putting people back in control of essential services.” It is expected to have new branding, covering buses and trams and other public transport, much like Manchester’s Bee Network. Google is reportedy poised to make its biggest acquisition ever – posing a test for competition regulators. Google parent Alphabet has agreed to buy cyber security start-up Wiz for at least $32bn, the Financial Times is reportiing, with an announcement expected today. Wiz, which offers a service that scans the data on cloud storage providers such as Amazon Web Services and Microsoft Azure for security risks, was founded by alumni of Israel’s elite cyber intelligence unit in 2020. It rejected a $23bn offer from Google last year, and recently opened its European headquarters in London. The FT says: The all-cash deal, which will rank as the biggest deal of the year so far, will be announced on Tuesday morning, the people said. It will probably still face scrutiny from the Federal Trade Commission under President Donald Trump, whose new chair Andrew Ferguson has maintained guidelines giving the agency the ability to block large deals used by his predecessor Lina Khan. There will be an additional retention bonus offered to employees as part of the deal, which could be worth an extra $1bn, the people added. More here: Google parent Alphabet agrees to buy cyber security group Wiz for $32bn Germany’s blue-chip share index has hit a new intraday record high, as investors hope that the Bundestag will approve Berlin’s new proposed debt reforms today. The DAX is up 1.15%, or 268 points, at 23,423 points. Trade between Europe and the United States accelerated in January, as firms on both sides of the Atlantic raced to avoid a new trade war. New data from eurostat shows that European Union exports to the US rose by 16% year-on-year in January, to €46.7b, while shipments the other way rose by 7.5% to €30.5bn. That swelled the EU’s trade surplus with the US to €16.2bn, up from €11.9bn in January 2024. In contrast, Europe’s trade deficit with China ballooned to €30.1bn, from €20.6bn, due too a drop in exports and a rise in imports. Analysts at ING say “some tariff war anticipation effects can be seen in the US trade data”, adding: The outlook for 2025 is highly uncertain due to the trade war, despite new export orders finally showing signs of bottoming out. Last week, Donald Trump imposed 25% tariffs on steel and aluminium imports, including from the EU, and is threatening a 200% tariff on wine and champagne from European Union countries unless the EU’s retaliatory 50% levy on American bourbon whiskey is dropped. The EU also faces the threat of new reciprical and sectorial tariffs being imposed by the US in early April. The number of companies in England and Wales falling into administration rose last month, but remained lower than a year ago. There were 2,035 registered company insolvencies in England and Wales last month, 3% more than in January, but 7% lower than in February 2024. Company insolvencies over the past year have been slightly lower than in 2023, which saw a 30-year high annual number, but have remained high relative to historical levels, the Insolvency Service reports. The five industries with the most insolvencies in the last year are: Construction (4,031, 17% of cases) Wholesale and retail trade; repair of motor vehicles and motorcycles (3,631, 15% of cases) Accommodation and food service activities (3,474, 15% of cases) Administrative and support service activities (2,389, 10% of cases) Manufacturing (1,962, 8% of cases). Kelly Boorman, national head of construction at accountancy firm RSM UK, says: “Construction continues to experience the highest number of insolvencies above any other sector, which is to be expected given the ongoing burden of expensive debt and fragile supply chain. We are seeing a strong pipeline of work, however we’re not seeing the volume of delivery increase due to delays in mobilisation and the financial constraints, along with uncertainty in the aftermath of the Autumn Budget. Businesses are therefore preserving working capital and are yet to see the growth they anticipated in 2025. One of the main financial challenges for construction is the incoming increase to employers’ NIC. The industry is already under-resourced, and the increase to labour costs will squeeze margins. Britain’s accounting watchdog is investigating accountancy firm MHA for its audit of the collapsed construction company ISG, in a blow to MHA’s hopes to raise £125m through a stock market flotation. The Financial Reporting Council said it had begun an investigation of MHA’s audit of IGS’s accounts for 2022. The construction firm, which held more than £1bn of government contracts, fell into administration last September, and 2,200 workers lost their jobs. IGS, which built the velodrome for the 2012 London Olympics, had been struggling financially for some time and failed to secure a rescue deal. Neil Hallsworth from Nottingham, who worked for ISG as a project manager for more than 15 years, told the BBC at the time that he was “gutted” and that some of the contractors were “owed a fortune”. It was the biggest collapse in the construction sector since Carillion’s failure in 2018, and forced government officials to look for other contracts to take over ISG’s projects, including prisons upgrades and work to school buildings. The FRC investigation into MHA’s audit comes just a day after it announced plans for a public listing to raise up to £125m, including a £6m offer to small investors. On Monday, the accounting firm, which is the UK arm of the international network Baker Tilly, said it planned to float on London’s junior market Aim in the coming weeks to raise money for technology investments such as AI and the company’s expansion. It employs 43,515 people in 143 territories and made worldwide revenues of $5.6bn last year. MHA also said it is looking at buying up other Baker Tilly firms. Today, the firm said: “MHA is committed to audit quality and we will be co-operating fully with the FRC as part of this investigation.” Oil is pushing higher, with Brent crude is now up 1.5% today at $72.10 per barrel. Escalating geopolitical tensions are pushing oil higher, while fears of trade wars are dampening energy prices: Paul Donovan, chief economist at UBS Global Wealth Management, says: Israel’s overnight attacks on Gaza have contributed to a slightly higher oil price, but markets are not likely to react strongly. Energy supply seems unlikely to be disrupted, and investors are more likely to focus on the growth narrative and demand. Back in Germany, investor morale improved more than expected in March. The ZEW economic research institute’s monthly economic sentiment index has jumped to 51.6 points this month, up from 26.0 points in February. That’s an indication that Friedrich Merz’s push to increase borrowing and spending is being welcomed by companies across Germany’s economy. Elsewhere in the currency markets, the Russian rouble has rallied by 2.5% this morning ahead of planned talks between Donald Trump and Vladimir Putin. The rouble has strengthened to 81.45 roubles to the dollar, the strongest level since last June. Virtual reality headsets, yoga mats and men’s pool sliders have been added to the shopping basket used to calculate the cost of living in Britain, while local newspaper adverts and oven-ready gammon joints have been removed. In a snapshot of an increasingly online, time-pressed nation, the Office for National Statistics said the annual review of its inflation basket had taken into account shifting fashion trends, as well as growing consumer appetite for faster food and future technologies. Sales of VR headsets, which allow users to immerse themselves in digital worlds, have grown rapidly in recent years, and the goggles are used for everything from gaming to virtual therapy sessions to recreating the acid house rave scene of the 1980s and 1990s. More here: The euro is also rising against the US dollar this moring, ahead of a crucial vote in the German parliament about a plan to lift borrowing and spending drastically. The vote is an important test for Germany’s next chancellor, Friedrich Merz. The plan will release a €500bn infrastructure fund and relax debt rules – currently protected by the constitution – via the outgoing parliament, where parties in favour of the proposals – his conservatives, the Social Democrats (SPD) and the Greens – have the necessary two-thirds majority. But, Merz has faced criticism for not tying the historic levels of spending planned – as much as €1tn (£840bn) – to economic reforms. Kit Juckes, currency expert at Société Générale, says: There’s a lot riding on this morning’s German Bundestag vote on the fiscal package that future Chancellor Merz has put together. With the CDU/CSU, SPD and Greens all on board and carrying a significant majority onto the vote, there is room for a few rebels to fail to support the motion, but even so, moving the proposal forwards to the Bundesrat could still help the EUR. The result of the vote is expected around lunchtime… Sterling is also having a good morning against the weakening US dollar. The pound has traded at $1.30 for the first time since early November (just before Donald Trump’s election win sparked a dollar rally). The dollar is generally weaker again today, due to uncertainty over trade tariffs and concerns that the US economy is weakening. Expectations that sticky inflation will make it hard for the Bank of England to cut interest rates this year are also supporting the point, Bloomberg reports, adding: By year-end, traders see the BOE lowering borrowing costs by 51 basis points, less than the 60 basis points expected from the Federal Reserve. The US central bank also meets this week and is forecast to keep rates at 4.5%. [51 basis points would imply two rate cuts in the UK this year, with very little chance of a third, while 60bps implies that a third cut in the US is a possibility]. The BoE and the Fed both set interest rates later this week – neither is expected to cut, though. Gold is continuing to hit new heights this morning – it’s now trading at $3,027 per ounce. “In the current environment, every day seems to offer a new catalyst for the gold price,” comments Kathleen Brooks, research director at XTB. Today, it’s tensions in the Middle East, where the Gaza ceasefire has been shattered as hundreds of people are killed and injured as Israeli military forces hit dozens of targets. But, growth fears are also fuelling the price surge, she adds: In uncertain times, central banks and individuals demand gold, while inflation concerns emanating from President Trump’s tariffs and trade war are also boosting the price of gold. Life above $3,000 per ounce could be the norm for the gold price in 2025, it is already higher by 15% YTD, easily outpacing gains for global equities. Oil is trading near a two-week high this morning, with Brent crude up 1% at $71.73 per barrel. Matt Britzman, senior equity analyst at Hargreaves Lansdown, reports that concerns over supply disruptions due to ongoing conflicts in the Middle East are lifting oil, adding: Israel’s large-scale attack on Gaza and President Trump’s threats against Iran have added to the uncertainty, while expectations of increased demand from China, fuelled by stimulus plans and strong economic data, are acting as another tailwind.“ In the City, shares in banking group Close Brothers have tumbled after it reported that the UK’s motor finance scandal dragged it into a loss. Close Brothers reported an operating pre-tax loss of £103m for the six months to 31 January 2025, and a loss after tax ofo £111.8m. It was dragged into the red by a £165m provision relating to motor finance commissions, the practice where UK lenders made undisclosed payments to car dealers when customers bought cars on credit. Close Brothers is continuing to not pay a dividend, until the cost of motor finance compensation claims is known. The company expects to spend £22m this financial year on complaints handling and other operational and legal costs – more than the £10m-£15m it had previously forecast. That increase is due to additional costs associated with an appeal to the Supreme Court over a court of appeal ruling against Close Brothers, which widened the potential scale of the scandal. Close Brothers’ shares are down 13% in early trading. Speaking of Lloyds… the bank has apologised after accidentally sending a customer hundreds of pages of information about other clients’ investments. According to the FT, the customer of its retail investing business, Lloyds Bank Direct Investment, received a package containing bank statements showing the names, addresses and portfolio movements of a dozen other clients. The package also contained information about his own portfolio. Most of the documents tracked the movements of others’ investments over time, and included one portfolio worth more than £5m. The astonishing error occured, it seems, after Lloyds printed off the quarterly statements of some randomly chosen customers “to ensure accuracy” before posting the whole lot out. Unfortunately, a Lloyds staffer opened the collection, and mistakenly posted the entire package to the address on the top of the pile of statements…. More here. More than 6,000 IT staff at Lloyds Banking Group are due to learn their fate today, more than a month after the high street lender put their jobs under review. Line managers are due to speak to staff individually this morning, with a company-wide announcement due Tuesday afternoon. Overall, there is expected to be a net increase in IT vacancies - totalling around 1, 200 according to the banking group, which owns the Lloyds, Halifax and Bank of Scotland brands. But the problem is how many existing IT staff will be deemed fit to fill them. Some are expected to be pushed out as a result of a change in job location (with new roles being too far from their home,) their position no longer existing, or requiring more specialised skills. It is all part of a wider reshuffle related to a major digitisation plan under CEO Charlie Nunn. However, a reshuffle that puts some staff at risk comes at an awkward time, given how hard existing IT staff feel they’ve been working to help the bank through high-profile outages, that are now under scrutiny by MPs on the Treasury Committee. Lloyds was among a raft of banks whose customers struggled to log into online bank accounts or suffered payment delays at the end of February. Overall, MPs are concerned that customers at Britain’s major banks and building societies have suffered the equivalent of more than one month’s worth of IT failures in the last two years. One of Lloyds’ staff unions, Accord, said it would not be commenting about the IT reshuffle until employees were informed. Lloyds said: “Making changes means not only creating new roles and upskilling colleagues but also saying goodbye to talented people who have been part of the group’s success in the past. Where that is the case, we will do everything we can to support them with the changes recently announced. “We know change can be uncomfortable, but we are excited about the opportunities ahead as we propel forward to achieve our growth ambitions and delivering exceptional customer experiences.” The Financial Times’s Lex column has a good take on gold today, arguing that it is “unlikely to lose its lustre any time soon”, given its status as protection against risks. Lex writes: It is the ultimate shock absorber: against geopolitical maelstroms, inflation and — as a non-yielding asset — lower interest rates. This trio of latter-day horsemen is galloping across the horizon. Natural orders are being ripped apart as US President Donald Trump toys with ideas like modern-day colonisation, civil-service defenestration and swingeing tariffs. The latter could well tip the US into recession. Since November’s election US gold stockpiles have more than doubled. We appear to be in the third major bull run in gold since Richard Nixon withdrew America from the gold standard on 15 August 1971, reckons AJ Bell investment director Russ Mould. He explains: “The first surge took place in the 1970s, after Nixon’s policy switch that was designed to free up room for US government spending, particularly in Vietnam. Two oil price shocks, in 1973 and 1979, stoked inflation and investors took fright from paper assets and promises, such as government debt, and sought out ‘real’ assets where supply only grew slowly instead. “The second took place in the early 2000s, as central banks played increasingly fast and easy with monetary policy in response to a series of crises, real or perceived. They ranged from the collapse of the LTCM hedge fund in 1998, the millennium IT bug, the collapse of the technology, media and telecoms bubble and then the Great Financial Crisis and the European Debt Crisis. Record-low interest rates and Quantitative Easing followed, to persuade some investors that central banks and policymakers had lost control, just as it seemed they had in the 1970s. “The third, and current surge, has its origins in the last decade, as central banks continued to run zero-interest rate policies and did little to sterilise QE. Then came the Covid pandemic, and a crisis for which already-tattered government balance sheets were, in many cases, ill-prepared. Government borrowing surged, especially in the UK and USA, and in the latter the federal debt has continued to grow at an unprecedented pace. The result is that the annual interest bill is now $1.2 trillion, or more than a fifth of the federal tax take, a situation that seems unsustainable. The Trump administration is trying to tackle this head on, with tariffs and efforts to boost America’s manufacturing base, but perhaps gold bugs are sensing another shift in global monetary policy and how the system is managed, especially as inflation remains stubbornly above central banks’ 2% target. Back when Nixon took the US off the gold standard, bullion was valued at $35 per ounce under the Bretton Woods fixed exchange rate system – a price that proved impossible for the US to stick to, as the money supply increased and other countries swapped their dollar reserves for gold. Once the US was no longer committed to backing every dollar overseas with gold, at that price, gold began to climb steeply, and by January 1980 it had hit $835 per ounce. Australian bank ANZ reckons gold has further to climb. ANZ raised its zero to 3-month gold price forecast to $3,100 per ounce and 6-month forecast to $3,200 per ounce, according to a research note on Tuesday, Reuters reports. They say: [For gold] we maintain our bullish view, amid strong tailwinds from escalating geopolitical and trade tensions, easing monetary policy, and strong central bank buying. They also point out that physical gold has been moving from London to the US, as fears that Donald Trump could impose tariffs on precious metal imports have raised prices States-side: “As for the gold market, fear of import tariffs has tightened liquidity in the London spot market, as supply flows to the U.S. This has triggered arbitrage trades, with a widening spread between Comex futures and London spot”. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. It’s been a record-breaking year for gold, as nervous investors have sought out safe-haven assets. And this morning, the precious metal has hit a fresh all-time high above $3,000 per ounce, driven by escalating geopolitical tensions in the Middle East, trade war fears and the weakening US dollar. Gold touched $3,017.64 per ounce, as news broke that Israeli military forces have launched widespread strikes on targets across Gaza early today, leading to fears that the shaky ceasefire in the region is over. This means gold has climbed by 15% since the start of this year, having ended December at $2,623/ounce, adding to its 27% surge during 2024. As this chart shows, it has now doubled over the last five years: The recent weakness of the US dollar has also pushed up the gold price. The greenback is trading near a five-month low against a basket of other currencies, as traders worry that Donald Trump’s enthusiasm for tariffs will trigger a full-blown trade war, that could push the US into recession. As analysts at Deutshe Bank put it: Investors continue to rotate away from the US dollar and find perceived safe havens amidst the heightened policy uncertainty. Linh Tran, market analyst at XS.com, reports that rising tensions in the Middle East and the escalating U.S.-China trade conflict have both driven investors toward gold as a safe investment channel, adding: These uncertainties have not only increased demand for gold but have also pushed significant capital inflows into the precious metals market, contributing to gold reaching record-high prices. The agenda 9.30am: ONS releases changes to the UK inflation basket 10am GMT: ZEW eurozone economic confidence survey 12.30pm GMT: US housing starts/building permits data for February 1.15pm GMT: US industrial production for February</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>The dollar has recovered ground after slipping to a four-month low. The pound is trading at $1.30 for the first time since November. Geopolitical tensions have pushed the gold price to a new all-time high of $3,038.</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>The UK’s financial watchdog has bowed to longstanding pressure and ditched a plan to frequently “name and shame” companies it is investigating. The Financial Conduct Authority (FCA) has decided not to go ahead with applying a new public interest test for announcing investigations into regulated firms “given the lack of consensus” over the plans. The decision comes as the government puts pressure on regulators to help “rip out bureaucracy that blocks investment” as part of its growth agenda. Critics had pushed back against the FCA’s plan to be more transparent with the public and whistleblowers when investigating potential wrongdoing in the City. The FCA had already watered down the proposals, first announced early last year, after an outcry from businesses and criticism from the then-City minister, Tulip Siddiq. The revised plan would have given companies 10 days’ notice before any public announcement was made. Siddiq had publicly called on the regulator to rethink its plans and suggested she could overrule it if it pressed ahead with disclosing the companies it investigated. Nikhil Rathi, chief executive of the FCA, said: “Considerable concerns remain about our proposal to change the way we publicise investigations into regulated firms, so we will stick to publicising in exceptional circumstances, as we do today.” He said it was not possible to move forward with naming and shaming firms without consensus. The drive towards naming and shaming firms was partly prompted by an outcry after the FCA was unable to publish names of financial advisers who gave flawed advice to pensioners at British Steel. The FCA argued that earlier disclosure of an investigation may have prevented some pensioners from being harmed. “We will implement changes which have commanded wider support and which we believe will help support our efforts to protect consumers from harm,” Rathi said. He said there was a broader conversation to be had about what regulations the public, government, and business wanted. “What we need to have is a proper debate,” he said. For every step towards deregulation, the tolerance for the results needed to be considered, he added, using an example of how relaxing mortgage lending rules would result in higher default rates. The government has abolished the Payment Systems Regulator (PSR) as part of an “efficiency drive” and the FCA will absorb it and its 160 staff. The government presented the step as part of its efforts to boost UK economic growth. The FCA and PSR share premises in Stratford, east London. PSR staff are on FCA contracts. Separately, the Guardian has reported on how peers linked to big City firms also sit on a new Lords committee scrutinising regulation of the financial services industry. The Lords committee warned in February that announcing enforcement investigations early without addressing concerns over the plans could damage the reputation of companies that may never face regulatory action. Meanwhile, the FCA and its sister organisation at the Bank of England, the Prudential Regulation Authority, have dropped work on rules to improve diversity and inclusion, the watchdog confirmed. Rathi dismissed suggestions this was part of a US-led trend towards killing off diversity initiatives, and instead pointed to new government legislation on workers’ rights. He said there was a need to avoid “duplication” in this area and ensure FCA rules were in line with the legislation. The regulator would monitor enforcement of employer responsibilities to protect its staff against harassment. This would inform its work on taking a tougher line on allegations of bullying, sexual harassment, and discrimination against financial professionals or firms, he added. The FCA, which plans to publish its final policy in June, remains “committed” to investigating non-financial misconduct and considered it essential for “market integrity”, Rathi said.</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>The Financial Conduct Authority (FCA) has decided not to go ahead with applying a new public interest test for announcing investigations. Critics had pushed back against the FCA’s plan to be more transparent with the public and whistleblowers when investigating potential wrongdoing in the City.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Time to wrap up, after another day in which Donald Trump has moved the markets. European carmakers’ shares have slid today after the US president said he planned to impose 25% tariffs on EU imports soon. The selloff has intensified through the day – BMW are now down 4% on the Frankfurt stock market, followed by Porsche (3.6%). Analysts at the Kiel Institute warned that new tariffs would hurt both the European and US economies, especially if the EU retaliated. And the European Central Bank pointed out that eurozone businesses could suffer if cheap Chinese goods flooded to Europe rather than into the US. The US dollar has rallied against other major currencies, after Trump announced that tariffs against Mexico, Canada and China will kick-in next week. Matthew Ryan, head of market strategy at global financial services firm Ebury, says: “The dollar is trading higher across the board this afternoon after President Trump cooked up another storm on his Truth Social account, proclaiming that tariffs aimed at Canada and Mexico would go ahead as planned next week. Markets have been caught wrong-footed by the news, seemingly due to the belief that these levies would again be delayed and/or watered down relative to his initial threats - alas, there is no sign of that at this stage. Our US Politics Live blog has more details: A surprise jump in the number of Americans filing new claims for unemployment support has raised concerns that the US economy could be slowing. Elsewhere today… Gatwick has been given a qualified green light to operate a second runway after the government “set out a path to expansion” for London’s second biggest airport. But, the deadline for the government to make a final decision has been extended to late October…. Rolls-Royce has said it will return £1.5bn to shareholders as the British jet engine manufacturer paid its dividend for the first time since the coronavirus pandemic. Its shares have soared 15% to a new alltime high. But advertising firm WPP’s shares have slumped 15%, after it reported a slowdown in activity at the end of laast year. Kyle Chapman, FX markets analyst at Ballinger Group, says Trump’s post has shaken the markets out of their complacency about tariffs: “The dollar has surged today after a Truth Social post in which Trump assured markets that the Mexico and Canada 25% blanket tariffs would indeed be implemented on Tuesday. He also threw in an extra 10% on China for good measure. “A complacency has built up in markets since the first tariff delay, and that always meant that a big correction was on the cards if calling Trump’s bluff turned out to be the wrong move. Before yesterday the euro was priced as if there was no longer any tariff risk, and Trump appears to be hell-bent on rectifying that this week. Much has been said about the market’s fatigue in responding to each and every tariff headline – that is not what is on display today. “I am not going to pretend that I have any accurate foresight on where the tariff story goes from here. For a while there, investors seemed to think that they had figured Trump out. But the unknowability of Trump’s eventual policy moves is going to feed into higher volatility for some time. “The chances are small at this stage, but for what it’s worth I think there is still time for a trade war to be avoided. That tariffs will be in place ‘until [the flow of fentanyl] stops, or is seriously limited’ sounds like a possible off-ramp to me.” Newsflash: Donald Trump has announced that his proposed tariffs on Mexico and Canada will go into effect on 4 March, dashing hopes of another delay. Trump has also revealed that the planned additional 10% tariff for China will kick in on the same day, next Tuesday. Trump had delayed the introduction of new 25% tariffs on Mexico and Canada at the start of this month, after both countries pledged to boost their efforts to police their borders. But today, Trump claims that illicit drugs are still pouring into the US from Mexico and Canada “at very high and unacceptable levels.” Writing on his Truth Social site, Trump says: “We cannot allow this scourge to continue to harm the USA, and therefore, until it stops, or is seriously limited, the proposed TARIFFS scheduled to go into effect on MARCH FOURTH will, indeed, go into effect, as scheduled. China will likewise be charged an additional 10% Tariff on that date. The April Second Reciprocal Tariff date will remain in full force and effect. Thank you for your attention to this matter. GOD BLESS AMERICA! The news has driven up the value of the US dollar by around 0.6% against a basket of currencies. The pound has dropped by a third of a cent to $1.264, while the euro is down half a cent at $1.0437. The jump in US jobless claims last week doesn’t appear to be driven by Elon Musk’s ‘department of government efficiency’ program, which has been laying off government staff. Today’s report says: Initial claims for UI benefits filed by former Federal civilian employees totaled 614 in the week ending February 15, an increase of 1 from the prior week. The number of Americans filing new claims for unemployment benefits has risen to its highest level this year. A total of 242,000 initial claims were filed in the week to 22 February, up from 220,000 in the previous week. That’s the highest level since the first week of December, when 242,000 initial claims were also recorded. It’s also a bigger jump than expected – economists had expected only a small rise, to 221,000. It may show that US firms are getting more nervous about economic prospects, and laying off staff. The repoort says the largest increases in initial claims for the week ending February 15 were in Kentucky (+3,012), Tennessee (+2,766), Washington (+735), Michigan (+452), and Minnesota (+83), while the largest decreases were in California (-5,530), Pennsylvania (-1,110), Florida (-981), New Jersey (-903), and New York (-698). Donald Trump’s tariff threats towards Europe have become “more concrete”, say analysts at ABN AMRO, following last night’s threat to impose a 25% levy. They add: We estimate the. eurozone and the US stand to take a 1.3% and 0.5% GDP hit from these tariffs. Policymakers at the European Central Bank were concerned about the impact of new US tariffs on the eurozone, when they met last month. The minutes of the ECB governing council’s last meeting, in late January, have just been released, and show concerns about new trade restrictions. The minutes say: Members concurred that the outlook for the international economy remained highly uncertain. The United States was the only advanced economy that was showing sustained growth dynamics. Global trade might be hit hard if the new US Administration were to implement the measures it had announced. The ECB was also conscious that more low-price Chinese goods could be sent to Europe, due to US tariffs, which would push down inflation but hurt European manufacturers. The ECB’s minutes say: The challenges faced by the Chinese economy also remained visible in prices. Chinese inflation had declined further on the back of weak domestic demand. In this context, it was pointed out that, no matter how severe the new US trade measures turned out to be, the euro area would be affected either indirectly by disinflationary pressures or directly, in the event of retaliation, by higher inflation. In particular, if China were to redirect trade away from the United States and towards the euro area, this would make it easier to achieve lower inflation in the euro area but would have a negative impact on domestic activity, owing to greater international competition. The oil price has risen today, after Donald Trump cancelled a license given to energy giant Chevron to operate in Venezuela. US crude oil is up 0.9% at $69.23 per barrel, while Brent crude, the international benchmark, is up 1% at $73.22 per barrel. Trump announced yesterday that a permit issued by the US government allowing Chevron to pump and export Venezuelan oil will be terminated this week, which will end a financial lifeline for the South American country. The US president accused his Venezuelan counterpart, Nicolás Maduro, of not meeting democratic conditions. Trump wrote on his Truth Social site: “We are hereby reversing the concessions that Crooked Joe Biden gave to Nicolás Maduro, of Venezuela, on the oil transaction agreement.” Both the European and US economies would suffer from a new trade war, the Kiel Institute for the World Economy has warned today. A simulation created by the Kiel Institute has calculated that there would be economic contraction in both the EU and the United States if the US imposed 25% tariffs on European goods. The economic damage would be worse if Europe retaliated with its own tariffs. The Kiel Institute says: According to the simulations, the European economy would shrink by an average of 0.4 percent in real GDP terms within the first year, a significant impact for a short-run scenario. The U.S. itself would not be spared, experiencing a contraction of 0.17 percent. Should the EU retaliate with its own 25 percent tariffs, the economic damage to the U.S. would double and increase own costs for the EU by another 0.14 percentage points. Furthermore, price levels in the U.S. could increase by up to 1.5 percent due to higher costs for imported final goods and intermediate inputs, making domestic production more expensive and reducing overall competitiveness. Kiel’s calculations show that European exports to the US would decline by 15% to 17% in the first year, including 20% plunge in Germany’s sales to the US. In other trade news, France’s industry minister has called for more protection for Europe’s steel sector. Marc Ferracci told a news conference on the future of the European steel industry that this could include stronger safeguard measures. Ferracci says: “The European industry and the steel sector need protection, which in the short term means beefing up safeguard measures.” The existing safeguard measures include tariffs on steel imports over a set quote. Last summer they were extended until June 2026. Polish prime minister Donald Tusk has responded to US president Donald Trump’s claim that the EU was formed “to screw the United States.” In a social media post in English, Tusk said: The EU wasn’t formed to screw anyone. Quite the opposite. It was formed to maintain peace, to build respect among our nations, to create free and fair trade, and to strengthen our transatlantic friendship. As simple as that. 🇪🇺🇺🇸 My colleague Jakub Krupa’s Europe liveblog has more details. The New Economics Foundation (NEF) has warned that growing Gatwick airport will not create economic growth. Dr Alex Chapman, senior economist at NEF, says: “Growing Gatwick will not magic up the economic growth the government so desperately wants. Business air travel has collapsed while expansion will see three times as many tourists leave the country as come in. “Voters living outside London and the south east will not thank the government for this decision. Expanding airports like Gatwick doesn’t create new jobs - it displaces jobs from the wider UK regions, and particularly the domestic tourism industry which is a key source of spending outside London and the south east. “The UK is small country with a remarkably high number of international airports. People are already perfectly able to catch cheap flights on holiday or travel for business. If this government is so desperate for growth, it should focus on investing properly in the vital public services upon which the health of our economy really depends.” The Unite union have welcomed the goverment’s decision to say it is ‘minded to approve’ the expansion of Gatwick. Unite, which represents 7,000 workers at the airport, believes the expansion should boost highly skilled, well-paid, unionised jobs. Unite general secretary, Sharon Graham says” “Unite welcomes the announcement of the expansion of Gatwick but it needs to come with guarantees of well paid, unionised jobs and proper facilities for workers. “It is also ever more urgent with every airport expansion that we ensure domestic production of sustainable aviation fuel (SAF) to offset carbon emissions and meet the government’s own targets on net zero. Unite is also pushing for the Grangemouth refinery in Scotland to be upgraded to produce SAF, rather than being closed this summer. A final decision on Gatwick’s push to open a second runway will not come for several months, though, even though a ‘minded to approve’ letter was released today. Transport minister Heidi Alexander has extended the deadline for deciding for certain whether Gatwick can turn its back-up emergency runway into a second runway until 27 October. Alexander says: The decision to set a new deadline is without prejudice to the decision on whether to give development consent… Donald Trump’s enthusiasm for tariffs is creating economic uncertainty, and volatility in the finaancial markets. Dan Ivascyn, group CIO at bond-trading giant PIMCO, explains: “You do not only have uncertainty here in the United States, but you have a lot of uncertainty in terms of relationships with other countries, impact on markets. And that’s creating not only a lot of localized volatility but volatility across countries, across sectors, across yield curves and that’s a great opportunity as well. So I think the key theme going into this year is to have a healthy degree of humility around the uncertainty. Acknowledge the uncertainty, but look to take advantage of the full global opportunity set, both within the liquid higher quality areas of the market, as well as in some of the more credit sensitive areas as well.” Here’s our news story about Gatwick being given qualified consent to operate a second runway after the government “set out a path to expansion” for London’s second biggest airport. UK transport secretary Heidi Alexander has reportedly “set out a path to approving” Gatwick airport’s expansion project, to open a second runway. That’s according to PA Media, who are citing a Government source. They explain: This comes after the Planning Inspectorate initially rejected the West Sussex airport’s application to bring its emergency runway into routine use. The Planning Inspectorate then recommended that Ms Alexander should give the project the go-ahead if adjustments are made on issues such as the proportion of passengers who travel to and from the airport by public transport, and noise mitigation. It is understood to be the first time the body has recommended an alternative plan when assessing a project. Gatwick has until April 24 to respond to the new proposals, shortly after which Ms Alexander is expected to make a final decision. Shares in European automakers are falling this morning after Donald Trump threatened to slap 25% tariffs on imports from the EU. President Trump’s statement yesterday that new European tariffs will be announced “very soon” and fall “on cars and all other things” (see opening post) has hit Europe’s stock markets this morning. Germany’s DAX index has dropped by 1.2%, with carmaker such as BMW (-2.9%), Porsche (-2.8%), Volkswagen (-2.75%) and Mercedes-Benz (-2.5%) leading the fallers. Across Europe, car giant Stellantis are down 2.75% while Renault have lost 1.2%. Li Xing financial markets strategist consultant to Exness, explains: President Donald Trump’s announcement of a 25% tariff on EU cars and goods has reignited global trade worries, although the lack of clarity surrounding the policy may limit its immediate market impact. Trump is hoping to close the US’s $208bn trade in goods deficit with the EU by imposing tariffs (which will make imports from Europe more expensive). That’s the second largest trade in goods deficit, following China’s $279bn. Should Trump impose tariffs on the EU, some countries are likely to be hit harder than others. Germany has by far the most goods exports, worth €158bn (£131bn) in 2023. The Netherlands imports the most goods from the US, worth €76bn. Trump also caused a stir by claiming that the EU “was formed to screw the United States”. Carl Bildt, the former prime miniser of Sweden, points out there were other motivations…. Grocery delivery firm Ocado’s shares are also sliding, down 13% this morning, after it reported another annual loss. Ocado made a statutory loss of £373m in the 12 months to 1 December 2024, lower than the £387m it lost in 2023. Total revenues rose 14%. City investors may be disappointed that Ocado hasn’t announced any fresh deals for its robotic warehouses this morning. It launched three of these customer fulfillment centres (CFCs) last year, in Sydney, Melbourne and Madrid, and is planning at least seven more over the next three years, starting with Warsaw this year. But the opening dates of two of those CFCs, in Charlotte, North Carolina, and Phoenix, Arizona, has slipped to early 2026, following a “new Auto Freezer order”. Adam Vettese, market analyst at eToro, says: “A familiar story from Ocado’s results: on the surface there is plenty to be optimistic about - the loss has narrowed, on track to be cash-flow-positive, fastest growing UK grocer. Unfortunately, optimism isn’t going to pay the bills. “The trouble is that while all of these things are great, the sticking point is that operationally there are still some issues. The rollout of robotic grocery warehouses to partners isn’t where the firm would want it to be, and of those confirmed in the pipeline, we are seeing them kicked back towards 2026. “The firm insists more warehouse deals are coming. But just how much longer will they have to burn cash for is the question investors eagerly await to be answered. Shares are trading at less than half of what they were at the beginning of last year, some investors might be looking at this as a cheap play with things seemingly only able to improve. If the orders don’t come and there are more delays on what Ocado does have then this may not be the case.” Ocado’s shares are down 15%, the worst performer on the FTSE 250 index, at 281p While Rolls-Royce’s shares soar to the top of the FTSE 100 leaderboard, advertising group WPP have slumped 18% to the bottom of the pack. WPP missed sales forecasts this morning, reporting a 0.7% drop in reported revenues in 2024. The slowdown worsened in the last quarter of the year, when revenues fell in North America, the UK, and China, although they rose in Western Continental Europe. Mark Read, chief executive officer of WPP, says Q4 was hit by “weaker client discretionary spend”. We did see growth from our top 25 clients of 2.0% and an improving new business performance in the second half of the year with wins from Amazon, J&amp;amp;J, Kimberly-Clark and Unilever reflecting the strength of our integrated offer. “The actions we are taking across WPP will strengthen our existing client relationships and drive our new business results. We expect some improvement in the performance of our integrated creative agencies in the year ahead. At the same time, we have comprehensive efforts underway to improve our competitive positioning through new leadership at GroupM, with further investment in AI, data and proprietary media. “Though we remain cautious given the overall macro environment, we are confident in our medium-term targets and believe our focus on innovation, a simpler client-facing offer and operational excellence will support our growth and deliver greater value for our shareholders.” On the UK specifically, WPP reports: The United Kingdom declined in 2024 reflecting a strong comparison (2023: +5.6%) and the impact of slower client spending in Q4 with further weakness in project-based work across creative and specialist agencies exacerbated by an uncertain macro outlook, only partially offset by growth in GroupM and Ogilvy. BOOM! Shares in Rolls-Royce are soaring at the start of trading, as investors hail its financial recovery. Rolls-Royce’s stock has jumped by over 15% to 735p per share, a new all-time high. The City will be impressed with Rolls’s upgraded forecasts for profit growth (see 7.48am), as well as relieved that the dividend has been restored (as had been expected). In another sign of confidence, Rolls-Royce has lifted its mid-term financial targets. It tells shareholders: Upgraded mid-term targets of £3.6bn-£3.9bn underlying operating profit, 15%-17% operating margin, £4.2bn-£4.5bn free cash flow, and 18%-21% return on capital based on a 2028 timeframe. The company is also aiming for between £2.7bn and £2.9bn underlying operating profits this year, up from the £2.5bn in 2024. This shows that CEO Erginbilgiç’s turnaround plan – dubbed “the most astonishing turnaround at a major FTSE 100 company in decades” by my colleague Nils Pratley – is continuing to pay off. UK engineering firm Rolls-Royce is resuming payouts to shareholders for the first time since the Covid-19 pandemic hit its operations. Following “strong results” in 2024, Rolls-Royce has announced it will pay a dividend of 6.0p per share to investors. It also plans to spend £1bn on a share buyback scheme – another way of returning cash to shareholders. The news comes as Rolls-Royce annouces that earnings rose by over 50% last year – with underlying operating profit up to £2.5bn, from £1.6bn in 2023. Chief executive Tufan Erginbilgiç says Rolls-Royce is being transformed into a “high-performing, competitive, resilient, and growing business”. All core divisions delivered significantly improved performance, despite a supply chain environment that remains challenging. We are moving with pace and intensity. Based on our 2025 guidance, we now expect to deliver underlying operating profit and free cash flow within the target ranges set at our Capital Markets Day, two years earlier than planned. Significantly improved performance and a stronger balance sheet gives us confidence to reinstate shareholder dividends and announce a £1bn share buyback in 2025. It’s quite a turnaround since Covid-19 buffeted Rolls-Royce, which makes and services jet engines, runs a defence arm, and produces a range of power and propulsion products, including nuclear propulsion plants for the Royal Navy’s nuclear submarines. It is also developing small modular nuclear reactors. Rolls suspended dividend payments in April 2030, as its airline customers kept flights grounded due to the pandemic. The crisis, drove its share price down below 40p in October 2020. Last night they closed at 631p, having hit a record high earlier this month. The company has been cutting costs under Erginbilgiç, and also reported record-breaking orders amid mounting military tension around the world. We’re expecting to learn later today whether Gatwick airport will be allowed to open a second runway. The Transport Secretary, Heidi Alexander, is due to announce today whether she has granted a development consent order which could allow more than 100,000 extra flights a year at the West Sussex airport. Gatwick wants to modify an emergency runway and taxiway to allow it to be used alongside its existing main runway. The BBC reports that on Tuesday Alexander told the annual dinner of trade body Airlines UK in London that she had “no intention of clipping anyone’s wings,” and said aviation was good for growth, adding: “I am not some sort of flight-shaming eco warrior. I love flying – I always have.” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. The spectre of tariffs is stalking Europe today after Donald Trump announced last night he will soon hit goods made in the European Union with tariffs of 25%. Trump told his first cabinet meeting, on Wednesday, that he will soon release details of the latest tariff threat, declaring: “We have made a decision and we’ll be announcing it very soon. It’ll be 25%.” Trump did not give further details but mentioned carmakers and said the levies would be applied “generally”, adding: “And that’ll be on cars and all other things.” European stock markets are expected to open in the red, as investors anticipate a new front opening up in Trump’s tradae wars. Traders were already bracing for the looming March 4 deadline for US tariffs against Canada and Mexico, and for the steel and aluminum duties set to drop on March 12. Each of these points could rattle markets, warns Stephen Innes, managing partner at SPI Asset Management, adding: For now, markets are still fixated on tariff risk, not the impact. Absolute volatility begins when investors fully price these tariffs’ inflationary and/or growth ripple effects. The dollar, bonds, and equities are about to enter the trade war vortex again, and positioning will be everything. The agenda 12.30pm ECB minutes from Jan meeting 1.30pm US GDP (1st revision) for Q4 1.30pm US initial jobless claims data</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>BMW and Porsche down 4% and 3.6%, respectively, on the Frankfurt stock market. Analysts warn new tariffs would hurt both the European and US economies. US dollar rallies against other major currencies, after Trump announced that tariffs against Mexico, Canada and China will kick-in next week.</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Time to wrap up: The number of people going financially insolvent across England and Wales jumped by 12% in January compared with the same month a year earlier, according to Insolvency Service figures. More businesses also failed, with analysts warning that high taxes and a slow economy could lead to more insolvencies through this year. Thames Water has avoided collapse, with a high court judge today giving approval for up to £3bn of high-cost borrowing. But campaigners are vowing to fight the decision – arguing that Thames should be put into a special administration. A rival group of creditors who had pushed an alternative package are also planning to appeal. Elsewhere in economics, UK wage growth accelerated at the end of last year – with total pay rising 6% in October-December. Bank of England governor Andrew Bailey, though, has insisted that this doesn’t change the BoE’s view of the economy. UK energy customers have been warned that bills are likely to jump by 5% in April, when the price cap is next adjusted. Steel giant Tata has welcomed planning approval for its proposals for huge changes to steelmaking at its biggest plant. Neath Port Talbot Council’s planning committee gave the go-ahead at a meeting on Tuesday to the way steel is produced at the South Wales site. Tata has closed blast furnaces and is switching to an electric arc furnace-based steelmaking process which is greener, but needs fewer workers. Almost 2,000 jobs will be lost, although the company and the Government have announced plans to help find new jobs for those affected and Tata says thousands of jobs will be preserved. Rajesh Nair, chief executive of Tata Steel UK, said: “We are very pleased to have secured approval to build sustainable steelmaking in Port Talbot. “Amidst a challenging global market, this is a significant milestone for the project and we are committed to begin large-scale work on site this summer, ahead of the Electric Arc Furnace starting up from the end of 2027. “This £1.25 billion investment is the most significant investment made in the UK steel industry in decades. “The facility will secure high-quality steel production, preserve thousands of jobs, and safeguard steel making in Port Talbot for generations to come.” The closure of the last blast furnace at Port Talbot last year has led to job losses and higher rates of mental illness, with unions warning that for every job that goes in the steel plant, about three or four jobs are supported in the wider community. Ouch! Confidence among US homebuilders has dropped, on concerns over president Trump’s plans to impose tariffs on imports. A gauge of housing market conditions produced by the National Association of Home Builders and Wells Fargo fell 5 points to 42, the lowest since September. Worres about high mortgage rates are also weighing on the housing market, the survey shows, with the US Federal Reserve not expected to cut interest rates for several months yet. Despite today’s High Court ruling, “the ongoing financial drama at Thames Water shows no sign of abating”, says. Mark Lloyd, chief executive of The Rivers Trust. Indeed, Lloyd adds, it merely adds to “the public despair and lack of trust” in the water industry. He says: “The astounding level of debt and punitive interest rates agreed mean that a large proportion of customer bills will be spent on paying financiers rather than improving the environment, when we know that Thames Water are already not delivering many of their promised environmental improvements. This is a reflection of poor regulation over decades, which has driven companies to debt rather than equity finance, and some very greedy owners who siphoned too much funding out of the company to make themselves rich rather than fix our creaking infrastructure. Back in Germany, auto supplier Continental has announced plans to cut a further 3,000 jobs by the end of 2026. The job reductions will be in research and development, it said, with less than half of the cuts will be in Germany. Continental said the cuts would “to a large extent” take place via natural turnover, such as from retirement. Philipp von Hirschheydt, head of the automotive division at Continental, says: “We are continuously improving our competitive strengths in the interest of our sustainable market success.” Continental had already announced plans last February to cut 7,150 jobs by 2025. Farmers have expressed their “disappointment” and “fury” following a meeting with the government over the planned changes to inheritance tax for agricultural properties. Tom Bradshaw, the president of the National Farmers’ Union (NFU) which represents 40,000 farmers across England and Wales, said he had taken proposals to the Treasury to reduce the impact of the changes to agricultural and business property relief on family farms. However he said the exchequer secretary James Murray, and farming minister Daniel Zeichner were not receptive to their proposals. “Disappointment doesn’t describe how I feel at the moment,” said Bradshaw, adding: “There is no movement, the government resolutely believes that they are correct in the decision they have made and that they are generous in the exemptions they are giving us. They don’t care about the human impact, they don’t care about the intergenerational impact.” Farmers have been protesting against the planned changes to agricultural property relief and business property relief since they were announced in October’s budget, which would see farms and other business property fall within inheritance tax from April 2026. Inheritors would have to pay 20% of the value of agricultural and business property above, which the government said would raise money to help improve public services. The NFU and farming groups have warned that the proposed changes would push up food prices, impact domestic food supply and force many family farms to sell up to pay their tax bill. Bradshaw told reporters he and representatives from other farming and countryside groups - the Tenant Farmers’ Association (TFA), Country Land and Business Association (CLA), and Central Association of Agricultural Valuers (CAAV) - proposed a “clawback” mechanism. The clawback would see those inheriting a farming business only eligible for paying tax if they decided to sell the business within a certain time period after inheritance, which the NFU says would be at a time when cash was available to pay the tax bill. “We are offering them a solution which still raises the funds, but at the moment the door is shut from Treasury,” Bradshaw said. “The reaction from our members is going to be one of fury, one of real anger, one of desperation.” He added: “We recognise the fiscal hole that the country faces and we recognise the challenges that government are under”. Bradshaw insisted the prime minister was “disingenuous” to suggest that there was a choice between inheritance tax and funding the NHS The meeting came just days after Keir Starmer cut short a visit to a housing development in Bedfordshire after it was interrupted by a protest of tractor-driving farmers. That day, Stamer defended the introduction of inheritance tax for farms as necessary for the sustainability of public services such as the NHS. Victoria Vyvyan, president of the CLA, said she left the meeting with “boiling blood”. “They were adamant and deaf to what we trying to say,” she said. The Treasury has been contacted for comment. Just in: Thames Water’s Class B creditors have been granted permission to appeal today’s court ruling in favour of their rival Class A creditors. The Class B creditors are lower-ranked in the pecking order, meaning they would be repaid after the As. The Bs had proposed a rival debt restructuring plan to the one approved today – which had a lower interest rate. The judge, though, was withering in his assessment of the Class B’s offer. He wrote in his judgment that “I am very far from satisfied that the Class B AHG have made a binding commitment” for their own £3bn plan. He also wrote that he was “less than impressed” by the evidence of one of the class B investors, an investor from hedge fund Polus Capital. Newsflash: Millions of households acrss Britain face a greater than expected increase to their energy bills of £85 a year from April after Europe’s gas storage levels slumped, according to analysts. The average gas and electricity bill for households across England, Scotland and Wales is expected to rise by nearly 5% from April to £1,823 a year for a typical household under the energy regulator’s price cap. The forecast by the influential consulting firm Cornwall Insight is higher than its earlier prediction that prices would rise to £1,785 a year this spring after colder weather and limited renewables caused gas storage levels to fall across Europe. The energy industry regulator for Great Britain, Ofgem, will confirm the figure for the energy price cap covering the three months from 1 April on 25 February. The regulator increased the cap in January by 1.2% to a rate equivalent to £1,738. Dr Craig Lowrey, Principal Consultant at Cornwall Insight, says: “Households have been hit hard over the past few months, and with bills set to rise for a third consecutive time the pressure is not letting up. While we’re not seeing a return to the peak of the energy crisis, the market is more volatile than it has been in quite some time, and households are bearing the brunt of cold weather and low gas storage levels across Europe. Over in Germany, investor morale has risen at the fastest rate in two years this month, on hopes that the economy will pick up under a new government after Sunday’s election. The ZEW economic reseach institute has reported that investor morale improved this month; its economic sentiment index increased to 26.0 points from 10.3 points in January. Analysts polled by Reuters had pointed to a reading of 20.0. ZEW president Achim Wambach says: “This rising optimism is probably due to hopes for a new German government capable of action.” The centre-right CDU party are leading in the polls, followed by the far-right AfD, with current chancellor Olaf Scholz’s SPD party third. A Liberal Democrat MP is vowing to appeal against today’s High Court judge’s decision to approve plans for a £3bn rescue loan for Thames Water from some of its existing creditors. Charlie Maynard, MP for Witney in Oxfordshire, has claimed that the restructuring approved today was “simply throwing good money after bad”. Maynard had led a group of clean river campaigners arguing that Thames Water should be put into a government-handled administration, rather than getting a loan lifeline. At a hearing in London earlier this month, lawyers for Maynard said that the company plan was a “poor short-term fix” and a “bridge to nowhere”, and that the company should be put into special administration (SAR) instead. And today, Maynard says (via PA Media): “I stand by my evidence to the court that allowing Thames Water to take on £3 billion more debt is not in the interests of their millions of customers. “They will all be paying the price for this futile, expensive and extremely short-term bailout. “This restructuring is simply throwing good money after bad. The money from our bills which is being spent on interest repayments is desperately needed to repair water infrastructure, improve customer service and clean up our rivers. “I intend to keep fighting for Thames Water’s customers by appealing this judgment. “The only way to get Thames out from under this mountain of debt and back onto a stable financial footing at this point is to put the company into special administration with a swift exit plan.” The number of companies and individuals falling into insolvency in England and Wales jumped, year-on-year, last month. New data from the Insolvency Service shows there were 1,971 registered company insolvencies in England and Wales in January 2025, 6% higher than in December 2024. and 11% higher than in January 2024. This included 269 compulsory liquidations, 1,546 creditors’ voluntary liquidations (CVLs), 142 administrations and 14 company voluntary arrangements (CVAs). Company insolvencies over the past year have been slightly lower than in 2023, which saw a 30-year high annual number, but have remained high relative to historical levels, the Insolvency Service says. Seperately, 9,706 individuals entered insolvency in England and Wales in January 2025 – that’s 12% more than a year ago, but 3% lower than in December 2024. These year-on-year increases highlight the economic pressures on households and companies, as they juggle inflationary pressures, higher borrowing costs and higher taxes. Sophie Burke, restructuring and insolvency partner at City law firm Fladgate, predicts we could see a further rise in corporate failures, saying: ‘’The latest insolvency statistics reflect weak consumer confidence and sustained economic pressure on businesses, in particular in consumer-facing sectors. Administrations have increased from December 2024 to January 2025 and Fladgate LLP has witnessed this directly in a sharp increase in the number of administrations that Fladgate has advised on since the start of 2025. The operating landscape for businesses in 2025 has had a turbulent start and this may lead to further increases in insolvencies.’’ Gavin Kramer, senior associate at law firm Collyer Bristow, warns that any increases in taxes coud push more firms under: “While the number of insolvencies has not reached the level of the 2008 recession, it’s nonetheless clear that businesses are still struggling, and that there remain very few signs of growth in the British economy. Many major sectors, especially retail, are already operating on thin profit margins. If, as seems possible, the Spring Budget includes further tax rises on either businesses or consumers, this may result in an increase in businesses’ operating costs increase and lead consumers to rein in their spending. When a business is in financial difficulties there are of course restructuring options which can keep the business afloat as a going concern and save as many jobs as possible. However, unless growth and consumer confidence pick up, it may be difficult for financially precarious businesses to successfully restructure and recover.” Here’s a handy Q&amp;amp;A about the approval of Thames Water’s £3bn rescue loan deal by a high court judge today, from PA Media: Q: What happened? After weeks of hearings in the High Court, a £3 billion funding plan for Thames Water has been approved as part of a loan deal agreed internally last year. The utility company supplies about 16 million households across London and the South East. But it has at least £16 billion of debt, and had previously warned it only had enough money to keep running until March 24. The new financing is designed to stop it from going bust, albeit temporarily. Q: Why are people angry about Thames Water? Thames Water has been at the centre of a growing scandal in the wider water industry. Bills will climb steeply over the coming years, while privately-run water firms are still pumping raw sewage into rivers and waterways. That is despite a succession of penalties from regulators Ofwat and the Environment Agency. Meanwhile, many bosses, including those at Thames Water, have still been given large bonuses in the last year. Thames Water also requested last week that Ofwat allows it to raise consumer bills over the next five years by more than the 35% it previously granted. Q: Why does Thames Water need this emergency money? The company’s debts are so high and its cash reserves are so low that it would have gone out of business in March. The taps in people’s homes would still work - but it would be damaging for the big finance firms to which Thames owes billions of pounds. Many of them would have seen those debts written off, resulting in hefty losses. Thames Water would instead come under temporary government control until a new buyer is found. Labour previously said it wants to avoid that scenario, citing extra costs to taxpayers of running the water company. Q: So what happens next? The £3 billion is thought to be enough to last Thames Water for about one year. It buys bosses some more time to find a permanent source of funding, which will likely come by selling the company. Potential suitors are lining up, with four bidders understood to have thrown their hat in the ring to buy Thames. One is Castle Water, a firm owned by the Conservative Party treasurer Graham Edwards. Another is investment firm Covalis Capital, which would bring in French utility giant Suez to run Thames day-to-day. Q: What’s the catch? The new loan is being provided by Thames’ creditors - namely companies it already owes about £11.5 billion. They are mostly made up of hedge funds and other big finance firms, including Abrdn, M&amp;amp;G and others. They are charging an unusually high interest rate of 9.75%, plus fees. Over the 2.5-year life of the loan, and including fees, that could mean about £800 million in interest payments, experts have said. Earlier this year, a group of MPs said it would force households to pay an extra £250 over the next five years to cover the costs. Currently, about 28% of Thames’ bills service its debts, a figure which is expected to rise to 31% this year. Q: How did things get this bad? When Thames Water was privatised in 1989, it had no debt. It has had a succession of different owners since then, including an Australian investment bank called Macquarie. In December 2005, before Macquarie bought the utility, Thames Water’s net debt was £2.4 billion. When Macquarie sold it around a decade later, the debt pile had ballooned to more than £10 billion. The other problem is that interest payments on much of its debts rise with inflation, which has been high in recent years, adding to the pressure. Mr Justice Leech, who approved Thames Water’s £3bn rescue loan, has also hit out at the “eye-watering” costs of finance and adviser fees involved in the deal. That includes £210m paid by Thames to its legal and other advisers, and a total of £800m for finance, debt servicing and professional and advisory fees, according to today’s ruling. He says: Customers and residents who are struggling with their bills will be horrified at these costs and mystified how the Thames Water Group has been able to fund them or why it has agreed to do so. Indeed, Mr Justice Leech adds that he might have been tempted to block the plan, if he had believed Thames would actually incur those £800m of costs – but in reality, he suspects the Class A creditors who proposed the loan will end up taking ‘a substantial haircut’ on their loans in future… Campaigners for a better water system are renewing calls for Thames Water to be put into public ownership, after the high court granted the company a £3bn debt lifeline this morning. Matthew Topham, lead campaigner at campaign group We Own It, said: “This judgment is nothing but a stay of execution for Thames Water. The privatised company will limp on for a few more months like a profit-thirsty zombie. “This crisis loan will keep Thames afloat in the short-term, but their underlying business model is rotten and should be condemned. “It relies on piling up debt and raising customer bills so they can pay huge bonuses and dividends – all whilst pumping raw sewage into our waterways. “The reason they’re getting bailed out is because they ran out of other people’s money to line their pockets with. It’s only a matter of time before they end up on the edge of bankruptcy again. “This is the ‘doom loop’ of privatised water and there is only one way to break the cycle – public ownership. “The Environment Secretary, Steve Reed, has the power to put Thames into a special administration regime (SAR), effectively a form of temporary nationalisation. “Under the SAR it’s possible to negotiate a significant reduction in the corporate debt, putting the company on a much better financial footing. “Once the debt has been slashed, the only long-term solution is full public ownership. Handing it back to the private sector would be a betrayal of the customers and our environment. In that scenario we’d end up back here again in a year’s time, just with more sewage in our rivers and more money in the water bosses’ pockets.” The governor of the Bank of England, Andrew Bailey, has downplayed concerns that this morning’s jump in UK wage growth might change its position on the economy. Speaking in Brussels this morning, Bailey argued that the latest UK jobs market data does not change the Bank of England’s broad expectations for the economy Bailey told an event in Brussels organised by the Bruegel think tank: “I don’t think we saw anything this morning that fundamentally changes that.” He was speaking after this morning’s labour market report showed total pay grew by 6% per year in October-December. The £3bn loan aproved for Thames Water today comes with a relatively high interest rate of 9.75%, and is structured in two parts. First, the company gets an “initial tranche” of £1.5bn to give it liquidity until September 2025. It could then receive two further tranches of £750m each, to further extend liquidity to May 2026 if required – depending on the success of Thames’s appeal to raise customer bills by more than Ofwat has allowed. The loan comes from a group of creditors who own Thames’s class A debt, and was opposed by a second group who own class B debt (which is riskier and thus less protected than A). The chief executive of Thames Water, Chris Weston, says the court’s decision to approve the £3bn emergency debt package will help the company push through its turnaround plan. Weston says: “We are pleased the Court sanctioned the Company Plan. This is good news for our customers, puts our business on a firmer financial footing and enables us to continue to invest in our network and deliver critical infrastructure upgrades for our customers and the environment. Importantly, this decision will support the delivery of our turnaround which is underway.” Had the debt deal not been approved, Thames Water had warned it could run out of cash at the end of March. Even so, it is still in a sticky situation. The court heard evidence this month that the indebted company may need as much as £10bn in debt and equity investment to repair its finances… Newsflash: Thames Water has won court approval for an emergency debt package worth up to £3bn that should stave off the collapse of Britain’s biggest water company for at least another few months. The company has just told the stock market that London’s high court has decided that the deal could proceed, after hearing four days of complex arguments earlier this month over whether it should go ahead. Thames, which has 16 million customers and 8,000 employees, has been on the verge of collapse for months, with debts of about £19bn. The financial difficulties have contributed to underinvestment in the pipes and drains needed to prevent sewage overflows into rivers and seas. The deal will give Thames £1.5bn in upfront cash, plus up to £1.5bn more to see it through an appeal to try to increase bills by more than the 35% allowed by the industry regulator for England and Wales, Ofwat. Thames had argued in court that it would run out of money on 24 March if the emergency debt deal did not go through. It will still have to raise billions of pounds more of equity to repair its finances over the longer term. Sir Adrian Montague, Chairman of Thames Water, has welcomed the decision, saying: “The Court’s approval of the Company Plan marks a significant milestone for Thames Water, enabling us to proceed with the implementation of the Liquidity Extension Transaction. Its implementation is a key step in strengthening our long-term financial resilience and will allow us to continue progressing the equity raise process and a holistic recapitalisation transaction as well as complete the CMA appeal process in respect of Ofwat’s PR24 price review. Critically, it enables the management team to continue progressing the turnaround.” Britain’s water quality at some sites is notoriously revolting, and now the water companies are revolting too! South East Water and Anglian Water have both announced today they are appealing to be allowed to raise customers’ bills by more than regulator Ofwat approved last year. Anglian Water says Ofwat’s decision to only allows its bills to rise by 29% in 225-2030 was unacceptable, as it plans an £11bn programme of infrastructure improvement. It is asking the Competition and Markets Authority to consider the issue. Chief Executive Mark Thurston says: “In the East of England, with four of the fastest growing cities in the UK, as well as the Cambridge-Oxford Arc, the levels of investment needed are significant. As a long term, purpose-driven business we are planning sustained investment over decades to build resilience against a changing climate, deliver essential investment in water and sewerage infrastructure, and protect and enhance the environment – all of which will create jobs and bolster the local economy, helping our region to thrive. South East Water, which was allowed to raise bills by 24%, is also appealing. Its chairman, Chris Train. says: “Asking for the Final Determination to be referred to the Competition and Markets Authority for redetermination is not a decision we took lightly. We have scrutinised the Final Determination and agree unanimously that in its current format, it presents a risk to water security for our customers in the region.” Last week, Thames Water announced it will also appeal against Ofwat’s decision: The increase in UK wage growth in the last quarter is likely to deter the Bank of England from rapid cuts to interest rates this year. Currently, the City expect two more quarter-point cuts to Bank rate by the end of the year, to 4%, following the reduction from 4.75% to 4.5% earlier this month. But with total wages rising at 6% in the last quarter – three times as fast as the BoE’s inflation target – policymakers may be cautious. Currently, the money markets say there’s a 78% chance that the Bank leaves rates on hold next month. A cut isn’t fully priced in until June – earlier this month it was May. And the third cut of the year might not happen until September or even November’s meeting – rather than coming as early as August, as had been pencilled in recently. Today’s data illustrates the challenge facing the Bank’s Monetary Policy Committee (MPC), says Matt Swannell, chief economic advisor to the EY ITEM Club, adding: Having weakened over the course of 2024, there were no clear signs that the prospects for the jobs market are improving. At the same time, pay growth is still too high to get inflation back to the 2% target, and firms will soon face the extra cost burden of higher employer National Insurance Contributions (NICs). Faced with this trade-off, we think the MPC will continue to lower Bank Rate gradually, with the next cut likely to come in May, and that the Bank of England will use this extra time to gauge just how sticky inflation will be. But some experts argue that the Bank will cut rates four times this year – not just the three expected by the markets. Thomas Pugh, economist at leading audit, tax and consulting firm RSM UK, says: “The further rise in pay growth, combined with signs of a gradual easing in employment rather than a collapse, will keep the Bank of England on its “gradual and careful” rate cutting path. We still expect the MPC to cut rates at every other meeting this year, which would leave interest rates at 3.75% by the end of the year. The UK labour market looks better than some of the gloom swirling about the economy, argues James Smith, developed markets economist at ING. He tells clients: An air of pessimism is befalling the UK jobs market right now, ahead of a sizeable increase in employer’s National Insurance (social security) in April. The surveys on hiring are turning increasingly sour and there’s growing talk of redundancies as firms grapple with the combined hit of tax hikes and a near-7% increase in the National Living Wage. Bank of England policymaker Catherine Mann, explaining her vote for a bumper rate cut this month, spoke of “non-linear” falls in employment. Despite that gloomy backdrop, the hard numbers on the jobs market currently don’t look so bad. Unemployment is broadly stable, though remember this data is highly dubious right now. But even the supposedly more reliable payroll-based numbers were more stable in January. The steady 1% fall in those numbers across 2024, once government-heavy sectors are excluded, stalled last month. More importantly, there’s no discernible increase in redundancies. So-called HR1 notifications, which companies are required to submit to the government if they are planning layoffs, are bouncing around their lows. The major question is whether that changes as the tax and Living Wage changes come through in the second quarter. That’s not to say the jobs market hasn’t cooled materially, though. Vacancies have fallen steadily over the past couple of years, back to pre-Covid levels. On a sector basis, vacancy rates in the likes of retail and hospitality are well below the levels seen in 2019. And that makes it all the more puzzling that wage growth is still up around 6%. Work and Pensions Secretary Liz Kendall is pledging to bring down the UK’s economic inactivity levels, saying: “Since July, wages have continued to grow at pace, putting vital money back in people’s pockets as we work to make work pay and improve living standards for all. “But these figures also show that too many people are being locked out of work and denied that chance, including those sick and disabled. “Instead of writing people off and labelling them, we must step up our support.” A new rail watchdog will give passengers a voice and hold the railway to account, the government has promised, as it launched a public consultation ahead of legislation to create Great British Railways. Ministers intend it to have a beefed-up role in the future nationalised railway, with train operators having an obligation to consult the watchdog – which will replace the current Transport Focus – ahead of major decisions affecting passengers. The new body will be tasked with setting standards for passengers on journey information and assistance, publishing reports on poor service and potentially referring instances to the railway regulator for enforcement action. The eight-week consultation will also lay out plans to unite train and track operations and give devolved leaders more of a say on services. Transport secretary Heidi Alexander said it was a “landmark reform [to] sweep away decades of failure, adding: “We’re giving passengers a powerful voice with a new watchdog dedicated to addressing their biggest concerns, building railways people can trust, improving our services and boosting the economy in the process.” Laura Shoaf, chair of shadow GBR, said: “GBR will fundamentally change our railways, delivering growth, connections and opportunities across the country. The plans set out today will mean a better railway for everyone that uses it, allowing industry to work closer together, putting passengers and customers first and providing better value for money for taxpayers. Campaigners welcomed the consultation. “Giving the public a say in what rail reform should look like is key to making it a success,” said Paul Tuohy, chief executive of Campaign for Better Transport. He said they backed the creation of a new watchdog, adding: “We will need to see what this means in practice, and whether this new watchdog will have any teeth to hold GBR to account when it needs to.”. The latest drop in job vacancies (see earlier post) shows that businesses lack confidence to hire new staff, the Institute of Directors warns this morning. Alex Hall-Chen, Principal Policy Advisor for Employment at the IoD, says: “The cumulative impact of recent employment reforms, coupled with upcoming increases to employer National Insurance Contributions and the National Living Wage, is significantly weakening the business case for hiring. Our latest data indicates that firms’ headcount expectations remain at historically low levels, comparable to those seen during the early stages of the COVID-19 pandemic in 2020. “Immediate action is needed to address the mounting pressures on businesses and to restore confidence in the labour market. As the Employment Rights Bill approaches its Report stage, we urge the government to introduce targeted changes that will support employers and stimulate job creation. Our data shows that 41% of bus</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Thames Water has avoided collapse, with a high court judge giving approval for up to £3bn of high-cost borrowing. But campaigners are vowing to fight the decision – arguing that Thames should be put into a special administration. UK wage growth accelerated at the end of last year – with total pay rising 6% in October-December. UK energy customers have been warned that bills are likely to jump by 5% in April.</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Never confuse a stock market index with a symbol of national economic health. The truth of that old piece of wisdom was demonstrated on Thursday as the FTSE 100 went on a rip-roaring run – up 104 points, or 1.2%, to a new closing high of 8,727 – while the Bank of England cut interest rates because the UK economy was flat on its back. The point always to remember about the Footsie is that its constituents are an international crew, or at least they operate internationally. Goldman Sachs’ analysts calculated recently that, in aggregate, only 22% of the revenues of FTSE 100 companies were generated in the UK. North America, at 29%, and the Asia-Pacific region, at 23%, are more important. Think of the likes of index heavyweights AstraZeneca, BP, GSK and Shell: their UK revenue exposures are measured in low single-digit percentages. Thus if lower UK interest rates also mean a lower pound – and sterling fell almost a cent against the US dollar as the Bank cut by a quarter-point to 4.5% – there is a straightforward translational effect. Earnings made in dollars are suddenly worth slightly more in terms of sterling-denominated share prices. Those companies exporting from the UK also become marginally more competitive. There are probably also other factors at play. If it is now more likely that UK interest rates will be 4% by the end of year (and possibly a notch lower, according to market prices), the plumpish dividend yield on the Footsie starts to look positively fat. It is 3.4%. Throw in share buybacks, companies’ other way to distribute earnings, and the dividend yield is in effect even higher. Those statistics reinforce another point that analysts have been making for ages: the UK stock market looks cheap versus its international peers. “Comparing valuation to profitability, the UK is one of the cheapest regions in the world,” said the fund manager Fidelity International at the start of this year. At the time, Goldman’s calculations showed the UK stocks as a whole priced at 11.9 times expected earnings, compared with 22.9 times for the US market. Yes, as everybody knows, the US picture is distorted by the huge and richly valued “magnificent seven” tech stocks – the likes of Apple and the chipmaker Nvidia. But, even when big tech was removed from the sums, the US market was still on 19.9 times, way above the UK. Then there are recent market-moving events. Investors are starting to fret about the solidity of the seven at current valuation if a chatbot out of China can knock 17% off Nvidia’s share price in a day. The Footsie, previously derided as Jurassic on account of its overrepresentation of boring banks and commodity stocks, can suddenly be viewed as a way to add safety and diversity to a portfolio. And that 29% exposure to North America still provides lots of exposure to a hot US economy without the hard-to-value AI bits. Then there’s a crucial factor in the background: tariffs. It is possible to believe the UK will be out of Donald Trump’s firing line because it has a trade deficit in goods with the US, unlike the European Union where German carmakers and others may become the president’s targets. Again, the possible advantage is strictly relative – nobody truly wins in a trade war – but they all count. None of the above should provide any consolation to Rachel Reeves. The first mission of the mission-led government was to “kickstart economic growth” and the Bank has halved its forecast for GDP growth in 2025 to just 0.75%. There are no positives for the chancellor there, especially if spending cuts have to follow. It’s just that the Footsie is not the economy.</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>The Bank of England cut interest rates because the UK economy was flat on its back. The point always to remember about the Footsie is that its constituents are an international crew. North America, at 29%, and the Asia-Pacific region, at 23%, are more important.</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Time to recap… The merger between Nissan and Honda to create a new automobile giant is reportedly on the brink of collapse. UK government borrowing costs have dropped to their lowest since December, easing fears that Rachel Reeves’s fiscal headroom has been squished. Borrowing costs fell after data showed a slowdown in the US economy last month, while in the UK firms cut jobs at the fastest rate in several years. Calm has returned to the financial markets, after two days in which trade war fears gripped investors. The yuan has weakened, though, as trading resumed in China after the lunar new year break. America’s trade deficit has widened, as firms rushed to avoid tariffs by importing goods in December. Gold, seen as a hedge against disruption caused by Donald Trump, hit a new all-time high. We’ll be back tomorrow, when the Bank of England is expected to cut UK interest rates at noon…. GW Britain’s stock market has closed higher tonight, as shares recovered some of their losses from earlier this week. The blue-chip FTSE 100 index has ended the day 52.5 points higher at 8623 points, heading back towards last week’s record highs. Pharmaceuticals firm GSK was the top rises, surging 7.6% today after raising its sales target this morning (see earlier post). That’s its biggest daily rise since 2008! Donald Trump’s pledge to crack down on countries who treat the US badly by running a trade surplus may have backfired! New data today shows that America’s goods and services deficit swelled to $98.4bn in December, up $19.5bn from the $78.9bn recorded in November. The increase was driven by a rise in imports – which rose by $12.4bn to $364.9bn, perhaps as US companies tried to beat tariffs by shipping more goods into the country. Exports fell by $7.1bn to $266.5bn, adding to the deficit. Ransomware payments fell by more than a third last year to $813m (£650m) as victims refused to pay cybercriminals and law enforcement cracked down on gangs, figures reveal. The decline in such cyber-attacks – where access to a computer or its data is blocked and money is then demanded to release it – came despite a number of high-profile cases in 2024, with victims including NHS trusts in the UK and the US doughnut firm Krispy Kreme. Ransomware payments last year fell from a record $1.25bn in 2023, said the research firm Chainalysis, which published the payment data on Wednesday. It said payments dropped off sharply in the second half of the year, reflecting the impact of action taken against cybercriminals and a refusal to pay. Good news for Rachel Reeves! The UK government’s borrowing costs have hit their lowest levels since last December. The yield, or interest rate, on UK 10-year gilts has dropped by 10 basis points (0.1 percentage point) to 4.424%, the lowest since December 16th. Longer-dated borrowing costs are also falling, with UK 30-year gilt yields down 11 basis points to 5.013%, also the lowest since mid-December. That means the jump in borrowing costs last month has been entirely wiped out. That jump had sparked much concern that the chancellor might break her fiscal rules unless she raises taxes or cuts spending. The drop in UK bond yields follows a similar recovery in US borrowing costs today, which have dropped in the last few minutes after a survey of the US services sector showed growth slowed last month. The Institute for Supply Management’s services PMI fell to 52.8 percent, down from 54 percent in December, showing slower growth. The report shows that business activity, new orders and employment continued to rise across America’s services companies, but a falling PMI may encourage the US central bank to ease interest rates this year (or at least not put them up!). The US Postal Service has reversed a decision to suspend international parcel deliveries from China and Hong Kong. It has announced it will continue accepting incoming international parcels from China and Hong Kong, after saying late Tuesday night that it would suspend them. CNN has the details: Although no reason was given for the initial suspension of package deliveries from China, the Postal Service suggested Wednesday it was related to broad-based new tariffs imposed Tuesday and elimination of the de minimis exemption. This exemption had allowed anyone, including exporters, to ship packages worth less than $800 to the United States without duties or needing to undergo inspections. Inspecting incoming parcels to collect the new import taxes could prove extremely difficult. “The USPS and Customs and Border Protection are working closely together to implement an efficient collection mechanism for the new China tariffs to ensure the least disruption to package delivery,” the Postal Service said in a statement Wednesday. Trading has begun on Wall Street in a muted fashion. The Dow Jones industrial average rose by 12 points, or 0.03%, at the open, while the S&amp;amp;P 500 dipped by 0.2%. The tech-focused Nasdaq fell 0.6%, dragged down by Google’s parent company, Alphabet, which is off 8% after missing Wall Street expectations last night. Although the Nissan-Honda deal appears to be in serious trouble, 2025 could be a stronger year for M&amp;amp;A activity than 2024. Consultancy firm Bain and Company’s annual global M&amp;amp;A report predicts that two of the fiercest M&amp;amp;A headwinds – the cost of capital and regulatory scrutiny – will ease this year, helping dealmakers. They say: Technology disruption, post-globalization, and shifting profit pools will drive dealmaking in the year ahead as interest rates and regulatory challenges are likely to recede. The report shows that over the past three years, global M&amp;amp;A as a percentage of nominal GDP has hovered around the lowest levels in nearly 30 years: Trade war fears could also drive mergers. Bain say M&amp;amp;A will continue to be a big part of the response to the realignment of the global economic landscape, adding: National economic interests are being reasserted through reviews of foreign direct investment and M&amp;amp;A activity on national interest grounds – and tariff policies, too. To prepare for the second Trump administration’s proposed move to stiffen tariffs, executives are reevaluating global footprints to ensure access to attractive end markets and security of supply, which could prompt both acquisition and divestiture activity. Artificial intelligence is also taking a bite out of M&amp;amp;A work. A Bain survey found one in three M&amp;amp;A practitioners will be using generative AI in dealmaking by the end of the year, and the company predicts gen-AI will enable every step of the M&amp;amp;A process in the next five years. “Whatever you say about the automotive sector right now, it is not boring,” comments Russ Mould, investment director at AJ Bell. He writes: “After the week started with European carmakers staring down the barrel of tariffs from the Trump administration, there is now the news that Nissan’s merger with Honda is falling apart. “Honda executing a three-point turn to propose Nissan becomes a fully owned subsidiary rather than bringing both names together under a jointly owned holding company means already fractious talks on the tie-up may have run out of road. “Nissan’s negotiating position hasn’t been helped by its weak financial performance which has seen its market value plummet. “Elsewhere, Toyota is in an acceleration phase after upgrading its full-year profit forecast and announcing plans to expand in China. “While the West struggles with the transition to electric vehicles, China is pulling ahead in terms of adoption and Toyota has a bold plan to capture share in this market with plans to build a Lexus factory in Shanghai. “Domestic electric vehicle makers have managed to undercut their global counterparts in China but Toyota clearly feels it can compete and, unlike some rivals, it has a strong balance sheet to underwrite its expansion strategy. “The company has been well placed thanks to its focus on hybrid vehicles which are proving popular with motorists in the West beset with range anxiety about EVs, however there are signs this hybrid boom is starting to ease.” Employment at US companies picked up last month by more than forecast, an indication of resilient job growth. Despite mounting geopolitical uncertainty. US private payrolls rose by 183,000 last month, beating forecasts of a 150,000 gain. ADP Research also revised December’s payroll growth higher too, to 176,000. The popularity of Moana 2 has helped Disney grow its revenues despite the disruption caused by a brutal hurricane season. Disney has posted a 5% rise in its earnings in the last quarter – the three months to 28 December – with pretax profits up 27%. Content sales and licensing returned to profit, with earnings up $536m to $312m “driven by the performance of Moana 2”. But hurricanes Milton and Helene cost Disney $120m of profit. The company says: Domestic Parks &amp;amp; Experiences operating income declined 5%, reflecting a 9 percentage-point adverse impact to year-over-year growth due to the hurricanes and cruise pre-opening expenses French carmaker Renault, which owns around a third of Nissan, says it will “vigorously” defend the interests of the group and its stakeholders. A spokesperson for Renault added that recent press information indicates that no decision had yet been made on the possible end of merger talks between Honda and Nissan. It was reported last week that Renault has urged Nissan to negotiate a higher premium from Honda in the merger. Scrapping the Honda deal would leave Nissan stranded, fears Bloomberg Opinion columnist Gearoid Reidy. He writes: Like the driver who stubbornly insists they know where they’re going but ends up lost, pride may have caught up with Nissan Motor Co. Now, the Japanese automaker might be stranded in a place even AAA can’t reach it. News reports on Wednesday said Nissan has withdrawn from the agreement to combine with Honda Motor Co. in a $60 billion deal, just over a month after the two firms formally entered talks on what would have been a historic merger. The sticking point appears to be Nissan’s demand that the merger be one of equals despite Honda having a market capitalization more than five times its size. Honda in turn had proposed first making Nissan into its unit, the reports said, ostensibly to quicken the pace of restructuring at the troubled firm — a proposal unlikely to have gone down well with executives at a company that traces its roots back to before World War I. Reidy adds that Nissan needs the deal more than Honda, after years of cost-cutting by Carlos Ghosn left the automaker trailing in R&amp;amp;D in both electric vehicles and hybrids… More here. At their current market capitalisations, a Honda-Nissan merger would have created a company worth around $60bn, or £48bn. Honda is the more valuable of the two, with a value of ¥7.92trn according to LSEG data, or $51.8bn/£41.3bn. Nissan is worth ¥1.44trn ($9.4bn/£7.5bn). Perhaps that difference is why Honda reportedly sounded out Nissan about becoming a subsidiary – a proposal that seems to have gone down badly! The merger between Nissan and Honda to create the world’s third-largest carmaker is reportedly close to collapse. Sources close to the deal have told Reuters that Nissan is set to call off merger talks with rival Honda, abandoning the £46bn tie-up. Those sources say that talks have been complicated by growing differences between the two Japanese automakers. The news has moved both companies’ share price – Nissan’s stock fell almost 5%, with trading briefly suspended after the Nikkei newspaper reported that it has called off merger talks with Honda. Nissan is reportedly unhappy that Honda had suggested it could become a subsidiary, rather than the two companies joining together in a merger of equals. Honda’s shares, which continued to trade, jumped over 8%. According to Reuters, Nissan and Honda said in separate statements that the Nikkei report was not based on information announced by the companies and that they aimed to finalise a future direction by mid-February and announce it at that time. The news that Honda, Nissan and Mitsubishi were in talks over a possible merger broke just before Christmas last year. If completed, it would combine Japan’s second- and third-largest carmakers, and add the smaller Mitsubishi, in a defensive effort to join forces as the automotive industry goes through its biggest ever period of upheaval Apple could soon find itself pulled into the trade war bubbling away between the US and China. Bloomberg are reporting that China’s antitrust watchdog is laying the groundwork for a potential probe into Apple’s policies and the fees it charges app developers. They report: The State Administration for Market Regulation is examining Apple’s policies, which include taking a cut of as much as 30% on in-app spending and barring external payment services and stores, people familiar with the matter said. Agency officials have spoken with Apple executives and app developers since last year, said the people, who asked for anonymity to discuss sensitive moves. The conversations stem from long-running disputes between Apple and developers such as Tencent Holdings Ltd. and ByteDance Ltd. over iOS store policies — a source of tension between the US company and regulators worldwide. While Beijing has since 2024 targeted the practices of US tech firms from Nvidia Corp. to most recently Alphabet Inc.’s Google, regulators may not formally move against Apple if the current conversations go well. More here: China Weighs Probe Into Apple’s App Store Fees, Practices Both Apple and Google are also being investigated in the UK, where the CMA is looking into the tech firms’ mobile operating systems, app stores and browsers. Container shipping liner Hapag-Lloyd believes it will be able to cope with the imposition of US tariffs on Chinese products, and Beijing’s retaliation. Chief executive Rolf Habben Jansen told reporters on Tuesday. “It is too early to push the panic button.” Habben Jansen added that foreseeable events were easier to handle than the unexpected ones (such as the recent Houthi attacks on vessels in the Red Sea), saying: “Fortunately we are able to react when transport flows change.” The pound has risen to a one-month high this morning, as the US dollar weakens. Sterling is up half a cent against the US dollar to $1.2538, the highest since 7 January. It has nudged higher after this morning’s PMI report (see earlier post), showed that input price inflation hit an 18-month high in January. The pound could be volatile tomorrow, though, when the Bank of England is expected to cut UK interest rates and could also lower its growth forecasts. With gold at a record high, Ricardo Evangelista, senior analyst at ActivTrades, says: The precious metal is finding support amid dollar weakness and growing apprehension over the escalating trade war between the US and China, as well as its likely negative impact on global economic growth prospects. The US dollar’s decline this week, which began after the administration’s last-minute U-turn on imposing additional tariffs on imports from Mexico and Canada, continued Tuesday following the release of disappointing labor and industrial data indicating a slowdown in the world’s largest economy. A weaker dollar is supportive of gold prices. At the same time, US tariffs on China and Beijing’s retaliation are ominous for the global economy, increasing the appeal of safe-haven gold. This demand is further reinforced by renewed uncertainty in the Middle East, following Donald Trump’s comments about taking over Gaza and displacing the Palestinian population.” Donald Trump’s astonishing declaration overnight that the US will take long-term ownership of the Gaza Strip could also be pushing gold higher, as investors wonder what impact this will have on the Middle East. That move, and the new trade war with China, are both worrying markets, says Achilleas Georgolopoulos, senior market analyst at IG: From a market perspective, Trump has essentially brought two new reasons into the spotlight that could potentially result in severe risk-off episodes. At this juncture, the main beneficiary of Trump’s comments has been gold. At the time of writing, it is trading at $2,865, a new all-time high, as market participants are extremely concerned about Trump’s intentions regarding Iran. UK companies cut staffing levels for the fourth month running in January, the latest survey of purchasing managers at British firms has confirmed. S&amp;amp;P Global reports that aside from the pandemic, the pace of job shedding was the steepest since the global financial crisis more than 15 years ago. They blame the increase in payroll costs, following the increase to employer national insurance contributions and the national minimum wage in last autumn’s budget, saying: Lower workforce numbers reflected subdued demand conditions and ongoing efforts to mitigate higher payroll costs. Overall input price inflation hit an 18-month high in January. That matches the message from the ‘flash’ PMI report in mid-January, which we covered here. S&amp;amp;P Global also report that that UK services sector continued to expand last month. Its UK Services PMI Business Activity Index has come in at 50.8 in January, down from 51.1 in December, and the joint-lowest for 15 months (but still over the 50-point mark showing stagnation). The eurozone’s private sector returned to growth, marginally, last month, a new survey shows. S&amp;amp;P Global’s monthly poll of purchasing managers across the euro area has found that the region’s economy was able to eke out growth in January, for the first time since August. It’s HCOB Eurozone Composite PMI Output Index has risen to 50.2, up from December’s 49.6, which is a five-month high. Any reading over 50 indicates a rise in activity. Spain was again the main growth engine, while Germany saw its best monthly performance since last May. On the downside, Italy’s economy was again virtually stagnant, while private sector business activity in France contracted for the fifth month running. Dr Cyrus de la Rubia, chief economist at Hamburg Commercial Bank, says: “The slow pace of growth in the services sector, which was evident almost all of last year, continued at the start of 2025. Putting it more positively, growth at service companies played a crucial role in keeping the eurozone economy in expansion over the past year. Sluggish, but slightly accelerating growth in new orders and employment gives hope that this sector will gain a bit more momentum in the first quarter of this year. Over in Reykjavik, Iceland’s central bank has announced a sharp cut to interest rates. The Monetary Policy Committee (MPC) of the Central Bank of Iceland has voted unanimously to lower its key interest rate by half a percentage point, from 8.5% to 8%. They acted after inflation in Iceland eased to 4.6% in January. But they also warned that global economic uncertainty has risen – presumably a nod to Donald Trump’s return to the White House. Iceland’s MPC says: Demand growth has subsided in line with a tight monetary stance, and the positive output gap in the economy is narrowing. Housing market activity has eased, and house price inflation has lost pace. There are signs that economic activity is stronger than preliminary national accounts figures imply, however, and wage costs continue to rise. Although inflation has eased and inflation expectations have fallen, inflation pressures remain, which calls for a continued tight monetary stance and caution regarding decisions going forward. This is compounded by elevated global economic uncertainty. GSK has lifted its long-term sales targets as it hailed a strong drug pipeline, sending its shares to the top of the FTSE 100 leaderboard this morning. Britain’s second-biggest drugmaker raised its sales target to more than £40bn by 2031, and the shares have jumped by 5.8%, and are on track for their biggest one-day gain since 2022. GSK said its sales rose by 7% to £31.4bn at constant exchange rates last year, as revenues from specialty medicines, HIV and oncology medications grew while vaccine sales fell. The company is now forecasting that sales will rises to more than £40bn by 2031. However, its profits dropped by 34% to £3.5bn last year after it took a £1.8bn charge to settle thousands of cases in US courts over its heartburn Zantac drug, amid claims that the drug caused cancer. It said the vast majority of state court cases had been resolved or dismissed leaving less less than 1% of cases. Emma Wamsley, the GSK chief executive, said: We are increasing and prioritising R&amp;amp;D investment to promising new long-acting and specialty medicines in respiratory, immunology &amp;amp; inflammation, oncology and HIV. Gold is continuing to climb, and has now hit $2,866.54 per ounce. Kelvin Wong, OANDA’s senior market analyst for Asia Pacific, says: “Gold continues to see safe-haven demand given the current situation on the trade tension front.” Novo Nordisk has reported better-than-expected revenues, with sales of its Wegovy obesity drug surging by 86% last year, but expects growth to slow this year. The Danish company has struggled to keep up with demand for its obesity and diabetes treatments Wegovy and Ozempic, which have to be injected by users once a week. The demand has turned Novo into Europe’s biggest company, but it briefly lost the title to French luxury goods giant LVMH last month after it released disappointing trial results for a next-generation obesity drug, CagriSema. The drug did not achieve its target of 25% weight loss in a late-stage trial, sending the company’s share price sharply lower. Novo said today it plans to submit it for regulatory approval early next year, slightly later than its previous expectation of late 2025. The chief executive, Lars Fruergaard Jørgensen, said CagriSema is more potent than Wegovy, and that a new trial will look at different doses and duration. The recent trial data showed some people reached adequate weight loss on lower doses. Another new obesity drug called amycretin had positive results in an early stage trial. Sales of Wegovy jumped by 86% last year, contributing to a 26% increase in overall sales to DKr290bn (£32bn) last year, higher than analysts’ forecasts, and a pre-tax profit of DKR127bn (£14bn), up 22%. It expects sales growth to slow to between 16% and 24% this year. Novo shares have fallen more than 40% since hitting a record high last June. US rival Eli Lilly, which makes the obesity drug Zepbound and Mounjaro for diabetes, reported weaker-than-expected sales last month. Novo bought Catalent, a drug manufacturer for $16.5bn last year to ramp up production of its weight loss drugs. Jørgensen said: “We are pleased with the performance in 2024, where 26% sales growth reflects that more than 45 million people are now benefiting from our treatments. Further, we completed the acquisition of the three Catalent sites, and during the year, we progressed our R&amp;amp;D pipeline, including obesity projects such as CagriSema and amycretin.” Gold has hit a new record high this morning, as nervous investors seek out a safe haven asset. The spot price of gold has gained 0.6% today, to a new alltime high of $2,861.78 per ounce. Gold has now gained 9% so far this year, adding to the 26% gain posted in 2024. Analysts say that gold is benefitting from concerns about the prospect of disruption under Donald Trump, and fears over the disruption tariffs could cause. Jim Reid, strategist at Deutsche Bank, told clients: Investors have grown hopeful that the tariff delays for Mexico and Canada will mean that tariffs are ultimately avoided, whether that’s via further delays or some kind of deal. If that does transpire, then that would avoid a major trade shock that hits growth and raises US inflation, hence the more positive market reaction over the last 24 hours. Nevertheless, there’s little doubt that markets remain pretty nervous about the whole situation, with tariff risk still being priced in to several key assets, and gold prices hit an all-time high. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, says gold could be “the ultimate Trump hedge”, explaining: Investors may look more relaxed now than they did at the start of the week, but havens continue to see increased demand on the back of growing global uncertainties under Trump’s hectic lead and with the prospects that the first weeks under Trump is just a foretaste of what’s to come in the next four years. And there is not a better hedge than gold for protecting a portfolio from Trump worries: the more chaotic international relations become, the greater the demand—especially from central banks looking to reduce US exposure should Trump turn his focus on them. As a result, gold hit a record high for the fourth straight session, reaching $2,860 per ounce in Asia for the first time ever. At this pace, Trump makes $3,000 look like an easy target… Chinese stocks have slipped on the first day of trading after the lunar New Year holidays. The CSI 300 index of big Chinese companies traded in Shanghai or Shenzhen has slipped by almost 0.6% today. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, says: The Chinese markets opened for the first time after a long Lunar New Year holiday, and they opened down on a set of weaker-than-expected PMI figures, on the news of 10% tariff on its exports toward Trump’s USA, and a further escalation of the trade war with the tit-for-tat measures announced yesterday from Beijing, including 15% tariffs on US coal and LNG imports and an antitrust probe into Google. But losses in the CSI 300 index remained measured, as the 10% tariffs from the US were considered as being quite modest – compared to the chatter of up to 60% tariffs, and China’s response to the US was also seen moderated. After the mayhem of ‘Manic Monday’, a level of calm has returned to the financial markets today (despite the weakening yuan). The pound has hit a one -week high of $1.249 last night, recovering all its losses earlier this week as fears of a global trade war hit investor confidence. Wall Street recovered its poise too yesterday, with the Dow Jones industrial average gaining 0.3%. Traders are relieved that Donald Trump suspended US tariffs on Canada and Mexico for 30 days on Monday night – although also aware that only kicks the can down the road for a month. Michael Brown, senior research strategist at Pepperstone, says: In fact, this whole saga could well rumble on until the start of April, when the review ordered by President Trump into US trade policy is due to report back. Perhaps, it is at that point, that we will see tariffs shift from being used as a bargaining chip to further certain political aims, to actually being used as a measure to address trade imbalances. Still, whatever the purpose, the whole thing remains a zero-sum game. China’s currency has weakened as financial traders return to work after the Lunar new year. The eruption of the new US-China trade war this week, which saw tariffs added to exports between the two countries yesterday, has ended the holiday spirits. This pushed the yuan towards the 16-month low set last month. But the fall in the yuan has been cushioned by China’s central bank, as Reuters explains: The dollar rose more than 0.5% against the yuan to a high of 7.2863 in onshore trade, though its gains were capped by the People’s Bank of China (PBOC) setting a stronger-than-expected yuan midpoint rate, around which the currency is allowed to trade in a 2% band. The fixing had been closely watched by investors for clues on whether Beijing would allow the currency to weaken to blunt the impact of sweeping new tariffs imposed by U.S. President Donald Trump. Economists have suggested that China could respond to US tariffs by allowing its currency to weaken, which would boost exports and fight deflation. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. New car registrations in the UK dropped in January, preliminary industry data showed on Wednesday, due to slower demand from both fleet and private buyers. The Society of Motor Manufacturers and Traders (SMMT) reported that overall registrations fell to approximately 137,000 units in January, with over a fifth of those being electric vehicles, aligning with the industry’s continued commitment to the shift towards EVs. That means a small year-on-year drop in car sales – in January 2024, 142,876 new cars were registered. The SMMT is due to release their full report at 9am. Ian Plummer, commercial director at Auto Trader, reports an increase in interest in electric cars – which could help the UK hit its target of banning the sale of new petrol and diesel cars by 2035. “January marked a lacklustre start to 2025 for the new car market, as registrations fell for the fourth month in a row. This year will offer its fair share of challenges for established brands, amid economic uncertainty, tariff threats from the US and fierce competition from a growing array of new Chinese entrants. “A look under the bonnet however does offer some optimism for the industry, with visits to our new car platform up over 20% following the festive lull. “And we can also see the big increase in electric car enquiries made on our platform late last year already playing through into the market, which will come as some relief to manufacturers facing another steep increase in ZEV mandate targets in 2025. There’ll be no let-up in pressure to maintain electric vehicle demand and hit the 28% target, likely resulting in offers to entice buyers over the coming months.” The agenda 9am GMT: eurozone services and composite PMI for January 9am GMT: SMMT data on UK car sales in January 9.30am GMT: UK services and composite PMI for January 3pm GMT: US services and composite PMI for January</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>UK government borrowing costs have dropped to their lowest since December. Borrowing costs fell after data showed a slowdown in the US economy. In the UK firms cut jobs at the fastest rate in several years. Calm has returned to the financial markets, after two days of uncertainty.</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Calm has returned to the markets today, despite the anxiety caused by the new trade conflict between the US and China. The Dow Jones industrial average is now flat, while the broader S&amp;amp;P 500 is now up 0.5%, as investors take the latest tariffs imposed by Washington DC and China on each others exports in their stride. In London, the FTSE 100 share index has clawed back most of its earlier losses – and is now down just 0.1%, or 10 pints, at 8572 points. Despite Goldman Sachs’s warnings that the eurozone faces a ‘sizeable hit’ from rising trade tensions, shares are now higher in Frankfurt and Paris. And the pound has now recovered its earlier losses against the dollar, to trade around $1.246. Our US Politics Live blog is covering the latest action in America: The number of job openings across the US fell at the end of last month, a possible sign that America’s labor market is cooling. Job openings fell to 7.6m at the end of December, down from over 8m at the end of November, a three-month low according to Bloomberg. The US Bureau of Labour Statistics reports: The job openings rate, at 4.5%, decreased over the month. The number of job openings decreased in professional and business services (-225,000), health care and social assistance (-180,000), and finance and insurance (-136,000). Job openings increased in arts, entertainment, and recreation (+65,000). Shares in Palantir, the US spy tech company, have surged by a quarter in early trading after it beat expectations in is results last night. Palantir’s shares are up 26% at $105.53, taking its gains over the last year to 382%. Last night it reported stronger-than-expected fourth-quarter results and guidance driven by AI, including $828m in revenue, beating estimates of $776m. Palantir was co-founded by Peter Thiel, the major Silicon Valley supporter of Donald Trump, who was singled out by prime minister Pedro Sánchez in a speech in Davos last month warning that tech billionaires want to overthrow democracy. Trading in New York has begun in a subdued fashion. The Dow Jones industrial average has dipped by 0.1%, or 44 points, to 44,370 points. The S&amp;amp;P 500 share index has nudged slightly higher, up amost 0.1%. Samer Hasn, senior market analyst at XS.com, says: US stocks are set to fall further today despite the de-escalation of the trade war with the suspension of tariffs from the US on Canada and Mexico. Meanwhile, the market is still waiting for the start of this war with China, which in turn responded with steps that will remind us of the consequences of the escalation on the US domestic front. The Financial Times are reporting that Beijing has revived an antitrust investigation into Nvidia and is considering a new probe against Intel, as part of its response to Donald Trump’s new 10% tariff on Chinese imports. That’s on top of the investigation into Google announced earlier today. The FT says: China’s State Administration for Market Regulation announced on Tuesday that it had opened an competition investigation into Google, which two people familiar with the matter said would focus on dominance of the US group’s Android operating system and any harm caused to Chinese phonemakers, such as Oppo and Xiaomi, which use the software. Chinese regulators, who announced a similar antitrust investigation into Nvidia in December, were now also looking at launching a formal probe into Intel, said two people familiar with the situation. However, the nature of the probe into the US chipmaker remained unclear, one of the people said, adding whether it was officially launched could be affected by the state of US-China relations. President Xi Jinping is expected to speak to Trump in the coming days. More here: China targets Google, Nvidia and Intel as Trump tariffs bite Beauty firm Estee Lauder has announced plans to cut up to 7,000 jobs, as it braces for a global trade war. Estee Lauder is “significantly expanding” a restructuring programme, and now expects to cut between 5,800 to 7,000 positions in a drive to cut costs by $1bn per year. It says this “expanded plan” will fund a return to sales growth, lift operating margins, and allow it to “continue to manage external volatility, such as potential tariff increases globally”. The company announced the planned job cuts in its latest financial results, which show a 6% fall in net sales in the last quarter, and a fall in profit margins. It adds: The Company continues to monitor the effects of the global macro environment, including the risk of recession; currency volatility; inflationary pressures; supply chain challenges; social and political issues; competitive pressures; legal and regulatory matters, including the imposition of tariffs and sanctions; geopolitical tensions; and global security issues Donald Trump’s attention is likely to soon turn to the European Union, predicts Lindsay James, investment strategist at Quilter Investors. Trump has already claimed the EU treats the US “very badly”, and military spending – as well as trade levels – are a sore point. James explains: As well as being upset that EU countries still spend far less than the US on defence, at 1.9% of GDP in 2024 vs around 3.4% in the US, at a time when it is the EU rather than the US that is being threatened, spending on energy is also likely to be a sore subject. In 2024 Europe has sought to evade sanctioned Russian gas by instead importing its unsanctioned LNG at the expense of US volumes. In 2024 US LNG imports to Europe fell 15% year on year whilst Russian imports rose 11%. This funded the Russian war machine to the tune of 7.3bn euros, whilst the EU simultaneously relied on the US to supply ammunition that is in desperately short supply, following years of underfunding of its defence capability and capacity. “With Germany two years into a mild recession, parties such as the AfD, which are openly calling for Nordstream to be restored, are now second place in the polls with around 25% of the vote, closing the gap with the CDU to just two points in recent polls. With the global LNG market expected to move into surplus in 2025, as the dominant supplier, the US will be keen to ensure Russia does not strengthen its foothold into European markets, particularly given the winds of political change that are now being felt across the continent. Christine Lagarde, as Head of the ECB, has already urged leaders to buy more US LNG and weaponry in order to avoid tariffs. The alternative is likely to be a further hit on the already weak European automotive sector, with over a fifth of EU car exports going to the US. With this sector representing approximately 7% of GDP and a similar proportion of the workforce, EU leaders would be well advised to listen. The oil price has fallen back today, amid relief that the US delayed tariffs on Canada – which sends most of its oil exports across its southern border – and Mexico. The US crude oil price has dropped by 2.25% to $71.53 per barrel, while Brent crude is down 1.4%. Both benchmarks rose yesterday as the markets anticipated that a trade war would cause supply disruption. Today’s falls may also reflect concerns that the new US-China tariffs will weaken economic growth. Razan Hilal, market analyst at City Index, says “bearish sentiment dominates crude oil,” adding: Crude oil dipped below $72 following a short-lived rally on tariff concerns. The next key support levels to watch are $69.50 and $66. A deeper decline could signal the start of a more extended bearish trend. Shares in gambling group Entain have jumped by 8% after its US sports betting arm, BetMGM, announced it expects to make a profit this year. BetMGM, joint owned by Entain and MGM Resorts, told shareholders that it expects the 2025 financial year to be EBITDA positive, with net revenue of $2.4bn to $2.5bn. In a financial update, BetMGM also reports it made a loss of $244m in 2024. Adam Greenblatt, chief executive officer of BetMGM, says: “2024 was a year of investment and rebuilding of momentum for BetMGM. Our successful strategic refinement saw BetMGM exit the year with encouraging run rates across our key metrics and Q4 EBITDA trend towards breakeven on a normalized basis. Our leading iGaming business continues to grow strongly and deliver attractive returns. The financial markets are calmer today than during yesterday’s gyrations, and Jefferies’ analyst Brad Bechtel suspects some complacency is setting in. Bechtel writes: The dust settled a bit on the tariff noise with the Mexican and Canadian situations postponed for 30 days. The assumption in markets seems to be that the issue is resolved, and we can all move on but I am not so sure it will be that easy. The market is also glossing over the reality that the 10% tariffs on China did in fact come into effect as of midnight last night, NY time, and China quickly responded with levies of it’s own. It also announced it was looking into the activities locally of Google. China’s tone, in terms of headlines and public comments, remains one in which they seem willing to work with Trump and the US while pushing back lightly on the implementation of tariffs. Their response with taxes and tariffs of their own indicate they will push back that way as well. Another day, another defeat for Saba. The New York hedge fund has been rebuffed by another UK investment trust, Henderson Opportunities Trust, whose shareholders have rejected a proposal to oust four existing directors and install two Saba representatives. Henderson reports that 65.36% of the total votes cast were voted against the Resolutions, which is quite unanimous given Saba controlled almost 25% of the companys shares, and 33.66% of votes cast. Back at parliament, the UK’s national statistician has insisted that data showing high levels of economic inactivity are reliable – despite the well-known problems with the labour force statistics. Ian Diamond told MPs: “Please, please, please don’t think I am being complacent. I lie awake at night worrying about this the whole time.” That data shows around nine million people (corrected!) have dropped out of the labour market due to economic inactivity, including a rise in ill health since the Covid-19 pandemic. Diamond says the ONS works closely with the data it gets from payrolls and employers, and has found the data “hang up pretty well”, especially when compared to records of benefit claimants and from the NHS. The copper price has risen today, amid relief that the US delayed import tariffs on Mexican and Canadian goods last night. Three-month copper on the London Metal Exchange (LME) rose 0.5% to $9,146 a metric ton this morning, Reuters reports Copper, which is seen as a gauge of global growth prospects, had hit a four-week low yesterday, before Donald Trump suspended the imposition of steep tariffs on Mexico and Canada for a month. Audio streaming company Spotify has reported ‘record profitability’ at the end of last year, and predicted earnings will continue to rise in the current quarter. In its fourth-quarter results, just released, Spotify says almost all its key performance indicators (KPIs) exceeded guidance and “profitability reached record levels”. Following price hikes and job cuts over the last year or so, Spotify made an operating profit of €477m in Q4, up from €454m in Q3 and a loss of €75m in Q4 2023. It expects to grow its operating income to €548m for January-March. Spotify has also reported: Monthly Active Users grew 12% Y/Y to 675 million. Subscribers increased 11% Y/Y to 263 million. Total Revenue was up 16% Y/Y to €4.2 billion. Gross Margin climbed by 555 bps YoY to 32.2%. Operating Income rose to €477 million. The company says it recorded its first full year of profitability in 224 Daniel Ek, Spotify founder &amp;amp; CEO, says: “I am very excited about 2025 and feel really good about where we are as both a product and as a business. We will continue to place bets that will drive long term impact, increasing our speed while maintaining the levels of efficiency we achieved last year. It’s this combination that will enable us to build the best and most valuable user experience, grow sustainably and deliver creativity to the world.” Shares in Spotify have jumped over 8% in pre-market trading. Over in Brasilia, Brazil’s central bank has warned that asset prices could be hit by Donald Trump’s policies. In the minutes of its latest policy meeting, Banco Central do Brasil points out that the value of the Brazilian real could be affected by US economic policies. It says: The Committee closely followed the movements of the exchange rate, which has reacted notably to domestic fiscal news, U.S. economic policy news, and the interest rate differential. The implementation of certain policies in the U.S. may pressure domestic asset prices. The bank’s monetary policy committee is concerned about the risk of a deanchoring of inflation expectations, which would force tighter monetary policy for longer. A weaker exchange rate could be inflationary. The head of the Office for National Statistics then called for more cash to help combat falling response rates to its surveys, and to improve the quality of data. Sir Ian Diamond, ONS chief statistician, said it “routinely” offers people incentives to respond to its surveys and it needs “more resources” to improve rates. He told the Treasury Committee of MPs that the public body also needs better data sharing between Government departments to support its work. He said: “Really important is the potential of administrative data to support… and that does require a culture of data sharing in government, one that so many people have commented on as not being in the right place that it should be”. Diamond also tells MPs that the ONS has increased the incentive it provides to people who take part in its surveys, from £10 to £50 [which I think is paid as a voucher]. Shares in Vodafone slumped almost 7% in early trading making the telecoms company the biggest faller among FTSE100 stocks, after reporting a further slump in performance in its biggest market Germany. The fall in market value, which more than wiped out gains over the last year, came despite strong results in the group’s other regions including the UK. Service revenue in Germany fell 6.4% in the company’s third quarter to the end of 2024, a deterioration from the 6.2% recorded in the previous three months. The company blames the ongoing impact of a change in pay-TV laws in Germany, which prohibits landlords from billing cable TV fees to tenants freeing them up to choose their own TV technology for the first time in decades, as well as “intensifying competitive pressure” in the market. Margherita Della Valle, the chief executive of Vodafone, said that the impact of the TV law impact is now over in Germany but that it would take several quarters for the “financial drag to wash through”. However, even excluding the impact of the law change service revenue in Germany declined by 2.6%, with the company losing just over half of the customers affected by the change. “On top of that the market has been a lot more promotional than usual around Christmas and Black Friday and that is also impacting all players in the market,” she said, as the company re-iterated its full year guidance on profit and free cashflow. Della Valle said that the prospects of tariffs on the European Union would have “no real direct impact” on Vodafone, which operates in 50 countries but not the US. Overall, Vodafone group service revenues rose 5.2%, up from 4.2% in the previous quarter, with Della Valle saying that the 70% of its business outside of Germany is performing “exceedingly well”. In the UK, service revenue rose 7.6% as the company looks ahead to completing its merger with rival operator 3 UK, as Vodafone added 37,000 mobile and 72,000 broadband customers. Britain’s labour market statistics were undermined by a rise in people refusing to take part in the survey, MPs have heard. The UK’s national statistician, Ian Diamond, has told the Treasury Commmittee that there was a plunge in engagement with the survey after the pandemic. The labour force survey was suspended in October 2023 when response rates fell. Diamond explains that low response rates have been a challenge since the data series began in the 80s. The problem became worse after Covid-19, Diamond says. The pandemic forced the ONS to suspend its face-to-face interviews, in which a researcher visited people for a 45-minute interview over their jobs situation, and replaced it with telephone interviews. But the ONS found that as the UK came out of the pandemic, people didn’t return to being happy to host interviewers. This led to a steady reduction in response rates, forcing the ONS to suspend the survey in October 2023 because the risk of bias was too high. Diamond tells MPs is it taking “two times” the effort to arrange an interview as before the pandemic. The ONS samples the population to choose candidates for an interview, asking them to phone up to arrange an appointment. But under a third of people actually do that. The ONS is now conducting a “knock-to-nudge” programme, contacting 3,000 people per week to encourage them to take part. But resistance is high, Diamond explains, saying: “We’re finding very, very, very high levels of flat refusal compared with pre-pandemic [levels].” He explains that the ONS doesn’t have a directory of mobile phones, or email addressses, to contact peopel with. All they have is a list of addresses, and landlines to nudge them on. [Committee chair Meg Hillier asks for a show of hands of which MPs have a landline – less than half the committee appear to have one!]. The committee quizzed Diamond and ONS staff about how long they had known about the problem before October 2023. Diamond said the low response rate had been monitored very closely, but did concede that the ONS’s board felt they hadn’t been made aware of the problem. Diamond added that, “with the benefit of hindsight”, he would have put fixing the LFS into its own programme, rather than keeping it within its ARIES programme – which addresses the development for economic statistics Last month, Hillier warned that policymakers risk making “misinformed” decisions because of the defects in the jobs survey. European markets are slightly lower today, with Germany’s DAX down 0.1%. The automobile sector are down another 0.6%, on fears that the US will impose tariffs on the EU. Wall Street is expected to dip into the red when trading resumes in New York, in five hours time. The Dow Jones industrial average is down 0.2% in the futures market, as is the broader S&amp;amp;P 500 share index, after the US imposed 10% tariffs on China, and Beijing retaliated with its own tariffs. The eurozone economy will suffer a “sizeable hit to activity” from the rise in trade tensions, Goldman Sachs warns. They say today that recent events support their forecast of weak Euro area growth, ongoing disinflation and continued sequential interest rate cuts by the European Central Bank. Goldman say: First, we expect a sizeable hit to activity from the ongoing rise in trade tensions. While the Euro area might benefit slightly from trade diversion associated with any US tariffs on Canada and Mexico, President Trump has reiterated his plan to also raise tariffs on the EU. They predict that “elevated trade policy uncertainty” will weigh on growth in coming months, mainly via lower investment and confidence. “Trade diversion” refers to the possibility that manufacturers in countries facing new US tariffs decide to sell their goods in Europe rather than the US. Goldman also warn that the eurozone labour market is slowing, with unemployment ticking up in France and Italy, and wages cooling. The 10% US tariff on all imports from China that kicked in today is not a “game changer” for China’s growth forecasts, says European bank ABN Amro. They predict Beijing will respond with “a further stepping up of monetary easing and fiscal support” – meaning interest rate cuts and more government spending. But, they also warn that America could potentially impose further tariffs. In a note titled US-China tariff war 2.0 kicks off, economist Arjen van Dijkhuizen explains: Although the first tariff implementation now seems to have come even earlier than anticipated in our Global Outlook, The Year of the Tariff, in our base case we already anticipate a material (gradual) stepping up of US import tariffs on China to an average effective tariff rate of 45% per Q2-2026. While talks between Trump and Xi may potentially smoothen the risk of a further escalation for now, Trump stated earlier this week that he sees the 10% tariffs as a first salvo, with tariffs on China potentially moving much higher if no agreement is reached. UBS are sticking with their forecast for the US stock market to keep rising this year, despite the escalating trade tensions. Mark Haefele, chief investment officer at UBS Global Wealth Management, explains: “Although we will continue to monitor trade policy closely, our base case remains for the S&amp;amp;P 500 to rise to 6,600 by year-end. If implemented, tariffs on Canada and Mexico are unlikely to be sustained, resilient US economic growth should support stocks, and we continue to believe that AI presents a powerful structural tailwind for earnings and equity markets. We believe that the recent development of DeepSeek, a lower-cost AI model, will lead to even broader proliferation of AI, enhancing growth and productivity.” UK grocery inflation has eased back for the first time in six months – as retailers ramped up promotions to attract budget-conscious shoppers. The price of groceries increased by 3.3% in the year to January, down from 3.7% in December, with prices falling in toilet roll and cat food but rising in chocolate, butter and chilled juices according to analysts at Kantar. The figure is a drop of potentially good news for the government, as the pace of price rises on food as been one element underpinning persistent inflation in the UK, putting pressure on households’ disposable income. It could also include the Bank of England to lower interest rates on Thursday – the money markets suggest there’s a 98% chance that the BoE lowers Bank Rate from 4.75% to 4.5%. Stocks in London are dropping in early trading, with the FTSE 100 dropping by around 40 points or 0.5%. Vodafone are the top faller, down almost 6%, after reporting a drop in sales in Germany. It blamed a 6.4%% drop in revenues in Germany on the “TV law change”, which prevents landlords from bundling TV services at apartment blocks. Diageo are down 3% after warning of the impact of tariffs on its North America business. Tech stocks in Hong Kong have rallied by 5% today, despite the tit-for-tat tariffs between the US and China. The wider Hang Seng index gained 2.8%. Drinks giant Diageo has warned that its profits will be hit if the US imposes tariffs on imports from Canada and Mexico. Diageo withdrew its medium-term profit guidance this morning, blaming “the current macroeconomic and geopolitical uncertainty” in many of its key markets, which are slowing its recovery plan. Diageo’s brands include Canadian whisky Crown Royal, and tequila brands which need to be made in Mexico for geographic origin requirements. Chief executive Debra Crew told shareholders: Diageo has anticipated and planned for a number of potential scenarios regarding tariffs in recent months. The confirmation at the weekend of the implementation of tariffs in the US, whilst anticipated, could very well impact this building momentum. It also adds further complexity in our ability to provide updated forward guidance given this is a new and dynamic situation. We are taking a number of actions to mitigate the impact and disruption to our business that tariffs may cause, and we will also continue to engage with the US administration on the broader impact that this will have on everyone supporting the US hospitality industry, including consumers, employees, distributors, restaurants, bars and other retail outlets. Speaking to reporters this morning, Crew indicated that Diageo sees a gross impact of $200m to its operating profits from the tariffs on Mexico and Canada, which have now been delayed until 1 March. Consumer rights champion and regular US presidential candidate Ralph Nader has warned that the market mayhem created by Donald Trump’s tariff announcements creates a lucrative insider trading opportunity. Posting on X, Nader says: The plunge in the stock market based on Trump’s announcement of 25% tariffs on Mexico and Canada was suddenly reversed when he paused for a month. The market then surged back. This is the first of many vast insider trading opportunities for the Trumpsters who get advance notice about how Trump’s impulsive actions are going to be announced. Will the Securities and Exchange Commission apply the requisite staff to track these possible serious violations? There will be many more surges up and down in the stock market to come given the preliminary dictates and announcements of the Trump Administration. A quick factcheck, though: Although the US stock market did recover from its lows yesterday, it still finished in the red. The S&amp;amp;P 500, for example, was down 1.9% in early trading, before closing just 0.75% lower – recovering once Mexico’s president announced the breakthrough that delayed tariffs by a month. Also, there’s no suggestion (that I’ve seen, anyway) of insider trading by Trump insiders. China has criticised the US’s decision to slap a 10% tariffs on its imports into America. In a statement announcing retaliatory tariffs, China’s finance ministry said: “The unilateral imposition of tariffs by the US seriously violates the rules of the World Trade Organization. “It is not only unhelpful in solving its own problems, but also damages the normal economic and trade cooperation between China and the US.” Those retaliatory measures by China include: 15% tariffs on US coal and liquefied natural gas 10% tariffs on crude oil, farm equipment, large-displacement vehicles and pickup trucks from the US. An anti-monopoly investigation into Google Adding US companies PVH Corp and Illumina to China’s “unreliable entities list”. Asia-Pacific markets are rallying this morning, despite the trade war breaking out between China and the US. In Hong Kong, the Hang Seng share index has jumped by almost 2.5% while South Korea’s KOSPI has jumped 1.3%. This suggests relief that Donald Trump delayed the tariffs on Mexico and Canada yesterday, and hopes that he might reach a similar agreement when he speaks with China’s president, Xi Jinping, later this week. Chinese markets remain closed due to the Lunar New Year holiday and will reopen tomorrow, giving traders a chance to react to the tariffs imposed by Washington DC and Beijing today. Jim Reid, strategist at Deutsche Bank, says: While markets are generally breathing a sigh of relief, relative to where we were over the weekend, the past few days have raised ongoing questions over Trump’s tariff policy plans. Some immediate concessions on the border issues have avoided immediate severe escalation, but Trump’s comments suggest that he will look to use the delay to leverage broader economic concessions. Indeed, with tariffs being arguably the strongest economic tool that is almost fully at the President’s discretion, we should surely expect that these will continue to be used to both create negotiating leverage and pursue different objectives such as supply security, revenue generation and trade deficit reduction. And some of these, notably using tariff revenue to help fund offset tax cuts, would require actual implementation of new tariffs. So there are reasons to expect lingering uncertainty in markets, and we are seeing this to some extent. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. The US dollar is strengthening this morning, after a day of drama in the world of trade. Overnight, the US has imposed additional 10% tariffs on Chinese imports, implementing what Donald Trump signed off last weekend – and Beijjing has hit back, with retaliatory levies on some US goods and an investigation into Google. But after the leaders of Mexico and Canada agreed to take new measures at their borders with the US, their 25% tariffs have been delayed for a month – easing fears of a global trade war (at least for the moment). That reverse-ferret yesterday helped to lift stock markets off their lows. Addressing reporters in the Oval Office on Monday, Trump maintained that tariffs were a “very powerful” means of both strengthening the US economically and “getting everything else you want”. Every country wants to agree a way to avoid US tariffs, the president claimed. “In all cases, they all wanna make deals.” The feeling in the City is that Trump is using tariffs as a negotiating tool to push other nations into supporting his political priorities – namely border control – rather than tackling trade deficits. Michael Brown, senior research strategist at brokerage Pepperstone, says: In reality, tariffs appear to have little-to-nothing to do with trade agreements, or narrowing the US trade deficit, whatever pretences might be thrown around. So while investors digest the situation – and brace for the next Trump-related newsflash – they’re seeking the safe haven of the dollar. This morning, sterling has dropped by half a cent against the US dollar to $1.24, while the euro is down a similar amount at $1.03 – putting parity in sight again. The Canadian dollar, which slumped to a 20-year low yesterday before rebounding, has weakened again this morning too – to 1.445 to the dollar (still above Monday’s low, though). The Mexican peso has dipped by 0.1% to 20.35/$, again higher than the three-year low hit at one stage yesterday. The agenda 8am GMT: Kantar UK supermarket share data 3pm GMT:: US JOLTS job vaacancies report 3pm GMT: US factory orders for December</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>The Dow Jones industrial average is now flat, while the broader S&amp;amp;P 500 is now up 0.5%. In London, the FTSE 100 share index has clawed back most of its earlier losses – and is now down just 0.1%, or 10 pints, at 8572 points. Despite Goldman Sachs’s warnings that the eurozone faces a ‘sizeable hit’ from rising trade tensions, shares are now higher in Frankfurt and Paris.</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>The European Central Bank did nothing to direct investors away from the consensus view that it plans to ease interest rates further over the course of 2024. It announced fifth cut in seven months on Thursday. President Christine Lagarde said that ECB policy is still “restrictive”, meaning it is bearing down on growth and inflation. Much of the discussion in the press conference revolved around the “neutral rate” at which monetary policy neither stimulates nor restricts growth. Lagarde suggested that any esimates of that were “premature”, suggesting that the bank has further to go in cutting rates. Meanwhile, economic growth in the eurozone is “set to remain weak in the near term”, she said. Financial markets were mostly unmoved on Thursday as Lagarde delivered a message very much in line with expectations. Perhaps the statement that will live on the longest from the press conference was Lagarde’s strong disavowal of bitcoin having any chance of entering central bank reserves. She said that reserve assets must be liquid, safe, and secure. I am confident that bitcoins will not enter the reserves of any of the central banks of the members of the general council. It came after the head of the Czech central bank said that he would consider shifting reserves into bitcoin, and Donald Trump said the US would build up a strategic bitcoin reserve after allying himself with cryptocurrency advocates during the presidential election campaign. You can continue to follow our live coverage from around the world: In the US, Washington DC officials believe there are no survivors after jet carrying 64 people collided with military helicopter In US politics, RFK Jr and Trump FBI pick Kash Patel face Senate confirmation hearings In the UK, Labour is warned tough laws against people smugglers in new bill could penalise asylum seekers And in our coverage of the Middle East crisis, Israel delays freeing of Palestinian prisoners after chaotic scenes during Gaza hostage release That’s all for today, but please do join me tomorrow for more live coverage of business, economics and financial markets. JJ Back to that US GDP reading, at a 2.3% annualised rate for the fourth quarter it was the weakest end to a year since 2018. Samuel Tombs, chief US economist at Pantheon Macroeconomics, said that the world’s largest economy was held up by the consumer, but that may not last. He wrote: Economic growth became increasingly reliant on households last year, with the 4.2% surge in consumers’ spending in Q4 driving essentially all of the overall increase in GDP, offsetting a big drag from inventories and weakness in investment. However, we would caution against concluding that underlying domestic demand remains unassailably strong. We think that a substantial share of the gain in consumption in Q4 reflected households pulling forward purchases in anticipation of tariffs threatened by the new administration. “Consumer spending remained resilient, while investment was weaker,” said Richard Flax, chief investment officer at Moneyfarm, an online wealth manager. Despite [the weakening growth], the US economy has managed to avoid the long-feared recession following the Covid-19 pandemic. Investors are now trying to determine if the Federal Reserve will begin cutting interest rates again in 2025, after maintaining them on Wednesday. In a press conference, Powell stated that the economy “remains strong” while inflation “remains somewhat elevated.” The last questions focus on real incomes and Bulgaria’s economic convergence with the EU. Lagarde says that there has been a catch-up in real incomes compared with pre-pandemic levels. She says that she hopes that consumers will spend more (rather than saving) despite “a degree of uncertainty about European political developments”. The convergence between Bulgaria and the rest of the EU is going well, she says. And with that the press conference is over. The next questions covered her discussions with European Commission president Ursula von der Leyen and the relationship with the US Federal Reserve after it withdrew from a green policy forum. Von der Leyen gave a presentation about the Commission’s policies on restoring competitiveness and innovation, but also to hear from ECB governors, Lagarde says. On the Fed, she says that there is “huge value” in the Network for Greening the Financial System, from which the US central bank withdrew. It has “great value” for policymakers, she said. The next question goes back to the neutral rate debate. Christine Lagarde says the debate about what the neutral rate is is “entirely premature” because European monetary policy is still restrictive. She says that it’s not possible to say whether the bank would lower rates below the notional netural rate to stimulate growth. She says: I cannot tell you that! Lagarde is asked if the eurozone economic recovery is delayed. First of all, there is recovery, she says. The economy is not at potential yet, but it is certainly a recovery, she says. The ECB has good reason to believe that consumption will pick up, and the weak fourth quarter in the eurozone does not reflect the whole year of 2024. Recovery there is; stagflation there is not. Asked about recent bond yield increases that have troubled governments around the world (including the UK), she says that most of that is “largely spillovers” from the US as investors adjusted to Trump’s inflationary policies. Lagarde is asked her confidence on the inflation target, and about a strategic bitcoin reserve. On bitcoin, she says the cryptocurrency will not be added to the reserves of the central banks that make up the European Central Bank. She says that bitcoin is plagued by the suspicion of money laundering and other criminal activity. She says: I am confident that bitcoins will not enter the reserves of any of the central banks of the members of the general council. On the inflation target, there is one item that is still resisting the disinflation (fall in inflation) seen everywhere else – services inflation – Lagarde says. We look carefully at services, she says. All the indicators on wages are heading down at the moment. She said: We are not celebrating that, but we are taking note. The ECB has confidence that wages are on their way down and will impact on the price of services, she says. Lagarde is asked whether it is realistic to believe that exports will contribute to economic growth in light of Trump’s tariffs, and why the ECB didn’t discuss a bigger cut of 50 basis points. Lagarde says: We did not even utter the two numbers five-zero. 50 was not in the discussion at all. On exports, she says they analyse uncertainty around trade as a potential risk, but they don’t have enough certainty on Trump’s trade policy to be confident. There are rumours, there are statements, there are assumptions, but we don’t have any clear, tangible numbers. By March, “we will still be plagued by uncertainty” on trade, Lagarde says. On to the questions. Lagarde is asked about the future direction of interest rates and the neutral rate (at which policy is perceived as neither inflationary nor disinflationary). All governors supported the ECB’s position in a unanimous vote. She says the ECB is still in “restrictive” territory. We know the direction of travel, Lagarde says, but emphasises that the pace will depend on data that comes in after that. And on the neutral interest rate, Lagarde says that the ECB will publish details of changes to the estimated rate. Greater friction in global trade could weigh on growth, Christine Lagarde said. Global economic risks “remain tilted to the downside”, she said. Heightened geopolitical tensions could increase inflation if it pushes up logistical costs. However, she did not come down either way on whether Trump’s proposed tariffs will add to eurozone inflation. She said: Greater friction in global trade would make the inflation outlook in the euro area more uncertain. Inflation is expected to fluctuate around its current level in the near term, Lagarde said. Recent signals point to moderating wage pressures. Most measures of longer-term inflation expectations remain around 2%. European Central Bank president Christine Lagarde has said that the “economy stagnated” and “It is set to remain weak in the near term”. Manufacturing is contracting, while “consumer confidence is fragile”, she said. However, she said that cheaper credit will increase spending. She said: Nevertheless, the conditions for a recovery remain in place. However, she added an early warning that US tariffs could be a problem, saying exports will help “provided trade tensions do not escalate”. European Central Bank president Christine Lagarde has started a press conference on the decision to cut interest rates. She is speaking at a press conference in Frankfurt after the European Central Bank’s announcement. We will bring more details as they come. Melanie Debono, senior Europe economist at Pantheon Macroeconomics, another consultancy, has done a bit of central bank rune-reading. Her verdict is that the ECB is sticking to the same path outlined in December. She wrote: The key line in the decision statement is unchanged, which means that it still includes little in the way of forward guidance, instead pledging data-dependency. It again states that “The Governing Council is determined to ensure that inflation stabilises sustainably at its 2% medium-term target. It will follow a data-dependent and meeting-by-meeting approach to determining the appropriate monetary policy stance.” Recall that the text was edited in December to remove the reference to the need for a “sufficiently restrictive” policy rate. These words were removed to pave the way for further easing. We continue to look for the ECB to trim rates twice more in the current easing cycle, specifically by 25 basis points in March and in June, such that the deposit rate reaches a terminal rate of 2.25%. Back to the European Central Bank, Jack Allen-Reynolds, deputy chief eurozone economist at Capital Economics, a consultancy, said the rate cut was “no surprise”. The accompanying statement implies that more cuts are coming, as is widely anticipated. We think the bank will have to lower interest rates further than most investors expect. The statement is very similar to last month’s. It describes domestic inflation as “high” but notes that this is mostly due to the lagging components of inflation. The overall tone shows that policymakers are confident that inflation will soon return sustainably to the target. The US economy expanded slower than economists had expected in the last three months of the year, according to new government figures. US GDP grew by 2.3% on an annualised basis in the final three months of the year, according to the Bureau of Economic Analysis. That was slower than the 2.6% annualised growth expected by economists polled by Reuters. It was also slower than the previous quarter, when growth was 3.1% annualised. The euro has remained steady in the minutes after the European Central Bank made an announcement firmly in line with market expectations. The euro is down by 0.1% today against the US dollar, with only a marginal uptick since the announcement was published. European bond yields have remained steady as well. Reuters reported: The German 10-year bond yield, the benchmark for the euro area, was last down six basis points [0.06 percentage points] on the day at 2.51%, having dropped earlier after weak growth data. The European Central Bank has said that “the disinflation process is well on track”, suggesting that it is comfortable with cutting interest rates. The bank noted that the eurozone “economy is still facing headwinds but rising real incomes and the gradually fading effects of restrictive monetary policy should support a pick-up in demand over time”. On inflation, it said: The disinflation process is well on track. Inflation has continued to develop broadly in line with the staff projections and is set to return to the Governing Council’s 2% medium-term target in the course of this year. Most measures of underlying inflation suggest that inflation will settle at around the target on a sustained basis. Domestic inflation remains high, mostly because wages and prices in certain sectors are still adjusting to the past inflation surge with a substantial delay. But wage growth is moderating as expected, and profits are partially buffering the impact on inflation. And on the broader economy’s performance, it said: The Governing Council’s recent interest rate cuts are gradually making new borrowing less expensive for firms and households. At the same time, financing conditions continue to be tight, also because monetary policy remains restrictive and past interest rate hikes are still transmitting to the stock of credit, with some maturing loans being rolled over at higher rates. The economy is still facing headwinds but rising real incomes and the gradually fading effects of restrictive monetary policy should support a pick-up in demand over time. You can read the full statement here. The European Central Bank has cut its key interest rate by 0.25 percentage points to 2.75% in an effort to stimulate growth in the struggling eurozone economy. The rate-setting governing council has now cut interest rates five times since the start of summer 2024. The cut was widely expected by financial market traders and economists as the ECB responds to weak growth in the eurozone’s key economies. Eurozone GDP did not grow in the last three months of 2024, according to a preliminary reading published on Thursday. The bank’s president, Christine Lagarde, will give more details of the reasons behind the rate cut at a press conference at 1:45pm GMT. Let’s get the lay of the land ahead of the European Central Bank’s interest rate announcement at 1:15pm GMT. Economists and investors will be taken by surprise if the ECB does not cut its deposit rate by 0.25 percentage points (25 basis points), down to 2.75% from 3%. The bank, led by Christine Lagarde, cut interest rates four times in 2024, down from 4%. The most recent cut was in December last year. The ECB is expected to continue further down that path this year, as many of Europe’s major economies struggle with tepid growth and political volatility. Jim Reid and analyst colleagues at Deutsche Bank said that a 25 basis point cut is widely expected. They wrote: So the bigger question will be how long they’ll continue to cut rates, particularly with core inflation still lingering above 2%. For today, our European economists share that view expecting another 25bp cut, and think the description of the policy stance will be unchanged relative to the last meeting in December. However, the main risk for them is that the ECB will tweak the description of recent data in a hawkish-leaning direction. Another key issue will be the judgement from Lagarde on the likely impact of Donald Trump’s tariff policy – although given that his administration has not revealed any details there will be some uncertainty from the ECB. Holger Schmieding, an economist at Berenberg, an investment bank, said: For the Eurozone, the impact of US tariffs would show up mostly in less growth rather than in changes in prices. As a rough guess, a 10% US tariff on all imports from the Eurozone and the ensuing uncertainty about future US-EU commercial relations could reduce Eurozone growth by 0.3-0.5 percentage points within one year after the start of such a trade war. For the ECB, this would be an argument to cut rates below the 2.25% which we currently project as the trough for the deposit rate. New FTSE 100 record high klaxon! The FTSE 100 is up 0.5%, touching a new high of 8,600.81 points. St James’s Place and Airtel Africa are the biggest movers on strong results, as explained earlier – both are now up more than 9%. Airline EasyJet is also up by 4%. But investor payouts from Shell, a true heavyweight in terms of market capitalisation, are one of the biggest drivers of the benchmark index’s increase. Before the European Central Bank’s interest rate announcement at 1:15pm GMT (2:15pm in Frankfurt), let’s have a quick round-up of some of the US tech results from last night. Questions over multibillion-dollar spending on AI still hang over the US big tech, spurred by Chinese start-up DeepSeek’s shock to the US stock market just days ago. But the companies still reported relatively solid earnings. Microsoft beat market expectations with earnings per share of $3.23, an increase of 10% on a year earlier. Chief executive Satya Nadella was bullish about the prospects for AI spending. Its share price fell 4.2% ahead of the Wall Street opening bell. Tesla shares are up 2% in pre-market trading after the electric carmaker’s boss, Elon Musk, said that the cheaper Cybercab model would start production next year. Musk’s vocal support for Donald Trump has been a key driver of the company’s stock market surge since November. Facebook owner Meta’s share price has risen 1.2% pre-market after it beat fourth-quarter revenue estimates. However, it predicted sales in the first quarter of 2025 might miss estimates. Its results were somewhat overshadowed by the news that it had agreed to pay Donald Trump $25m to settle a lawsuit. Meta boss Mark Zuckerberg has sought a closer relationship with Trump. American Airlines shares are down in pre-market trading, after one of the company’s aircraft, carrying 60 people, collided in mid-air with a US Army helicopter in Washington DC. Local media have reported that at least 30 bodies have been recovered from the Potomac river, where the plane crashed after the collision. Video footage shows the two aircraft colliding in the darkness, with an explosion before both aircraft fell. American Airlines shares are down 2.7% in pre-market trading, according to MarketWatch data. So far there is no indication of any fault on the part of the airline, with investigations into the disaster at an early stage. Shell has given its investors a multibillion-dollar windfall despite reporting weaker-than-expected profits of $23.7bn (£19bn) for last year as global oil and gas prices tumbled. Shareholders of Europe’s biggest oil company are in line for a 4% dividend increase alongside share buybacks of $3.5bn for the last three months of the year. This marks the 13th consecutive quarter in which Shell has given its investors buybacks of more than $3bn, despite falling earnings from its oil and gas. The company reported adjusted annual earnings of $23.7bn for 2024, narrowly missing the forecasts of City analysts who had expected an annual profit of just over $24bn for the year. You can read the full report here: US economic data is also due later today, during the European Central Bank’s press conference. Unlike Europe, the US GDP data is expected to show an economy that was performing well during the last full quarter under former president Joe Biden. Economists expect the data to show growth of 2.6% during 2024. That has not stopped Donald Trump from griping about the Federal Reserve’s decision last night to leave its interest rates on hold. Posting on his social network, Trump wrote: Because Jay Powell and the Fed failed to stop the problem they created with Inflation, I will do it by unleashing American Energy production, slashing Regulation, rebalancing International Trade, and reigniting American Manufacturing Trump has previously called for the Federal Reserve to cut interest rates. That makes his complaint about the Fed’s handling of inflation somewhat contradictory: the central bank held interest rates steady rather than cutting in an effort to push inflation down. And many economists believe that several of Trump’s policies could themselves be inflationary. Most notably, tariffs are almost always passed onto consumers directly, raising prices of imports or forcing them towards higher-priced products from their home country. Jerome Powell, the Fed chair, last night declined to provide “any response or comment whatsoever” on the president’s public demands for lower rates. During a press conference, he said: The public should be confident that we will continue to do our work as we always have, focusing on using our tools to achieve our goals. If the European Central Bank does not cut interest rates this afternoon it would count as a real shock. The eurozone economy is already struggling, and the prospect of US tariffs further hitting growth is adding to worries for politicans and central bankers. Neil Birrell, chief investment officer at Premier Miton Investors, said: Eurozone GDP stagnated in the fourth quarter, yet again showing that the economy is in need of some stimulus. It’s a tough outlook globally at present and uncertainty over White House policy measures aren’t helping. The political issues in Germany and France are adding to the strain, creating a cocktail that is making it difficult for businesses and consumers alike. The ECB will no doubt step up the plate to help out. The euro has edged down today, with most of the movement coming at 9am after the weaker-than-expected German GDP reading. But it has not been a dramatic shift: the euro is down 0.1% against the US dollar at $1.04. Traders will wait for Christine Lagarde’s comments at the European Central Bank press conference this afternoon. Against the pound the euro has fallen by 0.2%. A pound buys €1.20. It was a flash reading on the Eurozone economy, so we don’t have the details on what the drivers were. But it’s clear that it was a weak end to 2024. But the European Central Bank might be able to spur a bit of economic growth in the eurozone with looser monetary policy. Charlie Cornes, senior economist at the Centre for Economics and Business Research, a consultancy, said: This marks a weak end to last year, following positive growth in the first three quarters of 2024. As a result, first estimates suggest that the currency bloc as a whole grew by 0.7% in 2024. Declining activity in Germany – the Eurozone’s largest economy – has weighed on the bloc’s growth, with German GDP contracting by 0.2% on the quarter. This suggests Germany has now seen annual declines in activity for two consecutive years. In 2025, further loosening of monetary conditions is expected to provide a modest uptick in activity for both Germany and the Eurozone, with growth expected to amount to 0.3% and 1.0% respectively. The decision to greenlight a giant new oilfield off Shetland has been ruled unlawful by the courts in a major win for environmental campaigners. The proposed Rosebank development – the UK’s biggest untapped oilfield, due to be developed by Norwegian oil company Equinor – had been given the go-ahead in 2023 under the previous government. But on Thursday the court of session in Edinburgh sided with campaigners and climate experts in ruling that the original decisions to permit Rosebank and a second, smaller, gas field called Jackdaw were unlawful, as they had not taken into account the carbon emissions created by burning any oil and gas produced. British oil company Shell is due to develop Jackdaw. Tessa Khan, from the campaign group Uplift which has been at the forefront of the campaign to stop Rosebank, said the court ruling was a significant milestone. “This … means that Rosebank cannot go ahead without accounting for its enormous climate harm,” she said. A spokesperson for Equinor said it welcomed the judgment, which allows it to continue preparation work on the Rosebank field although it prohibits any drilling. They said the project would bring investment and jobs to the UK, adding: “We will continue to work closely with the regulators and DESNZ to progress the Rosebank project.” A spokesperson for Shell, the company behind the Jackdaw field, also welcomed the decision, saying it allowed its preparatory work to continue “while new consents are sought. Swift action is needed from the government so that we and other North Sea operators can make decisions about vital UK energy infrastructure.” They added that if Jackdaw went ahead it would provide “enough fuel to heat 1.4m UK homes, at a time when older gas fields are reaching the end of their production and the UK is reliant on imported gas to meet its energy needs.” The eurozone economy did not grow in the final three months of 2024, adding weight to the argument that the European Central Bank will ease interest rates further this year. Eurozone GDP growth came in at 0% quarter-on-quarter for the fourth quarter of 2024, according to the European Commission. That was a steep drop from the 0.4% growth rate in the previous quarter. It was also unexpected: a poll of economists by Reuters found that the consensus expectation was for growth of 0.1%. Germany has now gone two consecutive years with a shrinking economy. The only reason that it has not been called a “recession” so far is that by convention that word applies to two consecutive quarters of contraction. As the below quarterly GDP chart from Trading Economics shows, the country has narrowly avoided that fate over the last nine quarters. The economy has spent the last two years narrowly avoiding the “recession” word, but that will not be much comfort to its citizens – or to chancellor Olaf Scholz as he tries to retain his position at the German elections on 23 February. The GDP data today show that the German economy shrank by 0.2% year-on-year in 2024, after shrinking by 0.3% in 2023. It’s the first time since the early 2000s that the German economy contracted for two consecutive years, according to Carsten Brzeski, global head of macro at ING, an investment bank. He wrote: The German economy has now been stuck between cyclical and structural headwinds for several years, and 2024 was finally the year that many politicians realised that the old macro business model of cheap energy and easily accessible large export markets was no longer working. Ten years of underinvesting, deteriorating competitiveness and China’s shift from an export destination to a fierce industrial competitor have taken – and will continue to take – their toll on the German economy. Contrary to the early 2000s when Germany’s economic “sickness” or problem was high unemployment and a rigid labour market, the current problems are much more diverse and hence even more difficult to solve than they were 20 years ago. Let’s also not forget that the external environment in the early 2000s was far more favourable for Germany, with China’s entry into the World Trade Organization and the EU’s enlargement. This contrasts sharply with today’s geopolitical tensions, a nearby war, and the rise of protectionism. Germany’s economy contracted by more than expected in the fourth quarter of 2024, according to data that suggest the Eurozone economy as a whole may not have expanded. Germany’s GDP dropped by 0.2% quarter-on-quarter in the last three months of the year, according to preliminary data from the statistics office. That was worse than the 0.1% contraction expected by economists polled by Reuters. France’s economy shrank by 0.1% in the quarter, while Italy’s economy also recorded zero growth. The figures underline the rationale for interest rate cuts from the European Central Bank later today. Andrew Kenningham, chief Europe economist at Capital Economics, a consultancy, said: With national data now available for all larger euro-zone countries, it looks as if GDP growth in the region slowed to 0.1% q/q or even zero in Q4 last year. The region’s two largest economies both contracted and Italy recorded no growth. With the major economies set to remain lacklustre this year even if a major tariff war is avoided, we expect the ECB to cut its deposit rate by 150bp this year to 1.50%, starting with 25bp later today. One of the driving forces of market gyrations this week has been concerns over the emergence of DeepSeek, a Chinese artificial intelligence company that appears to have blown rivals out of the water with an AI model that used a fraction of the resources of others. That threatened to undermine the narrative of ever-increasing use of resources – particularly computing power – that had fuelled the AI boom. Chip maker Nvidia’s share price duly plummeted on Monday in the biggest one-day fall in notional value in stock market history. There has been a notable round of briefing since then from the US competitors led by OpenAI as they try to reassure investors. The latest news reported by the Financial Times, with very helpful timing, is that Japanese investor SoftBank is in talks to invest as much as $25bn in OpenAI. Donald Trump last week announced a data centre joint venture, dubbed Stargate, between SoftBank and OpenAI – only for it to be overshadowed by DeepSeek. Yet SoftBank, led by Masayoshi Son, wants to break into AI. The FT cited a person familiar with the matter saying: The talks are ongoing and the amount that SoftBank could invest in primary equity into OpenAI is a moving target. That followed briefing yesterday that OpenAI has alleged that DeepSeek “distilled” data from its model, allowing it to skip much of the expensive effort of training AI models. If confirmed, that would violate OpenAI’s terms of service. Owners of the data used by the American company to train its model may be forgiven for at least one eyebrow hitting the ceiling at that complaint. OpenAI has argued in submissions to the UK’s House of Lords that it would be impossible for its technology to exist without training on copyrighted material – without the consent of the owners of that material. Tech website Gizmodo wrote: “OpenAI Claims DeepSeek Plagiarized Its Plagiarism Machine”. Germany’s Dax stock market index is also in on the party with a new record high, while Spain’s Ibex benchmark is at its highest since 2008, before the Eurozone crisis crunched its economy for a decade. Spain’s stock market has risen strongly in the last couple of years, as the country has become the surprise leader of the European economy – with a growth rate far outstripping the EU’s largest economy, Germany. However, the stock market has a long way to go before it surpasses that level, pumped up by the country’s housing bubble. The biggest gainer on the FTSE 100 is telecoms company Airtel Africa. Its share price rose 7.2% after it reported a 20% increase in revenues for the first nine months of its financial year. It is vying with St James’s Place, after the wealth manager enjoyed stronger inflows. Reuters reported: Posts record funds under management of £190.21bn at 2024-end, above analysts’ views of £187.4bn, according to company-compiled consensus. It has started off as a fairly mild trading day across European stock markets. All the major indices have gained ground in early trading. But that has still pushed the Euro Stoxx 600 index to its latest record high. The Stoxx 600 reached 535.9 points on Thursday morning. It has risen from below 500 in mid-December as investors expect the European Central Bank to act to support the economy. The FTSE 100 is up by 0.1%, or eight points, at 8,566.3. That leaves it 20 points short of its all-time high of 8,586.68 from a week ago. Could the ECB also help it to a new record later? Good morning, and welcome to our live coverage of business, economics and financial markets. Royal Mail is set to be allowed to deliver second-class letters only on alternate weekdays and not on Saturdays after the industry regulator announced a shake-up of postal service rules. Communications regulator Ofcom has proposed that Royal Mail would still be required to deliver first-class letters six days a week and the price cap on second-class stamps would remain, but the company will be allowed to make cost savings by cutting the number of days it goes to every address. The changes could save Royal Mail between £250m and £425m each year. The cuts would be a boon to Czech billionaire Daniel Křetínský’s EP Group, as it nears a £3.6bn takeover of Royal Mail’s FTSE 250-listed parent company, International Distribution Services. Shell profits fall, but investor payouts rise Shell has handed its investors a multibillion-dollar windfall despite reporting weaker than expected profits of $23.7bn for last year as global oil and gas prices tumbled. Shareholders of Europe’s biggest oil company are in line for a 4% dividend hike alongside share buybacks of $3.5bn for the last three months of the year. This marks the thirteenth consecutive quarter in which Shell has handed its investors buy backs of more than $3bn, despite falling earnings from its oil and gas. European Central Bank expected to cut interest rates The European Central Bank, led by Christine Lagarde, is widely expect</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Christine Lagarde said that ECB policy is still “restrictive”, meaning it is bearing down on growth and inflation. Economic growth in the eurozone is “set to remain weak in the near term’ Lagarde disavowed bitcoin having any chance of entering central bank reserves.</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>The second Trump administration is expected to strike a blow to efforts to align the global financial sector with the path to net zero, with banks, asset managers and industry groups already moving to accommodate the incoming president’s avowed policy of “drill, baby, drill”. As authorities declared 2024 the hottest on record, atmospheric carbon dioxide leapt by a record amount and fires ravaged Los Angeles, a key private sector climate alliance, the Glasgow Financial Alliance for Net Zero (GFANZ) abandoned a requirement that members be aligned to the Paris agreement. That was followed by a network of net zero asset managers suspending work, and deleting from its website its statement of commitments that members must adopt, after BlackRock, the biggest of them all, quit its ranks. As Trump takes office with an agenda of reversing US green policies, seen as part of a “woke” agenda at which he and his followers have taken aim, analysts and observers expect that worse is yet to come. “Honestly, even if you look at politics around the world, it feels like the populist right is pushing hard on an anti-net zero ticket,” said James Alexander, the chief executive at the UK Sustainable Investment and Finance Association. “It is particularly disheartening to see this news come right at the time of, you know, the worst wildfires we’ve ever seen in Los Angeles, floods across the world, heat waves, and right on the eve of Donald Trump’s inauguration. “The inauguration doesn’t look like a coincidence. And it’s really disappointing to see that this is the effect that … political attacks are having on the commitments of institutions to these alliances.” Launched with fanfare at Cop26 in Scotland three years ago, GFANZ was intended to be a sector-wide collaboration to “mobilise the trillions of dollars necessary to … deliver the goals of the Paris agreement”. At the time, Mark Carney, the UK government’s climate finance adviser for Cop26, said: “This is the breakthrough in mainstreaming climate finance the world needs.” He became chair of the new groups, which he said would be “the gold standard for net zero commitments in the financial sector”. But on the eve of the new year, Carney announced a major revision to those commitments, as GFANZ in effect dropped its requirement for members’ activities to be aligned with Paris, amid a drip-drip exodus of major US banks – the six biggest of which have quit the banking industry’s net zero group since December. But Andrew Garraway, the head of climate policy at climate analytics firm Risilience, said: “It would be wrong to ascribe the difficulties at GFANZ and the sectoral alliances solely to Trump, as they’ve faced increasing Republican resistance since their establishment in 2021. “However, the Trump presidency is indeed the catalyst for many US financial firms stepping back from GFANZ and the sectoral alliances, with firms nervous of the potential political and legal ramifications of being seen to be too active on decarbonisation.” BlackRock, which manages funds worth $11.5tn, quit the Net Zero Asset Managers (NZAM) initiative, saying its membership had “caused confusion regarding BlackRock’s practices and subjected us to legal inquiries from various public officials”. Almost immediately, NZAM suspended its monitoring of members’ progress towards commitments, and announced a review “to ensure NZAM remains fit for purpose in the new global context”. Paddy McCully, a senior energy transition analyst at Reclaim Finance, said: “NZAM’s requirements of its members were so weak as to be to mainly symbolic, but symbolism can be important, and Wall Street saying it will no longer cooperate to finance the energy transition sends a message to big polluters that they can carry on with business as usual.” Alexander said firms were not just trying to please the incoming Trump administration and a few rightwing politicians, but that there was a widespread mistrust of progressive policies among the US electorate. “And our analysis is the ESG [environmental, social and governance investing principle] backlash is not a grassroots thing,” he said. “It’s something that has been created by those that stand to lose the most from the net zero energy transition. And they are, of course, oil and gas firms, some of the most well capitalised companies in the entire economy. “They’re facing an existential threat in the sense of their licence to operate being removed. And they are fighting back really, really big-time. And it’s working really well in America for them right now.” GFANZ and NZAM have been approached for comment.</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Glasgow Financial Alliance for Net Zero (GFANZ) abandoned a requirement that members be aligned to the Paris agreement. Network of net zero asset managers suspending work, and deleting from its website its statement of commitments.</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Time to wrap up…. The UK’s blue-chip stock index hit a record high on Friday, as rising hopes of interest rate cuts this year drove down government borrowing costs. Almost every share on the FTSE 100 rose on Friday, as a fall in the value of the pound boosted multinational companies listed in London and propelled the index above 8,500 points for the first time. The “Footsie”, which tracks the 100 biggest London-listed companies, rose 1.6% to hit a fresh intraday high of 8,533.43 points amid growing confidence that the Bank of England will ease monetary policy this year, before closing at 8505 points… UK government bond prices have also eased back from their recent highs, helped by expectations of interest rate cuts this year. The International Monetary Fund has upgraded its forecast for UK growth this year in an update to its biannual assessment of the global economy, while taking a swipe at plans by Donald Trump’s incoming US administration for the potentially destabilising effect of large-scale tax cuts, import tariffs and weaker regulations. In a fillip to the Labour government, the Washington-based organisation said it expected the UK economy to grow by 1.6% in 2025, up from an earlier forecast of 1.5%. The IMF judged that Labour’s increase in investment spending, improved household finances and a series of interest rate cuts by the Bank of England would give the UK economy a lift, after growing by 0.9% in 2024 according to the fund’s expectations. The Bank of England will further delay capital rules meant to prevent another 2008-style crash, as it weighs the impact of Donald Trump’s return to the White House and the chancellor Rachel Reeves’s call for regulators to help drive UK growth. The US supreme court has issued a ruling upholding a nationwide ban on TikTok unless it sells to an owner in the US. The nine justices voted unanimously in a decision on Friday that sides with the majority of US Congress and the US Department of Justice that the hugely popular social media app is a threat to US national security. The FTSE 100 has topped off its surge by ending the day at a new closing high of 8,505 points. Jo Rands, portfolio manager at Martin Currie, says: “The FTSE100 has hit an all-time high, despite the negative rhetoric around rising gilt yields and the outlook for the UK economy. The large cap index is traditionally a low beta defensive market, which is predominantly composed of very international businesses. The FTSE 100 generates c.80% of its revenues from outside the UK, which also means the weaker pound has been a positive influence for the index. “The year has started with the index being powered by index heavy weights such as BP and Shell, which have advanced following rising oil prices, and with the Banks benefitting from a pushback on interest rate cuts. The IMF has credited Rachel Reeves’s first budget with having a positive impact on growth, despite the increased taxes on businesses. Discussing today’s upgraded UK growth forecast, from 1.5% to 1.6% for this year, the Fund’s chief economist, Pierre-Olivier Gourinchas, said it reflected measures in the budget as well as the impact of real wage growth, and likely interest rate cuts this year. Gourinchas says: Some of that revision is reflecting the fact that we have a continued pick-up in real incomes and in consumption in the UK. But it also reflects some of the effect of the fiscal measures that have been announced by the authorities in their October budget that are expected to lead to higher public investment, in particular. That will support economic activity. The forecasts also assume “continued easing of monetary policy”, with the IMF expecting the Bank of England will cut interest rates once per quarter this year. Gourinchas does point out that some of the increases in public spending in budget are funded by increases in taxes, such as higher national insurance contributions for businsses. That could weigh down, but the net effect in our assessment is still positive for growth for the UK economy in 2025. Over in the US, the supreme court has upheld a divest-or-ban law targeting TikTok. The deicsion means that a law forcing TikTok’s Chinese owner to sell its US business by Sunday, or face a ban, will go into effect. Our Politics Live blog has the details: Stocks are also rallying on Wall Street, helped by falling bond yields and better-than-forecast growth data from China overnight. The Dow Jones industrial average is up 0.8%, or 350 points, at 43,504 points, with the broader S&amp;amp;P 500 index up 0.9%. Newsflash: The UK is expected to post the fastest growth among major European economies this year, although still lag behind the United States and Canada. The International Monetary Fund has raised its forecast for UK growth this year to 1.6%, up from 1.5% predicted in October. That would mean Britain would outpace Germany, whose predicted growth in 2025 has been cut to just 0.3% from 0.8%, as well as France (expected to grow by 0.8% this year) and Italy (0.7%). The Fund has raised its forecast for US growth this year to 2.7%, up from 2.2%, while Canada’s forecast has been cut from 2.4% to 2%. Japan is still forecast to grow by 1.1%. However, these forecasts don’t seem to include the possibility that Donald Trump triggers a damaging trade war. Pierre-Olivier Gourinchas, the IMF’s Economic Counsellor, says: Our projections incorporate recent market developments and the impact of heightened trade policy uncertainty, assumed to be temporary, but refrain from making assumptions about potential policy changes that are currently under public debate. Gourinchas warns that policies such as higher tariffs or immigration curbs would reducing US economic output and add to price pressures. Gourinchas also predicts that central banks will be able to lower interest rates this year, saying: Inflation is declining, to 4.2 percent this year and 3.5 percent next year, in a return to central bank targets that will allow further normalization of monetary policy. There’s encouraging news for Rachel Reeves in the bond markets today. UK borrowing costs have fallen, and are now almost back at their levels early last week before bond yields surged. The yield, or interest rate, on 10-year UK government bonds has dipped by four basis points, or 0.04 percentage points, to 4.627%. That’s the lowest level since last Tuesday, 7 January, the first day of the sell-off in UK debt that drove 10-year borrowing costs to their highest since 2008. The yield on 30-year UK bonds has also dropped by 4bps, down to 5.187%. Last week it hit 5.474%, the highest since 1998, but has fallen for the last three days. The recovery comes after the UK government insisted it would stick to its fiscal rules, an indication that spending cuts or tax rises might be implemented rather than increased borrowing. It also reflects expectations that the Bank of England may cut interest rates several times this year, after the latest inflation, growth and retail sales figures were lower than expected this week. But it is also part of a wider recovery in bond prices in recent days. US Treasury yields have also dropped this week, following reports that Donald Trump’s administration may take a more gradual approach to tariffs. The FTSE 100 is continuing to rally, and just poked its nose over the 8,500-point mark for the first time ever. The blue-chip share index has now hit a new alltime high of 8506.80 points. As we covered late last year, analysts had predicting stock markets would rally this year – with AJ Bell suggesting the FTSE 100 could reach 9,000 points. The recent jump in Britain’s bond market borrowing costs are a “concern”, according to credit ratings agency S&amp;amp;P Global today. However, S&amp;amp;P said it wasn’t severe enough yet to have an immediate impact on the UK’s AA credit rating. In a research note, S&amp;amp;P argue that the situation is “manageable”, although higher borrowing costs may lead to a fall in investment. S&amp;amp;P Global Ratings credit analyst Frank Gill says: “The selloff, which started at the end of 2024, has been fairly broad-based across the safe asset space. Yet G7 governments with larger net borrowing requirements--including France, the U.S., and the U.K.--have underperformed, pointing to a rise in risk premia.” S&amp;amp;P point out that UK policymakers have options – the Bank of England could slow the pace of its sales of UK debt (under its QT programme, which is unwinding stimulus). City traders are increasingly confident that the Bank of England will cut UK interest rates next month. The money markets now indicate there’s an 81.5% chance that Bank rate is lowered to 4.5%, from 4.75%, at the BoE’s next meeting on 6 February. Those interest rate expectations have pushed the pound down to $1.22 this morning. Raffi Boyadjian, lead market analystat XM, says: The pound stands out as being the weak link among the majors, as it looks set to post a third straight weekly decline. It’s been a busy week for UK data releases consisting of CPI, GDP and retail sales figures. But all three reports came in below expectations, boosting the odds that the Bank of England will lower rates at its February 6 meeting. Nevertheless, the pound’s freefall has been good news for UK stocks, with the FTSE 100 hitting intra-day record highs today. The FTSE 100 has been derided as a ‘Jurassic Park’ index over the years, for its lack of exciting technology companies. But that boring nature is actually attractive to investors because it provides some protection for investors in a time of geopolitical uncertainty, says Susannah Streeter, head of money and markets at Hargreaves Lansdown. Streeter says: FTSE 100 stars like Rolls Royce and NatWest, which saw their share prices double over the [last] year, are among the climbers today. The FTSE 100 has been a laggard compared to US indices. They surged higher in 2024, with the S&amp;amp;P 500 gaining more than 23%, helped by big gains among the mighty tech stocks, fuelled by AI optimism. But appetite for UK market is being revived, as investors are attracted by its defensive characteristics in an era of global uncertainty. Sectors like healthcare, utilities, consumer staples and telecoms companies can offer stable returns. The impressive dividend-paying potential is a key attraction to the UK stock market. There are plenty of mature companies boasting strong dividend cover and the potential for income to grow over the long term. The government has announced a £60m funding package for the creative industries, including investment in British film and TV, grass roots music and start-up video game companies. The government said that the investment, £40m of which will be spent over the next financial year, will benefit hundreds of creative businesses “marking the first step of the government’s sector plan for the creative industries. Chancellor Rachel Reeves says: “Our number one mission is to grow the economy and our creative industries are a British success story with a big part to play.” The announcement was made as Lisa Nandy, the culture secretary, held a creative industries summit in Gatehead attended by more than 250 businesses and cultural leaders including Netflix, Spotify, Warner Bros, the National Theatre and British Museum. Nandy says: “From film and fashion to music and advertising, our creative industries are truly world-class and play a critical role in helping us deliver on this Government’s mission to drive economic growth in all parts of the UK. The British Business Bank, which supports £17.4bn of finance to over 64,000 smaller businesses, has committed to increase its support for creative businesses to access the finance they need to grow. The government also formally announced the creation of a Soft Power Council, which will advise the government on driving growth and investment at home and abroad, comprised of leading executives including former ITV chairman Sir Peter Bazalgette, Roland Rudd, the co-chair of PR giant FGS Global and Victoria and Albert Museum director Tristram Hunt. Sir David Lammy, the foreign secretary, said that its aim is to “re-imagine Britain’s role on the world stage”, adding: “Soft power is fundamental to the UK’s impact and reputation around the world. I am often struck by the enormous love and respect which our music, sport and educational institutions generate on every continent. But we have not taken a sufficiently strategic approach to these huge assets as a country.” The FTSE 100 has hit a new record high despite the much-discussed impact of higher taxes on UK businesses contained in last year’s budget, and the recent turmoil in the bond market. Dan Coatsworth, investment analyst at AJ Bell, says: “It’s refreshing to see positive news around the UK stock market given its unloved reputation. “Helping to drive the index up more than 1% and above its previous intraday record of 8,474 in May 2024 was a further slump in the pound as retail sales came in below expectations for December. “Three quarters of companies in the FTSE 100 generate their earnings overseas, and the relative value of those foreign earnings is boosted when the pound weakens. The natural resources sector was also lifted by merger and takeover chatter, encouraging investors to bid up shares in the likes of Glencore and Anglo American. “Weak UK retail sales in December are a worry as they indicate further pressure on the economy following weak GDP data yesterday. Traders are pricing in an 81.5% probability that the Bank of England will cut interest rates by a quarter percentage point next month. Retailers will be keeping their fingers crossed this happens as it could help to take some of the pressure off household finances and encourage more spending.” The FTSE 100 has hit a record high after a strong start to the year. Since the beginning of January, the index has climbed by 3.75%, adding to the 5.7% it gained during the whole of 2024. Other equity markets have also started the new year well; Germany’s DAX has gained 4.6%, despite its economic malaise, while France’s CAC has shrugged off the endless political turmoil in Paris by gaining 4.5%. Boom! Britain’s blue-chip share index has hit a new alltime high. The FTSE 100 index, which tracks the hundred largest companies listed in London, has jumped by over 1% to 8480.36 points in early trading, above its previous intraday high of 8474 points set last May. Stocks are on a three-day rally, which started on Wednesday when UK inflation dropped unexpectedly, potentially paving the way for several interest rate cuts this year. Today’s disappointing retail sales figures, folowing Thursday’s weaker-than-expected growth data for December, have added to hopes that the Bank of England will ease monetary policy this year. This morning, the financial markets are pricing in between two and three interest rate cuts this year – last week, duing the bond market mayhem, fewer than two were expected. That has pushed down the pound, which raises the value of multinational companies listed in London (it makes their earnings in other currencies more valuable). Global stocks have also benefited from reports that Donald Trump could take a more cautious approach to implementing tariffs than feared. Mining companies are rallying in London this morning, following reports that Rio Tinto and Glencore have discussed combining their businesses (see earlier post) In the City, shares in mining giants Glencore and Rio Tinto have jumped following reports they have held talks about combining part or all of their businesses. The Financial Times and Bloomberg both reported that the two mining giants held “early stage” talks about a possible combination last year. Bloomberg explains: A potential combination of the two companies would rank as the largest-ever mining deal, but any transaction would be complex and face multiple potential hurdles. While Glencore has large copper assets at a time when the world’s biggest producers are all seeking to expand in the metal crucial to the energy transition, it also owns a massive coal business that would likely be unattractive to Rio. The larger miner’s chief executive has repeatedly expressed wariness about mega deals, and the two companies have vastly different cultures. The discussions follow BHP’s failed £39bn bid for Anglo American last year, which led companies across the sector to review strategic options. Glencore’s share price has risen by 3% in early trading, while Rio Tinto are up 1.5%. Several economists report that the 0.3% drop in retail sales volumes across Britain last month was disappointing. Alex Kerr, UK economist at Capital Economics, says the economy clearly struggled at the end of last year, but expects the retail sector will have a better 2025: After big declines of 4.1% in 2022 and 2.9% in 2023, sales rose only by 0.7% in 2024. And as with the wider economy, most of that growth in sales was from earlier last year and the year finished with very little momentum. Indeed, the level of sales volumes in December was just 0.1% higher than in June and the 3m/3m growth rate has slowed from a healthy +1.2% in September to -0.8% in December. That said, the breakdown was a bit more encouraging with sales rising in four of the seven sub-sectors. Admittedly, food and online sales both fell by 1.9% m/m. But the rises in sales in department, clothing and household goods stores suggests that, after big falls in October and November, households were holding back some of their spending for the Christmas period and may be in a better position than the recent retail weakness suggests. Jacqui Baker, head of retail at RSM UK, says December’s drop in sales marks a disappointing end to tough year: “Despite record-breaking sales for some retailers over Christmas, plus the later than usual Black Friday event, it was a disappointing end to 2024 for the sector. A lacklustre Golden Quarter is particularly concerning after a tough year as retailers would have been hoping for a Christmas boost. However, retail sales excluding fuel did increase 2.9% year-on-year due to poor sales figures in December 2023. “Many retailers had little choice but to launch their Boxing Day discounting early to maximise sales and clear as much stock as possible ahead of the seasonal slowdown in January. However, without the ‘golden’ boost to sales many retailers will find it difficult to navigate the imminent headwinds post-Budget and we could see prominent brands struggle to compete in 2025. But there are questions about the data. Matt Swannell, chief economic advisor to the EY ITEM Club, points out that these figures are volatile. “Seasonal spending has a large impact on the retail sector at the end of the year, and recent shifts in spending patterns can introduce large volatility into official estimates of retail activity, so the EY ITEM Club wouldn’t recommend reading too much into December’s fall. Indeed, December 2023 saw retail activity fall by nearly 4%, also with a collapse in food sales, only for most of this lost ground to be made up in January 2024. However, when considering the last three months, the picture remains soft, with retail sales falling 0.8% across Q4. Retailing analyst Nick Bubb has his own doubts, saying… Well, City economists will lap up the news that the ONS Retail Sales figures for December were down, but they should be asking if the figures are simply wrong, as the ONS must be living on a different planet if it thinks that Large Food Retailers saw sales fall by 0.2% last month (year-on-year, non-seasonally adjusted value), given what we’ve heard from Kantar and Nielsen. The retail sales picture is rosier if you take an annual view. Compared with December 2023, sales volumes were 2.9% higher last year, while sales values (the amount spent) rose by 3.5%. Kris Hamer, director of insight at the British Retail Consortium, said: Retail sales picked up in December, but this unfortunately did not offset the shaky start to the ‘Golden Quarter’. In non-food, electricals, beauty and books made for popular presents. Meanwhile, sales of furniture and other large ticket items were hard hit as families continued to think twice before making larger purchases, and clothing and footwear sales remained muted. The pound has weakened following this morning’s weaker-than-expected retail sales figures. Sterling has fallen by over half a cent to $1.218, towards the 14-month lows hit against the US dollar last week. Traders are calculating that the Bank of England could be spurred to cut interest rates by the weak spending in the shops last month. Neil Birrell, chief investment officer at Premier Miton Investors, says: Consumers in the UK obviously had a quiet Christmas. December’s retail sales are reflective of the general tone in the country, coming in much worse than expected. Whilst that might be good news on the inflation front, it does nothing for the economy’s growth prospects. The numbers will no doubt encourage the Bank of England to cut interest rates when they meet, but they must worry the government at the same time. The economy is in need of stimulus. Despite December’s drop, retail sales did rise across Britain during 2024 – the first annual increase in three years. The ONS reports that retail sales volumes rose by 0.7% in 2024, following a fall of 2.9% in 2023 and of 4.1% in 2022. “Although this marked the first rise in three years, sales volumes have not returned to 2022 levels,” it adds. Today’s retail sales report shows that the drop in food sales (-1.9% on the month) was strongest at supermarkets. However, sales volumes also fell in specialist food stores, such as butchers and bakers, and alcohol and tobacco stores (including vaping shops), the ONS reports. Retail sales across Great Britain shrank last month, as consumers took a cautious approach to Christmas shopping. Retail sales volumes dipped by 0.3% month-on-month in December, the Office for National Statistics has reported, missing forecasts of a 0.4% rise. The ONS reports that sales volumes at supermarkets fell, with food stores sales volumes down 1.9%, which was partly offset by a rise in sales at non-food stores such as clothing shops. That drop in food sales is surprising, as several retailers have reported strong festive sales. Tesco said it had its biggest ever Christmas, for example. December’s drop in retail sales followed a small, 0.1%, rise in November. And over the last three months, the sales volumes (the amount of stuff bought in the shops or online) fell by 0.8% compared the three months to September. This suggests consumer spending weakened towards the end of last year – several surveys have suggested that confidence declined, However, there is a wrinkle – the ONS seasonally adjusts its data, to adjust for the impact of Christmas spending, and because Black Friday (29th November this year) fell in its December reporting period this year, which muddied the data. On a non-seasonally adjusted basis, sales volumes rose by 10.0% in December! ONS senior statistician Hannah Finselbach says: “Retail sales fell in December following last month’s slight increase. “This was driven by a very poor month for food sales, which sank to their lowest level since 2013, with supermarkets particularly affected. “It was a better month for clothing shops and household goods stores, where retailers reported strong Christmas trading. “With the timing of Black Friday falling within these latest data, our figures when not adjusted for seasonal spending show overall retail sales grew more strongly than in recent Decembers.” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Along with death and taxes, you can usually rely on China to hit its economic growth targets. And it’s done it again, with the National Bureau of Statistics of China reporting overnight that China’s economy grew by 5% in 2024. That means it hit Beijing’s official target of “around 5%.” The target was reached thanks to a burst of activity in the fourth quarter of last year. GDP rose at an annual rate of 5.4% in October-December, beating the market’s expectation, helped by a flurry of stimulus measures powered the economy to meet Beijing’s growth target. China’s economy shrugged off “a relentless barrage of economic pessimism,” says Stephen Innes, managing partner at SPI Asset Management, to hit Beijing’s growth target, adding: “This surge was fueled by a vigorous export boom and aggressive stimulus measures that counterbalanced the sluggish domestic demand. Although slightly outpacing analyst forecasts, this growth fell just shy of the 5.2% expansion seen in 2023, painting a picture of an economy with both promising highs and undeniable challenges” The NSB also reported that China’s retail sales rose 3.7% year-on-year in December, while industrial output expanded by 6.2% – both faster than expected. The agenda 7am GMT: UK retail sales report for December 2pm GMT: IMF to release its latest World Economic Outlook</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Almost every share on the FTSE 100 rose on Friday, as a fall in the value of the pound boosted multinational companies listed in London. UK government bond prices have also eased back from their recent highs, helped by expectations of interest rate cuts this year. IMF has upgraded its forecast for UK growth this year in an update to its biannual assessment of the global economy.</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Profits at the hedge fund co-founded by the GB News and Spectator owner Sir Paul Marshall plunged by almost two-thirds last year, resulting in significantly reduced payouts for its partners. Marshall Wace, one of London’s most successful hedge funds, has declared profits of £192m in the year to the end of February 2024, a sharp fall of 64% compared with the £538m the previous year. Marshall Wace was founded in 1997 by Marshall and Ian Wace and manages more than $71bn (£57.2bn) in funds, making it one of the largest of its kind in the world. Last year, Marshall sealed a £100m takeover of the Spectator magazine, adding to a media empire that includes backing the often controversial GB News TV channel and the UnHerd website. Total turnover at Marshall Wace dropped from £1.2bn in 2023 to £768m last year, according to accounts filed this week at Companies House. The latest accounts show that management fees and other income fell from £637m to £605m. The company’s profits will be shared between its 24 partners, including Marshall and Wace. The biggest hit to those earnings came from an almost 75% drop in performance fees for the year, from £598m in 2023 to £163m last year. As well as the partners, Marshall Wace Asset Management is listed as a member. An equal share of the earnings would equate to £8m for each member – down from £22m each a year earlier – if the services company is included. In reality, the earnings of senior members among the group are likely to be significantly higher. Marshall Wace’s Eureka fund made a return of 14% last year, according to Reuters. The US hedge fund Citadel, run by the billionaire Ken Griffin, who last year considered joining a group of investors led by Marshall exploring a bid to buy the Telegraph, gained 15.1% as the US stock market performed strongly. The rival Millennium Management, run by Izzy Englander, made a return of 15%. Citadel and Millennium, which have $66bn and $72.1bn in assets under management respectively, outperformed the wider hedge fund industry. In 2016, Marshall, a former lead non-executive board member at the Department for Education, received a knighthood for services to education and philanthropy. Marshall was a prominent donor to the campaign to leave the EU, while Wace donated to the campaign to remain.</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Marshall Wace declared profits of £192m in the year to the end of February 2024. Last year, Marshall sealed a £100m takeover of the Spectator magazine. Total turnover dropped from £1.2bn in 2023 to £768m last year. Management fees and other income fell from £637m to £605m.</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Global stock markets climbed in 2024, helped by falling inflation and the US economy’s success in avoiding a hangover from a strong post-pandemic recovery. While Europe and the UK struggled to make headway, the US maintained pole position at the top of the rich nations’ growth league, pushing shares in New York to new record highs. However,the year ended with jitters in the bond market, as investors feared that central bankers had failed to slay inflationary pressures, forcing many to rip up forecasts about likely cuts in interest rates. Daniele Antonucci, chief investment officer at Quintet Private Bank, says “2024 was a masterclass in unpredictability.” “Despite earlier concerns, the US avoided a recession, the eurozone and UK experienced only mild downturns, and China picked up steam towards the end of the year. While there were occasional spikes in market volatility, the overall story of 2024 was one of growth – powered in no small part by structural themes, including the rapid rise of new technologies,” Antonucci adds. Shares Equities, especially technology stocks listed in the US, had another good year in 2024. Markets shrugged off a brief plunge in early August, but did end the year with a slight wobble, as global stocks fell by 2.7% during December. The tech-focused Nasdaq had its second strong year in a row, surging by over 28% during 2024. Chipmaker Nvidia led the charge, up over 170% over the last 12 months, as frenzied demand for its semiconductors to run artificial intelligence systems swelled its revenues and profits. Other tech companies also boomed: Alphabet gained 35%, Meta rose 65% while Tesla had a very strong year too, gaining 62%. The broader S&amp;amp;P 500 hit a series of record highs, prompting Wall Street forecasters to revise up their targets for the index during the year. In the private markets, Elon Musk’s SpaceX doubled in value to $350bn, based on the price of anemployee share buyback programme. “It has been Elon Musk’s year,” said Bill Blain, market strategist at Windshift Capital, adding that Musk, an adviser to president-elect Donald Trump, may have a difficult year ahead. “They say pride cometh before a fall. Whom the gods intend to destroy they first build up,” he added. The UK market lagged behind the US, though, with London’s FTSE 100 rising by 5.7% in 2024. It was a year of two halves for the Footsie. Strong gains early in 2024 drove the index to a record high of 8474 points in May, before it weakened in September, October and December, to finish at 8173 points, up 440 points in the year. It was a better year for investors in Frankfurt, while those in Paris had a tougher time. Germany’s DAX gained 19% in 2024, despite a political crisis, economic stagnation and a slump at its carmarkers. France’s CAC dipped by 2.1%, in a year which brought the country four prime ministers. Lori Heinel, global chief investment officer at State Street Global Advisors, says “2024 was no ordinary year, with elections around the world, persistent inflation and market volatility all playing their part in building an uncertain macroeconomic environment. Despite these challenges, markets continued to be resilient.” The pound Sterling ended 2024 roughly where it began against the dollar, at about $1.25. A strong third-quarter drove the pound to a two-year high of more than $1.34 in September, when the Bank of England left interest rates on hold. But since then, sterling has been on the slide against a strengthening dollar. The pound had a better year against the euro, rising from €1.15 to €1.20, on expectations that the European Central Bank will cut interest rates faster than the Bank of England this year. Bonds The interest rate on government bonds from many advanced economies actually rose in 2024, defying expectations. These rates, known as yields, remained high because central banks cut borrowing costs at a rather lower pace than forecast, a trend that may continue if inflation picks up. UK 10-year bond yields climbed from 3.6% at the start of January 2024 to almost 4.6% by the end of December. That puts them back at levels seen after Liz Truss’s calamitous mini-budget (although it was the speed at which bond yields surged that really alarmed the markets in September 2022). Rising UK bond yields will worry Rachel Reeves, as it eats into the headroom available to the chancellor to hit her fiscal rules at current tax and spending levels. US 10-year Treasury yields have also climbed in 2024, notably in the last three months of the year. Worryingly, US borrowing costs have risen since the Federal Reserve began cutting interest rates last autumn. The Fed has lowered its key rate by 100 basis points, or 1%, since it started cutting in September. Over the same time, US 10-year Treasury yields have risen by about 100bps – a sign that investors don’t believe inflation is beaten. Oil Brent crude ended the year lower than where it started it, pulled down by forecasts that the oil market could be over-supplied in 2025. Having touched $79/barrel at the start of January, Brent crude was changing hands for $74/barrel on the last day of the year. At one stage oil threatened to hit $100/barrel, amid fears that the Middle East crisis would hurt production and output. Although oil prices were supported by geopolitical tensions, they were also pulled down by concerns that demand was weakening. During the year, Opec cut its outlook for demand in 2024 five times, due to weakness in China, India and other regions. Matt Britzman, senior equity researcher at Hargreaves Lansdown, says the oil market was grappling with a “slippery slope of oversupply concerns” heading into 2025. “Opec’s efforts to boost production face headwinds, with weaker demand from China, the world’s largest importer, weighing on prices. Adding fuel to the fire, president-elect Trump’s proposed tariffs and sanctions could shake the energy market, leaving oil poised for an annual decline after months of turbulent trading,” Britzman adds. Bitcoin Bitcoin gained 120% over the last 12 months, in another lively year for crypto assets. Having begun the year about $43,000, bitcoin climbed to $71,000 by mid-March before spending much of the year in the $60,000 region. But Donald Trump’s election win in November sent bitcoin surging over $100,000 for the first time on expectations of a pro-crypto White House. But while the world’s largest cryptocurrency traded as high as $108,000 in mid-December, it dropped by about $15,000 from that peak by the end of the year to near $93,700. Bitcoin benefited from growing acceptance from traditional investors; in October, BlackRock CEO Larry Fink described it as “an alternative to other commodities like gold,” though its volatility and a lack of regulation keep it off limits for many investors.</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Global stock markets climbed in 2024, helped by falling inflation and the US economy’s success in avoiding a hangover from a strong post-pandemic recovery. While Europe and the UK struggled to make headway, the US maintained pole position at the top of the rich nations’ growth league. However,the year ended with jitters in the bond market, as investors feared that central bankers had failed to slay inflationary pressures.</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>A late PS: The three major U.S. stock indices closed in negative territory tonight. The S&amp;amp;P 500 lost 25 points, or 0.4%, to end at 5,881 points, while the Nasdaq Composite fell by 0.90%. For 2024, the Nasdaq surged nearly 30%, while the bellwether S&amp;amp;P 500 notched more than a 23% gain, marking the index’s best two-year run since 1997-1998. The Dow Jones Industrial Average dipped slightly, to finish at 42,544.22 points, meaning it gained almost 13% during the year. Time to wrap up, for the last time this year. The UK’s blue-chip stock index has recorded its strongest annual gain since 2021, despite lagging behind Wall Street over the past year. The FTSE 100 index, which tracks the largest companies listed in London, posted a rise of 5.7% for 2024. Having begun the year at 7,733 points, the FTSE closed 440 points higher at 8,173 points today. That was its fourth year of gains in a row, after rising 14.3% in 2021, 0.9% in 2022 and 3.8% in 2023, which came in the wake of a 14.3% plunge in 2020, when the Covid-19 pandemic rocked markets. But London stocks have lagged behind New York, where the S&amp;amp;P 500 index gained over 23% this year. Russian gas supplies to Europe via Ukraine are set to end on New Year’s Day, ending Moscow’s long dominance of supply in the European gas market. Russia’s oldest gas export route to Europe - a pipeline dating back to Soviet days - was set to shut at the end of 2024, as a five-year transit deal between Russia and Ukraine expires. Data from Ukraine’s gas transit operator showed on Tuesday that Russia had not requested any gas flows for January 1st. China’s economy is on course to expand by 5% in 2025, according to its president, Xi Jinping, meeting official growth targets and rebutting concerns that Donald Trump’s incoming US administration will harm Beijing’s prospects in the new year. A US government fund to compensate people swindled by Bernie Madoff is making its final round of payments, taking the total paid from the fund to the late fraudster’s victims to $4.3bn (£3.4bn). The boss of Britain’s biggest building society has warned that working from home could harm women’s careers because they are less likely to come into the office than their male colleagues. Passengers on the London to Glasgow main line face disruption to services in the coming days because of strikes by train managers at Avanti West Coast. For those planning their finances next year… There could be a flurry of takeover action in London next year too. UK investment bank Peel Hunt has predicted that 2025 will bring a major and sustained flow of UK takeovers. Peel Hunt’s head of M&amp;amp;A advisory, Michael Nicholson, says: “Bid defence manuals are no longer an item to be left on the shelf, ready to grab if needed. They ought to be front of mind for all UK boards.” Nicholson estimates that a third of stocks on the alternative AIM market are at risk of a takeover approach as private equity “barbarians at the gate” prepare to strike in 2025. With the London market now closed until 2nd January 2025, investors’ minds are turning to what might happen in the new year. The brokerage firm AJ Bell has predicted shares will rally in London next year. It has a target price of 9,000 points for the FTSE 100 by the end of 2025, arguing that “prevailing gloom” means UK equities look cheap on an earnings and yield basis. AJ Bell investment director Russ Mould, explained: “Total returns from the UK stock market in 2024 handily beat cash, bonds and inflation, but the poor comparisons with the USA remain the stick with which the FTSE 100 is constantly beaten. Whether the NASDAQ and S&amp;amp;P 500 will finally run out of puff in 2025 remains a matter of debate, but value- and income-seeking contrarians could be forgiven for giving the UK a closer look, given consensus forecasts for earnings and dividend growth. The opening bell has rung on Wall Street for the final time in another blockbuster year for stocks. The main indices in New York have risen in early trading, with the Dow Jones industrial average up 79 points or 0.2% at 42,653 points. The broader S&amp;amp;P 500 index is up 0.1%, while the tech-focused Nasdaq Composite nudged up by just 0.018%. For the year, the Dow has gained 13% and the S&amp;amp;P 500 24%, while the Nasdaq is up around 30% thanks to hot tech stocks such as Nvidia (up 177% this year). The top FTSE 100 risers this year were airline group IAG and engineering firm Rolls-Royce, which both gained over 90% during 2024. They were followed by NatWest bank, whose shares rose by 82%, and packaging firm DS Smith which gained 77%. Britain’s FTSE 100 share index has closed for the year, posting a 5.7% gain for 2024. The index of blue-ship shares listed in London has gained 440 points this year. As the market closed early for New Year, the FTSE 100 ended the day up 52 points or 0.65% today at 8173 points, having begun 2024 at 7733 points. This is the fourth year in a row that the FTSE 100 has risen, after it plunged in 2020 in the first year of the Covid-19 pandemic. But it’s a smaller gain than Germany’s DAX and Japan’s Nikkei, which both gained around 19% this year, while in New York the S&amp;amp;P 500 has risen by over 23%. Earlier this year the FTSE 100 hit a record high of 8474 points, in May, before slipping in the second half of the year. Matt Britzman, senior equity analyst at Hargreaves Lansdown, says. “The FTSE 100 wrapped up 2024 on a high note, shaking off a slow start to the session to finish the year in positive territory. After an impressive climb early on, the index hit an all-time high in May but couldn’t quite muster the momentum to break out of a rangebound pattern in the months that followed. Meanwhile, it played second fiddle to the tech-fuelled US markets, where AI excitement sent the S&amp;amp;P 500 soaring. Back home, UK investors navigated a year of twists and turns, with two interest rate cuts offering relief while a tax-hiking budget put pressure on some domestic companies. It was a year of resilience rather than runaway success for the UK’s blue-chip benchmark. Santa has made a late appearance at the London stock exchange! With less than an hour’s trading to go this year, the FTSE 100 index is now rallying – it’s up 55 points or 0.7% at 8176. Fashion retailer JD Sports are the top riser today, up 2.8%. That means the FTSE 100 has gained around 5.7% so far this year….. 2024 was a busy year for takeovers of UK companies. Data from the London Stock Exchange Group shows that the amount of domestic merger and acquisitions (in which one UK company buys another) doubled year-on-year, while deals from overseas rose 21%. This lifted the total M&amp;amp;A involving a UK target to $182.9bn (£148.8bn) so far this year. Fifty-one percent of UK target M&amp;amp;A involved an overseas acquiror, with the remaining 49% involving domestic buyers, LSEG reports. During 2024 the UK was the third most targeted country for M&amp;amp;A globally this year, after the United States and China; deals involving UK targets accounting for 6% of the global M&amp;amp;A total, up from 4% last year. LSEG adds: Financials is the most targeted sector in the UK so far this year, accounting for 17% of overall UK target M&amp;amp;A activity, with multi-billion dollar bids for asset management firm Hargreaves Lansdown and Nationwide Building Society’s plan to buy Virgin Money. The Ministry of Defence’s acquisition of military housing, LondonMetric Property’s merger with LXi REIT, and the Barratt/Redrow merger boosted the Real Estate sector to second place. Wall Street is set for a calm final session of 2024, judging by the latest futures prices which show the Dow flat: European gas prices are also higher today, with the month-ahead contract up 0.8% at €48.25/MWh. Reuters reports that Russia’s Gazprom said it will pump a reduced volume of gas to Europe via Ukraine today, the last day before the expiry of a deal that had kept the gas flowing throughout nearly three years of war, adding: Gazprom said it would send only 37.2 million cubic metres on Tuesday compared to 42.4 mcm on Monday. Flows are expected to fall to zero from the early hours of Jan. 1 after the expiry of the five-year transit agreement. Its demise marks the almost complete loss of Moscow’s once mighty hold over the European gas market. Ukraine refused to negotiate a new deal because of the war. The halting of supplies via Ukraine will be a major blow to Moldova, a country that was once part of the Soviet Union. Among European Union countries, Slovakia will be the most affected. Hungary will continue to receive Russian gas from the south, via the TurkStream pipeline on the bed of the Black Sea, although it had been keen to keep the Ukrainian route as well. Looking at the wholesale gas market, prices are notably higher than a year ago. On January 2 2024, the day-ahead price of UK gas was around 74p per therm. Today it’s 120p per therm, having gained 2.5% so far this morning. British energy bills will rise tomorrow, when the next price cap kicks in, and consumers could face further increases in April. Regulator Ofgem announced last month that the average annual energy bill in England, Scotland and Wales will increase to £1,738 from January, due to a 1.2% increase in its quarterly price cap. Consultancy group Cornwall Insight has predicted today that the cap will rise again in April to £1,785 a year for a typical dual fuel consumer, nearly a 3% increase on January’s level. Cornwall had previously expected a smaller rise next April, of around 1%. Today Cornwall says: Early December saw a slight dip in wholesale energy prices, driven by easing supply tensions in Europe. However, geopolitical instability saw prices rebound in the second half of December, with the market surging last week due to new uncertainty over the Ukraine transit deal and the higher level of withdrawals from EU gas storage facilities. This all affected our view of consumer bills in 2025. These factors, combined with the significant uncertainty over the US LNG export plans under a second Trump presidency, mean we are expecting that our cap forecasts will continue to display a high degree of variability. Trading has started cautiously in Europe this morning. The FTSE 100 index did open in the red, but has now nudged up by 2 points, or 0.03%. France’s CAC dipped by 0.02%, while the Netherlands’ AEX crept up by 0.06%. Germany’s DAX closed for the year yesterday, cementing a 18% gain for 2024, while Italy’s FTSE Mib recorded a 12% rise for the year. China’s stock market has ended the year on a weak note. The CSI 300 index fell by 1.6% today, despite president Xi predicting China’s growth target would be hit, while stocks in Shenzhen fell by 2.5%. For the year, though, the CSI 300 index – which measures the 300 largest stocks listed in Shanghai and Shenzhen – has risen by over 14%. Those gains were driven by China’s latest stimulus programme, which stocks surging in late September and early October: China’s president Xi Jinping has predicted that the country’s economy will grow by around 5% this year. Xi’s comments, in a speech published by the official Xinhua News Agency, are a signal that the world’s second-largest economy is on track to meet its official target. Xi also reiterated a call to adopt more proactive macroeconomic policies. Speaking to a gathering of China’s top political advisory body to usher in the new year, he said: “On the journey of Chinese modernization, we will not only encounter clear skies and gentle breezes, but also face high winds, choppy waters, and even dangerous storms. We must maintain strategic resolve and pool the great strength of all Chinese people striving in unity to cut through the waves and forge ahead with courage.” More here: Xi calls for forging ahead to build strong China 2025 could bring more gains on the UK stock market, brokerage AJ Bell has predicted. It has predicted the FTSE 100 could hit 9,000 points by the end of 2025, which would be require a roughly 10% jump next year. Their investment director Russ Mould argues that the “prevailing gloom” means UK equities look cheap on an earnings and yield basis, adding: “Political uncertainty should now be receding in the UK, given the Labour government’s thumping majority, and this offers a favourable comparison with Europe, where coalition administrations now seem to be falling over at a pace to match that of the Conservative Party’s enthusiastic sacking of its leaders, prime ministers and chancellors in recent years. The jury may still be out on the new chancellor’s first Budget, but some credit should be given for at least acknowledging the fiscal deficit which faces the country, a topic barely mentioned during the US election campaign and one that is now coming home to roost in France. 2024 has also been a strong year for the US dollar, whcih is on track to record strong gains against most currencies. The dollar index, which measures the greenback against a basket of rival currencies, is up 6.5% over the last year. It has been lifted by expectations that the US Federal Reserve will be slower to cut interest rates than rival central banks in 2025, if the incoming Trump administration’s policies – such as new tariffs on imports – are inflationary. Trump’s election victory is expected to lead to US fiscal expansion characterised by increased spending and tax cuts. Tony Sycamore, market analyst at IG, explains: This, in turn, is likely to result in stronger US growth, higher inflation, and, subsequently, higher interest rates, all of which contribute to a stronger US dollar. Furthermore, Trump’s election victory is anticipated to result in tariffs on imports from countries, including China. Mexico, Canada and the EU which will dampen growth expectations outside the US and weigh on commodity prices. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. It’s the final trading day of the year, when investors will be adding up their profits (or losses) and turning their attention to 2025. 2024 has been another year of gains in the stock markets, with record highs seen on both sides of the Atlantic. Wall Street has led the charge, helped by the boom in tech stocks which continued over the last 12 months. Investors in the UK stock market have enjoyed gains too – the blue-chip FTSE 100 index is on track to record a 5% rise this year, broadly in line with the European average. That would be its best year since 2021, when it rose 14.3%, and follows a 0.9% rise in 2022 and a 3.8% gain in 2023. The ‘Footsie’ is ending the year on the back foot, though, down 2% in December. Yesterday it closed at 8121 points, a fair way shy of the record high of 8,474 set in May when falling inflation and hopes of interest rate cuts were lifting stocks. The smaller FTSE 250 index, seen as a better barometer of the UK economy, has gained around 3.6%. That doesn’t include the income from dividends, though, which shareholders received over the year. As AJ Bell investment director Russ Mould puts it: “Total returns from the UK stock market in 2024 handily beat cash, bonds and inflation, but the poor comparisons with the USA remain the stick with which the FTSE 100 is constantly beaten. Whether the NASDAQ and S&amp;amp;P 500 will finally run out of puff in 2025 remains a matter of debate, but value- and income-seeking contrarians could be forgiven for giving the UK a closer look, given consensus forecasts for earnings and dividend growth. Across the channel, France’s CAC 40 has lost around 3% during a year punctuated by political drama in Paris. But Germany’s DAX, which closed for the year yesterday, has gained almost 19% – driven by software company SAP which rose 60% in the year. Tech stocks also drove Wall Street higher, lifting the Nasdaq by almost 30% so far this year, and the S&amp;amp;P 500 index by over 23%. Tom Stevenson, investment director for personal investing at Fidelity International, explains: “After the turbulence of 2023, we’ve seen a marked shift towards growth, driven by stabilising inflation and a more positive outlook for interest rates.” But in December alone, equity markets have been on the back foot – seemingly worried by ructions in the bond market where yields (interest rates) have been rising amid fears of sticky inflation in 2025. This year has not brought much of a Santa Rally, and we may not get one today either – with the futures market indicating shares may dip in London. London’s market will close early at lunchtime, giving traders time to spruce up for New Year festivities. The agenda 12.30pm GMT: London stock market closes early for New Year 2pm GMT: CaseShiller index of house prices for October</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Three major U.S. stock indices closed in negative territory tonight. The S&amp;amp;P 500 lost 25 points, or 0.4%, to end at 5,881 points. The Nasdaq Composite fell by 0.90%. For 2024, the Nasdaq surged nearly 30%, while the bellwether S&amp;P 500 notched more than a 23% gain.</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Time to wrap up. Stock markets in Japan and Germany have closed for the year, posting 19% gains on another strong 12 months for equities. But major bourses are weaker today, as investors worry that inflation may be sticky in 2025, hampering central banks from cutting interest rates. Britain’s FTSE 100 index is down 51 points or 0.6% in late trading, while the US Dow Jones industrial average has lost 690 points or 1.6% – with Boeing leading the fallers, following the aeroplane crash in South Korea yesterday. 2024 has been tough for the pub industry, with more than 400 sites closing across England and Wales in the last year. Here’s the rest of today’s news so far: Chicago’s manufacturing sector contracted more sharply than expected this month, new data shows. The Chicago Purchasing Managers’ Index has dropped to 36.9, indicating a contraction in the region’s factory sector. Aircraft maker Boeing are the biggest faller on the Dow Jones industrial average in early trading, down 3.5%. This follows the crash of a Jeju Air Boeing B737-800 at Muan international airport in South Korea on Sunday, in which all 175 passengers and four of the six crew members were killed after an emergency landing. A team of US team air accident investigators will assist Korean air investigators, as air safety experts questioned why the plane had not been able to lower its undercarriage after one engine was hit by what appeared to be a bird strike. South Korea plans to inspect all B737-800 Boeing aircraft operated by domestic airlines following the disaster. Wall Street has opened in the red too, with the main indices dropping over 1%. Although it’s been a strong year for stock markets, many of them are in the red today as 2024 rather fizzles out. The UK’s FTSE 100 index is still down today, off 32 points (-0.4%) at 8117 points; France’s CAC 40 index is off by a similar amount, but Italy’s FTSE Mib is flat. David Morrison, senior market analyst at Trade Nation, says European indices were mixed this morning in “quiet, low volume trade”, explaining: Asian Pacific stock indices were generally softer overnight, taking their lead from Friday’s Wall Street sell-off. Trading volumes were light, and no doubt this contributed to overall weakness. While it has been an impressive year for many global stock markets, with the US tech giants leading the charge higher, there have been areas of disappointment. This is especially apparent in countries which have faced political difficulties, with South Korea and France both obvious casualties. Although interestingly, the German DAX has easily outperformed its European rivals, despite having its own political uncertainties and an imminent General Election which has the potential to upend years of centrist control. Over the last two years, Germany’s DAX share index has rallied by over 40% – despite the country’s economic problems. Bloomberg has the details: On Monday, the DAX Index closed the year 19% higher to extend a rally since January 2023 to 43%. While the export-heavy gauge has lagged the S&amp;amp;P 500 in the US for 2024, it far outpaced regional peers including the UK’s FTSE 100 and France’s CAC 40. Today is also the final trading session in Frankfurt, where stocks have had a strong year despite plenty of upheaval. The DAX share index has climbed almost 19% during 2024, making it the best-performing of the major European indices. SAP SE was the biggest contributor to 2024’s gains, Bloomberg points out, as investors sought technology plays, accounting for nearly a third of the index’s rally. The last trading session of the year in Tokyo ended on a somber note, Marketwatch reports, with the Japan Exchange Group’s CEO Hiromi Yamaji apologizing during the traditional yearend ceremony over a recent insider trading case. Yamaji said: “I acknowledge trust towards the market is essential for investors to trade with confidence” The exchange is working to improve training and verify findings of an independent investigation, he said, adding that “we are doing are our utmost best to rebuild trust and prevent this from happening again.” Japan’s blue-chip stock index has ended the year at its highest year-end finish on record, despite a small selloff today. The Nikkei stock average ended down 386.62 points, or almost 1%, today at 39,894 points. For the year, it gained 19%, as a weaker yen supported exporters. Kazuo Kamitani, a strategist in the Investment Content Department of Nomura Securities Co, says: “There was much optimism in the first half of the year with hope for a favorable cycle in which wages increase in tandem with prices, alongside the weak yen for corporate profits.” 2024 was an eventful year for Japanese investors – on one day in August, the Nikkei 225 plunged 12% in its biggest decline since the Black Monday crash of 1987. That was followed by a 10% surge the next day. Theleme Partners, the hedge fund where the former prime minister Rishi Sunak was a founding partner, has suffered a sharp drop in performance fees, resulting in annual profits halving. Profit fell to £32m in the year to 31 March from £64.7m the year before, according to accounts filed with Companies House. Performance fees declined to £14.9m from £45.9m, while management fees fell to £322.9m from £24.7m. Last year Sunak came after fire for his links with the hedge fund, which earned big returns from its investment in the US vaccine maker Moderna. Moderna’s fortunes were transformed by its Covid-19 jab, and it went from a lossmaking to a profitable company. Sunak co-founded Theleme in 2009 but quit to join politics in 2013. The hedge fund’s profits more than doubled to £109m in the year to 31 March 2022, thanks to its investment in Moderna, which signed a 10-year partnership with the UK government in June of that year. Under the £1bn deal, it committed to build a major research and manufacturing centre for mRNA vaccines against new Covid variants and other respiratory illnesses, in an effort to improve readiness for future pandemics. The centre is being built in Harwell. House prices in prime central London have dropped this year, estate agent Savills reports, as wealthy buyers were scared off by October’s budget. Savills reports that average prices across prime central London dropped by 0.8% in the last three months. That included a 2% drop in Knightsbridge, a 1.6% fall in South Kensington and a 1.5% decline in Belgravia, as areas with the highest concentrations of wealth, and a more international buyer base, were hit by the budget. Over the last year, values in prime central London have dropped by -1.9%, Savills reports, while they rose by 1.4% in “outer prime London” during 2024. Lucian Cook, head of residential research at Savills, says: “The cautious mentality that we observed ahead of this summer’s general election and the Autumn Budget has persisted across prime markets as the year draws to a close, although properties continue to sell where they are priced competitively. “Generally, needs-based buyers have underpinned market activity post-Budget, as they have benefited from relatively stable mortgage rates and the prospect of further base rate cuts in 2025. As a result, these sub-markets have been the strongest performers in London. “However, prime central London locations remain the most price sensitive, as buyers and sellers adjust to the winding down of the ‘non-doms’ tax regime and the new SDLT surcharge for second home purchases. We expect market conditions to remain challenging in central London next year as the impact of these changes continues to be felt.” Here’s a chart from Altus Group, showing how the number of pubs in England and Wales has fallen steadily over the last five years. Pubs which have ‘vanished’ from the communities that they once served have either been demolished or converted into other types of use such as homes, offices or even day nurseries with a total of 2,074 being lost for good in just the last 5 years, Altus say. European Central Bank Governing Council member Klaas Knot has predicted that China may start selling its products to Europe at discounted rates if the US starts a trade war by imposing new tariffs on imports. In an interview published in Dutch newspaper Volkskrant, Knot says: “There is a chance that the Chinese will start offering their goods in Europe at lower and lower prices. “We are already seeing that happening in the steel market. In this way, China is, as it were, exporting its deflation to us.” 2024 was also a tough year in the UK retail sector, where nearly 170,000 UK shop workers lost their jobs in the last year. The collapse of big chains such as Homebase and The Body Shop put thousands of jobs at risk and contributed to 169,395 retail jobs disappearing during 2024 – a 42% rise on 2023 levels, new data shows. European stock markets have opened in the red, on the final full trading day of the year. In London, the FTSE 100 index has dipped by 32 points, or 0.4%, to 8115. Germany’s DAX dropped 0.5%, while France’s CAC was 0.3% lower. In other alcohol-related news, Mexico has a 500m-litre tequila lake as demand for the spirit has ebbed. The Financial Times reports this morning that Mexico is sitting on more than half a billion litres of tequila in inventory, which is nearly a whole year’s production. Data shows that around one-sixth of the 599mn litres of tequila produced last year is unsold, sitting alongside the 525mn litres that Mexico already had in inventory at the end of 2023. This growing tequila lake is due to an ebbing of the pandemic spirits boom in the US, as consumers cut back on their drinking. Bernstein analyst Trevor Stirling says: “Much more new spirit is being distilled than is being sold, and inventories are starting to accumulate. “The tequila industry is set for a very turbulent 2025.” Some of the inventory is in the process of being aged – but distillers also run the risk that Donald Trump imposes new tariffs on Mexico, making it harder to sell tequila to the US market. The drinks industry is urging the government to ease the load on publicans, following this latest drop in pub numbers. Emma McClarkin, chief executive of the British Beer and Pub Association, says: “Brewers and pubs pour billions into the economy and support more than a million jobs, so we know that closures can have a disastrous impact for both the nation’s coffers and the job market. “For the sector to remain a stalwart of the economy and continue to be the beating heart of our communities, the Government must swiftly deliver permanent and meaningful business rate reforms. “We stand ready to help the Government bring in sorely-needed change that will break down the barriers that stop our sector from contributing even more to the economy and employing more people than ever before.” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. The number of pubs in England and Wales has fallen again, as the trend of public houses disappearing from local communities accelerated in 2024. Altus Group, the commercial real estate company, reports this morning that 412 pubs were demolished or converted for other uses over the last year. That pulls the number of pubs in operation across England and Wales down to 38,989, below 39,000 for the first time. Pub owners have warned that rising costs, and changes to the alcohol excise duty system, have made it harder to keep operating, while the rising price of a pint has also led to pub closures. The sector also fears a hangover from October’s budget in 2025. Altus Group’s Alex Probyn says: “Many publicans that I speak to are extremely worried that this could be their last Christmas given the combination of hiking the amount employers will have to pay in National Insurance, increases to the minimum wage and the business rates discount being slashed from 75% to 40% in 2025. The leisure industry was also badly hit by the Covid-19 pandemic, leading to a sharp drop in the number of nightclubs in operation – down from 1,700 in 2013 to just 787 by June this year. The agenda 3pm GMT: US pending home sales for November 3.30pm GMT: Dallas Fed Manufacturing Index</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Britain’s FTSE 100 index is down 51 points or 0.6% in late trading. The US Dow Jones industrial average has lost 690 points or 1.6%. Boeing are the biggest faller on the Dow Jones in early trading, down 3.5%. This follows the crash of a Jeju Air Boeing B737-800 at Muan international airport in South Korea on Sunday, in which all 175 passengers and four of the six crew members were killed.</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>The government’s new value for money tsar has been challenged to examine the costs of a nuclear power station to be given final approval next year, as ministers attempt to shore up private investment for the project. New nuclear plants are a key part of the government’s plan to have clean power by 2030. The Sizewell C reactor, billed as generating enough energy to power 6m homes, is expected to be given the final go ahead in June’s review of public spending. Its projected costs are in excess of £20bn. However, Labour donor and green energy entrepreneur Dale Vince has written to the chair of the governments’ new Office for Value for Money (OVfM), David Goldstone, arguing that a nuclear plant already being built has seen spiralling costs. He also warns the construction of Sizewell C “will saddle consumers with higher bills long before it delivers a single unit of electricity”. The government and the French state-owned company EDF will fund about 40% of the Sizewell C project, with ministers currently rounding up private investors to meet the rest of the costs. In his letter, Vince claims that billions have already been spent on the project, even “before a final investment decision has been made”. He also raises concerns about the ballooning costs and delays of Sizewell C’s sister project, Hinkley Point C, in Somerset. “If Hinkley Point C is anything to go by, Sizewell C really should have rigorous financial scrutiny,” he writes. “Originally priced at £18bn, the cost of Hinkley has ballooned to £46bn and then there’s the delays. Back in 2007, the then EDF chief executive Vincent de Rivaz said that by Christmas 2017 we would be using electricity generated from atomic power at Hinkley. We’re now in Christmas 2024 and Hinkley isn’t due to be completed until 2031. “Due to a novel funding method, a lengthy construction timeline for Sizewell will saddle consumers with higher bills long before it delivers a single unit of electricity at a time when there is clear evidence that we can secure a cleaner, cheaper energy future without nuclear.” It comes after a similar warning by Citizens Advice earlier this year. The charity warned that the Suffolk project may offer “poor value for money” and called for greater clarity on its funding, in a letter to the Department for Energy Security and Net Zero. It has warned that the project’s funding model could expose households to cost overruns. Vince, whose Ecotricity business owns a series of renewable energy projects, also raised concerns about the money being invested in carbon capture technology. The government recently committed almost £22bn over 25 years to fund carbon capture and storage projects. However, some campaigners question the technology and argue the money could be better spent eliminating the production of carbon emissions in the first place. “Carbon capture has not been proved to work at scale anywhere in the world today and the announced £1bn a year for almost a quarter of a century shows it’s not expected to be working any time soon,” Vince writes. “I’m just not convinced that it’s worth the money. The 4,000 jobs to be created in the first year will be costing £250,000 each – not exactly good value in my opinion.” Vince calls on Goldstone, who oversaw the government’s £9.3bn investment for the 2012 Olympics, to examine the two projects should his remit allow him to do so. “I’d like to formally request you start a process and please let me know how we can take part,” he writes. A government spokesperson said: “Nuclear and carbon capture are key to our ambitious target of delivering clean power by 2030. The £2.7bn settlement for Sizewell C provides the required funding for 2025-26, and work will begin this coming year on major carbon capture, usage and storage projects in the north-east to harness this gamechanging technology – helping to protect bill payers and secure thousands of good, skilled jobs across the country.”</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>New nuclear plants are a key part of the government’s plan to have clean power by 2030. The Sizewell C reactor is billed as generating enough energy to power 6m homes. Its projected costs are in excess of £20bn. Labour donor Dale Vince has written to the chair of the governments’ new Office for Value for Money (OVfM)</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>A late newsflash: UK fashion brand Quiz has just warned shareholders that it will need extra funding by early next year, after a disappointing Christmas. Quiz has told the City that it made a loss of £4.7m in the six months to 30 September, compared with a loss of £1.5m a year earlier. Since then, it admits, it suffered a “marked decline in traffic both online and in-store” in November. And in December, while online revenues have been broadly stable year-on-year, they have fallen again in physical stores. As of yesterday, Quiz says, it had net borrowings of £3.5m, giving it £500,000 of headroom within its £4.0m of bank facilities. It warns: Given the disappointing level of revenues in the important Christmas trading period, as announced on 6 December 2024, the cash headroom available to the business is less than previously anticipated. As a result, the Board anticipates that additional funding will be required by the Group in early 2025. Time to wrap up… After a weak Boxing Day, UK, shoppers are returning to the high street today in greater numbers than last year. New data from MRI Software shows that footfall across all UK retail destinations had risen by +8% as of 12pm, compared to 27th December 2023. That might help the sector, where the number of UK retailers on the brink of collapse has risen by a quarter in the final three months of the year, driven by a combination of rising business costs and weak consumer confidence, according to a report. The proportion of retail businesses classed as being in “critical” financial distress increased by 25% to 2,124 in the fourth quarter compared with the previous three months, the insolvency specialists Begbies Traynor said. The general retail sector is under most pressure, with a 29% quarterly increase in businesses in critical financial distress, rising to 1,457 from 1,127 in the third quarter. Stocks on Wall Street have fallen in morning trading in New York… …while a rally in Japan pushed the Nikkei to a five-month closing high…. …and South Korea’s won has dropped to a 16-year low after lawmakers voted to impeach the country’s acting president. Thousands of Land Registry workers have voted to strike in a dispute over office working. Katie Wyle, head of shopping centre management UK at Unibail-Rodamco-Westfield, reports that shopper numbers at their two sites in London have been similar to last year, saying: “This year Boxing Day attracted over 320,000 shoppers to Westfield London and Stratford City which is on par with 2024 and takes our total number of visitors since festivities began to over 10m. We’re seeing lots of people coming with friends and family to dine out and enjoy leisure activities like karting at Gravity, ice skating and bowling, as well as bagging some bargains in the sales.” The selloff in New York is gathering pace, with the Nasdaq Composite now down 1.25% at 19,771 points. There’s no sign of a festive Santa Rally on Wall Street, where the US stock market has fallen at the start of trading. The Dow Jones Industrial Average dropped by 270 points, or 0.6%, to 43,055 at the open. The broader S&amp;amp;P 500 index, and the tech-focused Nasdaq, have both also fallen by 0.6%. Thousands of staff at the Land Registry have voted for strike action after being ordered back to the office for three days a week. The Public and Commercial Services (PCS) union says 3,800 workers based in 14 offices across England and Wales have voted to strike, and are also concerned about the employer inappropriately using personal data and having to accept extra responsibilities without extra pay. The Land Registry is a goverment agency that handles the registration of land and property ownership in England and Wales. PCS general secretary Fran Heathcote said: “The government doesn’t seem to learn that applying arbitrary targets on office attendance doesn’t increase productivity and is unpopular with staff members. “If they want a motivated, hard-working workforce, ministers should trust their own employees to have some say over their working conditions, rather than acting like Victorian bosses. “It’s not too late for management to avoid strike action by ending this dispute.” A Land Registry spokesperson has said the agency “will respond as needed to maintain essential services as we have done during previous periods of industrial action.” The pound is enjoying a little post-Christmas bounce. Sterling has gained 0.35% against the US dollar today, to $1.257, the highest since Monday. After yesterday’s drop in footfall, shoppers are returning to the high street today in greater numbers than last year. New dat from MRI Software shows that footfall across all UK retail destinations had risen by +8% as of 12pm, compared to 27th December 2023. They report that shopper numbers on the high street is up 8.7% year-on-year, alongside a 7.3% increase in footfall at retail parks, and 7.2% at shopping centres. This suggests that consumers are on the lookout for post-Christmas bargains, or restocking their fridges and cupboards after a flurry of festive feasting. Shoppers are “shaking off their post-Christmas slumber”, says Jenni Matthews, marketing and insights director at MRI Software, adding: Following a subdued start to the Boxing Day sales, this uplift is promising for for retail stores and destinations. It’s expected that footfall will continue to rise as the day progresses and into the weekend as consumers restock on groceries, prepare for New Years celebrations, and hunt for Boxing Day bargains. In a sign of how quiet things are in the City today, the most read article on the London Stock Exchange’s Regulatory News Service (RNS) is the test message they put out at 5am to show it was working. Russia’s rouble has fallen sharply against the US dollar today. The rouble is currently down 3.7% at 103.7 roubles to the dollar, having hit a two-week low of almost 107/$ earlier today. The weakness comes after Reuters reported yesterday that Russia’s central bank would withdraw some support for the currency in the first working week of 2025 after the New Year break. That would reverse some of the recent actions to prop up the rouble after it weakened in November, by deferring some foreign currency purchases. The London-listed mining company Gemfields said it had temporarily halted its ruby mining operation in Mozambique after groups “took advantage” of political unrest to set fire and attempt to invade its site, resulting in two fatalities. Gemfields, one of the world’s largest miners of coloured gemstones, said that more than 200 people associated with illegal ruby mining attempted to invade the residential village built by the company next to its Montepuez Ruby Mining (MRM) operation in northern Mozambique on Christmas Eve. The company, which is incorporated in Guernsey and is listed on the London and Johannesburg stock exchanges, said that the groups were trying to take advantage of the widespread civil unrest after the controversial and disputed recent national election. The oil price has risen today, amid hopes of a pick-up in demand from China. Brent crude is up 0.8% at $73.83 per barrel, after the World Bank yesterday lifted its growth forecasts for China’s economy. Shares in some UK retailers are lower today, as traders digest the drop in Boxing Day footfall yesterday. Next, the high street, online and catalogue shopping firm, are down 1.4%, putting them among the FTSE 100 fallers this morning. Marks &amp;amp; Spencer are down 0.1%. On the smaller FTSE 250 index, online electricals retailer AO World are the top faller, down almost 3%. Thames Water’s finances are on “shaky grounds” even if it secures investor and court approval to restructure its debts, analysts have warned. The company’s woe are set against an challenging outlook for the rest of the English and Welsh water sector too, according to financial services and research firm Morningstar. While regulator Ofwat has greenlit significant bill increases for consumers of £31 a year on average up to 2030, companies may still face an uphill climb to secure the necessary investment to meet increasingly stringent standards. Morningstar said in a research note: “We believe the UK water utilities will still face considerable challenges over this period given the heightened environmental concerns and large funding needs for their capital programmes.” Water companies have two months to lodge an appeal with the UK’s Competition and Markets authority if they believe the bill increases signed off by Ofwat before Christmas are unfair. Still, even if other companies face higher borrowing costs and greater investment demands, Thames stands out as a troubled case. It is battling to secure court approval for a £3bn credit lifeline and it has said it needs to raise an additional £3.25bn in equity funding. “However, both funding plans remain on shaky grounds as equity investors are concerned with the viability of the utility and the investability of the industry, while a smaller group of B-class debtholders oppose the emergency cash line as it will likely wipe out their investments in a restructuring scenario,” Morningstar said. More drama in the currency markets! India’s currency, the rupee, hit an all-time low today before rebounding – sparking speculation that the Indian central bank was selling dollars via state-run banks to curb the weakness. The rupee fell as low as 85.8075 to the dollar today, before a partial recovery to 85.48/$, down 0.25% today. Reuters reports: The Reserve Bank of India “stepped in heavily” near the 85.80 level, which helped the rupee recover, a trader at a foreign bank said. Dollar demand related to maturing non-deliverable forwards (NDF) and currency futures weighed on the rupee on Friday while panic dollar buying from importers compounded the pressure, traders said. The South Korean won has dropped to a near-16 year low against the US dollar today, amid a political crisis in Seoul. The won fell by 0.6% today, extending its recent losses, to 1,475 won to the dollar, its weakest level since March 2009. The selloff came before South Korea’s opposition-controlled National Assembly voted to impeach the country’s acting leader, Han Duck-soo. Han had only been South Korea’s caretaker leader since President Yoon Suk Yeol was impeached by the assembly after he imposed martial law earlier this month. South Korea’s main opposition Democratic party filed the impeachment motion after Han refused to fill three vacant seats in the Constitutional Court, which is set to adjudicate Yoon’s impeachment trial. Shares were also hit in Seoul, pulling the Kospi 200 index down by 0.75% today. Just in: full-day retail footfall data for Boxing Day has just been released, confirming that shopper numbers fell. There was a -4.9% drop in footfall across all UK retail destinations compared to Boxing Day last year, MRI Software reports. That implies a late-evening surge in shoppers, as footfall up to 8pm yesterday was down by -7.6%. German business associations see their current situation as worse than it was a year ago and remain pessimistic about the coming year, economic institute IW has reported today. A new survey from IW found that 31 out of 49 business associations see the current situation as worse than in 2023 and 20 out of 49 industry representatives expect lower production next year, while only 16 expect an increase. IW director Michael Huether says: “The German economy won’t get off the ground in 2025 either.” German firms are suffering from high for energy, labour and materials costs, IW says, while the geopolitical uncertainty is hampering exports, the institute added. The political crisis in Germany is also hurting investment, with a general election set for February. Many European stock markets have reopened after the Christmas break, but there’s not much festive excitement this morning! In London, the FTSE 100 index of blue-chip shares has dropped by 22 points, or 0.27%, to 8113 points. Mining company Anglo American (-1.5%) and online property portal Rightmove (-1.4%) at the top fallers. Germany’s DAX index has dipped by 0.1%, while the wider Stoxx 600 index was flat In Tokyo, Japan’s Nikkei share average has hit a five-month closing high today. The Nikkei gained 1.8% today to finish at 40,821.16, its highest close since July 17, with investors optimistic they’ll see corporate growth in the coming year. Kentaro Hayashi, senior strategist at Daiwa Securities, says: “The market cheered recent news of domestic firms, such as merger talks between Honda and Nissan. That drove expectations that Japanese firms will continue to improve investor returns.” Away from the retail sector, Britain’s steel industry is calling on the government to buy more domestic produce, as it prepares for a major expansion of offshore wind generation. Only 2% of the steel used in British offshore wind projects over the past five years was made in the UK, and the industry wants ministers to aim to dramatically increase that proportion. The business secretary, Jonathan Reynolds, is preparing to publish a new steel strategy in the spring that will look at how to “increase steel capacity and capability in the UK” even as the industry struggles with the costs of decarbonising. Gareth Stace, the UK Steel chief executive, said there was a “great opportunity” in offshore wind, but the industry wanted the Labour government to pledge to favour British-made steel in its procurement. Begbies Traynor also reports that an additional 28,747 retail businesses in the UK are in ‘significant’ financial distress – less severe than ‘critical’, but still concerning. Begbies Traynor partner Julie Palmer says: “As we look ahead to 2025, the outlook is very mixed. While some retail businesses are adapting to these pressures, many others remain vulnerable, especially in the face of rising wages, online competition from the likes of Temu and Shein, and fragile consumer confidence. With mounting challenges on the horizon, weaker businesses are likely to find little joy as we enter the New Year.” The number of UK retailers facing “critical” financial problems has risen by more than 25% in the last three months, new data shows. Highlighting the pressures on the sector, after a disappointing Boxing Day, restructuring specialist Begbies Traynor has reported there were 2,124 retailers in “critical financial distress” in the first 11 weeks of the October-December quarter. That’s a jump from 1696 in July-September, but slightly lower than the 2,142 recorded in the last quarter of 2023. Begbies, the UK’s largest insolvency practitioner, says the quarter-on-quarter increase reflects subdued consumer confidence and rising costs. Julie Palmer, partner at Begbies Traynor, says retailers are under ongoing pressures, including rising operational costs and squeezed consumer spending. Palmer adds: “Moreover, the weaker-than-expected retail sales performance in November, traditionally a critical month for the sector, further underscores the tough trading conditions, as consumers hold off on purchases amid low confidence and rising prices. “Adding to this uncertainty, the measures announced in the Autumn Budget, including the planned increase to employers’ National Insurance Contributions, will significantly dial-up the challenges faced by these businesses. These changes, alongside increases to the Minimum Wage, will negatively impact cash flow and, consequently, we expect elevated insolvency levels across this sector during 2025. “Even for more resilient businesses, the pressures remain relentless, and many will likely face financial challenges next year as they navigate these compounded difficulties. Good morning, and welcome to our rolling coverage of business, the financial markets, and the world economy. Cost-of-living pressures have been blamed for a drop in shoppers hitting the UK high street yesterday. The traditional Boxing Day sales seem to have been something of a flop, with a 7.6% drop in footfall compared to 26th December 2023 as of 8pm last night, according to data from MRI Software. Jenni Matthews, marketing and insights director at MRI Software, explains: The decline in Boxing Day activity may reflect a shift in consumer behaviour, influenced by the ongoing cost-of-living crisis. With footfall levels +18.1% higher in all UK retail destinations on Christmas Eve this year compared to Christmas Eve last year, suggesting that many shoppers concentrated much of their spending in a pre-Christmas rush. There are other factors. For starters, online shopping means many retailers began their Boxing Day sales late on Christmas Day (handy for those sober enough to operate a computer or mobile phone). Shoppers had been expected to spend £3.7bn on Boxing Day, only a 1.3% increase on last year. Secondly, many stores remained closed on Boxing Day – including John Lewis, Marks &amp;amp; Spencer, Next and Aldi – to give their staff more of a Christmas break. As Kien Tan, a senior retail adviser at PwC, puts it: “The key thing about footfall numbers is that they don’t tell the whole story. Lots of shops are now closed on Boxing Day. It used to be just John Lewis, but now Next, M&amp;amp;S and most big supermarkets close.” Thirdly, rising concerns about Christmas consumerism may have encouraged some potential shoppers to stay at home. Yesterday’s slump in the number of people tramping around the shops could show a return to the declining levels of excitement about Boxing Day that were recorded before the Covid-19 pandemic. As Matthews explained to PA Media: “We’ve got to bear in mind that (last year) was our first proper Christmas without any (Covid-19) restrictions or limitations. “Figures have come out that things have stabilised, we’re almost back to what we saw pre-pandemic.” The agenda 4pm GMT: Russia’s retail sales and unemployment rate for November</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>UK fashion brand Quiz has just warned shareholders that it will need extra funding by early next year, after a disappointing Christmas. Thousands of Land Registry workers have voted to strike in a dispute over office working. Stocks on Wall Street have fallen in morning trading in New York.</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Time to wrap up…. and get ready for Christmas! Here’s a quick recap. American Airlines has lifted an hour-long ground stop of all its flights in the US due to an unspecified technical issue, a notice on the US aviation regulator’s website showed. The ground stop, ahead of the busy Christmas travel, had threatened the holiday plans of thousands. AA had told customers: “A technical issue is affecting American flights this morning. Our teams are working to resolve the issue as quickly as possible, and we apologize to our customers for the inconvenience.” Shares have risen in London, on the final trading day before Christmas. Stocks are also rallying on Wall Street, where the S&amp;amp;P 500 is now up 0.6%. But footfall at UK shopping outlets yesterday was lower than a year earlier, in a worrying sign for the retail sector. The British car industry has welcomed government proposals that could allow Toyota Prius-style hybrids to continue to be sold in the UK after 2030, as part of a package of measures to ease regulations on carmakers. UK housebuilder Vistry has issued its third profit warning in three months, in a year-end blow to the construction company that sent its shares to a two-year low. Very best wishes for Christmas and the festive season! Bitcoin is enjoying a pre-Christmas rally, towards the record highs seen earlier this month. The world’s largest cryptocurrency is up 3.75% today at 97,341. This follows reports that the cryptocurrency industry is pushing President-elect Donald Trump’s team to kick start an overhaul of US crypto policy once he has been sworn in next month. Industry officials hope this could mean executive orders creating a bitcoin stockpile, ensuring the industry can access banking services, and creating a crypto council, in the first 100 days of Trump’s second term…. American Airlines’ shares aren’t suffering badly from this morning’s disruption. They’re down 0.4% in early trading at $17.18, having recovered most of their pre-market losses before Wall Street opened. The disruption at American Airlines came today as the industry prepared for its busiest Christmas season ever. A record 54mn passengers are forecast to fly on US carriers between December 19 and January 6, according to trade group Airlines for America (A4A). UK carriers are also expecting a record-breaking festive period, with 6.1m seats expected to be flown between December 20 and January 2, aviation data company Cirium has predicted. The FT has more details. Wall Street trading has begun, rather gently, on the final day before the Christmas break. Barely a mouse is stirring on the Dow Jones industrial average, which has gained 4 points, or 0.0097%, in early trading to 42,911 points. There’s a little more action on the broader S&amp;amp;P 500 index – it’s risen by 17.5 points, or 0.29%, to 5,991 points. Palantir Technologies are the top riser, up 4.6%, following reports the company is in talks to create a consortium to jointly bid for US government work. Elon Musk’s Tesla is close behind, up 3.7%. This is helping to lift the Nasdaq composite index of tech stocks up by 0.5%. American Airline’s shares had dropped by around 3.8% in pre-market trading after reporting the technical problem that forced a temporary stop to flights. But now that the ground has been cancelled, they’ve recovered most of that ground – and are down just 0.8% with 30 minutes before Wall Street opens. CNN confirms that American Airlines is boarding flights again, after the FAA lifted its nationwide groundstop. They say: “We apologize to our customers for the inconvenience,” American Airlines said in a statement. David Myers, a 62-year-old disaster consultant traveling from from Salisbury, Maryland, to New Orleans with a layover in Charlotte said he was first alerted to the issue at 6 am Tuesday morning. He and his wife are trying to spend Christmas with their children. “It’s Christmas Eve, so complaining doesn’t seem quite right,” Myers told CNN. “And safety always comes first. But more information at the gate would be helpful.” There’s been some worrying disruption to pre-Christmas flights in the US today – but happily, the problem may now be fixed. An unspecified technical issue forced American Airlines to suspend all flights earlier today, which must have delayed travel plans for some passengers across the country. The airline told one passenger, on X, that it was “currently experiencing a technical issue with all American Airlines flights”. But after roughly an hour, the ground stop has now been lifted, according to a notice on the U.S. aviation regulator’s website. London’s stock market has closed for Christmas, after a morning in which shares have risen in the City. The blue-chip FTSE 100 share index has closed up 34 points, or 0.4%, at 8136 – meaning the traditional seven day “Santa Claus Rally” period has got off to a solid, if unspectacular start (see earlier post for details of this festive stock market theme). AirTel Africa finished the shortened session as the top riser, up 3.8%, after beginning a new share buyback progrmme, followed by Pershing Square (+2.2%), mining company Anglo American (+2%) and Vodafone (+1.9%). Housbuilders, though, had a poor day following this morning’s profits warning from Vistry. Persimmon was the top FTSE 100 faller, down 2.4%. Vistry itself has posted a 16% plunge today, putting it firmly at the bottom of the FTSE 250 share index. Matt Britzman, senior equity analyst at Hargreaves Lansdown, says the FTSE 100 has risen despite recent “lacklustre economic data”, adding: Monday’s session saw the index close slightly lower after opening in the red, as final GDP figures revealed the UK economy stalled in the third quarter with no growth from the prior period and just a 0.9% annual rise. Adding to the wintry chill, second-quarter growth was revised down from 0.5% to 0.4%, stoking concerns about the UK’s slowing momentum heading into the new year. With 30 minutes trading to go… the London stock market is still showing gains. The FTSE 100 index is up 0.57%, while the samller FTSE 250 index has gained 0.7% – despite Vistry dragging it down after this morning’s profit warning. We have further signs today that this is not a brilliant Christmas for the retail sector. Yesterday, year-on-year footfall at UK shopping destinations was 1.2% lower than on 23rd December 2023 (a Saturday), according to retail technology firm MRI Software. Visits to UK high streets were 5.3% lower than a year ago, reflecting the general decline in physical shopping since the Covid-19 pandemic, although this was somewhat balanced out by a 4.9% rise at retail parks. On a weekly basis, footfall was up 28.5% in all UK retail destinations compared to the week before. Jenni Matthews, marketing and insights director at MRI Software, says: This spike reflects the attraction of the vast leisure and retail options available to consumers especially large families buying those last-minute gifts, groceries and also looking for that experiential element to keep the children entertained. High streets also saw strong week on week growth (+18.8%) however this was over half of what was seen in shopping centres. However, footfall remained 5.3% lower in high streets compared to the same date last year suggesting the cost of living pressures continue for many families. This was also reflected in modest year on year rises recorded in shopping centres and retail parks of +1.4% and +4.9%, respectively. Elsewhere in the car industry, shares in Honda and Nissan have jumped today after the two car makers confirmed they are in talks about a possible three-way merger with Mitsubishi. Honda shares have jumped 12% today, while Nissan gained 6%. Combining Japan’s second- and third-largest carmakers, plus Mitsubishi, would create the world’s third-largest carmaker in terms of annual sales, behind only Japanese rival Toyota and Germany’s Volkswagen. It’s a defensive effort to join forces as the automotive industry goes through its biggest ever period of upheaval. Jonathan Webster-Smith, chief investment officer at Bowmore Asset Management, makes an important point about the Santa rally concept: “Every year investors hope for a Santa rally – but they should be careful about trading on the back of it.” “The years in which this occurs are a bit too random”. Helpfully, Webster-Smith, has also pulled together some stats to back up the idea that stock markets tend to rise at this time of year. The FTSE 100 has risen in three of the past five years (2019-2023, inclusive) for the ten-day period leading up to New Year Since its creation in 1896, the Dow Jones index has historically risen in 77% of years for the period between December 26 and January 2 – averaging +1.5% The ‘Santa rally’ rise has occurred in 75% of the years since 1950 for the Dow Jones, according to one study US stock market has averaged +1.3% over the last 70 years for the period between December 24 and December 31 according to another study These gains significantly outperform the average six day return throughout the rest of the year – averaging just +0.2% But why? Well, there’s a few likely causes – from improved sentiment over the Christmas break (unless you’re working, perhaps…), money flowing into the market from bonuses at the end of the year, and the publication of lists of shares which may do well in the new year. The French stock market is also feeling a little pre-Christmas cheer, despite the recent political turmoil. The CAC 40 index is up 0.5% this morning, at 7311 points, as traders digest the news that France’s new prime minister François Bayrou has selected Eric Lombard, head of state-backed financial group Caisse des Dépôts, as the country’s finance minister. Over in Madrid, the IBEX is 0.16% higher. Across Europe, travel and leisure stocks, and shares in energy companies, are leading the gains. Germany and Italy’s markets are closed today. The Santa Rally is picking up pace! The UK’s FTSE 100 index is now up 0.5% or 45 points at 8147 points, led by telecoms firm Airtel Africa (+2.5%), which has begun a new $100m share buyback this week. Its followed by retailer JD Sports (+2.1%) and private equity group Pershing Square (+1.6%). Today’s gains mean the FTSE 100 has gained over 5.3% so far this year, although it’s still down 1.7% during December. It’s been quite a busy year for takeovers in the City, and the drama isn’t over yet. Maritime analytics firm Windward has agreed to be snapped up by an investment fund in a £216m deal announced this morning. The company, which is chaired by former BP boss Lord John Browne, is to be bought by Octopus UK Bidco, a subsidiary of an FTV Capital investment fund. The deal will see the FTV fund pay 215p per Windward share, a 47% premium on its previous closing price. Shares in Windward have jumped 42% to 207p, their highest since January 2022, shortly after it floated on the stock market. Lord Browne says: “Windward has become firmly established on the world stage, but as an organisation we recognise there remains an untapped opportunity ahead to further transform additional spheres of global trade. Following due consideration, the Windward Independent Directors believe this transaction is in the best interests of all stakeholders, including our shareholders and employees; providing the environment to facilitate this expansion and support the future growth of the company.” The UK auto industry is welcoming the government’s decision to launch a consultation into how to phase out new petrol and diesel cars by 2030. Transport Secretary Heidi Alexander has launched the consultation this morning, asking automotive and charging experts to give their views on how to end the sale of internal combustion engine-powered vehicles by the end of the decade. In this year’s election campaign, Labour pledged to restore the 2030 phase-out date for new purely petrol and diesel cars, after the previous UK government extended the phase out to 2035. Under the UK’s current targets, carmakers must ensure that a certain percentage of their sales are zero emission vehicles, or face financial penalties. The new consultation will run for eight weeks, and will be “focused on how, not if, we reach the 2030 target”, the Department for Transport says. It is in two parts – the first will look at whether hybrids, and plug-in hybrids should count towards the EV targets, and the second will consider technical changes to the mandate. Mike Hawes, chief executive of industry body the SMMT, says it is “imperative” the government resolves the uncertainty around the move to electric cars: “The automotive industry welcomes government’s review of both the end of sale date for cars powered solely by petrol or diesel, and possible changes to the flexibilities around the Zero Emission Vehicle Mandate. These are both critical issues for an industry that is facing significant challenges globally as it tries to decarbonise ahead of natural market demand. Aside from the billions invested in new technologies and products, it has cost manufacturers in excess of £4 billion in discounting in the UK this year alone. This is unsustainable and, with the 2025 market looking under even greater pressure, it is imperative we get an urgent resolution, with a clear intent to adapt the regulation to support delivery, backed by bold incentives to stimulate demand. Such action will support not only the industry, but also deliver for the economy, consumer, government and the environment.” Matthew Adams, head of transport at the Association for Renewable Energy and Clean Technology, says the consultion should help speed up the rollout of electric car infrastructure: “Today is welcome news that the Government will look to restore the end of sale of internal combustion engines to 2030. For the EV infrastructure sector this will help provide investor certainty and allow us to deploy charging infrastructure further and quicker than ever before. Decarbonising road transport is crucial to hitting net zero and this consultation is the best next step in getting us there.” Edmund King, AA president, says new clarity on the UK’s plans will help consumers move to EVs: “The AA supported the original zero emission new cars sales deadline of 2030 as ‘challenging but ambitious’ and the results of this consultation should define the firm route to zero emissions. Understandably drivers have been ‘hesitant not hostile’ about the transition but more clarity on hybrids, vans and planning support for accelerated charging infrastructure should give them more certainty. Climate change is a critical global challenge and decarbonising transport is essential.” Housebuilder Vistry is firmly on the City’s naughty list, after reporting its third profit warning of the year (see earlier post). Shares in Vistry have plunged by almost 20% at the start of trading, making it the worst performer on the FTSE 250 index of medium-sized companies. Matt Britzman, senior equity analyst at Hargreaves Lansdown, says: Vistry’s festive season is anything but merry, with profit guidance sliding down the chimney once again, this time from £300m to c.£250m, as delays to year-end transactions failed to make it onto the nice list. This marks the group’s third profit downgrade of the year, a troubling trend driven by a string of poor management decisions and forecasting missteps that have left investors feeling far from jolly. Even a late cash influx in December couldn’t light up the season, with net debt now expected to close the year at around £200m - a far cry from the neutral footing investors had hoped for. As the year ends on a sour note, Vistry faces a long winter of rebuilding trust, leaving investors with little choice but to mull over their options. The London stock market is open, and shares are rising. It’s not exactly a full-blown Santa rally, though. The FTSE 100 index is up 32 points, or 0.4%, to 8,135 points, its highest level since last Thursday (when a hawkish message from the US Federal Reserve spooked investors). Top risers in London include gold producer Endeavour Mining (+1.6%), retailers Next (+1%) and Associated British Foods (+1.1%) and Lloyds Banking Group (+0.8%). British housebuilder Vistry has issued its third profit warning in three months, resulting in a year-end blow to the construction company. The business, which was relegated from the FTSE 100 share index on Monday, now expects annual adjusted pre-tax profit of just £250m, down from previous guidance of around £300m. The group – once known as Bovis Homes - said this is partly due to delays, with a number of developments having not yet been completed, and transactions with partners having been kicked down the road to 2025. Vistry also said that it had also ditched a number of proposed deals “where the commercial terms on offer were not sufficiently attractive.” It is expecting that better terms and options will open up next year. But this is the third profit warning from Vistry in as many months. In October, Vistry launched an independent review of operations in its south division after revealing it had “understated” total build costs by about 10%. It estimated at the time that this would knock profits by £115m over the next two years, and ultimately cut annual profit for 2024 to £350m, well below the £419m last year. The news sent its shares plummeting, wiping £1bn off the company’s value. A month later, in November, Vestry said it expected a bigger hit to profit of around £165m, and downgraded its 2024 profit expectations to £300m. Commenting on the third profit warning on Tuesday, chairman and chief executive Greg Fitzgerald said it had been a “challenging past few months”: “Today’s announcement and the financial outcome for FY24 is disappointing. Our top priority for 2025 is to continue building and delivering high quality mixed tenure new homes for our partners and private customers, and to do our part in addressing the country’s acute housing shortage. We remain committed to our partnership housing strategy and are firmly focused on positioning the business to move forwards and rebuild profitability.” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. It’s the final trading day in global stock markets before Christmas, and traders will be hoping for a visit from Santa. The Santa Rally is a stock market phenomenon where shares on developed markets tend to rise around the Christmas period. And there are signs today that it’s arrived – late. Stocks are rallying across the Asia-Pacific region, where China’s CSI 300 index has gained 1.27% today, and Hong Kong’s Hang Seng is up 1%. Australia’s S&amp;amp;P/ASX 200 has nudged up by 0.25% and South Korea’s KOSPI index has risen by a more modest 0.13% That follows gains on Wall Street last night, where the S&amp;amp;P 500 rose by 0.7%. This sets the UK market up for gains in a shortened Christmas Eve session today; FTSE futures are up 0.6%, which would lift the London market away from last week’s one-month low. Market sentiment has been rattled in recent weeks by concerns that central banks may not lower interest rates as swiftly as expected in 2025. Investors now expect just two US interest rate cuts next year, and two in the UK as well. Global growth is also expected to slow next year, while the return of Donald Trump to the White House raises the risk of fresh tariffs on global trade. Trump’s election win sparked a rally in November, so perhaps Santa just came early this year. Ipek Ozkardeskaya, senior analyst at Swissquote Bank, sets the scene: It’s never too late to believe in Santa. Investors on Monday were shrugging off the bad news of past week – especially the one that suggested that the Federal Reserve (Fed) would cut its rates only two times in 2025 due to a too resilient US economy. Yesterday’s data that showed that the US durable goods orders fell more than expected in November, the new home sales rebounded slightly less than expected and the consumer confidence unexpectedly dropped in December. This bag of bad news helped tempering the latest hawkish shift in Fed expectations. As such, the buyers are out and buying. The S&amp;amp;P500 rebounded 0.73%, Nasdaq 100 rallied more than 1% and even the European Stoxx 600 eked out a small gain, as Novo Nordisk in Denmark jumped more than 5.5% as investors rushed in to buy a dip on bet that the weight loss drugs are here to stay. The agenda 12.30pm GMT: UK stock market to close early for Christmas 1.55pm GMT: US Redbook index of US retail sales 3pm GMT: Richmond Federal Reserve</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>American Airlines has lifted an hour-long ground stop of all its flights in the US due to an unspecified technical issue. Shares have risen in London on the final trading day before Christmas. Stocks are also rallying on Wall Street, where the S&amp;amp;P 500 is now up 0.6%. But footfall at UK shopping outlets yesterday was lower than a year earlier.</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Time to wrap up. The last full trading week of the year has ended on a poor note in London. The FTSE 100 share index lost 2.6% this week, its biggest weekly loss since October 2023. Fears of a US government shutdown weighed on European markets, along with concerns that central banks may not cut interest rates as fast as hoped. Trade war fears also grew, after US president-elect Donald Trump warned the EU that it will face trade tariffs on its exports to the US unless its member states buy more American oil and gas. UK borrowing in November fell to a three-year low, helped by falling debt repayment costs and higher taxes. The data was seen as an early Christmas present for Rachel Reeves. However, economists are warning that the chancellor’s headroom is being squeezed. UK retail sales rose by less than expected last month, suggesting consumers remained cautious. Millions of last-minute Christmas shoppers are expected to spend £3bn over what has been called Super Weekend, with retailers eager to make up lost ground after a “shaky start” to the festive sales season. Boohoo shareholders have rejected efforts by Sports Direct founder Mike Ashley to get himself appointed to the online fashion firm’s board. Goodnight (and good luck getting ready for Christmas). GW Despite a late mini-recovery, the UK’s FTSE 100 has indeed posted its worst weekly fall in over a year. The index of blue-chip shares listed in London has recorded a 2.6% drop this week, the biggest one-week decline since October 2023. Anxiety that central bankers won’t cut interest rates as fast as hoped in 2025, plus concerns that UK inflation is rising as the economy stagnates, weighed on the City this week. Today, the FTSE 100 lost almost 21 points or 0.26% to end at 8,084 points, with other European markets also lower. Markets remain worried about the risk of a US government shutdown, after the House of Representatives rejected a Donald Trump-backed budget package: Trump has posted that he wants any shutdown to happen now, while Joe Biden is president, saying: If there is going to be a shutdown of government, let it begin now, under the Biden Administration, not after January 20th, under “TRUMP.” This is a Biden problem to solve, but if Republicans can help solve it, they will! US consumer sentiment has risen to its highest level since April this month, after strengthening for five months in a row. The University of Michigan’s index of consumer sentiment has come in at 74.0 for December, up from November’s 71.8. It was lifted by a sharp increase in the measure of current economic conditions, with Republican voters more optimistic – and Democrats less so. Surveys of Consumers Director Joanne Hsu says: Buying conditions exhibited a particularly strong 32% improvement, primarily due to a surge in consumers expecting future price increases for large purchases. The expectations index continued the post-election re-calibration that began last month, climbing for Republicans and declining for Democrats in December. Importantly, for Independents, expectations were essentially unchanged from the past month or so for personal finances, short-run business conditions, and long-run business conditions. Broadly speaking, consumers believe that the economy has improved considerably as inflation has slowed, but they do not feel that they are thriving; sentiment is currently about midway between the all-time low reached in June 2022 and pre-pandemic readings. That early selloff in New York didn’t last long, though! The S&amp;amp;P 500 share index is now in posiive territory, up 0.7% at 5,907 points. Wall Street has opened in the red, as the risk of a US government shutdown tonight rattles traders. The S&amp;amp;P 500 share index has dipped by 0.25%, or 15 points, to 5,852 points, while the Nasdaq Composite index of tech shares is down 0.6%. Charalampos Pissouros, senior market analyst at XM, says Congress’s rejection of the spending bill backed by president-elect Donald Trump has left policymakers with no clear plan to avert a government shutdown tonight. Pissouros adds: If lawmakers fail to extend the deadline, the US government will begin a partial shutdown that could cut off paychecks for more than 2 million federal workers. With that in mind and should today’s PCE price data corroborate expectations of further stickiness in US inflation, investors may continue to reduce their risk exposure. The dollar has dipped on the foreign exchange markets, as traders react to the lower-than-forecast PCE inflation readings for November. Sterling is up half a cent today, at $1.254, suggesting that cooler-than-expected PCE is reigniting hopes of US interest rate cuts in 2025. Just in: The Federal Reserve’s preferred measure of inflation remained unchanged last month, lower than forecast. The core personal consumption index rose by 2.8% year-over-year in November, data from the US Commerce Department shows. That matches October’s core PCE reading, and was lower than the 2.9% which investors expected. Headline PCE inflation came in at 2.4%, below estimates of 2.5%, but higher than October’s reading of 2.3%. On a monthly basis, both core PCE (which excludes food and energy) and headline PCE rose by just 0.1%, below expectations of a 0.2% rise. A long awaited Swiss parliamentary inquiry into Credit Suisse has concluded that the country’s regulator was ineffective in tackling scandals at the banking giant, and that years of mismanagement had put the bank in a “precarious situation” that nearly sparked a global financial crisis. The 500-page report is the result of an 18-month investigation into the role that Swiss authorities - including FINMA and the Swiss National Bank - played in the eventual collapse of Credit Suisse, which was taken over by UBS in a forced merger during the mini banking crisis of March 2023. Commenting on FINMA (the Financial Market Supervisory Authority), the report said its supervision: “Its supervisory activities, while intensive – lacked sufficient impact. Despite numerous enforcement proceedings and warnings issued by FINMA, Credit Suisse continued to be plagued by a series of scandals. The PInC finds it regrettable that FINMA did not opt for a withdrawal of recognition for guarantees of proper business conduct during this period.” However, overall, it said that the inquiry: “Does not find any misconduct on the part of the authorities as a causative factor in the Credit Suisse crisis and acknowledges that the authorities prevented a global financial crisis in March 2023.” Instead, it said the crisis at Credit Suisse was attributed to “years of mismanagement at the bank.” “Responsibility for the loss of confidence in Credit Suisse and the difficulties that jeopardised its existence in March 2023 lies with its Board of Directors and Executive Board, who had defied numerous interventions by FINMA in the preceding years.” Credit Suisse had for years been mired in scandals, but panic over its future grew in March 2023 after its largest shareholder, Saudi National Bank, ruled out any extra funding for the Swiss lender despite the growing turmoil. The crisis of confidence first forced Swiss authorities to offer emergency loans, before eventually orchestrating a shotgun takeover by Switzerland’s largest bank, UBS, which bought the lender for a cut price of 3bn Swiss francs. The report issued a series of recommendations, including a review of emergency planning for systemically important banks in Switzerland, which failed to take into account crises of confidence and market turmoil. UBS, which now owns the remaining Credit Suisse assets, said: “The report confirms that the collapse of Credit Suisse was driven by years of strategic errors, mismanagement and reliance on substantial regulatory concessions….UBS supports most of the recommendations made by the Federal Council to strengthen the resilience of the financial center. Any adjustment to the current regime must be targeted, proportionate and internationally aligned, balancing financial stability and economic impact. This is essential for a strong and competitive UBS and a Swiss financial center that supports our economy.” British retailers have reported that sales are weakening in the run-up to the Christmas holidays. The latest data from the Confederation of British Industry shows there has been a “moderate” fall in year-on-year sales volumes during December, and that retailers expect another fall in January. CBI principal economist Martin Sartorius says: “Retailers have endured a gloomy festive period.” “Looking ahead, retailers expect sales to fall again in January, while wholesalers and motor traders are braced for sharper sales declines.” Boohoo chair Tim Morris has told the Guardian that shareholders have given “a resounding vote of confidence in our board” at the special meeting which rejected the appointment of Sports Direct founder Mike Ashley to the struggling group’s board (see earlier post). Morris said 99% of of those that voted - excluding the stake controlled by Ashley’s Frasers Group stake - had chosen to block Ashley’s appointment. Morris said Boohoo would now “like to get on with running our business” - although it is not clear how Frasers will respond to the vote. Dan Finley, the new chief executive who has already helped Boohoo drive growth at its Debenhams online department store, said he was “really excited about the opportunities ahead”. Boohoo has said Frasers, which has a 27% stake in the online specialist, could appoint an alternative to Ashley to represent its interest on Boohoo’s board. However, Morris said any candidate would have to meet certain conditions to ensure there was not a conflict of interest given Frasers’ position as a competitor. Boohoo shareholders have voted to block Sports Direct founder Mike Ashley and his associate Mike Lennon from joining its board in a blow to his efforts to wrest control of the struggling online fashion retailer. Investors representing nearly two-thirds of Bohoo’s stock – almost 64% – voted against appointing the two men at a special meeting called by Ashley on Friday morning. Dan Finley, the chief executive of Boohoo, said: “Our Group is a dynamic business, with great brands and extremely talented people, underpinned by best-in-class infrastructure. Since my appointment, I have hit the ground running, taking immediate and decisive actions to maximise and unlock value for all shareholders. “I am super energised to realise the significant opportunities I see for this business. I continue to believe this group is materially undervalued. Our most important work is ahead of us, and we will drive value for all shareholders.” Ashley had sought to become chief executive of Boohoo but was blocked by the company from putting that proposal to shareholders. He offered to he “work collaboratively” with the boss Finley if he won a board post and has convened a further meeting to oust Boohoo’s founder and executive vice-chair, Mahmud Kamani which is set for 21 January. Ashley has made Boohoo the latest in a long line of targets for his corporate empire. Ashley made his fortune with Sports Direct, but has expanded via a long string of acquisitions of retailers and brands ranging from House of Fraser to Flannels and Evans Cycles under the London-listed Frasers Group. The Boohoo chair, Tim Morris, has said Ashley and Lennon were “not appropriate candidates to join the board in any circumstances” because of “obvious conflict points”. Earlier this month, a prominent shareholder advisory firm, Institutional Shareholder Services (ISS), urged Boohoo investors to reject Ashley’s bid for a seat at the meeting on 20 December. However, Ashley has criticised Kamani for being an “egotistical founder who has an unhealthy grip on the board”. He also said Boohoo was “in desperate need of the guidance I can provide”. Europe’s STOXX 600 share index is now down 2%, on track for its biggest daily drop since August. For the last week, the Stoxx 600 has dropped by over 3.7%, which would be its biggest weekly fall since March 2023. Bitcoin is falling for the third day running. The world’s largest cryptocurrency is down over 3% today at around $94,000 this morning. Back on Monday, it hit a record high of $108,379. But it began sliding on Wednesday, the day when Federal Reserve chair Jerome Powell said the US central bank has no desire to be involved in any government effort to stockpile large amounts of bitcoin. Developments in El Salvador may also have hit bitcoin. Its government reached a financing agreement with the International Monetary Fund, which has said El Salvador should limit its exposure to the cryptocurrency, this week. But yesterday, El Salvador insisted it would keep buying bitcoin, possibly at an accelerated pace. UK food and drink exports tumbled by 10.2% in the first nine months of the year, driven by a drop in alcohol sales, according to new data from trade body the Food and Drink Federation. The EU remains the UK’s largest trading partner for food and drink, but exports to the bloc have fallen by 5.3% so far this year. Post-Brexit administrative burdens for shipments have been blamed for the slump in exports to the EU. The FDF is calling for a focus on “removing unnecessary paperwork” and targeted export support particularly for small and medium sized businesses to help them clear post-Brexit trade barriers and recover lost trade. “These figures highlight the challenges that UK food and drink continue to face when selling their products abroad,” said Balwinder Dhoot, director of industry growth and sustainability at the Food and Drink Federation. Dhoot added: “This is particularly true for the 12,000 SMEs in our industry, who struggle to overcome the administrative burdens of exporting. Providing more support for these businesses will help the UK strengthen its international trade and maintain its position on the global stage.” The US is the UK’s third largest export market - with classic British tastes like cups of tea and biscuits proving especially popular - but exports to the US still fell by nearly 8% in the year to the end of September, although the UK still retains a trade surplus with the US. Newsflash: Russia’s central bank has surprised economists by leaving interest rates on hold. At their final monetary policy meeting of the year, the Bank of Russia Board of Directors decided to keep the key rate at 21.00% per annum. Investors had expected a hike to 23%. But, the Bank of Russia explains that monetary conditions have “tightened more significantly than envisaged” in October when it raised rates to 21%. That, it believes, will be enough to cool credit activity and bring inflation down to its 4% target. Looking ahead, it adds: The Bank of Russia will assess the need for a key rate increase at its upcoming meeting taking into account further lending and inflation dynamics. According to the Bank of Russia’s forecast, given the monetary policy stance, annual inflation will decline to 4.0% in 2026 and stay at the target further on. US president-elect Donald Trump has warned European governments to buy more US energy, or face tariffs on their exports to America. In a post on his Truth Social site, Trump warned: “I told the European Union that they must make up their tremendous deficit with the United States by the large scale purchase of our oil and gas. “Otherwise, it is TARIFFS all the way!!!.” (whatever happened to ‘jingle all the way’, Donald?). After the Ukraine war began, Europe couldn’t get enough oil and gas from the US, mind you. According to the US Energy Information Administration, the United States remained the largest liquefied natural gas supplier to Europe in 2023. The US stock market is set to fall too, as government shutdown fears sweep Wall Street. London’s stock market is sliding this morning, as investors worry that the US government could shut down tonight in a spending row. The FTSE 100 index of blue-chip shares has dropped by 55 points, or 0.7%, to 8050 points, with banks among the big fallers. That means the FTSE 100 has lost 3% of its value this week, the worst weekly drop since August 2023. European stock markets are also in the red, with Germany’s DAX and France’s CAC 40 both down 1.15%. The selloff comes as the US government teeters on the brink of a shutdown, after a budget deal backed by President-elect Trump failed to pass Congress last night. Congress failed to pass a pared-down spending bill, after an earlier bipartisan deal was scuppered by Trump and Elon Musk. The new bill had included the suspension on the US debt limit fro two years, which would have make it easier for Trump to pass large tax cuts and drive the US national debt even higher. Government funding is due to expire at midnight on Friday. If Congress fails to extend that deadline, the US government will begin a partial shutdown. Paul Donovan, chief economist at UBS Global Wealth Management,says: Absent a deal, the US government starts to shut down tonight. A short-lived shutdown affects government workers, but has limited economic impact. The longer a shutdown lasts, the more disruptive it is to the US economy. Economic data may not get published in a shutdown (a problem for Federal Reserve Chair Powell with their addiction to data dependency). There wasn’t much pre-Christmas cheer in the UK automobile sector last month. The UK recorded its worst November car production numbers in over 40 years, as manufacturers were hit by amid weak demand both in Britain and across Europe. Just 64,216 new cars rolled off UK factory lines, the worst performance for any November since 1980. Output for the domestic market fell 56%, while exports were down 21%. Output was also hit by factory disruption as manufacturers transition to mak electric vehicles. Mike Hawes, SMMT chief executive, says: While a decline was to be expected given the extensive changes underway at many plants, manufacturing is under pressure at home and abroad, with billions of pounds committed to new technologies, new models and new production tooling. Government can help by supporting consumers in the transition, fast tracking its Industrial Strategy for advanced manufacturing and, most urgently, reviewing the market regulation which is putting enormous strain on the sector. “Christmas has come early” for chancellor Rachel Reeves with borrowing undershooting expectations in November (see earlier post). So says Ruth Gregory, deputy chief UK economist at City consultancy Capital Economics, who told clients: Not only was borrowing (on the PSNB ex banks measure) of £11.2bn well below the consensus forecast of £13.0bn, but it was £3.4bn lower than in November 2023 and the lowest November borrowing in three years. The breakdown revealed that £2.4bn higher spending on public sector pay left total current expenditure in the year-to-date £17.7bn higher than at the same stage last year. But due to the recent strength in wage growth and fixed personal tax thresholds, total tax receipts were £3.2bn higher than in November 2023. But while borrowing has dipped to just over £11bn last month, the recent weakening the economy – and the rise in market interest rates – could make it hard for Reeves to bring the deficit down as quickly as planned. That raises the chances that extra revenue-raising tax hikes or spending cuts will be required, Gregory says: Charlie Huggins, manager of the Quality Shares Portfolio at Wealth Club, also sees little Christmas cheer in the retail sales report: “The UK consumer appears to be limping towards the finish line in 2024 - retail sales volumes came in slightly below expectations in November, with a good performance from food the only real highlight. Online sales were weak across the board and there was little Christmas cheer on offer for clothing retailers. The 2.6% decline in clothing sales in November means clothing sales volumes are at their lowest in almost three years. With clothing often the first category consumers cut back on in difficult times, this is not a good omen. There’s “little festive cheer for retailers” in today’s sales figures, reports Alex Kerr, UK economist at Capital Economics. Not only was the rise in sales lower than expected on November, sales are still on course to decline in the October-December period, Kerr explains, adding; Given that October’s 0.7% m/m (month-on-month) fall in sales volumes appeared to be driven by households spending cautiously ahead of possible tax rises in the Budget and that the Chancellor avoided large personal tax rises, it is somewhat encouraging that sales volumes rebounded in November. That was helped by the ONS seasonal adjustment capturing the unusually late timing of Black Friday this year. But the breakdown of sub-sectors was “a mixed bag”, Kerr explains: Sales volumes in ‘other’ stores and household goods stores rose by 2.5% m/m and 1.1% m/m respectively. And food stores posted a 0.5% m/m gain. But sales at department stores fell by 0.9% m/m and sales at clothing stores followed October’s 3.5% m/m drop with a further 2.6% m/m decline as households continued to delay spending on winter clothing. And fuel sales fell by 0.7% m/m, probably as petrol pump prices rose by 0.9% m/m. We also have new data showing a fall in government borrowing. The UK government borrowed almost £11.25bn last month, the lowest November figure in three years, helped by a rise in tax receipts and a drop in interest payments on the national debt. The Office for National Statistics (ONS) reports that public sector net borrowing was £3.4bn lower than in November 2023 – lower than the £13bn expected. Happily for the Treasury, the interest bill on central government debt more than halved to £3bn in November; that’s £4.7bn less than in November 2023 and the lowest November figure for five years. The drop was due to the recent fall in the RPI inflation measure, which is used to set the interest rate on many government gilts. ONS deputy director for Public Sector Finances Jessica Barnaby says: “Borrowing this month was over £3 billion less than this time last year and the lowest November borrowing for three years. Central government tax receipts grew compared with last year, while increased spending on public services and on benefits were offset by lower debt interest payable.” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. After a disappointing autumn, retail sales across Great Britain have returned to growth – helped by early Black Friday offers. Retail sales volumes across the country rose by 0.2% month-on-month in November, new data from the Office for National Statistics show – following a 0.7% fall in October when budget uncertainty gripped the economy. November is a key month in the Golden Quarter for retailers, but these figure aren’t exactly sparkling. While retailers will welcome any pick-up in trading, November’s sales are weaker than expected – economists had forecast a 0.5% rise. Sales rose at supermarkets and other non-food stores, but there was a drop in takings at clothing retailers. Neil Birrell, chief investment officer at Premier Miton Investors, says the data suggests consumers are “feeling the pinch in a sluggish economy”. Birrell adds: With the Bank of England keeping interest rates on hold [yesterday] and inflation in the system, there are concerns around growth prospects as we go into the new year. Christmas is a key period for retail sales and will give a further clue on short term outlook and may influence the BoE at its next meeting. Unfortunately, the data doesn’t directly capture what happened on Black Friday, which fell on 29th November – but the ONS has adjusted its data to reflect that. ONS senior statistician Hannah Finselbach explains: “Retail sales increased slightly in November following last month’s fall. “For the first time in three months there was a boost for food store sales, particularly supermarkets. It was also a good month for household goods retailers, most notably furniture shops. “Clothing store sales dipped sharply once again, as retailers reported tough trading conditions. “With November’s retail sales survey covering the four weeks to the 23 November, Black Friday itself will fall within December’s figures. However, our figures account for this shift in timing to give us the best picture of what is happening in the shops.” The agenda 7am GMT: UK retail sales report for November 7am GMT: UK public finances report fro November. 10.30am GMT: Bank of Russia’s interest rate decision 1.30pm GMT: US PCE inflation measure for November 3pm GMT: Universiy of Michigan survey of US consumer confidence 3pm</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>The FTSE 100 share index lost 2.6% this week, its biggest weekly loss since October 2023. Fears of a US government shutdown weighed on European markets, along with concerns that central banks may not cut interest rates as fast as hoped. UK borrowing in November fell to a three-year low, helped by falling debt repayment costs and higher taxes.</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Time to recap… The shock news that martial law has been declared in South Korea has rocked its currency, and hit shares in the company’s stocks. The won has fallen to a two-year low today, as traders react to president Yoon Suk Yeol’s stunning decision to challenge the left-wing parliamentary group that controls the national assembly, by banning political activity. Shares in South Korean ETFs tumbled, while Samsung’s stock fell over 5% in London. Here’s the latest: The worrying news from Seoul took the shine off a rally in European stocks today, where the FTSE 100 is on track for a six-week closing high. In Germany, the DAX index climbed over the 20,000 point mark for the first time, sparking talk that a Santa Rally may be taking off in Europe. In London, anti-Barclays protesters have gathered at a banking summit…. ….where its former CEO accused the UK government of a “get those fuckers” attitude towards bankers. Luxury carmaker Jaguar has unveiled its much-anticipated concept electric car, to a better reception than it may have feared. The boss of the Japanese bank Nomura has apologised and taken a voluntary pay cut after a former employee was charged with robbery and attempted murder of a customer. Labour will miss its manifesto target of building 1.5m homes in England before the end of this parliament without more radical reform to the planning system, the thinktank the Centre for Cities has warned. The Office for National Statistics has conceded it may not be ready to replace its defective employment survey with a more accurate series until 2027, despite complaints from policymakers about the quality of the existing data. Exports of British food to the EU have dropped by nearly £3bn a year since Brexit, a trade thinktank has said, with new physical and documentary checks at the border complicating trade. South Korea’s finance minister has declared that the government will deploy all possible measures to stabilize financial markets if needed. Following an emergency meeting with top economic officials in Seoul, Choi Sang-mok said: “We will mobilize all possible financial and foreign exchange market stabilization measures, including unlimited liquidity injections.” Back in London, ex-Barclays CEO Bob Diamond says one of the reasons that UK banks are struggling compared to their US counterparts, is that the UK government doled out “biblical justice” in response to the 2008 financial crisis. This, he says, resulted in a “get those fuckers” attitude towards bankers. Diamond said the US had a relatively pragmatic response to the crisis, which amounted to three rules: one, that the banks had to repay their government bailouts; two, that they couldn’t repay those government debts until they passed stress tests; and three, until they repaid the government, those banks could not pay bonuses to bankers or dividends to shareholders. Across the pond, it was a very different story. Diamond told the FT Banking Summit: “In the UK and in Europe, it was biblical justice: ‘Let’s get those fuckers. Let’s get those banks. Let’s really hurt them’. “And I think the result of that has been very, very apparent, which is Royal Bank of Scotland is still owned by the government, and Barclays is still under pressure because they didn’t take money from the government. So my view is it was very, very different in the US than it was in the UK and Europe. And I think the US economy has been a beneficiary.” South Korea’s martial law commander Park An-su has declared that all political activities are banned, and all media will be subject to government monitoring. The Yonhap News Agency is reporting that members of the national assembly have been banned from entering the building, with the South Korean military having reportedly announced the suspension of all parliamentary activity. Our liveblog has more details: Great Britain’s energy generators were called on to ramp up their electricity output after the energy system operator warned that the country faced an energy supply crunch this evening, before dropping the warning. The National Energy System Operator (Neso) triggered an official warning over Britain’s power supplies shortly after lunchtime on Tuesday, just hours before an expected squeeze on the country’s electricity forecast for 17.30pm (as covered earlier). It later removed the warning notice saying it had “enough electricity generation to meet demand and continue to operate the system as normal”. Power supplies were expected to be tight due to a drop in wind power generation which has coincided with higher demand due to the cold snap. In the early afternoon wind power contributed just 7% to the UK’s electricity supplies, while gas-fired power plants made up 55% of all power generation, according to Neso data. As a result by the early evening Britain’s electricity supplies were expected to be less than 1% above the forecast peak in power demand. This is well below the threshold set out in market rules to operate the power system safely. Neso raised a red flag weeks after predicting that the risk of winter blackouts in Great Britain had tumbled to its lowest in four years – even after the shutdown of the UK’s last coal plant, thanks to investments in low-carbon electricity sources. In its winter outlook report Neso said it expects Britain’s winter power supplies to outstrip demand by almost 9% this year in its base case scenario, the greatest margin since the winter of 2019 to 2020. The capacity market notice is intended to spur generators to step in to sell electricity to the grid at short notice, often for lucrative fees, or encourage companies that use energy to reduce their demand in return for payments. New York-listed shares in South Korean companies have also dropped. POSCO, the South Korean steel manufacturer, are down 7% on Wall Street. Telecoms giant KT Corp are down 3.8% in New York. Exchange traded funds which track South Korean shares are also falling sharply. The MSCI South Korea ETF is down 5.1%, while the Franklin FTSE South Korea ETF has dropped by 3.9%. London-listed depository receipts in South Korean tech giant Samsung have tumbled by 5.4%, Reuters reports. Those depositary receipts are financial instruments that represents shares of a foreign company that are traded on a local stock exchange. It’s a sign that stocks on the South Korean stock market may fall sharply when trading resumes on Wednesday. The South Korean currency has fallen to as low as 1,430 won to the dollar, the lowest since late October 2022. That’s a drop of over 1.8% today. Newsflash: the South Korean won has dropped to a two year low after the country’s president stunned citizens by declarinig martial law is in place. In an unannounced late night TV broadcast, South Korean President Yoon Suk Yeol declared he would eradicate “shameless pro-North Korean anti-state forces”. Reuters reports that he did not cite any specific threat from the nuclear-armed North, however, instead focusing on his domestic political opponents instead. Yoon said he had no choice but to resort to such a measure in order to safeguard free and constitutional order, insisting: “I declare martial law to protect the free Republic of Korea from the threat of North Korean communist forces, to eradicate the despicable pro-North Korean anti-state forces that are plundering the freedom and happiness of our people, and to protect the free constitutional order.” Lee Jae-myung, leader of the opposition Democratic Party, which has the majority in parliament, warned in response that “The economy of the Republic of Korea will collapse irretrievably”, adding: “My fellow citizens, please come to the National Assembly.” Britain’s power supply margins could fall below target tonight, partly due to low wind speeds hitting renewable power generation. The National Energy System Operator has reported that the country’s electricity supply margin could drop below the threshold set out in its capacity market rules by 1730 GMT on Tuesday. Under the capacity market scheme, generators are paid to make sure power generation is available at times when demand is high. National Grid’s Electricity System Operator said on its website that expected aggregate capacity was 47,166 megawatts (MW), compared with a transmission demand and operating margin of 46,717 MW. ESO added: “No definitive information regarding additional capacity is currently available to the Electricity System Operator.” Currently, wind is only providing 14.5% of the UK’s power generration, with over half coming from gas. France’s risk premium against Germany has narrowed today, even though Michel Barnier’s government may collapse tomorrow. The yield, or interest rate, on 10-year French bonds has dipped very slightly today, to 2.91%, while the yield on the German equivalent has risen slightly, to 2.05%. That narrows France’s debt premium over Germany, which hit a 12-year high last week. That’s despite the likelihood that Barnier loses a no-confidence vote tomorrow, over his decision to force the social security budget through parliament. The CEO of BBVA says he has not yet decided whether he will sell UK high street lender TSB if his bank succeeds in its $13bn hostile takeover of rival and TSB owner Sabadell. Onur Genc told the FT Banking Summit that he was “neutral” about whether to keep TSB in any future combined banking group: “We have to see once we complete the deal.” He insisted that his main focus is on bolstering its operations across Spain. “Local scale is important and that’s why we are doing the deal” Last week, the European Commission said it did not have any objections to the takeover of Sabadell – the Spanish lender that was created in 1881 by 127 families in Catalonia – after completing a foreign subsidies review.However, the bid still faces a longer antitrust review by Spain’s competition watchdog, the CNMC, that could extend the process well into next year. A sale of TSB would mark the third major ownership change for the UK bank, which was hived off from Lloyds in 2013 as part of efforts to boost competition following its £20.3bn government bailout in 2008. TSB returned as a standalone high street bank nearly 20 years after it was snapped up by Lloyds in 1995. Led by chief executive Paul Pester, the new TSB spanned 631 branches and boasted 8,500 staff. It eventually floated on the UK stock exchange in 2014, but was bought by Sabadell a year later, marking one of the biggest cross-border banking deals since the financial crisis. Sabadell explored a potential sale of the bank in 2020 but later abandoned those plans, even as it continued to nurse the fallout of a major IT meltdown in 2018. The oil price is also rallying today, but Opec+ – rather than Santa – is responsible. The oil producers’ cartel and its allies are due to meet on Thursday, and is expected to extend its latest round of oil output cuts until the end of the first quarter. Opec+ had been hoping to unwind its recent output cuts, but is rethinking that plan as global demand slows, and output rises among non-Opec members. Brent crude is up 1%, or 70 cents per barrel, at $72.55/barrel. Fawad Razaqzada, market analyst at City Index and FOREX.com, explains: Elevated interest rates, a strong US dollar, and weak global economic growth are weighing on the oil market from the demand side of things. On the supply side, with US output already at record levels in 2024, the risk of market oversupply looms unless global growth picks up or OPEC+ implements significant production cuts. Adding to the uncertainty, speculation around a potential second Trump term has fuelled expectations of higher US oil production. This makes the OPEC’s job quite tough, complicating the crude oil forecast: does it want to achieve higher oil prices but lose market share to US shale producers, or allow oil prices to fall to potentially support demand? Well, according to Reuters, the OPEC+ is reportedly considering postponing the planned production hike for January, something which is now the base case scenario for many oil analysts. This decision, tied to resolving issues like the UAE’s agreed production increase for 2025, is expected to be finalized at the December 5 meeting. However, a substantial delay will be necessary to meaningfully support prices; otherwise, oil could quickly resume its downward trajectory amid persistent macroeconomic pressures. Barclays CEO CS Venkatakrishnan says banks have to be alive to potential risks when working with firms in the shadow banking sector, including private equity houses and private credit providers. Regulated lenders like Barclays have been trying to ensure they don’t miss out on the financial successes of the less regulated non-bank financial institutions. But Venkatakrishan said banks have to be aware of the activities of companies they lend to, and be careful about how concentrated their operations are. Speaking at the FT Banking Summit this morning, he said: “Absolutey it’s a risk…you have to be careful.” That means screening those firms in the same way they would any other client, he explained: “Whether we deal with private credit funds or private equity funds or we deal with industrial companies, you’ve got to understand the business they’re in. Decide how much you’re still willing to lend to them. Make sure you’ve got good collateral. Ensure you monitor it. Make sure you understand the ins and outs, choose your clients carefully. That’s the basics of banking. That’s what we should have been doing, and should do, for the last couple of 100 years, and the next couple of 100 years. Those things don’t change.” His comments come just days after the Bank of England released the results of their first stress test into the shadow banking sector. It found that hedge funds, pension funds and other companies in the largely unregulated sector were at risk of amplifying market shocks and triggering a £17bn asset sell-off. It seems that equity traders are not that concerned about Trump’s tariff policies, suggests Charalampos Pissouros, senior market analyst at XM: They may even feel confident that, if he is sticking to his tariff pledges, he will be similarly determined to proceed with the massive tax cuts as well. With regards to a potential Fed pause [to US interest rates], given that equity traders are longer-term investors than forex participants, they may not care that much about delayed rate cuts, as long as the rate path remains to the downside. Recent analysis from Nutmeg, the digital wealth manager owned by J.P. Morgan, shows that the Santa Rally is stronger in the City than in other markets. The FTSE 100 share index has delivered positive returns in December more often than its peer group, and has outperformed both the S&amp;amp;P 500 and Japan Index during December. Pacome Breton, head of portfolio management at J.P. Morgan owned digital wealth manager, Nutmeg, said: “While the Santa Rally has been an attractive theory for investors to believe in over the last few years, and there is some logic to this belief, it is clear from the data that market performance in December can be volatile.” But Breton warns that after a strong November, following Donald Trump’s election win, December could be quieter across markets, “as investors take a deeper look at what 2025 could bring for central banks, geopolitics and the future of the world’s largest economy.” Here’s the moment the German DAX share index hit a new all-time high this morning, hitting 20,000 points for the first time: The rally means the DAX has now risen by around 3,000 points over the course of 2024, after cracking the 17,000-point mark in December 2023. Matt Britzman, senior equity analyst at Hargreaves Lansdown, says: December is here, and while the famed “Santa rally” doesn’t typically kick in until Christmas week, this remains the most likely month for market gains. For US markets, positive economic data - including strong manufacturing and consumer spending - helped kick things off yesterday evening, though rising yields and tariff uncertainty kept investors on edge. Large-cap techs led the charge, but geopolitical tensions and the new US administration are shaping up to be the real drivers in the weeks ahead. A Santa rally may be building in Europe’s financial markets today, despite worries about the economic outlook and political instability in France and Germany. In London, the FTSE 100 share index has risen to a six-week high this morning, up 56 points or 0.7% at 8369 points. Budget airline easyJet is the top riser (+4%), after a stock upgrade from UBS, with mining company Antofagasta (+2.3%) and banks Barclays (+1.9%) and NatWest (+1.8%) not far behind. In Berlin, Germany’s benchmark DAX stock index has broken through the 20,000-point barrier for the first time, despite the recent government collapse that has led to a new election being called for next February. Paris’s CAC 40 has gained 0.6% today; risers include luxury goods makers Hermes and LVMH, on hopes of more stimulus measures in China. Europe’s gains follow a strong day on Wall Street, where the S&amp;amp;P 500 and the Nasdaq finished at new all-time closing highs last night. Kathleen Brooks, research director at XTB, says: December is Santa rally territory and so far, it’s got off to a good start. European equity markets are a sea of green on Tuesday, and French markets are bouncing back. For now, the markets are ignoring the geopolitical risks bubbling around the world. The French government is poised to collapse at some point this week, and China has decided to ban the export to the US of some items that can be used for military purposes, including gallium, geranium and other superhard materials. It will also use implement a stricter screening process for graphite exports to the US, which is a crucial input to produce lithium batteries. It will be interesting to see how Elon Musk reacts to this, and it suggests that the rest of the world will meet President Trump’s war on global trade blow for blow. French stocks are rallying despite the prospect of Michel Barnier’s government falling this week. Yesterday, leftwing and far-right parties lodged motions of no confidence after Barnier decided to push through a belt-tightening budget without a vote. Mujtaba Rahman. managing director of Eurasia Group, reckons Barnier has only a 20% chance of surviving the censure vote on Wednesday afternoon. If his government falls, all Barnier’s unfinished legislation—including the rest of the 2025 budget plan—falls too. Rahman says: France now faces its second period of political turmoil in less than five months at a time of gathering international crisis; President Emmanuel Macron will have to appoint a new Prime Minister rapidly—just possibly Barnier again but more likely a stopgap figure—in order to pass emergency tax legislation to keep the French government functioning beyond 1 January. Tiz the season for annual forecasts, and investment bank Saxo has got into the Christmas spirit by releasing its latest Outrageous Predictions, for 2025. These are events which are highly unlikely, but not impossible, and which would send shockwaves across financial markets if they did occur. The kind of things to keep at the back of the mind, just in case. And here’s this year’s list: Trump 2.0 blows up the US dollar Nvidia balloons to twice the value of Apple China unleashes CNY 50 trillion stimulus to reflate economy First bio-printed human heart ushers in new era of longevity Electrification boom ends OPEC US imposes AI data centre tax as power prices run wild A natural disaster bankrupts a large insurance company for the first time Pound erases post-Brexit discounts versus the Euro You can read all the details here. Protesters are out in full force ahead of an appearance by Barclays CEO CS Venkatakrishnan at the FT Banking Summit in London this morning. Dozens of activists are gathered outside of the Convene Centre near St Pauls - next to the London Stock Exchange - where Venkatakrishan is due to be interviewed as part of the FT Banking Summit at 10:15am. They’re protesting what they claim is the UK bank’s support for arms companies supplying Israel in its attacks on Palestinians in Gaza. Barclays has long been a target for both climate and anti-war campaigners, some of whom have vandalised Barclays branches across the UK in protest. Venkatakrishnan has continued to condemn their behaviour, and said this summer that he believed public opinion was more balanced that the protesters would lead some to believe. NatWest CEO Paul Thwaite says the bank is on a “fast trajectory to private ownership”, with the government likely to fully exit its stake within the first half of 2025. Kicking the FT Banking Summit at the Convene Centre near London’s St Paul’s Cathedral this morning, Thwaite said this will be “symbolic” for both NatWest staff and the entire banking sector, allowing the industry to close another chapter of the fallout from the 2008 banking crash. The Treasury spent nearly £46bn to bailout NatWest - back when it was known as Royal Bank of Scotland - at the height of the financial crisis. The resulting nationalisation left taxpayers owning around 84% of the lender. But a rapid sell-off over the past year has cut the remaining public stake in Natwest from 38% in December 2023 to just under 11% today. Thwaite says: “Absent some big kind of dislocation and economic events, you know, we’ll be back to private ownership next year, maybe as early the first half of the year, and that will be a great moment” And reaching that point will mean the bank can draw a line under a tumultuous chapter in the bank’s near-300 year history, Thwaite explained: “It means we can talk about the future of the bank and the potential of the bank, rather than having to talk about its past. So yeah, all, as you say, All things being well, but I think we’re on a very fast trajectory to private ownership, and I’m very proud of that” Jaguar’s new concept car has been given the thumbs up, by the Daily Telegraph. And, er, the thumbs down too. Despite not usually being a fan of change, El Tel is hailing the new electric car as “a design triumph” in an early review this morning. Their motoring correspondent, Andrew English, writes: Certainly Jaguar has traditionally been at its best when it’s done something different, but this strategy is also fantastically risky – even if it is perhaps the only path left open. For all the misleading and occasionally barbed PR and social media, it’s all window dressing until the new car is in the showrooms and they’re trying to sell it. Then the truth will out. One can’t help wishing them luck and hoping that McGovern is right when he says in uncharacteristically modest tone: “We’re taking Jaguar back to a time when it was truly loved, because it was unique.” The bodywork of the concept car, English reports, is “largely unadorned”, but with details including “almost industrial slatted ventilator panels at front and rear”, and the raw brass hinge-out panels at the base of the front wings containing the rear-view cameras. The two-seat interior is “ voluptuous” with a suitcase rack behind. English got a peek at Jaguar’s concept car yesterday at Gaydon, the company’s headquarters (The Guardian declined to sign a non-disclosure agreement (NDA), so couldn’t go). He reports that the new car has a long, untreated brass interior door handle, which will react with the sweat on hands to produce “a distinctive odour”. That, apparently, is a good thing. Mary Crisp, chief of materiality design, explains: “It’s about how car materials age. They don’t have to stay the same, they can grow and change during the life of the vehicle.” But…. down the corridor at the Telegraph, Matthew Lynn reckons the ‘Barbie’ relaunch is a disaster for an iconic brand, adding: And instead of breaking new ground, and revolutionising the way its machines are designed as promised, it looks, well, sort of like a lot of the other upmarket cars on the market. It could be the new Audi, Tesla, or Lexus. Britain’s economic inactivity problem isn’t quite as bad as feared, the country’s statistics body has revealed. The Office for National Statistics has updated its assessment of the labour force, based on new population estimates – a calculation that has increased the number of 16 to 64 year olds in the UK by 484,000. This has lifted the estimated number of people in work by 402,000 in the April-June quarter, while the number unemploywed has been raised by 30,000. An extra 60,000 people were economically inactive – neither in work nor looking for a job – the ONS estimates. These changes mean the the employment rate is revised up 0.1 percentage points to 74.6% in April to June 2024, while the unemployment rate is largely unchanged at 4.2% and the economic inactivity rate is down 0.1 percentage points to 22.1%. These changes, though, won’t fix the wider peoblems with the ONS’s labour force statistics, which have been hampered by low response rates. It says today it has reweighted data going back to 2019, and will release the results on 17 December with its next jobs report. Speaking in Miami last night, Jaguar’s creative chief Professor Gerry McGovern has said that the new brand was “influenced by the desire to recapture the essence of Jaguar’s original creative conviction”. PA Media reports: “Some may love it now, some may love it later and some may never love it. That’s what fearless creativity does,” he said, citing David Bowie, Vivienne Westwood and architect Richard Rogers as some of his creative heroes “They were British trailblazers who challenged convention and had no desire to copy the norm. “Controversy has always surrounded British creativity when it’s been at its best.” Among the design work on the new Jag is a laser-etching of the Jaguar logo in brass ingots on each side of the car. You get into the vehicle through two “butterfly” doors; inside are three hand-finished brass lines which run the length of the interior. One, down the middle, splits a pair of floating instrument panels. The “floating” front seats are finished in a wool blend which is also used on the flooring and other areas. Here are more photos of the Type 00 concept car from Miami overnight: Adrian Mardell, JLR’s chief executive officer, is promising “spectacular” results from Jaguar’s new shift, saying: The magic of Jaguar is close to my heart – an original British luxury brand unmatched in its heritage, artistry and emotional magnetism. That’s the Jaguar we are recapturing and we will create the same sense of awe that surrounded iconic models like the E‑type. Our journey is already underway, guided by our original ethos to Copy Nothing – and the results will be spectacular.” The scale of the backlash last month following Jaguar’s 30-second teaser trailer in which a group of brightly dressed models, but no actual cars, was rather over the top. The adverts came with a “Copy nothing” tagline, channelling Jaguar founder William Lyons, while signalling a decisive break with the company’s past as an old school luxury brand. If it was designed to attract attention, it certainly succeeded; critics included Elon Musk and Nigel Farage. But today, Jaguar is keen to focus on its plan to be “bold and disruptive” with its new electric car and redesign, announced last night in Miami. Managing director Rawdon Glover told Sky News: “We’ve certainly gathered an awful lot of attention over the last few weeks, but now I think its really important to talk about the vehicle.” As Glover points out, few car launches get quite as much attention, adding that the industry is at a crucial point: We need to make sure that Jaguar is relevant, is desirable, is future proof for the next 90 years of its history. “At the moment, the industry is going through huge disruption: technology changes, as we all figure out actually what an electrified world means for our brand. “At Jaguar, we’ve looked at that and we think we have to make a really bold step forward. But actually, the step we’re going to take is completely in keeping in ethos with the brand.” Glover was also pressed about the backlash against that advert, and insisted: “We absolutely don’t want to alienate any of our loyal fans. “Quite the opposite - we want to take as many of our current fans with us on that journey... We need to also appeal to a new audience. That’s what we need to do.” Good morning, and welcome to our rolling coverage of business, the financial markets, and the world economy. “There is only one thing in the world worse than being talked about, and that is not being talked about,” as Oscar Wilde reminded us. And carmaker Jaguar has avoided the latter fate, in the build-up to the unveiling of its vision for its new electric car. After an advertising campaign that led to accusations Jaguar was brusquely ditching its old followers, it now unveiled its Type 00 electric model at Miami Art Week in Florida. Described as as “design vision concept,” Jaguar says the model is a “concept with bold forms and exuberant proportions to inspire future Jaguars”. Shown in two colours, Miami Pink and London Blue, it has a long bonnet, 23‑inch alloy wheels, and a glassless rear tailgate. That means you can’t look out through the back window, and must use rear-view cameras installed near the front wheel instead. But this is just the first step. Jaguar’s first production car under this new strategy will be an electric four‑door GT, which will be unveiled late next year. This new model will target a range of up to 770km/478 miles. under the Worldwide Harmonised Light Vehicle Test Procedure testing system, while rapid charging will add 200 miles of charge in 15 minutes. Jaguar’s chief creative officer, professor Gerry McGovern OBE, says: Type 00 is a pure expression of Jaguar’s new creative philosophy. It has an unmistakable presence. This is the result of brave, unconstrained creative thinking, and unwavering determination. It is our first physical manifestation and the foundation stone for a new family of Jaguars that will look unlike anything you’ve ever seen. A vision which strives for the highest level of artistic endeavour. The agenda 8.25am GMT: FT Banking Summit in London, including NatWest CEO Paul Thwaite, Barclays CEO CS Venkatakrisnan, and former Bank of England deputy governor Sir Jon Cunliffe 9:45am GMT: Treasury Committee hearing on Work of the FCA 3pm GMT: US JOLTS survey of job openings</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>The won has fallen to a two-year low today, as traders react to president Yoon Suk Yeol’s decision to challenge the left-wing parliamentary group that controls the national assembly. Shares in South Korean ETFs tumbled, while Samsung's stock fell over 5% in London. Ex-Barclays CEO Bob Diamond says one of the reasons that UK banks are struggling is that the UK government doled out “biblical justice” in response to the 2008 financial crisis.</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Time to recap… The US economy expanded at a solid pace in the third quarter of the year, new data has confirmed. US gross domestic product increased at a 2.8% annualized pace in July-September, the second estimate of the figures from the Bureau of Economic Analysis showed today. Analysts said it showed America’s economy was ‘motoring’ along. But policymakers fear that new tariffs imposed by Donald Trump could hit growth at home and abroad. Price pressures seem to be picking up a little in the US, with the PCE inflation measure rising to 2.3% in the year to October. Coffee prices are certainly rising – they have jumped to their highest level in almost 50 years today, with analysts blaming fears of supply shortages. There have been some jitters on the French stock market, on concerns that the Paris government could be brought down by a row over a belt-tightening draft budget. Elsewhere: Wholesale coffee prices have hit their highest level in around half a century today. World arabica coffee price benchmarks climbed to their highest since 1977 on the ICE exchange today, Reuters reports, at $3.21 per lb (£2.53/lb). Reuters attributes the rally to farmers in Brazil still reluctant to sell, speculators piling in, and talk of panic buying amongst the trade. A coffee expert at one of the world’s top agricultural trade houses explained: “Brazil farmers are not interested in selling, the trade has no cash and can’t sell or put on new hedges, and speculators will certainly not sell, so there are not many sellers.” Analysts at Saxo Bank said coffee prices were rising due to “sustained worries about Brazil’s 2025 output after trees were hurt by a long drought earlier this year”. There are also concerns that next year’s harvest could suffer from the long dry and hot period that affected arabica coffee crops earlier this year, analysts at Rabobank explained. Arabica is the high-end variety favored for specialty brews. The price of robusta coffee, used to price the cheaper coffee variety typically used in instant coffee blends, has risen by almost 5% today, to the highest since the start of October. The US central bank’s favourite inflation measure has risen. The PCE price index rose by 2.3% in the year to October, up from 2.1% in September to match August’s reading. Stripping out food and energy, and core PCE rose to 2.8% from 2.7%. The Federal Reserve favours PCE as a good measure of inflationary pressures in the US economy, so Fed policymakers may be concerned to see prices rising faster than its 2% inflation target. The increase in US GDP in the last quarter was due to increases in consumer spending, exports, federal government spending, and business investment. The BEA reports: The increase in consumer spending reflected increases in both goods and services. Within goods, the leading contributors to the increase were other nondurable goods (led by prescription drugs) and motor vehicles and parts (led by used light trucks). Within services, the leading contributor to the increase was health care (both outpatient services and hospitals). The increase in exports primarily reflected an increase in goods (led by capital goods, excluding automotive). The increase in federal government spending primarily reflected an increase in defense spending. The increase in business investment primarily reflected an increase in equipment (led by information processing equipment as well as transportation equipment). The increase in imports primarily reflected an increase in goods (led by capital goods, excluding automotive). There’s a subdued start to trading on Wall Street, where the Dow Jones industrial average has gained 75 points, or 0.17%, to 44,935 points. There’s more action among small company stocks, though, lifting the Russell 2000 index by 1%. The Russian rouble has lurched to its lowest level since the early days of the full-scale invasion of Ukraine. The rouble has plunged by over 7.3% today to 113 roubles to the dollar, its weakest level since mid-March 2022. The latest drop came just days after the US introduced sanctions against Gazprombank, Russia’s third-largest bank, which played a key role in processing payments for the remaining Russian natural gas exports to Europe. My colleague Pjotr Sauer reports: Earlier rounds of sanctions had spared Russian gas because Europe’s economy was so dependent on it, but it is now far less reliant on Russian supplies. The Gazprombank sanctions raise the prospect of a further decrease in gas revenues and foreign currency for Moscow. The rouble’s weakening threatens to erode Russians’ purchasing power by increasing the cost of imported goods and could further increase inflation. The country is already contending with runaway inflation, which could climb to 8.5% this year – twice the Central Bank’s target. US unemployment claims remained low last week. There were 213,000 new initial claims for jobless support last week, a drop of 2,000 compared with the previous week. Today’s US GDP report shows that disposable personal incomes kept rising in the last quarter, despite inflation taking a bite out of pay packets. The Bureau of Economic Activity says: Disposable personal income increased $122.9 billion, or 2.3 percent, in the third quarter, a downward revision of $43.1 billion from the previous estimate. Real disposable personal income increased 0.8 percent, a downward revision of 0.8 percentage point. Today’s US GDP report looks to be good news for Donald Trump – suggesting he will take control of an economy in good shape. Lindsay James, investment strategist at Quilter Investors, says: “The US economy is clearly motoring. The second reading of Q3 annualised US real GDP growth has come in at 2.8%, in line with expectations and following 3% growth delivered in Q2, and 1.6% seen in Q1. “Rising real wages, falling interest rates and likely falling taxes and deregulation are all factors that are usually good news for stocks, and markets are already performing strongly in factoring in the better than expected growth. “US GDP has defied expectations throughout 2024, having been helped along by numerous factors. Consumer confidence levels, which have been consistently dreadful and would have indicated otherwise, do not seem to have deterred spending. Instead, US consumers continued with purchases, if more selectively in lower income households, which has played a significant role in boosting the economy. “While growth has proven unexpectedly strong this year, looking ahead, Trump’s Cabinet picks combined with a set of economic policies that are substantially un-tested in modern developed world economies mean that the range of outcomes for 2025 is wide. Nonetheless, expectations for the US economy are now much higher than they were, reflected by stock market gains of around 30% year to date. “With an impending sugar high from Donald Trump on the horizon, the US economy should continue to grow at a similar rate. However, it will take some time for the true nature and impact of the president-elect’s policies to materialise. As covered in the introduction, Bank of England deputy governor Clare Lombardelli have warned that the president-elect’s proposed trade tariff would pose a risk to economic growth in countries including the UK. Orders for durable goods at US factories rose last month, but by less than expected. Orders for durable goods – tangible products that can be stored or inventoried and that have an average life of at least three years – increased by 0.2% in October, less than the 0.5% expected. That follows a 0.4% fall in September – possibly a sign that customers are getting orders in before new tariffs are imposed on imports? Excluding transportation equipment, new orders increased 0.1%. Excluding defense products, new orders increased 0.4%. A flurry of US economic data has just been released, as statistics bodies clear the decks ahead of the Thanksgiving holiday tomorrow. First of all, we have confirmation that the US economy grew faster than European rivals in the last quarter. US GDP is estimated to have risen by an annualised rate of 2.8% in July-September, the same as was estimated last month. That’s the equivalent of 0.7% growth quarter-on-quarter, much faster than the UK’s 0.1% growth, and the 0.4% recorded in the eurozone. On trade, the US trade deficit has narrowed – to $99.1bn in October, down $9.6bn from the $108.7bn deficit recorded in September. Imports fell faster than exports: Exports of goods for October were $168.7bn, $5.6bn less than September exports. Imports of goods for October were $267.8bn, $15.2bn less than September imports. New US tariffs could push up the cost of furniture at IKEA. The chief financial officer of the world’s biggest furniture retailer has told Reuters that the proposed tariffs would make it harder for IKEA to keep prices low. Juvencio Maeztu explained that some 30% of IKEA products are sourced from Asian countries including China, with 70% coming from Europe, adding: “For us, trade barriers around the world, whether it is from one country or another country, are limiting the possibilities to make things more affordable for the many people. “We will keep working with governments and with our supply chain to try to mitigate the impact and to hope to secure affordability.” Donald Trump’s threat of a 25% tariff on Canadian imports could push Canada into recession, fears Rogier Quaedvlieg, senior US Economist at ABN AMRO. Quaedvlieg told clients today: From the perspective of Canada and Mexico, the tariffs are a hard blow. Exports to the US account for 74 and 80% of all exports of Canada and Mexico, and 20 and 26% of total GDP. Tariffs in the first Trump administration led to a percentage decrease in real consumption of about half the magnitude of the tariff percentage. This very conservative estimate gives a GDP hit of 2.5 and 3.25% to Canada and Mexico, enough to push at least Canada into a recession. Second order effects on dependent industries would amplify the impact. The countries reacted with shock to the announcement of such a strong measure. Canada seemed to try and appease President Trump, while Mexico threatened retaliatory tariffs. China on the other hand reacted mildly, seeing their promised 60% tariff downgraded to a mere 10%, although there is nothing to suggest that this proposal would replace the universal tariff touted during the elections. Manufacturers across the US are bracing for disruption from Donald Trump’s planned new tariffs – and warning their customers could be hit – my colleague Callum Jones reports: Donald Trump set the business and political world alight late on Monday. The incoming president said he would impose a 25% tariff on goods from Mexico and Canada and hit China with more levies on day one of his term. “This Tariff will remain in effect until such time as Drugs, in particular Fentanyl, and all Illegal Aliens stop this Invasion of our Country!” he wrote on Truth Social. Scott Harris has been here before. Eight years ago Catoctin Creek, the Virginia whiskey distillery he runs with his wife, Becky, was generating 11% of its sales in Europe – and expecting to more than double its business there the next year. Then the trade war kicked in. After Trump imposed steep tariffs on foreign steel and aluminum, the European Union hit back with retaliatory duties, including 25% on American whiskey. “That 11% went to zero,” recalled Harris. While that initial wave of tariffs was repealed, today Catoctin Creek has “no meaningful business” left in Europe, he said. “A few thousand dollars, but nothing to speak of.” Trump’s return to power sets the stage for a new trade war. The president-elect campaigned on a pledge to impose sweeping tariffs in a bid to revitalize the US economy. Officials in key markets are already considering if, and how, they would retaliate. More here: Back in Paris, shares in French financial companies are continuing to fall – amid worries that PM Michel Barnier’s government could be brought down by a row over a belt-tightening draft budget. Insurance group AXA are down 5%, with bank Société Générale losing 3.5%. Yesterday, Barnier warned that France could face fiscal calamity should lawmakers decide to topple his government over a budget dispute. He told French broadcaster TF1 that “There’s likely to be a serious storm and serious turbulence on the financial markets” if the government were to collapse. French bond prices are pretty flat, though. But with German bond price rising, the spread between Paris and Berlin’s borrowing costs has widened to a 12-year high: Bob Savage of BNY says: The French markets today are back to worrying about the risk of another election. The coalition government is stuck with 2025 budget battles and cracks in support with the National Rally far-right pushing back. There are broader implications about political risks everywhere. First is that in 2024, the voters have kicked on incumbents -signaling frustration over cost of living and national interests. Second is that deficits built up from pandemic responses are now problematic as debt servicing and austerity plans clash against fragmented coalitions. Setting what is most important in the years to come is the role of political leaders – and the best way forward will be to lead with growth but spending more money will not work in the same way it did during 2020. The problems of current policy and future policies show up most clearly not in FX or Equities but in Bonds. The risk premium for French debt is an example and a lesson for other governments. Britain’s financial regulator has fined the former chief supply chain officer of budget airline Wizz Air Holding over £125,000 for trading company shares when he wasn’t allowed to. András Sebők breached City rules by trading Wizz Air shares in the restricted 30-day period leading up to the firm’s financial results announcements, the FA says, and also didn’t notify the FCA and Wizz Air of his personal trades within the required 3 business days. The trading took place between April 2019 and November 2020, when Sebők made 115 trades in Wizz Air shares, worth over £4m in total. This is the first time the FCA has fined a person discharging managerial responsibility (PDMR) for trading company shares during closed periods, under Article 19(11) of the Market Abuse Regulations (MAR), it says. Pets at Home boss Lyssa McGowan has broken ranks on the implications of cost rises linked to the government’s budget - saying they won’t necessarily lead to price rises. McGowan said Pets at Home’s bill from the changes to National Insurance and the minimum wage would mean £18m in extra costs for the specialist retailer, but this was in line additional cost from the increase in the minimum wage last year, which the chain had been able to absorb through various efficiencies helped by new technology. “We absorbed that [£18m] and kept costs flat,” McGowan said, adding that the company had no plans to change its strategy because of the budget measures. “£18m, some of which was unexpected, is a lot of money but like all retailers we are looking at all avenues to ameliorate that. It is not a given at all that we will have to put up prices.” She said she was feeling “confident and optimistic” about the run up to Christmas despite a “subdued consumer” environment, as households were turning to Pets at Home’s own-label pet food, for example, as a way to save money helping the business grow in a flat market. She said shoppers were still prepared to buy treats - with the group’s premium pet advent calendars quickly selling out, for example - but were being careful in many other areas. Pet food has seen high levels of price inflation in recent years, and McGowan said prices had now flattened, but not come down. In addition a surge in the number of pets in the UK has now flattened out, with the number of pets stabilising, so that Pets at Home is signing up 15,000 kittens and puppies a year to its loyalty scheme, half the level during the height of the pandemic pet boom. Pets at Home’s share price dived 13% this morning, as the retailer warned that the subdued consumer environment would continue into the spring, hitting annual profits. Analysts at Peel Hunt trimmed £10m off their forecast, taking it down to £135m. Here’s Susannah Streeter, head of money and markets at Hargreaves Lansdown, on Aston Martin’s cash call: Aston Martin might be known for its association with James Bond, but there’s no secret agent in sight to pull it out of its latest scrape. Instead, it’s gone cap in hand to investors to raise money by issuing new shares after posting another profit warning, just months after flagging difficulties in September. The company has hit another troublesome speed bump, with production slowed down by supply chain issues, affecting deliveries of its super-high end Valiant models. This is coming on top of a deceleration of demand in China, a crucial market for the luxury car maker.’’ Trump’s tariffs will lead to higher prices in the shops, and weaker currencies for Canada, China and Mexico, explains Holger Schmieding, chief economist at Berenberg Bank. Schmieding says Taken at face value, such tariffs could raise the level of US consumer prices by c1% within a year if we assume that producers and distributors can pass on roughly 70% of higher import prices to consumers at a time of buoyant domestic demand. However, a depreciation of the Canadian, Mexican and Chinese currencies relative to the US dollar will likely absorb a significant part of that impact, perhaps up to half as a back-of-the envelope guess. Trump’s tariff statement is probably merely the opening salvo of a series of tariff threats. But interestingly, he has tied his announcement of extra tariffs on the top three exporters to the US to specific complaints about immigration and drug trafficking. That seems to open the door for negotiations. If the three countries do his bidding on immigration and drugs control to some extent, the tariffs may not be fully imposed or be partly rescinded again afterwards. The Chinese yuan, Mexican peso and Canadian dollar all fell yesterday, with the latter hitting a four-year low against the US dollar. Shares in luxury car market Aston Marton have hit a two-year low in London this morning, after it tapped its investors for more cash and cut its profit forecast. Aston, which has been hit by softening demand in China, has raised £111m by issuing new shares worth 100p each – a near-8% discount to last night’s close of 107.9p. It also raised £100m through new debt, and plans to use its new funds to invest in “future growth opportunities” and on its electrification strategy. Aston also warned shareholders last night that it has suffered delays in the delivery of its ultra-exclusive luxury car, Valiant, which cos £2m each. While deliveries are still on track to start before the end of 2024, Aston now only expects to deliver around half of the 38 Valiant models by the end of the year, havng previously expected to get the majority into customers’ hands. This will reduce operating profits to £270m-£280m, down from £285m previously expected. This morning, Aston’s shares have dropped as low as 98.1p, the weakest since October 2022, before recovering slightly to 102.4p (-5%). Lawrence Stroll, executive chairman of Aston Martin – who rescued the company in 2000 – insists it can deliver “long-term value” to shareholders, as it enters 2025 with “a stronger and more resilient balance sheet”. But, shares are down roughly 97% since its stock market float in 2018…. The London stock market has suffered another blow this morning, with the news that food delivery company Just Eat Takeaway is to delist. Just Eat is also listed on the Amsterdam stock market, where the company is headquartered, and said the delisting resulted from restarting a review into where its shares should be listed. Citing the “administrative burden, complexity and costs associated with the disclosure and regulatory requirements of maintaining the LSE listing” as its reasons for the decision, Just Eat said it was also because of low liquidity and trading volumes of its shares on the London market. The French stock exchange, the Cac 40, has dropped to its lowest level since the market wobble of early August. The Cac 40 is down 0.8% at a three-month low, led by bank stocks, and exporters such as Renault (-2.1%) and STMicroelectronics (-1.7%). Back in the UK, the competition watchdog has reported that loyalty card pricing at UK supermarkets is not always the cheapest option for consumers. In a new report, the Competition and Markets Authority (CMA) has found that loyalty prices do offer “genuine savings”; after analysing 50,000 loyalty-priced products, it found 92% offered savings on the usual price. Customers can make savings of up to 25% by buying loyalty priced products, according to the CMA. But it stressed that while they offer “legitimate” discounts, supermarket customers could still find cheaper alternative options by shopping around. George Lusty, interim executive director of consumer protection, explains: “We know many people don’t trust loyalty card prices, which is why we did a deep dive to get to the bottom of whether supermarkets were treating shoppers fairly. “After analysing tens of thousands of products, we found that almost all the loyalty prices reviewed offered genuine savings against the usual price – a fact we hope reassures shoppers throughout the UK. “While these discounts are legitimate, our review has shown that loyalty prices aren’t always the cheapest option, so shopping around is still key.” US tariffs would also have an impact on American consumers. Economists at Deutsche Bank have calculated that if Trump’s threatened tariffs were fully implemented, US core PCE inflation for 2025 could increase from 2.6% to 3.7%. Before Trump’s victory the assumption was for 2.3% inflation in 2025. Share have rallied in China today, on hopes that Beijing may roll out new stimulus measures to protect its economy from Trump’s tariffs. The CSI 300 index has rallied by 1.75%, while stocks in Shenzhen are up over 2%. Vis Nayar, chief investment officer at Eastspring Investments in Singapore, explains: “With the potential threat of tariff hikes in 2025, it’s likely China’s policymakers would come up with further stimulus packages to counter downward economic growth pressure from domestic cyclical weakness and increased external uncertainty. There remains plenty of scope for China to surprise the markets.” Budget airline easyJet has swelled its profits, despite the turmoil in the Middle East hitting demand. EasyJet has reported a pre-tax profit of £602m for the year to 30 September, £170m than the previous year. This earnings surge was driven by strong demand over the summer; easyJet had made a loss of £350m in the six months to 31 March, as conflict in the Middle East led to flight cancellations, extra costs and revenues. Outgoing CEO Johan Lundgren, says: “This strong performance - resulting in a 34% increase in our annual profits - reflects the effectiveness and execution of our strategy as well as continued popularity of our flights and holidays. It also represents a significant step towards our goal of sustainably generating over £1 billion annual profit before tax. Profits were also lifted by charges for cabin bags and “leisure bundles”; last week, easyJet was one of five airlines fined in Spain for charging passengers for hand luggage and seat reservations…. Overnight, Donald Trump has picked a protegé of Robert Lighthizer, his trade representative in the first Trump administration, to lead trade policy in Trump 2.0. Jamieson Greer, an attorney, will serve as the next US trade representative, Trump announced ovenight, and will be tasked with reining in the trade deficit and opening up “export markets everywhere”. Greer, 44, served as chief of staff to Lighthizer, who designed Trump’s original tariffs on some $370bn worth of Chinese imports, and also renegotiated the North American free trade deal with Canada and Mexico. Lighthizer, an arch protectionist and sometime free-trade skeptic, blasted “globalists” and other ideological free-traders in his recent book, “No Trade Is Free”. Kathleen Brooks, research director at XTB, says: Trump has made more picks for his cabinet, including the trade representative, Jamieson Greer. He was a protégé of the tariff tzar in Trump’s first term as president, Robert Lighthizer, and he is seen as trade hawk. This suggests that tariffs will be at the heart of Trump’s trade agenda. However, it is worth noting that as trade representative, Greer’s office will be overshadowed by the US Treasury. The new Treasury secretary, Scott Bessent, is moderate on tariffs, and has espoused free trade ideals in the past. This suggests that Trump’s tariff talk may be more bark than bite, although Greer’s appointment is a nod to the trade hawks in his team. Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. A day after Donald Trump announced plans for fresh tariffs on Canada, Mexico and China, policymakers around the world are digesting the consequences of “Tariff Man” Trump returning to the White House. A deputy governor at the Bank of England, Clare Lombardelli, has warned that the president-elect’s proposed trade tariff would pose a risk to economic growth in countries including the UK. Speaking to the Financial Times, Lombardelli explained that Trump’s trade policies could hit growth in the short term, while long-term productivity also suffers from increased trade frictions. She says: “I don’t want to speculate on the specifics but we know barriers to trade are not a good thing, whether they are tariffs or regulatory or others. “Whether you are an economic historian, an economic theorist or a data-driven economist, the impact is clear in terms of its direction. In terms of its size, that depends on the circumstances.” Trump rattled the financial markets yesterday by announcing he would impose 25% tariffs on Canada and Mexico, and an extra 10% on China, in a crackdown on immigration and drugs. Trade experts fear that Trump could spark a global trade war, if other countries retaliate with their own tariffs in response. Keith Rockwell, a former director at the World Trade Organization, explained: “The United States exports hundreds of billions of dollars worth of goods to these countries. Anyone who expects that they will stand pat and not retaliate has not been paying attention.” Trump’s proposed tariffs are likely to push up inflation in the US, as importers will pass the higher costs onto consumers – and possibly add a bit more on top! But they could have a deflationary impact on other countries; China, for example, could reroute shipments to Europe rather than the US, cutting prices to support its sales. They also pose a political dilemma for the UK – should it try to align with the US, to avoid being hit by tariffs too, or try to get closer to the EU? Simon Sutcliffe, Customs &amp;amp; Excise Duty Partner at accountancy firm Blick Rothenberg, says the US hasn’t considered such a protectionist trade policy since the 1930s with the Smoot-Hawley Act – which ended up fuelling the Great Depression. Sutcliffe says Sir Keir Starmer faces a dilemma: One of the biggest stumbling blocks in the UK’s trading relationship with the EU is the control and administration surrounding the movement of food products. Moving closer to the EU may allow development of a consistent and streamlined food policy which would reduce trade red tape and extra charges.” “However, aligning with the US would undermine that attempt, as the EU would be exceptionally resistant to allow US originating food products to ‘seep’ into its marketplace, resulting in the administrative burden on food movements being cemented in for longer.” “But ‘Refusing’ the US may result in UK exporters being subject to US tariffs on their products. The US is the largest individual trading partner of the UK trading with roughly 30% of our total exports going to the US and the US exporting 10% of its goods to the UK, so any tariffs would have a big impact on UK trade.” Also coming up today We’ll get a full-body health check on the US economy today, with a flurry of economic data – from GDP to trade and jobless claims – being rushed out ahead of the Thanksgiving holiday tomorrow. The agenda 9.30am GMT: GfK survey of German consumer confidence Noon GMT: US weekly mortgage approvals data 1.30pm GMT: US Q3 GDP report (second reading) 1.30pm GMT: US durable goods orders for October 1.30pm GMT: US weekly jobless claims data 1.30pm GMT: US trade balance for October 3pm GMT: US PCE inflation measure for October</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>US economy expanded at a solid pace in the third quarter of the year. But policymakers fear that new tariffs imposed by Donald Trump could hit growth at home and abroad. Price pressures seem to be picking up a little in the US, with the PCE inflation measure rising to 2.3% in the year to October. Coffee prices have jumped to their highest level in almost 50 years today.</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Stocks in some European and Asian markets took a hit as investors digested the ramifications of Donald Trump’s vow to slap a 25% tariff on products from Canada and Mexico, and 10% on goods coming from China. Shares in companies with signifcant operational links to the nations in Trump’s line of fire were the hardest hit, such as automotive firms and alcohol producers. While in general markets in Europe and Asia were hit over fears that Trump could target more countries and spark a potential global trade war. The announcement, made on Trump’s Truth Social platform, saw the dollar jump 1.5% against the Mexican Peso, 1% against the Canadian dollar and hit a four-month high against the Chinese Yuan. Economists at IMG have estimated that if the full cost of the tariffs are passed on to consumers, then Americans will face having to pay $2,4000 more per capital annually for goods. An exclusive poll for the Guardian found that consumers agree, with two-thirds of Americans polled saying that they think Trump’s tariffs will mean higher prices. John Roberts, the boss of British online electrical goods seller AO.com, has said that if the tariffs on Chinese goods are implemented it could mean lower prices on electricals in the UK. “Fundamentally if less product is being made in China and shipped to the US then they will want to find another home for that output which might reduce prices for us,” Roberts said. Meanwhile, optimism amongst British retailers has hit a two-year low off the back of expectations of gloomy Christmas sales, and the prospect of the increase in Employers’ National Insurance contributions next April, according to the latest quarterly survey by the Confederation of British Industry (CBI). And, the British government is expected to stick to headline targets for increasing electric car sales each year, but will consider adding extra loopholes to help carmakers, after a barrage of lobbying by the car industry. Keir Starmer’s spokesperson on Tuesday announced that the government will bring forward the consultation on the zero-emission vehicle (ZEV) mandate which will look at changes to the rules which impose fines of up to £15,000 per petrol or diesel vehicle sold above a quota. Carmakers have privately warned that they will miss the targets, forcing them to stump up millions of pounds to buy “credits” from rivals, or else pay the fines. Wall Street has opened with a mixed reaction from investors to Donald Trump’s announcement to put a 25% tariff on products from Canada and Mexico, and 10% on Chinese imports. The Dow Jones was down 0.29% at the opening bell with biotech company Amgen (11.3%), retailer Best Buy (7.9%) and General Motors (6.6%) among the biggest fallers in early trading. The tech stock heavy Nasdaq opened up 0.28%, while the benchmark S&amp;amp;P 500 rose 0.21%, as investors started to weigh the US president-elect’s plan to impose the new tariffs on his first day in the White House on 20 January. The British government is expected to stick to headline targets for increasing electric car sales each year, but will consider adding extra loopholes to help carmakers, after a barrage of lobbying by the car industry. Keir Starmer’s spokesperson on Tuesday announced that the government will bring forward the consultation on the zero-emission vehicle (ZEV) mandate which will look at changes to the rules which impose fines of up to £15,000 per petrol or diesel vehicle sold above a quota. Carmakers have privately warned that they will miss the targets, forcing them to stump up millions of pounds to buy “credits” from rivals, or else pay the fines. Business Jonathan Reynolds is expected to tell car companies that the government is listening to their concerns, at a dinner this evening hosted by the Society of Motor Manufacturers and Traders (SMMT), a lobby group. The government is likely to stick firmly to its goal of phasing out new petrol and diesel car sales from 2030, and all hybrids by 2035, according to a person with knowledge of internal discussions. The person said the government is also very likely to stick to headline targets which mandate that sales of electric cars must account for 22% of new sales in 2024 for each manufacturer, rising to 28% next year and 80% by 2030, despite reports they could change. However, the government will consider changes to “flexibilities” that effectively allow carmakers to reduce the number of electric cars that they need to sell. Those loopholes include the ability to “over-comply” in later years to make up for a slow start in the coming two or three years, and lowering the average emissions of the fossil fuel cars they sell. The “fast-track” consultation is expected to launch before Christmas, before reporting back in the first few months in 2025 - faster than most policy consultations of that type. It is also expected to include details of which hybrid cars can continue to be sold after 2030. The expected changes to the ZEV mandate would come despite opposition from charger companies, fleet owners and environmental campaigners, who argue that delays will hit investment and imperil emissions targets. Dan Caesar, chief executive of Electric Vehicles UK, a pro-battery car campaign group, said: The ZEV mandate is world-leading legislation that will put the UK firmly on the map with green tech investors and send a clear signal that the country means business when it comes to the global energy transition. Clean air and sustainable employment are surely the legacy we all want, and the existing zero emissions mechanisms is critical. Ten takeaways from Donald Trump’s new tariffs announcement Deutsche Bank has published ten conclusions, ramifications and observations following Trump’s social media posts about the impending imposition of a 25% tariff on products from Mexico and Canada, and 10% on Chinese imports, that he intends to make policy when he formally enters the White House on 20 January. 1. Free trade agreements (FTAs) are not safe Canada and Mexico are part of the United States-Mexico-Canada Agreement (USMCA) which was negotiated by Trump himself. It is clear that even countries with existing agreements with the US can be subject to tariffs. 2. Right after the Treasury Secretary announcement Tariffs are being announced just a few hours after the nomination of Scott Bessent as Treasury Secretary. This is pushback to the argument that tariffs are taking a backseat to the Trump agenda. 3. The tariffs cover 40% of total US trade While only limited to three countries, the impact is economically large at it applies to America’s three largest trading partners after the Euro-area. 4. Presidential authority, for now It is explicitly mentioned that executive authority will be used to impose these tariffs rather than the legislative route. We suspect that the most likely avenue will the International Economic Emergency Powers Act (IEEPA). 5. Tactical and transactional, for now The announcement is only targeted at three countries and leaves the prospect of tariff removal open. There is no mention of tariffs as a strategic tool to deal with trade imbalances or as a revenue-raiser. The optimistic take is that this means that some of the most extreme scenarios under universal tariffs will not happen. The pessimistic interpretation (which we favour) is that this is an opening salvo and the targeted focus on immigration and drugs is required to trigger broad-based executive authority under the IEEPA. 6. Watch the China legislation in Congress Just last week a new bill was submitted to the Senate removing permanent trade relations with China and targeting 50%-100% tariffs. There is already a similar bill in the US House of Representatives. For us, whether the tariff discussion turns strategic via legislation is a big outstanding question to be resolved. 7. Beware complex supply chains EUR/USD is reacting with relief that no mention of European trade was made. But note for example that German car manufacturers have huge production capacity in Mexico that is then on-sold to the US. Also note the complex inter-play of Chinese and Mexico trade which makes the negative impact of tariffs on Mexico even bigger. 8. Canada most under-priced The Canadian dollar has had the largest risk-adjusted weakening move since the tariffs were announced. Canada is the most vulnerable developed market country to extra tariffs but also the least under-priced in terms of risks. 9. The softer the market reaction, the greater the likelihood of more tariffs The equity market reaction has so far been very benign, we would argue likely on the back of the transactional interpretation. That US domestic small-caps have been leading the recent market rally also helps reduce the impact. The first Trump administration showed that the more benign the market reaction, the greater the likelihood of further escalation. 10. Truth Social is the new avenue for announcements During the first Trump administration, it was Twitter. Market participants need to be watching the President’s new social media platform now. Two-thirds of Americans think Donald Trump’s tariff plans will only add to rising costs if implemented, and many are planning purchases ahead of his inauguration anticipating higher prices, according to a Harris poll conducted exclusively for the Guardian. Trump declared on Monday evening that he would impose 25% tariffs on all goods from Canada and Mexico, and an additional 10% on China, if they did not stop what he claimed was illegal immigration and fentanyl smuggling. But although he has called tariffs the most “beautiful word in the dictionary”, about 69% of Americans think tariffs on imports will lead to higher prices, according to the poll. The majority of Democrats (79%), independents (68%) and Republicans (59%) all believe that tariffs will increase the prices of the goods they pay for in the US. Nearly the same percentage of respondents said that tariffs will have a significant effect on what they can afford. The poll chimes with reseaarch by ING published on Tuesday which predicts that the US president-elect’s 25% tariff on products from Mexico and Canada, and 10% on China, could cost US consumers $2,400 a year. Optimism amongst British retailers has fallen to a two-year low, according to industry body the CBI. The Confederation of British Industry (CBI) said that its quarterly survey of retailer sentiment has fallen to its lowest level since Novermber 2022, when consumers were hit by surging energy prices and markets reacted to former prime minister Liz Truss’s disastrous mini-budget. Retailers are expecting a gloomy Christmas forecasting annual sales growth to deteriorate, with volumes set to remain below seasonal norms. Firms also expect to scale back investment over the next 12 months, in part due to cost increases due to the increase in Employers’ National Insurance contributions announced in last month’s budget which come into force from April. Ben Jones, lead economist at the CBI, said: The last time retailers felt this gloomy was back in November 2022, at the peak of the inflation shock. The stark rise in Employers’ National Insurance next year will hit retailers hard. And the planned increase in business rates for higher-value properties will add significant operational costs for distribution centres. The chief executive of the UK water regulator has defended allowing the privatisation of water companies in the 1980s, despite criticism of their financial performance and environmental track record. David Black, the chief executive of Ofwat, defended the regulator’s record at a select committee on Tuesday following criticism it allowed water companies to load up on unsutainable amounts of debt, while failing to invest in infrastruture and continuing to spill sewage into rivers and seas. Asked by committee chair, the Liberal Democrat MP Alistair Carmichael whether these issues show the privatisation model has failed, Black said: “I wouldn’t agree - it shows the need for strong regulation of the sector. It’s very clear the sector needs to change. That said it’s important to bear in mind the sector has raised over £240bn since privatisation and there has been significant reduction in leakage and there’s more to do. Customer bills since privatisation have increased but we have saved billions of pounds for customers at each price review.” He added that “we can point to real successes in the model since privatisation.” The water companies in England were privatised in 1989 and since then they have come under fire for presiding over leakages of tap water, sewage spills and a lack of reservoirs being built meaning the country is at risk of running out of water. The Labour government is currently running a review into the privatised model. Carmichael asked if the situation with Thames Water, the largest water company in England, which has been at risk of collapse due to its high levels of debt, illustrates an issue with the privatised model. Black said: “Thames Water very clearly have issues with their financial structures and we have taken action to make sure customers don’t bear the consequences. With privatisation we were always very clear that we might see companies fail, that’s why we have the special administration regime, we were always very clear it wasn’t Ofwat’s role to stop companies going bust it is our role to ensure customers are protected when they are unable to meet their obligations but the fact is the sector has raised finance.” John Roberts, the boss of British online electrical goods seller AO.com, said it was too early to tell if Donald Trump’s administration would follow through with its threat to slap more tariffs on Chinese goods, but such a move could mean lower prices on electricals in the UK. “Fundamentally if less product is being made in China and shipped to the US then they will want to find another home for that output which might reduce prices for us,” Roberts said. But he cautioned: “We are a long way from it happening and tariffs biting and the follow through so I personally wouldn’t read too much into [Trump’s threats].” “Donald is a deal maker and he is laying the ground for negotiation and he is not going to lay the ground by saying I am not going to put any tariffs. This is his opening gambit and it was always going to be sensational.” Roberts made the comments as he warned that UK chancellor Rachel Reeves’ budget would push up prices for UK consumers because it meant more cost for business. AO said direct and indirect costs would rise £8m, including higher payments for self-employed drivers as well as higher national insurance contributions and the minimum wage rises for employees. “I’m no economist, I’m a washer flogger from Bolton, but if you dramatically increase all the costs then prices will go up as night follows day. They have to.” He said he was concerned as “inflation hurts the people that can afford it the least the most.” The US president-elect’s social media post announcing 25% import tariffs on products from Mexico and Canada, and 10% from China, when he takes power in January has sent global stockmarkets into a spin. Research by ING has estimated that if the costs of the new tariffs are fully passed on to consumers, then Americans will face having to pay $2,400 more per capita annually for goods. The report says that also taking into account potential labour shortages due to Trump’s plans to crackdown on immigration – with a vow to stage the “largest deportation operation in American history” – there could be a 1% increase in inflation in the US. James Knightley, ING chief international economist for the US, said: “President-elect Donald Trump has promised to implement sweeping new tariffs aimed at protecting American industries, promoting domestic manufacturing, and reducing reliance on foreign imports. “However, tariffs imposed during the first Trump term – and continued and extended under Biden – did not achieve all of the promised outcomes. Furthermore, our research shows that if the new tariffs are fully passed on, they could increase inflation and cost American consumers up to $2,400 per capita annually. The report points to policies implemented under the first Trump administration, such as a 20% tariff on all imported large residential washing machines introduced in 2018, which resulted in the retail cost climbing 12%. Unlike Halfords, which reported a £23m hit from tax rises in the budget this morning, Compass Group, Europe’s biggest catering company, talks about the “opportunity rather than threats” this brings to its business. Dominic Blakemore, the Compass chief executive, told analysts and investors that the “cost and complexity” of the increase in national insurance contributions for employers will pile pressure on many UK companies, and may prompt them to outsource catering to save money. “The NIC rate increase increases cost for everyone. We see an opportunity in first-time outsourcing.” He argues that Compass, given its size and presence in other countries, can manage those cost rises more efficiently. The company employs 55,000 people in the UK, and 580,000 globally. His comments came as the catering group reported a 10% rise in revenues to $42bn in the year to 30 September, while underlying profit before tax rose to $2.7bn from $2.4bn. Robert Habeck, Germany’s economy minister, has said that Donald Trump’s announcements about tariffs on products from China, Mexico and Canada should be taken seriously. A number of analysts have said that markets should view the US president-elect’s proposed tariffs more positively, given he has threatened a hike of as much as 60% on Chinese imports if the country doesn’t agree with his policies. However, Habeck said that Europe and Germany need to seek urgent talks with the US to head off a potential trade war and stand united. European markets and listed companies operating in sectors including automotive and alcohol are a “sea of red” this morning as investors react to the impact of Trump’s announcements, and the possibility other countries could be targeted with tariffs next. Shares in European brewers have been hit by Donald Trump’s threats to introduce aa 25% tariff on products from Mexico and Canada Trump, who posted the policy announcement on his social media site Truth Social, has also said that Chinese imports will be hit with a 10% tariff when he officially takes over at the White House on 20 January. Budweiser and Stella Artois maker AB Inbev and Heineken, which both have operations in Mexico, fell 2.3% and 2.2% respectively. Guinness maker Diageo, which also has operations in Mexico, was the biggest faller down 2.5%. Meanwhile, Campari fell 2.3%, Remy Cointreau slid almost 2%, Pernod Ricard fell 1.7% and Carlsberg dropped by just over 1%. Kathleen Brooks, research director at XTB, said that European stocks are a “sea of red” this morning following Trump’s policy-by-social media announcement. She pointed out that London’s FTSE 100 has proved to be the most resilient of the European markets as the UK is “expected to be shielded from the worst of Trump’s tariff plans”. Mohit Kumar, in the global economics team at Jefferies, sees the move by Trump as an “opening move for negotiations” given he has threatened that tariffs on Chinese imports could go up to 60%. Our view remains that tariffs will eventually not end up as bad as feared, but we will see increased uncertainty over the coming months. Waking up to check the tweets for any policy announcements could become the norm. Tariffs will further support the view of US over rest of the world from an investment perspective. Halfords could raise prices for car servicing and repair to help it cope with a £23m cost increase after the autumn budget, and called for more business support from the government. The cycling and motoring retailer, which has more than 12,000 employees, reported on Tuesday that the budget measures add £23m of direct labour costs, of which £9m was already included in its planning assumptions. Fears of a potential global trade war has fuelled a sell-off of European automotive stocks. Shares in Stellantis, the owner of brands including Fiat, Chrysler, Peugeot and Vauxhall, have been hit the hardest falling almost 6% in early trading. Germany’s Volkswagen fell 2.7%, Mercedes-Benz tumbled 2.2%, BMW dropped 2.4%, and luxury brand Porsche fell 2.3%. Marc Ostwald, chief economist and global strategist at ADM Investor Services, said that markets will have to “reattune” to Trump’s “frequently erratic” approach to policymaking. Trump’s promise overnight to implement tariffs immediately on taking office in January were no great surprise, though the fact that he is taking initial aim at Mexico and Canada as much as China may have surprised some, though it is in line with his narrative during the election. Still it serves as a reminder that markets will have to reattune themselves to his frequently erratic approach to policymaking, and his likely hefty reliance on executive orders where possible to circumvent the legislature. European stock markets have fallen at the start of trading as investors worry about the ramifications of Trump’s international tariff threats, with the pan-European STOXX 600 index down 0.5%. The FTSE 100 index of blue-chip stocks in London fell by 0.3% in early trading, while Germany’s DAX fell 0.5%. In France, the CAC 40 share index dropped 0.8% Chris Turner, global head of markets at ING, published a note saying that Europe will not be “breathing a sigh of relief” despite not being targeted by Trump in his first round of tariffs. That Europe was not mentioned in Trump’s first tariff post could perhaps be welcome news on the continent. Yet local policymakers will remain fearful that it will just be a matter of time before Trump turns his attention to the European auto sector or tariffs more broadly. In any case, the threat of further tariffs on China shows the direction of travel on world trade, which is bearish for the euro. Copper prices have fallen, weighed down by a stronger US dollar and US President-elect Donald Trump’s pledge to levy more tariffs on Chinese products. Three-month copper on the London Metal Exchange (LME) was down 0.6% at $8,990.50 per metric ton by 7am, while the most-traded January copper contract on the Shanghai Futures Exchange (SHFE) closed down 0.3% to 73,740 yuan ($10,162.48) a ton, Reuters reported. Investor Bill Ackman said that markets should be up as Trump is using the threat of tariffs as a weapon to achieve wider US economic goals. “To be clear, according to Trump the 25% tariffs will not be implemented, or if implemented will be removed, once Mexico and Canada stop the flow of illegal immigrants and fentanyl into the U.S,” he posted on X. “In other words, @realDonaldTrump is going to use tariffs as a weapon to achieve economic and political outcomes which are in the best interest of America, fulfilling his America first policy. This is a great way for Trump to effect foreign policy changes even before he takes office.” Good morning, and welcome to our coverage of business, the financial markets and the world economy. Donald Trump has kicked-off his long feared plan for new tariffs sending shockwaves through the markets. The US dollar rose and shares dipped after Donald Trump said he will impose additional tariffs on products coming into the US from China, Mexico and Canada. Posting on his social media site Truth Social, Trump said that when he becomes president on January 20th he will “sign all necessary documents to charge Mexico and Canada a 25% Tariff on ALL products coming into the United States, and its ridiculous Open Borders.” The levy on products from Mexico and Canada – and 10% on Chinese imports – saw the dollar rise almost 2% against the Mexican peso and hit a four and a half year high against the Canadian dollar. The US currency also rose to its highest level since July against China’s yuan as markets reacted to Trump’s comments. Most Asian equities declined with share benchmarks in Japan, Australia and South Korea all dropping. The news on tariffs reversed a 0.6% fall in the dollar index on Monday, following Trump’s nomination of hedge fund manager Scott Bessent as Treasury secretary, an appointment investors took as a sign that the president-elect’s policies may be moderated. Stephen Innes, managing partner, SPI Asset Manager, said: In a striking return to hardline policies, President-elect Trump has dramatically escalated tensions with a brash promise to impose a sweeping 25% tariff on all imports from Canada and Mexico the moment he reassumes office. This bold declaration shatters any lingering hopes that the new Treasury Secretary, Scott Bessent, might usher in an era of moderation. Initially hailed as a beacon of stability, Bessent’s influence now seems overshadowed by a resurgence of Trump’s uncompromising “America First” doctrine, which starkly excludes even the closest of allies from its protective embrace. The agenda 9am: FCA to release consumer research on crypto assets, and its crypto ‘roadmap’ 10.00am: The EFRA Committee will hold an evidence session to scrutinise the work of Ofwat 11.15am: UK Treasury minister expected to speak at TheCityUK National Conference in Birmingham 2:30pm: Business and Trade select committee session with UK business secretary Jonathan Reynolds</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>European and Asian markets took a hit as investors digested the ramifications of Donald Trump’s vow to slap a 25% tariff on products from Canada and Mexico. Shares in companies with signifcant operational links to the nations in Trump's line of fire were the hardest hit. Economists at IMG have estimated that if the full cost of the tariffs are passed on to consumers, then Americans will face having to pay $2,4000 more per capital annually.</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Trade War Impacts Markets</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>When Margot Robbie made a surprise cameo in the 2015 film adaptation of Michael Lewis’s book The Big Short, she did more to educate the general population about the risks of securitisation than most financial experts. The Australian actor’s brief monologue, notoriously delivered from a champagne bubble bath, explained how banks were bundling up their growing cache of risky sub-prime mortgages into investable bonds, before slicing them up and selling them off for profit. But the proliferation of these mortgage-backed securities in the early 2000s meant there was a catastrophic ripple effect across the global financial system when borrowers started to default on their home loans. The resulting crisis in 2008 triggered a crackdown by regulators. They introduced new rules that could help ensure that asset-backed securities – once allegedly referred to as “crack cocaine of the financial services industry” by the billionaire Guy Hands – would never again spark such a massive meltdown. But, 16 years later, some experts believe new risks are emerging. And this time, they are linked to highly indebted companies backed by private equity firms, which are part of the growing but opaque portion of the financial system known as the shadow banking sector. Shadow banking refers to financial firms that face little to no regulation compared with traditional lenders, and includes businesses such as hedge funds, private credit and private equity funds. While the use of securitisation dipped in the wake of the 2008 financial crisis, as a result of a tarnished reputation and regulatory backlash, its popularity has subsequently risen. Today, the global securitisation market covers about £4.7tn of assets, according to estimates by analysts at RBC Capital. The UK accounts for about £300bn of that total, but more than half – about £180bn – is part of the so-called public securitisation market. In this public market, bundled loans are rated by credit rating agencies and sold on to a broad range of investors, and their terms, structure and sales are openly disclosed. These are the routes typically taken by traditional banks, which face far more stringent regulation. The remaining £120bn is made up of securitised loans bundled up by the shadow banking sector. Private securities are sold directly to a limited pool of sophisticated investors. They are less regulated, need not be reviewed by ratings agencies, and are far more opaque. Some believe that the growth of the private market, and its lack of transparency, could pose a problem. “It probably is an under-appreciated risk, given the lack of regulation in that space and the complexities of the instruments that are being held there,” Benjamin Toms, an analyst at RBC Capital, said. But even the public securities market warrants close review, according to Natacha Postel-Vinay, an assistant professor at the London School of Economics and expert in regulation and financial history. That includes risks related to collateralised loan obligations (CLOs). These are types of securities that are backed by a pool of debt, including loans to companies with low credit ratings, or struggling businesses that have been snapped up by private equity firms with the help of big loans, in what are known as leveraged buyouts. “The private equity firms invest in companies that are almost failing, and in order to make these companies survive, they load them up with debt,” said Postel-Vinay. “These loans end up being repackaged as well, a little bit like the junk mortgages before the 2008 crisis.” And although CLOs are usually made up of different kinds of loans to businesses in a variety of sectors, this does not entirely eradicate risk. “It’s a game of whack-a-mole. You regulate stuff, but then the financial system finds ways around the regulation very quickly,” Postel-Vinay said. The Bank of England is in the midst of compiling the results of its first stress test involving the shadow banking sector, the results of which are expected to be released at the end of next week. Although it will not focus directly on securitisation, the Bank has not been shy in flagging its concerns. It warned last December that, while UK banks were partly shielded from losses on CLOs by generally holding the highest-quality slices of the securities, the UK financial system was indirectly at risk through its connection to foreign banks and insurers that have a high and growing exposure to the loans held by already highly indebted companies. And in June, the financial policy committee highlighted risks related to the private equity industry more broadly: “Vulnerabilities from high leverage, opacity around valuations, variable risk management practices and strong interconnections with riskier credit markets mean the sector has the potential to generate losses for banks and institutional investors.” Postel-Vinay said it was important to determine who should be held responsible before things go wrong. “We want to make sure that we don’t repeat the mistakes [of the 2000s] and that it’s super, super clear who is responsible for the underlying credit risk in these loans. “There are underlying loans that need to be repaid, and they need to be screened, and they need to be monitored … And in these cases, I have to say, there is a lack of transparency. I think a lot of people don’t know exactly what’s going on.”</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>The proliferation of mortgage-backed securities in the early 2000s meant there was a catastrophic ripple effect across the global financial system. The resulting crisis in 2008 triggered a crackdown by regulators. But, 16 years later, some experts believe new risks are emerging. This time, they are linked to highly indebted companies backed by private equity firms.</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Time for a recap. Evidence is growing that the UK economy is weakening, while the eurozone is also lurching deeper into trouble … as the US pushes ahead. UK business activity shrank for the first time in over a year this month, according to the latest poll of purchasing managers, in a sign that corporate confidence has been hit by last month’s budget. Chris Williamson, chief business economist at S&amp;amp;P Global Market Intelligence, says: Business optimism has slumped sharply since the General Election, dropping further in November to hit the lowest since late 2022. Companies are giving a clear ‘thumbs down’ to the policies announced in the Budget, especially the planned increase in employers’ National Insurance contributions. UK retail sales also took an downturn turn last month, dropping by 0.7% in October led by a decline in turnover at clothing stores. The weak data hit the pound, which dropped to a six-month low below $1.25 against the US dollar. It all piles the pressure on Rachel Reeves, who last night held an event with senior women in finance in a bid to improve the “measly increase” in women in top jobs. The picture is also deteriorating in the eurozone, where the services sector has now joined manufacturing in contraction. German business activity fell at the quickest rate for nine months, while the French economy is shrinking at the fastest pace since January. But the US private sector is growing at the fastest pace in two and a half years, with American factories stockpiling products ahead of new tariffs on imports. UK households face a 1% rise in energy bills in January, after regulator Ofgem lifted its quarterly price cap. Charities warned that strugging families would find it hard to warm their homes this winter. Cryptocurrency prices jumped, after SEC chair Gary Gensler announced he would step down in January, clearing the way for Donald Trump to appoint a more crypto-friendly successor. Spain has fined five budget airlines, including Ryanair, a total of €179m (£150m) for charging passengers for hand luggage and seat reservations, prompting the Irish carrier to say banning the practices would “destroy” the ability to offer cheap tickets. The chief executive of Northvolt has resigned, after the Swedish battery startup filed for bankruptcy protection in the US. And in the media world, National World, the owner of the Scotsman and Yorkshire Post and underbidder in the auction for the Telegraph titles, has received a buyout proposal from its largest shareholder, Media Concierge. Expectations for the US economy among Republican supporters have surged this month, while Democrats are much gloomier. That’s according to the University of Michigan’s consumer sentiment index, just released, which highlights the two groups’ incongruous views of how president-elect Trump’s policies will influence the economy. Overall, the consumer sentiment index rose by 1.3 points this month, up to 71.8 points from October’s 70.5. However, that’s also 1.3 points lower than the preliminary estimate earlier this month, of 73. Surveys of Consumers director Joanne Hsu says: Current conditions saw insignificant changes this month across the political spectrum, consistent with the fact that the resolution of the election exerted little immediate impact on the current state of the economy. Ultimately, substantial uncertainty remains over the future implementation of Trump’s economic agenda, and consumers will continue to re-calibrate their views in the months ahead. Boom! Growth in the US economy has hit its highest level in two and a half years this month, following this month’s election. There was a “marked upturn in growth of business activity in November”, according to the latest poll of purchasing managers at American companies. It shows that growth this month was a 31-month high, with output buoyed by the sharpest rise in demand for two-and-a half years. That’s a much brighter picture than we’ve seen in the US or the eurozone this morning. US factories are stepping up their purchases of imported inputs as they seek to front-run tariffs, the survey shows, which is putting pressure on supply chains. Business confidence also picked up, with firms’ expectations of output in the coming year rose to the highest since May 2022. S&amp;amp;P Global, which compiles the survey, attributes this optimism to the prospect of lower interest rates, improved economic growth, and more supportive business policies from the new administration in 2025. Chris Williamson, chief business economist at S&amp;amp;P Global Market Intelligence, says: “The business mood has brightened in November, with confidence about the year ahead hitting a two-and-a-half year high. The prospect of lower interest rates and a more probusiness approach from the incoming administration has fueled greater optimism, in turn helping drive output and order book inflows higher in November. “The rise in the headline flash PMI indicates that economic growth is accelerating in the fourth quarter, while at the same time inflationary pressures are cooling. The survey’s price gauge covering goods and services signalled only a marginal increase in prices in November, pointing to consumer inflation running well below the Fed’s 2% target. Stocks have opened higher on Wall Street, on the final trading day of the week. The Dow Jones industrial average has gained nearly 0.5%, or 197 points, to 44,068 at the open. Almost every one of the 30 companies on the index is up, led by Nike (+2.1%) and IBM (+1.5%). Chipmaker Nvidia is the only laggard, down 1.3%. The broader S&amp;amp;P 500 index is up 0.2%, while the tech-focused Nasdaq is flat. The chief executive of Northvolt has resigned, after the Swedish battery startup filed for bankruptcy protection in the US. Peter Carlsson, who has led Northvolt since 2016, will step aside with immediate effect, the company said on Friday. Carlsson said Northvolt, which is widely seen as a leading player in European efforts to build an electric vehicle battery industry, needs to raise between $1bn (£800m) and $1.2bn in order to restore the business. Northvolt has built a factory in northern Sweden where it hopes to use green energy to produce hundreds of thousands of EV batteries each year. It was the most prominent of a host of European startups hoping to challenge the dominant Asian battery industry. However, the company has tipped into crisis in recent months as cash ran dry and it experienced problems getting its first factory up and running properly. More here… Defence firm Thales has just told the Paris stock market that it denies allegations of misconduct, following a joint UK-French investigation. News broke last night that Thales, the multinational aerospace and defence electronics contractor, was being investigated by the UK’s Serious Fraud Office and its French equivalent, Parquet National Financier (PNF), over suspected bribery and corruption. In a statement to the stock market, Thales says: Thales confirms that the Parquet National Financier (PNF) in France and the Serious Fraud Office (SFO) in the United Kingdom have initiated an investigation in relation to four Thales entities located in France and the UK, regarding the performance of a contract in Asia. Thales denies the allegations brought to its knowledge. The Group is fully cooperating with the PNF in France and the SFO in the UK. Thales complies with all national and international regulations. Shares in Thales have fallen 6% so far today. While the pound is sliding, shares on the London stock market are rising. Hopes of faster cuts to UK interest rates have helped push up the share prices of construction firms such as Barratt Redrow (+3.5%) and Vistry (+3.6%). Shares in retailers are also higher, with B&amp;amp;M up 4.1% and Sainsbury’s 3.4% higher, despite this morning’s drop in UK retail sales. They may be benefitting from a pick-up in UK consumer confidence this month, according to the latest poll from GfK, which found that consumers have turned less pessimistic following the government’s first budget and the U.S. presidential election and they are showing more appetite for spending in the run-up to Christmas. The UK’s competition regulator is gearing up to launch a new probe into Apple and Google. The Competition and Markets Authority’s (CMA) independent inquiry group has carried out an in-depth assessment of the mobile browser markets and has provisionally concluded that they are not working well for UK businesses and millions of phone users. The group is recommending that the CMA board consider investigating Apple and Google’s mobile ecosystem activities using new digital markets powers. The group has provisionally found that Apple’s rules restrict other competitors from being able to deliver new, innovative features that could benefit consumers. Other browser providers have highlighted concerns that they have been unable to offer a full range of browser features, such as faster webpage loading on iPhone. Apple, though, denies it is holding back innovation in smartphone browsers. It says: “We disagree with the findings in the report regarding Safari, WebKit, and in-app browsing on iOS. “We are concerned that the interventions discussed in the report for future consideration under the Digital Markets, Competition, and Consumers Act would undermine user privacy and security and hinder our ability to make the kind of technology that sets Apple apart.” The euro could have further to fall once the financial markets fully price in Donald Trump’s upcoming second presidential term, argues George Saravelos of Deutsche Bank. He told clients last night that “Trump is only 30% priced”, and that the euro could fall to parity against the US dollar – from $1.04 today – or lower, once the markets adjust further to the likely net fiscal spending, tariffs and immigration clampdowm. Saravelos says: The bottom line is the market is still not pricing a lot of Trump. We remain bullish on the dollar and would view EUR/USD levels of 1.00 as pricing the intensity of the Trump policy mix at closer to 50%, with potential for even greater downside depending on what happens next year. Here’s a chart showing the details of today’s UK PMI report: National World, the owner of the Scotsman and Yorkshire Post and underbidder in the auction for the Telegraph titles, has received a buyout proposal from its largest shareholder. Media Concierge, the biggest player in the Irish newspaper market with 22 local titles including the Derry News, Limerick Leader and Kilkenny People, has submitted a non-binding proposal valuing one of the UK’s biggest regional and local newspaper groups at £56.2m. The cash offer by Media Concierge, which is controlled by the media tycoon and racehorse owner Malcom Denmark and owns a UK direct marketing business, represents a 40% premium to National World’s closing share price on Thursday. The proposal to take the business private fuels doubt about whether National World will be able to compete for the Telegraph should the preferred bidder, the New York Sun owner Dovid Efune, fails to secure financing before exclusivity expires at the end of the month. More here: The Financial Conduct Authority has hit out at life insurers over “unnecessary delays” in settling claims for bereaved customers, and threatened to take action if the industry fails to improve. The regulator said that while there was evidence that some insurers provide good service to bereaved customers, they need to settle claims quicker and improve how they measure customer experience. It found that on average, firms took between 53 and 122 days to process a claim, from start to finish, for a term insurance policy, within 36 days for group life cover, 20 days for over 50 plans, and 53 days for whole of life. The FCA said it will now be “engaging with industry to collectively improve customer outcomes” and address its findings. It will then do further work to understand what kind of changes have been made, and warned it “will take action if it doesn’t see improvements.” Matt Brewis, director of insurance at the FCA, said: The loss of a loved one can be intensely stressful and we expect firms to offer the right support to help their customers during this difficult time. We expect all life insurers to act on our findings and avoid unnecessary delays with claims. Investors have hiked their bets on another cut to eurozone interest rates before the end of 2024, following the slump in activity at European companies highlighted in today’s PMI report. Money market pricing suggested that investors now price a 50% chance of a 50 basis point rate cut (ie, half a percentage point) at the ECB’s December meeting, up from 20% before the data, according to Reuters. A 25 bps cut (a quarter of one percentage point) is fully discounted. Bank stocks have been hit by the weak PMI data from the UK and the eurozone today. Financial companies are leading the fallers on the FTSE 100 share index in London, with Barclays down 3.1%, Standard Chartered off 2.7% and NatWest losing 2.2%. The pan-European Stoxx 600 Banks Index is down 2%, and hit the lowest since 9 October. Today’s (disappointing) UK PMI data is the first real test of Rachel Reeves’s budget, says Sanjay Raja, chief UK economist at Deutsche Bank, as well as “unfolding geopolitical events” around the world. Raja explains: PMI output indices slipped in November. Notably, the services headline print moved down to a stagnant 50, with the headline manufacturing print slipping further into contraction territory at 48.6. Overall, the composite output index fell into negative territory for the first time since Octover 2023. Underneath the hood, we are seeing stress on hiring plans. Both the manufacturing and services sectors reported falls in hiring plans. And (input) prices – particularly for services – have started to firm – as businesses digest the Budget tax implications. The torrent of bad economic news from the UK, and the eurozone, this morning has hit the pound and the euro. Sterling has hit a new six-month low, dropping below $1.25 against the US dollar this morning as traders reacted to the news that UK private sector output is falling this month, and that retail sales fell in October. That’s a fall of almost a cent today, and the lowest level since mid-May. It has now lost almost 10 cents since the end of September, when one pound was worth $1.34. The euro has slumped to its lowest level against the US dollar since November 2022, after today’s PMI data showed the eurozone private sector is shrinking. It’s down three-quarters of a cent, to $1.04. Kathleen Brooks, research director at XTB, says: It’s been a bad day for economic data this side of the Atlantic. European and UK PMIs fell into contraction territory for November, and UK retail sales for October were much weaker than expected. This does not paint a pretty picture for the European and UK economies in Q4, and contrasts sharply with the outlook for the US, the Atlanta Fed’s GDPNow estimate of Q4 YoY GDP is 2.6%. The budget and Donald Trump’s election win may both have triggered the fall in activity at UK companies last month, says Elias Hilmer, assistant economist at Capital Economics. Hilmer explains that November’s PMI report suggests the UK’s real GDP growth is contracting in the middle of the final quarter of this year. Hilmer told clients: The fall in the Composite PMI suggests that tax hikes announced in the Budget seem to have restrained some private sector activity. Equally so, the prospect of new tariffs imposed by the incoming Trump administration may have weighed on activity too. Indeed, S&amp;amp;P Global said that respondents cited subdued consumer demand as well a worsening domestic and geopolitical uncertainty as a constraint to activity. Overall, November’s PMI points to GDP falling by 0.2% 3m/3m in the middle of Q4. S&amp;amp;P Global’s Chris Williamson adds that this morning’s PMI report suggests the economy could be contracting, saying: “The November PMI is indicative of the economy slipping into a modest decline, with GDP dropping at a 0.1% quarterly rate, but the loss of confidence hints at worse to come – including further job losses –unless sentiment revives. Newsflash: UK business output is contracting this month for the first time in over a year, as the tax increases announced in last month’s budget hit companies. Data firm S&amp;amp;P Global says British firms are giving “a clear thumbs down” to the measures in Rachel Reeves’s first budget, such as the increase in employers’ national insurance contributions. Its flash UK PMI Composite Output Index, which tracks activity across the UK economy, has dropped to a 13-month low of 49.9 this month, down from October’s 51.8. That shows a marginal contraction (50 points = stagnation), but is at least better than in the eurozone (see earlier post). UK companies reported that new order growth fell to its lowest for one year amid “widespread reports of fragile business confidence”. UK retailers warned this week that the budget would drive up their costs, and lead them to cut staff – today’s PMI report has found that service providers “overwhelmingly” linked weaker optimism to forthcoming increases in payroll costs. Chris Williamson, chief business economist at S&amp;amp;P Global Market Intelligence says: “The first survey on the health of the economy after the Budget makes for gloomy reading. Businesses have reported falling output for the first time in just over a year while employment has now been cut for two consecutive months. Although only marginal, the downturns in output and hiring represent marked contrasts to the robust growth rates seen back in the summer and are accompanied by deepening concern about prospects for the year ahead. Business optimism has slumped sharply since the General Election, dropping further in November to hit the lowest since late 2022. Companies are giving a clear ‘thumbs down’ to the policies announced in the Budget, especially the planned increase in employers’ National Insurance contributions. Newsflash: The eurozone’s private sector is shrinking this month at the fastest pace since January, as companies struggle to secure new orders amid political instability. A new survey of decision makers at companies across Europe has found that activity in the service sector decreased for the first time in ten months, while the downturn in manufacturing deepened. The eurozone’s two largest countries are having a dire month: German business activity fell at the quickest rate for nine months, while the French economy is shrinking at the fastest pace since January. Data firm S&amp;amp;P Global, which compiles the poll of purchasing managers, reports that confidence in the outlook for output has dropped to the lowest for just over a year. New orders at eurozone companies fell for the sixth month running, leading firms to cut back workforce numbers as they ran down their backlog of work. Its HCOB Flash Eurozone Composite PMI Output Index has fallen to 48.1 for November, down from 50.0 in October, with any reading below 50 showing a contraction. That’s the lowest reading since January. “Things could hardly have turned out much worse,” says Dr Cyrus de la Rubia, chief economist at Hamburg Commercial Bank, adding: The eurozone’s manufacturing sector is sinking deeper into recession, and now the services sector is starting to struggle after two months of marginal growth. It is no surprise really, given the political mess in the biggest eurozone economies lately – France’s government is on shaky ground, and Germany’s heading for early elections. Throw in the election of Donald Trump as US president, and it is no wonder the economy is facing challenges. Businesses are just navigating by sight. Campaign group Fuel Poverty Action has warned that thousands of people will die because they cannot afford to keep warm this winter. Following the news that the UK energy price cap will rise in January, Jonathan Bean, spokesperson for Fuel Poverty Action, says the most vulnerable households are suffering under the current system: “Millions of us are freezing today in cold damp homes, as energy prices remain 65% inflated and 2.5 million low-income pensioners lose heating support. Many will end up in hospital, and thousands will die. “Ofgem pricing punishes the most vulnerable, with four times higher pricing for those with only electric heating, and cruel standing charges. Energy firms exploit the millions stuck with only storage heaters, whilst giving the cheap energy tariffs to affluent households with electric vehicles. “The Labour government needs to fix our cruel and dangerous pricing system, which is harming millions of us whilst gifting energy firms billions in profits The great and the good of women in finance were invited to Number 11 Downing Street last night in a bid to improve the “measly increase” in women in top jobs. The chancellor, Rachel Reeves, convened prominent City women in a bid to reinvigorate the Women in Finance charter, first launched in 2016. The signatories agree to drive up the proportion of women in senior roles towards parity with their male counterparts as soon as possible. With the present rate of progress this will not be achieved until 2038, with women currently in just a third of the top jobs, a source of frustration for the high flyers in the room as they traded tales over tea and sandwiches. Reeves said: “At the moment, it will still take another 14 years until we have an equal number of women and men on the leadership team in financial services. And I hope that whoever is standing here in 14 years can say it didn’t take 14 years.” “Diversity in boardrooms is not a tick-box exercise. It’s an economic imperative.” Dame Amanda Blanc, chief executive of Aviva, called for figures across the sector to redouble their efforts, otherwise, the industry was telling its talented women “they’re not worth helping”, with “painfully slow” progress. The single percentage point annual increase in female representation at the top was “measly” she said, adding she was eager to help others improve their efforts: Blanc says: “We hit our target at Aviva and that’s not showing off and we did it by applying the same discipline that we do to our financial targets of profit of sales...It can be done, but it takes a lot to do that.” Cryptocurrency prices are rallying today after America’s top financial regulator announced his resignation. Securities and Exchange Commission chair Gary Gensler will resign on 20 January, the SEC announced last night, the day when Donald Trump will be inaugurated as US president. Gensler has been a critic of the crypto industry during his stint at the SEC, calling it a “wild west” riddled with fraud and investor risk back in 2021. It’s likely that his replacement will be more friendly to the sector, given Trump has pledged to make the US “the crypto capital of the planet“. Bitcoin has extended its rally, hitting $99,500 for the first time this morning. Ether is up over 7% in the last 24 hours, while ‘meme coin’ doge is up 2%. According to Coindesk, the total market capitalisation of crypto coins is now a record $3.4tn, having added 4.5% in the past 24 hours. Over in Spain, the Consumer Rights Ministry has upheld fines imposed on budget airlines for policies such as passengers extra for cabin luggage. Ryanair, easyJet, Vueling, Norwegian and Volotea have been fined €179m (£150m), with the ministry dismissing appeals from the company’s after penalties were announced in May. Reuters has the details: The fine set on Ryanair was the highest at €108m, while IAG’s low cost unit Vueling was fined €39m, easyJet €29m, Norwegian €1.6m and Volotea €1.2m. The pound has dropped to a six-month low against the US dollar, after this morning’s weaker-than-expected retail sales report. Sterling fell as low as $1.255, its weakest level since 14 May, extending recent losses as economic worries have risen. The dollar has also been strengthening since Donald Trump won this month’s US election; traders believe his policies to deport undocumented immigrants and impose trade tariffs would be inflationary, leading to higher US interest rates. The 0.7% drop in retail sales across Britain last month are the latest sign that the economy is losing momentum. A Reuters poll of economists had forecast a monthly fall of 0.3% in sales volumes from September. The 0.7% drop was the sharpest since June when sales fell by 1.0% month-on-month. Retail sales across Britain have dropped, as uncertainty before last month’s budget hit consumers. The Office for National Statistics has reported that retail sales volumes fell by 0.7% in October, ending a three-month run of growth. The decline was driven by a decline in demand at “non-food stores” such as clothing outlets, where sales fell by 3.1%. The ONS says that “retailers reported that Budget uncertainty affected sales”. The drop in clothing sales followed growth in previous months, as shoppers had taken advantage of end of season sales. ONS senior statistician Hannah Finselbach said: “Retail sales fell back in October following three months of growth. The fall was driven by a notably poor month for clothing stores, but retailers across the board reported consumers held back on spending ahead of the Budget. “However, when we look at the wider trend, retail sales are increasing across the three month and annual periods, although they remain below pre-pandemic levels.” A Labour Party spokesperson has blame the previous government for the rise in energy bills inked in for January, saying: “The Conservatives trashed Britain’s energy security by leaving us exposed to global shocks and working people are still paying the price. From banning onshore wind to failing to deliver new nuclear, their reckless decisions sent bills soaring. “Labour is fixing the mess the Conservatives created, with our clean energy mission that will protect consumers and boost our energy security.” We should remember, though, that former PM Liz Truss freeze energy bills at an average of £2,500 a year two years ago. That protected households from even higher bills, as the Ofgem cap (which was trumped by the ‘Truss cap’) actually rose over £4,000 per year in early 2023. Citizens Advice fears that households with children and those on lower incomes will struggle to keep warm this winter: Alex Belsham-Harris, head of energy policy at Citizens Advice says: “Energy prices remaining relatively stable over winter will offer cold comfort to millions across the country already struggling to afford bills. It comes as people are falling further and further behind on their energy bills, with the amount owed to suppliers now a record £3.7 billion. “As colder weather sets in, we’re particularly worried about households with children and those on lower incomes, who are most likely to struggle with their heating costs. “Without government action, millions are at risk of being left in the cold this winter and beyond. We’re calling for the urgent introduction of energy bill support that is targeted at people who need it most.” As temperatures across Britain plummet, a fourth winter of the energy bills now crisis looms large in people’s minds, says Simon Francis, coordinator of the End Fuel Poverty Coalition. Francis says it is “vital” that ministers bring in more support for vulnerable households, explaining: “The decision to introduce a price cap change in the middle of winter was taken by Ofgem in 2022 and was described as an inhumane policy at the time. No wonder it has been opposed by campaigners ever since as households will have to find more money to keep themselves warm at the worst possible time. “Already the average household will have paid over £2,500 extra for their energy than had we not been so exposed to volatile energy markets. “To make matters worse, the new Government has cut back the levels of support available to some of the most at-risk elderly households. “While we welcome the Government’s long term plans to boost home energy efficiency to bring down bills and to improve energy security by stabilising prices, these reforms will take time to take effect and will be no comfort to those struggling this winter. “That’s why it is so vital the ministers bring in more support for vulnerable households this winter and speed up plans to bring in a social tariff for next winter - a move that is backed by the vast majority of voters.” National Energy Action chief executive Adam Scorer is calling on the government to take steps now to help strugging households with their energy bills. Following this morning’s news that the price cap will rise in January-March, by 1.2%, Scorer says: ‘Today’s news that the price cap is rising by 1% will impact millions of vulnerable households. Bills are around 50% higher than pre crisis levels. ‘With temperatures now plunging and far less support available many are getting deeper into debt trying to keep warm. Now we know there will be no let up into January and beyond. Targeted government support is essential to save millions from the misery and danger of a cold home.’ On Wednesday, we reported that energy suppliers will spend £500m helping customers with their energy bills this winter, in a deal brokered by the government. But the government has also removed the winter fuel payment for millions of pensioners, which is expected to push 100,000 pensioners in England and Wales into relative fuel poverty. Newsflash: Energy regulator Ofgem has announced that the price cap on British gas and electricity costs will rise next year, as feared. The average annual energy bill in England, Scotland and Wales will rise to £1,738 per year from January, putting more pressure on household finances – at a time when cold weather drives up demand for energy. That will push up the average annual cost of energy by £21, or by £1.75 per month, for the January-March quarter. Tim Jarvis, director general of markets at Ofgem, says: “While today’s change means the cap has remained relatively stable, we understand that the cost of energy remains a challenge for too many households. However, with more tariffs coming into the market, there are ways for customers to bring their bill down so please shop around and look at all the options. “Our reliance on volatile international markets - which are affected by factors such as events in Russia and the Middle East – means the cost of energy will continue to fluctuate. So it’s more important than ever to stay focused on building a renewable, home-grown energy system to bring costs down and give households stability. “In the short term though, anyone struggling with bills should speak to their supplier to make sure they’re getting the help they need and look around to make sure they’re on the best, most affordable deal for them.” As explained in the introduction, the cap applies to the unit cost of energy (there’s no limit on high an individual bill can rise). The increase for the January-to-April cap comes on top of a 10% rise for the period between October and December, when it was £1,717 a year. For comparison, prices will still be around a third higher than three years earlier. In October 2021, the cap was set at £1,277 per year. Charities are concerned about the impact another rise in energy prices will have. David Southgate, policy manager at disability equality charity Scope, says: “This is a bitter pill to swallow for the many disabled people who face sky-high bills because they have no choice but to use more energy. Life costs a lot more when you’re disabled, because of needing to use more heating to stay warm and healthy, or charging vital equipment like wheelchairs and breathing machines. Our disability energy support services are hearing from disabled people who have cut back everything they can and racked up huge amounts of debt. The Government urgently needs to step in and bring in discounted energy bills for disabled people.” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Britain’s long-running cost of living squeeze may tighten this morning, when households across the country learn whether average energy bills will rise, or fall, in January. Regulator Ofgem is due to announce how Britain’s price cap will change in January-March at 7am today, and analysts fear the cap will rise slightly. The cap sets the maximum that suppliers can charge their 29 million household customers per unit of gas and electricity. It is calculated based on the wholesale price of energy, which are still above historic averages despite dropping back from the highs seen shortly after Russia’s full-scale invasion of Ukraine in 20</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>UK business activity shrank for the first time in over a year this month. UK retail sales also took an downturn turn last month, dropping by 0.7%. Weak data hit the pound, which dropped to a six-month low below $1.25.</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Time to recap… Bank of England policymakers have told MPs that they will take a ‘gradual approach’ to cutting interest rates, as they assess the inflationary impact of last month’s budget. BoE governor Andrew Bailey told MPs: “A gradual approach to removing monetary policy restraint will help us to observe how this plays out, along with other risks to the inflation outlook.” MPC member Alan Taylor suggested the Bank could cut rates more rapidly than the market expect, if inflation remains lower than expected, while colleague Catherine Mann argued that rates should have remained on hold this month until there was proof that inflation was beaten. Bailey offered support to UK retailers who fear that increases in national insurance contributions will cost jobs and push up costs. Bailey also warned against “fragmenting” the world economy, given the threat that Donald Trump imposes steep trade tariffs on other countries. Global stock markets have dropped, after Ukraine fired US-made long-range missiles into Russia for the first time since the Biden administration lifted restrictions on their use, drawing a warning from Moscow that it would respond “accordingly”. Here’s the rest of today’s news stories: Over on Wall Street, stocks have opened lower as investors react to rising geopolitical tensions. The Dow Jones industrial average of 30 large US companies has dipped by 0.8%, down 355 points at 43,033, while the broader S&amp;amp;P 500 index is 0.4% lower. Wall Street’s ‘fear index’, the Chicago Board Options Exchange’s CBOE Volatility Index, has jumped almost 10%. Traders have noted that Ukraine has fired US-made long-range missiles into Russia for the first time, drawing a warning from Moscow that it would respond “accordingly”. The missile attack came shortly after Vladimir Putin signed a revised nuclear doctrine which lowers the threshold for using nuclear weapons. Meanwhile in Canada, inflation has risen back to 2% in October. The increase, from 1.6% in September, was due to a pick-up in fuel prices; prices for gasoline were up 0.7% on a monthly basis in October, following a 7.1% decline in September. Professor Costas Milas of the University of Liverpool’s management school argues that the ‘gradualist’ approach to rate cuts has its merits over the ‘activist’ approach advocated by Catherine Mann today. He explains that it’s all a question of the merits of one large rate cut versus several small interest rate cuts, saying: Catherine Mann is actually asking the well-known question: “Is it better to cut by (say) 75 basis points only once rather than making three successive interest rate cuts of 25 basis points each?” The answer is far from clear: A large interest rate cut might actually spook markets as these will surely be thinking: Does the MPC know/worry about something we do not know ourselves and, therefore, have decided to take “radical” action? More, fundamentally, however, BoE’s quantitative models do not currently allow for full assessment of the above question because this type of monetary policy asymmetry is not built in the modelling approach. In the absence of a robust answer to the above essential question, it makes sense to favour a gradualist approach to setting interest rates! Here are the key points from today’s session with top Bank of England officials at the Treasury Committee today. The impact of the measures in last week’s budget will be crucial in determining how quickly UK interest rates fall, MPs have heard. BoE governor Andrew Bailey told the Treasury commmittee that the Bank doesn’t yet know how firms will handle the rise in their national insurance contributions – but it’s likely to involve higher prices, lower wages and some job cuts. Bailey explained that the rise in social security contributions that employers must pay “represents an increase in the cost of employment”, adding: “A gradual approach to removing monetary policy restraint will help us to observe how this plays out, along with other risks to the inflation outlook.” Bailey also said UK retailers were right to warn that the NICs increases will lead to job cuts, warning: “I think there is a risk here that the reduction in employment could be more. Yes, I think that’s a risk.” He then explained that the budget could either be inflationary, if firms push up prices, or deflationary, if they make lower wage rises and increase job cuts. Bailey, deputy governor Clare Lombardelli and new MPC member Alan Taylor all said recent progress in disinflation had encouraged them to cut interest rates this month. But… fellow policymaker Catherine Mann disagreed; she favours holding rates until there are clear signs that inflationary pressures have been squeezed, followed by hefty rate cuts afterwards. Mann also said Rachel Reeves’s budget had deterred her from leaning towards a rate cut this month, due to its inflationary impact. MPs pressed the BoE about what its policy of ‘gradual’ rate cuts would mean in practice. Taylor said the markets are forecasting four quarter-point rate cuts in the next year, but that the Bank could cut faster than expected if developments on inflation remain positive. Bailey was also quizzed about the dangers of Donald Trump launching a new trade war. He said we need to see what the US actually does, adding: Fragmenting the world economy is not a good thing, quite clearly. Bailey also said the UK should engage in “active dialogue” about trade with both the Trump administration and Brussels, adding: I find it hard to understand people who seem to say we should implement Brexit in the most hostile fashion possible. The world’s biggest pharmaceutical companies have failed to increase access to life-saving medicines in poorer countries, which can result in illness or death for billions of people that could be avoided, according to a new report. Industry performance has fallen in the past two years, according to the latest ranking of the world’s top 20 pharmaceutical companies from the Netherlands-based, non-profit Access to Medicine foundation, which is funded by the UK and Dutch governments and the Bill &amp;amp; Melinda Gates Foundation. Only 43% of clinical trials take place in the 113 low and middle income countries covered by the analysis, even though they are home to 80% of the global population; as companies typically prioritise access planning in countries where they conduct trials, this leaves much of the world behind. Just 3.5% of trials – where new medicines are tested on volunteers – are conducted in the poorest countries. Examples include Californian firm Gilead’s clinical trials in Uganda for lenacapavir, a long-acting injectable for HIV prevention, and trials by Germany’s Merck and Switzerland’s Novartis in low-income countries for new antimalarials. Jay Iyer, the foundation’s chief executive, said: “Companies have very clearly said we will register and prioritise registration in countries where the trials are running, but if they don’t run the trials in more areas,… then you’re never going to solve this health equity problem for all the innovative new products.” Only three new non-exclusive voluntary drug licences have been issued, compared with six in the 2022 report, signalling a missed opportunity to improve local availability of new medicines. Voluntary licenses enable generic drugmakers to make cheaper copies of patented medicines. The new voluntary licences include GSK’s long-acting HIV treatment cabotegravir, along with a Novartis drug for chronic myeloid leukaemia, and Gilead’s agreements with six generic manufacturers to produce and sell lenacapavir, for HIV prevention. The Access to Medicine foundation hailed these licences as “promising milestones”. British drugmaker GSK, which has been top of the Access to Medicine index since it was first compiled in 2008, has lost the top spot to Novartis, while AstraZeneca, Britain’s biggest pharmaceutical firm, slipped from third to fifth place. France’s Sanofi and New York-based Pfizer were in third and fourth place respectively. GSK said it is committed to investing £1bn over next 10 years on global health research &amp;amp; development to tackle infectious diseases, such as tuberculosis and malaria, and that it is one of the largest suppliers of of vaccines of the vaccine alliance GAVI, with 1.2bn vaccines supplied since 2010. Emma Walmsley, the GSK chief executive, said: “As the report makes clear, partnership with governments, multilateral organisations and others is critical to making progress here. We are committed to achieving health impact at scale as a growing, successful business, positively impacting the health of 2.5 billion people by the end of the decade, including more than 1.3 billion people in lower-income countries.” AstraZeneca’s drop in the ranking partly reflects its focus on getting its Covid vaccine to over 180 countries at no profit pricing, which impacted on other drug programmes. The research does not include rare diseases which is a large part of the firm’s portfolio. The research will be launched by Goldman Sachs and the investment firm AllianceBernstein at investor events in London and New York today. David Reddy, director general of the International Federation of Pharmaceutical Manufacturers &amp;amp; Associations, said: “The Access to Medicine Index highlights important industry progress, such as tiered pricing models, inclusive business strategies, and voluntary licensing agreements. These efforts demonstrate the value of partnerships with governments, healthcare systems, and local organizations to improve access.” “Despite these strides, the report underscores the need for accelerated efforts to close persistent gaps in access, particularly in low-income countries. To achieve sustainable impact, stronger collaboration among companies, governments, and global health stakeholders remains essential.” Finally, the Treasury Committee turned to the speed at which commercial banks are passing on changes to interest rates. Andrew Bailey says the Bank does expect passthrough to happen. When rates were going up, he says, the passthrough was faster on fixed-term deposits than on sight deposits (where there is very little, or no, delay to accessing money). It’s too early to assess this month’s cut in rates, Bailey says. But if you look at the August rate cut, about half of that cut has fed through to sight deposits – so savers are still getting the other half – while more of the cut has reached fixed-term deposit rates. Mortgages tend to be priced off the swap curvey, Bailey reminds MPs, rather than off Bank rate. Q: So you’re not worried about passthrough rates? Bailey doesn’t really say whether he’s worried or not, simply that the Bank “monitor it very carefully”. That’s the end of the session. Q: What needs to happen to fix the UK’s labour force statistics? The Bank of England is helping the Office for National Statistics try to fix its jobs data, Andrew Bailey says. The key is to get the participation rate of the ONS’s surveys up, but it’s not clear how long it will take to happen. The committee then have a long discussion of the UK’s labour force inactivity – the number of people who have droopped out of the jobs market and not returned. The Bank’s problem is that the official labour force data does not give a clear picture of what’s happening; the extent to which it’s because people can’t work due to long-term sickness, or mental health issues among young people, or because older people have taken early retirement on generous pensions, and won’t return to work. Hawkish policymaker Catherine Mann declares that she does not support the Bank of England’s policy of taking a ‘gradual’ approach to cutting interest rates. Even though she was the only MPC member to vote to hold, rather than cut, rates this month, Mann insists she takes the view that “a more activist strategy is superior”. Mann argues that monetary policy is currently less restritive than you might think, as the ‘neutral level’ of interest rates is probably much higher than is incorporated in the Bank’s models. Mann insists that she isn’t going to vote to hold rates “forever”, pledging: When I do cut, it will be more aggressive. That point will be reached when Mann has seen signals in the data that a larger cut is needed, she says, as firms would react immediately to a large cut in rates. [however, the MPC may have moved ahead of her, though its gradual approach….] She also argues that a large cut sends a clearer signal to the economy, and “cuts through the noise” of financial market behaviour. Q: Why does the Bank forecast that the government will raise fuel duty in future years, when ministers continually keep freezing it? Andrew Bailey says the Bank bases its decisions on announced government policy – it can’t start forecating what policy might be. John Glen MP returns to the impact of last month’s budget, on inflation, interest rates and growth. Q: What assumptions have the Bank made about the ‘growing out’ impact, is it different than the OBRs? Clare Lombardelli says the ‘big picture’ of the two assessments are broadly the same. But they do have slightly different figures, because of uncertainty over how the impact of budget measures will land. Andrew Bailey says the Bank doesn’t forecast interest rates, but he notes that the market priced in one fewer quarter-point rate cut after the budget was delivered, which basically matched the OBR’s prediction. Onto the sticky issue of quantitative tightening (unwinding the Bank’s QE programme by selling off bonds it bought in recent crises). Q: How much interest will The Treasury pay out to commercial banks in this parliament on their cash deposits built up through these stimulus measures? Bailey won’t give a figure. But he says the Bank did hand £124bn to the Treasury in the QE phase, when interest rates were very low. The flow is now happening the other way, as the Bank is now paying more interest on commercial bank reserves. But only £54bn has been paid out so far, meaning the Bank is still up £70bn Bailey then explains that other central banks handle it differently. They are allowed to hang onto the interest they receive from lending money, or on assets they hold, which can be used to cover these costs. Due to an act passed in 1844 by Sir Robert Peel, the Bank of England has to hand over that “seniorage” immediately. That means the situation looks different in the UK, he adds. Q: Has the Bank done any analysis of the impact of potentially using $300bn of frozen Russian assets to reconstruct Ukraine? Governor Bailey says very little of those frozen funds are in the UK. The issue has been discussed a lot at G7 meetings, he reveals. Q: Vietman and Germany were major beneficiaries from the US trade war with China in the first Trump administration. Could the UK have a similar opportunity if we see a EU-US trade war? Alan Taylor says it’s well understood in trade theory that interventions in trade policy cause trade diversion. The country imposing tariffs sees its imports fall, but ‘water finds its level’ and those goods will end up elsewhere, he suggests. Q: What impact would new US tariffs would it have on the UK’s relationship with Europe – last week, you warned that Brexit had undermined our economy? Bailey says the Bank will be very transparent in its analysis, and share it with the committee. On Brexit, he says the UK should look to trade freely with all parts of the world, and in an “active dialogue” with both the US about its plans, and Europe. Bailey says a lot of effort has gone into maintaining open relations with Europe, as they have to trust the UK with financial services. Bailey adds that he doesn’t take a position on Brexit, but it’s his job to deal with it, adding: I find it hard to understand people who seem to say we should implement Brexit in the most hostile fashion possible. Q: But the new US president may see this as a binary choice – with the UK choosing between allying with Washington or Brussels. When does that moment crystallise? Bailey says that moment can only come once we know what Donald Trump’s trade policies are. Conservative MP John Glen turns to events across the Atlantic. Q: What impact will Donald Trump’s policy on tariffs have on the UK economy? Credible sources say it could knock 0.8% off UK GDP, and hurt exports from the UK into the US? Andrew Bailey says the Bank wasn’t able to incorporate the impact of the US election into its forecasts, as the result came in on the day it was setting UK interest rates. It’s very important to wait and see what the administration does, rather than simply says, Bailey explains, adding: US elections don’t quite have the same tightness of tie to the manifesto than UK elections do. We would need to know a lot of other things, not just what new tariffs the US deploys but what how other countries respond, and what the impact on exchange rates is. Bailey says: Fragmenting the world economy is not a good thing, quite clearly. But the precise effect of particular tariffs, especially if there are different levels set for different countries, is hard to predict – also as the UK has a more services-dominated economy. Incidentally, unions do not share the Bank of England governor’s support for UK retailers unhappy about paying a higher minimum wage and more national insurance contributions. The GMB Union has described big retailers warning they will have to slash jobs if forced to pay a bit more tax as ‘utterly pathetic.’ Nadine Houghton, GMB National Officer, says: “Multi billion pound businesses pleading poverty because they’re being made to pay more to support public services is utterly pathetic. “Most of these companies’ fortunes are already subsidised by the tax payer - they pay very low wages which then have to be topped up by in work benefits. “And some - for example Asda - have been systematically trousering fortunes made by underpaying women workers. “It’s only right that they should now contribute a bit more to rebuilding our country.” On the other hand, if firms passed on the impact of the budget entirely in higher prices, it would push inflation up by more. The Bank’s latest forecasts, released two weeks ago, suggested the budget would raise inflation by half a percentage point at its peak (but that was based on the impact being split across prices, profit margins, workforce levels and wages). MPC member Catherine Mann says it all depends on the underlying demand conditions (ie, if demand is high, you can get away with price rises, but if sales are strugging, then not). Q: Your latest forecasts show a 40% chance that inflation rises to 3% – would that be a failure? Andrew Bailey points out that the Bank’s forecasts also show inflation at target at the end of its forecast horizon. That’s why the Bank is taking a ‘gradual approach’ to lowering rates, the governor explains. He tells the Treasury Committee at today’s hearing: The evidence we’ve seen recently is that the outturns have been lower than we thought they would be, but we don’t know if that’s going to continue. We’ll see. Q: Does your model show how many jobs will be lost due to the rise in employers’ national insurance rates? Bailey says the Bank has not made a calculation. He says the Office for Budget Responsibility’s forecast of 50,000 job cuts is based on ‘pretty similar assumptions’ to the Bank as to how the NICs changes will be passed through the various channels. (prices, wages, profit warnings or job cuts). And he says UK retailers are right to warn that the NICs changes will lead to jobs cuts, as they did in a letter organised by the British Retail Consortium this morning (see opening post). Bailey says: I saw the BRC’s letter. I think they’re right to say… I think there is a risk here that the reduction in employment could be more. I think that’s a risk. Governor Andrew Bailey also explains that Budget measures such as the increase in employers’ national insurance contributions could actually be deflationary – allowing faster cuts to interest rates. It all depends how firms handle the increase – do they raise prices, or cut wages? As Bailey tells the Treasury committee: You could get higher inflation, but you could get quite a weakening of the labour market, and downside pressure on pay. MPC member Alan Taylor says UK households are being cautious about spending their savings, following the Covid-19 pandemic, which is weighing on the economy. Taylor explains that we saw a similar phenomenen after the Great Depression of the 1930s (he remember his parents explaining how their approach to money changed at that time.). Taylor, who is based in New York, adds that he’s planning to visit the UK regularly to assess the situation – he’s already visited Scotland, and has trips to Leeds and Bristol lined up in early 2025. Labour MP Lola McEvoy takes the Bank of England onto mortgages…. Q: We’ve seen mortgage rates go up, since you cut interest rates earlier this month. That’s a blow to hard-working households trying to get by – did you expect it, and why did it happen? BoE governor Andrew Bailey points out that mortgages rates have fallen since August, when the Bank made its first cut to interest rates in this cycle. He points out that most UK mortgages are fixed-rate, and priced off the ‘swap curve’ (which measures where the markets expect interest rates to be in future). Bailey concedes that the curve has risen, due to ‘event risk’ – namely the reaction to the UK budget at the end of October, and the US presidential election this month. He says it’s not unusual for the UK swap curve to be influenced by the US curve, and points out that they’re both down today*. * – due to worries of escalating tensions in Russia-Ukraine, as covered earlier. Andrew Bailey then offers a supportive arm to the hawkish Catherine Mann, saying he agrees with many of the points she just made (even though the pair disagreed on this month’s interest rate decision). He says the Bank has not decided how the increase in employment costs will feed through – it could mean higher prices, lower pay rises, lower headcounts, or improved productivity (although the latter takes a while to feed through…) Q: What market conditions would be needed to go faster than traders expect? Clare Lombardelli says the key is conditions in the economy. That includes levels of demand and potential supply in the economy, what that means for firms’ ability to raise prices, and how cost pressures play out. Plus, the supply side of the labour market – and how close the jobs market is to full capacity. Expectations for next year for price rises, especially in the services sector, are also important. Q: What does the Bank mean when it talks about taking a ‘gradual’ approach to rates – how quickly might they fall? Monetary policy committee member Alan Taylor says this is the question on everyone’s mind, and the word ‘gradual’ means different things to different people. Taylor suggests that some in the markets believe ‘gradual’ means a cut at every other Bank of England meeting, while ‘aggressive’ would mean a cut at every meeting. But, he points out, the Bank has eight meetings per year, and makes a decision each time. His view is that the key is the labour market, warning: We don’t necessarily have the best statistics there. [the Office for National Statistics has been struggling for months to get accurate data on the jobs market] Right now, the ‘gradual’ pledge is aligned closely with market expectations of about one percentage point of cuts this year, Taylor explains. But that doesn’t mean that’s what will unfold. Taylor says: If conditions are weaker, and my own view is skewed to the downside risks now versus the upside risk of a year ago, then we could go faster. BoE policymaker Catherine Mann adds that the measures in Rachel Reeves’s budget encouraged her to vote– alone - to hold interest rates at 5% this month. Mann says she concluded that the budget was “front-loaded”, meaning it lifted demand in the near term, and also “geographically dispersed” across the country. That could allow firms to push through the price rises they are planning, she says. [Reminder: the MPC voted 8-1 to cut rates on 7 November] Q: What impact did the increase in the national minimum wage, and employers’ national insurance contributions, in the budget have on your vote? Mann says the firms were already struggling to incorporate previous increases in minimum wage rates, which have squeezed the differential in wages across their businesses. A higher-than-inflation increase in the living wage next April will add to those pressures, she argues. Mann adds that companies can pass the NIC increase on through higher prices, or lower wages, or by cutting their workforce, or invest in raising productivity. These are upside risks to inflation, she argues, so the Bank should have waited to see what happens…. Labour MP Dame Meg Hillier, who chairs the Treasury committee, begins today’s session by asking the Bank of England about this month’s decision to cut interest rates, from 5% to 4.75%. Q: What tipped the balance on your decision? Governor Andrew Bailey says he voted to cut borrowing costs due to the “pace and progress on disinflation”, which has been faster than expected – with inflation dropping below target to 1.7% in September. Bailey says the Bank also flagged that it emphasises the word ‘gradual’ when looking forwards, due to the various risks to inflation. Deputy governor Clare Lombardelli says the dominating factor for her vote to cut rates was the drop in inflation, and the fall in services inflation, and in wage settlements. Taken together, that suggests the drivers of inflation were less strong than in the past. But, Lombardelli warns, there are “risks on both sides” on the inflation outlook. Professor Alan Taylor says he’s “broadly in agreement” with Bailey and Lombardelli. Taylor says that historical patterns show that energy shocks feed into some sectors quickly – such as goods and foods – but arrive later in other sectors. What’s happening in the UK isn’t abnormal, Taylor says, but there is still the possibility that inflation beomes embedded. But as inflation has been lower than forecast, that gave “reassurance” that it was OK to make a second cut to interest rates. Catherine Mann, who opposed the rate cut, says she looks at the data in a slightly different way. She points out that recent earnings growth was higher than the Bank had forecast back in August, and that wage settlements are running higher than is compatible with hitting the Bank’s 2% inflation target. Forward-looking measures of future prices and wages have been over target for the last four months, and haven’t fallen, Mann adds – that’s a sign that inflationary expectations may be higher than the Bank would like. Over in Westminster, top officials from the Bank of England are appearing before the Treasury Committee. Governor Andrew Bailey is in the hot seat, flanked by the new boy on the Monetary Policy Committee, Alan Taylor, plus deputy governor Clare Lombardelli, and Catherine Mann. Mann is the most hawkish member of the monetary policy committee – the only one to oppose this month’s cut in UK interest rates, to 4.75%. The committee point out that this is their first session with the Bank since the July general election (s well as last month’s budget). They say: MPs are likely to ask witnesses about the current economic picture and how it affects the Bank’s interest rate decisions, particularly in relation to the measures announced in the Chancellor’s 2024 Autumn Budget. MPs may also choose to probe the Bank’s plans for unwinding its QE portfolio and the most recent pay and jobs figures, including the continued issues with the reliability of official data. A shiver of fear just rippled through the financial markets, after Vladimir Putin approved an updated Russian nuclear doctrine today. Kremlin spokesperson Dmitry Peskov has said the use of western non-nuclear missiles by the Ukrainian armed forces against the Russian Federation under the new doctrine could lead to a nuclear response. The warning came after US president Joe Biden gave approval for Ukraine to strike targets within Russia with US-supplied long-range missiles. And there are reports that Ukrainian armed forces have carried out their first strike in a border region within Russian territory with a ATACMS missile, according to news agency RBC Ukraine. This has triggered a flight to safety, with investors piling into the US dollar, the Swiss franc and the Japanese yen. The British pound is down half a cent against the dollar, at $1.262. US and European bond prices are also jumping, pushing down government borrowing costs. But Ukraine’s bonds are falling, having rallied earlier this month on hopes that Donald Trump might end the war with Russia. Equities are dropping, with the FTSE 100 share index down 40 points or 0.5% at 8067 points, with bank stocks among the fallers. And the Euro stoxx volatility index – a measure of fear in the markets – is up 1.3 points to 19.1 points. Rachel Reeves is feeling pressure from farmers, as well as retailers, over the tax changes in last month’s budget. Thousands of farmers are descending on central London this morning, arguing that changes to inheritance tax rules will destroy family farms. The government, though, says it will make no difference to food security. My colleague Joanna Partridge is attending an event organied by the National Farmers Union, where emotions are running high, and reports: Our Politics Live blog is tracking all the developments: Developments in think tank circles…. The Resolution Foundation has appointed a new chief executive, from the Treasury. Ruth Curtice, currently director of fiscal policy at HM Treasury (HMT), has been appointed to succeed Torsten Bell (who has effectively moved the other way, to Westminster, having become an MP in July). Curtice says: “I am excited to be leading the Resolution Foundation into the next phase of its valuable work. I have seen at first hand the impact its excellent analysis has had on policy in the UK. I look forward to furthering its mission to improve the living standards of low-to-middle income households.” This is a pretty significant role, given Resolution’s focus on improving the living standards for those on low to middle incomes – at a time when the Labour government are under fire for raising taxes to fund better public services. Staff have resigned at Starling Bank after its new chief executive demanded thousands of workers attend its offices more regularly, despite lacking enough space to host them. In his first major policy change since taking over from the UK digital bank’s founder, Anne Boden, in March, Raman Bhatia has ordered all hybrid staff – many of whom were in the office only one or two days a week, or on an ad-hoc basis – to travel to work for a minimum of 10 days each month. But the bank, which operates online only, admitted that some of its offices would not be equipped to handle the influx. An email sent by Starling’s human resources team and seen by the Guardian said: “We are aware that in some office locations we may not be able to accommodate 10 office working days per month for everyone right now. We are considering ways in which we can create more space,” Starling has 3,231 staff, the vast majority of whom are in the UK with some also in Dublin. However, the Guardian understands that the bank has only about 900 desks, including 260 at its Cardiff site, 320 in its London headquarters and 155 in Southampton. More here: Small investors are gloomier about the prospects for the UK stock market, according to financial services company Hargreaves Landsown. The latest HL Investor Confidence Index, released this morning, has found that confidence in UK equities has decreased 11% month on month, while confidence in UK economic growth has also decreased by 13 points. Emma Wall, head of platform investments at Hargreaves Lansdown, says that the London market have been hit by two headwinds: a UK Budget deemed by the market as potentially inflationary, and Donald Trump’s election victory, which pushed up shares but hurt bond prices. Conviction in European stocks (down 4%) and Japanese stocks (down 10%) has also fallen this month, but investors are more confident in Asia Pacific (up 8%), Global Emerging (up 7%) and North American equities (up 5%). Bloomberg have a corking exclusive: they’ve heard that antitrust officials at the US Department of Justice have decided to ask a judge to force Alphabet’s Google to sell off its Chrome browser. They say: The department will ask the judge, who ruled in August that Google illegally monopolized the search market, to req</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>BoE governor Andrew Bailey told MPs: ‘A gradual approach to removing monetary policy restraint will help us to observe how this plays out’ MPC member Alan Taylor suggested the Bank could cut rates more rapidly than the market expect, if inflation remains lower than expected. Catherine Mann argued that rates should have remained on hold this month until there was proof that inflation was beaten.</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Spirit Airlines said on Monday that it had filed for bankruptcy protection and would attempt to reboot as it struggles to recover from the pandemic-caused decrease in travel and a failed attempt to sell the airline to JetBlue. Spirit, the biggest US budget airline, has lost more than $2.5bn since the start of 2020 and faces looming debt payments totaling more than $1bn over the next year. Spirit said it expected to operate as normal as it works its way through a prearranged Chapter 11 bankruptcy process and that customers could continue to book and fly without interruption. All existing tickets, credits and loyalty points can be used as normal. The bankruptcy will not affect employee wages or benefits. The company said in a statement that it had $300m in financing from bondholders that, along with the company’s cash reserves and revenue, was expected to keep the company running during the bankruptcy process. Shares of the Miramar, Florida-based Spirit dropped 25% on Friday, after the Wall Street Journal reported that the airline was discussing terms of a possible bankruptcy filing with its bondholders. It was just the latest in a series of blows that have sent the stock crashing down by 97% since late 2018 – when Spirit was still making money. The airline expected its stock to be delisted from the New York Stock Exchange “in the near term”, the company said in a statement. Ted Christie, Spirit CEO, confirmed in August that the company was talking to advisers of its bondholders about the upcoming debt maturities. He called the discussions a priority, and said the airline was trying to get the best deal it could as quickly as possible. “The chatter in the market about Spirit is notable, but we are not distracted,” he told investors during an earnings call. “We are focused on refinancing our debt, improving our overall liquidity position, deploying our new reimagined product into the market, and growing our loyalty programs.” People are still flying on Spirit Airlines. They are just not paying as much. In the first six months of this year, Spirit passengers flew 2% more than they did in the same period last year. However, they are paying 10% less a mile, and revenue per mile from fares is down nearly 20%, contributing to Spirit’s red ink. It is not a new trend. Spirit failed to return to profitability when the coronavirus pandemic eased and travel rebounded. There are several reasons behind the slump. Spirit’s costs, especially for labor, have risen. The biggest US airlines have snagged some of Spirit’s budget-conscious customers by offering their own brand of bare-bones tickets. And fares for US leisure travel – Spirit’s core business – have sagged because of a glut of new flights. Last month, Spirit announced it would conduct layoffs as part of $80m in cost-saving measures, though it did not specify how many employees would be affected. The company also announced it had agreed to sell 23 airplanes to GA Telesis, an aviation services company, for $519m. The October announcement briefly boosted the stock, before it came down as bankruptcy appeared likely. The airlines also said in October that it planned to furlough about 330 pilots starting 31 January 2025, in addition to the 186 pilots it furloughed in September. The company downgraded 120 captains to first officers at the time. The premium end of the air-travel market has surged while Spirit’s traditional no-frills end has stagnated. So this summer, Spirit decided to sell bundled fares that include a bigger seat, priority boarding, free bags, internet service and snacks and drinks. That is a huge change from Spirit’s longtime strategy of luring customers with rock-bottom fares and forcing them to pay extra for things such as bringing a carry-on bag or ordering a soda. In a highly unusual move, Spirit plans to cut its October-through-December schedule by nearly 20%, compared with the same period last year, which analysts say should help prop up fares. But that will help rivals more than it will boost Spirit. Analysts from Deutsche Bank and Raymond James say that Frontier, JetBlue and Southwest would benefit the most because of their overlap with Spirit on many routes. Spirit has also been plagued by required repairs to Pratt &amp;amp; Whitney engines, which is forcing the airline to ground dozens of its Airbus jets. Spirit has cited the recall as it furloughed pilots. The aircraft fleet is relatively young, which has made Spirit an attractive takeover target. Frontier Airlines tried to merge with Spirit in 2022 but was outbid by JetBlue. However, the justice department sued to block the $3.8bn deal, saying it would drive up prices for Spirit customers who depend on low fares, and a federal judge agreed in January. JetBlue and Spirit dropped their merger two months later. US airline bankruptcies were common in the 1990s and 2000s, as airlines struggled with fierce competition, high labor costs and sudden spikes in the price of jet fuel. PanAm, TWA, Northwest, Continental, United and Delta were swept up. Some liquidated, while others used favorable laws to renegotiate debts such as aircraft leases and keep flying. The last bankruptcy by a major US carrier ended when American Airlines emerged from Chapter 11 protection and simultaneously merged with US Airways in December 2013.</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Spirit has lost more than $2.5bn since the start of 2020 and faces looming debt payments. The company said it had $300m in financing from bondholders that, along with the company’s cash reserves and revenue, was expected to keep the company running.</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Time to recap…. UK consumer confidence has fallen this month, as households report that their current finances continued to deteriorate in November, while pessimism about the financial outlooks for the year ahead has risen. Britain and the United States have signed a new agreement for civil nuclear collaboration at the COP29 summit, that could speed up the development of new technologies. Thames Water has £23bn of assets that are in urgent need of repair and the supply of water to its 16 million customers is “on a knife-edge”, a Guardian investigation has found Sources have also warned that Thames Water’s IT ‘falling apart’ and is being hit by cyber-attacks. Economists at the CEBR have calculated that Donald Trump could wipe 1% off the UK economy by imposing new import tariffs. The rise in UK employment costs is going to hit growth and wages next year, Goldman Sachs have forecast. UK households will also face a 1% rise in energy bills in January, when the price cap is next changed, analysts at Cornwall Insight have calculated. The average asking price on a UK home has dropped by more than £5,000 this month as the autumn budget caused housing market jitters. US budget airline Spirit has filed for bankruptcy protection. Britain and the United States have signed a new agreement to collaborate on civil nuclear technology at the COP29 summit. The agreement, signed by UK Energy Secretary Ed Miliband and US Deputy Secretary of Energy David Turk today, aims to pool billions in research funds and share information on advanced nuclear technologies. The goal is to speed up the development of new technologies, such as advanced modular reactors, to help decarbonise industry and boost energy security. The new agreement will come into force from 1 March 2025. Energy Secretary Ed Miliband says: “Nuclear will play a vital role in our clean energy future. “That is why we are working closely with our allies to unleash the potential of cutting-edge nuclear technology. “Advanced nuclear technology will help decarbonise industry by providing low-carbon heat and power, supporting new jobs and investment here in the UK.” The UK government says the agreement builds on a pledge made last year at COP28 to triple nuclear energy capacity globally by 2050. It expects this new agreement will also be signed by Canada, France, Japan, Republic of Korea, Republic of South Africa, China, Euratom, Switzerland and Australia. You can track the latest action at COP 29 here: The owners of Scotland’s only oil refinery, which is scheduled to close next summer, have reportedly rejected a US-led approach about a possible bid. A consortium said to be led by Robert McKee, an American energy industry veteran, wrote to Petroineos, the owner of the Grangemouth site, to express an interest in buying it, according to Sky News. But the approach has been rejected by Petroineos, which is 50%-owned by Sir Jim Ratcliffe’s petrochemicals empire. The consortium is understood to comprise The Canal Group, which is reportedly developing a green energy refinery in Texas, and Trading Stack, a Middle East-based commodities trader, Sky say. Petroineos is planning to shut Grangemouth by the end of June next year, a move that could cost 500 employees their jobs. Thames Water’s IT systems are in the spotlight again today, with sources telling the Guardian they are so antiquated they have been easy for cybercriminals to attack. My colleague Anna Isaac reports: “The software we use is older than me, and some of the hardware is older than my dad,” says Siddharth*. He is one of a team fighting a daily battle to sustain ancient IT infrastructure at Thames Water. Sometimes the defences are breached. Thames, the UK’s largest water and waste treatment company, is on a “knife-edge” according to sources, with its resilience in doubt because it depends on an array of creaking – often Victorian – infrastructure. While plenty of attention has been paid to its pipes, trunk mains and sewage overflows, less well understood is another big problem: its computer systems. Some IT systems date back to the 1980s, and have long been declared obsolete. More here: *Names have been changed Trading has begun cautiously on Wall Street. The S&amp;amp;P 500 stock index has inched up by 4 points to 5,874, a gain of less than 0.1%, while the tech-focused Nasdaq is 0.2% higher. Tesla are among the top risers, up over 7% following reports that President-elect Donald Trump’s transition team are planning to make a federal framework to regulate self-driving vehicles a top priority for the U.S. Transport Department (see earlier post). Nvidia is a leading faller, down 2.5%, after reports of overheating snags with its Blackwell chip (see earlier post). Top European Central Bank policymakers are concerned that new US tariffs could hurt growth. ECB vice-president Luis de Guindos told an event in Frankfurt that trade tensions could damage Europe’s economy, saying: “The balance of macro-risks has shifted from concerns about high inflation to fears over economic growth. The growth outlook is clouded by uncertainty about economic policies and the geopolitical landscape, both in the euro area and globally. Trade tensions could rise further, increasing the risk of tail events materialising.” Bundesbank president Joachim Nagel is also concerned, telling an event in Tokyo that tariffs promised by Trump would upend international trade. However, Nagel was not too concerned that they could push up inflation, saying: “Global integration would have to decrease substantially to cause a noticeable rise in inflationary pressures. “And, so far, we have not seen this.” Shares in Nvidia are down almost 2% in premarket trading, on reports of an overheating problem with its new Blackwell chips. Website The Information reported yesterday that the Blackwell graphics processing units – designed to be used in artificial intelligence systems – has an overheating problem when connected together in Nvidia’s customised server racks. Nvidia has reportedly asked its suppliers to change the design of the racks “several times” as it tries to overcome the problem. More here. Blackwell, launched earlier this year, is targetted at datacentres that train AI models such as the latest generations of GPT, Claude and Gemini, and which run AI chatbots. Revolut, Britain’s most valuable fintech firm, has been granted a UK trading licence by the FCA. The decision will allow Revolut to offer new trading products and features for UK customers next year, thought to include trading of UK and EU stocks and ETFs. Until now, Revolut has operated its Trading feature in the UK as “an Appointed Representative with a Principal”, meaning it could allow retail customers to buy and sell shares listed in the US. Yana Shkrebenkova, Head of Wealth and Trading UK at Revolut, explains: “Today’s announcement is a significant milestone for Revolut Trading. Having launched our successful investment product five years ago, we strive to bring best in class investment products to our customers in the UK. We know that there is so much more our Revolut Trading customers want from our platform and we are working hard to deliver on this, rolling out new features safely and considerately. Revolut was granted a UK banking licence – with “restrictions” – in July, after a three-year wrangle with regulators. Bitcoin is slipping back from its recent record highs today. The world’s largest cryptocurrency is down 2% today, at $89,000, away from the record high of almost $93,500 set last week. The dip comes after a dormant bitcoin wallet that had been inactive for 14 years sprung into life last week. Some 2,000 bitcoin, worth almost $180m, were moved from the wallet. The sudden activity caused a lot of excitement in crypto circles, as its last transaction took place in 2010 – when one bitcoin was worth less than a dollar. Bitcoin has been on quite the rally in the last fortnight; it was trading below $70,000 on 5 November, the day of the US election, but started rallying once Donald Trump’s victory was clear. Bill Blain, market strategist at Wind Shift Capital, suggests Bitcoin may have been experiencing “a classic greater fool moment”, saying: As Bitcoin soars 30%, there are signs long-term holders’ wallets are being opened to sell as new buyers are persuaded to pile-in on stories about deregulation, crypto as an asset, and the usual get rich scams. Classic pump and dump. Shares in Tesla have jumped almost 7% in pre-market trading, following a report that Donald Trump’s administration could ease US rules for self-driving cars. According to Bloomberg, the Trump team plan to make a federal framework for fully self-driving vehicles one of the Transportation Department’s priorities, As Bloomberg point out, that’s good news for leading Trump supporter Elon Musk: If new rules enable cars without human controls, it will directly benefit Elon Musk, the Tesla Inc. chief executive officer and Trump mega-donor who’s become a powerful fixture in the president-elect’s inner circle. He’s bet the future of the EV maker on self-driving technology and artificial intelligence. More here: Trump Team Is Seeking to Ease US Rules for Self-Driving Cars While Tesla’s shares are on track to jump when trading begins in under two hours, shares in Uber – who could lose out if Tesla succeeds in launching autonomous robotaxis – are down 2.7% in pre-market. The Czech Republic’s top central banker is concerned that consumer prices around the worlw will be more volatile than in the past. This will mean tighter monetary and fiscal policies than before to keep inflation near target, Czech central bank Governor Ales Michl believes. In remarks posted on the Czech National Bank’s website on Monday, Michl says: After a period of high inflation, we are now entering a phase of higher inflation volatility around central bank targets, with an upside risk. Michl argued that there had been excessive money creation in the run-up to the Covid-19 pandemic, because interest rates were kept near zero for over a decade after the financial crisis. He told a central banking conference in Mexico City: This has led to persistent inflationary pressures. To address this, the policy mix should consist of two elements: firstly, maintaining interest rates higher than pre-COVID levels for a prolonged period; and secondly, governments must balance their budgets. Failure to do so could risk a second wave of inflation, with another cost shock potentially acting as a trigger. Donald Trump’s immigration pledges may be the real macro threat to economic growth, rather than tariffs, suggests Neil Shearing, group chief economist at Capital Economics. Shearing told clients: As the dust settles on Donald Trump’s stunning election victory, attention has quickly turned to his policy pledges and their implications for the US economic outlook. Global policymakers and investors are understandably focused on his pledges to raise tariff barriers across the board – and by significant amounts in some US trading relationships. But the economic hit from efforts to raise trade barriers isn’t likely to be as large as many fear. The major threat from Donald Trump’s pledges will instead come from his stated intention to remove millions of migrant workers from the US. One of Britain’s biggest housebuilders, Vistry Group, still reeling from two profit warnings, is also under pressure from shareholders over its boss’s multiple roles and corporate governance concerns. Greg Fitzgerald, Vistry’s chief executive, also chairs the company, which breaches corporate governance code guidance. It means he is running both the business and the board of directors. At the company’s last general meeting in May, Fitzgerald’s re-election was only backed by 79.3% of shareholders - with more than a fifth voting against or abstaining. Vistry, formerly known as Bovis Homes, said in a statement today: “The board has actively engaged with shareholders both before and after the AGM in respect of a range of corporate governance matters and has a detailed understanding of shareholder views. The board understands that the primary concerns from some shareholders was in relation to the combination of the role of the CEO and chair, which was a departure from the UK Corporate Governance Code.” The housebuilder said it had appointed a senior independent director, Rob Woodward, to “provide additional oversight on governance matters and serve as an alternative point of communication for investors and the other non-executive directors”. He has held a series of calls with shareholders to discuss corporate governance. Vistry said the results of an external assessment of the combined role of CEO and chair will be published in is 2024 annual report. It said that through the process, shareholders “have expressed different perspectives”. “The company remains committed to ongoing dialogue with shareholders and will continue to engage to ensure that the company understands shareholders’ views and is able to consider feedback, as well as to provide clarity on the company’s approach to succession planning going forward.” It is not only Fitzgerald’s combined role that has raised eyebrows. He owns a 40% stake in the Devon-based developer Baker Estates and has banked £5.2m in the past three years, while also owning shares in Ardent Hire, which supplies forklift trucks to Vistry, according to the Sunday Times. Corporate governance experts have raised concerns about Fitzgerald’s multiple roles and stakes in related companies, raising potential conflicts of interest, and “inadequate disclosures” by Vistry, according to the paper. A Perth-headquartered goldminer has agreed to give the equivalent of £130m – more than its entire cash reserves – to the government of Mali after its chief executive and two other employees were detained by authorities in the West African country. Resolute Mining CEO Terence Holohan and the other two employees – all British citizens – were unexpectedly detained on 8 November in Mali’s capital of Bamako, at the conclusion of a meeting with government mining and tax officials. The meeting was to progress what Resolute described as unsubstantiated open claims against the company regarding taxes, custom levies, maintenance and management of offshore accounts. To resolve the matter, Resolute said on Monday it had paid Mali $80m out of its $157m in cash reserves, and promised to pay another $80m more in coming months. Britain’s financial watchdog has banned a company director after he failed to tell them he had been imprisoned for grievous bodily harm. The Financial Conduct Authority has banned Ari Harris from working in financial services, following his failure to disclose he had been jailed for three years in 2022. Harris, the FCA says, stabbed a man twice in the neck with a kitchen knife in 2018, during a confrontation in a public carpark, and pleaded guilty to GBH. He, and his firm Reeds Motors, should have notified the FCA of his offending, conviction and custodial sentence. Instead, the regulator, says they provided false and misleading information to cover up the fact that he was in prison. In a ruling today, the FCA says: Following an application in October 2022, the FCA asked the firm why it needed an additional approved person. Both Mr Harris and the firm stated that this was required as Mr Harris was currently overseas and looking into a business abroad. Mr Harris continued to mislead the FCA during a telephone call, failing to mention that he was actually in prison at the time. The FCA has concluded that there is “a severe risk of an erosion of public confidence” if those who are convicted of violent offences and who “lack honesty, integrity and reputation” are permitted to continue working in the financial services industry. Over in the US, Spirit Airlines has filed for bankruptcy protection today after being dragged down by mounting debts and losses. Spirit, which has been struggling to recover from the drop in travel demand caused by the Covid-19 pandemic, has announced it is entering Chapter 11 proceedings as part of a debt restructuring deal. Spirit, the biggest budget airline. in the US, has lost more than $2.5bn since the start of 2020 and faces looming debt payments totaling more than $1bn, Associated Press reports. The company has reassured customers it will continue operating while the restructuring is conducted, telling them: We are writing to let you know about a proactive step Spirit has taken to position the company for success. Spirit has entered into an agreement with our bondholders that is expected to reduce our total debt, provide increased financial flexibility, position Spirit for long-term success and accelerate investments providing Guests with enhanced travel experiences and greater value. Part of this financial restructuring includes filing a “prearranged” chapter 11. The eurozone’s trade surplus with the rest of the world has widened, partly thanks to a drop in imports from the UK. Data firm eurostat has reported that the eurozone recorded a €12.5bn trade surplus with the rest of the world in September, up from €9.8bn in September 2023. Eurozone exports rose by 0.6%, to €237.8bn, while imports from the rest of the world fell by 0.6% to €225.3bn. While European companies shipped €28.5bn of goods to the UK, up 2%, there was a 10.7% drop in imports from the UK, to €13.1bn. Imports from the US, Switzerland, Norway, Japan, India and Brazil also fell year-on-year: The UK government is being urged to “act fast” over the Thames Water crisis, after the Guardian reported that water supplies are “on a knife-edge” due to serious underinvestment. Our investigation has found that Thames has failed to tackle serious safety concerns or upgrade vital IT systems, meaning that £23bn of its assets that are in urgent need of repair. It appears Thames is in a worse financial state than previously admitted, and neither its managers nor regulators appear to have grasped the perilous state of some of its reservoirs and pipes. As my colleague Anna Isaac reported: Sources described how concerns about the company’s governance and operations had been raised at the highest levels of management. Yet they claimed that the problems had not been tackled, suggesting that the scale of the turnaround required at Thames may have been underestimated. “Operations have been hollowed out and cut to the bone,” a senior source at Thames said. “We’re putting the public at risk by failing to invest in the most basic needs.” They added that, in their view, management had not moved quickly enough to address problems such as weakening explosive infrastructure – such as containers holding the gas produced by sewage – and cracks in reservoirs. They said Thames’s management and the regulator, Ofwat, had been slow to address these problems, allowing them to escalate. Gary Carter, GMB National Officer, says Thames’s previous owners have left it “in a perilous state” (it has £15bn of debt), adding that ministers should be ready to put it into a special administration regime if new investment isn’t agreed: “Thames needs committed long term investment just to keep operating, never mind stop the leaks and cut the sewage spills. “Then it must be held to account and deliver for customers, with its skilled workforce central to the turnaround. If that investment isn’t forthcoming then the Government must act fast and put Thames into special administration. Ministers can’t sit back and watch the car crash.” UK consumer confidence has fallen this month, as households grow gloomier about their financial prospects. The latest poll of consumer sentiment, just released by data firm S&amp;amp;P Global, shows that households reported that their current finances continued to deteriorate in November, while pessimism about the financial outlooks for the year ahead has risen. Households across the UK reported further pressure on their everyday spending, which ate into the amount of cash they had available to spend. It has fallen again this month, at a faster rate than in October. Debt levels rose in November for the first time in three months, the survey found. A gauge of job security also declined, which could be driven by the increase in employer National Insurance contributions announced in the Budget. The poll shows that the budget, at the end of October, has not lifted confidence among households. Worryingly, confidence dropped this month despite the Bank of England cutting interest rates two weeks ago, just as S&amp;amp;P Global began polling households. Chris Williamson, chief business economist at S&amp;amp;P Global Market Intelligence, said: “November is seeing households grow somewhat gloomier again, failing to build on the underlying improvement seen in the months leading up to the General Election. Consumer confidence has fallen back since spiking higher in July amid the election buzz, as ongoing pressure on household finances has resulted in squeezed spending, higher debt and lower savings. A key concern going forward will be the labour market. Rising incomes and busier workplaces have underpinned much of the improvement in consumer sentiment over the past two years, but job security is showing signs of waning. Any intensification of job worries, spurred perhaps the recent measures announced in the Budget, including higher employer National Insurance contributions, could result in a further loss of consumer confidence. This would likely in turn hit consumer spending and economic growth. Analysts at Goldman Sachs have predicted that the increase in employers’ national insurance contributions will weigh on the economy in 2025. In their outlook for the UK economy next year, just released, Goldman say they think growth is likely to cool later in 2025. They believe that wage growth will slow, as firms pass on the impact of higher NICS bills onto their workforce. Goldman say: We expect consumer spending growth to moderate in H2 next year as real disposable income growth falls back. This partly reflects slowing real wage growth; we expect private sector pay increases to cool, partly because of the employer National Insurance Contributions increase being passed on to consumers. Net interest is likely to become a headwind as effective mortgage rates continue to drift up while deposit rates gradually decline. And there is likely to be a continued drag on disposable income from the ongoing freeze on personal income tax thresholds. Trade tensions under the Trump administration will also hurt the UK economy next year, Goldman predict, even if Britain avoids tough new tariffs. They say: Although our base case is that the US only imposes very limited tariffs on the UK, the threat of more significant tariffs is likely to generate uncertainty in the near term, which should weigh on demand. And we expect that uncertainty around tariffs will notably reduce Euro area growth, which is likely to generate spillovers to the UK. Begbies Traynor also reveals that their employment costs are expected to rise by £1.25m due to the increase in employers’ national insurance contributions. The company is “reviewing options to mitigate the impact where possible”. The higher employment costs announced in last month’s budget are likely to push more companies into financial trouble, insolvency advisers Begbies Traynor warned this morning. Begbies Traynor also cautioned that firms will be hurt by the prospect that UK borowing costs remain high for longer than hoped. In a trading update, Ric Traynor, executive chairman of Begbies Traynor Group, told the City: “Additional headwinds for UK business from increased employment costs and the prospect of higher for longer interest rates are likely to extend the period of elevated insolvency levels, increasing the need for advice and support from our insolvency and business recovery professionals.” Begbies has already been busy; it has reported a 16% increase in revenues and adjusted pre-tax profits for the six months to the end of October. Ric Traynor says: “We have made a very good start to the year with double digit growth in revenue and profits driven by positive momentum across the group. This gives us confidence that we will deliver market expectations for the year as a whole. Reeves’s decision to raise employers’ national insurance contributions (NICs) has been criticised by retailers, especially in the services sector, and disability charities. The UK minimum wage is also increasing from April. Marks &amp;amp; Spencer have warned that budget measures could cost it more than £60m next year, while Sainsbury’s expects to pay another £140m in NICs, which could push up prices on the shelves. The Bank of England expects interest rates to fall more slowly, as inflation is likely to be higher due to the measures in the Budget. Donald Trump could knock almost 1% off the size of the UK economy if he imposes new tariffs on imports into the US, analysts have warned. The CEBR thinktank have calculated that if the US imposes a 20% tariff on all imports, and a 60% tafiff on China, it could reduce the UK economy by 0.9% by the end of the Trump administration, even if other countries don’t retaliate. The CEBR cautions that Trump’s re-election could reshape global dynamics, “particularly in trade, energy, and environmental policy”. There is also a risk that energy prices are pushed higher (leading to higher bills) if retaliatory action is taken agaisnt US tariff. The CEBR say: During Trump’s first term, the Brent-WTI price differential peaked at $7.34 per barrel in 2019, roughly a 118% increase from the start of his administration, despite a drive to boost domestic oil and gas production. This was largely driven by buyers’ reluctance to purchase US energy exports. However, shifts in global energy dynamics mean significant oil price rises are less likely this time around. China, once a major importer of US energy commodities, now sources discounted supplies from Russia, while its domestic economic slowdown has dampened its energy demand. OPEC also has spare production capacity, given it is currently implementing an output cut of 2.2 million barrels a day to support prices. The easiest way for the UK to avoid Trump tariffs would be to agree to a Free Trade Agreement, the CEBR adds. This could reduce existing trade barriers, as well as dodging new tariffs. CEBR adds: Unfortunately, the major sticking point to a deal remains food standards, and tariffs may be used to pressure the UK to accept US demands in this regard. Last weekend, one of Trump’s senior advisers said the UK “has to choose” between the European Union and US economic models, and that the next president would be more willing to clinch a free trade agreement with the UK if it turns away from the EU’s “socialism”. Today’s prediction that energy prices for those on default tariffs will rise again in January are another kick in the teeth for households, says Richard Neudegg, director of regulation at Uswitch.com. “This price hike would mean the average household on a standard variable tariff would pay 1% more on their rates from January, just at the time when households typically use the most energy. “The price cap is supposed to protect consumers, but millions face paying more during the coldest months of the year. Neudegg adds that customers can fix their bills below January’s predicted price cap level*, saying: “There are now a range of fixed deals available that are significantly cheaper than the predicted price cap for January, so it is well worth running a comparison to see how much you could save. Right now, the average household could save up to £120 per year against the current price cap by switching to a fixed deal. “Consumers who are worried about paying their energy bill should check what energy help they are eligible for, and contact their supplier who may be able to offer support.” * – reminder: Cornwall Insight expect prices to drop in April and October, when the quarterly cap changes again. The oil price is rising this morning, after the conflict between Russia and Ukraine intensified last weekend. Brent crude, the international benchmark, is up 0.3% at $71.26 per barrel, having hit its lowest level since the start of October on Friday. The rise follows the fierce missile and drone attack launched by Russia last weekend at Ukraine’s energy grid, which killed seven people and forced nationwide electricity rationing to be introduced today. Ukrenergo, Ukraine’s principal energy supplier, said blackouts and consumption restrictions would be introduced “in all regions” as engineers tried to repair as much of the damage to power facilities as possible. Russia has also accused Joe Biden’s administration of “trying to escalate the situation to the maximum”, after the White House lifted the ban on Ukraine using long-range missiles to fire into Russian territory yesterday. Here’s the details of Cornwall Insight’s forecasts for Britain’s energy price cap from January. This morning’s prediction of a small rise in energy bills in January will be “disappointing”, says Dr Craig Lowrey, Principal Consultant at Cornwall Insight, especially as the weather gets chillier. “Our final price cap forecast for January indicates, as expected, bills will remain largely unchanged from October. Supply concerns have kept the market as volatile as earlier in the year, and additional charges have remained relatively stable, so prices have stayed flat. While we may have seen this coming, the news that prices will not drop from the rises in the Autumn will still be disappointing to many as we move into the colder months. “Fuel poverty has occupied political agendas for years, with little long-term progress. This winter, millions of households say they will not heat their homes to recommended temperatures, risking serious health consequences. With it being widely accepted that high prices are here to stay, we need to see action. Options like social tariffs, adjustments to price caps, benefit restructuring, or other targeted support for vulnerable households must be seriously considered. “Long-term, our transition away from the volatile global wholesale market toward sustainable, home-produced renewables can help to secure our energy future. Although the transition does require upfront investment, it promises lower bills down the line. The government needs to keep momentum on the transition while acknowledging that immediate support is essential for those struggling now. Inaction is a choice to leave people in the cold.” Good morning, and welcome to our rolling coverage of business, the financial markets and the world economy. Household energy bills across Great Britain are set to rise at the start of next year, analysts predict, putting more pressure on household finances. Officially, the price cap for January-March 2025 will be set on Friday morning by regulator Ofgem, limiting what energy providers can charge in England, Scotland and Wales. But analysts at Cornwall Insight have crunched the numbers, and predict that the cap for a typical dual fuel household will rise to £1,736 per annum in January, up from the current level of £1,717 per year set in October. This is a rise of 1% from the current price cap – a blow to hopes that bills might drop at the start of 2025. Importantly, though, the cap limits the amount that a consumer can be charged for each unit of energy – not a ceiling on potential bills, which are usually higher in the winter as households spend more to keep warm. Cornwall Insight, whose calculations are based on the wholesale price of energy, say: The cap level is a reflection of a relatively volatile wholesale market, influenced by supply concerns tied to geopolitical tensions, maintenance on Norwegian gas infrastructure, weather disruptions, amongst other smaller factors. Despite prices stabilising in comparison to the past two years, the market remains very sensitive to global events. This is leaving prices substantially above historic averages. At the end of September, Cornwall had expected the price cap would dip in January, but wholesale energy prices have been higher than hoped. Last Friday, the month-ahead price of UK gas rose to a one-year high of almost 120p per therm. Gas prices rose last week, after Austrian group OMV warned of a potential disruption to supplies from Russia. On Saturday, Gazprom did indeed stop supplies to Austria, after OMV won a €230m arbitration award against Russia’s state-owned natural gas company. Looking further ahead, Cornwall currently forecast the cap will drop slightly in April 2025 and again in October 2025. The agenda 8am GMT: Bundesbank President Joachim Nagel gives speech 10am GMT: Euroz</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Britain and the United States have signed a new agreement for civil nuclear collaboration at the COP29 summit. The agreement aims to pool billions in research funds and share information on advanced nuclear technologies. The goal is to speed up the development of new technologies, such as advanced modular reactors, to help decarbonise industry.</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>The financial regulator has been ordered to encourage more risk-taking across the City, raising concerns that the Labour government is in danger of watering down rules meant to avoid another financial crisis. In an official “remit” letter addressed to Financial Conduct Authority (FCA) boss, Nikhil Rathi, the chancellor, Rachel Reeves, said regulations meant to protect consumers should not stand in the way of “sensible risk-taking” by investors and the wider financial sector, which includes banks, asset managers and insurers. The remit letter, which is sent to regulators once a parliament to outline government priorities, explained that the FCA should be accelerating efforts to support the growth and competitiveness of City firms, as part of new responsibilities handed to watchdogs last year. “I recognise that there are difficult trade-offs to make,” the chancellor’s letter said. “Ultimately we must trust in the systems that we have put in place to manage the impact when things do go wrong – so that problems with one firm don’t create wider risks, or lead to an over-correction in the future.” As part of its response to the chancellor, the FCA said: “When it comes to growth, regulation is one part of the picture. We know there’s more to do but we are committed to playing our part.” It came hours after Reeves told City bankers gathered for the annual Mansion House dinner that regulations put in place to protect the economy after the 2007-08 global financial crisis had “gone too far”, raising concerns among campaigners. “A strong financial system is crucial for sustainable growth, but promoting the growth of the financial sector as an end in itself would be a mistake,” said Jesse Griffiths, the chief executive of the leading UK charity Finance Innovation Lab. “There is ample evidence to show that this leads to a focus on the needs of international capital rather than domestic businesses. We must heed the lessons of the global financial crisis, which showed how dangerous a focus on financial deregulation can be for the economy,” Griffiths added. Labour’s lax regulation of the City was blamed for contributing to the collapse of Royal Bank of Scotland in 2008, which exacerbated the global financial crisis. The government was forced spend tens of billions of pounds to bail out a string of banks, leading to years of recession and austerity across the UK. EU and UK governments later tightened regulations, in order to rein in risk-taking and avoid another financial crisis. But Tory ministers began dismantling some of those protections after the Covid-19 pandemic. That included reintroducing a competitiveness objective for regulators, which critics warned could create the same light-touch approach that led to the 2008 crisis. The Labour government has continued tinkering with post-crisis reforms. That includes reforming banker bonus deferral rules, which could lead to bankers getting their payouts three years earlier, and replacing the certification regime that ensures City managers are fit and proper for the job. The Treasury also plans to ease regulations on smaller banks by reforming ringfencing rules, which protect consumer deposits by separating lenders’ retail and investment banking operations. The economist Sir John Kay said the Labour government needed to ensure that reforms were not simply serving City bankers. “Our objective should be the financial sectors serves the needs of the non-financial economy, rather than the needs of the people in it,” Kay told the Guardian. “And these things seem to be confused and conflated in what is being talked about in, for example, the Mansion House speech last night.” The Treasury said: “Robust regulatory standards are the cornerstone of the attractiveness of UK markets, and the stability and soundness of the UK’s financial system is an important priority for the government. “The UK will remain a global leader in promoting high industry standards, while ensuring regulation supports growth so that everyone is better off.” Alongside the new instructions to City regulators, the chancellor published an updated remit for the Bank of England’s monetary policy committee (MPC). The inflation target remains unchanged at 2%, but Reeves – a former Bank economist herself – tweaked the description of the government’s economic policy, to encourage “broad based and resilient growth built on strong and secure foundations”. The phrase “broad based” is likely to be a reference to the need to rebalance the UK economy so that growth is less concentrated in the south-east.</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Financial Conduct Authority (FCA) ordered to encourage more risk-taking. Labour government in danger of watering down rules to avoid another financial crisis. Chancellor Rachel Reeves said regulations should not stand in the way of ‘sensible risk taking’ by investors and the wider financial sector.</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Rachel Reeves has told City bankers attending her Mansion House speech that regulations put in place to protect the economy after the global financial crisis had “gone too far”. Speaking at the glitzy annual gathering in the Square Mile on Thursday, the chancellor called the financial services sector the “crown jewel” of the UK economy. She argued that tighter rules on banks and investment institutions after the 2007-8 crash had created “a system which sought to eliminate risk-taking”. “While it was right that successive governments made regulatory changes after the global financial crisis, to ensure that regulation kept pace with the global economy of the time, it is important that we learn the lessons of the past,” Reeves said. “These changes have resulted in a system which sought to eliminate risk-taking. That has gone too far and, in places, it has had unintended consequences, which we must now address.” The last Labour government had encouraged the City regulator to take a “light touch” approach to regulating the financial services sector, but was then forced to step in and bail out a string of banks when the US sub-prime mortgage crisis prompted a catastrophic chain reaction. At the time, regulators were accused of failing to rein in the risky behaviours that had led to the crisis, which plunged the UK into recession. But Reeves suggested she now believed it was time to loosen some of the constraints that were subsequently imposed on the sector. “We cannot take the UK’s status as a global financial centre for granted. In a highly competitive world we need to earn that status and we need to work to keep it,” she said. The Bank of England governor, Andrew Bailey, also addressed the Mansion House dinner, stressing the UK’s longstanding support for free trade, as Donald Trump prepares to slap US tariffs on imports. “I will own up to being an old fashioned free trader at heart. It’s a British characteristic, I like to think. My point is this: amidst the important need to be alert to threats to economic security, let’s please remember the importance of openness,” Bailey said. Economists have said that if Trump goes ahead with his plan for a universal tariff of 10% on all imports, it could cut the UK’s growth rate next year to a sickly 0.4%. Bailey also underlined the continued impact of Brexit on the UK economy. “The changing trading relationship with the EU has weighed on the level of potential supply,” he said, adding that the government should, “be alert to and welcome opportunities to rebuild relations while respecting the decision of the British people. The chancellor set out a series of changes, some of which were proposed by her immediate predecessor, Jeremy Hunt. These include obliging regulators to take into account growth, as well as financial stability; and replacing the current “certification” regime for investment professionals, with a “more proportionate approach”. The Financial Conduct Authority has already announced plans to streamline its rulebook for firms to reduce compliance costs, in the hope of promoting growth. Reeves believes that bolstering private investment is key to improving the UK’s growth rate. She has also announced plans for a mega-merger of public sector pension funds, in the hope of unleashing capital to back UK infrastructure projects. The chancellor is keen to stress Labour’s pro-business credentials after her first budget, which increased employer national insurance contributions (NICs) from April.”</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Rachel Reeves tells City bankers that regulations have 'gone too far' She calls the financial services sector the 'crown jewel' of the UK economy. The Bank of England governor Andrew Bailey also addressed the Mansion House dinner.</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>UK Economic Challenges Overview</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Time to recap. Average UK mortgage rates have risen as major lenders hike their rates, despite the Bank of England’s cut to borrowing costs last week. The European Commission has fined Meta almost €800m for breaching EU competition law with its classified ads service, Facebook Marketplace. Luxury goods maker Burberry has posted its biggest share price jump in the last 20 years, after announcing a cost-cutting scheme and a turnaround plan. The pound has recovered earlier losses, which saw it hit its lowest level against the US dollar since July. Gas prices in the UK and Europe hit their highest level in a year, due to fears of supply disruption from Russia and the colder weather. Shares in Disney have hit a six-month high, after it beat Wall Street expectations thanks to its Inside Out 2 and Deadpool &amp;amp; Wolverine films. Rachel Reeves will announce plans to merge local government retirement schemes into “megafunds” as she tries to revive long-running efforts to overhaul the public pension system. Burberry has posted its best day on the London stock market in at least the last 20 years. Shares in the luxury goods maker have closed for the night up 18.6%, which is its biggest daily rise since at least November 2004 (my data doesn’t go any further back!). The City are welcoming Burberry’s new £40m cost-cutting programme and turnaround plan to revive the fortunes of the ailing British luxury fashion brand. Geopolitical uncertainties and rising costs are encouraging companies to ‘reshore’ their operations closer to home, a new survey from Bain &amp;amp; Company shows. Bain’s biennial operations survey of CEOs and chief operating officers has found a rise in companies planning, or already investing in and executing, reshoring and near-shoring. According to Bain, 81% of CEOs and COOs say their companies have plans to bring supply chains closer to home or to their main market, up from 63% in 2022. There’s also increased interest in ‘split-shoring’, where businesses balance a mix of offshore production with other key manufacturing activity close to home. One factor is that companies are trying to cut their dependence on China. A second is Joe Biden’s 2022 Inflation Reduction Act, which provides US companies with subsidies and tax credits to incentivize reshoring and near-shoring. Hernan Saenz, partner at Bain &amp;amp; Company and global head of its Performance Improvement practice, says: “We believe the current acceleration of reshoring across key markets worldwide is a crucial trend that demands CEOs’ attention. The multiple disruptions companies have grappled with since the pandemic mean the question for company leaders is no longer whether to reinvent supply chains but how to do that so their operations are made more cost-competitive, resilient, sustainable, and agile in responding to evolving markets and customer needs.” Although the euro has also recovered from its earlier lows, the growing economic gap between the US and Europe threatens to weigh on the currency in future, economist Mohamed El-Erian has warned. El-Erian, the chief economic adviser to Allianz, told Bloomberg TV today: “If you look at the good, the bad and the ugly of the global economy, unfortunately Europe is the ugly. The market has understood that divergence is a major story going forward.” Back in the financial markets, the pound has recovered its earlier losses against the US dollar to trade just over $1.27. Meta has pledged to appeal against the EU’s fine. It says: “Today, the European Commission announced a decision claiming that Facebook Marketplace has hindered competition for online marketplaces in Europe. “This decision ignores the realities of the thriving European market for online classified listing services and shields large incumbent companies from a new entrant, Facebook Marketplace, that meets consumer demand in innovative and convenient new ways. “We will appeal this decision to ensure that consumers are well served in the EU.” The European Commission has fined Meta almost €800m for breaching EU competition law with its classified ads service, Facebook Marketplace. The Commission fined Meta €797.72m for tying Marketplace to its Facebook social media platform, which meant consumers on Facebook were regularly exposed to Marketplace whether or not they wanted to be. This gave Meta a “substantial distribution advantage” over rival classified ad platforms. The ruling also said Meta had unilaterally imposed unfair trading conditions on other classified ads services providers who advertise on Meta’s platforms, including allowing Meta to use ad-related data generated by other advertisers for the benefit of Facebook Marketplace. It orders Meta to bring the conduct to an end and refrain from repeating the infringement, in addition to the fine. The Commission said that while market dominance was in itself not illegal under EU antitrust rules, dominant companies have a special responsibility not to abuse their powerful market position by restricting competition. Margrethe Vestager, executive vice-president of the Commission in charge of competition policy, says: “Today we fine Meta 797.72 million euros for abusing its dominant positions in the markets for personal social network services and for online display advertising on social media platforms. “Meta tied its online classified ads service Facebook Marketplace to its personal social network Facebook and imposed unfair trading conditions on other online classified ads service providers. “It did so to benefit its own service Facebook Marketplace, thereby giving it advantages that other online classified ads service providers could not match. This is illegal under EU antitrust rules. “Meta must now stop this behaviour.” The average cost of household building work is up by almost a fifth (19%) on the last quarter, according to new data reported by PA Media today. The average cost of a building job is now £12,634 due to the higher cost of labour and materials, up from £10,626 in July to September this year, Checkatrade’s inaugural UK Home Improvement Index found. However the increase has not dampened consumer demand, with the number of building jobs up by 1% between quarters one and three, the data, based on more than 10.5 million jobs carried out by tradespeople in the UK, shows. The average cost of a kitchen fitting has gone up by 12% on the previous quarter – now £7,376 compared with £6,574, while insulation installation costs are up 20% to an average £4,634. The average cost of a plastering job in the third quarter was up 16% to £2,343 and gardening jobs increased by 10% to £679. The average “handyman” job – typically of a smaller scale than building work – increased by 25% from to £563. Shares in Disney have jumped almost 10% at the start of trading in New York, as traders welcome its forecast-beating results. They’re up 9.8% at $112.77, their highest level since May. The UK and Scottish governments are to pump £100m into new energy and economic regeneration projects around the closure-hit Grangemouth oil refinery and the neighbouring town of Falkirk. The deal, which is being signed in Falkirk by Scottish and UK ministers today, includes a new “carbon utilisation” centre to reuse waste CO2, and a bioeconomy accelerator pilot project for the whisky and food sectors at Grangemouth, where Petro-Ineos plans to close down Scotland’s last oil refinery in June 2025. Its closure, which will lead to more than 400 direct job losses and hit several thousand people in the wider economy, is the most serious immediate challenge to the UK government’s green jobs and energy transition agenda in Scotland, where the oil industry is a powerful force. Highly skilled workers may emigrate, as most face significant uncertainty. There are proposals for carbon capture pilots, and sustainable aviation fuel and hydrogen production projects there but widespread scepticism about their likely success. The Scottish and UK governments are co-investing £80m in the overall growth deal and £20m on new energy projects at Grangemouth; Falkirk council and Scottish Canals are spending a further £49m. Forth V